<commit_message>
Start input Q321 & Q320 info
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4BAA1B-58E5-4F7B-8CBE-F8C410342AC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA67803A-2104-4C35-B8E7-B518DEF62D0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="185">
   <si>
     <t>$ERJ</t>
   </si>
@@ -613,17 +613,30 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/6180d10a-38ab-421f-9f8b-22fbb0bcd380?origin=1</t>
+  </si>
+  <si>
+    <t>Embraer 190-E2</t>
+  </si>
+  <si>
+    <t>Large Jets</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,6 +715,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arai"/>
     </font>
   </fonts>
   <fills count="5">
@@ -823,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -906,37 +925,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -965,14 +953,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -980,13 +982,34 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1083,7 +1106,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1100,7 +1123,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13315950" y="0"/>
-          <a:ext cx="0" cy="21402675"/>
+          <a:ext cx="0" cy="21564600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1133,7 +1156,7 @@
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1475,59 +1498,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:X42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+    <row r="5" spans="1:24">
+      <c r="B5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="G5" s="44" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+      <c r="G5" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="46"/>
-      <c r="U5" s="44" t="s">
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="62"/>
+      <c r="U5" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="46"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="V5" s="61"/>
+      <c r="W5" s="61"/>
+      <c r="X5" s="62"/>
+    </row>
+    <row r="6" spans="1:24">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>9.84</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="D6" s="18"/>
       <c r="G6" s="9">
@@ -1553,7 +1576,7 @@
       <c r="W6" s="37"/>
       <c r="X6" s="38"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1578,20 +1601,20 @@
       <c r="P7" s="37"/>
       <c r="Q7" s="37"/>
       <c r="R7" s="38"/>
-      <c r="U7" s="59" t="s">
+      <c r="U7" s="46" t="s">
         <v>84</v>
       </c>
       <c r="V7" s="37"/>
       <c r="W7" s="37"/>
       <c r="X7" s="38"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12">
         <f>C6*C7</f>
-        <v>7228.4639999999999</v>
+        <v>6941.9699999999993</v>
       </c>
       <c r="D8" s="18"/>
       <c r="G8" s="10"/>
@@ -1608,19 +1631,19 @@
       <c r="P8" s="37"/>
       <c r="Q8" s="37"/>
       <c r="R8" s="38"/>
-      <c r="U8" s="58" t="s">
+      <c r="U8" s="45" t="s">
         <v>137</v>
       </c>
       <c r="V8" s="37"/>
       <c r="W8" s="37"/>
       <c r="X8" s="38"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="12">
-        <f>'Financial Model'!S105</f>
+        <f>'Financial Model'!S106</f>
         <v>2102.6</v>
       </c>
       <c r="D9" s="18" t="str">
@@ -1639,19 +1662,19 @@
       <c r="P9" s="37"/>
       <c r="Q9" s="37"/>
       <c r="R9" s="38"/>
-      <c r="U9" s="60" t="s">
+      <c r="U9" s="47" t="s">
         <v>151</v>
       </c>
       <c r="V9" s="37"/>
       <c r="W9" s="37"/>
       <c r="X9" s="38"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="12">
-        <f>'Financial Model'!T106</f>
+        <f>'Financial Model'!T107</f>
         <v>3173.8999999999996</v>
       </c>
       <c r="D10" s="18" t="str">
@@ -1674,14 +1697,14 @@
       <c r="P10" s="37"/>
       <c r="Q10" s="37"/>
       <c r="R10" s="38"/>
-      <c r="U10" s="60" t="s">
+      <c r="U10" s="47" t="s">
         <v>152</v>
       </c>
       <c r="V10" s="37"/>
       <c r="W10" s="37"/>
       <c r="X10" s="38"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1707,20 +1730,20 @@
       <c r="P11" s="37"/>
       <c r="Q11" s="37"/>
       <c r="R11" s="38"/>
-      <c r="U11" s="60" t="s">
+      <c r="U11" s="47" t="s">
         <v>153</v>
       </c>
       <c r="V11" s="37"/>
       <c r="W11" s="37"/>
       <c r="X11" s="38"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="13">
         <f>C8-C11</f>
-        <v>8299.7639999999992</v>
+        <v>8013.2699999999986</v>
       </c>
       <c r="D12" s="19"/>
       <c r="G12" s="10"/>
@@ -1740,7 +1763,7 @@
       <c r="W12" s="37"/>
       <c r="X12" s="38"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24">
       <c r="G13" s="10"/>
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
@@ -1753,14 +1776,14 @@
       <c r="P13" s="37"/>
       <c r="Q13" s="37"/>
       <c r="R13" s="38"/>
-      <c r="U13" s="58" t="s">
+      <c r="U13" s="45" t="s">
         <v>138</v>
       </c>
       <c r="V13" s="37"/>
       <c r="W13" s="37"/>
       <c r="X13" s="38"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24">
       <c r="G14" s="10"/>
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
@@ -1773,19 +1796,19 @@
       <c r="P14" s="37"/>
       <c r="Q14" s="37"/>
       <c r="R14" s="38"/>
-      <c r="U14" s="60" t="s">
+      <c r="U14" s="47" t="s">
         <v>154</v>
       </c>
       <c r="V14" s="37"/>
       <c r="W14" s="37"/>
       <c r="X14" s="38"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="44" t="s">
+    <row r="15" spans="1:24">
+      <c r="B15" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -1798,24 +1821,24 @@
       <c r="P15" s="37"/>
       <c r="Q15" s="37"/>
       <c r="R15" s="38"/>
-      <c r="U15" s="60" t="s">
+      <c r="U15" s="47" t="s">
         <v>155</v>
       </c>
       <c r="V15" s="37"/>
       <c r="W15" s="37"/>
       <c r="X15" s="38"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="66"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -1828,21 +1851,21 @@
       <c r="P16" s="37"/>
       <c r="Q16" s="37"/>
       <c r="R16" s="38"/>
-      <c r="U16" s="60" t="s">
+      <c r="U16" s="47" t="s">
         <v>156</v>
       </c>
       <c r="V16" s="37"/>
       <c r="W16" s="37"/>
       <c r="X16" s="38"/>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24">
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="48"/>
+      <c r="D17" s="66"/>
       <c r="G17" s="9">
         <v>43922</v>
       </c>
@@ -1864,10 +1887,10 @@
       <c r="W17" s="37"/>
       <c r="X17" s="38"/>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="66"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
         <v>169</v>
@@ -1882,17 +1905,17 @@
       <c r="P18" s="37"/>
       <c r="Q18" s="37"/>
       <c r="R18" s="38"/>
-      <c r="U18" s="59" t="s">
+      <c r="U18" s="46" t="s">
         <v>139</v>
       </c>
       <c r="V18" s="37"/>
       <c r="W18" s="37"/>
       <c r="X18" s="38"/>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:24">
       <c r="B19" s="17"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="68"/>
       <c r="G19" s="10"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
@@ -1904,17 +1927,17 @@
       <c r="O19" s="37"/>
       <c r="P19" s="37"/>
       <c r="Q19" s="37"/>
-      <c r="R19" s="64" t="s">
+      <c r="R19" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="U19" s="58" t="s">
+      <c r="U19" s="45" t="s">
         <v>142</v>
       </c>
       <c r="V19" s="37"/>
       <c r="W19" s="37"/>
       <c r="X19" s="38"/>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:24">
       <c r="G20" s="10"/>
       <c r="H20" s="37"/>
       <c r="I20" s="37"/>
@@ -1927,14 +1950,14 @@
       <c r="P20" s="37"/>
       <c r="Q20" s="37"/>
       <c r="R20" s="38"/>
-      <c r="U20" s="58" t="s">
+      <c r="U20" s="45" t="s">
         <v>141</v>
       </c>
       <c r="V20" s="37"/>
       <c r="W20" s="37"/>
       <c r="X20" s="38"/>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:24">
       <c r="G21" s="10"/>
       <c r="H21" s="37"/>
       <c r="I21" s="37"/>
@@ -1947,19 +1970,19 @@
       <c r="P21" s="37"/>
       <c r="Q21" s="37"/>
       <c r="R21" s="38"/>
-      <c r="U21" s="58" t="s">
+      <c r="U21" s="45" t="s">
         <v>140</v>
       </c>
       <c r="V21" s="37"/>
       <c r="W21" s="37"/>
       <c r="X21" s="38"/>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B22" s="44" t="s">
+    <row r="22" spans="2:24">
+      <c r="B22" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="62"/>
       <c r="G22" s="10"/>
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
@@ -1972,21 +1995,21 @@
       <c r="P22" s="37"/>
       <c r="Q22" s="37"/>
       <c r="R22" s="38"/>
-      <c r="U22" s="58" t="s">
+      <c r="U22" s="45" t="s">
         <v>157</v>
       </c>
       <c r="V22" s="37"/>
       <c r="W22" s="37"/>
       <c r="X22" s="38"/>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24">
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="48"/>
+      <c r="D23" s="66"/>
       <c r="G23" s="10"/>
       <c r="H23" s="37"/>
       <c r="I23" s="37"/>
@@ -2004,14 +2027,14 @@
       <c r="W23" s="37"/>
       <c r="X23" s="38"/>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24">
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="65">
         <v>1969</v>
       </c>
-      <c r="D24" s="48"/>
+      <c r="D24" s="66"/>
       <c r="G24" s="10"/>
       <c r="H24" s="37"/>
       <c r="I24" s="37"/>
@@ -2024,17 +2047,17 @@
       <c r="P24" s="37"/>
       <c r="Q24" s="37"/>
       <c r="R24" s="38"/>
-      <c r="U24" s="59" t="s">
+      <c r="U24" s="46" t="s">
         <v>143</v>
       </c>
       <c r="V24" s="37"/>
       <c r="W24" s="37"/>
       <c r="X24" s="38"/>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="66"/>
       <c r="G25" s="9">
         <v>43770</v>
       </c>
@@ -2051,24 +2074,24 @@
       <c r="P25" s="37"/>
       <c r="Q25" s="37"/>
       <c r="R25" s="38"/>
-      <c r="U25" s="58" t="s">
+      <c r="U25" s="45" t="s">
         <v>144</v>
       </c>
       <c r="V25" s="37"/>
       <c r="W25" s="37"/>
       <c r="X25" s="38"/>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:24">
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="70">
-        <f>'Financial Model'!T58</f>
+      <c r="C26" s="63">
+        <f>'Financial Model'!T59</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="71"/>
+      <c r="D26" s="64"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="63" t="s">
+      <c r="H26" s="50" t="s">
         <v>168</v>
       </c>
       <c r="I26" s="37"/>
@@ -2081,17 +2104,17 @@
       <c r="P26" s="37"/>
       <c r="Q26" s="37"/>
       <c r="R26" s="38"/>
-      <c r="U26" s="58" t="s">
+      <c r="U26" s="45" t="s">
         <v>145</v>
       </c>
       <c r="V26" s="37"/>
       <c r="W26" s="37"/>
       <c r="X26" s="38"/>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="66"/>
       <c r="G27" s="10"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
@@ -2104,14 +2127,14 @@
       <c r="P27" s="37"/>
       <c r="Q27" s="37"/>
       <c r="R27" s="38"/>
-      <c r="U27" s="58" t="s">
+      <c r="U27" s="45" t="s">
         <v>146</v>
       </c>
       <c r="V27" s="37"/>
       <c r="W27" s="37"/>
       <c r="X27" s="38"/>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24">
       <c r="B28" s="10" t="s">
         <v>23</v>
       </c>
@@ -2139,21 +2162,21 @@
         <v>180</v>
       </c>
       <c r="R28" s="38"/>
-      <c r="U28" s="58" t="s">
+      <c r="U28" s="45" t="s">
         <v>147</v>
       </c>
       <c r="V28" s="37"/>
       <c r="W28" s="37"/>
       <c r="X28" s="38"/>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:24">
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="54"/>
+      <c r="D29" s="72"/>
       <c r="G29" s="10"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
@@ -2171,7 +2194,7 @@
       <c r="W29" s="37"/>
       <c r="X29" s="38"/>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:24">
       <c r="G30" s="10"/>
       <c r="H30" s="37"/>
       <c r="I30" s="37"/>
@@ -2189,7 +2212,7 @@
       <c r="W30" s="37"/>
       <c r="X30" s="38"/>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:24">
       <c r="G31" s="10"/>
       <c r="H31" s="37"/>
       <c r="I31" s="37"/>
@@ -2202,19 +2225,19 @@
       <c r="P31" s="37"/>
       <c r="Q31" s="37"/>
       <c r="R31" s="38"/>
-      <c r="U31" s="59" t="s">
+      <c r="U31" s="46" t="s">
         <v>149</v>
       </c>
       <c r="V31" s="37"/>
       <c r="W31" s="37"/>
       <c r="X31" s="38"/>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B32" s="44" t="s">
+    <row r="32" spans="2:24">
+      <c r="B32" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="46"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
       <c r="G32" s="10"/>
       <c r="H32" s="37"/>
       <c r="I32" s="37"/>
@@ -2227,22 +2250,22 @@
       <c r="P32" s="37"/>
       <c r="Q32" s="37"/>
       <c r="R32" s="38"/>
-      <c r="U32" s="58" t="s">
+      <c r="U32" s="45" t="s">
         <v>150</v>
       </c>
       <c r="V32" s="37"/>
       <c r="W32" s="37"/>
       <c r="X32" s="38"/>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:24">
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="67">
-        <f>C6/'Financial Model'!T103</f>
-        <v>2.5162613569116163</v>
-      </c>
-      <c r="D33" s="68"/>
+      <c r="C33" s="73">
+        <f>C6/'Financial Model'!T104</f>
+        <v>2.4165314860584122</v>
+      </c>
+      <c r="D33" s="74"/>
       <c r="G33" s="10"/>
       <c r="H33" s="37"/>
       <c r="I33" s="37"/>
@@ -2260,12 +2283,12 @@
       <c r="W33" s="37"/>
       <c r="X33" s="38"/>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:24">
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="55"/>
-      <c r="D34" s="56"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="76"/>
       <c r="G34" s="9">
         <v>43282</v>
       </c>
@@ -2287,12 +2310,12 @@
       <c r="W34" s="35"/>
       <c r="X34" s="36"/>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:24">
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="70"/>
       <c r="G35" s="10"/>
       <c r="H35" s="8" t="s">
         <v>163</v>
@@ -2308,9 +2331,9 @@
       <c r="Q35" s="37"/>
       <c r="R35" s="38"/>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:24">
       <c r="G36" s="11"/>
-      <c r="H36" s="69" t="s">
+      <c r="H36" s="54" t="s">
         <v>165</v>
       </c>
       <c r="I36" s="35"/>
@@ -2324,15 +2347,15 @@
       <c r="Q36" s="35"/>
       <c r="R36" s="36"/>
     </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="U37" s="44" t="s">
+    <row r="37" spans="2:24">
+      <c r="U37" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="V37" s="45"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="46"/>
-    </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="V37" s="61"/>
+      <c r="W37" s="61"/>
+      <c r="X37" s="62"/>
+    </row>
+    <row r="38" spans="2:24">
       <c r="U38" s="42" t="s">
         <v>159</v>
       </c>
@@ -2340,29 +2363,29 @@
       <c r="W38" s="37"/>
       <c r="X38" s="38"/>
     </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="U39" s="57" t="s">
+    <row r="39" spans="2:24">
+      <c r="U39" s="44" t="s">
         <v>160</v>
       </c>
       <c r="V39" s="37"/>
       <c r="W39" s="37"/>
       <c r="X39" s="38"/>
     </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="U40" s="57" t="s">
+    <row r="40" spans="2:24">
+      <c r="U40" s="44" t="s">
         <v>161</v>
       </c>
       <c r="V40" s="37"/>
       <c r="W40" s="37"/>
       <c r="X40" s="38"/>
     </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:24">
       <c r="U41" s="42"/>
       <c r="V41" s="37"/>
       <c r="W41" s="37"/>
       <c r="X41" s="38"/>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:24">
       <c r="U42" s="43"/>
       <c r="V42" s="35"/>
       <c r="W42" s="35"/>
@@ -2405,24 +2428,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
-  <dimension ref="B1:AL120"/>
+  <dimension ref="B1:AL121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V4" sqref="V4:V8"/>
+      <selection pane="bottomRight" activeCell="W118" sqref="W118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="2:38" s="15" customFormat="1">
+      <c r="B1" s="53" t="s">
         <v>170</v>
       </c>
       <c r="C1" s="15" t="s">
@@ -2467,7 +2490,7 @@
       <c r="P1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="58" t="s">
         <v>46</v>
       </c>
       <c r="R1" s="15" t="s">
@@ -2528,14 +2551,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="2:38" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:38" s="21" customFormat="1">
       <c r="B2" s="20"/>
+      <c r="M2" s="22">
+        <v>44104</v>
+      </c>
       <c r="O2" s="22">
         <v>44286</v>
       </c>
       <c r="P2" s="22">
         <v>44377</v>
       </c>
+      <c r="Q2" s="22">
+        <v>44469</v>
+      </c>
       <c r="R2" s="22">
         <v>44196</v>
       </c>
@@ -2546,9 +2575,12 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="3" spans="2:38" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:38" s="21" customFormat="1">
       <c r="B3" s="20"/>
       <c r="P3" s="23"/>
+      <c r="Q3" s="23">
+        <v>44505</v>
+      </c>
       <c r="S3" s="23">
         <v>44679</v>
       </c>
@@ -2556,117 +2588,153 @@
         <v>44777</v>
       </c>
     </row>
-    <row r="4" spans="2:38" s="65" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="72" t="s">
+    <row r="4" spans="2:38" s="52" customFormat="1">
+      <c r="B4" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="O4" s="65">
+      <c r="M4" s="52">
+        <v>177.2</v>
+      </c>
+      <c r="O4" s="52">
         <v>272.2</v>
       </c>
-      <c r="P4" s="65">
+      <c r="P4" s="52">
         <v>388.5</v>
       </c>
-      <c r="R4" s="65">
+      <c r="Q4" s="52">
+        <v>242</v>
+      </c>
+      <c r="R4" s="52">
         <v>413.7</v>
       </c>
-      <c r="S4" s="65">
+      <c r="S4" s="52">
         <v>169.2</v>
       </c>
-      <c r="T4" s="65">
+      <c r="T4" s="52">
         <v>299.89999999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:38" s="65" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="72" t="s">
+    <row r="5" spans="2:38" s="52" customFormat="1">
+      <c r="B5" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="O5" s="65">
+      <c r="M5" s="52">
+        <v>212.3</v>
+      </c>
+      <c r="O5" s="52">
         <v>152.1</v>
       </c>
-      <c r="P5" s="65">
+      <c r="P5" s="52">
         <v>266.2</v>
       </c>
-      <c r="R5" s="65">
+      <c r="Q5" s="52">
+        <v>256.39999999999998</v>
+      </c>
+      <c r="R5" s="52">
         <v>455.4</v>
       </c>
-      <c r="S5" s="65">
+      <c r="S5" s="52">
         <v>89.9</v>
       </c>
-      <c r="T5" s="65">
+      <c r="T5" s="52">
         <v>266.7</v>
       </c>
     </row>
-    <row r="6" spans="2:38" s="65" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="72" t="s">
+    <row r="6" spans="2:38" s="52" customFormat="1">
+      <c r="B6" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="O6" s="65">
+      <c r="M6" s="52">
+        <v>154.69999999999999</v>
+      </c>
+      <c r="O6" s="52">
         <v>128.5</v>
       </c>
-      <c r="P6" s="65">
+      <c r="P6" s="52">
         <v>174.9</v>
       </c>
-      <c r="R6" s="65">
+      <c r="Q6" s="52">
+        <v>176.5</v>
+      </c>
+      <c r="R6" s="52">
         <v>114.5</v>
       </c>
-      <c r="S6" s="65">
+      <c r="S6" s="52">
         <v>68.3</v>
       </c>
-      <c r="T6" s="65">
+      <c r="T6" s="52">
         <v>126.6</v>
       </c>
     </row>
-    <row r="7" spans="2:38" s="65" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="72" t="s">
+    <row r="7" spans="2:38" s="52" customFormat="1">
+      <c r="B7" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="O7" s="65">
+      <c r="M7" s="52">
+        <v>212.9</v>
+      </c>
+      <c r="O7" s="52">
         <v>250.6</v>
       </c>
-      <c r="P7" s="65">
+      <c r="P7" s="52">
         <v>298</v>
       </c>
-      <c r="R7" s="65">
+      <c r="Q7" s="52">
+        <v>276.2</v>
+      </c>
+      <c r="R7" s="52">
         <v>307.39999999999998</v>
       </c>
-      <c r="S7" s="65">
+      <c r="S7" s="52">
         <v>271.2</v>
       </c>
-      <c r="T7" s="65">
+      <c r="T7" s="52">
         <v>320.10000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:38" s="65" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="72" t="s">
+    <row r="8" spans="2:38" s="52" customFormat="1">
+      <c r="B8" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="O8" s="65">
+      <c r="M8" s="52">
+        <v>1.6</v>
+      </c>
+      <c r="O8" s="52">
         <v>3.9</v>
       </c>
-      <c r="P8" s="65">
+      <c r="P8" s="52">
         <v>2.9</v>
       </c>
-      <c r="R8" s="65">
+      <c r="Q8" s="52">
+        <v>7</v>
+      </c>
+      <c r="R8" s="52">
         <v>10.3</v>
       </c>
-      <c r="S8" s="65">
+      <c r="S8" s="52">
         <v>2.2999999999999998</v>
       </c>
-      <c r="T8" s="65">
+      <c r="T8" s="52">
         <v>5.6</v>
       </c>
     </row>
-    <row r="9" spans="2:38" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:38" s="26" customFormat="1">
       <c r="B9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="73"/>
+      <c r="C9" s="56"/>
+      <c r="M9" s="26">
+        <v>758.7</v>
+      </c>
       <c r="O9" s="26">
         <v>807.3</v>
       </c>
       <c r="P9" s="26">
         <v>1130.5</v>
       </c>
+      <c r="Q9" s="26">
+        <v>958.1</v>
+      </c>
       <c r="R9" s="26">
         <v>1301.3</v>
       </c>
@@ -2677,16 +2745,22 @@
         <v>1018.9</v>
       </c>
     </row>
-    <row r="10" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:38">
       <c r="B10" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="M10" s="27">
+        <v>703.9</v>
+      </c>
       <c r="O10" s="3">
         <v>730.9</v>
       </c>
       <c r="P10" s="27">
         <v>924.8</v>
       </c>
+      <c r="Q10" s="3">
+        <v>776.4</v>
+      </c>
       <c r="R10" s="3">
         <v>1105.5</v>
       </c>
@@ -2697,41 +2771,55 @@
         <v>785.6</v>
       </c>
     </row>
-    <row r="11" spans="2:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:38" s="2" customFormat="1">
       <c r="B11" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="M11" s="26">
+        <f>M9-M10</f>
+        <v>54.800000000000068</v>
+      </c>
       <c r="O11" s="26">
-        <f>O9-O10</f>
+        <f t="shared" ref="O11:T11" si="0">O9-O10</f>
         <v>76.399999999999977</v>
       </c>
       <c r="P11" s="26">
-        <f>P9-P10</f>
+        <f t="shared" si="0"/>
         <v>205.70000000000005</v>
       </c>
+      <c r="Q11" s="26">
+        <f t="shared" si="0"/>
+        <v>181.70000000000005</v>
+      </c>
       <c r="R11" s="26">
-        <f>R9-R10</f>
+        <f t="shared" si="0"/>
         <v>195.79999999999995</v>
       </c>
       <c r="S11" s="26">
-        <f>S9-S10</f>
+        <f t="shared" si="0"/>
         <v>120.69999999999999</v>
       </c>
       <c r="T11" s="26">
-        <f>T9-T10</f>
+        <f t="shared" si="0"/>
         <v>233.29999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:38">
       <c r="B12" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="M12" s="27">
+        <v>35</v>
+      </c>
       <c r="O12" s="3">
         <v>34.4</v>
       </c>
       <c r="P12" s="27">
         <v>40.799999999999997</v>
       </c>
+      <c r="Q12" s="3">
+        <v>35.700000000000003</v>
+      </c>
       <c r="R12" s="3">
         <v>42.3</v>
       </c>
@@ -2742,16 +2830,22 @@
         <v>43.9</v>
       </c>
     </row>
-    <row r="13" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:38">
       <c r="B13" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="M13" s="27">
+        <v>45.4</v>
+      </c>
       <c r="O13" s="3">
         <v>45.8</v>
       </c>
       <c r="P13" s="27">
         <v>50.2</v>
       </c>
+      <c r="Q13" s="3">
+        <v>59.7</v>
+      </c>
       <c r="R13" s="3">
         <v>70.7</v>
       </c>
@@ -2762,16 +2856,22 @@
         <v>67.400000000000006</v>
       </c>
     </row>
-    <row r="14" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:38">
       <c r="B14" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="M14" s="27">
+        <v>14</v>
+      </c>
       <c r="O14" s="3">
         <v>0.1</v>
       </c>
       <c r="P14" s="27">
         <v>-2.2999999999999998</v>
       </c>
+      <c r="Q14" s="3">
+        <v>-1.8</v>
+      </c>
       <c r="R14" s="3">
         <v>-9</v>
       </c>
@@ -2782,36 +2882,48 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="15" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:38">
       <c r="B15" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="M15" s="27">
+        <v>7.1</v>
+      </c>
       <c r="O15" s="3">
         <v>8.4</v>
       </c>
       <c r="P15" s="27">
         <v>9.3000000000000007</v>
       </c>
-      <c r="R15" s="3">
+      <c r="Q15" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="R15" s="59">
         <v>15</v>
       </c>
-      <c r="S15" s="3">
+      <c r="S15" s="59">
         <v>17.399999999999999</v>
       </c>
       <c r="T15" s="27">
         <v>24.9</v>
       </c>
     </row>
-    <row r="16" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:38">
       <c r="B16" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="M16" s="27">
+        <v>9.1</v>
+      </c>
       <c r="O16" s="3">
         <v>-21.8</v>
       </c>
       <c r="P16" s="27">
         <v>35.5</v>
       </c>
+      <c r="Q16" s="3">
+        <v>-49.1</v>
+      </c>
       <c r="R16" s="3">
         <v>-14.4</v>
       </c>
@@ -2822,16 +2934,22 @@
         <v>-13.5</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:20">
       <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="M17" s="27">
+        <v>-0.1</v>
+      </c>
       <c r="O17" s="3">
         <v>1</v>
       </c>
       <c r="P17" s="27">
         <v>0.6</v>
       </c>
+      <c r="Q17" s="3">
+        <v>1.3</v>
+      </c>
       <c r="R17" s="3">
         <v>-1.8</v>
       </c>
@@ -2842,41 +2960,55 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:20" s="2" customFormat="1">
       <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="M18" s="26">
+        <f>M11-M12-M13-M14-M15+M16+M17</f>
+        <v>-37.699999999999932</v>
+      </c>
       <c r="O18" s="26">
-        <f>O11-O12-O13-O14-O15+O16+O17</f>
+        <f t="shared" ref="O18:T18" si="1">O11-O12-O13-O14-O15+O16+O17</f>
         <v>-33.100000000000023</v>
       </c>
       <c r="P18" s="26">
-        <f>P11-P12-P13-P14-P15+P16+P17</f>
+        <f t="shared" si="1"/>
         <v>143.80000000000004</v>
       </c>
+      <c r="Q18" s="26">
+        <f t="shared" si="1"/>
+        <v>30.000000000000053</v>
+      </c>
       <c r="R18" s="26">
-        <f>R11-R12-R13-R14-R15+R16+R17</f>
+        <f t="shared" si="1"/>
         <v>60.599999999999945</v>
       </c>
       <c r="S18" s="26">
-        <f>S11-S12-S13-S14-S15+S16+S17</f>
+        <f t="shared" si="1"/>
         <v>-36.300000000000011</v>
       </c>
       <c r="T18" s="26">
-        <f>T11-T12-T13-T14-T15+T16+T17</f>
+        <f t="shared" si="1"/>
         <v>66.69999999999996</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:20">
       <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="M19" s="27">
+        <v>-94.6</v>
+      </c>
       <c r="O19" s="3">
         <v>-75.400000000000006</v>
       </c>
       <c r="P19" s="27">
         <v>-65.5</v>
       </c>
+      <c r="Q19" s="3">
+        <v>-51.7</v>
+      </c>
       <c r="R19" s="3">
         <v>-6.8</v>
       </c>
@@ -2887,16 +3019,22 @@
         <v>-38</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:20">
       <c r="B20" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="M20" s="27">
+        <v>-16.3</v>
+      </c>
       <c r="O20" s="3">
         <v>19.600000000000001</v>
       </c>
       <c r="P20" s="27">
         <v>5.3</v>
       </c>
+      <c r="Q20" s="3">
+        <v>-3.3</v>
+      </c>
       <c r="R20" s="3">
         <v>3.9</v>
       </c>
@@ -2907,41 +3045,55 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:20">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="M21" s="27">
+        <f>M18+M19+M20</f>
+        <v>-148.59999999999994</v>
+      </c>
       <c r="O21" s="27">
-        <f>O18+O19+O20</f>
+        <f t="shared" ref="O21:T21" si="2">O18+O19+O20</f>
         <v>-88.900000000000034</v>
       </c>
       <c r="P21" s="27">
-        <f>P18+P19+P20</f>
+        <f t="shared" si="2"/>
         <v>83.600000000000037</v>
       </c>
+      <c r="Q21" s="27">
+        <f t="shared" si="2"/>
+        <v>-24.99999999999995</v>
+      </c>
       <c r="R21" s="27">
-        <f>R18+R19+R20</f>
+        <f t="shared" si="2"/>
         <v>57.699999999999946</v>
       </c>
       <c r="S21" s="27">
-        <f>S18+S19+S20</f>
+        <f t="shared" si="2"/>
         <v>-81</v>
       </c>
       <c r="T21" s="27">
-        <f>T18+T19+T20</f>
+        <f t="shared" si="2"/>
         <v>49.499999999999957</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:20">
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="M22" s="27">
+        <v>-29.1</v>
+      </c>
       <c r="O22" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="P22" s="27">
         <v>-5.6</v>
       </c>
+      <c r="Q22" s="3">
+        <v>20.7</v>
+      </c>
       <c r="R22" s="3">
         <v>54.7</v>
       </c>
@@ -2952,41 +3104,55 @@
         <v>-24.6</v>
       </c>
     </row>
-    <row r="23" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:20" s="2" customFormat="1">
       <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="M23" s="26">
+        <f>M21-M22</f>
+        <v>-119.49999999999994</v>
+      </c>
       <c r="O23" s="26">
-        <f>O21-O22</f>
+        <f t="shared" ref="O23:T23" si="3">O21-O22</f>
         <v>-90.000000000000028</v>
       </c>
       <c r="P23" s="26">
-        <f>P21-P22</f>
+        <f t="shared" si="3"/>
         <v>89.200000000000031</v>
       </c>
+      <c r="Q23" s="26">
+        <f t="shared" si="3"/>
+        <v>-45.699999999999946</v>
+      </c>
       <c r="R23" s="26">
-        <f>R21-R22</f>
+        <f t="shared" si="3"/>
         <v>2.9999999999999432</v>
       </c>
       <c r="S23" s="26">
-        <f>S21-S22</f>
+        <f t="shared" si="3"/>
         <v>-30.700000000000003</v>
       </c>
       <c r="T23" s="26">
-        <f>T21-T22</f>
+        <f t="shared" si="3"/>
         <v>74.099999999999966</v>
       </c>
     </row>
-    <row r="24" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:20" s="2" customFormat="1">
       <c r="B24" s="29" t="s">
         <v>72</v>
       </c>
+      <c r="M24" s="26">
+        <v>-121.2</v>
+      </c>
       <c r="O24" s="2">
         <v>-89.7</v>
       </c>
       <c r="P24" s="26">
         <v>87.9</v>
       </c>
+      <c r="Q24" s="2">
+        <v>-45</v>
+      </c>
       <c r="R24" s="2">
         <v>2.1</v>
       </c>
@@ -2997,16 +3163,22 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:20">
       <c r="B25" s="30" t="s">
         <v>73</v>
       </c>
+      <c r="M25" s="27">
+        <v>1.7</v>
+      </c>
       <c r="O25" s="3">
         <v>-0.3</v>
       </c>
       <c r="P25" s="27">
         <v>1.3</v>
       </c>
+      <c r="Q25" s="3">
+        <v>-0.7</v>
+      </c>
       <c r="R25" s="3">
         <v>0.9</v>
       </c>
@@ -3017,41 +3189,55 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:20">
       <c r="B26" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="M26" s="28">
+        <f>M24/M27</f>
+        <v>-0.16462917685411571</v>
+      </c>
       <c r="O26" s="28">
-        <f>O24/O27</f>
+        <f t="shared" ref="O26:T26" si="4">O24/O27</f>
         <v>-0.12204081632653062</v>
       </c>
       <c r="P26" s="28">
-        <f>P24/P27</f>
+        <f t="shared" si="4"/>
         <v>0.11962438758845946</v>
       </c>
+      <c r="Q26" s="28">
+        <f t="shared" si="4"/>
+        <v>-6.1241154055525319E-2</v>
+      </c>
       <c r="R26" s="28">
-        <f>R24/R27</f>
+        <f t="shared" si="4"/>
         <v>2.8583095140873828E-3</v>
       </c>
       <c r="S26" s="28">
-        <f>S24/S27</f>
+        <f t="shared" si="4"/>
         <v>-4.3152736182956709E-2</v>
       </c>
       <c r="T26" s="28">
-        <f>T24/T27</f>
+        <f t="shared" si="4"/>
         <v>0.10100735093928669</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:20">
       <c r="B27" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="M27" s="3">
+        <v>736.2</v>
+      </c>
       <c r="O27" s="27">
         <v>735</v>
       </c>
       <c r="P27" s="27">
         <v>734.8</v>
       </c>
+      <c r="Q27" s="3">
+        <v>734.8</v>
+      </c>
       <c r="R27" s="3">
         <v>734.7</v>
       </c>
@@ -3062,10 +3248,15 @@
         <v>734.6</v>
       </c>
     </row>
-    <row r="30" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:20" s="2" customFormat="1">
       <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="Q30" s="34">
+        <f>Q9/M9-1</f>
+        <v>0.26281797812046914</v>
+      </c>
+      <c r="R30" s="34"/>
       <c r="S30" s="34">
         <f>S9/O9-1</f>
         <v>-0.25566703827573389</v>
@@ -3075,7 +3266,7 @@
         <v>-9.8717381689517936E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:20" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:20" s="25" customFormat="1">
       <c r="B31" s="25" t="s">
         <v>67</v>
       </c>
@@ -3083,6 +3274,14 @@
         <f>P9/O9-1</f>
         <v>0.40034683512944391</v>
       </c>
+      <c r="Q31" s="25">
+        <f t="shared" ref="Q31:R31" si="5">Q9/P9-1</f>
+        <v>-0.15249889429455987</v>
+      </c>
+      <c r="R31" s="25">
+        <f t="shared" si="5"/>
+        <v>0.35820895522388052</v>
+      </c>
       <c r="S31" s="25">
         <f>S9/R9-1</f>
         <v>-0.53823099976946132</v>
@@ -3092,9 +3291,13 @@
         <v>0.69562323181893837</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:20">
       <c r="B34" s="3" t="s">
         <v>68</v>
+      </c>
+      <c r="M34" s="25">
+        <f>M11/M9</f>
+        <v>7.2228812442335658E-2</v>
       </c>
       <c r="O34" s="25">
         <f>O11/O9</f>
@@ -3104,12 +3307,16 @@
         <f>P11/P9</f>
         <v>0.18195488721804515</v>
       </c>
+      <c r="Q34" s="25">
+        <f t="shared" ref="Q34:R34" si="6">Q11/Q9</f>
+        <v>0.18964617472080164</v>
+      </c>
       <c r="R34" s="25">
-        <f t="shared" ref="R34" si="0">R11/R9</f>
+        <f t="shared" si="6"/>
         <v>0.1504649196956889</v>
       </c>
       <c r="S34" s="25">
-        <f t="shared" ref="S34:T34" si="1">S11/S9</f>
+        <f t="shared" ref="S34" si="7">S11/S9</f>
         <v>0.20086536861374604</v>
       </c>
       <c r="T34" s="25">
@@ -3117,9 +3324,13 @@
         <v>0.2289724212385906</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:20">
       <c r="B35" s="3" t="s">
         <v>69</v>
+      </c>
+      <c r="M35" s="25">
+        <f>M18/M9</f>
+        <v>-4.9690259654672372E-2</v>
       </c>
       <c r="O35" s="25">
         <f>O18/O9</f>
@@ -3129,12 +3340,16 @@
         <f>P18/P9</f>
         <v>0.12720035382574085</v>
       </c>
+      <c r="Q35" s="25">
+        <f t="shared" ref="Q35:R35" si="8">Q18/Q9</f>
+        <v>3.1311971610479127E-2</v>
+      </c>
       <c r="R35" s="25">
-        <f t="shared" ref="R35" si="2">R18/R9</f>
+        <f t="shared" si="8"/>
         <v>4.6568815799584988E-2</v>
       </c>
       <c r="S35" s="25">
-        <f t="shared" ref="S35:T35" si="3">S18/S9</f>
+        <f t="shared" ref="S35" si="9">S18/S9</f>
         <v>-6.0409385921118344E-2</v>
       </c>
       <c r="T35" s="25">
@@ -3142,9 +3357,13 @@
         <v>6.5462753950338556E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:20">
       <c r="B36" s="3" t="s">
         <v>70</v>
+      </c>
+      <c r="M36" s="25">
+        <f>M23/M9</f>
+        <v>-0.15750626070910759</v>
       </c>
       <c r="O36" s="25">
         <f>O23/O9</f>
@@ -3154,12 +3373,16 @@
         <f>P23/P9</f>
         <v>7.8903140203449823E-2</v>
       </c>
+      <c r="Q36" s="25">
+        <f t="shared" ref="Q36:R36" si="10">Q23/Q9</f>
+        <v>-4.7698570086629734E-2</v>
+      </c>
       <c r="R36" s="25">
-        <f t="shared" ref="R36" si="4">R23/R9</f>
+        <f t="shared" si="10"/>
         <v>2.3053869207714925E-3</v>
       </c>
       <c r="S36" s="25">
-        <f t="shared" ref="S36:T36" si="5">S23/S9</f>
+        <f t="shared" ref="S36" si="11">S23/S9</f>
         <v>-5.1090031619237815E-2</v>
       </c>
       <c r="T36" s="25">
@@ -3167,9 +3390,13 @@
         <v>7.2725488271665487E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:20">
       <c r="B37" s="3" t="s">
         <v>71</v>
+      </c>
+      <c r="M37" s="25">
+        <f>M22/M21</f>
+        <v>0.19582772543741597</v>
       </c>
       <c r="O37" s="25">
         <f>O22/O21</f>
@@ -3179,12 +3406,16 @@
         <f>P22/P21</f>
         <v>-6.6985645933014315E-2</v>
       </c>
+      <c r="Q37" s="25">
+        <f t="shared" ref="Q37:R37" si="12">Q22/Q21</f>
+        <v>-0.82800000000000162</v>
+      </c>
       <c r="R37" s="25">
-        <f t="shared" ref="R37" si="6">R22/R21</f>
+        <f t="shared" si="12"/>
         <v>0.94800693240901301</v>
       </c>
       <c r="S37" s="25">
-        <f t="shared" ref="S37:T37" si="7">S22/S21</f>
+        <f t="shared" ref="S37" si="13">S22/S21</f>
         <v>0.62098765432098757</v>
       </c>
       <c r="T37" s="25">
@@ -3192,52 +3423,63 @@
         <v>-0.49696969696969745</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:20">
       <c r="B40" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:20" s="2" customFormat="1">
       <c r="B41" s="29" t="s">
         <v>83</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" ref="P41:S41" si="8">P42+P46</f>
+        <f t="shared" ref="P41:S41" si="14">P42+P47</f>
         <v>34</v>
       </c>
+      <c r="Q41" s="2">
+        <f t="shared" si="14"/>
+        <v>30</v>
+      </c>
       <c r="S41" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="T41" s="2">
-        <f>T42+T46</f>
+        <f>T42+T47</f>
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="2:20" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="62" t="s">
+    <row r="42" spans="2:20" s="40" customFormat="1">
+      <c r="B42" s="49" t="s">
         <v>84</v>
       </c>
       <c r="P42" s="40">
-        <f>P43+P44</f>
+        <f>P43+P44+P45</f>
         <v>14</v>
       </c>
+      <c r="Q42" s="40">
+        <f>Q43+Q44+Q45</f>
+        <v>9</v>
+      </c>
       <c r="S42" s="40">
-        <f>S43+S44</f>
+        <f t="shared" ref="S42:T42" si="15">S43+S44+S45</f>
         <v>6</v>
       </c>
       <c r="T42" s="40">
-        <f>T43+T44</f>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="2:20" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="61" t="s">
+    <row r="43" spans="2:20" s="39" customFormat="1">
+      <c r="B43" s="48" t="s">
         <v>85</v>
       </c>
       <c r="P43" s="39">
         <v>7</v>
       </c>
+      <c r="Q43" s="39">
+        <v>6</v>
+      </c>
       <c r="S43" s="39">
         <v>4</v>
       </c>
@@ -3245,917 +3487,1017 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="2:20" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="61" t="s">
+    <row r="44" spans="2:20" s="39" customFormat="1">
+      <c r="B44" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="P44" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="39">
+        <v>0</v>
+      </c>
+      <c r="S44" s="39">
+        <v>0</v>
+      </c>
+      <c r="T44" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" s="39" customFormat="1">
+      <c r="B45" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="P44" s="39">
+      <c r="P45" s="39">
         <v>7</v>
       </c>
-      <c r="S44" s="39">
+      <c r="Q45" s="39">
+        <v>3</v>
+      </c>
+      <c r="S45" s="39">
         <v>2</v>
       </c>
-      <c r="T44" s="39">
+      <c r="T45" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:20" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="61"/>
-    </row>
-    <row r="46" spans="2:20" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="62" t="s">
+    <row r="46" spans="2:20" s="39" customFormat="1">
+      <c r="B46" s="48"/>
+    </row>
+    <row r="47" spans="2:20" s="40" customFormat="1">
+      <c r="B47" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P46" s="40">
-        <f>P47+P48</f>
+      <c r="P47" s="40">
+        <f>P48+P49+P50</f>
         <v>20</v>
       </c>
-      <c r="S46" s="40">
-        <f>S47+S48</f>
+      <c r="Q47" s="40">
+        <f>Q48+Q49+Q50</f>
+        <v>21</v>
+      </c>
+      <c r="S47" s="40">
+        <f>S48+S49+S50</f>
         <v>20</v>
       </c>
-      <c r="T46" s="40">
-        <f>T47+T48</f>
+      <c r="T47" s="40">
+        <f>T48+T49+T50</f>
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="2:20" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="61" t="s">
+    <row r="48" spans="2:20" s="39" customFormat="1">
+      <c r="B48" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="P47" s="39">
+      <c r="P48" s="39">
         <v>12</v>
       </c>
-      <c r="S47" s="39">
+      <c r="Q48" s="39">
+        <v>14</v>
+      </c>
+      <c r="S48" s="39">
         <v>12</v>
       </c>
-      <c r="T47" s="39">
+      <c r="T48" s="39">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="2:20" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="61" t="s">
+    <row r="49" spans="2:20" s="39" customFormat="1">
+      <c r="B49" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="P48" s="39">
+      <c r="P49" s="39">
         <v>8</v>
       </c>
-      <c r="S48" s="39">
+      <c r="Q49" s="39">
+        <v>0</v>
+      </c>
+      <c r="S49" s="39">
         <v>8</v>
       </c>
-      <c r="T48" s="39">
+      <c r="T49" s="39">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B51" s="33" t="s">
+    <row r="50" spans="2:20" s="39" customFormat="1">
+      <c r="B50" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="P50" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="39">
+        <v>7</v>
+      </c>
+      <c r="S50" s="39">
+        <v>0</v>
+      </c>
+      <c r="T50" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20">
+      <c r="B52" s="33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="2" t="s">
+    <row r="53" spans="2:20" s="2" customFormat="1">
+      <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P52" s="26"/>
-      <c r="Q52" s="26"/>
-      <c r="R52" s="26"/>
-      <c r="S52" s="26">
-        <v>1129.8</v>
-      </c>
-      <c r="T52" s="26">
-        <v>1041.3</v>
-      </c>
-    </row>
-    <row r="53" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="P53" s="26"/>
-      <c r="Q53" s="26"/>
       <c r="R53" s="26"/>
       <c r="S53" s="26">
+        <v>1129.8</v>
+      </c>
+      <c r="T53" s="26">
+        <v>1041.3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" s="2" customFormat="1">
+      <c r="B54" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P54" s="26"/>
+      <c r="R54" s="26"/>
+      <c r="S54" s="26">
         <v>802.9</v>
       </c>
-      <c r="T53" s="26">
+      <c r="T54" s="26">
         <v>753.8</v>
       </c>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B54" s="3" t="s">
+    <row r="55" spans="2:20">
+      <c r="B55" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="P54" s="27"/>
-      <c r="Q54" s="27"/>
-      <c r="R54" s="27"/>
-      <c r="S54" s="27">
-        <v>197</v>
-      </c>
-      <c r="T54" s="27">
-        <v>240.4</v>
-      </c>
-    </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B55" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="P55" s="27"/>
-      <c r="Q55" s="27"/>
       <c r="R55" s="27"/>
       <c r="S55" s="27">
-        <v>9.6999999999999993</v>
+        <v>197</v>
       </c>
       <c r="T55" s="27">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.2">
+        <v>240.4</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20">
       <c r="B56" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
       <c r="R56" s="27"/>
       <c r="S56" s="27">
-        <v>9.8000000000000007</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="T56" s="27">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20">
       <c r="B57" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P57" s="27"/>
-      <c r="Q57" s="27"/>
       <c r="R57" s="27"/>
       <c r="S57" s="27">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="T57" s="27">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20">
+      <c r="B58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="P58" s="27"/>
+      <c r="R58" s="27"/>
+      <c r="S58" s="27">
         <v>615.5</v>
       </c>
-      <c r="T57" s="27">
+      <c r="T58" s="27">
         <v>620</v>
       </c>
     </row>
-    <row r="58" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="2" t="s">
+    <row r="59" spans="2:20" s="2" customFormat="1">
+      <c r="B59" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="P58" s="26"/>
-      <c r="Q58" s="26"/>
-      <c r="R58" s="26"/>
-      <c r="S58" s="26">
+      <c r="P59" s="26"/>
+      <c r="Q59" s="26"/>
+      <c r="R59" s="26"/>
+      <c r="S59" s="26">
         <v>2222.8000000000002</v>
       </c>
-      <c r="T58" s="26">
+      <c r="T59" s="26">
         <v>2392.9</v>
       </c>
     </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B59" s="3" t="s">
+    <row r="60" spans="2:20">
+      <c r="B60" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="P59" s="27"/>
-      <c r="Q59" s="27"/>
-      <c r="R59" s="27"/>
-      <c r="S59" s="27">
-        <v>105</v>
-      </c>
-      <c r="T59" s="27">
-        <v>101.9</v>
-      </c>
-    </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B60" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="P60" s="27"/>
       <c r="Q60" s="27"/>
       <c r="R60" s="27"/>
       <c r="S60" s="27">
-        <v>217</v>
+        <v>105</v>
       </c>
       <c r="T60" s="27">
-        <v>209.3</v>
-      </c>
-    </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.2">
+        <v>101.9</v>
+      </c>
+    </row>
+    <row r="61" spans="2:20">
       <c r="B61" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P61" s="27"/>
       <c r="Q61" s="27"/>
       <c r="R61" s="27"/>
       <c r="S61" s="27">
-        <v>227.1</v>
+        <v>217</v>
       </c>
       <c r="T61" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.2">
+        <v>209.3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:20">
       <c r="B62" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="P62" s="27">
-        <f>SUM(P52:P61)</f>
-        <v>0</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="P62" s="27"/>
       <c r="Q62" s="27"/>
       <c r="R62" s="27"/>
       <c r="S62" s="27">
-        <f>SUM(S52:S61)</f>
+        <v>227.1</v>
+      </c>
+      <c r="T62" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:20">
+      <c r="B63" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P63" s="27"/>
+      <c r="Q63" s="27"/>
+      <c r="R63" s="27"/>
+      <c r="S63" s="27">
+        <f>SUM(S53:S62)</f>
         <v>5536.6</v>
       </c>
-      <c r="T62" s="27">
-        <f>SUM(T52:T61)</f>
+      <c r="T63" s="27">
+        <f>SUM(T53:T62)</f>
         <v>5367.9000000000005</v>
       </c>
     </row>
-    <row r="63" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
+    <row r="64" spans="2:20" s="2" customFormat="1">
+      <c r="B64" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="P63" s="26"/>
-      <c r="Q63" s="26"/>
-      <c r="R63" s="26"/>
-      <c r="S63" s="26">
-        <v>169.9</v>
-      </c>
-      <c r="T63" s="26">
-        <v>169.9</v>
-      </c>
-    </row>
-    <row r="64" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="P64" s="26"/>
       <c r="Q64" s="26"/>
       <c r="R64" s="26"/>
       <c r="S64" s="26">
+        <v>169.9</v>
+      </c>
+      <c r="T64" s="26">
+        <v>169.9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:20" s="2" customFormat="1">
+      <c r="B65" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="P65" s="26"/>
+      <c r="Q65" s="26"/>
+      <c r="R65" s="26"/>
+      <c r="S65" s="26">
         <v>1.6</v>
       </c>
-      <c r="T64" s="26">
+      <c r="T65" s="26">
         <v>1.5</v>
       </c>
     </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B65" s="3" t="s">
+    <row r="66" spans="2:20">
+      <c r="B66" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="P65" s="27"/>
-      <c r="Q65" s="27"/>
-      <c r="R65" s="27"/>
-      <c r="S65" s="27">
-        <v>1.6</v>
-      </c>
-      <c r="T65" s="27">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B66" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="P66" s="27"/>
       <c r="Q66" s="27"/>
       <c r="R66" s="27"/>
       <c r="S66" s="27">
-        <v>23.4</v>
+        <v>1.6</v>
       </c>
       <c r="T66" s="27">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:20">
       <c r="B67" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="P67" s="27"/>
       <c r="Q67" s="27"/>
       <c r="R67" s="27"/>
       <c r="S67" s="27">
-        <v>0</v>
+        <v>23.4</v>
       </c>
       <c r="T67" s="27">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.2">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="68" spans="2:20">
       <c r="B68" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="P68" s="27"/>
       <c r="Q68" s="27"/>
       <c r="R68" s="27"/>
       <c r="S68" s="27">
-        <v>22.8</v>
+        <v>0</v>
       </c>
       <c r="T68" s="27">
-        <v>23.3</v>
-      </c>
-    </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="69" spans="2:20">
       <c r="B69" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="P69" s="27"/>
+        <v>99</v>
+      </c>
       <c r="Q69" s="27"/>
       <c r="R69" s="27"/>
       <c r="S69" s="27">
-        <v>142.9</v>
+        <v>22.8</v>
       </c>
       <c r="T69" s="27">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.2">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:20">
       <c r="B70" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P70" s="27"/>
       <c r="Q70" s="27"/>
       <c r="R70" s="27"/>
       <c r="S70" s="27">
-        <v>6.9</v>
+        <v>142.9</v>
       </c>
       <c r="T70" s="27">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="2:20">
       <c r="B71" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P71" s="27"/>
       <c r="Q71" s="27"/>
       <c r="R71" s="27"/>
       <c r="S71" s="27">
-        <v>1679.3</v>
+        <v>6.9</v>
       </c>
       <c r="T71" s="27">
-        <v>1652.5</v>
-      </c>
-    </row>
-    <row r="72" spans="2:20" x14ac:dyDescent="0.2">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="72" spans="2:20">
       <c r="B72" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P72" s="27"/>
       <c r="Q72" s="27"/>
       <c r="R72" s="27"/>
       <c r="S72" s="27">
-        <v>2227.5</v>
+        <v>1679.3</v>
       </c>
       <c r="T72" s="27">
-        <v>2231.3000000000002</v>
-      </c>
-    </row>
-    <row r="73" spans="2:20" x14ac:dyDescent="0.2">
+        <v>1652.5</v>
+      </c>
+    </row>
+    <row r="73" spans="2:20">
       <c r="B73" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P73" s="27"/>
       <c r="Q73" s="27"/>
       <c r="R73" s="27"/>
       <c r="S73" s="27">
-        <v>55.9</v>
+        <v>2227.5</v>
       </c>
       <c r="T73" s="27">
-        <v>59.5</v>
-      </c>
-    </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.2">
+        <v>2231.3000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="2:20">
       <c r="B74" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="P74" s="27">
-        <f>SUM(P63:P73)+P62</f>
-        <v>0</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="P74" s="27"/>
       <c r="Q74" s="27"/>
       <c r="R74" s="27"/>
       <c r="S74" s="27">
-        <f>SUM(S63:S73)+S62</f>
-        <v>9868.4</v>
+        <v>55.9</v>
       </c>
       <c r="T74" s="27">
-        <f>SUM(T63:T73)+T62</f>
-        <v>9698.7999999999993</v>
-      </c>
-    </row>
-    <row r="75" spans="2:20" x14ac:dyDescent="0.2">
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="75" spans="2:20">
+      <c r="B75" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="P75" s="27"/>
       <c r="Q75" s="27"/>
       <c r="R75" s="27"/>
-      <c r="S75" s="27"/>
-      <c r="T75" s="27"/>
-    </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B76" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="S75" s="27">
+        <f>SUM(S64:S74)+S63</f>
+        <v>9868.4</v>
+      </c>
+      <c r="T75" s="27">
+        <f>SUM(T64:T74)+T63</f>
+        <v>9698.7999999999993</v>
+      </c>
+    </row>
+    <row r="76" spans="2:20">
       <c r="P76" s="27"/>
       <c r="Q76" s="27"/>
       <c r="R76" s="27"/>
-      <c r="S76" s="27">
-        <v>562.70000000000005</v>
-      </c>
-      <c r="T76" s="27">
-        <v>727.4</v>
-      </c>
-    </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="S76" s="27"/>
+      <c r="T76" s="27"/>
+    </row>
+    <row r="77" spans="2:20">
       <c r="B77" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P77" s="27"/>
       <c r="Q77" s="27"/>
       <c r="R77" s="27"/>
       <c r="S77" s="27">
-        <v>14.1</v>
+        <v>562.70000000000005</v>
       </c>
       <c r="T77" s="27">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.2">
+        <v>727.4</v>
+      </c>
+    </row>
+    <row r="78" spans="2:20">
       <c r="B78" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P78" s="27"/>
       <c r="Q78" s="27"/>
       <c r="R78" s="27"/>
       <c r="S78" s="27">
+        <v>14.1</v>
+      </c>
+      <c r="T78" s="27">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="79" spans="2:20">
+      <c r="B79" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P79" s="27"/>
+      <c r="Q79" s="27"/>
+      <c r="R79" s="27"/>
+      <c r="S79" s="27">
         <v>11</v>
       </c>
-      <c r="T78" s="27">
+      <c r="T79" s="27">
         <v>11.3</v>
       </c>
     </row>
-    <row r="79" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="2" t="s">
+    <row r="80" spans="2:20" s="2" customFormat="1">
+      <c r="B80" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P79" s="26"/>
-      <c r="Q79" s="26"/>
-      <c r="R79" s="26"/>
-      <c r="S79" s="26">
+      <c r="P80" s="26"/>
+      <c r="Q80" s="26"/>
+      <c r="R80" s="26"/>
+      <c r="S80" s="26">
         <v>326.8</v>
       </c>
-      <c r="T79" s="26">
+      <c r="T80" s="26">
         <v>70.2</v>
       </c>
     </row>
-    <row r="80" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B80" s="3" t="s">
+    <row r="81" spans="2:20">
+      <c r="B81" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="P80" s="27"/>
-      <c r="Q80" s="27"/>
-      <c r="R80" s="27"/>
-      <c r="S80" s="27">
-        <v>263.3</v>
-      </c>
-      <c r="T80" s="27">
-        <v>258.8</v>
-      </c>
-    </row>
-    <row r="81" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B81" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="P81" s="27"/>
       <c r="Q81" s="27"/>
       <c r="R81" s="27"/>
       <c r="S81" s="27">
+        <v>263.3</v>
+      </c>
+      <c r="T81" s="27">
+        <v>258.8</v>
+      </c>
+    </row>
+    <row r="82" spans="2:20">
+      <c r="B82" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="P82" s="27"/>
+      <c r="Q82" s="27"/>
+      <c r="R82" s="27"/>
+      <c r="S82" s="27">
         <v>1301.8</v>
       </c>
-      <c r="T81" s="27">
+      <c r="T82" s="27">
         <v>1317.8</v>
       </c>
     </row>
-    <row r="82" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="2" t="s">
+    <row r="83" spans="2:20" s="2" customFormat="1">
+      <c r="B83" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P82" s="26"/>
-      <c r="Q82" s="26"/>
-      <c r="R82" s="26"/>
-      <c r="S82" s="26">
+      <c r="P83" s="26"/>
+      <c r="Q83" s="26"/>
+      <c r="R83" s="26"/>
+      <c r="S83" s="26">
         <v>3.2</v>
       </c>
-      <c r="T82" s="26">
+      <c r="T83" s="26">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B83" s="3" t="s">
+    <row r="84" spans="2:20">
+      <c r="B84" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="27"/>
-      <c r="R83" s="27"/>
-      <c r="S83" s="27">
-        <v>38</v>
-      </c>
-      <c r="T83" s="27">
-        <v>37.1</v>
-      </c>
-    </row>
-    <row r="84" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B84" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="P84" s="27"/>
       <c r="Q84" s="27"/>
       <c r="R84" s="27"/>
       <c r="S84" s="27">
-        <v>71.400000000000006</v>
+        <v>38</v>
       </c>
       <c r="T84" s="27">
-        <v>79.8</v>
-      </c>
-    </row>
-    <row r="85" spans="2:20" x14ac:dyDescent="0.2">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:20">
       <c r="B85" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P85" s="27"/>
       <c r="Q85" s="27"/>
       <c r="R85" s="27"/>
       <c r="S85" s="27">
-        <v>2.8</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="T85" s="27">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="86" spans="2:20" x14ac:dyDescent="0.2">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="86" spans="2:20">
       <c r="B86" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P86" s="27"/>
       <c r="Q86" s="27"/>
       <c r="R86" s="27"/>
       <c r="S86" s="27">
-        <v>113.8</v>
+        <v>2.8</v>
       </c>
       <c r="T86" s="27">
-        <v>111.8</v>
-      </c>
-    </row>
-    <row r="87" spans="2:20" x14ac:dyDescent="0.2">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="87" spans="2:20">
       <c r="B87" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P87" s="27"/>
       <c r="Q87" s="27"/>
       <c r="R87" s="27"/>
-      <c r="S87" s="3">
-        <v>47.4</v>
+      <c r="S87" s="27">
+        <v>113.8</v>
       </c>
       <c r="T87" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:20" x14ac:dyDescent="0.2">
+        <v>111.8</v>
+      </c>
+    </row>
+    <row r="88" spans="2:20">
       <c r="B88" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="P88" s="27">
-        <f>SUM(P76:P87)</f>
-        <v>0</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="P88" s="27"/>
       <c r="Q88" s="27"/>
       <c r="R88" s="27"/>
-      <c r="S88" s="27">
-        <f>SUM(S76:S87)</f>
-        <v>2756.3</v>
+      <c r="S88" s="3">
+        <v>47.4</v>
       </c>
       <c r="T88" s="27">
-        <f>SUM(T76:T87)</f>
-        <v>2640.1000000000004</v>
-      </c>
-    </row>
-    <row r="89" spans="2:20" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:20">
       <c r="B89" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="P89" s="27"/>
+        <v>115</v>
+      </c>
+      <c r="P89" s="27">
+        <f>SUM(P77:P88)</f>
+        <v>0</v>
+      </c>
       <c r="Q89" s="27"/>
       <c r="R89" s="27"/>
       <c r="S89" s="27">
+        <f>SUM(S77:S88)</f>
+        <v>2756.3</v>
+      </c>
+      <c r="T89" s="27">
+        <f>SUM(T77:T88)</f>
+        <v>2640.1000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="2:20">
+      <c r="B90" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P90" s="27"/>
+      <c r="Q90" s="27"/>
+      <c r="R90" s="27"/>
+      <c r="S90" s="27">
         <v>49</v>
       </c>
-      <c r="T89" s="27">
+      <c r="T90" s="27">
         <v>52.6</v>
       </c>
     </row>
-    <row r="90" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="2" t="s">
+    <row r="91" spans="2:20" s="2" customFormat="1">
+      <c r="B91" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P90" s="26"/>
-      <c r="Q90" s="26"/>
-      <c r="R90" s="26"/>
-      <c r="S90" s="26">
+      <c r="P91" s="26"/>
+      <c r="Q91" s="26"/>
+      <c r="R91" s="26"/>
+      <c r="S91" s="26">
         <v>3229</v>
       </c>
-      <c r="T90" s="26">
+      <c r="T91" s="26">
         <v>3092.7</v>
       </c>
     </row>
-    <row r="91" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B91" s="3" t="s">
+    <row r="92" spans="2:20">
+      <c r="B92" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="P91" s="27"/>
-      <c r="Q91" s="27"/>
-      <c r="R91" s="27"/>
-      <c r="S91" s="27">
-        <v>53.8</v>
-      </c>
-      <c r="T91" s="27">
-        <v>55.1</v>
-      </c>
-    </row>
-    <row r="92" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B92" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="P92" s="27"/>
       <c r="Q92" s="27"/>
       <c r="R92" s="27"/>
       <c r="S92" s="27">
-        <v>454.8</v>
+        <v>53.8</v>
       </c>
       <c r="T92" s="27">
-        <v>478.5</v>
-      </c>
-    </row>
-    <row r="93" spans="2:20" x14ac:dyDescent="0.2">
+        <v>55.1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:20">
       <c r="B93" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P93" s="27"/>
       <c r="Q93" s="27"/>
       <c r="R93" s="27"/>
       <c r="S93" s="27">
-        <v>13</v>
+        <v>454.8</v>
       </c>
       <c r="T93" s="27">
-        <v>12.1</v>
-      </c>
-    </row>
-    <row r="94" spans="2:20" x14ac:dyDescent="0.2">
+        <v>478.5</v>
+      </c>
+    </row>
+    <row r="94" spans="2:20">
       <c r="B94" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="P94" s="27"/>
       <c r="Q94" s="27"/>
       <c r="R94" s="27"/>
       <c r="S94" s="27">
-        <v>376.1</v>
+        <v>13</v>
       </c>
       <c r="T94" s="27">
-        <v>334.4</v>
-      </c>
-    </row>
-    <row r="95" spans="2:20" x14ac:dyDescent="0.2">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:20">
       <c r="B95" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P95" s="27"/>
       <c r="Q95" s="27"/>
       <c r="R95" s="27"/>
       <c r="S95" s="27">
-        <v>37.6</v>
+        <v>376.1</v>
       </c>
       <c r="T95" s="27">
-        <v>27.2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:20" x14ac:dyDescent="0.2">
+        <v>334.4</v>
+      </c>
+    </row>
+    <row r="96" spans="2:20">
       <c r="B96" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P96" s="27"/>
       <c r="Q96" s="27"/>
       <c r="R96" s="27"/>
       <c r="S96" s="27">
-        <v>141.9</v>
+        <v>37.6</v>
       </c>
       <c r="T96" s="27">
-        <v>133.4</v>
-      </c>
-    </row>
-    <row r="97" spans="2:20" x14ac:dyDescent="0.2">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:20">
       <c r="B97" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="P97" s="27">
-        <f>SUM(P89:P96)+P88</f>
-        <v>0</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="P97" s="27"/>
       <c r="Q97" s="27"/>
       <c r="R97" s="27"/>
       <c r="S97" s="27">
-        <f>SUM(S89:S96)+S88</f>
-        <v>7111.5000000000009</v>
+        <v>141.9</v>
       </c>
       <c r="T97" s="27">
-        <f>SUM(T89:T96)+T88</f>
-        <v>6826.0999999999995</v>
-      </c>
-    </row>
-    <row r="98" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="P98" s="27"/>
+        <v>133.4</v>
+      </c>
+    </row>
+    <row r="98" spans="2:20">
+      <c r="B98" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="P98" s="27">
+        <f>SUM(P90:P97)+P89</f>
+        <v>0</v>
+      </c>
       <c r="Q98" s="27"/>
       <c r="R98" s="27"/>
-      <c r="S98" s="27"/>
-      <c r="T98" s="27"/>
-    </row>
-    <row r="99" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B99" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="S98" s="27">
+        <f>SUM(S90:S97)+S89</f>
+        <v>7111.5000000000009</v>
+      </c>
+      <c r="T98" s="27">
+        <f>SUM(T90:T97)+T89</f>
+        <v>6826.0999999999995</v>
+      </c>
+    </row>
+    <row r="99" spans="2:20">
       <c r="P99" s="27"/>
       <c r="Q99" s="27"/>
       <c r="R99" s="27"/>
-      <c r="S99" s="27">
-        <v>2756.9</v>
-      </c>
-      <c r="T99" s="27">
-        <v>2872.7</v>
-      </c>
-    </row>
-    <row r="100" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="S99" s="27"/>
+      <c r="T99" s="27"/>
+    </row>
+    <row r="100" spans="2:20">
       <c r="B100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="P100" s="27">
-        <f>P99+P97</f>
-        <v>0</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="P100" s="27"/>
       <c r="Q100" s="27"/>
       <c r="R100" s="27"/>
       <c r="S100" s="27">
-        <f>S99+S97</f>
+        <v>2756.9</v>
+      </c>
+      <c r="T100" s="27">
+        <v>2872.7</v>
+      </c>
+    </row>
+    <row r="101" spans="2:20">
+      <c r="B101" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="P101" s="27">
+        <f>P100+P98</f>
+        <v>0</v>
+      </c>
+      <c r="Q101" s="27"/>
+      <c r="R101" s="27"/>
+      <c r="S101" s="27">
+        <f>S100+S98</f>
         <v>9868.4000000000015</v>
       </c>
-      <c r="T100" s="27">
-        <f>T99+T97</f>
+      <c r="T101" s="27">
+        <f>T100+T98</f>
         <v>9698.7999999999993</v>
       </c>
     </row>
-    <row r="102" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B102" s="3" t="s">
+    <row r="103" spans="2:20">
+      <c r="B103" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="P102" s="27">
-        <f>P74-P97</f>
+      <c r="P103" s="27">
+        <f>P75-P98</f>
         <v>0</v>
       </c>
-      <c r="Q102" s="27"/>
-      <c r="R102" s="27"/>
-      <c r="S102" s="27">
-        <f>S74-S97</f>
+      <c r="Q103" s="27"/>
+      <c r="R103" s="27"/>
+      <c r="S103" s="27">
+        <f>S75-S98</f>
         <v>2756.8999999999987</v>
       </c>
-      <c r="T102" s="27">
-        <f>T74-T97</f>
+      <c r="T103" s="27">
+        <f>T75-T98</f>
         <v>2872.7</v>
       </c>
     </row>
-    <row r="103" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B103" s="3" t="s">
+    <row r="104" spans="2:20">
+      <c r="B104" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="S103" s="3">
-        <f>S102/S27</f>
+      <c r="S104" s="3">
+        <f>S103/S27</f>
         <v>3.7529267628641421</v>
       </c>
-      <c r="T103" s="3">
-        <f>T102/T27</f>
+      <c r="T104" s="3">
+        <f>T103/T27</f>
         <v>3.9105635720119789</v>
       </c>
     </row>
-    <row r="105" spans="2:20" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="39" t="s">
+    <row r="106" spans="2:20" s="39" customFormat="1">
+      <c r="B106" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="S105" s="65">
-        <f>S52+S53+S63</f>
+      <c r="S106" s="52">
+        <f>S53+S54+S64</f>
         <v>2102.6</v>
       </c>
-      <c r="T105" s="65">
-        <f>T52+T53+T63</f>
+      <c r="T106" s="52">
+        <f>T53+T54+T64</f>
         <v>1965</v>
       </c>
     </row>
-    <row r="106" spans="2:20" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="39" t="s">
+    <row r="107" spans="2:20" s="39" customFormat="1">
+      <c r="B107" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="S106" s="65">
-        <f>S79+S82+S90</f>
+      <c r="S107" s="52">
+        <f>S80+S83+S91</f>
         <v>3559</v>
       </c>
-      <c r="T106" s="65">
-        <f>T79+T82+T90</f>
+      <c r="T107" s="52">
+        <f>T80+T83+T91</f>
         <v>3173.8999999999996</v>
       </c>
     </row>
-    <row r="107" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B107" s="3" t="s">
+    <row r="108" spans="2:20">
+      <c r="B108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S107" s="27">
-        <f>S105-S106</f>
+      <c r="S108" s="27">
+        <f>S106-S107</f>
         <v>-1456.4</v>
       </c>
-      <c r="T107" s="27">
-        <f>T105-T106</f>
+      <c r="T108" s="27">
+        <f>T106-T107</f>
         <v>-1208.8999999999996</v>
       </c>
     </row>
-    <row r="109" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="2" t="s">
+    <row r="110" spans="2:20" s="2" customFormat="1">
+      <c r="B110" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="110" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B110" s="3" t="s">
+    <row r="111" spans="2:20">
+      <c r="B111" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="T110" s="25">
-        <f>T58/S58-1</f>
+      <c r="T111" s="25">
+        <f>T59/S59-1</f>
         <v>7.6525103473096934E-2</v>
       </c>
     </row>
-    <row r="112" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B112" s="3" t="s">
+    <row r="113" spans="2:20">
+      <c r="B113" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B114" s="3" t="s">
+    <row r="115" spans="2:20">
+      <c r="B115" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="S114" s="3">
+      <c r="M115" s="3">
+        <v>4.41</v>
+      </c>
+      <c r="N115" s="3">
+        <v>6.81</v>
+      </c>
+      <c r="O115" s="3">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="P115" s="3">
+        <v>15.14</v>
+      </c>
+      <c r="Q115" s="27">
+        <v>17</v>
+      </c>
+      <c r="R115" s="3">
+        <v>13.9</v>
+      </c>
+      <c r="S115" s="3">
         <v>12.61</v>
       </c>
-      <c r="T114" s="3">
+      <c r="T115" s="3">
         <v>8.7799999999999994</v>
       </c>
     </row>
-    <row r="115" spans="2:20" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B115" s="27" t="s">
+    <row r="116" spans="2:20" s="27" customFormat="1">
+      <c r="B116" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="S115" s="27">
-        <f>S114*S27</f>
+      <c r="M116" s="27">
+        <f t="shared" ref="M116:R116" si="16">M115*M27</f>
+        <v>3246.6420000000003</v>
+      </c>
+      <c r="N116" s="27">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="O116" s="27">
+        <f t="shared" si="16"/>
+        <v>7320.6</v>
+      </c>
+      <c r="P116" s="27">
+        <f t="shared" si="16"/>
+        <v>11124.871999999999</v>
+      </c>
+      <c r="Q116" s="27">
+        <f t="shared" si="16"/>
+        <v>12491.599999999999</v>
+      </c>
+      <c r="R116" s="27">
+        <f t="shared" si="16"/>
+        <v>10212.330000000002</v>
+      </c>
+      <c r="S116" s="27">
+        <f>S115*S27</f>
         <v>9263.3060000000005</v>
       </c>
-      <c r="T115" s="27">
-        <f>T114*T27</f>
+      <c r="T116" s="27">
+        <f>T115*T27</f>
         <v>6449.7879999999996</v>
       </c>
     </row>
-    <row r="116" spans="2:20" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B116" s="27" t="s">
+    <row r="117" spans="2:20" s="27" customFormat="1">
+      <c r="B117" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="S116" s="27">
-        <f>S115-S107</f>
+      <c r="M117" s="27">
+        <f t="shared" ref="M117:R117" si="17">M116-M108</f>
+        <v>3246.6420000000003</v>
+      </c>
+      <c r="N117" s="27">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O117" s="27">
+        <f t="shared" si="17"/>
+        <v>7320.6</v>
+      </c>
+      <c r="P117" s="27">
+        <f t="shared" si="17"/>
+        <v>11124.871999999999</v>
+      </c>
+      <c r="Q117" s="27">
+        <f t="shared" si="17"/>
+        <v>12491.599999999999</v>
+      </c>
+      <c r="R117" s="27">
+        <f t="shared" si="17"/>
+        <v>10212.330000000002</v>
+      </c>
+      <c r="S117" s="27">
+        <f>S116-S108</f>
         <v>10719.706</v>
       </c>
-      <c r="T116" s="27">
-        <f>T115-T107</f>
+      <c r="T117" s="27">
+        <f>T116-T108</f>
         <v>7658.6879999999992</v>
       </c>
     </row>
-    <row r="118" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B118" s="3" t="s">
+    <row r="119" spans="2:20">
+      <c r="B119" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S118" s="74">
-        <f>-S114/S103</f>
+      <c r="S119" s="57">
+        <f>-S115/S104</f>
         <v>-3.3600442526025622</v>
       </c>
-      <c r="T118" s="74">
-        <f>-T114/T103</f>
+      <c r="T119" s="57">
+        <f>-T115/T104</f>
         <v>-2.2452006822849584</v>
       </c>
     </row>
-    <row r="119" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B119" s="3" t="s">
+    <row r="120" spans="2:20">
+      <c r="B120" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B120" s="3" t="s">
+    <row r="121" spans="2:20">
+      <c r="B121" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4163,29 +4505,38 @@
   <hyperlinks>
     <hyperlink ref="T1" r:id="rId1" xr:uid="{680599EF-35E5-444E-BE52-11E2AAE328C4}"/>
     <hyperlink ref="S1" r:id="rId2" xr:uid="{93CDF7DF-1EA6-42CA-BCC8-DA2865B51A26}"/>
+    <hyperlink ref="Q1" r:id="rId3" xr:uid="{9752E2CB-3CEF-4245-BFA9-C0218E68B8CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258CA0E5-563F-4C1F-B583-AD76D8E7BBD2}">
-  <dimension ref="D4"/>
+  <dimension ref="C4:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:4">
       <c r="D4" s="3" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FY20, FY21 & Q420 info to $ERJ model
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA67803A-2104-4C35-B8E7-B518DEF62D0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F149AB-BDA9-450C-911B-84BD9A776A2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="192">
   <si>
     <t>$ERJ</t>
   </si>
@@ -624,6 +624,27 @@
   </si>
   <si>
     <t>Large Jets</t>
+  </si>
+  <si>
+    <t>Guarantee Deposits</t>
+  </si>
+  <si>
+    <t>Dividends Payable</t>
+  </si>
+  <si>
+    <t>Financial Guarantee &amp; Residual</t>
+  </si>
+  <si>
+    <t>Q4 21</t>
+  </si>
+  <si>
+    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1</t>
+  </si>
+  <si>
+    <t>Embraer 190</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -842,7 +863,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -967,6 +988,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -976,26 +998,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1008,8 +1016,24 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1106,7 +1130,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>133</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1123,7 +1147,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13315950" y="0"/>
-          <a:ext cx="0" cy="21564600"/>
+          <a:ext cx="0" cy="22536150"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1149,15 +1173,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1172,8 +1196,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18173700" y="0"/>
-          <a:ext cx="0" cy="17764125"/>
+          <a:off x="18183225" y="0"/>
+          <a:ext cx="0" cy="22717125"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1499,7 +1523,7 @@
   <dimension ref="A2:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G27" sqref="G27:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1519,31 +1543,31 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="G5" s="60" t="s">
+      <c r="C5" s="62"/>
+      <c r="D5" s="63"/>
+      <c r="G5" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="62"/>
-      <c r="U5" s="60" t="s">
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="63"/>
+      <c r="U5" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="61"/>
-      <c r="W5" s="61"/>
-      <c r="X5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="62"/>
+      <c r="X5" s="63"/>
     </row>
     <row r="6" spans="1:24">
       <c r="B6" s="4" t="s">
@@ -1643,8 +1667,8 @@
         <v>6</v>
       </c>
       <c r="C9" s="12">
-        <f>'Financial Model'!S106</f>
-        <v>2102.6</v>
+        <f>'Financial Model'!S113</f>
+        <v>2104.1999999999998</v>
       </c>
       <c r="D9" s="18" t="str">
         <f>$C$28</f>
@@ -1674,7 +1698,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="12">
-        <f>'Financial Model'!T107</f>
+        <f>'Financial Model'!T114</f>
         <v>3173.8999999999996</v>
       </c>
       <c r="D10" s="18" t="str">
@@ -1710,7 +1734,7 @@
       </c>
       <c r="C11" s="12">
         <f>C9-C10</f>
-        <v>-1071.2999999999997</v>
+        <v>-1069.6999999999998</v>
       </c>
       <c r="D11" s="18" t="str">
         <f>$C$28</f>
@@ -1743,7 +1767,7 @@
       </c>
       <c r="C12" s="13">
         <f>C8-C11</f>
-        <v>8013.2699999999986</v>
+        <v>8011.6699999999992</v>
       </c>
       <c r="D12" s="19"/>
       <c r="G12" s="10"/>
@@ -1804,11 +1828,11 @@
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="63"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -1835,10 +1859,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="66"/>
+      <c r="D16" s="65"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -1862,10 +1886,10 @@
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="66"/>
+      <c r="D17" s="65"/>
       <c r="G17" s="9">
         <v>43922</v>
       </c>
@@ -1889,8 +1913,8 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
         <v>169</v>
@@ -1914,8 +1938,8 @@
     </row>
     <row r="19" spans="2:24">
       <c r="B19" s="17"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="68"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="73"/>
       <c r="G19" s="10"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
@@ -1978,11 +2002,11 @@
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="2:24">
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
       <c r="G22" s="10"/>
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
@@ -2006,10 +2030,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="66"/>
+      <c r="D23" s="65"/>
       <c r="G23" s="10"/>
       <c r="H23" s="37"/>
       <c r="I23" s="37"/>
@@ -2031,10 +2055,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="65">
+      <c r="C24" s="64">
         <v>1969</v>
       </c>
-      <c r="D24" s="66"/>
+      <c r="D24" s="65"/>
       <c r="G24" s="10"/>
       <c r="H24" s="37"/>
       <c r="I24" s="37"/>
@@ -2056,8 +2080,8 @@
     </row>
     <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65"/>
       <c r="G25" s="9">
         <v>43770</v>
       </c>
@@ -2085,11 +2109,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="63">
-        <f>'Financial Model'!T59</f>
+      <c r="C26" s="70">
+        <f>'Financial Model'!T60</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="64"/>
+      <c r="D26" s="71"/>
       <c r="G26" s="10"/>
       <c r="H26" s="50" t="s">
         <v>168</v>
@@ -2113,8 +2137,8 @@
     </row>
     <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="66"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="65"/>
       <c r="G27" s="10"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
@@ -2144,12 +2168,8 @@
       <c r="D28" s="32">
         <v>44777</v>
       </c>
-      <c r="G28" s="9">
-        <v>43586</v>
-      </c>
-      <c r="H28" s="37" t="s">
-        <v>166</v>
-      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" s="60"/>
       <c r="I28" s="37"/>
       <c r="J28" s="37"/>
       <c r="K28" s="37"/>
@@ -2173,12 +2193,16 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="71" t="s">
+      <c r="C29" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="72"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="37"/>
+      <c r="D29" s="67"/>
+      <c r="G29" s="9">
+        <v>43586</v>
+      </c>
+      <c r="H29" s="60" t="s">
+        <v>166</v>
+      </c>
       <c r="I29" s="37"/>
       <c r="J29" s="37"/>
       <c r="K29" s="37"/>
@@ -2233,11 +2257,11 @@
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="2:24">
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="63"/>
       <c r="G32" s="10"/>
       <c r="H32" s="37"/>
       <c r="I32" s="37"/>
@@ -2261,11 +2285,11 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="73">
-        <f>C6/'Financial Model'!T104</f>
+      <c r="C33" s="68">
+        <f>C6/'Financial Model'!T111</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="74"/>
+      <c r="D33" s="69"/>
       <c r="G33" s="10"/>
       <c r="H33" s="37"/>
       <c r="I33" s="37"/>
@@ -2287,8 +2311,11 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="75"/>
-      <c r="D34" s="76"/>
+      <c r="C34" s="68">
+        <f>C6/'Financial Model'!AB9</f>
+        <v>2.2515010006671113E-3</v>
+      </c>
+      <c r="D34" s="69"/>
       <c r="G34" s="9">
         <v>43282</v>
       </c>
@@ -2314,8 +2341,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="69"/>
-      <c r="D35" s="70"/>
+      <c r="C35" s="74">
+        <f>C6/'Financial Model'!AB26</f>
+        <v>-155.32248322147649</v>
+      </c>
+      <c r="D35" s="75"/>
       <c r="G35" s="10"/>
       <c r="H35" s="8" t="s">
         <v>163</v>
@@ -2348,12 +2378,12 @@
       <c r="R36" s="36"/>
     </row>
     <row r="37" spans="2:24">
-      <c r="U37" s="60" t="s">
+      <c r="U37" s="61" t="s">
         <v>158</v>
       </c>
-      <c r="V37" s="61"/>
-      <c r="W37" s="61"/>
-      <c r="X37" s="62"/>
+      <c r="V37" s="62"/>
+      <c r="W37" s="62"/>
+      <c r="X37" s="63"/>
     </row>
     <row r="38" spans="2:24">
       <c r="U38" s="42" t="s">
@@ -2393,13 +2423,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="B5:D5"/>
@@ -2413,6 +2436,13 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -2428,20 +2458,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
-  <dimension ref="B1:AL121"/>
+  <dimension ref="B1:AL128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W118" sqref="W118"/>
+      <selection pane="bottomRight" activeCell="T127" sqref="T127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="9.140625" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:38" s="15" customFormat="1">
@@ -2493,7 +2525,7 @@
       <c r="Q1" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="24" t="s">
         <v>47</v>
       </c>
       <c r="S1" s="24" t="s">
@@ -2517,7 +2549,7 @@
       <c r="AA1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AB1" s="24" t="s">
         <v>80</v>
       </c>
       <c r="AC1" s="15" t="s">
@@ -2556,6 +2588,9 @@
       <c r="M2" s="22">
         <v>44104</v>
       </c>
+      <c r="N2" s="22">
+        <v>44196</v>
+      </c>
       <c r="O2" s="22">
         <v>44286</v>
       </c>
@@ -2566,13 +2601,19 @@
         <v>44469</v>
       </c>
       <c r="R2" s="22">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="S2" s="22">
         <v>44651</v>
       </c>
       <c r="T2" s="22">
         <v>44742</v>
+      </c>
+      <c r="AA2" s="22">
+        <v>44196</v>
+      </c>
+      <c r="AB2" s="22">
+        <v>44561</v>
       </c>
     </row>
     <row r="3" spans="2:38" s="21" customFormat="1">
@@ -2581,11 +2622,17 @@
       <c r="Q3" s="23">
         <v>44505</v>
       </c>
+      <c r="R3" s="23">
+        <v>44629</v>
+      </c>
       <c r="S3" s="23">
         <v>44679</v>
       </c>
       <c r="T3" s="23">
         <v>44777</v>
+      </c>
+      <c r="AB3" s="23">
+        <v>44629</v>
       </c>
     </row>
     <row r="4" spans="2:38" s="52" customFormat="1">
@@ -2595,6 +2642,9 @@
       <c r="M4" s="52">
         <v>177.2</v>
       </c>
+      <c r="N4" s="52">
+        <v>689.4</v>
+      </c>
       <c r="O4" s="52">
         <v>272.2</v>
       </c>
@@ -2612,6 +2662,12 @@
       </c>
       <c r="T4" s="52">
         <v>299.89999999999998</v>
+      </c>
+      <c r="AA4" s="52">
+        <v>1114.4000000000001</v>
+      </c>
+      <c r="AB4" s="52">
+        <v>1316.4</v>
       </c>
     </row>
     <row r="5" spans="2:38" s="52" customFormat="1">
@@ -2621,6 +2677,9 @@
       <c r="M5" s="52">
         <v>212.3</v>
       </c>
+      <c r="N5" s="52">
+        <v>580</v>
+      </c>
       <c r="O5" s="52">
         <v>152.1</v>
       </c>
@@ -2638,6 +2697,12 @@
       </c>
       <c r="T5" s="52">
         <v>266.7</v>
+      </c>
+      <c r="AA5" s="52">
+        <v>1071.5</v>
+      </c>
+      <c r="AB5" s="52">
+        <v>1130.0999999999999</v>
       </c>
     </row>
     <row r="6" spans="2:38" s="52" customFormat="1">
@@ -2647,6 +2712,9 @@
       <c r="M6" s="52">
         <v>154.69999999999999</v>
       </c>
+      <c r="N6" s="52">
+        <v>311.10000000000002</v>
+      </c>
       <c r="O6" s="52">
         <v>128.5</v>
       </c>
@@ -2664,6 +2732,12 @@
       </c>
       <c r="T6" s="52">
         <v>126.6</v>
+      </c>
+      <c r="AA6" s="52">
+        <v>653.9</v>
+      </c>
+      <c r="AB6" s="52">
+        <v>594.4</v>
       </c>
     </row>
     <row r="7" spans="2:38" s="52" customFormat="1">
@@ -2673,6 +2747,9 @@
       <c r="M7" s="52">
         <v>212.9</v>
       </c>
+      <c r="N7" s="52">
+        <v>253.5</v>
+      </c>
       <c r="O7" s="52">
         <v>250.6</v>
       </c>
@@ -2690,6 +2767,12 @@
       </c>
       <c r="T7" s="52">
         <v>320.10000000000002</v>
+      </c>
+      <c r="AA7" s="52">
+        <v>920</v>
+      </c>
+      <c r="AB7" s="52">
+        <v>1132.2</v>
       </c>
     </row>
     <row r="8" spans="2:38" s="52" customFormat="1">
@@ -2699,6 +2782,9 @@
       <c r="M8" s="52">
         <v>1.6</v>
       </c>
+      <c r="N8" s="52">
+        <v>7.4</v>
+      </c>
       <c r="O8" s="52">
         <v>3.9</v>
       </c>
@@ -2716,6 +2802,12 @@
       </c>
       <c r="T8" s="52">
         <v>5.6</v>
+      </c>
+      <c r="AA8" s="52">
+        <v>11.3</v>
+      </c>
+      <c r="AB8" s="52">
+        <v>24.1</v>
       </c>
     </row>
     <row r="9" spans="2:38" s="26" customFormat="1">
@@ -2726,6 +2818,9 @@
       <c r="M9" s="26">
         <v>758.7</v>
       </c>
+      <c r="N9" s="26">
+        <v>1841.4</v>
+      </c>
       <c r="O9" s="26">
         <v>807.3</v>
       </c>
@@ -2743,6 +2838,12 @@
       </c>
       <c r="T9" s="26">
         <v>1018.9</v>
+      </c>
+      <c r="AA9" s="26">
+        <v>3771.1</v>
+      </c>
+      <c r="AB9" s="26">
+        <v>4197.2</v>
       </c>
     </row>
     <row r="10" spans="2:38">
@@ -2752,6 +2853,9 @@
       <c r="M10" s="27">
         <v>703.9</v>
       </c>
+      <c r="N10" s="27">
+        <v>1619</v>
+      </c>
       <c r="O10" s="3">
         <v>730.9</v>
       </c>
@@ -2769,6 +2873,12 @@
       </c>
       <c r="T10" s="27">
         <v>785.6</v>
+      </c>
+      <c r="AA10" s="27">
+        <v>3293.5</v>
+      </c>
+      <c r="AB10" s="27">
+        <v>3537.6</v>
       </c>
     </row>
     <row r="11" spans="2:38" s="2" customFormat="1">
@@ -2779,8 +2889,12 @@
         <f>M9-M10</f>
         <v>54.800000000000068</v>
       </c>
+      <c r="N11" s="26">
+        <f t="shared" ref="N11:T11" si="0">N9-N10</f>
+        <v>222.40000000000009</v>
+      </c>
       <c r="O11" s="26">
-        <f t="shared" ref="O11:T11" si="0">O9-O10</f>
+        <f t="shared" si="0"/>
         <v>76.399999999999977</v>
       </c>
       <c r="P11" s="26">
@@ -2803,6 +2917,14 @@
         <f t="shared" si="0"/>
         <v>233.29999999999995</v>
       </c>
+      <c r="AA11" s="26">
+        <f>AA9-AA10</f>
+        <v>477.59999999999991</v>
+      </c>
+      <c r="AB11" s="26">
+        <f>AB9-AB10</f>
+        <v>659.59999999999991</v>
+      </c>
     </row>
     <row r="12" spans="2:38">
       <c r="B12" s="3" t="s">
@@ -2811,6 +2933,9 @@
       <c r="M12" s="27">
         <v>35</v>
       </c>
+      <c r="N12" s="27">
+        <v>42.1</v>
+      </c>
       <c r="O12" s="3">
         <v>34.4</v>
       </c>
@@ -2828,6 +2953,12 @@
       </c>
       <c r="T12" s="27">
         <v>43.9</v>
+      </c>
+      <c r="AA12" s="27">
+        <v>143.4</v>
+      </c>
+      <c r="AB12" s="27">
+        <v>153.19999999999999</v>
       </c>
     </row>
     <row r="13" spans="2:38">
@@ -2837,6 +2968,9 @@
       <c r="M13" s="27">
         <v>45.4</v>
       </c>
+      <c r="N13" s="27">
+        <v>54</v>
+      </c>
       <c r="O13" s="3">
         <v>45.8</v>
       </c>
@@ -2854,6 +2988,12 @@
       </c>
       <c r="T13" s="27">
         <v>67.400000000000006</v>
+      </c>
+      <c r="AA13" s="27">
+        <v>194</v>
+      </c>
+      <c r="AB13" s="27">
+        <v>226.4</v>
       </c>
     </row>
     <row r="14" spans="2:38">
@@ -2863,6 +3003,9 @@
       <c r="M14" s="27">
         <v>14</v>
       </c>
+      <c r="N14" s="27">
+        <v>-7.9</v>
+      </c>
       <c r="O14" s="3">
         <v>0.1</v>
       </c>
@@ -2880,6 +3023,12 @@
       </c>
       <c r="T14" s="27">
         <v>21.3</v>
+      </c>
+      <c r="AA14" s="27">
+        <v>61.8</v>
+      </c>
+      <c r="AB14" s="27">
+        <v>-13</v>
       </c>
     </row>
     <row r="15" spans="2:38">
@@ -2889,6 +3038,9 @@
       <c r="M15" s="27">
         <v>7.1</v>
       </c>
+      <c r="N15" s="27">
+        <v>10.5</v>
+      </c>
       <c r="O15" s="3">
         <v>8.4</v>
       </c>
@@ -2906,6 +3058,12 @@
       </c>
       <c r="T15" s="27">
         <v>24.9</v>
+      </c>
+      <c r="AA15" s="27">
+        <v>29.8</v>
+      </c>
+      <c r="AB15" s="27">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:38">
@@ -2915,6 +3073,9 @@
       <c r="M16" s="27">
         <v>9.1</v>
       </c>
+      <c r="N16" s="27">
+        <v>-19.8</v>
+      </c>
       <c r="O16" s="3">
         <v>-21.8</v>
       </c>
@@ -2933,14 +3094,23 @@
       <c r="T16" s="27">
         <v>-13.5</v>
       </c>
-    </row>
-    <row r="17" spans="2:20">
+      <c r="AA16" s="27">
+        <v>-374.7</v>
+      </c>
+      <c r="AB16" s="27">
+        <v>-49.8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28">
       <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="M17" s="27">
         <v>-0.1</v>
       </c>
+      <c r="N17" s="27">
+        <v>-0.3</v>
+      </c>
       <c r="O17" s="3">
         <v>1</v>
       </c>
@@ -2959,8 +3129,14 @@
       <c r="T17" s="27">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="2:20" s="2" customFormat="1">
+      <c r="AA17" s="27">
+        <v>2.7</v>
+      </c>
+      <c r="AB17" s="27">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" s="2" customFormat="1">
       <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
@@ -2968,8 +3144,12 @@
         <f>M11-M12-M13-M14-M15+M16+M17</f>
         <v>-37.699999999999932</v>
       </c>
+      <c r="N18" s="26">
+        <f t="shared" ref="N18:T18" si="1">N11-N12-N13-N14-N15+N16+N17</f>
+        <v>103.60000000000011</v>
+      </c>
       <c r="O18" s="26">
-        <f t="shared" ref="O18:T18" si="1">O11-O12-O13-O14-O15+O16+O17</f>
+        <f t="shared" si="1"/>
         <v>-33.100000000000023</v>
       </c>
       <c r="P18" s="26">
@@ -2992,14 +3172,25 @@
         <f t="shared" si="1"/>
         <v>66.69999999999996</v>
       </c>
-    </row>
-    <row r="19" spans="2:20">
+      <c r="AA18" s="26">
+        <f t="shared" ref="AA18:AB18" si="2">AA11-AA12-AA13-AA14-AA15+AA16+AA17</f>
+        <v>-323.40000000000003</v>
+      </c>
+      <c r="AB18" s="26">
+        <f t="shared" si="2"/>
+        <v>201.29999999999987</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28">
       <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
       <c r="M19" s="27">
         <v>-94.6</v>
       </c>
+      <c r="N19" s="27">
+        <v>-64.599999999999994</v>
+      </c>
       <c r="O19" s="3">
         <v>-75.400000000000006</v>
       </c>
@@ -3018,14 +3209,23 @@
       <c r="T19" s="27">
         <v>-38</v>
       </c>
-    </row>
-    <row r="20" spans="2:20">
+      <c r="AA19" s="27">
+        <v>-232.7</v>
+      </c>
+      <c r="AB19" s="27">
+        <v>-199.4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28">
       <c r="B20" s="3" t="s">
         <v>61</v>
       </c>
       <c r="M20" s="27">
         <v>-16.3</v>
       </c>
+      <c r="N20" s="27">
+        <v>-27.6</v>
+      </c>
       <c r="O20" s="3">
         <v>19.600000000000001</v>
       </c>
@@ -3044,8 +3244,14 @@
       <c r="T20" s="27">
         <v>20.8</v>
       </c>
-    </row>
-    <row r="21" spans="2:20">
+      <c r="AA20" s="27">
+        <v>-79.099999999999994</v>
+      </c>
+      <c r="AB20" s="27">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
@@ -3053,38 +3259,53 @@
         <f>M18+M19+M20</f>
         <v>-148.59999999999994</v>
       </c>
+      <c r="N21" s="27">
+        <f t="shared" ref="N21:T21" si="3">N18+N19+N20</f>
+        <v>11.400000000000112</v>
+      </c>
       <c r="O21" s="27">
-        <f t="shared" ref="O21:T21" si="2">O18+O19+O20</f>
+        <f t="shared" si="3"/>
         <v>-88.900000000000034</v>
       </c>
       <c r="P21" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.600000000000037</v>
       </c>
       <c r="Q21" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24.99999999999995</v>
       </c>
       <c r="R21" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57.699999999999946</v>
       </c>
       <c r="S21" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-81</v>
       </c>
       <c r="T21" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.499999999999957</v>
       </c>
-    </row>
-    <row r="22" spans="2:20">
+      <c r="AA21" s="27">
+        <f t="shared" ref="AA21:AB21" si="4">AA18+AA19+AA20</f>
+        <v>-635.20000000000005</v>
+      </c>
+      <c r="AB21" s="27">
+        <f t="shared" si="4"/>
+        <v>27.399999999999864</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28">
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
       <c r="M22" s="27">
         <v>-29.1</v>
       </c>
+      <c r="N22" s="27">
+        <v>16.899999999999999</v>
+      </c>
       <c r="O22" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -3103,8 +3324,14 @@
       <c r="T22" s="27">
         <v>-24.6</v>
       </c>
-    </row>
-    <row r="23" spans="2:20" s="2" customFormat="1">
+      <c r="AA22" s="27">
+        <v>93.1</v>
+      </c>
+      <c r="AB22" s="27">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" s="2" customFormat="1">
       <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
@@ -3112,38 +3339,53 @@
         <f>M21-M22</f>
         <v>-119.49999999999994</v>
       </c>
+      <c r="N23" s="26">
+        <f t="shared" ref="N23:T23" si="5">N21-N22</f>
+        <v>-5.4999999999998863</v>
+      </c>
       <c r="O23" s="26">
-        <f t="shared" ref="O23:T23" si="3">O21-O22</f>
+        <f t="shared" si="5"/>
         <v>-90.000000000000028</v>
       </c>
       <c r="P23" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>89.200000000000031</v>
       </c>
       <c r="Q23" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-45.699999999999946</v>
       </c>
       <c r="R23" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.9999999999999432</v>
       </c>
       <c r="S23" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-30.700000000000003</v>
       </c>
       <c r="T23" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>74.099999999999966</v>
       </c>
-    </row>
-    <row r="24" spans="2:20" s="2" customFormat="1">
+      <c r="AA23" s="26">
+        <f>AA21-AA22</f>
+        <v>-728.30000000000007</v>
+      </c>
+      <c r="AB23" s="26">
+        <f>AB21-AB22</f>
+        <v>-43.500000000000142</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" s="2" customFormat="1">
       <c r="B24" s="29" t="s">
         <v>72</v>
       </c>
       <c r="M24" s="26">
         <v>-121.2</v>
       </c>
+      <c r="N24" s="26">
+        <v>-3.3</v>
+      </c>
       <c r="O24" s="2">
         <v>-89.7</v>
       </c>
@@ -3162,14 +3404,23 @@
       <c r="T24" s="26">
         <v>74.2</v>
       </c>
-    </row>
-    <row r="25" spans="2:20">
+      <c r="AA24" s="26">
+        <v>-731.9</v>
+      </c>
+      <c r="AB24" s="26">
+        <v>-44.7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28">
       <c r="B25" s="30" t="s">
         <v>73</v>
       </c>
       <c r="M25" s="27">
         <v>1.7</v>
       </c>
+      <c r="N25" s="27">
+        <v>-2.2000000000000002</v>
+      </c>
       <c r="O25" s="3">
         <v>-0.3</v>
       </c>
@@ -3188,8 +3439,14 @@
       <c r="T25" s="27">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="26" spans="2:20">
+      <c r="AA25" s="27">
+        <v>3.6</v>
+      </c>
+      <c r="AB25" s="27">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28">
       <c r="B26" s="3" t="s">
         <v>65</v>
       </c>
@@ -3197,38 +3454,53 @@
         <f>M24/M27</f>
         <v>-0.16462917685411571</v>
       </c>
+      <c r="N26" s="28">
+        <f t="shared" ref="N26:T26" si="6">N24/N27</f>
+        <v>-4.4824775876120618E-3</v>
+      </c>
       <c r="O26" s="28">
-        <f t="shared" ref="O26:T26" si="4">O24/O27</f>
+        <f t="shared" si="6"/>
         <v>-0.12204081632653062</v>
       </c>
       <c r="P26" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.11962438758845946</v>
       </c>
       <c r="Q26" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-6.1241154055525319E-2</v>
       </c>
       <c r="R26" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8583095140873828E-3</v>
       </c>
       <c r="S26" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-4.3152736182956709E-2</v>
       </c>
       <c r="T26" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.10100735093928669</v>
       </c>
-    </row>
-    <row r="27" spans="2:20">
+      <c r="AA26" s="28">
+        <f t="shared" ref="AA26:AB26" si="7">AA24/AA27</f>
+        <v>-0.99415919587068724</v>
+      </c>
+      <c r="AB26" s="28">
+        <f t="shared" si="7"/>
+        <v>-6.0841159657002861E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28">
       <c r="B27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M27" s="3">
         <v>736.2</v>
       </c>
+      <c r="N27" s="3">
+        <v>736.2</v>
+      </c>
       <c r="O27" s="27">
         <v>735</v>
       </c>
@@ -3247,8 +3519,14 @@
       <c r="T27" s="3">
         <v>734.6</v>
       </c>
-    </row>
-    <row r="30" spans="2:20" s="2" customFormat="1">
+      <c r="AA27" s="3">
+        <v>736.2</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>734.7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" s="2" customFormat="1">
       <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
@@ -3256,7 +3534,10 @@
         <f>Q9/M9-1</f>
         <v>0.26281797812046914</v>
       </c>
-      <c r="R30" s="34"/>
+      <c r="R30" s="34">
+        <f>R9/N9-1</f>
+        <v>-0.29330943847072888</v>
+      </c>
       <c r="S30" s="34">
         <f>S9/O9-1</f>
         <v>-0.25566703827573389</v>
@@ -3265,21 +3546,33 @@
         <f>T9/P9-1</f>
         <v>-9.8717381689517936E-2</v>
       </c>
-    </row>
-    <row r="31" spans="2:20" s="25" customFormat="1">
+      <c r="AB30" s="34">
+        <f>AB9/AA9-1</f>
+        <v>0.11299090451062033</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" s="25" customFormat="1">
       <c r="B31" s="25" t="s">
         <v>67</v>
+      </c>
+      <c r="N31" s="25">
+        <f t="shared" ref="N31:P31" si="8">N9/M9-1</f>
+        <v>1.4270462633451957</v>
+      </c>
+      <c r="O31" s="25">
+        <f t="shared" si="8"/>
+        <v>-0.56158357771261003</v>
       </c>
       <c r="P31" s="25">
         <f>P9/O9-1</f>
         <v>0.40034683512944391</v>
       </c>
       <c r="Q31" s="25">
-        <f t="shared" ref="Q31:R31" si="5">Q9/P9-1</f>
+        <f t="shared" ref="Q31:R31" si="9">Q9/P9-1</f>
         <v>-0.15249889429455987</v>
       </c>
       <c r="R31" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.35820895522388052</v>
       </c>
       <c r="S31" s="25">
@@ -3291,7 +3584,7 @@
         <v>0.69562323181893837</v>
       </c>
     </row>
-    <row r="34" spans="2:20">
+    <row r="34" spans="2:28">
       <c r="B34" s="3" t="s">
         <v>68</v>
       </c>
@@ -3299,6 +3592,10 @@
         <f>M11/M9</f>
         <v>7.2228812442335658E-2</v>
       </c>
+      <c r="N34" s="25">
+        <f t="shared" ref="N34:O34" si="10">N11/N9</f>
+        <v>0.12077766916476598</v>
+      </c>
       <c r="O34" s="25">
         <f>O11/O9</f>
         <v>9.4636442462529391E-2</v>
@@ -3308,23 +3605,31 @@
         <v>0.18195488721804515</v>
       </c>
       <c r="Q34" s="25">
-        <f t="shared" ref="Q34:R34" si="6">Q11/Q9</f>
+        <f t="shared" ref="Q34:R34" si="11">Q11/Q9</f>
         <v>0.18964617472080164</v>
       </c>
       <c r="R34" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.1504649196956889</v>
       </c>
       <c r="S34" s="25">
-        <f t="shared" ref="S34" si="7">S11/S9</f>
+        <f t="shared" ref="S34" si="12">S11/S9</f>
         <v>0.20086536861374604</v>
       </c>
       <c r="T34" s="25">
         <f>T11/T9</f>
         <v>0.2289724212385906</v>
       </c>
-    </row>
-    <row r="35" spans="2:20">
+      <c r="AA34" s="25">
+        <f>AA11/AA9</f>
+        <v>0.12664739731112937</v>
+      </c>
+      <c r="AB34" s="25">
+        <f>AB11/AB9</f>
+        <v>0.15715238730582293</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28">
       <c r="B35" s="3" t="s">
         <v>69</v>
       </c>
@@ -3332,6 +3637,10 @@
         <f>M18/M9</f>
         <v>-4.9690259654672372E-2</v>
       </c>
+      <c r="N35" s="25">
+        <f t="shared" ref="N35:O35" si="13">N18/N9</f>
+        <v>5.6261540132507927E-2</v>
+      </c>
       <c r="O35" s="25">
         <f>O18/O9</f>
         <v>-4.1000867087823641E-2</v>
@@ -3341,23 +3650,31 @@
         <v>0.12720035382574085</v>
       </c>
       <c r="Q35" s="25">
-        <f t="shared" ref="Q35:R35" si="8">Q18/Q9</f>
+        <f t="shared" ref="Q35:R35" si="14">Q18/Q9</f>
         <v>3.1311971610479127E-2</v>
       </c>
       <c r="R35" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>4.6568815799584988E-2</v>
       </c>
       <c r="S35" s="25">
-        <f t="shared" ref="S35" si="9">S18/S9</f>
+        <f t="shared" ref="S35" si="15">S18/S9</f>
         <v>-6.0409385921118344E-2</v>
       </c>
       <c r="T35" s="25">
         <f>T18/T9</f>
         <v>6.5462753950338556E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:20">
+      <c r="AA35" s="25">
+        <f>AA18/AA9</f>
+        <v>-8.5757471294847662E-2</v>
+      </c>
+      <c r="AB35" s="25">
+        <f>AB18/AB9</f>
+        <v>4.7960545125321614E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28">
       <c r="B36" s="3" t="s">
         <v>70</v>
       </c>
@@ -3365,6 +3682,10 @@
         <f>M23/M9</f>
         <v>-0.15750626070910759</v>
       </c>
+      <c r="N36" s="25">
+        <f t="shared" ref="N36:O36" si="16">N23/N9</f>
+        <v>-2.9868578255674411E-3</v>
+      </c>
       <c r="O36" s="25">
         <f>O23/O9</f>
         <v>-0.11148272017837239</v>
@@ -3374,23 +3695,31 @@
         <v>7.8903140203449823E-2</v>
       </c>
       <c r="Q36" s="25">
-        <f t="shared" ref="Q36:R36" si="10">Q23/Q9</f>
+        <f t="shared" ref="Q36:R36" si="17">Q23/Q9</f>
         <v>-4.7698570086629734E-2</v>
       </c>
       <c r="R36" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>2.3053869207714925E-3</v>
       </c>
       <c r="S36" s="25">
-        <f t="shared" ref="S36" si="11">S23/S9</f>
+        <f t="shared" ref="S36" si="18">S23/S9</f>
         <v>-5.1090031619237815E-2</v>
       </c>
       <c r="T36" s="25">
         <f>T23/T9</f>
         <v>7.2725488271665487E-2</v>
       </c>
-    </row>
-    <row r="37" spans="2:20">
+      <c r="AA36" s="25">
+        <f>AA23/AA9</f>
+        <v>-0.1931266739147729</v>
+      </c>
+      <c r="AB36" s="25">
+        <f>AB23/AB9</f>
+        <v>-1.0364052225293087E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28">
       <c r="B37" s="3" t="s">
         <v>71</v>
       </c>
@@ -3398,6 +3727,10 @@
         <f>M22/M21</f>
         <v>0.19582772543741597</v>
       </c>
+      <c r="N37" s="25">
+        <f t="shared" ref="N37:O37" si="19">N22/N21</f>
+        <v>1.4824561403508625</v>
+      </c>
       <c r="O37" s="25">
         <f>O22/O21</f>
         <v>-1.2373453318335205E-2</v>
@@ -3407,1098 +3740,2484 @@
         <v>-6.6985645933014315E-2</v>
       </c>
       <c r="Q37" s="25">
-        <f t="shared" ref="Q37:R37" si="12">Q22/Q21</f>
+        <f t="shared" ref="Q37:R37" si="20">Q22/Q21</f>
         <v>-0.82800000000000162</v>
       </c>
       <c r="R37" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0.94800693240901301</v>
       </c>
       <c r="S37" s="25">
-        <f t="shared" ref="S37" si="13">S22/S21</f>
+        <f t="shared" ref="S37" si="21">S22/S21</f>
         <v>0.62098765432098757</v>
       </c>
       <c r="T37" s="25">
         <f>T22/T21</f>
         <v>-0.49696969696969745</v>
       </c>
-    </row>
-    <row r="40" spans="2:20">
+      <c r="AA37" s="25">
+        <f>AA22/AA21</f>
+        <v>-0.14656801007556672</v>
+      </c>
+      <c r="AB37" s="25">
+        <f>AB22/AB21</f>
+        <v>2.5875912408759256</v>
+      </c>
+    </row>
+    <row r="40" spans="2:28">
       <c r="B40" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="2:20" s="2" customFormat="1">
+    <row r="41" spans="2:28" s="2" customFormat="1">
       <c r="B41" s="29" t="s">
         <v>83</v>
       </c>
+      <c r="N41" s="2">
+        <f>O42+O48</f>
+        <v>0</v>
+      </c>
       <c r="P41" s="2">
-        <f t="shared" ref="P41:S41" si="14">P42+P47</f>
+        <f t="shared" ref="O41:S41" si="22">P42+P48</f>
         <v>34</v>
       </c>
       <c r="Q41" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>30</v>
       </c>
+      <c r="R41" s="2">
+        <f t="shared" si="22"/>
+        <v>55</v>
+      </c>
       <c r="S41" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>26</v>
       </c>
       <c r="T41" s="2">
-        <f>T42+T47</f>
+        <f>T42+T48</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="2:20" s="40" customFormat="1">
+      <c r="AA41" s="2">
+        <f>AA42+AA48</f>
+        <v>129</v>
+      </c>
+      <c r="AB41" s="2">
+        <f>AB42+AB48</f>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" s="40" customFormat="1">
       <c r="B42" s="49" t="s">
         <v>84</v>
       </c>
+      <c r="N42" s="40">
+        <f>N43+N45+N46</f>
+        <v>28</v>
+      </c>
       <c r="P42" s="40">
-        <f>P43+P44+P45</f>
+        <f>P43+P45+P46</f>
         <v>14</v>
       </c>
       <c r="Q42" s="40">
-        <f>Q43+Q44+Q45</f>
+        <f>Q43+Q45+Q46</f>
         <v>9</v>
       </c>
+      <c r="R42" s="40">
+        <f>R43+R45+R46</f>
+        <v>16</v>
+      </c>
       <c r="S42" s="40">
-        <f t="shared" ref="S42:T42" si="15">S43+S44+S45</f>
+        <f t="shared" ref="S42:T42" si="23">S43+S45+S46</f>
         <v>6</v>
       </c>
       <c r="T42" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="2:20" s="39" customFormat="1">
+      <c r="AA42" s="40">
+        <f t="shared" ref="AA42:AB42" si="24">AA43+AA45+AA46</f>
+        <v>43</v>
+      </c>
+      <c r="AB42" s="40">
+        <f t="shared" si="24"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="2:28" s="39" customFormat="1">
       <c r="B43" s="48" t="s">
         <v>85</v>
       </c>
+      <c r="N43" s="39">
+        <v>21</v>
+      </c>
       <c r="P43" s="39">
         <v>7</v>
       </c>
       <c r="Q43" s="39">
         <v>6</v>
       </c>
+      <c r="R43" s="39">
+        <v>12</v>
+      </c>
       <c r="S43" s="39">
         <v>4</v>
       </c>
       <c r="T43" s="39">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="2:20" s="39" customFormat="1">
+      <c r="AA43" s="39">
+        <v>32</v>
+      </c>
+      <c r="AB43" s="39">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="2:28" s="39" customFormat="1">
       <c r="B44" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA44" s="39">
+        <v>1</v>
+      </c>
+      <c r="AB44" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" s="39" customFormat="1">
+      <c r="B45" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="P44" s="39">
+      <c r="N45" s="39">
+        <v>1</v>
+      </c>
+      <c r="P45" s="39">
         <v>0</v>
       </c>
-      <c r="Q44" s="39">
+      <c r="Q45" s="39">
         <v>0</v>
       </c>
-      <c r="S44" s="39">
+      <c r="R45" s="39">
         <v>0</v>
       </c>
-      <c r="T44" s="39">
+      <c r="S45" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:20" s="39" customFormat="1">
-      <c r="B45" s="48" t="s">
+      <c r="T45" s="39">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="39">
+        <v>4</v>
+      </c>
+      <c r="AB45" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" s="39" customFormat="1">
+      <c r="B46" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="P45" s="39">
+      <c r="N46" s="39">
+        <v>6</v>
+      </c>
+      <c r="P46" s="39">
         <v>7</v>
       </c>
-      <c r="Q45" s="39">
+      <c r="Q46" s="39">
         <v>3</v>
       </c>
-      <c r="S45" s="39">
+      <c r="R46" s="39">
+        <v>4</v>
+      </c>
+      <c r="S46" s="39">
         <v>2</v>
       </c>
-      <c r="T45" s="39">
+      <c r="T46" s="39">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="2:20" s="39" customFormat="1">
-      <c r="B46" s="48"/>
-    </row>
-    <row r="47" spans="2:20" s="40" customFormat="1">
-      <c r="B47" s="49" t="s">
+      <c r="AA46" s="39">
+        <v>7</v>
+      </c>
+      <c r="AB46" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" s="39" customFormat="1">
+      <c r="B47" s="48"/>
+    </row>
+    <row r="48" spans="2:28" s="40" customFormat="1">
+      <c r="B48" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P47" s="40">
-        <f>P48+P49+P50</f>
+      <c r="N48" s="40">
+        <f>N49+N50+N51</f>
+        <v>43</v>
+      </c>
+      <c r="P48" s="40">
+        <f>P49+P50+P51</f>
         <v>20</v>
       </c>
-      <c r="Q47" s="40">
-        <f>Q48+Q49+Q50</f>
+      <c r="Q48" s="40">
+        <f>Q49+Q50+Q51</f>
         <v>21</v>
       </c>
-      <c r="S47" s="40">
-        <f>S48+S49+S50</f>
+      <c r="R48" s="40">
+        <f>R49+R50+R51</f>
+        <v>39</v>
+      </c>
+      <c r="S48" s="40">
+        <f>S49+S50+S51</f>
         <v>20</v>
       </c>
-      <c r="T47" s="40">
-        <f>T48+T49+T50</f>
+      <c r="T48" s="40">
+        <f>T49+T50+T51</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="2:20" s="39" customFormat="1">
-      <c r="B48" s="48" t="s">
+      <c r="AA48" s="40">
+        <f>AA49+AA50+AA51</f>
+        <v>86</v>
+      </c>
+      <c r="AB48" s="40">
+        <f>AB49+AB50+AB51</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="2:28" s="39" customFormat="1">
+      <c r="B49" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="P48" s="39">
+      <c r="N49" s="39">
+        <v>23</v>
+      </c>
+      <c r="P49" s="39">
         <v>12</v>
       </c>
-      <c r="Q48" s="39">
+      <c r="Q49" s="39">
         <v>14</v>
       </c>
-      <c r="S48" s="39">
+      <c r="R49" s="39">
+        <v>26</v>
+      </c>
+      <c r="S49" s="39">
         <v>12</v>
       </c>
-      <c r="T48" s="39">
+      <c r="T49" s="39">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="2:20" s="39" customFormat="1">
-      <c r="B49" s="48" t="s">
+      <c r="AA49" s="39">
+        <v>56</v>
+      </c>
+      <c r="AB49" s="39">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="2:28" s="39" customFormat="1">
+      <c r="B50" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="P49" s="39">
+      <c r="N50" s="39">
+        <v>20</v>
+      </c>
+      <c r="P50" s="39">
         <v>8</v>
       </c>
-      <c r="Q49" s="39">
+      <c r="Q50" s="39">
         <v>0</v>
       </c>
-      <c r="S49" s="39">
+      <c r="R50" s="39">
+        <v>13</v>
+      </c>
+      <c r="S50" s="39">
         <v>8</v>
       </c>
-      <c r="T49" s="39">
+      <c r="T50" s="39">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="2:20" s="39" customFormat="1">
-      <c r="B50" s="48" t="s">
+      <c r="AA50" s="39">
+        <v>30</v>
+      </c>
+      <c r="AB50" s="39">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="2:28" s="39" customFormat="1">
+      <c r="B51" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="P50" s="39">
+      <c r="N51" s="39">
         <v>0</v>
       </c>
-      <c r="Q50" s="39">
+      <c r="P51" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="39">
         <v>7</v>
       </c>
-      <c r="S50" s="39">
+      <c r="R51" s="39">
         <v>0</v>
       </c>
-      <c r="T50" s="39">
+      <c r="S51" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:20">
-      <c r="B52" s="33" t="s">
+      <c r="T51" s="39">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:28">
+      <c r="B53" s="33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="2:20" s="2" customFormat="1">
-      <c r="B53" s="2" t="s">
+    <row r="54" spans="2:28" s="2" customFormat="1">
+      <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P53" s="26"/>
-      <c r="R53" s="26"/>
-      <c r="S53" s="26">
+      <c r="N54" s="26">
+        <v>1883.1</v>
+      </c>
+      <c r="P54" s="26">
+        <v>1351.2</v>
+      </c>
+      <c r="Q54" s="26">
+        <v>1596.8</v>
+      </c>
+      <c r="R54" s="26">
+        <v>1818.3</v>
+      </c>
+      <c r="S54" s="26">
         <v>1129.8</v>
       </c>
-      <c r="T53" s="26">
+      <c r="T54" s="26">
         <v>1041.3</v>
       </c>
-    </row>
-    <row r="54" spans="2:20" s="2" customFormat="1">
-      <c r="B54" s="2" t="s">
+      <c r="AA54" s="26">
+        <f>N54</f>
+        <v>1883.1</v>
+      </c>
+      <c r="AB54" s="26">
+        <f>R54</f>
+        <v>1818.3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:28" s="2" customFormat="1">
+      <c r="B55" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P54" s="26"/>
-      <c r="R54" s="26"/>
-      <c r="S54" s="26">
+      <c r="N55" s="26">
+        <v>817.5</v>
+      </c>
+      <c r="P55" s="26">
+        <v>1092.8</v>
+      </c>
+      <c r="Q55" s="26">
+        <v>855.3</v>
+      </c>
+      <c r="R55" s="26">
+        <v>750.8</v>
+      </c>
+      <c r="S55" s="26">
         <v>802.9</v>
       </c>
-      <c r="T54" s="26">
+      <c r="T55" s="26">
         <v>753.8</v>
       </c>
-    </row>
-    <row r="55" spans="2:20">
-      <c r="B55" s="3" t="s">
+      <c r="AA55" s="26">
+        <f>N55</f>
+        <v>817.5</v>
+      </c>
+      <c r="AB55" s="26">
+        <f>R55</f>
+        <v>750.8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:28">
+      <c r="B56" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="P55" s="27"/>
-      <c r="R55" s="27"/>
-      <c r="S55" s="27">
+      <c r="N56" s="27">
+        <v>203.4</v>
+      </c>
+      <c r="P56" s="27">
+        <v>198.8</v>
+      </c>
+      <c r="Q56" s="27">
+        <v>203.1</v>
+      </c>
+      <c r="R56" s="27">
+        <v>189</v>
+      </c>
+      <c r="S56" s="27">
         <v>197</v>
       </c>
-      <c r="T55" s="27">
+      <c r="T56" s="27">
         <v>240.4</v>
       </c>
-    </row>
-    <row r="56" spans="2:20">
-      <c r="B56" s="3" t="s">
+      <c r="AA56" s="27">
+        <f t="shared" ref="AA56:AA59" si="25">N56</f>
+        <v>203.4</v>
+      </c>
+      <c r="AB56" s="27">
+        <f>R56</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="2:28">
+      <c r="B57" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="P56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="27">
+      <c r="N57" s="27">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="P57" s="27">
+        <v>4.3</v>
+      </c>
+      <c r="Q57" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="R57" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="S57" s="27">
         <v>9.6999999999999993</v>
       </c>
-      <c r="T56" s="27">
+      <c r="T57" s="27">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="57" spans="2:20">
-      <c r="B57" s="3" t="s">
+      <c r="AA57" s="27">
+        <f t="shared" si="25"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AB57" s="27">
+        <f t="shared" ref="AB57:AB77" si="26">R57</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:28">
+      <c r="B58" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="P57" s="27"/>
-      <c r="R57" s="27"/>
-      <c r="S57" s="27">
+      <c r="N58" s="27">
+        <v>8.5</v>
+      </c>
+      <c r="P58" s="27">
+        <v>7.4</v>
+      </c>
+      <c r="Q58" s="27">
+        <v>7.9</v>
+      </c>
+      <c r="R58" s="27">
+        <v>9.6</v>
+      </c>
+      <c r="S58" s="27">
         <v>9.8000000000000007</v>
       </c>
-      <c r="T57" s="27">
+      <c r="T58" s="27">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="58" spans="2:20">
-      <c r="B58" s="3" t="s">
+      <c r="AA58" s="27">
+        <f t="shared" si="25"/>
+        <v>8.5</v>
+      </c>
+      <c r="AB58" s="27">
+        <f t="shared" si="26"/>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:28">
+      <c r="B59" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="P58" s="27"/>
-      <c r="R58" s="27"/>
-      <c r="S58" s="27">
+      <c r="N59" s="27">
+        <v>461.8</v>
+      </c>
+      <c r="P59" s="27">
+        <v>630.70000000000005</v>
+      </c>
+      <c r="Q59" s="27">
+        <v>618.79999999999995</v>
+      </c>
+      <c r="R59" s="27">
+        <v>582.29999999999995</v>
+      </c>
+      <c r="S59" s="27">
         <v>615.5</v>
       </c>
-      <c r="T58" s="27">
+      <c r="T59" s="27">
         <v>620</v>
       </c>
-    </row>
-    <row r="59" spans="2:20" s="2" customFormat="1">
-      <c r="B59" s="2" t="s">
+      <c r="AA59" s="27">
+        <f t="shared" si="25"/>
+        <v>461.8</v>
+      </c>
+      <c r="AB59" s="27">
+        <f t="shared" si="26"/>
+        <v>582.29999999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="2:28" s="2" customFormat="1">
+      <c r="B60" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="P59" s="26"/>
-      <c r="Q59" s="26"/>
-      <c r="R59" s="26"/>
-      <c r="S59" s="26">
+      <c r="N60" s="26">
+        <v>2437.9</v>
+      </c>
+      <c r="P60" s="26">
+        <v>2315</v>
+      </c>
+      <c r="Q60" s="26">
+        <v>2305</v>
+      </c>
+      <c r="R60" s="26">
+        <v>1986</v>
+      </c>
+      <c r="S60" s="26">
         <v>2222.8000000000002</v>
       </c>
-      <c r="T59" s="26">
+      <c r="T60" s="26">
         <v>2392.9</v>
       </c>
-    </row>
-    <row r="60" spans="2:20">
-      <c r="B60" s="3" t="s">
+      <c r="AA60" s="26">
+        <f>N60</f>
+        <v>2437.9</v>
+      </c>
+      <c r="AB60" s="26">
+        <f>R60</f>
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="61" spans="2:28">
+      <c r="B61" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="P60" s="27"/>
-      <c r="Q60" s="27"/>
-      <c r="R60" s="27"/>
-      <c r="S60" s="27">
+      <c r="N61" s="27">
+        <v>114.1</v>
+      </c>
+      <c r="P61" s="27">
+        <v>134.69999999999999</v>
+      </c>
+      <c r="Q61" s="27">
+        <v>128.19999999999999</v>
+      </c>
+      <c r="R61" s="27">
+        <v>114.5</v>
+      </c>
+      <c r="S61" s="27">
         <v>105</v>
       </c>
-      <c r="T60" s="27">
+      <c r="T61" s="27">
         <v>101.9</v>
       </c>
-    </row>
-    <row r="61" spans="2:20">
-      <c r="B61" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="P61" s="27"/>
-      <c r="Q61" s="27"/>
-      <c r="R61" s="27"/>
-      <c r="S61" s="27">
-        <v>217</v>
-      </c>
-      <c r="T61" s="27">
-        <v>209.3</v>
-      </c>
-    </row>
-    <row r="62" spans="2:20">
+      <c r="AA61" s="27">
+        <f t="shared" ref="AA61:AA64" si="27">N61</f>
+        <v>114.1</v>
+      </c>
+      <c r="AB61" s="27">
+        <f t="shared" si="26"/>
+        <v>114.5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:28">
       <c r="B62" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="P62" s="27"/>
-      <c r="Q62" s="27"/>
-      <c r="R62" s="27"/>
+        <v>185</v>
+      </c>
+      <c r="N62" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="P62" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="Q62" s="27">
+        <v>101.9</v>
+      </c>
+      <c r="R62" s="3">
+        <v>0.6</v>
+      </c>
       <c r="S62" s="27">
-        <v>227.1</v>
+        <v>0</v>
       </c>
       <c r="T62" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="2:20">
+      <c r="AA62" s="27">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+      <c r="AB62" s="27">
+        <f t="shared" si="26"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="63" spans="2:28">
       <c r="B63" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N63" s="27">
+        <v>180.9</v>
+      </c>
+      <c r="P63" s="27">
+        <v>194.2</v>
+      </c>
+      <c r="Q63" s="27">
+        <v>202.3</v>
+      </c>
+      <c r="R63" s="3">
+        <v>193.7</v>
+      </c>
+      <c r="S63" s="27">
+        <v>217</v>
+      </c>
+      <c r="T63" s="27">
+        <v>209.3</v>
+      </c>
+      <c r="AA63" s="27">
+        <f t="shared" si="27"/>
+        <v>180.9</v>
+      </c>
+      <c r="AB63" s="27">
+        <f t="shared" si="26"/>
+        <v>193.7</v>
+      </c>
+    </row>
+    <row r="64" spans="2:28">
+      <c r="B64" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N64" s="27">
+        <v>0</v>
+      </c>
+      <c r="P64" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="27">
+        <v>0</v>
+      </c>
+      <c r="R64" s="3">
+        <v>230.9</v>
+      </c>
+      <c r="S64" s="27">
+        <v>227.1</v>
+      </c>
+      <c r="T64" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="27">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="AB64" s="27">
+        <f t="shared" si="26"/>
+        <v>230.9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:28">
+      <c r="B65" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="P63" s="27"/>
-      <c r="Q63" s="27"/>
-      <c r="R63" s="27"/>
-      <c r="S63" s="27">
-        <f>SUM(S53:S62)</f>
+      <c r="N65" s="27">
+        <f>SUM(N54:N64)</f>
+        <v>6115.7</v>
+      </c>
+      <c r="P65" s="27">
+        <f>SUM(P54:P64)</f>
+        <v>5929.3</v>
+      </c>
+      <c r="Q65" s="27">
+        <f>SUM(Q54:Q64)</f>
+        <v>6019.7999999999993</v>
+      </c>
+      <c r="R65" s="27">
+        <f>SUM(R54:R64)</f>
+        <v>5875.7999999999993</v>
+      </c>
+      <c r="S65" s="27">
+        <f>SUM(S54:S64)</f>
         <v>5536.6</v>
       </c>
-      <c r="T63" s="27">
-        <f>SUM(T53:T62)</f>
+      <c r="T65" s="27">
+        <f>SUM(T54:T64)</f>
         <v>5367.9000000000005</v>
       </c>
-    </row>
-    <row r="64" spans="2:20" s="2" customFormat="1">
-      <c r="B64" s="2" t="s">
+      <c r="AA65" s="27">
+        <f>SUM(AA54:AA64)</f>
+        <v>6115.7</v>
+      </c>
+      <c r="AB65" s="27">
+        <f>SUM(AB54:AB64)</f>
+        <v>5875.7999999999993</v>
+      </c>
+    </row>
+    <row r="66" spans="2:28" s="2" customFormat="1">
+      <c r="B66" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P64" s="26"/>
-      <c r="Q64" s="26"/>
-      <c r="R64" s="26"/>
-      <c r="S64" s="26">
+      <c r="N66" s="26">
+        <v>51.7</v>
+      </c>
+      <c r="P66" s="26">
+        <v>47.3</v>
+      </c>
+      <c r="Q66" s="26">
+        <v>51.6</v>
+      </c>
+      <c r="R66" s="26">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="S66" s="26">
         <v>169.9</v>
       </c>
-      <c r="T64" s="26">
+      <c r="T66" s="26">
         <v>169.9</v>
       </c>
-    </row>
-    <row r="65" spans="2:20" s="2" customFormat="1">
-      <c r="B65" s="3" t="s">
+      <c r="AA66" s="26">
+        <f>N66</f>
+        <v>51.7</v>
+      </c>
+      <c r="AB66" s="26">
+        <f>R66</f>
+        <v>65.599999999999994</v>
+      </c>
+    </row>
+    <row r="67" spans="2:28">
+      <c r="B67" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="P65" s="26"/>
-      <c r="Q65" s="26"/>
-      <c r="R65" s="26"/>
-      <c r="S65" s="26">
+      <c r="N67" s="27">
+        <v>0</v>
+      </c>
+      <c r="P67" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="Q67" s="27">
+        <v>0</v>
+      </c>
+      <c r="R67" s="27">
+        <v>0</v>
+      </c>
+      <c r="S67" s="27">
         <v>1.6</v>
       </c>
-      <c r="T65" s="26">
+      <c r="T67" s="27">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="66" spans="2:20">
-      <c r="B66" s="3" t="s">
+      <c r="AA67" s="27">
+        <f t="shared" ref="AA67:AA77" si="28">N67</f>
+        <v>0</v>
+      </c>
+      <c r="AB67" s="27">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:28" s="2" customFormat="1">
+      <c r="B68" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P66" s="27"/>
-      <c r="Q66" s="27"/>
-      <c r="R66" s="27"/>
-      <c r="S66" s="27">
+      <c r="N68" s="26">
+        <v>1.3</v>
+      </c>
+      <c r="P68" s="26">
+        <v>23</v>
+      </c>
+      <c r="Q68" s="26">
+        <v>0</v>
+      </c>
+      <c r="R68" s="26">
+        <v>0</v>
+      </c>
+      <c r="S68" s="26">
         <v>1.6</v>
       </c>
-      <c r="T66" s="27">
+      <c r="T68" s="26">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="67" spans="2:20">
-      <c r="B67" s="3" t="s">
+      <c r="AA68" s="26">
+        <f>N68</f>
+        <v>1.3</v>
+      </c>
+      <c r="AB68" s="26">
+        <f>R68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:28">
+      <c r="B69" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="N69" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="P69" s="27"/>
+      <c r="Q69" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="R69" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="S69" s="27"/>
+      <c r="T69" s="27"/>
+      <c r="AA69" s="27">
+        <f t="shared" si="28"/>
+        <v>1.5</v>
+      </c>
+      <c r="AB69" s="27">
+        <f t="shared" si="26"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="70" spans="2:28">
+      <c r="B70" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="P67" s="27"/>
-      <c r="Q67" s="27"/>
-      <c r="R67" s="27"/>
-      <c r="S67" s="27">
+      <c r="N70" s="27">
+        <v>21.4</v>
+      </c>
+      <c r="P70" s="27">
+        <v>42.1</v>
+      </c>
+      <c r="Q70" s="27">
+        <v>25.4</v>
+      </c>
+      <c r="R70" s="27">
+        <v>22.4</v>
+      </c>
+      <c r="S70" s="27">
         <v>23.4</v>
       </c>
-      <c r="T67" s="27">
+      <c r="T70" s="27">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="68" spans="2:20">
-      <c r="B68" s="3" t="s">
+      <c r="AA70" s="27">
+        <f t="shared" si="28"/>
+        <v>21.4</v>
+      </c>
+      <c r="AB70" s="27">
+        <f t="shared" si="26"/>
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="71" spans="2:28">
+      <c r="B71" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="P68" s="27"/>
-      <c r="Q68" s="27"/>
-      <c r="R68" s="27"/>
-      <c r="S68" s="27">
+      <c r="N71" s="27">
         <v>0</v>
       </c>
-      <c r="T68" s="27">
+      <c r="P71" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="27">
+        <v>0</v>
+      </c>
+      <c r="R71" s="27">
+        <v>0</v>
+      </c>
+      <c r="S71" s="27">
+        <v>0</v>
+      </c>
+      <c r="T71" s="27">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="69" spans="2:20">
-      <c r="B69" s="3" t="s">
+      <c r="AA71" s="27">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AB71" s="27">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:28">
+      <c r="B72" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Q69" s="27"/>
-      <c r="R69" s="27"/>
-      <c r="S69" s="27">
+      <c r="N72" s="27">
+        <v>104.6</v>
+      </c>
+      <c r="P72" s="27">
+        <v>99.9</v>
+      </c>
+      <c r="Q72" s="27">
+        <v>77</v>
+      </c>
+      <c r="R72" s="27">
+        <v>97.6</v>
+      </c>
+      <c r="S72" s="27">
         <v>22.8</v>
       </c>
-      <c r="T69" s="27">
+      <c r="T72" s="27">
         <v>23.3</v>
       </c>
-    </row>
-    <row r="70" spans="2:20">
-      <c r="B70" s="3" t="s">
+      <c r="AA72" s="27">
+        <f t="shared" si="28"/>
+        <v>104.6</v>
+      </c>
+      <c r="AB72" s="27">
+        <f t="shared" si="26"/>
+        <v>97.6</v>
+      </c>
+    </row>
+    <row r="73" spans="2:28">
+      <c r="B73" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="P70" s="27"/>
-      <c r="Q70" s="27"/>
-      <c r="R70" s="27"/>
-      <c r="S70" s="27">
+      <c r="N73" s="27">
+        <v>120.7</v>
+      </c>
+      <c r="P73" s="27">
+        <v>126.9</v>
+      </c>
+      <c r="Q73" s="27">
+        <v>121.2</v>
+      </c>
+      <c r="R73" s="27">
+        <v>125.6</v>
+      </c>
+      <c r="S73" s="27">
         <v>142.9</v>
       </c>
-      <c r="T70" s="27">
+      <c r="T73" s="27">
         <v>165</v>
       </c>
-    </row>
-    <row r="71" spans="2:20">
-      <c r="B71" s="3" t="s">
+      <c r="AA73" s="27">
+        <f t="shared" si="28"/>
+        <v>120.7</v>
+      </c>
+      <c r="AB73" s="27">
+        <f t="shared" si="26"/>
+        <v>125.6</v>
+      </c>
+    </row>
+    <row r="74" spans="2:28">
+      <c r="B74" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="P71" s="27"/>
-      <c r="Q71" s="27"/>
-      <c r="R71" s="27"/>
-      <c r="S71" s="27">
+      <c r="N74" s="27">
+        <v>5.2</v>
+      </c>
+      <c r="P74" s="27">
+        <v>6.1</v>
+      </c>
+      <c r="Q74" s="27">
+        <v>6.6</v>
+      </c>
+      <c r="R74" s="27">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S74" s="27">
         <v>6.9</v>
       </c>
-      <c r="T71" s="27">
+      <c r="T74" s="27">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="72" spans="2:20">
-      <c r="B72" s="3" t="s">
+      <c r="AA74" s="27">
+        <f t="shared" si="28"/>
+        <v>5.2</v>
+      </c>
+      <c r="AB74" s="27">
+        <f t="shared" si="26"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="2:28">
+      <c r="B75" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="P72" s="27"/>
-      <c r="Q72" s="27"/>
-      <c r="R72" s="27"/>
-      <c r="S72" s="27">
+      <c r="N75" s="27">
+        <v>1956</v>
+      </c>
+      <c r="P75" s="27">
+        <v>1913.1</v>
+      </c>
+      <c r="Q75" s="27">
+        <v>1902</v>
+      </c>
+      <c r="R75" s="27">
+        <v>1687.6</v>
+      </c>
+      <c r="S75" s="27">
         <v>1679.3</v>
       </c>
-      <c r="T72" s="27">
+      <c r="T75" s="27">
         <v>1652.5</v>
       </c>
-    </row>
-    <row r="73" spans="2:20">
-      <c r="B73" s="3" t="s">
+      <c r="AA75" s="27">
+        <f t="shared" si="28"/>
+        <v>1956</v>
+      </c>
+      <c r="AB75" s="27">
+        <f t="shared" si="26"/>
+        <v>1687.6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:28">
+      <c r="B76" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="P73" s="27"/>
-      <c r="Q73" s="27"/>
-      <c r="R73" s="27"/>
-      <c r="S73" s="27">
+      <c r="N76" s="27">
+        <v>2075.6</v>
+      </c>
+      <c r="P76" s="27">
+        <v>2097.6999999999998</v>
+      </c>
+      <c r="Q76" s="27">
+        <v>2115.9</v>
+      </c>
+      <c r="R76" s="27">
+        <v>2213.4</v>
+      </c>
+      <c r="S76" s="27">
         <v>2227.5</v>
       </c>
-      <c r="T73" s="27">
+      <c r="T76" s="27">
         <v>2231.3000000000002</v>
       </c>
-    </row>
-    <row r="74" spans="2:20">
-      <c r="B74" s="3" t="s">
+      <c r="AA76" s="27">
+        <f t="shared" si="28"/>
+        <v>2075.6</v>
+      </c>
+      <c r="AB76" s="27">
+        <f t="shared" si="26"/>
+        <v>2213.4</v>
+      </c>
+    </row>
+    <row r="77" spans="2:28">
+      <c r="B77" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="P74" s="27"/>
-      <c r="Q74" s="27"/>
-      <c r="R74" s="27"/>
-      <c r="S74" s="27">
+      <c r="N77" s="27">
+        <v>62.3</v>
+      </c>
+      <c r="P77" s="27">
+        <v>55.8</v>
+      </c>
+      <c r="Q77" s="27">
+        <v>60.8</v>
+      </c>
+      <c r="R77" s="27">
+        <v>60.2</v>
+      </c>
+      <c r="S77" s="27">
         <v>55.9</v>
       </c>
-      <c r="T74" s="27">
+      <c r="T77" s="27">
         <v>59.5</v>
       </c>
-    </row>
-    <row r="75" spans="2:20">
-      <c r="B75" s="3" t="s">
+      <c r="AA77" s="27">
+        <f>N77</f>
+        <v>62.3</v>
+      </c>
+      <c r="AB77" s="27">
+        <f t="shared" si="26"/>
+        <v>60.2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28">
+      <c r="B78" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="P75" s="27"/>
-      <c r="Q75" s="27"/>
-      <c r="R75" s="27"/>
-      <c r="S75" s="27">
-        <f>SUM(S64:S74)+S63</f>
+      <c r="N78" s="27">
+        <f>SUM(N66:N77)+N65</f>
+        <v>10516</v>
+      </c>
+      <c r="P78" s="27">
+        <f>SUM(P66:P77)+P65</f>
+        <v>10341.299999999999</v>
+      </c>
+      <c r="Q78" s="27">
+        <f>SUM(Q66:Q77)+Q65</f>
+        <v>10382.700000000001</v>
+      </c>
+      <c r="R78" s="27">
+        <f>SUM(R66:R77)+R65</f>
+        <v>10155</v>
+      </c>
+      <c r="S78" s="27">
+        <f>SUM(S66:S77)+S65</f>
         <v>9868.4</v>
       </c>
-      <c r="T75" s="27">
-        <f>SUM(T64:T74)+T63</f>
+      <c r="T78" s="27">
+        <f>SUM(T66:T77)+T65</f>
         <v>9698.7999999999993</v>
       </c>
-    </row>
-    <row r="76" spans="2:20">
-      <c r="P76" s="27"/>
-      <c r="Q76" s="27"/>
-      <c r="R76" s="27"/>
-      <c r="S76" s="27"/>
-      <c r="T76" s="27"/>
-    </row>
-    <row r="77" spans="2:20">
-      <c r="B77" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="P77" s="27"/>
-      <c r="Q77" s="27"/>
-      <c r="R77" s="27"/>
-      <c r="S77" s="27">
-        <v>562.70000000000005</v>
-      </c>
-      <c r="T77" s="27">
-        <v>727.4</v>
-      </c>
-    </row>
-    <row r="78" spans="2:20">
-      <c r="B78" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="P78" s="27"/>
-      <c r="Q78" s="27"/>
-      <c r="R78" s="27"/>
-      <c r="S78" s="27">
-        <v>14.1</v>
-      </c>
-      <c r="T78" s="27">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="79" spans="2:20">
-      <c r="B79" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="AA78" s="27">
+        <f>SUM(AA66:AA77)+AA65</f>
+        <v>10516</v>
+      </c>
+      <c r="AB78" s="27">
+        <f>SUM(AB66:AB77)+AB65</f>
+        <v>10155</v>
+      </c>
+    </row>
+    <row r="79" spans="2:28">
       <c r="P79" s="27"/>
       <c r="Q79" s="27"/>
       <c r="R79" s="27"/>
-      <c r="S79" s="27">
+      <c r="S79" s="27"/>
+      <c r="T79" s="27"/>
+    </row>
+    <row r="80" spans="2:28">
+      <c r="B80" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="N80" s="27">
+        <v>502.3</v>
+      </c>
+      <c r="P80" s="27">
+        <v>515.4</v>
+      </c>
+      <c r="Q80" s="27">
+        <v>548.79999999999995</v>
+      </c>
+      <c r="R80" s="27">
+        <v>495.2</v>
+      </c>
+      <c r="S80" s="27">
+        <v>562.70000000000005</v>
+      </c>
+      <c r="T80" s="27">
+        <v>727.4</v>
+      </c>
+      <c r="AA80" s="27">
+        <f>N80</f>
+        <v>502.3</v>
+      </c>
+      <c r="AB80" s="27">
+        <f>R80</f>
+        <v>495.2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:28">
+      <c r="B81" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="N81" s="27">
+        <v>0</v>
+      </c>
+      <c r="P81" s="27">
+        <v>2</v>
+      </c>
+      <c r="Q81" s="27">
+        <v>6.5</v>
+      </c>
+      <c r="R81" s="27">
+        <v>14.8</v>
+      </c>
+      <c r="S81" s="27">
+        <v>14.1</v>
+      </c>
+      <c r="T81" s="27">
+        <v>12.3</v>
+      </c>
+      <c r="AA81" s="27">
+        <f t="shared" ref="AA81:AA93" si="29">N81</f>
+        <v>0</v>
+      </c>
+      <c r="AB81" s="27">
+        <f t="shared" ref="AB81:AB93" si="30">R81</f>
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="82" spans="2:28">
+      <c r="B82" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N82" s="27">
+        <v>11.4</v>
+      </c>
+      <c r="P82" s="27">
+        <v>10.8</v>
+      </c>
+      <c r="Q82" s="27">
+        <v>11.2</v>
+      </c>
+      <c r="R82" s="27">
+        <v>11.5</v>
+      </c>
+      <c r="S82" s="27">
         <v>11</v>
       </c>
-      <c r="T79" s="27">
+      <c r="T82" s="27">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="80" spans="2:20" s="2" customFormat="1">
-      <c r="B80" s="2" t="s">
+      <c r="AA82" s="27">
+        <f t="shared" si="29"/>
+        <v>11.4</v>
+      </c>
+      <c r="AB82" s="27">
+        <f t="shared" si="30"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="83" spans="2:28" s="2" customFormat="1">
+      <c r="B83" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="P80" s="26"/>
-      <c r="Q80" s="26"/>
-      <c r="R80" s="26"/>
-      <c r="S80" s="26">
+      <c r="N83" s="26">
+        <v>375.5</v>
+      </c>
+      <c r="P83" s="26">
+        <v>808.6</v>
+      </c>
+      <c r="Q83" s="26">
+        <v>783.8</v>
+      </c>
+      <c r="R83" s="26">
+        <v>574.20000000000005</v>
+      </c>
+      <c r="S83" s="26">
         <v>326.8</v>
       </c>
-      <c r="T80" s="26">
+      <c r="T83" s="26">
         <v>70.2</v>
       </c>
-    </row>
-    <row r="81" spans="2:20">
-      <c r="B81" s="3" t="s">
+      <c r="AA83" s="26">
+        <f>N83</f>
+        <v>375.5</v>
+      </c>
+      <c r="AB83" s="26">
+        <f>R83</f>
+        <v>574.20000000000005</v>
+      </c>
+    </row>
+    <row r="84" spans="2:28">
+      <c r="B84" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P81" s="27"/>
-      <c r="Q81" s="27"/>
-      <c r="R81" s="27"/>
-      <c r="S81" s="27">
+      <c r="N84" s="27">
+        <v>249.9</v>
+      </c>
+      <c r="P84" s="27">
+        <v>251.8</v>
+      </c>
+      <c r="Q84" s="27">
+        <v>283.89999999999998</v>
+      </c>
+      <c r="R84" s="27">
+        <v>241.3</v>
+      </c>
+      <c r="S84" s="27">
         <v>263.3</v>
       </c>
-      <c r="T81" s="27">
+      <c r="T84" s="27">
         <v>258.8</v>
       </c>
-    </row>
-    <row r="82" spans="2:20">
-      <c r="B82" s="3" t="s">
+      <c r="AA84" s="27">
+        <f t="shared" si="29"/>
+        <v>249.9</v>
+      </c>
+      <c r="AB84" s="27">
+        <f t="shared" si="30"/>
+        <v>241.3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:28">
+      <c r="B85" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="27"/>
-      <c r="R82" s="27"/>
-      <c r="S82" s="27">
+      <c r="N85" s="27">
+        <v>1033</v>
+      </c>
+      <c r="P85" s="27">
+        <v>991.7</v>
+      </c>
+      <c r="Q85" s="27">
+        <v>1041.4000000000001</v>
+      </c>
+      <c r="R85" s="27">
+        <v>1204.5999999999999</v>
+      </c>
+      <c r="S85" s="27">
         <v>1301.8</v>
       </c>
-      <c r="T82" s="27">
+      <c r="T85" s="27">
         <v>1317.8</v>
       </c>
-    </row>
-    <row r="83" spans="2:20" s="2" customFormat="1">
-      <c r="B83" s="2" t="s">
+      <c r="AA85" s="27">
+        <f t="shared" si="29"/>
+        <v>1033</v>
+      </c>
+      <c r="AB85" s="27">
+        <f t="shared" si="30"/>
+        <v>1204.5999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="2:28" s="2" customFormat="1">
+      <c r="B86" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P83" s="26"/>
-      <c r="Q83" s="26"/>
-      <c r="R83" s="26"/>
-      <c r="S83" s="26">
+      <c r="N86" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="P86" s="26">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q86" s="26">
+        <v>2.8</v>
+      </c>
+      <c r="R86" s="26">
+        <v>2.9</v>
+      </c>
+      <c r="S86" s="26">
         <v>3.2</v>
       </c>
-      <c r="T83" s="26">
+      <c r="T86" s="26">
         <v>11</v>
       </c>
-    </row>
-    <row r="84" spans="2:20">
-      <c r="B84" s="3" t="s">
+      <c r="AA86" s="26">
+        <f>N86</f>
+        <v>1.2</v>
+      </c>
+      <c r="AB86" s="26">
+        <f>R86</f>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="87" spans="2:28">
+      <c r="B87" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="27"/>
-      <c r="R84" s="27"/>
-      <c r="S84" s="27">
+      <c r="N87" s="27">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="P87" s="27">
+        <v>44.3</v>
+      </c>
+      <c r="Q87" s="27">
         <v>38</v>
       </c>
-      <c r="T84" s="27">
+      <c r="R87" s="27">
+        <v>40.4</v>
+      </c>
+      <c r="S87" s="27">
+        <v>38</v>
+      </c>
+      <c r="T87" s="27">
         <v>37.1</v>
       </c>
-    </row>
-    <row r="85" spans="2:20">
-      <c r="B85" s="3" t="s">
+      <c r="AA87" s="27">
+        <f t="shared" si="29"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AB87" s="27">
+        <f t="shared" si="30"/>
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="88" spans="2:28">
+      <c r="B88" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="P85" s="27"/>
-      <c r="Q85" s="27"/>
-      <c r="R85" s="27"/>
-      <c r="S85" s="27">
+      <c r="N88" s="27">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="P88" s="27">
+        <v>73.5</v>
+      </c>
+      <c r="Q88" s="27">
+        <v>85.3</v>
+      </c>
+      <c r="R88" s="27">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="S88" s="27">
         <v>71.400000000000006</v>
       </c>
-      <c r="T85" s="27">
+      <c r="T88" s="27">
         <v>79.8</v>
       </c>
-    </row>
-    <row r="86" spans="2:20">
-      <c r="B86" s="3" t="s">
+      <c r="AA88" s="27">
+        <f t="shared" si="29"/>
+        <v>40.700000000000003</v>
+      </c>
+      <c r="AB88" s="27">
+        <f t="shared" si="30"/>
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="89" spans="2:28">
+      <c r="B89" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N89" s="27">
+        <v>42.6</v>
+      </c>
+      <c r="P89" s="27">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="Q89" s="27">
+        <v>34.1</v>
+      </c>
+      <c r="R89" s="27">
+        <v>15.8</v>
+      </c>
+      <c r="S89" s="27">
+        <v>0</v>
+      </c>
+      <c r="T89" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="27">
+        <f t="shared" si="29"/>
+        <v>42.6</v>
+      </c>
+      <c r="AB89" s="27">
+        <f t="shared" si="30"/>
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="90" spans="2:28">
+      <c r="B90" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="P86" s="27"/>
-      <c r="Q86" s="27"/>
-      <c r="R86" s="27"/>
-      <c r="S86" s="27">
+      <c r="N90" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="P90" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="Q90" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="R90" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="S90" s="27">
         <v>2.8</v>
       </c>
-      <c r="T86" s="27">
+      <c r="T90" s="27">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="87" spans="2:20">
-      <c r="B87" s="3" t="s">
+      <c r="AA90" s="27">
+        <f t="shared" si="29"/>
+        <v>0.5</v>
+      </c>
+      <c r="AB90" s="27">
+        <f t="shared" si="30"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="91" spans="2:28">
+      <c r="B91" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="P87" s="27"/>
-      <c r="Q87" s="27"/>
-      <c r="R87" s="27"/>
-      <c r="S87" s="27">
+      <c r="N91" s="27">
+        <v>98.5</v>
+      </c>
+      <c r="P91" s="27">
+        <v>113.54</v>
+      </c>
+      <c r="Q91" s="27">
+        <v>114.1</v>
+      </c>
+      <c r="R91" s="27">
+        <v>108.9</v>
+      </c>
+      <c r="S91" s="27">
         <v>113.8</v>
       </c>
-      <c r="T87" s="27">
+      <c r="T91" s="27">
         <v>111.8</v>
       </c>
-    </row>
-    <row r="88" spans="2:20">
-      <c r="B88" s="3" t="s">
+      <c r="AA91" s="27">
+        <f t="shared" si="29"/>
+        <v>98.5</v>
+      </c>
+      <c r="AB91" s="27">
+        <f t="shared" si="30"/>
+        <v>108.9</v>
+      </c>
+    </row>
+    <row r="92" spans="2:28">
+      <c r="B92" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="N92" s="27">
+        <v>1.2</v>
+      </c>
+      <c r="P92" s="27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q92" s="27">
+        <v>1.2</v>
+      </c>
+      <c r="R92" s="27">
+        <v>0</v>
+      </c>
+      <c r="S92" s="27">
+        <v>0</v>
+      </c>
+      <c r="T92" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA92" s="27">
+        <f t="shared" si="29"/>
+        <v>1.2</v>
+      </c>
+      <c r="AB92" s="27">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:28">
+      <c r="B93" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="P88" s="27"/>
-      <c r="Q88" s="27"/>
-      <c r="R88" s="27"/>
-      <c r="S88" s="3">
+      <c r="N93" s="27">
+        <v>0</v>
+      </c>
+      <c r="P93" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="27">
+        <v>0</v>
+      </c>
+      <c r="R93" s="27">
+        <v>45.1</v>
+      </c>
+      <c r="S93" s="3">
         <v>47.4</v>
       </c>
-      <c r="T88" s="27">
+      <c r="T93" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="2:20">
-      <c r="B89" s="3" t="s">
+      <c r="AA93" s="27">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AB93" s="27">
+        <f t="shared" si="30"/>
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:28">
+      <c r="B94" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P89" s="27">
-        <f>SUM(P77:P88)</f>
+      <c r="N94" s="27">
+        <f>SUM(N80:N93)</f>
+        <v>2428.6999999999998</v>
+      </c>
+      <c r="P94" s="27">
+        <f>SUM(P80:P93)</f>
+        <v>2856.2400000000002</v>
+      </c>
+      <c r="Q94" s="27">
+        <f>SUM(Q80:Q93)</f>
+        <v>2953.6</v>
+      </c>
+      <c r="R94" s="27">
+        <f>SUM(R80:R93)</f>
+        <v>2828.8</v>
+      </c>
+      <c r="S94" s="27">
+        <f>SUM(S80:S93)</f>
+        <v>2756.3</v>
+      </c>
+      <c r="T94" s="27">
+        <f>SUM(T80:T93)</f>
+        <v>2640.1000000000004</v>
+      </c>
+      <c r="AA94" s="27">
+        <f>SUM(AA80:AA93)</f>
+        <v>2428.6999999999998</v>
+      </c>
+      <c r="AB94" s="27">
+        <f>SUM(AB80:AB93)</f>
+        <v>2828.8</v>
+      </c>
+    </row>
+    <row r="95" spans="2:28">
+      <c r="B95" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N95" s="27">
+        <v>53.3</v>
+      </c>
+      <c r="P95" s="27">
+        <v>48.2</v>
+      </c>
+      <c r="Q95" s="27">
+        <v>52.9</v>
+      </c>
+      <c r="R95" s="27">
+        <v>52.3</v>
+      </c>
+      <c r="S95" s="27">
+        <v>49</v>
+      </c>
+      <c r="T95" s="27">
+        <v>52.6</v>
+      </c>
+      <c r="AA95" s="27">
+        <f>N95</f>
+        <v>53.3</v>
+      </c>
+      <c r="AB95" s="27">
+        <f>R95</f>
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="96" spans="2:28" s="2" customFormat="1">
+      <c r="B96" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N96" s="26">
+        <v>4072.5</v>
+      </c>
+      <c r="P96" s="26">
+        <v>3523.2</v>
+      </c>
+      <c r="Q96" s="26">
+        <v>3523.5</v>
+      </c>
+      <c r="R96" s="26">
+        <v>3452.7</v>
+      </c>
+      <c r="S96" s="26">
+        <v>3229</v>
+      </c>
+      <c r="T96" s="26">
+        <v>3092.7</v>
+      </c>
+      <c r="AA96" s="26">
+        <f>N96</f>
+        <v>4072.5</v>
+      </c>
+      <c r="AB96" s="26">
+        <f>R96</f>
+        <v>3452.7</v>
+      </c>
+    </row>
+    <row r="97" spans="2:28">
+      <c r="B97" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N97" s="27">
+        <v>42.3</v>
+      </c>
+      <c r="P97" s="27">
+        <v>44.9</v>
+      </c>
+      <c r="Q97" s="27">
+        <v>39.6</v>
+      </c>
+      <c r="R97" s="27">
+        <v>57.6</v>
+      </c>
+      <c r="S97" s="27">
+        <v>53.8</v>
+      </c>
+      <c r="T97" s="27">
+        <v>55.1</v>
+      </c>
+      <c r="AA97" s="27">
+        <f t="shared" ref="AA97:AA104" si="31">N97</f>
+        <v>42.3</v>
+      </c>
+      <c r="AB97" s="27">
+        <f t="shared" ref="AB97:AB104" si="32">R97</f>
+        <v>57.6</v>
+      </c>
+    </row>
+    <row r="98" spans="2:28">
+      <c r="B98" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N98" s="27">
+        <v>262.39999999999998</v>
+      </c>
+      <c r="P98" s="27">
+        <v>267.5</v>
+      </c>
+      <c r="Q98" s="27">
+        <v>324.8</v>
+      </c>
+      <c r="R98" s="27">
+        <v>308.7</v>
+      </c>
+      <c r="S98" s="27">
+        <v>454.8</v>
+      </c>
+      <c r="T98" s="27">
+        <v>478.5</v>
+      </c>
+      <c r="AA98" s="27">
+        <f t="shared" si="31"/>
+        <v>262.39999999999998</v>
+      </c>
+      <c r="AB98" s="27">
+        <f t="shared" si="32"/>
+        <v>308.7</v>
+      </c>
+    </row>
+    <row r="99" spans="2:28">
+      <c r="B99" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N99" s="27">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="P99" s="27">
+        <v>4.7</v>
+      </c>
+      <c r="Q99" s="27">
+        <v>3.6</v>
+      </c>
+      <c r="R99" s="27">
+        <v>3</v>
+      </c>
+      <c r="S99" s="27">
         <v>0</v>
       </c>
-      <c r="Q89" s="27"/>
-      <c r="R89" s="27"/>
-      <c r="S89" s="27">
-        <f>SUM(S77:S88)</f>
-        <v>2756.3</v>
-      </c>
-      <c r="T89" s="27">
-        <f>SUM(T77:T88)</f>
-        <v>2640.1000000000004</v>
-      </c>
-    </row>
-    <row r="90" spans="2:20">
-      <c r="B90" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="P90" s="27"/>
-      <c r="Q90" s="27"/>
-      <c r="R90" s="27"/>
-      <c r="S90" s="27">
-        <v>49</v>
-      </c>
-      <c r="T90" s="27">
-        <v>52.6</v>
-      </c>
-    </row>
-    <row r="91" spans="2:20" s="2" customFormat="1">
-      <c r="B91" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="P91" s="26"/>
-      <c r="Q91" s="26"/>
-      <c r="R91" s="26"/>
-      <c r="S91" s="26">
-        <v>3229</v>
-      </c>
-      <c r="T91" s="26">
-        <v>3092.7</v>
-      </c>
-    </row>
-    <row r="92" spans="2:20">
-      <c r="B92" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P92" s="27"/>
-      <c r="Q92" s="27"/>
-      <c r="R92" s="27"/>
-      <c r="S92" s="27">
-        <v>53.8</v>
-      </c>
-      <c r="T92" s="27">
-        <v>55.1</v>
-      </c>
-    </row>
-    <row r="93" spans="2:20">
-      <c r="B93" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P93" s="27"/>
-      <c r="Q93" s="27"/>
-      <c r="R93" s="27"/>
-      <c r="S93" s="27">
-        <v>454.8</v>
-      </c>
-      <c r="T93" s="27">
-        <v>478.5</v>
-      </c>
-    </row>
-    <row r="94" spans="2:20">
-      <c r="B94" s="3" t="s">
+      <c r="T99" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA99" s="27">
+        <f t="shared" si="31"/>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AB99" s="27">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:28">
+      <c r="B100" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="P94" s="27"/>
-      <c r="Q94" s="27"/>
-      <c r="R94" s="27"/>
-      <c r="S94" s="27">
+      <c r="N100" s="27">
+        <v>11.8</v>
+      </c>
+      <c r="P100" s="27">
+        <v>12.4</v>
+      </c>
+      <c r="Q100" s="27">
+        <v>10</v>
+      </c>
+      <c r="R100" s="27">
+        <v>10</v>
+      </c>
+      <c r="S100" s="27">
         <v>13</v>
       </c>
-      <c r="T94" s="27">
+      <c r="T100" s="27">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="95" spans="2:20">
-      <c r="B95" s="3" t="s">
+      <c r="AA100" s="27">
+        <f t="shared" si="31"/>
+        <v>11.8</v>
+      </c>
+      <c r="AB100" s="27">
+        <f t="shared" si="32"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="2:28">
+      <c r="B101" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P95" s="27"/>
-      <c r="Q95" s="27"/>
-      <c r="R95" s="27"/>
-      <c r="S95" s="27">
+      <c r="N101" s="27">
+        <v>474.7</v>
+      </c>
+      <c r="P101" s="27">
+        <v>444.8</v>
+      </c>
+      <c r="Q101" s="27">
+        <v>428.6</v>
+      </c>
+      <c r="R101" s="27">
+        <v>505.8</v>
+      </c>
+      <c r="S101" s="27">
         <v>376.1</v>
       </c>
-      <c r="T95" s="27">
+      <c r="T101" s="27">
         <v>334.4</v>
       </c>
-    </row>
-    <row r="96" spans="2:20">
-      <c r="B96" s="3" t="s">
+      <c r="AA101" s="27">
+        <f t="shared" si="31"/>
+        <v>474.7</v>
+      </c>
+      <c r="AB101" s="27">
+        <f t="shared" si="32"/>
+        <v>505.8</v>
+      </c>
+    </row>
+    <row r="102" spans="2:28">
+      <c r="B102" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N102" s="27">
+        <v>82.6</v>
+      </c>
+      <c r="P102" s="27">
+        <v>73.8</v>
+      </c>
+      <c r="Q102" s="27">
+        <v>63.1</v>
+      </c>
+      <c r="R102" s="27">
+        <v>2.9</v>
+      </c>
+      <c r="S102" s="27">
+        <v>0</v>
+      </c>
+      <c r="T102" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA102" s="27">
+        <f t="shared" si="31"/>
+        <v>82.6</v>
+      </c>
+      <c r="AB102" s="27">
+        <f t="shared" si="32"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="103" spans="2:28">
+      <c r="B103" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="P96" s="27"/>
-      <c r="Q96" s="27"/>
-      <c r="R96" s="27"/>
-      <c r="S96" s="27">
+      <c r="N103" s="27">
+        <v>57.3</v>
+      </c>
+      <c r="P103" s="27">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="Q103" s="27">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="R103" s="27">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="S103" s="27">
         <v>37.6</v>
       </c>
-      <c r="T96" s="27">
+      <c r="T103" s="27">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="97" spans="2:20">
-      <c r="B97" s="3" t="s">
+      <c r="AA103" s="27">
+        <f t="shared" si="31"/>
+        <v>57.3</v>
+      </c>
+      <c r="AB103" s="27">
+        <f t="shared" si="32"/>
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="2:28">
+      <c r="B104" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="P97" s="27"/>
-      <c r="Q97" s="27"/>
-      <c r="R97" s="27"/>
-      <c r="S97" s="27">
+      <c r="N104" s="27">
+        <v>114.2</v>
+      </c>
+      <c r="P104" s="27">
+        <v>112.3</v>
+      </c>
+      <c r="Q104" s="27">
+        <v>108.4</v>
+      </c>
+      <c r="R104" s="27">
+        <v>120.5</v>
+      </c>
+      <c r="S104" s="27">
         <v>141.9</v>
       </c>
-      <c r="T97" s="27">
+      <c r="T104" s="27">
         <v>133.4</v>
       </c>
-    </row>
-    <row r="98" spans="2:20">
-      <c r="B98" s="3" t="s">
+      <c r="AA104" s="27">
+        <f t="shared" si="31"/>
+        <v>114.2</v>
+      </c>
+      <c r="AB104" s="27">
+        <f t="shared" si="32"/>
+        <v>120.5</v>
+      </c>
+    </row>
+    <row r="105" spans="2:28">
+      <c r="B105" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="P98" s="27">
-        <f>SUM(P90:P97)+P89</f>
-        <v>0</v>
-      </c>
-      <c r="Q98" s="27"/>
-      <c r="R98" s="27"/>
-      <c r="S98" s="27">
-        <f>SUM(S90:S97)+S89</f>
+      <c r="N105" s="27">
+        <f>SUM(N95:N104)+N94</f>
+        <v>7608.5</v>
+      </c>
+      <c r="P105" s="27">
+        <f>SUM(P95:P104)+P94</f>
+        <v>7455.6400000000012</v>
+      </c>
+      <c r="Q105" s="27">
+        <f>SUM(Q95:Q104)+Q94</f>
+        <v>7574.5</v>
+      </c>
+      <c r="R105" s="27">
+        <f>SUM(R95:R104)+R94</f>
+        <v>7379.9999999999991</v>
+      </c>
+      <c r="S105" s="27">
+        <f>SUM(S95:S104)+S94</f>
         <v>7111.5000000000009</v>
       </c>
-      <c r="T98" s="27">
-        <f>SUM(T90:T97)+T89</f>
+      <c r="T105" s="27">
+        <f>SUM(T95:T104)+T94</f>
         <v>6826.0999999999995</v>
       </c>
-    </row>
-    <row r="99" spans="2:20">
-      <c r="P99" s="27"/>
-      <c r="Q99" s="27"/>
-      <c r="R99" s="27"/>
-      <c r="S99" s="27"/>
-      <c r="T99" s="27"/>
-    </row>
-    <row r="100" spans="2:20">
-      <c r="B100" s="3" t="s">
+      <c r="AA105" s="27">
+        <f>SUM(AA95:AA104)+AA94</f>
+        <v>7608.5</v>
+      </c>
+      <c r="AB105" s="27">
+        <f>SUM(AB95:AB104)+AB94</f>
+        <v>7379.9999999999991</v>
+      </c>
+    </row>
+    <row r="106" spans="2:28">
+      <c r="P106" s="27"/>
+      <c r="Q106" s="27"/>
+      <c r="R106" s="27"/>
+      <c r="S106" s="27"/>
+      <c r="T106" s="27"/>
+    </row>
+    <row r="107" spans="2:28">
+      <c r="B107" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="P100" s="27"/>
-      <c r="Q100" s="27"/>
-      <c r="R100" s="27"/>
-      <c r="S100" s="27">
+      <c r="N107" s="27">
+        <v>2907.5</v>
+      </c>
+      <c r="P107" s="27">
+        <v>2885.7</v>
+      </c>
+      <c r="Q107" s="27">
+        <v>2808.2</v>
+      </c>
+      <c r="R107" s="27">
+        <v>2775</v>
+      </c>
+      <c r="S107" s="27">
         <v>2756.9</v>
       </c>
-      <c r="T100" s="27">
+      <c r="T107" s="27">
         <v>2872.7</v>
       </c>
-    </row>
-    <row r="101" spans="2:20">
-      <c r="B101" s="3" t="s">
+      <c r="AA107" s="27">
+        <f>N107</f>
+        <v>2907.5</v>
+      </c>
+      <c r="AB107" s="27">
+        <f>R107</f>
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="108" spans="2:28">
+      <c r="B108" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="P101" s="27">
-        <f>P100+P98</f>
-        <v>0</v>
-      </c>
-      <c r="Q101" s="27"/>
-      <c r="R101" s="27"/>
-      <c r="S101" s="27">
-        <f>S100+S98</f>
+      <c r="N108" s="27">
+        <f>N107+N105</f>
+        <v>10516</v>
+      </c>
+      <c r="P108" s="27">
+        <f>P107+P105</f>
+        <v>10341.34</v>
+      </c>
+      <c r="Q108" s="27">
+        <f>Q107+Q105</f>
+        <v>10382.700000000001</v>
+      </c>
+      <c r="R108" s="27">
+        <f>R107+R105</f>
+        <v>10155</v>
+      </c>
+      <c r="S108" s="27">
+        <f>S107+S105</f>
         <v>9868.4000000000015</v>
       </c>
-      <c r="T101" s="27">
-        <f>T100+T98</f>
+      <c r="T108" s="27">
+        <f>T107+T105</f>
         <v>9698.7999999999993</v>
       </c>
-    </row>
-    <row r="103" spans="2:20">
-      <c r="B103" s="3" t="s">
+      <c r="AA108" s="27">
+        <f>AA107+AA105</f>
+        <v>10516</v>
+      </c>
+      <c r="AB108" s="27">
+        <f>AB107+AB105</f>
+        <v>10155</v>
+      </c>
+    </row>
+    <row r="110" spans="2:28">
+      <c r="B110" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="P103" s="27">
-        <f>P75-P98</f>
-        <v>0</v>
-      </c>
-      <c r="Q103" s="27"/>
-      <c r="R103" s="27"/>
-      <c r="S103" s="27">
-        <f>S75-S98</f>
+      <c r="N110" s="27">
+        <f t="shared" ref="N110" si="33">N78-N105</f>
+        <v>2907.5</v>
+      </c>
+      <c r="P110" s="27">
+        <f t="shared" ref="P110:Q110" si="34">P78-P105</f>
+        <v>2885.659999999998</v>
+      </c>
+      <c r="Q110" s="27">
+        <f t="shared" si="34"/>
+        <v>2808.2000000000007</v>
+      </c>
+      <c r="R110" s="27">
+        <f t="shared" ref="R110" si="35">R78-R105</f>
+        <v>2775.0000000000009</v>
+      </c>
+      <c r="S110" s="27">
+        <f>S78-S105</f>
         <v>2756.8999999999987</v>
       </c>
-      <c r="T103" s="27">
-        <f>T75-T98</f>
+      <c r="T110" s="27">
+        <f>T78-T105</f>
         <v>2872.7</v>
       </c>
-    </row>
-    <row r="104" spans="2:20">
-      <c r="B104" s="3" t="s">
+      <c r="AA110" s="27">
+        <f t="shared" ref="AA110:AB110" si="36">AA78-AA105</f>
+        <v>2907.5</v>
+      </c>
+      <c r="AB110" s="27">
+        <f>AB78-AB105</f>
+        <v>2775.0000000000009</v>
+      </c>
+    </row>
+    <row r="111" spans="2:28">
+      <c r="B111" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="S104" s="3">
-        <f>S103/S27</f>
+      <c r="N111" s="3">
+        <f t="shared" ref="N111:Q111" si="37">N110/N27</f>
+        <v>3.9493344199945666</v>
+      </c>
+      <c r="P111" s="3">
+        <f t="shared" si="37"/>
+        <v>3.9271366358192683</v>
+      </c>
+      <c r="Q111" s="3">
+        <f t="shared" si="37"/>
+        <v>3.821720195971694</v>
+      </c>
+      <c r="R111" s="3">
+        <f t="shared" ref="R111" si="38">R110/R27</f>
+        <v>3.7770518579011854</v>
+      </c>
+      <c r="S111" s="3">
+        <f>S110/S27</f>
         <v>3.7529267628641421</v>
       </c>
-      <c r="T104" s="3">
-        <f>T103/T27</f>
+      <c r="T111" s="3">
+        <f>T110/T27</f>
         <v>3.9105635720119789</v>
       </c>
-    </row>
-    <row r="106" spans="2:20" s="39" customFormat="1">
-      <c r="B106" s="39" t="s">
+      <c r="AA111" s="3">
+        <f t="shared" ref="AA111" si="39">AA110/AA27</f>
+        <v>3.9493344199945666</v>
+      </c>
+      <c r="AB111" s="3">
+        <f>AB110/AB27</f>
+        <v>3.7770518579011854</v>
+      </c>
+    </row>
+    <row r="113" spans="2:28" s="39" customFormat="1">
+      <c r="B113" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="S106" s="52">
-        <f>S53+S54+S64</f>
-        <v>2102.6</v>
-      </c>
-      <c r="T106" s="52">
-        <f>T53+T54+T64</f>
-        <v>1965</v>
-      </c>
-    </row>
-    <row r="107" spans="2:20" s="39" customFormat="1">
-      <c r="B107" s="39" t="s">
+      <c r="N113" s="52">
+        <f t="shared" ref="N113" si="40">N54+N55+N66+N68</f>
+        <v>2753.6</v>
+      </c>
+      <c r="P113" s="52">
+        <f t="shared" ref="P113:Q113" si="41">P54+P55+P66+P68</f>
+        <v>2514.3000000000002</v>
+      </c>
+      <c r="Q113" s="52">
+        <f t="shared" si="41"/>
+        <v>2503.6999999999998</v>
+      </c>
+      <c r="R113" s="52">
+        <f t="shared" ref="R113" si="42">R54+R55+R66+R68</f>
+        <v>2634.7</v>
+      </c>
+      <c r="S113" s="52">
+        <f t="shared" ref="S113:T113" si="43">S54+S55+S66+S68</f>
+        <v>2104.1999999999998</v>
+      </c>
+      <c r="T113" s="52">
+        <f>T54+T55+T66+T68</f>
+        <v>1968.2</v>
+      </c>
+      <c r="AA113" s="52">
+        <f t="shared" ref="AA113:AB113" si="44">AA54+AA55+AA66+AA68</f>
+        <v>2753.6</v>
+      </c>
+      <c r="AB113" s="52">
+        <f>AB54+AB55+AB66+AB68</f>
+        <v>2634.7</v>
+      </c>
+    </row>
+    <row r="114" spans="2:28" s="39" customFormat="1">
+      <c r="B114" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="S107" s="52">
-        <f>S80+S83+S91</f>
+      <c r="N114" s="52">
+        <f t="shared" ref="N114" si="45">N83+N86+N96</f>
+        <v>4449.2</v>
+      </c>
+      <c r="P114" s="52">
+        <f t="shared" ref="P114:Q114" si="46">P83+P86+P96</f>
+        <v>4334.0999999999995</v>
+      </c>
+      <c r="Q114" s="52">
+        <f t="shared" si="46"/>
+        <v>4310.1000000000004</v>
+      </c>
+      <c r="R114" s="52">
+        <f t="shared" ref="R114" si="47">R83+R86+R96</f>
+        <v>4029.7999999999997</v>
+      </c>
+      <c r="S114" s="52">
+        <f>S83+S86+S96</f>
         <v>3559</v>
       </c>
-      <c r="T107" s="52">
-        <f>T80+T83+T91</f>
+      <c r="T114" s="52">
+        <f>T83+T86+T96</f>
         <v>3173.8999999999996</v>
       </c>
-    </row>
-    <row r="108" spans="2:20">
-      <c r="B108" s="3" t="s">
+      <c r="AA114" s="52">
+        <f t="shared" ref="AA114:AB114" si="48">AA83+AA86+AA96</f>
+        <v>4449.2</v>
+      </c>
+      <c r="AB114" s="52">
+        <f>AB83+AB86+AB96</f>
+        <v>4029.7999999999997</v>
+      </c>
+    </row>
+    <row r="115" spans="2:28">
+      <c r="B115" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S108" s="27">
-        <f>S106-S107</f>
-        <v>-1456.4</v>
-      </c>
-      <c r="T108" s="27">
-        <f>T106-T107</f>
-        <v>-1208.8999999999996</v>
-      </c>
-    </row>
-    <row r="110" spans="2:20" s="2" customFormat="1">
-      <c r="B110" s="2" t="s">
+      <c r="N115" s="27">
+        <f t="shared" ref="N115:R115" si="49">N113-N114</f>
+        <v>-1695.6</v>
+      </c>
+      <c r="P115" s="27">
+        <f t="shared" si="49"/>
+        <v>-1819.7999999999993</v>
+      </c>
+      <c r="Q115" s="27">
+        <f t="shared" si="49"/>
+        <v>-1806.4000000000005</v>
+      </c>
+      <c r="R115" s="27">
+        <f t="shared" si="49"/>
+        <v>-1395.1</v>
+      </c>
+      <c r="S115" s="27">
+        <f>S113-S114</f>
+        <v>-1454.8000000000002</v>
+      </c>
+      <c r="T115" s="27">
+        <f>T113-T114</f>
+        <v>-1205.6999999999996</v>
+      </c>
+      <c r="AA115" s="27">
+        <f t="shared" ref="AA115" si="50">AA113-AA114</f>
+        <v>-1695.6</v>
+      </c>
+      <c r="AB115" s="27">
+        <f>AB113-AB114</f>
+        <v>-1395.1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:28" s="2" customFormat="1">
+      <c r="B117" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="111" spans="2:20">
-      <c r="B111" s="3" t="s">
+      <c r="Q117" s="34"/>
+      <c r="R117" s="34">
+        <f t="shared" ref="Q117:S117" si="51">R60/N60-1</f>
+        <v>-0.18536445301283899</v>
+      </c>
+      <c r="S117" s="34"/>
+      <c r="T117" s="34">
+        <f>T60/P60-1</f>
+        <v>3.36501079913607E-2</v>
+      </c>
+      <c r="AB117" s="34">
+        <f>AB60/AA60-1</f>
+        <v>-0.18536445301283899</v>
+      </c>
+    </row>
+    <row r="118" spans="2:28">
+      <c r="B118" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="T111" s="25">
-        <f>T59/S59-1</f>
+      <c r="Q118" s="25">
+        <f>Q60/P60-1</f>
+        <v>-4.3196544276458138E-3</v>
+      </c>
+      <c r="R118" s="25">
+        <f t="shared" ref="R118:T118" si="52">R60/Q60-1</f>
+        <v>-0.13839479392624732</v>
+      </c>
+      <c r="S118" s="25">
+        <f t="shared" si="52"/>
+        <v>0.11923464249748239</v>
+      </c>
+      <c r="T118" s="25">
+        <f>T60/S60-1</f>
         <v>7.6525103473096934E-2</v>
       </c>
-    </row>
-    <row r="113" spans="2:20">
-      <c r="B113" s="3" t="s">
+      <c r="AA118" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB118" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="120" spans="2:28">
+      <c r="B120" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="115" spans="2:20">
-      <c r="B115" s="3" t="s">
+    <row r="122" spans="2:28">
+      <c r="B122" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="M115" s="3">
+      <c r="M122" s="3">
         <v>4.41</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N122" s="3">
         <v>6.81</v>
       </c>
-      <c r="O115" s="3">
+      <c r="O122" s="3">
         <v>9.9600000000000009</v>
       </c>
-      <c r="P115" s="3">
+      <c r="P122" s="3">
         <v>15.14</v>
       </c>
-      <c r="Q115" s="27">
+      <c r="Q122" s="27">
         <v>17</v>
       </c>
-      <c r="R115" s="3">
+      <c r="R122" s="3">
         <v>13.9</v>
       </c>
-      <c r="S115" s="3">
+      <c r="S122" s="3">
         <v>12.61</v>
       </c>
-      <c r="T115" s="3">
+      <c r="T122" s="3">
         <v>8.7799999999999994</v>
       </c>
-    </row>
-    <row r="116" spans="2:20" s="27" customFormat="1">
-      <c r="B116" s="27" t="s">
+      <c r="AA122" s="3">
+        <f>N122</f>
+        <v>6.81</v>
+      </c>
+      <c r="AB122" s="3">
+        <f>R122</f>
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="123" spans="2:28" s="27" customFormat="1">
+      <c r="B123" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="M116" s="27">
-        <f t="shared" ref="M116:R116" si="16">M115*M27</f>
+      <c r="M123" s="27">
+        <f>M122*M27</f>
         <v>3246.6420000000003</v>
       </c>
-      <c r="N116" s="27">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="O116" s="27">
-        <f t="shared" si="16"/>
+      <c r="N123" s="27">
+        <f>N122*N27</f>
+        <v>5013.5219999999999</v>
+      </c>
+      <c r="O123" s="27">
+        <f>O122*O27</f>
         <v>7320.6</v>
       </c>
-      <c r="P116" s="27">
-        <f t="shared" si="16"/>
+      <c r="P123" s="27">
+        <f>P122*P27</f>
         <v>11124.871999999999</v>
       </c>
-      <c r="Q116" s="27">
-        <f t="shared" si="16"/>
+      <c r="Q123" s="27">
+        <f>Q122*Q27</f>
         <v>12491.599999999999</v>
       </c>
-      <c r="R116" s="27">
-        <f t="shared" si="16"/>
+      <c r="R123" s="27">
+        <f>R122*R27</f>
         <v>10212.330000000002</v>
       </c>
-      <c r="S116" s="27">
-        <f>S115*S27</f>
+      <c r="S123" s="27">
+        <f>S122*S27</f>
         <v>9263.3060000000005</v>
       </c>
-      <c r="T116" s="27">
-        <f>T115*T27</f>
+      <c r="T123" s="27">
+        <f>T122*T27</f>
         <v>6449.7879999999996</v>
       </c>
-    </row>
-    <row r="117" spans="2:20" s="27" customFormat="1">
-      <c r="B117" s="27" t="s">
+      <c r="AA123" s="27">
+        <f t="shared" ref="AA123" si="53">AA122*AA27</f>
+        <v>5013.5219999999999</v>
+      </c>
+      <c r="AB123" s="27">
+        <f>AB122*AB27</f>
+        <v>10212.330000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="2:28" s="27" customFormat="1">
+      <c r="B124" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M117" s="27">
-        <f t="shared" ref="M117:R117" si="17">M116-M108</f>
+      <c r="M124" s="27">
+        <f>M123-M115</f>
         <v>3246.6420000000003</v>
       </c>
-      <c r="N117" s="27">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="O117" s="27">
-        <f t="shared" si="17"/>
+      <c r="N124" s="27">
+        <f>N123-N115</f>
+        <v>6709.1219999999994</v>
+      </c>
+      <c r="O124" s="27">
+        <f>O123-O115</f>
         <v>7320.6</v>
       </c>
-      <c r="P117" s="27">
-        <f t="shared" si="17"/>
-        <v>11124.871999999999</v>
-      </c>
-      <c r="Q117" s="27">
-        <f t="shared" si="17"/>
-        <v>12491.599999999999</v>
-      </c>
-      <c r="R117" s="27">
-        <f t="shared" si="17"/>
-        <v>10212.330000000002</v>
-      </c>
-      <c r="S117" s="27">
-        <f>S116-S108</f>
-        <v>10719.706</v>
-      </c>
-      <c r="T117" s="27">
-        <f>T116-T108</f>
-        <v>7658.6879999999992</v>
-      </c>
-    </row>
-    <row r="119" spans="2:20">
-      <c r="B119" s="3" t="s">
+      <c r="P124" s="27">
+        <f>P123-P115</f>
+        <v>12944.671999999999</v>
+      </c>
+      <c r="Q124" s="27">
+        <f>Q123-Q115</f>
+        <v>14298</v>
+      </c>
+      <c r="R124" s="27">
+        <f>R123-R115</f>
+        <v>11607.430000000002</v>
+      </c>
+      <c r="S124" s="27">
+        <f>S123-S115</f>
+        <v>10718.106</v>
+      </c>
+      <c r="T124" s="27">
+        <f>T123-T115</f>
+        <v>7655.4879999999994</v>
+      </c>
+      <c r="AA124" s="27">
+        <f t="shared" ref="AA124" si="54">AA123-AA115</f>
+        <v>6709.1219999999994</v>
+      </c>
+      <c r="AB124" s="27">
+        <f>AB123-AB115</f>
+        <v>11607.430000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="2:28">
+      <c r="B126" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S119" s="57">
-        <f>-S115/S104</f>
-        <v>-3.3600442526025622</v>
-      </c>
-      <c r="T119" s="57">
-        <f>-T115/T104</f>
-        <v>-2.2452006822849584</v>
-      </c>
-    </row>
-    <row r="120" spans="2:20">
-      <c r="B120" s="3" t="s">
+      <c r="N126" s="57">
+        <f>N122/N111</f>
+        <v>1.7243411865864144</v>
+      </c>
+      <c r="P126" s="57">
+        <f>P122/P111</f>
+        <v>3.8552261874233302</v>
+      </c>
+      <c r="Q126" s="57">
+        <f>Q122/Q111</f>
+        <v>4.4482586710348251</v>
+      </c>
+      <c r="R126" s="57">
+        <f>R122/R111</f>
+        <v>3.6801189189189176</v>
+      </c>
+      <c r="S126" s="57">
+        <f>S122/S111</f>
+        <v>3.3600442526025622</v>
+      </c>
+      <c r="T126" s="57">
+        <f>T122/T111</f>
+        <v>2.2452006822849584</v>
+      </c>
+      <c r="AA126" s="57">
+        <f>AA122/AA111</f>
+        <v>1.7243411865864144</v>
+      </c>
+      <c r="AB126" s="57">
+        <f>AB122/AB111</f>
+        <v>3.6801189189189176</v>
+      </c>
+    </row>
+    <row r="127" spans="2:28">
+      <c r="B127" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="121" spans="2:20">
-      <c r="B121" s="3" t="s">
+      <c r="P127" s="57">
+        <f t="shared" ref="P127:S127" si="55">P122/SUM(M9:P9)</f>
+        <v>3.3363450053989726E-3</v>
+      </c>
+      <c r="Q127" s="57">
+        <f t="shared" si="55"/>
+        <v>3.5885419964958943E-3</v>
+      </c>
+      <c r="R127" s="57">
+        <f t="shared" si="55"/>
+        <v>3.3117316306108839E-3</v>
+      </c>
+      <c r="S127" s="57">
+        <f t="shared" si="55"/>
+        <v>3.1597674651698908E-3</v>
+      </c>
+      <c r="T127" s="57">
+        <f>T122/SUM(Q9:T9)</f>
+        <v>2.2633532687151986E-3</v>
+      </c>
+      <c r="AA127" s="57">
+        <f t="shared" ref="AA127:AB127" si="56">AA123/AA9</f>
+        <v>1.3294587786057119</v>
+      </c>
+      <c r="AB127" s="57">
+        <f>AB123/AB9</f>
+        <v>2.4331292290098165</v>
+      </c>
+    </row>
+    <row r="128" spans="2:28">
+      <c r="B128" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="P128" s="57">
+        <f t="shared" ref="P128:S128" si="57">P122/SUM(M26:P26)</f>
+        <v>-88.265429889576552</v>
+      </c>
+      <c r="Q128" s="57">
+        <f t="shared" si="57"/>
+        <v>-249.48613055071797</v>
+      </c>
+      <c r="R128" s="57">
+        <f t="shared" si="57"/>
+        <v>-228.62115367889854</v>
+      </c>
+      <c r="S128" s="57">
+        <f t="shared" si="57"/>
+        <v>697.1161832155442</v>
+      </c>
+      <c r="T128" s="57">
+        <f>T122/SUM(Q26:T26)</f>
+        <v>-16621.554193892349</v>
+      </c>
+      <c r="AA128" s="57">
+        <f>AA122/AA26</f>
+        <v>-6.8500095641481078</v>
+      </c>
+      <c r="AB128" s="57">
+        <f>AB122/AB26</f>
+        <v>-228.46375838926176</v>
       </c>
     </row>
   </sheetData>
@@ -4506,10 +6225,16 @@
     <hyperlink ref="T1" r:id="rId1" xr:uid="{680599EF-35E5-444E-BE52-11E2AAE328C4}"/>
     <hyperlink ref="S1" r:id="rId2" xr:uid="{93CDF7DF-1EA6-42CA-BCC8-DA2865B51A26}"/>
     <hyperlink ref="Q1" r:id="rId3" xr:uid="{9752E2CB-3CEF-4245-BFA9-C0218E68B8CA}"/>
+    <hyperlink ref="R1" r:id="rId4" xr:uid="{BA3118D8-58BD-4D30-9D14-69D83EF60AFC}"/>
+    <hyperlink ref="AB1" r:id="rId5" xr:uid="{F4157810-6A61-4ACC-AAA5-22475F0942B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <ignoredErrors>
+    <ignoredError sqref="AA65:AB65 AA94:AB94" formula="1"/>
+    <ignoredError sqref="P127:T127" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -4518,7 +6243,7 @@
   <dimension ref="C4:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4531,6 +6256,14 @@
         <v>177</v>
       </c>
     </row>
+    <row r="6" spans="3:4">
+      <c r="C6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
     <row r="7" spans="3:4">
       <c r="C7" s="3" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
Update $ERJ key events
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F149AB-BDA9-450C-911B-84BD9A776A2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0497BF-6311-4CED-A70D-51D71A467584}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="193">
   <si>
     <t>$ERJ</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Embraer confident with a deal offered to Croatia airlines to replace all existing 6 Dash-8 &amp; 7 A320 aircraft with E2 jet</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1001,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1014,24 +1035,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1520,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:X42"/>
+  <dimension ref="A2:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:H28"/>
+      <selection activeCell="G17" sqref="G17:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1578,7 +1581,7 @@
       </c>
       <c r="D6" s="18"/>
       <c r="G6" s="9">
-        <v>44470</v>
+        <v>44835</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>11</v>
@@ -1706,7 +1709,7 @@
         <v>Q222</v>
       </c>
       <c r="G10" s="9">
-        <v>44470</v>
+        <v>44835</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>29</v>
@@ -1808,8 +1811,12 @@
       <c r="X13" s="38"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="G14" s="10"/>
-      <c r="H14" s="37"/>
+      <c r="G14" s="9">
+        <v>44805</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>192</v>
+      </c>
       <c r="I14" s="37"/>
       <c r="J14" s="37"/>
       <c r="K14" s="37"/>
@@ -1859,10 +1866,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="65"/>
+      <c r="D16" s="67"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -1886,25 +1893,21 @@
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="G17" s="9">
-        <v>43922</v>
-      </c>
-      <c r="H17" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
+      <c r="D17" s="67"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="60"/>
       <c r="R17" s="38"/>
       <c r="U17" s="42"/>
       <c r="V17" s="37"/>
@@ -1913,21 +1916,19 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
       <c r="R18" s="38"/>
       <c r="U18" s="46" t="s">
         <v>139</v>
@@ -1938,22 +1939,20 @@
     </row>
     <row r="19" spans="2:24">
       <c r="B19" s="17"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="73"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="69"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="51" t="s">
-        <v>31</v>
-      </c>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="38"/>
       <c r="U19" s="45" t="s">
         <v>142</v>
       </c>
@@ -1963,16 +1962,16 @@
     </row>
     <row r="20" spans="2:24">
       <c r="G20" s="10"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="60"/>
       <c r="R20" s="38"/>
       <c r="U20" s="45" t="s">
         <v>141</v>
@@ -1983,16 +1982,16 @@
     </row>
     <row r="21" spans="2:24">
       <c r="G21" s="10"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
       <c r="R21" s="38"/>
       <c r="U21" s="45" t="s">
         <v>140</v>
@@ -2008,16 +2007,16 @@
       <c r="C22" s="62"/>
       <c r="D22" s="63"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="60"/>
       <c r="R22" s="38"/>
       <c r="U22" s="45" t="s">
         <v>157</v>
@@ -2030,21 +2029,21 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="65"/>
+      <c r="D23" s="67"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
       <c r="R23" s="38"/>
       <c r="U23" s="42"/>
       <c r="V23" s="37"/>
@@ -2055,12 +2054,16 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="64">
+      <c r="C24" s="66">
         <v>1969</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="37"/>
+      <c r="D24" s="67"/>
+      <c r="G24" s="9">
+        <v>43922</v>
+      </c>
+      <c r="H24" s="37" t="s">
+        <v>164</v>
+      </c>
       <c r="I24" s="37"/>
       <c r="J24" s="37"/>
       <c r="K24" s="37"/>
@@ -2080,13 +2083,11 @@
     </row>
     <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="65"/>
-      <c r="G25" s="9">
-        <v>43770</v>
-      </c>
-      <c r="H25" s="37" t="s">
-        <v>167</v>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="I25" s="37"/>
       <c r="J25" s="37"/>
@@ -2109,15 +2110,13 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="70">
+      <c r="C26" s="64">
         <f>'Financial Model'!T60</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="71"/>
+      <c r="D26" s="65"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="50" t="s">
-        <v>168</v>
-      </c>
+      <c r="H26" s="37"/>
       <c r="I26" s="37"/>
       <c r="J26" s="37"/>
       <c r="K26" s="37"/>
@@ -2127,7 +2126,9 @@
       <c r="O26" s="37"/>
       <c r="P26" s="37"/>
       <c r="Q26" s="37"/>
-      <c r="R26" s="38"/>
+      <c r="R26" s="51" t="s">
+        <v>31</v>
+      </c>
       <c r="U26" s="45" t="s">
         <v>145</v>
       </c>
@@ -2137,8 +2138,8 @@
     </row>
     <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="65"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="67"/>
       <c r="G27" s="10"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
@@ -2169,7 +2170,7 @@
         <v>44777</v>
       </c>
       <c r="G28" s="10"/>
-      <c r="H28" s="60"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="37"/>
       <c r="J28" s="37"/>
       <c r="K28" s="37"/>
@@ -2178,9 +2179,7 @@
       <c r="N28" s="37"/>
       <c r="O28" s="37"/>
       <c r="P28" s="37"/>
-      <c r="Q28" s="37" t="s">
-        <v>180</v>
-      </c>
+      <c r="Q28" s="37"/>
       <c r="R28" s="38"/>
       <c r="U28" s="45" t="s">
         <v>147</v>
@@ -2193,16 +2192,12 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="67"/>
-      <c r="G29" s="9">
-        <v>43586</v>
-      </c>
-      <c r="H29" s="60" t="s">
-        <v>166</v>
-      </c>
+      <c r="D29" s="73"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="37"/>
       <c r="J29" s="37"/>
       <c r="K29" s="37"/>
@@ -2262,8 +2257,12 @@
       </c>
       <c r="C32" s="62"/>
       <c r="D32" s="63"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="37"/>
+      <c r="G32" s="9">
+        <v>43770</v>
+      </c>
+      <c r="H32" s="37" t="s">
+        <v>167</v>
+      </c>
       <c r="I32" s="37"/>
       <c r="J32" s="37"/>
       <c r="K32" s="37"/>
@@ -2285,13 +2284,15 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="68">
+      <c r="C33" s="74">
         <f>C6/'Financial Model'!T111</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="69"/>
+      <c r="D33" s="75"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="37"/>
+      <c r="H33" s="50" t="s">
+        <v>168</v>
+      </c>
       <c r="I33" s="37"/>
       <c r="J33" s="37"/>
       <c r="K33" s="37"/>
@@ -2311,17 +2312,13 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="68">
+      <c r="C34" s="74">
         <f>C6/'Financial Model'!AB9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="69"/>
-      <c r="G34" s="9">
-        <v>43282</v>
-      </c>
-      <c r="H34" s="37" t="s">
-        <v>162</v>
-      </c>
+      <c r="D34" s="75"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="37"/>
       <c r="I34" s="37"/>
       <c r="J34" s="37"/>
       <c r="K34" s="37"/>
@@ -2341,15 +2338,13 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="74">
+      <c r="C35" s="70">
         <f>C6/'Financial Model'!AB26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="75"/>
+      <c r="D35" s="71"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="8" t="s">
-        <v>163</v>
-      </c>
+      <c r="H35" s="60"/>
       <c r="I35" s="37"/>
       <c r="J35" s="37"/>
       <c r="K35" s="37"/>
@@ -2358,26 +2353,42 @@
       <c r="N35" s="37"/>
       <c r="O35" s="37"/>
       <c r="P35" s="37"/>
-      <c r="Q35" s="37"/>
+      <c r="Q35" s="37" t="s">
+        <v>180</v>
+      </c>
       <c r="R35" s="38"/>
     </row>
     <row r="36" spans="2:24">
-      <c r="G36" s="11"/>
-      <c r="H36" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="36"/>
+      <c r="G36" s="9">
+        <v>43586</v>
+      </c>
+      <c r="H36" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37"/>
+      <c r="Q36" s="37"/>
+      <c r="R36" s="38"/>
     </row>
     <row r="37" spans="2:24">
+      <c r="G37" s="10"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="38"/>
       <c r="U37" s="61" t="s">
         <v>158</v>
       </c>
@@ -2386,6 +2397,18 @@
       <c r="X37" s="63"/>
     </row>
     <row r="38" spans="2:24">
+      <c r="G38" s="10"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
+      <c r="R38" s="38"/>
       <c r="U38" s="42" t="s">
         <v>159</v>
       </c>
@@ -2394,6 +2417,18 @@
       <c r="X38" s="38"/>
     </row>
     <row r="39" spans="2:24">
+      <c r="G39" s="10"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="38"/>
       <c r="U39" s="44" t="s">
         <v>160</v>
       </c>
@@ -2402,6 +2437,18 @@
       <c r="X39" s="38"/>
     </row>
     <row r="40" spans="2:24">
+      <c r="G40" s="10"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="37"/>
+      <c r="O40" s="37"/>
+      <c r="P40" s="37"/>
+      <c r="Q40" s="37"/>
+      <c r="R40" s="38"/>
       <c r="U40" s="44" t="s">
         <v>161</v>
       </c>
@@ -2410,19 +2457,72 @@
       <c r="X40" s="38"/>
     </row>
     <row r="41" spans="2:24">
+      <c r="G41" s="9">
+        <v>43282</v>
+      </c>
+      <c r="H41" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="37"/>
+      <c r="O41" s="37"/>
+      <c r="P41" s="37"/>
+      <c r="Q41" s="37"/>
+      <c r="R41" s="38"/>
       <c r="U41" s="42"/>
       <c r="V41" s="37"/>
       <c r="W41" s="37"/>
       <c r="X41" s="38"/>
     </row>
     <row r="42" spans="2:24">
+      <c r="G42" s="10"/>
+      <c r="H42" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
+      <c r="O42" s="37"/>
+      <c r="P42" s="37"/>
+      <c r="Q42" s="37"/>
+      <c r="R42" s="38"/>
       <c r="U42" s="43"/>
       <c r="V42" s="35"/>
       <c r="W42" s="35"/>
       <c r="X42" s="36"/>
     </row>
+    <row r="43" spans="2:24">
+      <c r="G43" s="11"/>
+      <c r="H43" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="36"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="B5:D5"/>
@@ -2436,23 +2536,17 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
     <hyperlink ref="H10" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C29:D29" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R19" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="R26" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H14" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3556,7 +3650,7 @@
         <v>67</v>
       </c>
       <c r="N31" s="25">
-        <f t="shared" ref="N31:P31" si="8">N9/M9-1</f>
+        <f t="shared" ref="N31:O31" si="8">N9/M9-1</f>
         <v>1.4270462633451957</v>
       </c>
       <c r="O31" s="25">
@@ -3593,7 +3687,7 @@
         <v>7.2228812442335658E-2</v>
       </c>
       <c r="N34" s="25">
-        <f t="shared" ref="N34:O34" si="10">N11/N9</f>
+        <f t="shared" ref="N34" si="10">N11/N9</f>
         <v>0.12077766916476598</v>
       </c>
       <c r="O34" s="25">
@@ -3638,7 +3732,7 @@
         <v>-4.9690259654672372E-2</v>
       </c>
       <c r="N35" s="25">
-        <f t="shared" ref="N35:O35" si="13">N18/N9</f>
+        <f t="shared" ref="N35" si="13">N18/N9</f>
         <v>5.6261540132507927E-2</v>
       </c>
       <c r="O35" s="25">
@@ -3683,7 +3777,7 @@
         <v>-0.15750626070910759</v>
       </c>
       <c r="N36" s="25">
-        <f t="shared" ref="N36:O36" si="16">N23/N9</f>
+        <f t="shared" ref="N36" si="16">N23/N9</f>
         <v>-2.9868578255674411E-3</v>
       </c>
       <c r="O36" s="25">
@@ -3728,7 +3822,7 @@
         <v>0.19582772543741597</v>
       </c>
       <c r="N37" s="25">
-        <f t="shared" ref="N37:O37" si="19">N22/N21</f>
+        <f t="shared" ref="N37" si="19">N22/N21</f>
         <v>1.4824561403508625</v>
       </c>
       <c r="O37" s="25">
@@ -3778,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" ref="O41:S41" si="22">P42+P48</f>
+        <f t="shared" ref="P41:S41" si="22">P42+P48</f>
         <v>34</v>
       </c>
       <c r="Q41" s="2">
@@ -4505,7 +4599,7 @@
         <v>1.5</v>
       </c>
       <c r="AA67" s="27">
-        <f t="shared" ref="AA67:AA77" si="28">N67</f>
+        <f t="shared" ref="AA67:AA76" si="28">N67</f>
         <v>0</v>
       </c>
       <c r="AB67" s="27">
@@ -5783,7 +5877,7 @@
         <v>2872.7</v>
       </c>
       <c r="AA110" s="27">
-        <f t="shared" ref="AA110:AB110" si="36">AA78-AA105</f>
+        <f t="shared" ref="AA110" si="36">AA78-AA105</f>
         <v>2907.5</v>
       </c>
       <c r="AB110" s="27">
@@ -5849,7 +5943,7 @@
         <v>2634.7</v>
       </c>
       <c r="S113" s="52">
-        <f t="shared" ref="S113:T113" si="43">S54+S55+S66+S68</f>
+        <f t="shared" ref="S113" si="43">S54+S55+S66+S68</f>
         <v>2104.1999999999998</v>
       </c>
       <c r="T113" s="52">
@@ -5857,7 +5951,7 @@
         <v>1968.2</v>
       </c>
       <c r="AA113" s="52">
-        <f t="shared" ref="AA113:AB113" si="44">AA54+AA55+AA66+AA68</f>
+        <f t="shared" ref="AA113" si="44">AA54+AA55+AA66+AA68</f>
         <v>2753.6</v>
       </c>
       <c r="AB113" s="52">
@@ -5894,7 +5988,7 @@
         <v>3173.8999999999996</v>
       </c>
       <c r="AA114" s="52">
-        <f t="shared" ref="AA114:AB114" si="48">AA83+AA86+AA96</f>
+        <f t="shared" ref="AA114" si="48">AA83+AA86+AA96</f>
         <v>4449.2</v>
       </c>
       <c r="AB114" s="52">
@@ -5945,7 +6039,7 @@
       </c>
       <c r="Q117" s="34"/>
       <c r="R117" s="34">
-        <f t="shared" ref="Q117:S117" si="51">R60/N60-1</f>
+        <f t="shared" ref="R117" si="51">R60/N60-1</f>
         <v>-0.18536445301283899</v>
       </c>
       <c r="S117" s="34"/>
@@ -5967,7 +6061,7 @@
         <v>-4.3196544276458138E-3</v>
       </c>
       <c r="R118" s="25">
-        <f t="shared" ref="R118:T118" si="52">R60/Q60-1</f>
+        <f t="shared" ref="R118:S118" si="52">R60/Q60-1</f>
         <v>-0.13839479392624732</v>
       </c>
       <c r="S118" s="25">
@@ -6032,39 +6126,39 @@
         <v>179</v>
       </c>
       <c r="M123" s="27">
-        <f>M122*M27</f>
+        <f t="shared" ref="M123:T123" si="53">M122*M27</f>
         <v>3246.6420000000003</v>
       </c>
       <c r="N123" s="27">
-        <f>N122*N27</f>
+        <f t="shared" si="53"/>
         <v>5013.5219999999999</v>
       </c>
       <c r="O123" s="27">
-        <f>O122*O27</f>
+        <f t="shared" si="53"/>
         <v>7320.6</v>
       </c>
       <c r="P123" s="27">
-        <f>P122*P27</f>
+        <f t="shared" si="53"/>
         <v>11124.871999999999</v>
       </c>
       <c r="Q123" s="27">
-        <f>Q122*Q27</f>
+        <f t="shared" si="53"/>
         <v>12491.599999999999</v>
       </c>
       <c r="R123" s="27">
-        <f>R122*R27</f>
+        <f t="shared" si="53"/>
         <v>10212.330000000002</v>
       </c>
       <c r="S123" s="27">
-        <f>S122*S27</f>
+        <f t="shared" si="53"/>
         <v>9263.3060000000005</v>
       </c>
       <c r="T123" s="27">
-        <f>T122*T27</f>
+        <f t="shared" si="53"/>
         <v>6449.7879999999996</v>
       </c>
       <c r="AA123" s="27">
-        <f t="shared" ref="AA123" si="53">AA122*AA27</f>
+        <f t="shared" ref="AA123" si="54">AA122*AA27</f>
         <v>5013.5219999999999</v>
       </c>
       <c r="AB123" s="27">
@@ -6077,39 +6171,39 @@
         <v>9</v>
       </c>
       <c r="M124" s="27">
-        <f>M123-M115</f>
+        <f t="shared" ref="M124:T124" si="55">M123-M115</f>
         <v>3246.6420000000003</v>
       </c>
       <c r="N124" s="27">
-        <f>N123-N115</f>
+        <f t="shared" si="55"/>
         <v>6709.1219999999994</v>
       </c>
       <c r="O124" s="27">
-        <f>O123-O115</f>
+        <f t="shared" si="55"/>
         <v>7320.6</v>
       </c>
       <c r="P124" s="27">
-        <f>P123-P115</f>
+        <f t="shared" si="55"/>
         <v>12944.671999999999</v>
       </c>
       <c r="Q124" s="27">
-        <f>Q123-Q115</f>
+        <f t="shared" si="55"/>
         <v>14298</v>
       </c>
       <c r="R124" s="27">
-        <f>R123-R115</f>
+        <f t="shared" si="55"/>
         <v>11607.430000000002</v>
       </c>
       <c r="S124" s="27">
-        <f>S123-S115</f>
+        <f t="shared" si="55"/>
         <v>10718.106</v>
       </c>
       <c r="T124" s="27">
-        <f>T123-T115</f>
+        <f t="shared" si="55"/>
         <v>7655.4879999999994</v>
       </c>
       <c r="AA124" s="27">
-        <f t="shared" ref="AA124" si="54">AA123-AA115</f>
+        <f t="shared" ref="AA124" si="56">AA123-AA115</f>
         <v>6709.1219999999994</v>
       </c>
       <c r="AB124" s="27">
@@ -6159,19 +6253,19 @@
         <v>27</v>
       </c>
       <c r="P127" s="57">
-        <f t="shared" ref="P127:S127" si="55">P122/SUM(M9:P9)</f>
+        <f t="shared" ref="P127:S127" si="57">P122/SUM(M9:P9)</f>
         <v>3.3363450053989726E-3</v>
       </c>
       <c r="Q127" s="57">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>3.5885419964958943E-3</v>
       </c>
       <c r="R127" s="57">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>3.3117316306108839E-3</v>
       </c>
       <c r="S127" s="57">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>3.1597674651698908E-3</v>
       </c>
       <c r="T127" s="57">
@@ -6179,7 +6273,7 @@
         <v>2.2633532687151986E-3</v>
       </c>
       <c r="AA127" s="57">
-        <f t="shared" ref="AA127:AB127" si="56">AA123/AA9</f>
+        <f t="shared" ref="AA127" si="58">AA123/AA9</f>
         <v>1.3294587786057119</v>
       </c>
       <c r="AB127" s="57">
@@ -6192,19 +6286,19 @@
         <v>28</v>
       </c>
       <c r="P128" s="57">
-        <f t="shared" ref="P128:S128" si="57">P122/SUM(M26:P26)</f>
+        <f t="shared" ref="P128:S128" si="59">P122/SUM(M26:P26)</f>
         <v>-88.265429889576552</v>
       </c>
       <c r="Q128" s="57">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>-249.48613055071797</v>
       </c>
       <c r="R128" s="57">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>-228.62115367889854</v>
       </c>
       <c r="S128" s="57">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>697.1161832155442</v>
       </c>
       <c r="T128" s="57">

</xml_diff>

<commit_message>
Add Y/Y delivery cells for FY18,19,20,21
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E6B591-717E-4589-BADE-21D54D452D48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5602D85D-E87A-4A05-82BC-AD45D4BA84C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="215">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1064,6 +1064,14 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1073,28 +1081,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1109,13 +1105,17 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1606,7 +1606,7 @@
   <dimension ref="A2:X44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1626,31 +1626,31 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65"/>
-      <c r="G5" s="63" t="s">
+      <c r="C5" s="68"/>
+      <c r="D5" s="69"/>
+      <c r="G5" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="65"/>
-      <c r="U5" s="63" t="s">
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="69"/>
+      <c r="U5" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="65"/>
+      <c r="V5" s="68"/>
+      <c r="W5" s="68"/>
+      <c r="X5" s="69"/>
     </row>
     <row r="6" spans="1:24">
       <c r="B6" s="4" t="s">
@@ -1915,11 +1915,11 @@
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="69"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -1946,10 +1946,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="73"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -1973,10 +1973,10 @@
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="73"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
@@ -2000,8 +2000,8 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="69"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="73"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
         <v>201</v>
@@ -2025,8 +2025,8 @@
     </row>
     <row r="19" spans="2:24">
       <c r="B19" s="17"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="71"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
       <c r="G19" s="10"/>
       <c r="H19" s="8" t="s">
         <v>202</v>
@@ -2093,11 +2093,11 @@
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="2:24">
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="69"/>
       <c r="G22" s="10"/>
       <c r="H22" s="60"/>
       <c r="I22" s="60"/>
@@ -2121,10 +2121,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="69"/>
+      <c r="D23" s="73"/>
       <c r="G23" s="9">
         <v>44743</v>
       </c>
@@ -2150,10 +2150,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="68">
+      <c r="C24" s="72">
         <v>1969</v>
       </c>
-      <c r="D24" s="69"/>
+      <c r="D24" s="73"/>
       <c r="G24" s="10"/>
       <c r="H24" s="8" t="s">
         <v>206</v>
@@ -2177,8 +2177,8 @@
     </row>
     <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="69"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="73"/>
       <c r="G25" s="10"/>
       <c r="H25" s="50" t="s">
         <v>207</v>
@@ -2204,11 +2204,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="66">
+      <c r="C26" s="78">
         <f>'Financial Model'!T66</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="67"/>
+      <c r="D26" s="79"/>
       <c r="G26" s="10"/>
       <c r="H26" s="60"/>
       <c r="I26" s="60"/>
@@ -2230,8 +2230,8 @@
     </row>
     <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="69"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="73"/>
       <c r="G27" s="9">
         <v>43922</v>
       </c>
@@ -2352,11 +2352,11 @@
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="2:24">
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="69"/>
       <c r="G32" s="9">
         <v>43770</v>
       </c>
@@ -2438,11 +2438,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="72">
+      <c r="C35" s="70">
         <f>C6/'Financial Model'!AB26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="73"/>
+      <c r="D35" s="71"/>
       <c r="G35" s="10"/>
       <c r="H35" s="60"/>
       <c r="I35" s="37"/>
@@ -2489,12 +2489,12 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="U37" s="63" t="s">
+      <c r="U37" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="V37" s="64"/>
-      <c r="W37" s="64"/>
-      <c r="X37" s="65"/>
+      <c r="V37" s="68"/>
+      <c r="W37" s="68"/>
+      <c r="X37" s="69"/>
     </row>
     <row r="38" spans="2:24">
       <c r="G38" s="10"/>
@@ -2632,13 +2632,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="B5:D5"/>
@@ -2652,6 +2645,13 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -2675,10 +2675,10 @@
   <dimension ref="B1:AL137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB55" sqref="Z55:AB55"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2877,6 +2877,9 @@
       <c r="L3" s="23">
         <v>44048</v>
       </c>
+      <c r="M3" s="23">
+        <v>44140</v>
+      </c>
       <c r="O3" s="23">
         <v>44315</v>
       </c>
@@ -4709,11 +4712,11 @@
         <f t="shared" si="17"/>
         <v>-9.8717381689517936E-2</v>
       </c>
-      <c r="Y30" s="78" t="s">
+      <c r="Y30" s="63" t="s">
         <v>191</v>
       </c>
       <c r="Z30" s="34">
-        <f t="shared" ref="Z30:AB30" si="18">Z9/Y9-1</f>
+        <f t="shared" ref="Z30:AA30" si="18">Z9/Y9-1</f>
         <v>7.7202184930291295E-2</v>
       </c>
       <c r="AA30" s="34">
@@ -4729,7 +4732,7 @@
       <c r="B31" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="78" t="s">
+      <c r="C31" s="63" t="s">
         <v>191</v>
       </c>
       <c r="F31" s="25">
@@ -4792,16 +4795,16 @@
         <f>T9/S9-1</f>
         <v>0.69562323181893837</v>
       </c>
-      <c r="Y31" s="78" t="s">
+      <c r="Y31" s="63" t="s">
         <v>191</v>
       </c>
-      <c r="Z31" s="78" t="s">
+      <c r="Z31" s="63" t="s">
         <v>191</v>
       </c>
-      <c r="AA31" s="78" t="s">
+      <c r="AA31" s="63" t="s">
         <v>191</v>
       </c>
-      <c r="AB31" s="78" t="s">
+      <c r="AB31" s="63" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4818,7 +4821,7 @@
         <v>0.18873458121280079</v>
       </c>
       <c r="F34" s="25">
-        <f t="shared" ref="F34:G34" si="31">F11/F9</f>
+        <f t="shared" ref="F34" si="31">F11/F9</f>
         <v>0.15398209236569266</v>
       </c>
       <c r="G34" s="25">
@@ -4878,7 +4881,7 @@
         <v>0.2289724212385906</v>
       </c>
       <c r="Y34" s="25">
-        <f t="shared" ref="Y34:AA34" si="38">Y11/Y9</f>
+        <f t="shared" ref="Y34:Z34" si="38">Y11/Y9</f>
         <v>0.15144643174064798</v>
       </c>
       <c r="Z34" s="25">
@@ -4907,7 +4910,7 @@
         <v>4.6838609505736171E-2</v>
       </c>
       <c r="F35" s="25">
-        <f t="shared" ref="F35:G35" si="41">F18/F9</f>
+        <f t="shared" ref="F35" si="41">F18/F9</f>
         <v>3.8878416588123597E-3</v>
       </c>
       <c r="G35" s="25">
@@ -4967,7 +4970,7 @@
         <v>6.5462753950338556E-2</v>
       </c>
       <c r="Y35" s="25">
-        <f t="shared" ref="Y35:AA35" si="48">Y18/Y9</f>
+        <f t="shared" ref="Y35:Z35" si="48">Y18/Y9</f>
         <v>6.9610143755792601E-3</v>
       </c>
       <c r="Z35" s="25">
@@ -4996,7 +4999,7 @@
         <v>-9.1434486327957032E-3</v>
       </c>
       <c r="F36" s="25">
-        <f t="shared" ref="F36:G36" si="51">F23/F9</f>
+        <f t="shared" ref="F36" si="51">F23/F9</f>
         <v>2.2384542884070799E-3</v>
       </c>
       <c r="G36" s="25">
@@ -5056,7 +5059,7 @@
         <v>7.2725488271665487E-2</v>
       </c>
       <c r="Y36" s="25">
-        <f t="shared" ref="Y36:AA36" si="58">Y23/Y9</f>
+        <f t="shared" ref="Y36:Z36" si="58">Y23/Y9</f>
         <v>-3.3759933742186117E-2</v>
       </c>
       <c r="Z36" s="25">
@@ -5085,7 +5088,7 @@
         <v>2.3417721518987515</v>
       </c>
       <c r="F37" s="25">
-        <f t="shared" ref="F37:G37" si="61">F22/F21</f>
+        <f t="shared" ref="F37" si="61">F22/F21</f>
         <v>1.255033557046968</v>
       </c>
       <c r="G37" s="25">
@@ -5145,7 +5148,7 @@
         <v>-0.49696969696969745</v>
       </c>
       <c r="Y37" s="25">
-        <f t="shared" ref="Y37:AA37" si="67">Y22/Y21</f>
+        <f t="shared" ref="Y37:Z37" si="67">Y22/Y21</f>
         <v>-0.25697503671071947</v>
       </c>
       <c r="Z37" s="25">
@@ -5336,7 +5339,7 @@
         <v>11</v>
       </c>
       <c r="Y42" s="40">
-        <f t="shared" ref="Y42:AA42" si="81">SUM(Y43:Y48)</f>
+        <f t="shared" ref="Y42:Z42" si="81">SUM(Y43:Y48)</f>
         <v>90</v>
       </c>
       <c r="Z42" s="40">
@@ -6094,161 +6097,176 @@
       <c r="B55" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="C55" s="81" t="s">
+      <c r="C55" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="D55" s="81" t="s">
+      <c r="D55" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="E55" s="81" t="s">
+      <c r="E55" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="F55" s="81" t="s">
+      <c r="F55" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="G55" s="80">
+      <c r="G55" s="65">
         <f t="shared" ref="G55:S55" si="89">G41/C41-1</f>
         <v>-0.12</v>
       </c>
-      <c r="H55" s="80">
+      <c r="H55" s="65">
         <f t="shared" si="89"/>
         <v>6.25E-2</v>
       </c>
-      <c r="I55" s="80">
+      <c r="I55" s="65">
         <f t="shared" si="89"/>
         <v>0.12820512820512819</v>
       </c>
-      <c r="J55" s="80">
+      <c r="J55" s="65">
         <f t="shared" si="89"/>
         <v>0.17391304347826098</v>
       </c>
-      <c r="K55" s="80">
+      <c r="K55" s="65">
         <f t="shared" si="89"/>
         <v>-0.36363636363636365</v>
       </c>
-      <c r="L55" s="80">
+      <c r="L55" s="65">
         <f t="shared" si="89"/>
         <v>-0.66666666666666674</v>
       </c>
-      <c r="M55" s="80">
+      <c r="M55" s="65">
         <f t="shared" si="89"/>
         <v>9.0909090909090828E-2</v>
       </c>
-      <c r="N55" s="80">
+      <c r="N55" s="65">
         <f t="shared" si="89"/>
         <v>-0.12345679012345678</v>
       </c>
-      <c r="O55" s="80">
+      <c r="O55" s="65">
         <f t="shared" si="89"/>
         <v>0.5714285714285714</v>
       </c>
-      <c r="P55" s="80">
+      <c r="P55" s="65">
         <f t="shared" si="89"/>
         <v>1</v>
       </c>
-      <c r="Q55" s="80">
+      <c r="Q55" s="65">
         <f t="shared" si="89"/>
         <v>-0.375</v>
       </c>
-      <c r="R55" s="80">
+      <c r="R55" s="65">
         <f t="shared" si="89"/>
         <v>-0.22535211267605637</v>
       </c>
-      <c r="S55" s="80">
+      <c r="S55" s="65">
         <f t="shared" si="89"/>
         <v>0.18181818181818188</v>
       </c>
-      <c r="T55" s="80">
+      <c r="T55" s="65">
         <f>T41/P41-1</f>
         <v>-5.8823529411764719E-2</v>
       </c>
-      <c r="Z55" s="80">
-        <f t="shared" ref="Z55:AB55" si="90">Z9/Y9-1</f>
-        <v>7.7202184930291295E-2</v>
-      </c>
-      <c r="AA55" s="80">
+      <c r="Y55" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z55" s="65">
+        <f t="shared" ref="Z55:AB55" si="90">Z41/Y41-1</f>
+        <v>0.11235955056179781</v>
+      </c>
+      <c r="AA55" s="65">
         <f t="shared" si="90"/>
-        <v>-0.30965108190239088</v>
-      </c>
-      <c r="AB55" s="80">
-        <f>AB9/AA9-1</f>
-        <v>0.11299090451062033</v>
+        <v>-0.34343434343434343</v>
+      </c>
+      <c r="AB55" s="65">
+        <f>AB41/AA41-1</f>
+        <v>8.4615384615384537E-2</v>
       </c>
     </row>
     <row r="56" spans="2:28" s="39" customFormat="1">
       <c r="B56" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="C56" s="81" t="s">
+      <c r="C56" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="D56" s="79">
+      <c r="D56" s="64">
         <f t="shared" ref="D56" si="91">D41/C41-1</f>
         <v>0.91999999999999993</v>
       </c>
-      <c r="E56" s="79">
+      <c r="E56" s="64">
         <f t="shared" ref="E56" si="92">E41/D41-1</f>
         <v>-0.1875</v>
       </c>
-      <c r="F56" s="79">
-        <f t="shared" ref="F56:T56" si="93">F41/E41-1</f>
+      <c r="F56" s="64">
+        <f t="shared" ref="F56:S56" si="93">F41/E41-1</f>
         <v>0.76923076923076916</v>
       </c>
-      <c r="G56" s="79">
+      <c r="G56" s="64">
         <f t="shared" si="93"/>
         <v>-0.6811594202898551</v>
       </c>
-      <c r="H56" s="79">
+      <c r="H56" s="64">
         <f t="shared" si="93"/>
         <v>1.3181818181818183</v>
       </c>
-      <c r="I56" s="79">
+      <c r="I56" s="64">
         <f t="shared" si="93"/>
         <v>-0.13725490196078427</v>
       </c>
-      <c r="J56" s="79">
+      <c r="J56" s="64">
         <f t="shared" si="93"/>
         <v>0.84090909090909083</v>
       </c>
-      <c r="K56" s="79">
+      <c r="K56" s="64">
         <f t="shared" si="93"/>
         <v>-0.8271604938271605</v>
       </c>
-      <c r="L56" s="79">
+      <c r="L56" s="64">
         <f t="shared" si="93"/>
         <v>0.21428571428571419</v>
       </c>
-      <c r="M56" s="79">
+      <c r="M56" s="64">
         <f t="shared" si="93"/>
         <v>1.8235294117647061</v>
       </c>
-      <c r="N56" s="79">
+      <c r="N56" s="64">
         <f t="shared" si="93"/>
         <v>0.47916666666666674</v>
       </c>
-      <c r="O56" s="79">
+      <c r="O56" s="64">
         <f t="shared" si="93"/>
         <v>-0.6901408450704225</v>
       </c>
-      <c r="P56" s="79">
+      <c r="P56" s="64">
         <f t="shared" si="93"/>
         <v>0.54545454545454541</v>
       </c>
-      <c r="Q56" s="79">
+      <c r="Q56" s="64">
         <f t="shared" si="93"/>
         <v>-0.11764705882352944</v>
       </c>
-      <c r="R56" s="79">
+      <c r="R56" s="64">
         <f t="shared" si="93"/>
         <v>0.83333333333333326</v>
       </c>
-      <c r="S56" s="79">
+      <c r="S56" s="64">
         <f t="shared" si="93"/>
         <v>-0.52727272727272734</v>
       </c>
-      <c r="T56" s="79">
+      <c r="T56" s="64">
         <f>T41/S41-1</f>
         <v>0.23076923076923084</v>
+      </c>
+      <c r="Y56" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z56" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA56" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB56" s="66" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="2:28">

</xml_diff>

<commit_message>
Add deliveries chart into Data Visualisation
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F0F54F-20ED-4A16-BA25-4397442B8E96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3258551-B508-4399-B4EC-03D4AC4BF04E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -1216,6 +1216,16 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1225,16 +1235,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1249,28 +1271,6 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1574,215 +1574,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F0ED-4DAE-9383-B6CA67C32BB6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Financial Model'!$C$1:$T$1</c:f>
-              <c:strCache>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>Q118</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Q218</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Q318</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Q418</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Q119</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Q219</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Q319</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Q419</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Q120</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Q220</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Q320</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Q420</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Q121</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Q221</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Q321</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Q421</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q122</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Q222</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Financial Model'!$C$1:$T$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F0ED-4DAE-9383-B6CA67C32BB6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1982,6 +1773,2426 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Deliveries</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Deliveries</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$43:$T$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Commercial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$44:$T$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Embraer 170</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$45:$T$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Embraer 175</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$46:$T$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Embraer 190</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$47:$T$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Embraer 195</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent6">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$48:$T$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Embraer 190-E2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$49:$T$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Embraer 195-E2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$50:$T$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Executive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$52:$T$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Light Jets</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$53:$T$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Medium Jets</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$54:$T$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Financial Model'!$B$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Large Jets</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Financial Model'!$C$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Financial Model'!$C$55:$T$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-910E-42D2-98AE-6E9E7558FBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1867229503"/>
+        <c:axId val="1865061199"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="8"/>
+                <c:order val="8"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Financial Model'!$B$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Financial Model'!$C$1:$T$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="18"/>
+                      <c:pt idx="0">
+                        <c:v>Q118</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Q218</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Q318</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Q418</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Q119</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Q219</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Q319</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Q419</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Q120</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Q220</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>Q320</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>Q420</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>Q121</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>Q221</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>Q321</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>Q421</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>Q122</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>Q222</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Financial Model'!$C$51:$T$51</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="18"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000C-910E-42D2-98AE-6E9E7558FBE8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1867229503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1865061199"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1865061199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1867229503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2022,7 +4233,596 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2747,15 +5547,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>437205</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>361005</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2777,6 +5577,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>561969</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{469B1363-D592-4AEB-ABD4-61C23E9D3B35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3105,35 +5943,35 @@
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="72"/>
-      <c r="G5" s="70" t="s">
+      <c r="C5" s="77"/>
+      <c r="D5" s="78"/>
+      <c r="G5" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="72"/>
-      <c r="U5" s="70" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="78"/>
+      <c r="U5" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="71"/>
-      <c r="W5" s="71"/>
-      <c r="X5" s="72"/>
-      <c r="AA5" s="85" t="s">
+      <c r="V5" s="77"/>
+      <c r="W5" s="77"/>
+      <c r="X5" s="78"/>
+      <c r="AA5" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="AB5" s="86"/>
+      <c r="AB5" s="75"/>
     </row>
     <row r="6" spans="1:28">
       <c r="B6" s="4" t="s">
@@ -3165,7 +6003,7 @@
       <c r="V6" s="37"/>
       <c r="W6" s="37"/>
       <c r="X6" s="38"/>
-      <c r="AA6" s="87" t="s">
+      <c r="AA6" s="70" t="s">
         <v>217</v>
       </c>
       <c r="AB6" s="38"/>
@@ -3201,7 +6039,7 @@
       <c r="V7" s="37"/>
       <c r="W7" s="37"/>
       <c r="X7" s="38"/>
-      <c r="AA7" s="87" t="s">
+      <c r="AA7" s="70" t="s">
         <v>218</v>
       </c>
       <c r="AB7" s="38"/>
@@ -3235,7 +6073,7 @@
       <c r="V8" s="37"/>
       <c r="W8" s="37"/>
       <c r="X8" s="38"/>
-      <c r="AA8" s="88" t="s">
+      <c r="AA8" s="71" t="s">
         <v>219</v>
       </c>
       <c r="AB8" s="36"/>
@@ -3410,11 +6248,11 @@
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="72"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="78"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -3441,10 +6279,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="76"/>
+      <c r="D16" s="82"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -3468,10 +6306,10 @@
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="76"/>
+      <c r="D17" s="82"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
@@ -3495,8 +6333,8 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="76"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="82"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
         <v>201</v>
@@ -3588,11 +6426,11 @@
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="2:24">
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="72"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="78"/>
       <c r="G22" s="10"/>
       <c r="H22" s="60"/>
       <c r="I22" s="60"/>
@@ -3616,10 +6454,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="81" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="76"/>
+      <c r="D23" s="82"/>
       <c r="G23" s="9">
         <v>44743</v>
       </c>
@@ -3645,10 +6483,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="75">
+      <c r="C24" s="81">
         <v>1969</v>
       </c>
-      <c r="D24" s="76"/>
+      <c r="D24" s="82"/>
       <c r="G24" s="10"/>
       <c r="H24" s="8" t="s">
         <v>206</v>
@@ -3672,8 +6510,8 @@
     </row>
     <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="76"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="82"/>
       <c r="G25" s="10"/>
       <c r="H25" s="50" t="s">
         <v>207</v>
@@ -3699,11 +6537,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="79">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="82"/>
+      <c r="D26" s="80"/>
       <c r="G26" s="10"/>
       <c r="H26" s="60"/>
       <c r="I26" s="60"/>
@@ -3725,8 +6563,8 @@
     </row>
     <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="76"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="82"/>
       <c r="G27" s="9">
         <v>43922</v>
       </c>
@@ -3785,10 +6623,10 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="78"/>
+      <c r="D29" s="88"/>
       <c r="G29" s="10"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
@@ -3847,11 +6685,11 @@
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="2:24">
-      <c r="B32" s="70" t="s">
+      <c r="B32" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="71"/>
-      <c r="D32" s="72"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="78"/>
       <c r="G32" s="9">
         <v>43770</v>
       </c>
@@ -3879,11 +6717,11 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="79">
+      <c r="C33" s="89">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="80"/>
+      <c r="D33" s="90"/>
       <c r="G33" s="10"/>
       <c r="H33" s="50" t="s">
         <v>168</v>
@@ -3907,11 +6745,11 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="79">
+      <c r="C34" s="89">
         <f>C6/'Financial Model'!AB9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="80"/>
+      <c r="D34" s="90"/>
       <c r="G34" s="10"/>
       <c r="H34" s="37"/>
       <c r="I34" s="37"/>
@@ -3933,11 +6771,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="73">
+      <c r="C35" s="85">
         <f>C6/'Financial Model'!AB26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="74"/>
+      <c r="D35" s="86"/>
       <c r="G35" s="10"/>
       <c r="H35" s="60"/>
       <c r="I35" s="37"/>
@@ -3984,12 +6822,12 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="U37" s="70" t="s">
+      <c r="U37" s="76" t="s">
         <v>158</v>
       </c>
-      <c r="V37" s="71"/>
-      <c r="W37" s="71"/>
-      <c r="X37" s="72"/>
+      <c r="V37" s="77"/>
+      <c r="W37" s="77"/>
+      <c r="X37" s="78"/>
     </row>
     <row r="38" spans="2:24">
       <c r="G38" s="10"/>
@@ -4127,6 +6965,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C26:D26"/>
@@ -4141,13 +6986,6 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -4171,10 +7009,10 @@
   <dimension ref="B1:AL141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C131" sqref="C131:F131"/>
+      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12060,7 +14898,7 @@
         <v>120</v>
       </c>
       <c r="C119" s="27">
-        <f t="shared" ref="C119:E119" si="119">C118+C116</f>
+        <f t="shared" ref="C119:D119" si="119">C118+C116</f>
         <v>11995.1</v>
       </c>
       <c r="D119" s="27">
@@ -12076,7 +14914,7 @@
         <v>11293.3</v>
       </c>
       <c r="G119" s="27">
-        <f t="shared" ref="G119:H119" si="121">G118+G116</f>
+        <f t="shared" ref="G119" si="121">G118+G116</f>
         <v>11185.5</v>
       </c>
       <c r="H119" s="27">
@@ -12160,7 +14998,7 @@
         <v>121</v>
       </c>
       <c r="C121" s="27">
-        <f t="shared" ref="C121:E121" si="123">C87-C116</f>
+        <f t="shared" ref="C121:D121" si="123">C87-C116</f>
         <v>4183.8999999999978</v>
       </c>
       <c r="D121" s="27">
@@ -12168,7 +15006,7 @@
         <v>3990.0999999999985</v>
       </c>
       <c r="E121" s="27">
-        <f t="shared" ref="E121:F121" si="124">E87-E116</f>
+        <f t="shared" ref="E121" si="124">E87-E116</f>
         <v>3969.7000000000007</v>
       </c>
       <c r="F121" s="27">
@@ -12249,7 +15087,7 @@
         <v>122</v>
       </c>
       <c r="C122" s="3">
-        <f t="shared" ref="C122:E122" si="133">C121/C27</f>
+        <f t="shared" ref="C122:D122" si="133">C121/C27</f>
         <v>5.705577526251191</v>
       </c>
       <c r="D122" s="3">
@@ -12257,7 +15095,7 @@
         <v>5.4398091342876596</v>
       </c>
       <c r="E122" s="3">
-        <f t="shared" ref="E122:F122" si="134">E121/E27</f>
+        <f t="shared" ref="E122" si="134">E121/E27</f>
         <v>5.4097846824747897</v>
       </c>
       <c r="F122" s="3">
@@ -12344,7 +15182,7 @@
         <v>6</v>
       </c>
       <c r="C124" s="52">
-        <f t="shared" ref="C124:E124" si="143">C61+C62+C74+C76</f>
+        <f t="shared" ref="C124:D124" si="143">C61+C62+C74+C76</f>
         <v>3435.7999999999997</v>
       </c>
       <c r="D124" s="52">
@@ -12352,7 +15190,7 @@
         <v>3346.5</v>
       </c>
       <c r="E124" s="52">
-        <f t="shared" ref="E124:F124" si="144">E61+E62+E74+E76</f>
+        <f t="shared" ref="E124" si="144">E61+E62+E74+E76</f>
         <v>3147.6</v>
       </c>
       <c r="F124" s="52">
@@ -12433,7 +15271,7 @@
         <v>7</v>
       </c>
       <c r="C125" s="52">
-        <f t="shared" ref="C125:E125" si="154">C92+C96+C106+C93+C107</f>
+        <f t="shared" ref="C125:D125" si="154">C92+C96+C106+C93+C107</f>
         <v>4559.1000000000004</v>
       </c>
       <c r="D125" s="52">
@@ -12441,7 +15279,7 @@
         <v>4452.8</v>
       </c>
       <c r="E125" s="52">
-        <f t="shared" ref="E125:F125" si="155">E92+E96+E106+E93+E107</f>
+        <f t="shared" ref="E125" si="155">E92+E96+E106+E93+E107</f>
         <v>4399.8</v>
       </c>
       <c r="F125" s="52">
@@ -12505,7 +15343,7 @@
         <v>3173.8999999999996</v>
       </c>
       <c r="Z125" s="52">
-        <f t="shared" ref="Z125:AA125" si="162">Z92+Z96+Z106+Z93+Z107</f>
+        <f t="shared" ref="Z125" si="162">Z92+Z96+Z106+Z93+Z107</f>
         <v>3414.4</v>
       </c>
       <c r="AA125" s="52">
@@ -12522,7 +15360,7 @@
         <v>8</v>
       </c>
       <c r="C126" s="27">
-        <f t="shared" ref="C126:E126" si="164">C124-C125</f>
+        <f t="shared" ref="C126:D126" si="164">C124-C125</f>
         <v>-1123.3000000000006</v>
       </c>
       <c r="D126" s="27">
@@ -12530,7 +15368,7 @@
         <v>-1106.3000000000002</v>
       </c>
       <c r="E126" s="27">
-        <f t="shared" ref="E126:F126" si="165">E124-E125</f>
+        <f t="shared" ref="E126" si="165">E124-E125</f>
         <v>-1252.2000000000003</v>
       </c>
       <c r="F126" s="27">
@@ -12679,7 +15517,7 @@
         <v>3.36501079913607E-2</v>
       </c>
       <c r="AA128" s="34">
-        <f t="shared" ref="AA128:AB128" si="182">AA68/Z68-1</f>
+        <f t="shared" ref="AA128" si="182">AA68/Z68-1</f>
         <v>2.2609060402684511E-2</v>
       </c>
       <c r="AB128" s="34">
@@ -12861,19 +15699,19 @@
       <c r="B133" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C133" s="90">
+      <c r="C133" s="73">
         <v>26</v>
       </c>
-      <c r="D133" s="90">
+      <c r="D133" s="73">
         <v>24.9</v>
       </c>
-      <c r="E133" s="90">
+      <c r="E133" s="73">
         <v>19.59</v>
       </c>
-      <c r="F133" s="90">
+      <c r="F133" s="73">
         <v>22.13</v>
       </c>
-      <c r="G133" s="90">
+      <c r="G133" s="73">
         <v>19.010000000000002</v>
       </c>
       <c r="H133" s="3">
@@ -12933,7 +15771,7 @@
         <v>179</v>
       </c>
       <c r="C134" s="27">
-        <f t="shared" ref="C134:H134" si="203">C133*C27</f>
+        <f t="shared" ref="C134:G134" si="203">C133*C27</f>
         <v>19065.8</v>
       </c>
       <c r="D134" s="27">
@@ -13022,7 +15860,7 @@
         <v>9</v>
       </c>
       <c r="C135" s="27">
-        <f t="shared" ref="C135:H135" si="209">C134-C126</f>
+        <f t="shared" ref="C135:G135" si="209">C134-C126</f>
         <v>20189.099999999999</v>
       </c>
       <c r="D135" s="27">
@@ -13111,7 +15949,7 @@
         <v>26</v>
       </c>
       <c r="C137" s="57">
-        <f t="shared" ref="C137:H137" si="215">C133/C122</f>
+        <f t="shared" ref="C137:G137" si="215">C133/C122</f>
         <v>4.5569444776404806</v>
       </c>
       <c r="D137" s="57">
@@ -13183,7 +16021,7 @@
         <v>2.2452006822849584</v>
       </c>
       <c r="Z137" s="57">
-        <f t="shared" ref="Z137:AA137" si="219">Z133/Z122</f>
+        <f t="shared" ref="Z137" si="219">Z133/Z122</f>
         <v>3.9679884357881914</v>
       </c>
       <c r="AA137" s="57">
@@ -13351,7 +16189,7 @@
         <v>-16621.554193892349</v>
       </c>
       <c r="Z139" s="57">
-        <f t="shared" ref="Z139:AA139" si="239">Z133/Z26</f>
+        <f t="shared" ref="Z139" si="239">Z133/Z26</f>
         <v>-44.501058020477807</v>
       </c>
       <c r="AA139" s="57">
@@ -13371,7 +16209,7 @@
         <v>191</v>
       </c>
       <c r="D141" s="25">
-        <f t="shared" ref="D141:T141" si="240">D15:D15/D9</f>
+        <f t="shared" ref="D141:S141" si="240">D15:D15/D9</f>
         <v>8.0382013529645847E-3</v>
       </c>
       <c r="E141" s="25">
@@ -13485,13 +16323,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="89"/>
+    <col min="1" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add deliveries to data visualisation
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3258551-B508-4399-B4EC-03D4AC4BF04E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09753C38-A2FE-43AB-B1CD-D9C4786D7195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -830,11 +830,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0\x"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000\x"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1067,7 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1220,12 +1221,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1235,28 +1230,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1271,6 +1254,25 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5923,7 +5925,7 @@
   <dimension ref="A2:AB44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5943,35 +5945,35 @@
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="78"/>
-      <c r="G5" s="76" t="s">
+      <c r="C5" s="75"/>
+      <c r="D5" s="76"/>
+      <c r="G5" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="78"/>
-      <c r="U5" s="76" t="s">
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="76"/>
+      <c r="U5" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="78"/>
-      <c r="AA5" s="74" t="s">
+      <c r="V5" s="75"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="76"/>
+      <c r="AA5" s="85" t="s">
         <v>216</v>
       </c>
-      <c r="AB5" s="75"/>
+      <c r="AB5" s="86"/>
     </row>
     <row r="6" spans="1:28">
       <c r="B6" s="4" t="s">
@@ -6248,11 +6250,11 @@
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="78"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="76"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -6279,10 +6281,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="81" t="s">
+      <c r="C16" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="82"/>
+      <c r="D16" s="80"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -6306,10 +6308,10 @@
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="82"/>
+      <c r="D17" s="80"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
@@ -6333,8 +6335,8 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="82"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="80"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
         <v>201</v>
@@ -6358,8 +6360,8 @@
     </row>
     <row r="19" spans="2:24">
       <c r="B19" s="17"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="84"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="90"/>
       <c r="G19" s="10"/>
       <c r="H19" s="8" t="s">
         <v>202</v>
@@ -6426,11 +6428,11 @@
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="2:24">
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
       <c r="G22" s="10"/>
       <c r="H22" s="60"/>
       <c r="I22" s="60"/>
@@ -6454,10 +6456,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="82"/>
+      <c r="D23" s="80"/>
       <c r="G23" s="9">
         <v>44743</v>
       </c>
@@ -6483,10 +6485,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="81">
+      <c r="C24" s="79">
         <v>1969</v>
       </c>
-      <c r="D24" s="82"/>
+      <c r="D24" s="80"/>
       <c r="G24" s="10"/>
       <c r="H24" s="8" t="s">
         <v>206</v>
@@ -6510,8 +6512,8 @@
     </row>
     <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="82"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="80"/>
       <c r="G25" s="10"/>
       <c r="H25" s="50" t="s">
         <v>207</v>
@@ -6537,11 +6539,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="79">
+      <c r="C26" s="87">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="80"/>
+      <c r="D26" s="88"/>
       <c r="G26" s="10"/>
       <c r="H26" s="60"/>
       <c r="I26" s="60"/>
@@ -6563,8 +6565,8 @@
     </row>
     <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="82"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="80"/>
       <c r="G27" s="9">
         <v>43922</v>
       </c>
@@ -6623,10 +6625,10 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="87" t="s">
+      <c r="C29" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="88"/>
+      <c r="D29" s="82"/>
       <c r="G29" s="10"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
@@ -6685,11 +6687,11 @@
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="2:24">
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="78"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="76"/>
       <c r="G32" s="9">
         <v>43770</v>
       </c>
@@ -6717,11 +6719,11 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="89">
+      <c r="C33" s="83">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="90"/>
+      <c r="D33" s="84"/>
       <c r="G33" s="10"/>
       <c r="H33" s="50" t="s">
         <v>168</v>
@@ -6745,11 +6747,11 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="89">
+      <c r="C34" s="83">
         <f>C6/'Financial Model'!AB9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="90"/>
+      <c r="D34" s="84"/>
       <c r="G34" s="10"/>
       <c r="H34" s="37"/>
       <c r="I34" s="37"/>
@@ -6771,11 +6773,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="85">
+      <c r="C35" s="77">
         <f>C6/'Financial Model'!AB26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="86"/>
+      <c r="D35" s="78"/>
       <c r="G35" s="10"/>
       <c r="H35" s="60"/>
       <c r="I35" s="37"/>
@@ -6822,12 +6824,12 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="U37" s="76" t="s">
+      <c r="U37" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="V37" s="77"/>
-      <c r="W37" s="77"/>
-      <c r="X37" s="78"/>
+      <c r="V37" s="75"/>
+      <c r="W37" s="75"/>
+      <c r="X37" s="76"/>
     </row>
     <row r="38" spans="2:24">
       <c r="G38" s="10"/>
@@ -6965,13 +6967,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C26:D26"/>
@@ -6986,6 +6981,13 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -7009,10 +7011,10 @@
   <dimension ref="B1:AL141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="L129" sqref="L129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -16052,55 +16054,55 @@
       <c r="G138" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="H138" s="57">
+      <c r="H138" s="91">
         <f t="shared" ref="H138" si="220">H133/SUM(E9:H9)</f>
         <v>3.9969163256834486E-3</v>
       </c>
-      <c r="I138" s="57">
+      <c r="I138" s="91">
         <f t="shared" ref="I138" si="221">I133/SUM(F9:I9)</f>
         <v>3.3988808322824725E-3</v>
       </c>
-      <c r="J138" s="57">
+      <c r="J138" s="91">
         <f t="shared" ref="J138" si="222">J133/SUM(G9:J9)</f>
         <v>3.5678980705158708E-3</v>
       </c>
-      <c r="K138" s="57">
+      <c r="K138" s="91">
         <f t="shared" ref="K138" si="223">K133/SUM(H9:K9)</f>
         <v>1.3692135555934837E-3</v>
       </c>
-      <c r="L138" s="57">
+      <c r="L138" s="91">
         <f t="shared" ref="L138" si="224">L133/SUM(I9:L9)</f>
         <v>1.3493997653217802E-3</v>
       </c>
-      <c r="M138" s="57">
+      <c r="M138" s="91">
         <f t="shared" ref="M138" si="225">M133/SUM(J9:M9)</f>
         <v>1.0984631479313523E-3</v>
       </c>
-      <c r="N138" s="57">
+      <c r="N138" s="91">
         <f t="shared" ref="N138" si="226">N133/SUM(K9:N9)</f>
         <v>1.8058391450770329E-3</v>
       </c>
-      <c r="O138" s="57">
+      <c r="O138" s="91">
         <f t="shared" ref="O138" si="227">O133/SUM(L9:O9)</f>
         <v>2.5249708462201492E-3</v>
       </c>
-      <c r="P138" s="57">
+      <c r="P138" s="91">
         <f t="shared" ref="P138:S138" si="228">P133/SUM(M9:P9)</f>
         <v>3.3363450053989726E-3</v>
       </c>
-      <c r="Q138" s="57">
+      <c r="Q138" s="91">
         <f t="shared" si="228"/>
         <v>3.5885419964958943E-3</v>
       </c>
-      <c r="R138" s="57">
+      <c r="R138" s="91">
         <f t="shared" si="228"/>
         <v>3.3117316306108839E-3</v>
       </c>
-      <c r="S138" s="57">
+      <c r="S138" s="91">
         <f t="shared" si="228"/>
         <v>3.1597674651698908E-3</v>
       </c>
-      <c r="T138" s="57">
+      <c r="T138" s="91">
         <f>T133/SUM(Q9:T9)</f>
         <v>2.2633532687151986E-3</v>
       </c>
@@ -16324,7 +16326,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Start data entry for commercial order & backlog data
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09753C38-A2FE-43AB-B1CD-D9C4786D7195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735B4BD-28AD-C941-B05F-4910276F46B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10500" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="3" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -122,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="217">
   <si>
     <t>$ERJ</t>
   </si>
@@ -697,9 +707,6 @@
     <t>Others</t>
   </si>
   <si>
-    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/0552e176-6b29-4f1c-820c-8020af5b31eb?origin=1</t>
-  </si>
-  <si>
     <t>Share Price</t>
   </si>
   <si>
@@ -709,12 +716,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/6180d10a-38ab-421f-9f8b-22fbb0bcd380?origin=1</t>
-  </si>
-  <si>
     <t>Embraer 190-E2</t>
   </si>
   <si>
@@ -730,12 +731,6 @@
     <t>Financial Guarantee &amp; Residual</t>
   </si>
   <si>
-    <t>Q4 21</t>
-  </si>
-  <si>
-    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1</t>
-  </si>
-  <si>
     <t>Embraer 190</t>
   </si>
   <si>
@@ -745,12 +740,6 @@
     <t>Embraer confident with a deal offered to Croatia airlines to replace all existing 6 Dash-8 &amp; 7 A320 aircraft with E2 jet</t>
   </si>
   <si>
-    <t>Q2 20</t>
-  </si>
-  <si>
-    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/1083816a-dedc-4569-947a-0418e30ccac3?origin=1</t>
-  </si>
-  <si>
     <t>Embraer 195</t>
   </si>
   <si>
@@ -760,12 +749,6 @@
     <t>Recourse &amp; Non-Recourse Debt</t>
   </si>
   <si>
-    <t>Q1 21</t>
-  </si>
-  <si>
-    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a30b7884-cd47-4bdd-bad3-db5809146933?origin=1</t>
-  </si>
-  <si>
     <t>"This may result in a steady flow of contracts from the Pentagon involving the upgraded KC-390"</t>
   </si>
   <si>
@@ -796,12 +779,6 @@
     <t>turboprops</t>
   </si>
   <si>
-    <t>Q3 19</t>
-  </si>
-  <si>
-    <t>https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/8307c88a-cbb3-4e54-9db4-f192e081992a?origin=1</t>
-  </si>
-  <si>
     <t>Embraer 170</t>
   </si>
   <si>
@@ -824,6 +801,30 @@
   </si>
   <si>
     <t>Prev FY data entry</t>
+  </si>
+  <si>
+    <t>FY17</t>
+  </si>
+  <si>
+    <t>Firm Orders</t>
+  </si>
+  <si>
+    <t>Firm Order Backlog</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>Firm Orders Y/Y</t>
+  </si>
+  <si>
+    <t>Firm Orders Q/Q</t>
+  </si>
+  <si>
+    <t>Firm Order Backlog Y/Y</t>
+  </si>
+  <si>
+    <t>Firm Order Backlog Q/Q</t>
   </si>
 </sst>
 </file>
@@ -835,9 +836,9 @@
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0\x"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0000\x"/>
+    <numFmt numFmtId="168" formatCode="0.0000\x"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -941,6 +942,42 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1068,7 +1105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1221,6 +1258,13 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1230,16 +1274,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1254,25 +1310,20 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1300,7 +1351,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1778,7 +1829,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5925,12 +5976,12 @@
   <dimension ref="A2:AB44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:28" ht="15">
@@ -5945,35 +5996,35 @@
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="76"/>
-      <c r="G5" s="74" t="s">
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="G5" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="76"/>
-      <c r="U5" s="74" t="s">
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="79"/>
+      <c r="U5" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="75"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="76"/>
-      <c r="AA5" s="85" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB5" s="86"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="79"/>
+      <c r="AA5" s="75" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB5" s="76"/>
     </row>
     <row r="6" spans="1:28">
       <c r="B6" s="4" t="s">
@@ -6006,7 +6057,7 @@
       <c r="W6" s="37"/>
       <c r="X6" s="38"/>
       <c r="AA6" s="70" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="AB6" s="38"/>
     </row>
@@ -6042,7 +6093,7 @@
       <c r="W7" s="37"/>
       <c r="X7" s="38"/>
       <c r="AA7" s="70" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="AB7" s="38"/>
     </row>
@@ -6076,7 +6127,7 @@
       <c r="W8" s="37"/>
       <c r="X8" s="38"/>
       <c r="AA8" s="71" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="AB8" s="36"/>
     </row>
@@ -6230,7 +6281,7 @@
         <v>44805</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I14" s="37"/>
       <c r="J14" s="37"/>
@@ -6250,11 +6301,11 @@
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="75"/>
-      <c r="D15" s="76"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="79"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -6281,10 +6332,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="79" t="s">
+      <c r="C16" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="80"/>
+      <c r="D16" s="83"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -6308,15 +6359,15 @@
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="80"/>
+      <c r="D17" s="83"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="I17" s="60"/>
       <c r="J17" s="60"/>
@@ -6335,11 +6386,11 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="80"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="83"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="I18" s="60"/>
       <c r="J18" s="60"/>
@@ -6360,11 +6411,11 @@
     </row>
     <row r="19" spans="2:24">
       <c r="B19" s="17"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="90"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="85"/>
       <c r="G19" s="10"/>
       <c r="H19" s="8" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="I19" s="60"/>
       <c r="J19" s="60"/>
@@ -6386,7 +6437,7 @@
     <row r="20" spans="2:24">
       <c r="G20" s="10"/>
       <c r="H20" s="8" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="I20" s="60"/>
       <c r="J20" s="60"/>
@@ -6398,7 +6449,7 @@
       <c r="P20" s="60"/>
       <c r="Q20" s="60"/>
       <c r="R20" s="51" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="U20" s="45" t="s">
         <v>141</v>
@@ -6428,11 +6479,11 @@
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="2:24">
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="75"/>
-      <c r="D22" s="76"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="79"/>
       <c r="G22" s="10"/>
       <c r="H22" s="60"/>
       <c r="I22" s="60"/>
@@ -6456,15 +6507,15 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="80"/>
+      <c r="D23" s="83"/>
       <c r="G23" s="9">
         <v>44743</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="I23" s="60"/>
       <c r="J23" s="60"/>
@@ -6485,13 +6536,13 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="79">
+      <c r="C24" s="82">
         <v>1969</v>
       </c>
-      <c r="D24" s="80"/>
+      <c r="D24" s="83"/>
       <c r="G24" s="10"/>
       <c r="H24" s="8" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="I24" s="60"/>
       <c r="J24" s="60"/>
@@ -6512,11 +6563,11 @@
     </row>
     <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="80"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="83"/>
       <c r="G25" s="10"/>
       <c r="H25" s="50" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I25" s="60"/>
       <c r="J25" s="60"/>
@@ -6539,11 +6590,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="87">
+      <c r="C26" s="80">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="88"/>
+      <c r="D26" s="81"/>
       <c r="G26" s="10"/>
       <c r="H26" s="60"/>
       <c r="I26" s="60"/>
@@ -6565,8 +6616,8 @@
     </row>
     <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="80"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="83"/>
       <c r="G27" s="9">
         <v>43922</v>
       </c>
@@ -6625,10 +6676,10 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="82"/>
+      <c r="D29" s="89"/>
       <c r="G29" s="10"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
@@ -6687,11 +6738,11 @@
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="2:24">
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="76"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="79"/>
       <c r="G32" s="9">
         <v>43770</v>
       </c>
@@ -6719,11 +6770,11 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="83">
+      <c r="C33" s="90">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="84"/>
+      <c r="D33" s="91"/>
       <c r="G33" s="10"/>
       <c r="H33" s="50" t="s">
         <v>168</v>
@@ -6747,11 +6798,11 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="83">
+      <c r="C34" s="90">
         <f>C6/'Financial Model'!AB9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="84"/>
+      <c r="D34" s="91"/>
       <c r="G34" s="10"/>
       <c r="H34" s="37"/>
       <c r="I34" s="37"/>
@@ -6773,11 +6824,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="77">
+      <c r="C35" s="86">
         <f>C6/'Financial Model'!AB26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="78"/>
+      <c r="D35" s="87"/>
       <c r="G35" s="10"/>
       <c r="H35" s="60"/>
       <c r="I35" s="37"/>
@@ -6789,7 +6840,7 @@
       <c r="O35" s="37"/>
       <c r="P35" s="37"/>
       <c r="Q35" s="37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R35" s="38"/>
     </row>
@@ -6824,12 +6875,12 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="U37" s="74" t="s">
+      <c r="U37" s="77" t="s">
         <v>158</v>
       </c>
-      <c r="V37" s="75"/>
-      <c r="W37" s="75"/>
-      <c r="X37" s="76"/>
+      <c r="V37" s="78"/>
+      <c r="W37" s="78"/>
+      <c r="X37" s="79"/>
     </row>
     <row r="38" spans="2:24">
       <c r="G38" s="10"/>
@@ -6929,7 +6980,7 @@
       <c r="Q42" s="37"/>
       <c r="R42" s="38"/>
       <c r="U42" s="61" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="V42" s="60"/>
       <c r="W42" s="60"/>
@@ -6951,7 +7002,7 @@
       <c r="Q43" s="35"/>
       <c r="R43" s="36"/>
       <c r="U43" s="61" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="V43" s="60"/>
       <c r="W43" s="60"/>
@@ -6967,6 +7018,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C26:D26"/>
@@ -6981,13 +7039,6 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -7010,20 +7061,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
   <dimension ref="B1:AL141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L129" sqref="L129"/>
+      <selection pane="bottomRight" activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="19" width="9.140625" style="3"/>
-    <col min="20" max="20" width="9.140625" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="30.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="19" width="9.1640625" style="3"/>
+    <col min="20" max="20" width="9.1640625" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:38" s="15" customFormat="1">
@@ -7090,6 +7141,9 @@
       <c r="V1" s="15" t="s">
         <v>76</v>
       </c>
+      <c r="X1" s="15" t="s">
+        <v>209</v>
+      </c>
       <c r="Y1" s="15" t="s">
         <v>77</v>
       </c>
@@ -9073,16 +9127,16 @@
         <v>66</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G30" s="34">
         <f t="shared" ref="G30:H30" si="15">G9/C9-1</f>
@@ -9141,7 +9195,7 @@
         <v>-9.8717381689517936E-2</v>
       </c>
       <c r="Y30" s="63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Z30" s="34">
         <f t="shared" ref="Z30:AA30" si="18">Z9/Y9-1</f>
@@ -9161,7 +9215,7 @@
         <v>67</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D31" s="25">
         <f t="shared" ref="D31" si="19">D9/C9-1</f>
@@ -9232,16 +9286,16 @@
         <v>0.69562323181893837</v>
       </c>
       <c r="Y31" s="63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Z31" s="63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="AA31" s="63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="AB31" s="63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="2:28" s="64" customFormat="1">
@@ -9249,7 +9303,7 @@
         <v>57</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D32" s="64">
         <f t="shared" ref="D32" si="31">D15/C15-1</f>
@@ -9909,7 +9963,7 @@
     </row>
     <row r="45" spans="2:28" s="39" customFormat="1">
       <c r="B45" s="48" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C45" s="39">
         <v>0</v>
@@ -10051,7 +10105,7 @@
     </row>
     <row r="47" spans="2:28" s="39" customFormat="1">
       <c r="B47" s="48" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C47" s="39">
         <v>3</v>
@@ -10122,7 +10176,7 @@
     </row>
     <row r="48" spans="2:28" s="39" customFormat="1">
       <c r="B48" s="48" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C48" s="39">
         <v>0</v>
@@ -10193,7 +10247,7 @@
     </row>
     <row r="49" spans="2:28" s="39" customFormat="1">
       <c r="B49" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C49" s="39">
         <v>0</v>
@@ -10573,7 +10627,7 @@
     </row>
     <row r="55" spans="2:28" s="39" customFormat="1">
       <c r="B55" s="48" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C55" s="39">
         <v>3</v>
@@ -10647,19 +10701,19 @@
     </row>
     <row r="57" spans="2:28" s="40" customFormat="1">
       <c r="B57" s="29" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C57" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D57" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E57" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F57" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G57" s="65">
         <f t="shared" ref="G57:S57" si="95">G43/C43-1</f>
@@ -10718,7 +10772,7 @@
         <v>-5.8823529411764719E-2</v>
       </c>
       <c r="Y57" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Z57" s="65">
         <f t="shared" ref="Z57:AA57" si="96">Z43/Y43-1</f>
@@ -10735,10 +10789,10 @@
     </row>
     <row r="58" spans="2:28" s="39" customFormat="1">
       <c r="B58" s="30" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C58" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D58" s="64">
         <f t="shared" ref="D58" si="97">D43/C43-1</f>
@@ -10809,16 +10863,16 @@
         <v>0.23076923076923084</v>
       </c>
       <c r="Y58" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Z58" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="AA58" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="AB58" s="66" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="2:28">
@@ -11183,7 +11237,7 @@
     </row>
     <row r="66" spans="2:28">
       <c r="B66" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C66" s="27">
         <v>195.2</v>
@@ -11467,7 +11521,7 @@
     </row>
     <row r="70" spans="2:28">
       <c r="B70" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C70" s="27">
         <v>0</v>
@@ -11982,7 +12036,7 @@
     </row>
     <row r="77" spans="2:28">
       <c r="B77" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C77" s="27">
         <v>88.6</v>
@@ -12053,7 +12107,7 @@
     </row>
     <row r="78" spans="2:28">
       <c r="B78" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C78" s="27">
         <v>396.9</v>
@@ -13075,7 +13129,7 @@
     </row>
     <row r="93" spans="2:28" s="2" customFormat="1">
       <c r="B93" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C93" s="26">
         <v>21.7</v>
@@ -13501,7 +13555,7 @@
     </row>
     <row r="99" spans="2:28">
       <c r="B99" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C99" s="27">
         <v>35.9</v>
@@ -13714,7 +13768,7 @@
     </row>
     <row r="102" spans="2:28">
       <c r="B102" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C102" s="27">
         <v>23.3</v>
@@ -14087,7 +14141,7 @@
     </row>
     <row r="107" spans="2:28" s="2" customFormat="1">
       <c r="B107" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C107" s="26">
         <v>345.3</v>
@@ -14513,7 +14567,7 @@
     </row>
     <row r="113" spans="2:28">
       <c r="B113" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C113" s="27">
         <v>115.8</v>
@@ -15451,16 +15505,16 @@
         <v>134</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E128" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F128" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G128" s="34">
         <f t="shared" ref="G128" si="173">G68/C68-1</f>
@@ -15532,7 +15586,7 @@
         <v>135</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D129" s="25">
         <f t="shared" ref="D129" si="183">D68/C68-1</f>
@@ -15603,10 +15657,10 @@
         <v>7.6525103473096934E-2</v>
       </c>
       <c r="AA129" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="AB129" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="2:28">
@@ -15617,16 +15671,16 @@
         <v>136</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E131" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F131" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G131" s="25">
         <f t="shared" ref="G131" si="192">G68/SUM(D9:G9)</f>
@@ -15699,7 +15753,7 @@
     </row>
     <row r="133" spans="2:28">
       <c r="B133" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C133" s="73">
         <v>26</v>
@@ -15770,7 +15824,7 @@
     </row>
     <row r="134" spans="2:28" s="27" customFormat="1">
       <c r="B134" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C134" s="27">
         <f t="shared" ref="C134:G134" si="203">C133*C27</f>
@@ -16040,69 +16094,69 @@
         <v>27</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E138" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F138" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G138" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="H138" s="91">
+        <v>186</v>
+      </c>
+      <c r="H138" s="74">
         <f t="shared" ref="H138" si="220">H133/SUM(E9:H9)</f>
         <v>3.9969163256834486E-3</v>
       </c>
-      <c r="I138" s="91">
+      <c r="I138" s="74">
         <f t="shared" ref="I138" si="221">I133/SUM(F9:I9)</f>
         <v>3.3988808322824725E-3</v>
       </c>
-      <c r="J138" s="91">
+      <c r="J138" s="74">
         <f t="shared" ref="J138" si="222">J133/SUM(G9:J9)</f>
         <v>3.5678980705158708E-3</v>
       </c>
-      <c r="K138" s="91">
+      <c r="K138" s="74">
         <f t="shared" ref="K138" si="223">K133/SUM(H9:K9)</f>
         <v>1.3692135555934837E-3</v>
       </c>
-      <c r="L138" s="91">
+      <c r="L138" s="74">
         <f t="shared" ref="L138" si="224">L133/SUM(I9:L9)</f>
         <v>1.3493997653217802E-3</v>
       </c>
-      <c r="M138" s="91">
+      <c r="M138" s="74">
         <f t="shared" ref="M138" si="225">M133/SUM(J9:M9)</f>
         <v>1.0984631479313523E-3</v>
       </c>
-      <c r="N138" s="91">
+      <c r="N138" s="74">
         <f t="shared" ref="N138" si="226">N133/SUM(K9:N9)</f>
         <v>1.8058391450770329E-3</v>
       </c>
-      <c r="O138" s="91">
+      <c r="O138" s="74">
         <f t="shared" ref="O138" si="227">O133/SUM(L9:O9)</f>
         <v>2.5249708462201492E-3</v>
       </c>
-      <c r="P138" s="91">
+      <c r="P138" s="74">
         <f t="shared" ref="P138:S138" si="228">P133/SUM(M9:P9)</f>
         <v>3.3363450053989726E-3</v>
       </c>
-      <c r="Q138" s="91">
+      <c r="Q138" s="74">
         <f t="shared" si="228"/>
         <v>3.5885419964958943E-3</v>
       </c>
-      <c r="R138" s="91">
+      <c r="R138" s="74">
         <f t="shared" si="228"/>
         <v>3.3117316306108839E-3</v>
       </c>
-      <c r="S138" s="91">
+      <c r="S138" s="74">
         <f t="shared" si="228"/>
         <v>3.1597674651698908E-3</v>
       </c>
-      <c r="T138" s="91">
+      <c r="T138" s="74">
         <f>T133/SUM(Q9:T9)</f>
         <v>2.2633532687151986E-3</v>
       </c>
@@ -16124,19 +16178,19 @@
         <v>28</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E139" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F139" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G139" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H139" s="57">
         <f t="shared" ref="H139" si="230">H133/SUM(E26:H26)</f>
@@ -16205,10 +16259,10 @@
     </row>
     <row r="141" spans="2:28">
       <c r="B141" s="3" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D141" s="25">
         <f t="shared" ref="D141:S141" si="240">D15:D15/D9</f>
@@ -16326,12 +16380,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="72"/>
+    <col min="1" max="16384" width="9.1640625" style="72"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16341,63 +16395,1700 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258CA0E5-563F-4C1F-B583-AD76D8E7BBD2}">
-  <dimension ref="C4:D12"/>
+  <dimension ref="A2:AG46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45:D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4">
-      <c r="D4" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4">
-      <c r="C6" s="3" t="s">
+    <row r="2" spans="1:33" s="2" customFormat="1" ht="13">
+      <c r="B2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2" s="2">
+        <v>2016</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>2017</v>
+      </c>
+      <c r="Z2" s="97">
+        <v>2018</v>
+      </c>
+      <c r="AA2" s="97">
+        <f>Z2+1</f>
+        <v>2019</v>
+      </c>
+      <c r="AB2" s="97">
+        <f t="shared" ref="AB2:AG2" si="0">AA2+1</f>
+        <v>2020</v>
+      </c>
+      <c r="AC2" s="97">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="AD2" s="2">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="AE2" s="2">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="AF2" s="2">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="AG2" s="2">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" s="94" customFormat="1" ht="13">
+      <c r="A3" s="94" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="94">
+        <f t="shared" ref="B3" si="1">SUM(B4:B9)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="94">
+        <f t="shared" ref="C3" si="2">SUM(C4:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="94">
+        <f t="shared" ref="D3" si="3">SUM(D4:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="94">
+        <f t="shared" ref="E3" si="4">SUM(E4:E9)</f>
+        <v>1858</v>
+      </c>
+      <c r="F3" s="94">
+        <f t="shared" ref="F3" si="5">SUM(F4:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="94">
+        <f t="shared" ref="G3" si="6">SUM(G4:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="94">
+        <f t="shared" ref="H3" si="7">SUM(H4:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="94">
+        <f t="shared" ref="I3" si="8">SUM(I4:I9)</f>
+        <v>1917</v>
+      </c>
+      <c r="J3" s="94">
+        <f t="shared" ref="J3" si="9">SUM(J4:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="94">
+        <f t="shared" ref="K3" si="10">SUM(K4:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="94">
+        <f t="shared" ref="L3" si="11">SUM(L4:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="94">
+        <f t="shared" ref="M3:Q3" si="12">SUM(M4:M9)</f>
+        <v>1904</v>
+      </c>
+      <c r="N3" s="94">
+        <f t="shared" si="12"/>
+        <v>1904</v>
+      </c>
+      <c r="O3" s="94">
+        <f t="shared" ref="O3" si="13">SUM(O4:O9)</f>
+        <v>1952</v>
+      </c>
+      <c r="P3" s="94">
+        <f t="shared" si="12"/>
+        <v>1968</v>
+      </c>
+      <c r="Q3" s="94">
+        <f t="shared" si="12"/>
+        <v>1996</v>
+      </c>
+      <c r="R3" s="94">
+        <f>SUM(R4:R9)</f>
+        <v>1992</v>
+      </c>
+      <c r="S3" s="94">
+        <f t="shared" ref="S3" si="14">SUM(S4:S9)</f>
+        <v>2000</v>
+      </c>
+      <c r="Z3" s="94">
+        <f t="shared" ref="Z3" si="15">SUM(Z4:Z9)</f>
+        <v>1858</v>
+      </c>
+      <c r="AA3" s="94">
+        <f t="shared" ref="AA3" si="16">SUM(AA4:AA9)</f>
+        <v>1917</v>
+      </c>
+      <c r="AB3" s="94">
+        <f t="shared" ref="AB3" si="17">SUM(AB4:AB9)</f>
+        <v>1904</v>
+      </c>
+      <c r="AC3" s="94">
+        <f t="shared" ref="AC3" si="18">SUM(AC4:AC9)</f>
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A4" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="95">
+        <v>191</v>
+      </c>
+      <c r="I4" s="95">
+        <v>191</v>
+      </c>
+      <c r="M4" s="95">
+        <v>191</v>
+      </c>
+      <c r="N4" s="95">
+        <v>191</v>
+      </c>
+      <c r="O4" s="95">
+        <v>191</v>
+      </c>
+      <c r="P4" s="95">
+        <v>191</v>
+      </c>
+      <c r="Q4" s="95">
+        <v>191</v>
+      </c>
+      <c r="R4" s="95">
+        <v>191</v>
+      </c>
+      <c r="S4" s="95">
+        <v>191</v>
+      </c>
+      <c r="Z4" s="95">
+        <v>191</v>
+      </c>
+      <c r="AA4" s="95">
+        <v>191</v>
+      </c>
+      <c r="AB4" s="95">
+        <v>191</v>
+      </c>
+      <c r="AC4" s="95">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A5" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="95">
+        <v>771</v>
+      </c>
+      <c r="I5" s="95">
+        <v>815</v>
+      </c>
+      <c r="M5" s="95">
+        <v>798</v>
+      </c>
+      <c r="N5" s="95">
+        <v>798</v>
+      </c>
+      <c r="O5" s="95">
+        <v>816</v>
+      </c>
+      <c r="P5" s="95">
+        <v>832</v>
+      </c>
+      <c r="Q5" s="95">
+        <v>840</v>
+      </c>
+      <c r="R5" s="95">
+        <v>840</v>
+      </c>
+      <c r="S5" s="95">
+        <v>848</v>
+      </c>
+      <c r="Z5" s="95">
+        <v>771</v>
+      </c>
+      <c r="AA5" s="95">
+        <v>815</v>
+      </c>
+      <c r="AB5" s="95">
+        <v>798</v>
+      </c>
+      <c r="AC5" s="95">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A6" s="96" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="95">
+        <v>566</v>
+      </c>
+      <c r="I6" s="95">
+        <v>568</v>
+      </c>
+      <c r="M6" s="95">
+        <v>568</v>
+      </c>
+      <c r="N6" s="95">
+        <v>568</v>
+      </c>
+      <c r="O6" s="95">
+        <v>568</v>
+      </c>
+      <c r="P6" s="95">
+        <v>568</v>
+      </c>
+      <c r="Q6" s="95">
+        <v>568</v>
+      </c>
+      <c r="R6" s="95">
+        <v>568</v>
+      </c>
+      <c r="S6" s="95">
+        <v>568</v>
+      </c>
+      <c r="Z6" s="95">
+        <v>566</v>
+      </c>
+      <c r="AA6" s="95">
+        <v>568</v>
+      </c>
+      <c r="AB6" s="95">
+        <v>568</v>
+      </c>
+      <c r="AC6" s="95">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A7" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4">
-      <c r="C7" s="3" t="s">
+      <c r="E7" s="95">
+        <v>172</v>
+      </c>
+      <c r="I7" s="95">
+        <v>172</v>
+      </c>
+      <c r="M7" s="95">
+        <v>172</v>
+      </c>
+      <c r="N7" s="95">
+        <v>172</v>
+      </c>
+      <c r="O7" s="95">
+        <v>172</v>
+      </c>
+      <c r="P7" s="95">
+        <v>172</v>
+      </c>
+      <c r="Q7" s="95">
+        <v>172</v>
+      </c>
+      <c r="R7" s="95">
+        <v>172</v>
+      </c>
+      <c r="S7" s="95">
+        <v>172</v>
+      </c>
+      <c r="Z7" s="95">
+        <v>172</v>
+      </c>
+      <c r="AA7" s="95">
+        <v>172</v>
+      </c>
+      <c r="AB7" s="95">
+        <v>172</v>
+      </c>
+      <c r="AC7" s="95">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A8" s="96" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" s="95">
+        <v>47</v>
+      </c>
+      <c r="I8" s="95">
+        <v>27</v>
+      </c>
+      <c r="M8" s="95">
+        <v>22</v>
+      </c>
+      <c r="N8" s="95">
+        <v>22</v>
+      </c>
+      <c r="O8" s="95">
+        <v>22</v>
+      </c>
+      <c r="P8" s="95">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="95">
+        <v>22</v>
+      </c>
+      <c r="R8" s="95">
+        <v>20</v>
+      </c>
+      <c r="S8" s="95">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="95">
+        <v>47</v>
+      </c>
+      <c r="AA8" s="95">
+        <v>27</v>
+      </c>
+      <c r="AB8" s="95">
+        <v>22</v>
+      </c>
+      <c r="AC8" s="95">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A9" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="95">
+        <v>111</v>
+      </c>
+      <c r="I9" s="95">
+        <v>144</v>
+      </c>
+      <c r="M9" s="95">
+        <v>153</v>
+      </c>
+      <c r="N9" s="95">
+        <v>153</v>
+      </c>
+      <c r="O9" s="95">
+        <v>183</v>
+      </c>
+      <c r="P9" s="95">
+        <v>183</v>
+      </c>
+      <c r="Q9" s="95">
+        <v>203</v>
+      </c>
+      <c r="R9" s="95">
+        <v>201</v>
+      </c>
+      <c r="S9" s="95">
+        <v>201</v>
+      </c>
+      <c r="Z9" s="95">
+        <v>111</v>
+      </c>
+      <c r="AA9" s="95">
+        <v>144</v>
+      </c>
+      <c r="AB9" s="95">
+        <v>153</v>
+      </c>
+      <c r="AC9" s="95">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" s="95" customFormat="1" ht="13"/>
+    <row r="11" spans="1:33" s="94" customFormat="1" ht="13">
+      <c r="A11" s="94" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" s="94">
+        <f t="shared" ref="B11" si="19">SUM(B12:B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="94">
+        <f t="shared" ref="C11" si="20">SUM(C12:C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="94">
+        <f t="shared" ref="D11" si="21">SUM(D12:D17)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="94">
+        <f t="shared" ref="E11" si="22">SUM(E12:E17)</f>
+        <v>1490</v>
+      </c>
+      <c r="F11" s="94">
+        <f t="shared" ref="F11" si="23">SUM(F12:F17)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="94">
+        <f t="shared" ref="G11" si="24">SUM(G12:G17)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="94">
+        <f t="shared" ref="H11" si="25">SUM(H12:H17)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="94">
+        <f t="shared" ref="I11" si="26">SUM(I12:I17)</f>
+        <v>1579</v>
+      </c>
+      <c r="J11" s="94">
+        <f t="shared" ref="J11" si="27">SUM(J12:J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="94">
+        <f t="shared" ref="K11" si="28">SUM(K12:K17)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="94">
+        <f t="shared" ref="L11" si="29">SUM(L12:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="94">
+        <f t="shared" ref="M11" si="30">SUM(M12:M17)</f>
+        <v>1623</v>
+      </c>
+      <c r="N11" s="94">
+        <f t="shared" ref="N11:Q11" si="31">SUM(N12:N17)</f>
+        <v>1632</v>
+      </c>
+      <c r="O11" s="94">
+        <f t="shared" ref="O11" si="32">SUM(O12:O17)</f>
+        <v>1646</v>
+      </c>
+      <c r="P11" s="94">
+        <f t="shared" si="31"/>
+        <v>1655</v>
+      </c>
+      <c r="Q11" s="94">
+        <f t="shared" si="31"/>
+        <v>1671</v>
+      </c>
+      <c r="R11" s="94">
+        <f>SUM(R12:R17)</f>
+        <v>1677</v>
+      </c>
+      <c r="S11" s="94">
+        <f t="shared" ref="S11" si="33">SUM(S12:S17)</f>
+        <v>1688</v>
+      </c>
+      <c r="Z11" s="94">
+        <f t="shared" ref="Z11" si="34">SUM(Z12:Z17)</f>
+        <v>1490</v>
+      </c>
+      <c r="AA11" s="94">
+        <f t="shared" ref="AA11" si="35">SUM(AA12:AA17)</f>
+        <v>1579</v>
+      </c>
+      <c r="AB11" s="94">
+        <f t="shared" ref="AB11" si="36">SUM(AB12:AB17)</f>
+        <v>1623</v>
+      </c>
+      <c r="AC11" s="94">
+        <f t="shared" ref="AC11" si="37">SUM(AC12:AC17)</f>
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A12" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" s="95">
+        <v>191</v>
+      </c>
+      <c r="I12" s="95">
+        <v>191</v>
+      </c>
+      <c r="M12" s="95">
+        <v>191</v>
+      </c>
+      <c r="N12" s="95">
+        <v>191</v>
+      </c>
+      <c r="O12" s="95">
+        <v>191</v>
+      </c>
+      <c r="P12" s="95">
+        <v>191</v>
+      </c>
+      <c r="Q12" s="95">
+        <v>191</v>
+      </c>
+      <c r="R12" s="95">
+        <v>191</v>
+      </c>
+      <c r="S12" s="95">
+        <v>191</v>
+      </c>
+      <c r="Z12" s="95">
+        <v>191</v>
+      </c>
+      <c r="AA12" s="95">
+        <v>191</v>
+      </c>
+      <c r="AB12" s="95">
+        <v>191</v>
+      </c>
+      <c r="AC12" s="95">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A13" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="95">
+        <v>567</v>
+      </c>
+      <c r="I13" s="95">
+        <v>634</v>
+      </c>
+      <c r="M13" s="95">
+        <v>666</v>
+      </c>
+      <c r="N13" s="95">
+        <v>668</v>
+      </c>
+      <c r="O13" s="95">
+        <v>675</v>
+      </c>
+      <c r="P13" s="95">
+        <v>681</v>
+      </c>
+      <c r="Q13" s="95">
+        <v>693</v>
+      </c>
+      <c r="R13" s="95">
+        <v>697</v>
+      </c>
+      <c r="S13" s="95">
+        <v>705</v>
+      </c>
+      <c r="Z13" s="95">
+        <v>567</v>
+      </c>
+      <c r="AA13" s="95">
+        <v>634</v>
+      </c>
+      <c r="AB13" s="95">
+        <v>666</v>
+      </c>
+      <c r="AC13" s="95">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A14" s="96" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="95">
+        <v>559</v>
+      </c>
+      <c r="I14" s="95">
+        <v>564</v>
+      </c>
+      <c r="M14" s="95">
+        <v>565</v>
+      </c>
+      <c r="N14" s="95">
+        <v>565</v>
+      </c>
+      <c r="O14" s="95">
+        <v>565</v>
+      </c>
+      <c r="P14" s="95">
+        <v>565</v>
+      </c>
+      <c r="Q14" s="95">
+        <v>565</v>
+      </c>
+      <c r="R14" s="95">
+        <v>565</v>
+      </c>
+      <c r="S14" s="95">
+        <v>565</v>
+      </c>
+      <c r="Z14" s="95">
+        <v>559</v>
+      </c>
+      <c r="AA14" s="95">
+        <v>564</v>
+      </c>
+      <c r="AB14" s="95">
+        <v>565</v>
+      </c>
+      <c r="AC14" s="95">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A15" s="96" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="95">
+        <v>169</v>
+      </c>
+      <c r="I15" s="95">
+        <v>172</v>
+      </c>
+      <c r="M15" s="95">
+        <v>172</v>
+      </c>
+      <c r="N15" s="95">
+        <v>172</v>
+      </c>
+      <c r="O15" s="95">
+        <v>172</v>
+      </c>
+      <c r="P15" s="95">
+        <v>172</v>
+      </c>
+      <c r="Q15" s="95">
+        <v>172</v>
+      </c>
+      <c r="R15" s="95">
+        <v>172</v>
+      </c>
+      <c r="S15" s="95">
+        <v>172</v>
+      </c>
+      <c r="Z15" s="95">
+        <v>169</v>
+      </c>
+      <c r="AA15" s="95">
+        <v>172</v>
+      </c>
+      <c r="AB15" s="95">
+        <v>172</v>
+      </c>
+      <c r="AC15" s="95">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" s="95" customFormat="1" ht="13">
+      <c r="A16" s="96" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="95">
+        <v>4</v>
+      </c>
+      <c r="I16" s="95">
+        <v>11</v>
+      </c>
+      <c r="M16" s="95">
+        <v>15</v>
+      </c>
+      <c r="N16" s="95">
+        <v>17</v>
+      </c>
+      <c r="O16" s="95">
+        <v>17</v>
+      </c>
+      <c r="P16" s="95">
+        <v>17</v>
+      </c>
+      <c r="Q16" s="95">
+        <v>17</v>
+      </c>
+      <c r="R16" s="95">
+        <v>17</v>
+      </c>
+      <c r="S16" s="95">
+        <v>17</v>
+      </c>
+      <c r="Z16" s="95">
+        <v>4</v>
+      </c>
+      <c r="AA16" s="95">
+        <v>11</v>
+      </c>
+      <c r="AB16" s="95">
+        <v>15</v>
+      </c>
+      <c r="AC16" s="95">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A17" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="95">
+        <v>0</v>
+      </c>
+      <c r="I17" s="95">
+        <v>7</v>
+      </c>
+      <c r="M17" s="95">
+        <v>14</v>
+      </c>
+      <c r="N17" s="95">
+        <v>19</v>
+      </c>
+      <c r="O17" s="95">
+        <v>26</v>
+      </c>
+      <c r="P17" s="95">
+        <v>29</v>
+      </c>
+      <c r="Q17" s="95">
+        <v>33</v>
+      </c>
+      <c r="R17" s="95">
+        <v>35</v>
+      </c>
+      <c r="S17" s="95">
+        <v>38</v>
+      </c>
+      <c r="Z17" s="95">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="95">
+        <v>7</v>
+      </c>
+      <c r="AB17" s="95">
+        <v>14</v>
+      </c>
+      <c r="AC17" s="95">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A18" s="96"/>
+    </row>
+    <row r="19" spans="1:29" s="94" customFormat="1" ht="13">
+      <c r="A19" s="94" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="94">
+        <f t="shared" ref="B19" si="38">SUM(B20:B25)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="94">
+        <f t="shared" ref="C19" si="39">SUM(C20:C25)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="94">
+        <f t="shared" ref="D19" si="40">SUM(D20:D25)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="94">
+        <f t="shared" ref="E19" si="41">SUM(E20:E25)</f>
+        <v>368</v>
+      </c>
+      <c r="F19" s="94">
+        <f t="shared" ref="F19" si="42">SUM(F20:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="94">
+        <f t="shared" ref="G19" si="43">SUM(G20:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="94">
+        <f t="shared" ref="H19" si="44">SUM(H20:H25)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="94">
+        <f t="shared" ref="I19" si="45">SUM(I20:I25)</f>
+        <v>338</v>
+      </c>
+      <c r="J19" s="94">
+        <f t="shared" ref="J19" si="46">SUM(J20:J25)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="94">
+        <f t="shared" ref="K19" si="47">SUM(K20:K25)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="94">
+        <f t="shared" ref="L19" si="48">SUM(L20:L25)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="94">
+        <f t="shared" ref="M19" si="49">SUM(M20:M25)</f>
+        <v>281</v>
+      </c>
+      <c r="N19" s="94">
+        <f t="shared" ref="N19:Q19" si="50">SUM(N20:N25)</f>
+        <v>272</v>
+      </c>
+      <c r="O19" s="94">
+        <f t="shared" ref="O19" si="51">SUM(O20:O25)</f>
+        <v>306</v>
+      </c>
+      <c r="P19" s="94">
+        <f t="shared" si="50"/>
+        <v>313</v>
+      </c>
+      <c r="Q19" s="94">
+        <f t="shared" si="50"/>
+        <v>325</v>
+      </c>
+      <c r="R19" s="94">
+        <f>SUM(R20:R25)</f>
+        <v>315</v>
+      </c>
+      <c r="S19" s="94">
+        <f t="shared" ref="S19" si="52">SUM(S20:S25)</f>
+        <v>312</v>
+      </c>
+      <c r="Z19" s="94">
+        <f t="shared" ref="Z19" si="53">SUM(Z20:Z25)</f>
+        <v>368</v>
+      </c>
+      <c r="AA19" s="94">
+        <f t="shared" ref="AA19" si="54">SUM(AA20:AA25)</f>
+        <v>338</v>
+      </c>
+      <c r="AB19" s="94">
+        <f t="shared" ref="AB19" si="55">SUM(AB20:AB25)</f>
+        <v>281</v>
+      </c>
+      <c r="AC19" s="94">
+        <f t="shared" ref="AC19" si="56">SUM(AC20:AC25)</f>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A20" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="E20" s="95">
+        <v>0</v>
+      </c>
+      <c r="I20" s="95">
+        <v>0</v>
+      </c>
+      <c r="M20" s="95">
+        <v>0</v>
+      </c>
+      <c r="N20" s="95">
+        <v>0</v>
+      </c>
+      <c r="O20" s="95">
+        <v>0</v>
+      </c>
+      <c r="P20" s="95">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="95">
+        <v>0</v>
+      </c>
+      <c r="R20" s="95">
+        <v>0</v>
+      </c>
+      <c r="S20" s="95">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="95">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="95">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="95">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A21" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="95">
+        <v>204</v>
+      </c>
+      <c r="I21" s="95">
         <v>181</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4">
-      <c r="C9" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4">
-      <c r="C10" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4">
-      <c r="C12" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>211</v>
-      </c>
+      <c r="M21" s="95">
+        <v>132</v>
+      </c>
+      <c r="N21" s="95">
+        <v>130</v>
+      </c>
+      <c r="O21" s="95">
+        <v>141</v>
+      </c>
+      <c r="P21" s="95">
+        <v>151</v>
+      </c>
+      <c r="Q21" s="95">
+        <v>147</v>
+      </c>
+      <c r="R21" s="95">
+        <v>143</v>
+      </c>
+      <c r="S21" s="95">
+        <v>143</v>
+      </c>
+      <c r="Z21" s="95">
+        <v>204</v>
+      </c>
+      <c r="AA21" s="95">
+        <v>181</v>
+      </c>
+      <c r="AB21" s="95">
+        <v>132</v>
+      </c>
+      <c r="AC21" s="95">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A22" s="96" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="95">
+        <v>7</v>
+      </c>
+      <c r="I22" s="95">
+        <v>4</v>
+      </c>
+      <c r="M22" s="95">
+        <v>3</v>
+      </c>
+      <c r="N22" s="95">
+        <v>3</v>
+      </c>
+      <c r="O22" s="95">
+        <v>3</v>
+      </c>
+      <c r="P22" s="95">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="95">
+        <v>3</v>
+      </c>
+      <c r="R22" s="95">
+        <v>3</v>
+      </c>
+      <c r="S22" s="95">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="95">
+        <v>7</v>
+      </c>
+      <c r="AA22" s="95">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="95">
+        <v>3</v>
+      </c>
+      <c r="AC22" s="95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A23" s="96" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" s="95">
+        <v>3</v>
+      </c>
+      <c r="I23" s="95">
+        <v>0</v>
+      </c>
+      <c r="M23" s="95">
+        <v>0</v>
+      </c>
+      <c r="N23" s="95">
+        <v>0</v>
+      </c>
+      <c r="O23" s="95">
+        <v>0</v>
+      </c>
+      <c r="P23" s="95">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="95">
+        <v>0</v>
+      </c>
+      <c r="R23" s="95">
+        <v>0</v>
+      </c>
+      <c r="S23" s="95">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="95">
+        <v>3</v>
+      </c>
+      <c r="AA23" s="95">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="95">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A24" s="96" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="95">
+        <v>43</v>
+      </c>
+      <c r="I24" s="95">
+        <v>16</v>
+      </c>
+      <c r="M24" s="95">
+        <v>7</v>
+      </c>
+      <c r="N24" s="95">
+        <v>5</v>
+      </c>
+      <c r="O24" s="95">
+        <v>5</v>
+      </c>
+      <c r="P24" s="95">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="95">
+        <v>5</v>
+      </c>
+      <c r="R24" s="95">
+        <v>3</v>
+      </c>
+      <c r="S24" s="95">
+        <v>3</v>
+      </c>
+      <c r="Z24" s="95">
+        <v>43</v>
+      </c>
+      <c r="AA24" s="95">
+        <v>16</v>
+      </c>
+      <c r="AB24" s="95">
+        <v>7</v>
+      </c>
+      <c r="AC24" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" s="95" customFormat="1" ht="13">
+      <c r="A25" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="95">
+        <v>111</v>
+      </c>
+      <c r="I25" s="95">
+        <v>137</v>
+      </c>
+      <c r="M25" s="95">
+        <v>139</v>
+      </c>
+      <c r="N25" s="95">
+        <v>134</v>
+      </c>
+      <c r="O25" s="95">
+        <v>157</v>
+      </c>
+      <c r="P25" s="95">
+        <v>154</v>
+      </c>
+      <c r="Q25" s="95">
+        <v>170</v>
+      </c>
+      <c r="R25" s="95">
+        <v>166</v>
+      </c>
+      <c r="S25" s="95">
+        <v>163</v>
+      </c>
+      <c r="Z25" s="95">
+        <v>111</v>
+      </c>
+      <c r="AA25" s="95">
+        <v>137</v>
+      </c>
+      <c r="AB25" s="95">
+        <v>139</v>
+      </c>
+      <c r="AC25" s="95">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" s="2" customFormat="1" ht="13">
+      <c r="A28" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I28" s="34">
+        <f t="shared" ref="I28" si="57">I3/E3-1</f>
+        <v>3.1754574811625469E-2</v>
+      </c>
+      <c r="M28" s="34">
+        <f t="shared" ref="M28" si="58">M3/I3-1</f>
+        <v>-6.7814293166406081E-3</v>
+      </c>
+      <c r="Q28" s="34">
+        <f t="shared" ref="Q28" si="59">Q3/M3-1</f>
+        <v>4.8319327731092487E-2</v>
+      </c>
+      <c r="R28" s="34">
+        <f>R3/N3-1</f>
+        <v>4.6218487394958041E-2</v>
+      </c>
+      <c r="S28" s="34">
+        <f t="shared" ref="S28" si="60">S3/O3-1</f>
+        <v>2.4590163934426146E-2</v>
+      </c>
+      <c r="AA28" s="34">
+        <f t="shared" ref="AA28:AC28" si="61">AA3/Z3-1</f>
+        <v>3.1754574811625469E-2</v>
+      </c>
+      <c r="AB28" s="34">
+        <f t="shared" si="61"/>
+        <v>-6.7814293166406081E-3</v>
+      </c>
+      <c r="AC28" s="34">
+        <f>AC3/AB3-1</f>
+        <v>4.8319327731092487E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" s="98" customFormat="1" ht="13">
+      <c r="A29" s="98" t="s">
+        <v>213</v>
+      </c>
+      <c r="I29" s="98">
+        <f t="shared" ref="I29" si="62">I3-E3</f>
+        <v>59</v>
+      </c>
+      <c r="M29" s="98">
+        <f t="shared" ref="M29" si="63">M3-I3</f>
+        <v>-13</v>
+      </c>
+      <c r="Q29" s="98">
+        <f t="shared" ref="Q29:R29" si="64">Q3-M3</f>
+        <v>92</v>
+      </c>
+      <c r="R29" s="98">
+        <f t="shared" si="64"/>
+        <v>88</v>
+      </c>
+      <c r="S29" s="98">
+        <f>S3-O3</f>
+        <v>48</v>
+      </c>
+      <c r="AA29" s="98">
+        <f t="shared" ref="AA29:AC29" si="65">AA3-Z3</f>
+        <v>59</v>
+      </c>
+      <c r="AB29" s="98">
+        <f t="shared" si="65"/>
+        <v>-13</v>
+      </c>
+      <c r="AC29" s="98">
+        <f>AC3-AB3</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
+      <c r="A30" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N30" s="25">
+        <f t="shared" ref="N30:Q30" si="66">N3/M3-1</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="25">
+        <f t="shared" si="66"/>
+        <v>2.5210084033613356E-2</v>
+      </c>
+      <c r="P30" s="25">
+        <f t="shared" si="66"/>
+        <v>8.1967213114753079E-3</v>
+      </c>
+      <c r="Q30" s="25">
+        <f t="shared" ref="Q30:R30" si="67">Q3/P3-1</f>
+        <v>1.4227642276422703E-2</v>
+      </c>
+      <c r="R30" s="25">
+        <f>R3/Q3-1</f>
+        <v>-2.0040080160320661E-3</v>
+      </c>
+      <c r="S30" s="25">
+        <f t="shared" ref="S30" si="68">S3/R3-1</f>
+        <v>4.0160642570281624E-3</v>
+      </c>
+      <c r="Z30" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA30" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB30" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC30" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" s="99" customFormat="1">
+      <c r="A31" s="99" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="100"/>
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="N31" s="98">
+        <f>N3-M3</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="98">
+        <f>O3-N3</f>
+        <v>48</v>
+      </c>
+      <c r="P31" s="98">
+        <f>P3-O3</f>
+        <v>16</v>
+      </c>
+      <c r="Q31" s="98">
+        <f>Q3-P3</f>
+        <v>28</v>
+      </c>
+      <c r="R31" s="98">
+        <f>R3-Q3</f>
+        <v>-4</v>
+      </c>
+      <c r="S31" s="98">
+        <f>S3-R3</f>
+        <v>8</v>
+      </c>
+      <c r="Z31" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA31" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB31" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC31" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
+      <c r="AC32" s="25"/>
+    </row>
+    <row r="33" spans="1:29" s="2" customFormat="1" ht="13">
+      <c r="A33" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I33" s="34">
+        <f t="shared" ref="I33" si="69">I11/E11-1</f>
+        <v>5.9731543624160999E-2</v>
+      </c>
+      <c r="M33" s="34">
+        <f t="shared" ref="M33" si="70">M11/I11-1</f>
+        <v>2.7865737808739688E-2</v>
+      </c>
+      <c r="Q33" s="34">
+        <f t="shared" ref="Q33" si="71">Q11/M11-1</f>
+        <v>2.9574861367837268E-2</v>
+      </c>
+      <c r="R33" s="34">
+        <f>R11/N11-1</f>
+        <v>2.7573529411764719E-2</v>
+      </c>
+      <c r="S33" s="34">
+        <f t="shared" ref="S33" si="72">S11/O11-1</f>
+        <v>2.5516403402187082E-2</v>
+      </c>
+      <c r="AA33" s="34">
+        <f t="shared" ref="AA33:AB33" si="73">AA11/Z11-1</f>
+        <v>5.9731543624160999E-2</v>
+      </c>
+      <c r="AB33" s="34">
+        <f>AB11/AA11-1</f>
+        <v>2.7865737808739688E-2</v>
+      </c>
+      <c r="AC33" s="34">
+        <f>AC11/AB11-1</f>
+        <v>2.9574861367837268E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" s="98" customFormat="1" ht="13">
+      <c r="A34" s="98" t="s">
+        <v>202</v>
+      </c>
+      <c r="I34" s="98">
+        <f t="shared" ref="I34" si="74">I11-E11</f>
+        <v>89</v>
+      </c>
+      <c r="M34" s="98">
+        <f t="shared" ref="M34" si="75">M11-I11</f>
+        <v>44</v>
+      </c>
+      <c r="Q34" s="98">
+        <f t="shared" ref="Q34:R34" si="76">Q11-M11</f>
+        <v>48</v>
+      </c>
+      <c r="R34" s="98">
+        <f t="shared" si="76"/>
+        <v>45</v>
+      </c>
+      <c r="S34" s="98">
+        <f>S11-O11</f>
+        <v>42</v>
+      </c>
+      <c r="AA34" s="98">
+        <f t="shared" ref="AA34:AC34" si="77">AA11-Z11</f>
+        <v>89</v>
+      </c>
+      <c r="AB34" s="98">
+        <f t="shared" si="77"/>
+        <v>44</v>
+      </c>
+      <c r="AC34" s="98">
+        <f>AC11-AB11</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
+      <c r="A35" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N35" s="25">
+        <f t="shared" ref="N35:Q35" si="78">N11/M11-1</f>
+        <v>5.5452865064695711E-3</v>
+      </c>
+      <c r="O35" s="25">
+        <f t="shared" si="78"/>
+        <v>8.5784313725489891E-3</v>
+      </c>
+      <c r="P35" s="25">
+        <f t="shared" si="78"/>
+        <v>5.4678007290400732E-3</v>
+      </c>
+      <c r="Q35" s="25">
+        <f t="shared" ref="Q35:R35" si="79">Q11/P11-1</f>
+        <v>9.6676737160121817E-3</v>
+      </c>
+      <c r="R35" s="25">
+        <f>R11/Q11-1</f>
+        <v>3.5906642728904536E-3</v>
+      </c>
+      <c r="S35" s="25">
+        <f t="shared" ref="S35" si="80">S11/R11-1</f>
+        <v>6.5593321407275695E-3</v>
+      </c>
+      <c r="Z35" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA35" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB35" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC35" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" s="101" customFormat="1">
+      <c r="A36" s="101" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" s="102"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="102"/>
+      <c r="N36" s="98">
+        <f t="shared" ref="N36:S36" si="81">N11-M11</f>
+        <v>9</v>
+      </c>
+      <c r="O36" s="98">
+        <f t="shared" si="81"/>
+        <v>14</v>
+      </c>
+      <c r="P36" s="98">
+        <f t="shared" si="81"/>
+        <v>9</v>
+      </c>
+      <c r="Q36" s="98">
+        <f t="shared" si="81"/>
+        <v>16</v>
+      </c>
+      <c r="R36" s="98">
+        <f t="shared" si="81"/>
+        <v>6</v>
+      </c>
+      <c r="S36" s="98">
+        <f>S11-R11</f>
+        <v>11</v>
+      </c>
+      <c r="Z36" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA36" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB36" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC36" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29">
+      <c r="AC37" s="25"/>
+    </row>
+    <row r="38" spans="1:29" s="2" customFormat="1" ht="13">
+      <c r="A38" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I38" s="34">
+        <f t="shared" ref="I38" si="82">I19/E19-1</f>
+        <v>-8.1521739130434812E-2</v>
+      </c>
+      <c r="M38" s="34">
+        <f t="shared" ref="M38" si="83">M19/I19-1</f>
+        <v>-0.16863905325443784</v>
+      </c>
+      <c r="Q38" s="34">
+        <f t="shared" ref="Q38" si="84">Q19/M19-1</f>
+        <v>0.15658362989323837</v>
+      </c>
+      <c r="R38" s="34">
+        <f>R19/N19-1</f>
+        <v>0.15808823529411775</v>
+      </c>
+      <c r="S38" s="34">
+        <f t="shared" ref="S38" si="85">S19/O19-1</f>
+        <v>1.9607843137254832E-2</v>
+      </c>
+      <c r="AA38" s="34">
+        <f t="shared" ref="AA38:AB38" si="86">AA19/Z19-1</f>
+        <v>-8.1521739130434812E-2</v>
+      </c>
+      <c r="AB38" s="34">
+        <f>AB19/AA19-1</f>
+        <v>-0.16863905325443784</v>
+      </c>
+      <c r="AC38" s="34">
+        <f>AC19/AB19-1</f>
+        <v>0.15658362989323837</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" s="103" customFormat="1" ht="13">
+      <c r="A39" s="103" t="s">
+        <v>215</v>
+      </c>
+      <c r="I39" s="103">
+        <f>I19-E19</f>
+        <v>-30</v>
+      </c>
+      <c r="M39" s="103">
+        <f>M19-I19</f>
+        <v>-57</v>
+      </c>
+      <c r="Q39" s="103">
+        <f t="shared" ref="Q39:R39" si="87">Q19-M19</f>
+        <v>44</v>
+      </c>
+      <c r="R39" s="103">
+        <f t="shared" si="87"/>
+        <v>43</v>
+      </c>
+      <c r="S39" s="103">
+        <f>S19-O19</f>
+        <v>6</v>
+      </c>
+      <c r="AA39" s="103">
+        <f t="shared" ref="AA39:AC39" si="88">AA19-Z19</f>
+        <v>-30</v>
+      </c>
+      <c r="AB39" s="103">
+        <f t="shared" si="88"/>
+        <v>-57</v>
+      </c>
+      <c r="AC39" s="103">
+        <f>AC19-AB19</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29">
+      <c r="A40" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="N40" s="25">
+        <f t="shared" ref="N40:Q40" si="89">N19/M19-1</f>
+        <v>-3.2028469750889688E-2</v>
+      </c>
+      <c r="O40" s="25">
+        <f t="shared" si="89"/>
+        <v>0.125</v>
+      </c>
+      <c r="P40" s="25">
+        <f t="shared" si="89"/>
+        <v>2.2875816993463971E-2</v>
+      </c>
+      <c r="Q40" s="25">
+        <f t="shared" ref="Q40:R40" si="90">Q19/P19-1</f>
+        <v>3.833865814696491E-2</v>
+      </c>
+      <c r="R40" s="25">
+        <f>R19/Q19-1</f>
+        <v>-3.0769230769230771E-2</v>
+      </c>
+      <c r="S40" s="25">
+        <f t="shared" ref="S40" si="91">S19/R19-1</f>
+        <v>-9.52380952380949E-3</v>
+      </c>
+      <c r="Z40" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA40" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB40" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC40" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" s="101" customFormat="1">
+      <c r="A41" s="101" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" s="102"/>
+      <c r="C41" s="102"/>
+      <c r="D41" s="102"/>
+      <c r="N41" s="98">
+        <f t="shared" ref="N41:S41" si="92">N19-M19</f>
+        <v>-9</v>
+      </c>
+      <c r="O41" s="98">
+        <f t="shared" si="92"/>
+        <v>34</v>
+      </c>
+      <c r="P41" s="98">
+        <f t="shared" si="92"/>
+        <v>7</v>
+      </c>
+      <c r="Q41" s="98">
+        <f t="shared" si="92"/>
+        <v>12</v>
+      </c>
+      <c r="R41" s="98">
+        <f t="shared" si="92"/>
+        <v>-10</v>
+      </c>
+      <c r="S41" s="98">
+        <f>S19-R19</f>
+        <v>-3</v>
+      </c>
+      <c r="Z41" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA41" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB41" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC41" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29">
+      <c r="N44" s="93"/>
+    </row>
+    <row r="46" spans="1:29">
+      <c r="N46" s="92"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{3579012F-D250-C14B-8084-0358505A2D9B}"/>
+    <hyperlink ref="Q2" r:id="rId2" xr:uid="{77A3087C-239B-E34B-8F51-3E2EA54A463A}"/>
+    <hyperlink ref="P2" r:id="rId3" xr:uid="{614FFF93-232C-A94F-8FDC-F25E6D371847}"/>
+    <hyperlink ref="N2" r:id="rId4" xr:uid="{9287A329-D88E-784B-8BDF-1EDA927EB785}"/>
+    <hyperlink ref="S2" r:id="rId5" xr:uid="{6AF4C14B-B6A4-FE47-B0D3-A570A390AD5C}"/>
+    <hyperlink ref="O2" r:id="rId6" xr:uid="{0A17F8BF-EADB-DE42-994D-117A4F2CB3FE}"/>
+    <hyperlink ref="AC2" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
+    <hyperlink ref="M2" r:id="rId8" xr:uid="{F1748A46-ECC6-544E-9D30-C00CF38C6CF7}"/>
+    <hyperlink ref="AB2" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
+    <hyperlink ref="AA2" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
+    <hyperlink ref="I2" r:id="rId11" xr:uid="{998E2907-64B9-7A44-8D65-8083912D2D62}"/>
+    <hyperlink ref="E2" r:id="rId12" xr:uid="{5D689E99-05ED-E34E-9D87-28B9F22988C9}"/>
+    <hyperlink ref="Z2" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$ERJ FY16, FY17 order/backlog data entry
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735B4BD-28AD-C941-B05F-4910276F46B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84117D38-1E4F-584D-B495-3EBA820E4B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="3" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="218">
   <si>
     <t>$ERJ</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>Firm Order Backlog Q/Q</t>
+  </si>
+  <si>
+    <t>Embraer 175-E2</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1259,12 +1262,20 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1274,28 +1285,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1310,20 +1309,36 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5676,6 +5691,111 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8DE692B-E570-7CBF-AAEB-84E21515C477}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14147800" y="12700"/>
+          <a:ext cx="0" cy="10464800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B821CAC-8ED1-6044-8050-A5E1263607BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21145500" y="0"/>
+          <a:ext cx="0" cy="10464800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5976,7 +6096,7 @@
   <dimension ref="A2:AB44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -5996,35 +6116,35 @@
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
-      <c r="G5" s="77" t="s">
+      <c r="C5" s="88"/>
+      <c r="D5" s="89"/>
+      <c r="G5" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="79"/>
-      <c r="U5" s="77" t="s">
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="89"/>
+      <c r="U5" s="87" t="s">
         <v>133</v>
       </c>
-      <c r="V5" s="78"/>
-      <c r="W5" s="78"/>
-      <c r="X5" s="79"/>
-      <c r="AA5" s="75" t="s">
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
+      <c r="X5" s="89"/>
+      <c r="AA5" s="98" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="76"/>
+      <c r="AB5" s="99"/>
     </row>
     <row r="6" spans="1:28">
       <c r="B6" s="4" t="s">
@@ -6301,11 +6421,11 @@
       <c r="X14" s="38"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="79"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="89"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -6332,10 +6452,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="83"/>
+      <c r="D16" s="93"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -6359,10 +6479,10 @@
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="83"/>
+      <c r="D17" s="93"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
@@ -6386,8 +6506,8 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18" s="16"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="83"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="93"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
         <v>192</v>
@@ -6411,8 +6531,8 @@
     </row>
     <row r="19" spans="2:24">
       <c r="B19" s="17"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="85"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="103"/>
       <c r="G19" s="10"/>
       <c r="H19" s="8" t="s">
         <v>193</v>
@@ -6479,11 +6599,11 @@
       <c r="X21" s="38"/>
     </row>
     <row r="22" spans="2:24">
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="79"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="89"/>
       <c r="G22" s="10"/>
       <c r="H22" s="60"/>
       <c r="I22" s="60"/>
@@ -6507,10 +6627,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="92" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="83"/>
+      <c r="D23" s="93"/>
       <c r="G23" s="9">
         <v>44743</v>
       </c>
@@ -6536,10 +6656,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="82">
+      <c r="C24" s="92">
         <v>1969</v>
       </c>
-      <c r="D24" s="83"/>
+      <c r="D24" s="93"/>
       <c r="G24" s="10"/>
       <c r="H24" s="8" t="s">
         <v>197</v>
@@ -6563,8 +6683,8 @@
     </row>
     <row r="25" spans="2:24">
       <c r="B25" s="10"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="83"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="93"/>
       <c r="G25" s="10"/>
       <c r="H25" s="50" t="s">
         <v>198</v>
@@ -6590,11 +6710,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="80">
+      <c r="C26" s="100">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="81"/>
+      <c r="D26" s="101"/>
       <c r="G26" s="10"/>
       <c r="H26" s="60"/>
       <c r="I26" s="60"/>
@@ -6616,8 +6736,8 @@
     </row>
     <row r="27" spans="2:24">
       <c r="B27" s="10"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="83"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="93"/>
       <c r="G27" s="9">
         <v>43922</v>
       </c>
@@ -6676,10 +6796,10 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="89"/>
+      <c r="D29" s="95"/>
       <c r="G29" s="10"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
@@ -6738,11 +6858,11 @@
       <c r="X31" s="38"/>
     </row>
     <row r="32" spans="2:24">
-      <c r="B32" s="77" t="s">
+      <c r="B32" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="78"/>
-      <c r="D32" s="79"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="89"/>
       <c r="G32" s="9">
         <v>43770</v>
       </c>
@@ -6770,11 +6890,11 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="90">
+      <c r="C33" s="96">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="91"/>
+      <c r="D33" s="97"/>
       <c r="G33" s="10"/>
       <c r="H33" s="50" t="s">
         <v>168</v>
@@ -6798,11 +6918,11 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="90">
+      <c r="C34" s="96">
         <f>C6/'Financial Model'!AB9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="91"/>
+      <c r="D34" s="97"/>
       <c r="G34" s="10"/>
       <c r="H34" s="37"/>
       <c r="I34" s="37"/>
@@ -6824,11 +6944,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="86">
+      <c r="C35" s="90">
         <f>C6/'Financial Model'!AB26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="87"/>
+      <c r="D35" s="91"/>
       <c r="G35" s="10"/>
       <c r="H35" s="60"/>
       <c r="I35" s="37"/>
@@ -6875,12 +6995,12 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="U37" s="77" t="s">
+      <c r="U37" s="87" t="s">
         <v>158</v>
       </c>
-      <c r="V37" s="78"/>
-      <c r="W37" s="78"/>
-      <c r="X37" s="79"/>
+      <c r="V37" s="88"/>
+      <c r="W37" s="88"/>
+      <c r="X37" s="89"/>
     </row>
     <row r="38" spans="2:24">
       <c r="G38" s="10"/>
@@ -7018,13 +7138,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C26:D26"/>
@@ -7039,6 +7152,13 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -7062,7 +7182,7 @@
   <dimension ref="B1:AL141"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="S52" sqref="S52"/>
@@ -16380,7 +16500,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -16395,13 +16515,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258CA0E5-563F-4C1F-B583-AD76D8E7BBD2}">
-  <dimension ref="A2:AG46"/>
+  <dimension ref="A2:AG49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -16471,24 +16591,24 @@
       <c r="U2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="80">
         <v>2016</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="80">
         <v>2017</v>
       </c>
-      <c r="Z2" s="97">
+      <c r="Z2" s="80">
         <v>2018</v>
       </c>
-      <c r="AA2" s="97">
+      <c r="AA2" s="80">
         <f>Z2+1</f>
         <v>2019</v>
       </c>
-      <c r="AB2" s="97">
+      <c r="AB2" s="80">
         <f t="shared" ref="AB2:AG2" si="0">AA2+1</f>
         <v>2020</v>
       </c>
-      <c r="AC2" s="97">
+      <c r="AC2" s="80">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
@@ -16509,1569 +16629,1989 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="94" customFormat="1" ht="13">
-      <c r="A3" s="94" t="s">
+    <row r="3" spans="1:33" s="77" customFormat="1" ht="13">
+      <c r="A3" s="77" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="94">
-        <f t="shared" ref="B3" si="1">SUM(B4:B9)</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="94">
-        <f t="shared" ref="C3" si="2">SUM(C4:C9)</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="94">
-        <f t="shared" ref="D3" si="3">SUM(D4:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="94">
-        <f t="shared" ref="E3" si="4">SUM(E4:E9)</f>
+      <c r="B3" s="77">
+        <f t="shared" ref="B3" si="1">SUM(B4:B10)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="77">
+        <f t="shared" ref="C3" si="2">SUM(C4:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="77">
+        <f t="shared" ref="D3" si="3">SUM(D4:D10)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="77">
+        <f t="shared" ref="E3" si="4">SUM(E4:E10)</f>
         <v>1858</v>
       </c>
-      <c r="F3" s="94">
-        <f t="shared" ref="F3" si="5">SUM(F4:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="94">
-        <f t="shared" ref="G3" si="6">SUM(G4:G9)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="94">
-        <f t="shared" ref="H3" si="7">SUM(H4:H9)</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="94">
-        <f t="shared" ref="I3" si="8">SUM(I4:I9)</f>
+      <c r="F3" s="77">
+        <f t="shared" ref="F3" si="5">SUM(F4:F10)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="77">
+        <f t="shared" ref="G3" si="6">SUM(G4:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="77">
+        <f t="shared" ref="H3" si="7">SUM(H4:H10)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="77">
+        <f t="shared" ref="I3" si="8">SUM(I4:I10)</f>
         <v>1917</v>
       </c>
-      <c r="J3" s="94">
-        <f t="shared" ref="J3" si="9">SUM(J4:J9)</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="94">
-        <f t="shared" ref="K3" si="10">SUM(K4:K9)</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="94">
-        <f t="shared" ref="L3" si="11">SUM(L4:L9)</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="94">
-        <f t="shared" ref="M3:Q3" si="12">SUM(M4:M9)</f>
+      <c r="J3" s="77">
+        <f t="shared" ref="J3" si="9">SUM(J4:J10)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="77">
+        <f t="shared" ref="K3" si="10">SUM(K4:K10)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="77">
+        <f t="shared" ref="L3" si="11">SUM(L4:L10)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="77">
+        <f t="shared" ref="M3:Q3" si="12">SUM(M4:M10)</f>
         <v>1904</v>
       </c>
-      <c r="N3" s="94">
+      <c r="N3" s="77">
         <f t="shared" si="12"/>
         <v>1904</v>
       </c>
-      <c r="O3" s="94">
-        <f t="shared" ref="O3" si="13">SUM(O4:O9)</f>
+      <c r="O3" s="77">
+        <f t="shared" ref="O3" si="13">SUM(O4:O10)</f>
         <v>1952</v>
       </c>
-      <c r="P3" s="94">
+      <c r="P3" s="77">
         <f t="shared" si="12"/>
         <v>1968</v>
       </c>
-      <c r="Q3" s="94">
+      <c r="Q3" s="77">
         <f t="shared" si="12"/>
         <v>1996</v>
       </c>
-      <c r="R3" s="94">
-        <f>SUM(R4:R9)</f>
+      <c r="R3" s="77">
+        <f>SUM(R4:R10)</f>
         <v>1992</v>
       </c>
-      <c r="S3" s="94">
-        <f t="shared" ref="S3" si="14">SUM(S4:S9)</f>
+      <c r="S3" s="77">
+        <f t="shared" ref="S3" si="14">SUM(S4:S10)</f>
         <v>2000</v>
       </c>
-      <c r="Z3" s="94">
-        <f t="shared" ref="Z3" si="15">SUM(Z4:Z9)</f>
+      <c r="X3" s="77">
+        <f t="shared" ref="X3:Z3" si="15">SUM(X4:X10)</f>
+        <v>1749</v>
+      </c>
+      <c r="Y3" s="77">
+        <f t="shared" si="15"/>
+        <v>1835</v>
+      </c>
+      <c r="Z3" s="77">
+        <f t="shared" si="15"/>
         <v>1858</v>
       </c>
-      <c r="AA3" s="94">
-        <f t="shared" ref="AA3" si="16">SUM(AA4:AA9)</f>
+      <c r="AA3" s="77">
+        <f t="shared" ref="AA3" si="16">SUM(AA4:AA10)</f>
         <v>1917</v>
       </c>
-      <c r="AB3" s="94">
-        <f t="shared" ref="AB3" si="17">SUM(AB4:AB9)</f>
+      <c r="AB3" s="77">
+        <f t="shared" ref="AB3" si="17">SUM(AB4:AB10)</f>
         <v>1904</v>
       </c>
-      <c r="AC3" s="94">
-        <f t="shared" ref="AC3" si="18">SUM(AC4:AC9)</f>
+      <c r="AC3" s="77">
+        <f t="shared" ref="AC3" si="18">SUM(AC4:AC10)</f>
         <v>1996</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A4" s="96" t="s">
+    <row r="4" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A4" s="79" t="s">
         <v>201</v>
       </c>
-      <c r="E4" s="95">
+      <c r="E4" s="78">
         <v>191</v>
       </c>
-      <c r="I4" s="95">
+      <c r="I4" s="78">
         <v>191</v>
       </c>
-      <c r="M4" s="95">
+      <c r="M4" s="78">
         <v>191</v>
       </c>
-      <c r="N4" s="95">
+      <c r="N4" s="78">
         <v>191</v>
       </c>
-      <c r="O4" s="95">
+      <c r="O4" s="78">
         <v>191</v>
       </c>
-      <c r="P4" s="95">
+      <c r="P4" s="78">
         <v>191</v>
       </c>
-      <c r="Q4" s="95">
+      <c r="Q4" s="78">
         <v>191</v>
       </c>
-      <c r="R4" s="95">
+      <c r="R4" s="78">
         <v>191</v>
       </c>
-      <c r="S4" s="95">
+      <c r="S4" s="78">
         <v>191</v>
       </c>
-      <c r="Z4" s="95">
+      <c r="X4" s="78">
+        <v>193</v>
+      </c>
+      <c r="Y4" s="78">
         <v>191</v>
       </c>
-      <c r="AA4" s="95">
+      <c r="Z4" s="78">
         <v>191</v>
       </c>
-      <c r="AB4" s="95">
+      <c r="AA4" s="78">
         <v>191</v>
       </c>
-      <c r="AC4" s="95">
+      <c r="AB4" s="78">
         <v>191</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A5" s="96" t="s">
+      <c r="AC4" s="78">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A5" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="95">
+      <c r="E5" s="78">
         <v>771</v>
       </c>
-      <c r="I5" s="95">
+      <c r="I5" s="78">
         <v>815</v>
       </c>
-      <c r="M5" s="95">
+      <c r="M5" s="78">
         <v>798</v>
       </c>
-      <c r="N5" s="95">
+      <c r="N5" s="78">
         <v>798</v>
       </c>
-      <c r="O5" s="95">
+      <c r="O5" s="78">
         <v>816</v>
       </c>
-      <c r="P5" s="95">
+      <c r="P5" s="78">
         <v>832</v>
       </c>
-      <c r="Q5" s="95">
+      <c r="Q5" s="78">
         <v>840</v>
       </c>
-      <c r="R5" s="95">
+      <c r="R5" s="78">
         <v>840</v>
       </c>
-      <c r="S5" s="95">
+      <c r="S5" s="78">
         <v>848</v>
       </c>
-      <c r="Z5" s="95">
+      <c r="X5" s="78">
+        <v>525</v>
+      </c>
+      <c r="Y5" s="78">
+        <v>603</v>
+      </c>
+      <c r="Z5" s="78">
         <v>771</v>
       </c>
-      <c r="AA5" s="95">
+      <c r="AA5" s="78">
         <v>815</v>
       </c>
-      <c r="AB5" s="95">
+      <c r="AB5" s="78">
         <v>798</v>
       </c>
-      <c r="AC5" s="95">
+      <c r="AC5" s="78">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A6" s="96" t="s">
+    <row r="6" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A6" s="79" t="s">
         <v>185</v>
       </c>
-      <c r="E6" s="95">
+      <c r="E6" s="78">
         <v>566</v>
       </c>
-      <c r="I6" s="95">
+      <c r="I6" s="78">
         <v>568</v>
       </c>
-      <c r="M6" s="95">
+      <c r="M6" s="78">
         <v>568</v>
       </c>
-      <c r="N6" s="95">
+      <c r="N6" s="78">
         <v>568</v>
       </c>
-      <c r="O6" s="95">
+      <c r="O6" s="78">
         <v>568</v>
       </c>
-      <c r="P6" s="95">
+      <c r="P6" s="78">
         <v>568</v>
       </c>
-      <c r="Q6" s="95">
+      <c r="Q6" s="78">
         <v>568</v>
       </c>
-      <c r="R6" s="95">
+      <c r="R6" s="78">
         <v>568</v>
       </c>
-      <c r="S6" s="95">
+      <c r="S6" s="78">
         <v>568</v>
       </c>
-      <c r="Z6" s="95">
+      <c r="X6" s="78">
+        <v>590</v>
+      </c>
+      <c r="Y6" s="78">
+        <v>592</v>
+      </c>
+      <c r="Z6" s="78">
         <v>566</v>
       </c>
-      <c r="AA6" s="95">
+      <c r="AA6" s="78">
         <v>568</v>
       </c>
-      <c r="AB6" s="95">
+      <c r="AB6" s="78">
         <v>568</v>
       </c>
-      <c r="AC6" s="95">
+      <c r="AC6" s="78">
         <v>568</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A7" s="96" t="s">
+    <row r="7" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A7" s="79" t="s">
         <v>188</v>
       </c>
-      <c r="E7" s="95">
+      <c r="E7" s="78">
         <v>172</v>
       </c>
-      <c r="I7" s="95">
+      <c r="I7" s="78">
         <v>172</v>
       </c>
-      <c r="M7" s="95">
+      <c r="M7" s="78">
         <v>172</v>
       </c>
-      <c r="N7" s="95">
+      <c r="N7" s="78">
         <v>172</v>
       </c>
-      <c r="O7" s="95">
+      <c r="O7" s="78">
         <v>172</v>
       </c>
-      <c r="P7" s="95">
+      <c r="P7" s="78">
         <v>172</v>
       </c>
-      <c r="Q7" s="95">
+      <c r="Q7" s="78">
         <v>172</v>
       </c>
-      <c r="R7" s="95">
+      <c r="R7" s="78">
         <v>172</v>
       </c>
-      <c r="S7" s="95">
+      <c r="S7" s="78">
         <v>172</v>
       </c>
-      <c r="Z7" s="95">
+      <c r="X7" s="78">
+        <v>166</v>
+      </c>
+      <c r="Y7" s="78">
+        <v>169</v>
+      </c>
+      <c r="Z7" s="78">
         <v>172</v>
       </c>
-      <c r="AA7" s="95">
+      <c r="AA7" s="78">
         <v>172</v>
       </c>
-      <c r="AB7" s="95">
+      <c r="AB7" s="78">
         <v>172</v>
       </c>
-      <c r="AC7" s="95">
+      <c r="AC7" s="78">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A8" s="96" t="s">
+    <row r="8" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A8" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="E8" s="78">
+        <v>0</v>
+      </c>
+      <c r="F8" s="78">
+        <v>0</v>
+      </c>
+      <c r="G8" s="78">
+        <v>0</v>
+      </c>
+      <c r="H8" s="78">
+        <v>0</v>
+      </c>
+      <c r="I8" s="78">
+        <v>0</v>
+      </c>
+      <c r="J8" s="78">
+        <v>0</v>
+      </c>
+      <c r="K8" s="78">
+        <v>0</v>
+      </c>
+      <c r="L8" s="78">
+        <v>0</v>
+      </c>
+      <c r="M8" s="78">
+        <v>0</v>
+      </c>
+      <c r="N8" s="78">
+        <v>0</v>
+      </c>
+      <c r="O8" s="78">
+        <v>0</v>
+      </c>
+      <c r="P8" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="78">
+        <v>0</v>
+      </c>
+      <c r="R8" s="78">
+        <v>0</v>
+      </c>
+      <c r="S8" s="78">
+        <v>0</v>
+      </c>
+      <c r="X8" s="78">
+        <v>100</v>
+      </c>
+      <c r="Y8" s="78">
+        <v>100</v>
+      </c>
+      <c r="Z8" s="78">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="78">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="78">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A9" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="E8" s="95">
+      <c r="E9" s="78">
         <v>47</v>
       </c>
-      <c r="I8" s="95">
+      <c r="I9" s="78">
         <v>27</v>
       </c>
-      <c r="M8" s="95">
+      <c r="M9" s="78">
         <v>22</v>
       </c>
-      <c r="N8" s="95">
+      <c r="N9" s="78">
         <v>22</v>
       </c>
-      <c r="O8" s="95">
+      <c r="O9" s="78">
         <v>22</v>
       </c>
-      <c r="P8" s="95">
+      <c r="P9" s="78">
         <v>22</v>
       </c>
-      <c r="Q8" s="95">
+      <c r="Q9" s="78">
         <v>22</v>
       </c>
-      <c r="R8" s="95">
+      <c r="R9" s="78">
         <v>20</v>
       </c>
-      <c r="S8" s="95">
+      <c r="S9" s="78">
         <v>20</v>
       </c>
-      <c r="Z8" s="95">
+      <c r="X9" s="78">
+        <v>85</v>
+      </c>
+      <c r="Y9" s="78">
+        <v>74</v>
+      </c>
+      <c r="Z9" s="78">
         <v>47</v>
       </c>
-      <c r="AA8" s="95">
+      <c r="AA9" s="78">
         <v>27</v>
       </c>
-      <c r="AB8" s="95">
+      <c r="AB9" s="78">
         <v>22</v>
       </c>
-      <c r="AC8" s="95">
+      <c r="AC9" s="78">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A9" s="96" t="s">
+    <row r="10" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A10" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="95">
+      <c r="E10" s="78">
         <v>111</v>
       </c>
-      <c r="I9" s="95">
+      <c r="I10" s="78">
         <v>144</v>
       </c>
-      <c r="M9" s="95">
+      <c r="M10" s="78">
         <v>153</v>
       </c>
-      <c r="N9" s="95">
+      <c r="N10" s="78">
         <v>153</v>
       </c>
-      <c r="O9" s="95">
+      <c r="O10" s="78">
         <v>183</v>
       </c>
-      <c r="P9" s="95">
+      <c r="P10" s="78">
         <v>183</v>
       </c>
-      <c r="Q9" s="95">
+      <c r="Q10" s="78">
         <v>203</v>
       </c>
-      <c r="R9" s="95">
+      <c r="R10" s="78">
         <v>201</v>
       </c>
-      <c r="S9" s="95">
+      <c r="S10" s="78">
         <v>201</v>
       </c>
-      <c r="Z9" s="95">
+      <c r="X10" s="78">
+        <v>90</v>
+      </c>
+      <c r="Y10" s="78">
+        <v>106</v>
+      </c>
+      <c r="Z10" s="78">
         <v>111</v>
       </c>
-      <c r="AA9" s="95">
+      <c r="AA10" s="78">
         <v>144</v>
       </c>
-      <c r="AB9" s="95">
+      <c r="AB10" s="78">
         <v>153</v>
       </c>
-      <c r="AC9" s="95">
+      <c r="AC10" s="78">
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="95" customFormat="1" ht="13"/>
-    <row r="11" spans="1:33" s="94" customFormat="1" ht="13">
-      <c r="A11" s="94" t="s">
+    <row r="11" spans="1:33" s="78" customFormat="1" ht="13"/>
+    <row r="12" spans="1:33" s="77" customFormat="1" ht="13">
+      <c r="A12" s="77" t="s">
         <v>212</v>
       </c>
-      <c r="B11" s="94">
-        <f t="shared" ref="B11" si="19">SUM(B12:B17)</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="94">
-        <f t="shared" ref="C11" si="20">SUM(C12:C17)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="94">
-        <f t="shared" ref="D11" si="21">SUM(D12:D17)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="94">
-        <f t="shared" ref="E11" si="22">SUM(E12:E17)</f>
+      <c r="B12" s="77">
+        <f>SUM(B13:B19)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="77">
+        <f>SUM(C13:C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="77">
+        <f>SUM(D13:D19)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="77">
+        <f>SUM(E13:E19)</f>
         <v>1490</v>
       </c>
-      <c r="F11" s="94">
-        <f t="shared" ref="F11" si="23">SUM(F12:F17)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="94">
-        <f t="shared" ref="G11" si="24">SUM(G12:G17)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="94">
-        <f t="shared" ref="H11" si="25">SUM(H12:H17)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="94">
-        <f t="shared" ref="I11" si="26">SUM(I12:I17)</f>
+      <c r="F12" s="77">
+        <f>SUM(F13:F19)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="77">
+        <f>SUM(G13:G19)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="77">
+        <f>SUM(H13:H19)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="77">
+        <f>SUM(I13:I19)</f>
         <v>1579</v>
       </c>
-      <c r="J11" s="94">
-        <f t="shared" ref="J11" si="27">SUM(J12:J17)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="94">
-        <f t="shared" ref="K11" si="28">SUM(K12:K17)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="94">
-        <f t="shared" ref="L11" si="29">SUM(L12:L17)</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="94">
-        <f t="shared" ref="M11" si="30">SUM(M12:M17)</f>
+      <c r="J12" s="77">
+        <f>SUM(J13:J19)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="77">
+        <f>SUM(K13:K19)</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="77">
+        <f>SUM(L13:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="77">
+        <f>SUM(M13:M19)</f>
         <v>1623</v>
       </c>
-      <c r="N11" s="94">
-        <f t="shared" ref="N11:Q11" si="31">SUM(N12:N17)</f>
+      <c r="N12" s="77">
+        <f>SUM(N13:N19)</f>
         <v>1632</v>
       </c>
-      <c r="O11" s="94">
-        <f t="shared" ref="O11" si="32">SUM(O12:O17)</f>
+      <c r="O12" s="77">
+        <f>SUM(O13:O19)</f>
         <v>1646</v>
       </c>
-      <c r="P11" s="94">
-        <f t="shared" si="31"/>
+      <c r="P12" s="77">
+        <f>SUM(P13:P19)</f>
         <v>1655</v>
       </c>
-      <c r="Q11" s="94">
-        <f t="shared" si="31"/>
+      <c r="Q12" s="77">
+        <f>SUM(Q13:Q19)</f>
         <v>1671</v>
       </c>
-      <c r="R11" s="94">
-        <f>SUM(R12:R17)</f>
+      <c r="R12" s="77">
+        <f>SUM(R13:R19)</f>
         <v>1677</v>
       </c>
-      <c r="S11" s="94">
-        <f t="shared" ref="S11" si="33">SUM(S12:S17)</f>
+      <c r="S12" s="77">
+        <f>SUM(S13:S19)</f>
         <v>1688</v>
       </c>
-      <c r="Z11" s="94">
-        <f t="shared" ref="Z11" si="34">SUM(Z12:Z17)</f>
+      <c r="X12" s="77">
+        <f>SUM(X13:X19)</f>
+        <v>1299</v>
+      </c>
+      <c r="Y12" s="77">
+        <f>SUM(Y13:Y19)</f>
+        <v>1400</v>
+      </c>
+      <c r="Z12" s="77">
+        <f>SUM(Z13:Z19)</f>
         <v>1490</v>
       </c>
-      <c r="AA11" s="94">
-        <f t="shared" ref="AA11" si="35">SUM(AA12:AA17)</f>
+      <c r="AA12" s="77">
+        <f>SUM(AA13:AA19)</f>
         <v>1579</v>
       </c>
-      <c r="AB11" s="94">
-        <f t="shared" ref="AB11" si="36">SUM(AB12:AB17)</f>
+      <c r="AB12" s="77">
+        <f>SUM(AB13:AB19)</f>
         <v>1623</v>
       </c>
-      <c r="AC11" s="94">
-        <f t="shared" ref="AC11" si="37">SUM(AC12:AC17)</f>
+      <c r="AC12" s="77">
+        <f>SUM(AC13:AC19)</f>
         <v>1671</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A12" s="96" t="s">
+    <row r="13" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A13" s="79" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="95">
+      <c r="E13" s="78">
         <v>191</v>
       </c>
-      <c r="I12" s="95">
+      <c r="I13" s="78">
         <v>191</v>
       </c>
-      <c r="M12" s="95">
+      <c r="M13" s="78">
         <v>191</v>
       </c>
-      <c r="N12" s="95">
+      <c r="N13" s="78">
         <v>191</v>
       </c>
-      <c r="O12" s="95">
+      <c r="O13" s="78">
         <v>191</v>
       </c>
-      <c r="P12" s="95">
+      <c r="P13" s="78">
         <v>191</v>
       </c>
-      <c r="Q12" s="95">
+      <c r="Q13" s="78">
         <v>191</v>
       </c>
-      <c r="R12" s="95">
+      <c r="R13" s="78">
         <v>191</v>
       </c>
-      <c r="S12" s="95">
+      <c r="S13" s="78">
         <v>191</v>
       </c>
-      <c r="Z12" s="95">
+      <c r="X13" s="78">
+        <v>190</v>
+      </c>
+      <c r="Y13" s="78">
+        <v>190</v>
+      </c>
+      <c r="Z13" s="78">
         <v>191</v>
       </c>
-      <c r="AA12" s="95">
+      <c r="AA13" s="78">
         <v>191</v>
       </c>
-      <c r="AB12" s="95">
+      <c r="AB13" s="78">
         <v>191</v>
       </c>
-      <c r="AC12" s="95">
+      <c r="AC13" s="78">
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A13" s="96" t="s">
+    <row r="14" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A14" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="95">
+      <c r="E14" s="78">
         <v>567</v>
       </c>
-      <c r="I13" s="95">
+      <c r="I14" s="78">
         <v>634</v>
       </c>
-      <c r="M13" s="95">
+      <c r="M14" s="78">
         <v>666</v>
       </c>
-      <c r="N13" s="95">
+      <c r="N14" s="78">
         <v>668</v>
       </c>
-      <c r="O13" s="95">
+      <c r="O14" s="78">
         <v>675</v>
       </c>
-      <c r="P13" s="95">
+      <c r="P14" s="78">
         <v>681</v>
       </c>
-      <c r="Q13" s="95">
+      <c r="Q14" s="78">
         <v>693</v>
       </c>
-      <c r="R13" s="95">
+      <c r="R14" s="78">
         <v>697</v>
       </c>
-      <c r="S13" s="95">
+      <c r="S14" s="78">
         <v>705</v>
       </c>
-      <c r="Z13" s="95">
+      <c r="X14" s="78">
+        <v>421</v>
+      </c>
+      <c r="Y14" s="78">
+        <v>500</v>
+      </c>
+      <c r="Z14" s="78">
         <v>567</v>
       </c>
-      <c r="AA13" s="95">
+      <c r="AA14" s="78">
         <v>634</v>
       </c>
-      <c r="AB13" s="95">
+      <c r="AB14" s="78">
         <v>666</v>
       </c>
-      <c r="AC13" s="95">
+      <c r="AC14" s="78">
         <v>693</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A14" s="96" t="s">
+    <row r="15" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A15" s="79" t="s">
         <v>185</v>
       </c>
-      <c r="E14" s="95">
+      <c r="E15" s="78">
         <v>559</v>
       </c>
-      <c r="I14" s="95">
+      <c r="I15" s="78">
         <v>564</v>
       </c>
-      <c r="M14" s="95">
+      <c r="M15" s="78">
         <v>565</v>
       </c>
-      <c r="N14" s="95">
+      <c r="N15" s="78">
         <v>565</v>
       </c>
-      <c r="O14" s="95">
+      <c r="O15" s="78">
         <v>565</v>
       </c>
-      <c r="P14" s="95">
+      <c r="P15" s="78">
         <v>565</v>
       </c>
-      <c r="Q14" s="95">
+      <c r="Q15" s="78">
         <v>565</v>
       </c>
-      <c r="R14" s="95">
+      <c r="R15" s="78">
         <v>565</v>
       </c>
-      <c r="S14" s="95">
+      <c r="S15" s="78">
         <v>565</v>
       </c>
-      <c r="Z14" s="95">
+      <c r="X15" s="78">
+        <v>534</v>
+      </c>
+      <c r="Y15" s="78">
+        <v>546</v>
+      </c>
+      <c r="Z15" s="78">
         <v>559</v>
       </c>
-      <c r="AA14" s="95">
+      <c r="AA15" s="78">
         <v>564</v>
       </c>
-      <c r="AB14" s="95">
+      <c r="AB15" s="78">
         <v>565</v>
       </c>
-      <c r="AC14" s="95">
+      <c r="AC15" s="78">
         <v>565</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A15" s="96" t="s">
+    <row r="16" spans="1:33" s="78" customFormat="1" ht="13">
+      <c r="A16" s="79" t="s">
         <v>188</v>
       </c>
-      <c r="E15" s="95">
+      <c r="E16" s="78">
         <v>169</v>
       </c>
-      <c r="I15" s="95">
+      <c r="I16" s="78">
         <v>172</v>
       </c>
-      <c r="M15" s="95">
+      <c r="M16" s="78">
         <v>172</v>
       </c>
-      <c r="N15" s="95">
+      <c r="N16" s="78">
         <v>172</v>
       </c>
-      <c r="O15" s="95">
+      <c r="O16" s="78">
         <v>172</v>
       </c>
-      <c r="P15" s="95">
+      <c r="P16" s="78">
         <v>172</v>
       </c>
-      <c r="Q15" s="95">
+      <c r="Q16" s="78">
         <v>172</v>
       </c>
-      <c r="R15" s="95">
+      <c r="R16" s="78">
         <v>172</v>
       </c>
-      <c r="S15" s="95">
+      <c r="S16" s="78">
         <v>172</v>
       </c>
-      <c r="Z15" s="95">
+      <c r="X16" s="78">
+        <v>154</v>
+      </c>
+      <c r="Y16" s="78">
+        <v>164</v>
+      </c>
+      <c r="Z16" s="78">
         <v>169</v>
       </c>
-      <c r="AA15" s="95">
+      <c r="AA16" s="78">
         <v>172</v>
       </c>
-      <c r="AB15" s="95">
+      <c r="AB16" s="78">
         <v>172</v>
       </c>
-      <c r="AC15" s="95">
+      <c r="AC16" s="78">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="95" customFormat="1" ht="13">
-      <c r="A16" s="96" t="s">
+    <row r="17" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A17" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="E17" s="78">
+        <v>0</v>
+      </c>
+      <c r="F17" s="78">
+        <v>0</v>
+      </c>
+      <c r="G17" s="78">
+        <v>0</v>
+      </c>
+      <c r="H17" s="78">
+        <v>0</v>
+      </c>
+      <c r="I17" s="78">
+        <v>0</v>
+      </c>
+      <c r="J17" s="78">
+        <v>0</v>
+      </c>
+      <c r="K17" s="78">
+        <v>0</v>
+      </c>
+      <c r="L17" s="78">
+        <v>0</v>
+      </c>
+      <c r="M17" s="78">
+        <v>0</v>
+      </c>
+      <c r="N17" s="78">
+        <v>0</v>
+      </c>
+      <c r="O17" s="78">
+        <v>0</v>
+      </c>
+      <c r="P17" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="78">
+        <v>0</v>
+      </c>
+      <c r="R17" s="78">
+        <v>0</v>
+      </c>
+      <c r="S17" s="78">
+        <v>0</v>
+      </c>
+      <c r="X17" s="78">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="78">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="78">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="78">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="78">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A18" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="E16" s="95">
+      <c r="E18" s="78">
         <v>4</v>
       </c>
-      <c r="I16" s="95">
+      <c r="I18" s="78">
         <v>11</v>
       </c>
-      <c r="M16" s="95">
+      <c r="M18" s="78">
         <v>15</v>
       </c>
-      <c r="N16" s="95">
+      <c r="N18" s="78">
         <v>17</v>
       </c>
-      <c r="O16" s="95">
+      <c r="O18" s="78">
         <v>17</v>
       </c>
-      <c r="P16" s="95">
+      <c r="P18" s="78">
         <v>17</v>
       </c>
-      <c r="Q16" s="95">
+      <c r="Q18" s="78">
         <v>17</v>
       </c>
-      <c r="R16" s="95">
+      <c r="R18" s="78">
         <v>17</v>
       </c>
-      <c r="S16" s="95">
+      <c r="S18" s="78">
         <v>17</v>
       </c>
-      <c r="Z16" s="95">
+      <c r="X18" s="78">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="78">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="78">
         <v>4</v>
       </c>
-      <c r="AA16" s="95">
+      <c r="AA18" s="78">
         <v>11</v>
       </c>
-      <c r="AB16" s="95">
+      <c r="AB18" s="78">
         <v>15</v>
       </c>
-      <c r="AC16" s="95">
+      <c r="AC18" s="78">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A17" s="96" t="s">
+    <row r="19" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A19" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="95">
-        <v>0</v>
-      </c>
-      <c r="I17" s="95">
+      <c r="E19" s="78">
+        <v>0</v>
+      </c>
+      <c r="I19" s="78">
         <v>7</v>
       </c>
-      <c r="M17" s="95">
+      <c r="M19" s="78">
         <v>14</v>
       </c>
-      <c r="N17" s="95">
+      <c r="N19" s="78">
         <v>19</v>
       </c>
-      <c r="O17" s="95">
+      <c r="O19" s="78">
         <v>26</v>
       </c>
-      <c r="P17" s="95">
+      <c r="P19" s="78">
         <v>29</v>
       </c>
-      <c r="Q17" s="95">
+      <c r="Q19" s="78">
         <v>33</v>
       </c>
-      <c r="R17" s="95">
+      <c r="R19" s="78">
         <v>35</v>
       </c>
-      <c r="S17" s="95">
+      <c r="S19" s="78">
         <v>38</v>
       </c>
-      <c r="Z17" s="95">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="95">
+      <c r="X19" s="78">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="78">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="78">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="78">
         <v>7</v>
       </c>
-      <c r="AB17" s="95">
+      <c r="AB19" s="78">
         <v>14</v>
       </c>
-      <c r="AC17" s="95">
+      <c r="AC19" s="78">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A18" s="96"/>
-    </row>
-    <row r="19" spans="1:29" s="94" customFormat="1" ht="13">
-      <c r="A19" s="94" t="s">
+    <row r="20" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A20" s="79"/>
+    </row>
+    <row r="21" spans="1:29" s="77" customFormat="1" ht="13">
+      <c r="A21" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="B19" s="94">
-        <f t="shared" ref="B19" si="38">SUM(B20:B25)</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="94">
-        <f t="shared" ref="C19" si="39">SUM(C20:C25)</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="94">
-        <f t="shared" ref="D19" si="40">SUM(D20:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="94">
-        <f t="shared" ref="E19" si="41">SUM(E20:E25)</f>
+      <c r="B21" s="77">
+        <f>SUM(B22:B28)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="77">
+        <f>SUM(C22:C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="77">
+        <f>SUM(D22:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="77">
+        <f>SUM(E22:E28)</f>
         <v>368</v>
       </c>
-      <c r="F19" s="94">
-        <f t="shared" ref="F19" si="42">SUM(F20:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="94">
-        <f t="shared" ref="G19" si="43">SUM(G20:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="94">
-        <f t="shared" ref="H19" si="44">SUM(H20:H25)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="94">
-        <f t="shared" ref="I19" si="45">SUM(I20:I25)</f>
+      <c r="F21" s="77">
+        <f>SUM(F22:F28)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="77">
+        <f>SUM(G22:G28)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="77">
+        <f>SUM(H22:H28)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="77">
+        <f>SUM(I22:I28)</f>
         <v>338</v>
       </c>
-      <c r="J19" s="94">
-        <f t="shared" ref="J19" si="46">SUM(J20:J25)</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="94">
-        <f t="shared" ref="K19" si="47">SUM(K20:K25)</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="94">
-        <f t="shared" ref="L19" si="48">SUM(L20:L25)</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="94">
-        <f t="shared" ref="M19" si="49">SUM(M20:M25)</f>
+      <c r="J21" s="77">
+        <f>SUM(J22:J28)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="77">
+        <f>SUM(K22:K28)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="77">
+        <f>SUM(L22:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="77">
+        <f>SUM(M22:M28)</f>
         <v>281</v>
       </c>
-      <c r="N19" s="94">
-        <f t="shared" ref="N19:Q19" si="50">SUM(N20:N25)</f>
+      <c r="N21" s="77">
+        <f>SUM(N22:N28)</f>
         <v>272</v>
       </c>
-      <c r="O19" s="94">
-        <f t="shared" ref="O19" si="51">SUM(O20:O25)</f>
+      <c r="O21" s="77">
+        <f>SUM(O22:O28)</f>
         <v>306</v>
       </c>
-      <c r="P19" s="94">
-        <f t="shared" si="50"/>
+      <c r="P21" s="77">
+        <f>SUM(P22:P28)</f>
         <v>313</v>
       </c>
-      <c r="Q19" s="94">
-        <f t="shared" si="50"/>
+      <c r="Q21" s="77">
+        <f>SUM(Q22:Q28)</f>
         <v>325</v>
       </c>
-      <c r="R19" s="94">
-        <f>SUM(R20:R25)</f>
+      <c r="R21" s="77">
+        <f>SUM(R22:R28)</f>
         <v>315</v>
       </c>
-      <c r="S19" s="94">
-        <f t="shared" ref="S19" si="52">SUM(S20:S25)</f>
+      <c r="S21" s="77">
+        <f>SUM(S22:S28)</f>
         <v>312</v>
       </c>
-      <c r="Z19" s="94">
-        <f t="shared" ref="Z19" si="53">SUM(Z20:Z25)</f>
+      <c r="X21" s="77">
+        <f>SUM(X22:X28)</f>
+        <v>450</v>
+      </c>
+      <c r="Y21" s="77">
+        <f>SUM(Y22:Y28)</f>
+        <v>435</v>
+      </c>
+      <c r="Z21" s="77">
+        <f>SUM(Z22:Z28)</f>
         <v>368</v>
       </c>
-      <c r="AA19" s="94">
-        <f t="shared" ref="AA19" si="54">SUM(AA20:AA25)</f>
+      <c r="AA21" s="77">
+        <f>SUM(AA22:AA28)</f>
         <v>338</v>
       </c>
-      <c r="AB19" s="94">
-        <f t="shared" ref="AB19" si="55">SUM(AB20:AB25)</f>
+      <c r="AB21" s="77">
+        <f>SUM(AB22:AB28)</f>
         <v>281</v>
       </c>
-      <c r="AC19" s="94">
-        <f t="shared" ref="AC19" si="56">SUM(AC20:AC25)</f>
+      <c r="AC21" s="77">
+        <f>SUM(AC22:AC28)</f>
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A20" s="96" t="s">
+    <row r="22" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A22" s="79" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="95">
-        <v>0</v>
-      </c>
-      <c r="I20" s="95">
-        <v>0</v>
-      </c>
-      <c r="M20" s="95">
-        <v>0</v>
-      </c>
-      <c r="N20" s="95">
-        <v>0</v>
-      </c>
-      <c r="O20" s="95">
-        <v>0</v>
-      </c>
-      <c r="P20" s="95">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="95">
-        <v>0</v>
-      </c>
-      <c r="R20" s="95">
-        <v>0</v>
-      </c>
-      <c r="S20" s="95">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="95">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="95">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="95">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A21" s="96" t="s">
+      <c r="E22" s="78">
+        <v>0</v>
+      </c>
+      <c r="I22" s="78">
+        <v>0</v>
+      </c>
+      <c r="M22" s="78">
+        <v>0</v>
+      </c>
+      <c r="N22" s="78">
+        <v>0</v>
+      </c>
+      <c r="O22" s="78">
+        <v>0</v>
+      </c>
+      <c r="P22" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="78">
+        <v>0</v>
+      </c>
+      <c r="R22" s="78">
+        <v>0</v>
+      </c>
+      <c r="S22" s="78">
+        <v>0</v>
+      </c>
+      <c r="X22" s="78">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="78">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="78">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="78">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="78">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A23" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="95">
+      <c r="E23" s="78">
         <v>204</v>
       </c>
-      <c r="I21" s="95">
+      <c r="I23" s="78">
         <v>181</v>
       </c>
-      <c r="M21" s="95">
+      <c r="M23" s="78">
         <v>132</v>
       </c>
-      <c r="N21" s="95">
+      <c r="N23" s="78">
         <v>130</v>
       </c>
-      <c r="O21" s="95">
+      <c r="O23" s="78">
         <v>141</v>
       </c>
-      <c r="P21" s="95">
+      <c r="P23" s="78">
         <v>151</v>
       </c>
-      <c r="Q21" s="95">
+      <c r="Q23" s="78">
         <v>147</v>
       </c>
-      <c r="R21" s="95">
+      <c r="R23" s="78">
         <v>143</v>
       </c>
-      <c r="S21" s="95">
+      <c r="S23" s="78">
         <v>143</v>
       </c>
-      <c r="Z21" s="95">
+      <c r="X23" s="78">
+        <v>104</v>
+      </c>
+      <c r="Y23" s="78">
+        <v>103</v>
+      </c>
+      <c r="Z23" s="78">
         <v>204</v>
       </c>
-      <c r="AA21" s="95">
+      <c r="AA23" s="78">
         <v>181</v>
       </c>
-      <c r="AB21" s="95">
+      <c r="AB23" s="78">
         <v>132</v>
       </c>
-      <c r="AC21" s="95">
+      <c r="AC23" s="78">
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A22" s="96" t="s">
+    <row r="24" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A24" s="79" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="95">
+      <c r="E24" s="78">
         <v>7</v>
       </c>
-      <c r="I22" s="95">
+      <c r="I24" s="78">
         <v>4</v>
       </c>
-      <c r="M22" s="95">
+      <c r="M24" s="78">
         <v>3</v>
       </c>
-      <c r="N22" s="95">
+      <c r="N24" s="78">
         <v>3</v>
       </c>
-      <c r="O22" s="95">
+      <c r="O24" s="78">
         <v>3</v>
       </c>
-      <c r="P22" s="95">
+      <c r="P24" s="78">
         <v>3</v>
       </c>
-      <c r="Q22" s="95">
+      <c r="Q24" s="78">
         <v>3</v>
       </c>
-      <c r="R22" s="95">
+      <c r="R24" s="78">
         <v>3</v>
       </c>
-      <c r="S22" s="95">
+      <c r="S24" s="78">
         <v>3</v>
       </c>
-      <c r="Z22" s="95">
+      <c r="X24" s="78">
+        <v>56</v>
+      </c>
+      <c r="Y24" s="78">
+        <v>46</v>
+      </c>
+      <c r="Z24" s="78">
         <v>7</v>
       </c>
-      <c r="AA22" s="95">
+      <c r="AA24" s="78">
         <v>4</v>
       </c>
-      <c r="AB22" s="95">
+      <c r="AB24" s="78">
         <v>3</v>
       </c>
-      <c r="AC22" s="95">
+      <c r="AC24" s="78">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A23" s="96" t="s">
+    <row r="25" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A25" s="79" t="s">
         <v>188</v>
       </c>
-      <c r="E23" s="95">
+      <c r="E25" s="78">
         <v>3</v>
       </c>
-      <c r="I23" s="95">
-        <v>0</v>
-      </c>
-      <c r="M23" s="95">
-        <v>0</v>
-      </c>
-      <c r="N23" s="95">
-        <v>0</v>
-      </c>
-      <c r="O23" s="95">
-        <v>0</v>
-      </c>
-      <c r="P23" s="95">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="95">
-        <v>0</v>
-      </c>
-      <c r="R23" s="95">
-        <v>0</v>
-      </c>
-      <c r="S23" s="95">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="95">
+      <c r="I25" s="78">
+        <v>0</v>
+      </c>
+      <c r="M25" s="78">
+        <v>0</v>
+      </c>
+      <c r="N25" s="78">
+        <v>0</v>
+      </c>
+      <c r="O25" s="78">
+        <v>0</v>
+      </c>
+      <c r="P25" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="78">
+        <v>0</v>
+      </c>
+      <c r="R25" s="78">
+        <v>0</v>
+      </c>
+      <c r="S25" s="78">
+        <v>0</v>
+      </c>
+      <c r="X25" s="78">
+        <v>12</v>
+      </c>
+      <c r="Y25" s="78">
+        <v>5</v>
+      </c>
+      <c r="Z25" s="78">
         <v>3</v>
       </c>
-      <c r="AA23" s="95">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="95">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A24" s="96" t="s">
+      <c r="AA25" s="78">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="78">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A26" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" s="78">
+        <v>0</v>
+      </c>
+      <c r="F26" s="78">
+        <v>0</v>
+      </c>
+      <c r="G26" s="78">
+        <v>0</v>
+      </c>
+      <c r="H26" s="78">
+        <v>0</v>
+      </c>
+      <c r="I26" s="78">
+        <v>0</v>
+      </c>
+      <c r="J26" s="78">
+        <v>0</v>
+      </c>
+      <c r="K26" s="78">
+        <v>0</v>
+      </c>
+      <c r="L26" s="78">
+        <v>0</v>
+      </c>
+      <c r="M26" s="78">
+        <v>0</v>
+      </c>
+      <c r="N26" s="78">
+        <v>0</v>
+      </c>
+      <c r="O26" s="78">
+        <v>0</v>
+      </c>
+      <c r="P26" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="78">
+        <v>0</v>
+      </c>
+      <c r="R26" s="78">
+        <v>0</v>
+      </c>
+      <c r="S26" s="78">
+        <v>0</v>
+      </c>
+      <c r="X26" s="78">
+        <v>100</v>
+      </c>
+      <c r="Y26" s="78">
+        <v>100</v>
+      </c>
+      <c r="Z26" s="78">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="78">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="78">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A27" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="E24" s="95">
+      <c r="E27" s="78">
         <v>43</v>
       </c>
-      <c r="I24" s="95">
+      <c r="I27" s="78">
         <v>16</v>
       </c>
-      <c r="M24" s="95">
+      <c r="M27" s="78">
         <v>7</v>
       </c>
-      <c r="N24" s="95">
+      <c r="N27" s="78">
         <v>5</v>
       </c>
-      <c r="O24" s="95">
+      <c r="O27" s="78">
         <v>5</v>
       </c>
-      <c r="P24" s="95">
+      <c r="P27" s="78">
         <v>5</v>
       </c>
-      <c r="Q24" s="95">
+      <c r="Q27" s="78">
         <v>5</v>
       </c>
-      <c r="R24" s="95">
+      <c r="R27" s="78">
         <v>3</v>
       </c>
-      <c r="S24" s="95">
+      <c r="S27" s="78">
         <v>3</v>
       </c>
-      <c r="Z24" s="95">
+      <c r="X27" s="78">
+        <v>85</v>
+      </c>
+      <c r="Y27" s="78">
+        <v>74</v>
+      </c>
+      <c r="Z27" s="78">
         <v>43</v>
       </c>
-      <c r="AA24" s="95">
+      <c r="AA27" s="78">
         <v>16</v>
       </c>
-      <c r="AB24" s="95">
+      <c r="AB27" s="78">
         <v>7</v>
       </c>
-      <c r="AC24" s="95">
+      <c r="AC27" s="78">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="95" customFormat="1" ht="13">
-      <c r="A25" s="96" t="s">
+    <row r="28" spans="1:29" s="78" customFormat="1" ht="13">
+      <c r="A28" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="95">
+      <c r="E28" s="78">
         <v>111</v>
       </c>
-      <c r="I25" s="95">
+      <c r="I28" s="78">
         <v>137</v>
       </c>
-      <c r="M25" s="95">
+      <c r="M28" s="78">
         <v>139</v>
       </c>
-      <c r="N25" s="95">
+      <c r="N28" s="78">
         <v>134</v>
       </c>
-      <c r="O25" s="95">
+      <c r="O28" s="78">
         <v>157</v>
       </c>
-      <c r="P25" s="95">
+      <c r="P28" s="78">
         <v>154</v>
       </c>
-      <c r="Q25" s="95">
+      <c r="Q28" s="78">
         <v>170</v>
       </c>
-      <c r="R25" s="95">
+      <c r="R28" s="78">
         <v>166</v>
       </c>
-      <c r="S25" s="95">
+      <c r="S28" s="78">
         <v>163</v>
       </c>
-      <c r="Z25" s="95">
+      <c r="X28" s="78">
+        <v>90</v>
+      </c>
+      <c r="Y28" s="78">
+        <v>106</v>
+      </c>
+      <c r="Z28" s="78">
         <v>111</v>
       </c>
-      <c r="AA25" s="95">
+      <c r="AA28" s="78">
         <v>137</v>
       </c>
-      <c r="AB25" s="95">
+      <c r="AB28" s="78">
         <v>139</v>
       </c>
-      <c r="AC25" s="95">
+      <c r="AC28" s="78">
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="2" customFormat="1" ht="13">
-      <c r="A28" s="2" t="s">
+    <row r="31" spans="1:29" s="2" customFormat="1" ht="13">
+      <c r="A31" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="I28" s="34">
-        <f t="shared" ref="I28" si="57">I3/E3-1</f>
+      <c r="I31" s="34">
+        <f>I3/E3-1</f>
         <v>3.1754574811625469E-2</v>
       </c>
-      <c r="M28" s="34">
-        <f t="shared" ref="M28" si="58">M3/I3-1</f>
+      <c r="M31" s="34">
+        <f>M3/I3-1</f>
         <v>-6.7814293166406081E-3</v>
       </c>
-      <c r="Q28" s="34">
-        <f t="shared" ref="Q28" si="59">Q3/M3-1</f>
+      <c r="Q31" s="34">
+        <f>Q3/M3-1</f>
         <v>4.8319327731092487E-2</v>
       </c>
-      <c r="R28" s="34">
+      <c r="R31" s="34">
         <f>R3/N3-1</f>
         <v>4.6218487394958041E-2</v>
       </c>
-      <c r="S28" s="34">
-        <f t="shared" ref="S28" si="60">S3/O3-1</f>
+      <c r="S31" s="34">
+        <f>S3/O3-1</f>
         <v>2.4590163934426146E-2</v>
       </c>
-      <c r="AA28" s="34">
-        <f t="shared" ref="AA28:AC28" si="61">AA3/Z3-1</f>
+      <c r="Y31" s="34">
+        <f t="shared" ref="Y31:AA31" si="19">Y3/X3-1</f>
+        <v>4.9170954831332159E-2</v>
+      </c>
+      <c r="Z31" s="34">
+        <f t="shared" si="19"/>
+        <v>1.2534059945504161E-2</v>
+      </c>
+      <c r="AA31" s="34">
+        <f>AA3/Z3-1</f>
         <v>3.1754574811625469E-2</v>
       </c>
-      <c r="AB28" s="34">
-        <f t="shared" si="61"/>
+      <c r="AB31" s="34">
+        <f>AB3/AA3-1</f>
         <v>-6.7814293166406081E-3</v>
       </c>
-      <c r="AC28" s="34">
+      <c r="AC31" s="34">
         <f>AC3/AB3-1</f>
         <v>4.8319327731092487E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="98" customFormat="1" ht="13">
-      <c r="A29" s="98" t="s">
+    <row r="32" spans="1:29" s="81" customFormat="1" ht="13">
+      <c r="A32" s="104" t="s">
         <v>213</v>
       </c>
-      <c r="I29" s="98">
-        <f t="shared" ref="I29" si="62">I3-E3</f>
+      <c r="I32" s="81">
+        <f>I3-E3</f>
         <v>59</v>
       </c>
-      <c r="M29" s="98">
-        <f t="shared" ref="M29" si="63">M3-I3</f>
+      <c r="M32" s="81">
+        <f>M3-I3</f>
         <v>-13</v>
       </c>
-      <c r="Q29" s="98">
-        <f t="shared" ref="Q29:R29" si="64">Q3-M3</f>
+      <c r="Q32" s="81">
+        <f>Q3-M3</f>
         <v>92</v>
       </c>
-      <c r="R29" s="98">
-        <f t="shared" si="64"/>
+      <c r="R32" s="81">
+        <f>R3-N3</f>
         <v>88</v>
       </c>
-      <c r="S29" s="98">
+      <c r="S32" s="81">
         <f>S3-O3</f>
         <v>48</v>
       </c>
-      <c r="AA29" s="98">
-        <f t="shared" ref="AA29:AC29" si="65">AA3-Z3</f>
+      <c r="Y32" s="81">
+        <f t="shared" ref="Y32:AA32" si="20">Y3-X3</f>
+        <v>86</v>
+      </c>
+      <c r="Z32" s="81">
+        <f t="shared" si="20"/>
+        <v>23</v>
+      </c>
+      <c r="AA32" s="81">
+        <f>AA3-Z3</f>
         <v>59</v>
       </c>
-      <c r="AB29" s="98">
-        <f t="shared" si="65"/>
+      <c r="AB32" s="81">
+        <f>AB3-AA3</f>
         <v>-13</v>
       </c>
-      <c r="AC29" s="98">
+      <c r="AC32" s="81">
         <f>AC3-AB3</f>
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
-      <c r="A30" s="3" t="s">
+    <row r="33" spans="1:29">
+      <c r="A33" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="N30" s="25">
-        <f t="shared" ref="N30:Q30" si="66">N3/M3-1</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="25">
-        <f t="shared" si="66"/>
+      <c r="N33" s="25">
+        <f>N3/M3-1</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="25">
+        <f>O3/N3-1</f>
         <v>2.5210084033613356E-2</v>
       </c>
-      <c r="P30" s="25">
-        <f t="shared" si="66"/>
+      <c r="P33" s="25">
+        <f>P3/O3-1</f>
         <v>8.1967213114753079E-3</v>
       </c>
-      <c r="Q30" s="25">
-        <f t="shared" ref="Q30:R30" si="67">Q3/P3-1</f>
+      <c r="Q33" s="25">
+        <f>Q3/P3-1</f>
         <v>1.4227642276422703E-2</v>
       </c>
-      <c r="R30" s="25">
+      <c r="R33" s="25">
         <f>R3/Q3-1</f>
         <v>-2.0040080160320661E-3</v>
       </c>
-      <c r="S30" s="25">
-        <f t="shared" ref="S30" si="68">S3/R3-1</f>
+      <c r="S33" s="25">
+        <f>S3/R3-1</f>
         <v>4.0160642570281624E-3</v>
       </c>
-      <c r="Z30" s="63" t="s">
+      <c r="X33" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AA30" s="63" t="s">
+      <c r="Y33" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AB30" s="63" t="s">
+      <c r="Z33" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AC30" s="63" t="s">
+      <c r="AA33" s="63" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="31" spans="1:29" s="99" customFormat="1">
-      <c r="A31" s="99" t="s">
+      <c r="AB33" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC33" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" s="82" customFormat="1">
+      <c r="A34" s="105" t="s">
         <v>214</v>
       </c>
-      <c r="B31" s="100"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="N31" s="98">
-        <f>N3-M3</f>
-        <v>0</v>
-      </c>
-      <c r="O31" s="98">
-        <f>O3-N3</f>
+      <c r="B34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="N34" s="81">
+        <f t="shared" ref="N34:S34" si="21">N3-M3</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="81">
+        <f t="shared" si="21"/>
         <v>48</v>
       </c>
-      <c r="P31" s="98">
-        <f>P3-O3</f>
+      <c r="P34" s="81">
+        <f t="shared" si="21"/>
         <v>16</v>
       </c>
-      <c r="Q31" s="98">
-        <f>Q3-P3</f>
+      <c r="Q34" s="81">
+        <f t="shared" si="21"/>
         <v>28</v>
       </c>
-      <c r="R31" s="98">
-        <f>R3-Q3</f>
+      <c r="R34" s="81">
+        <f t="shared" si="21"/>
         <v>-4</v>
       </c>
-      <c r="S31" s="98">
-        <f>S3-R3</f>
+      <c r="S34" s="81">
+        <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="Z31" s="63" t="s">
+      <c r="X34" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AA31" s="63" t="s">
+      <c r="Y34" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AB31" s="63" t="s">
+      <c r="Z34" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AC31" s="63" t="s">
+      <c r="AA34" s="63" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="32" spans="1:29">
-      <c r="AC32" s="25"/>
-    </row>
-    <row r="33" spans="1:29" s="2" customFormat="1" ht="13">
-      <c r="A33" s="2" t="s">
+      <c r="AB34" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC34" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
+      <c r="AC35" s="25"/>
+    </row>
+    <row r="36" spans="1:29" s="2" customFormat="1" ht="13">
+      <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="I33" s="34">
-        <f t="shared" ref="I33" si="69">I11/E11-1</f>
+      <c r="I36" s="34">
+        <f>I12/E12-1</f>
         <v>5.9731543624160999E-2</v>
       </c>
-      <c r="M33" s="34">
-        <f t="shared" ref="M33" si="70">M11/I11-1</f>
+      <c r="M36" s="34">
+        <f>M12/I12-1</f>
         <v>2.7865737808739688E-2</v>
       </c>
-      <c r="Q33" s="34">
-        <f t="shared" ref="Q33" si="71">Q11/M11-1</f>
+      <c r="Q36" s="34">
+        <f>Q12/M12-1</f>
         <v>2.9574861367837268E-2</v>
       </c>
-      <c r="R33" s="34">
-        <f>R11/N11-1</f>
+      <c r="R36" s="34">
+        <f>R12/N12-1</f>
         <v>2.7573529411764719E-2</v>
       </c>
-      <c r="S33" s="34">
-        <f t="shared" ref="S33" si="72">S11/O11-1</f>
+      <c r="S36" s="34">
+        <f>S12/O12-1</f>
         <v>2.5516403402187082E-2</v>
       </c>
-      <c r="AA33" s="34">
-        <f t="shared" ref="AA33:AB33" si="73">AA11/Z11-1</f>
+      <c r="Y36" s="34">
+        <f t="shared" ref="Y36:AA36" si="22">Y12/X12-1</f>
+        <v>7.7752117013087041E-2</v>
+      </c>
+      <c r="Z36" s="34">
+        <f t="shared" si="22"/>
+        <v>6.4285714285714279E-2</v>
+      </c>
+      <c r="AA36" s="34">
+        <f>AA12/Z12-1</f>
         <v>5.9731543624160999E-2</v>
       </c>
-      <c r="AB33" s="34">
-        <f>AB11/AA11-1</f>
+      <c r="AB36" s="34">
+        <f>AB12/AA12-1</f>
         <v>2.7865737808739688E-2</v>
       </c>
-      <c r="AC33" s="34">
-        <f>AC11/AB11-1</f>
+      <c r="AC36" s="34">
+        <f>AC12/AB12-1</f>
         <v>2.9574861367837268E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:29" s="98" customFormat="1" ht="13">
-      <c r="A34" s="98" t="s">
+    <row r="37" spans="1:29" s="81" customFormat="1" ht="13">
+      <c r="A37" s="104" t="s">
         <v>202</v>
       </c>
-      <c r="I34" s="98">
-        <f t="shared" ref="I34" si="74">I11-E11</f>
+      <c r="I37" s="81">
+        <f>I12-E12</f>
         <v>89</v>
       </c>
-      <c r="M34" s="98">
-        <f t="shared" ref="M34" si="75">M11-I11</f>
+      <c r="M37" s="81">
+        <f>M12-I12</f>
         <v>44</v>
       </c>
-      <c r="Q34" s="98">
-        <f t="shared" ref="Q34:R34" si="76">Q11-M11</f>
+      <c r="Q37" s="81">
+        <f>Q12-M12</f>
         <v>48</v>
       </c>
-      <c r="R34" s="98">
-        <f t="shared" si="76"/>
+      <c r="R37" s="81">
+        <f>R12-N12</f>
         <v>45</v>
       </c>
-      <c r="S34" s="98">
-        <f>S11-O11</f>
+      <c r="S37" s="81">
+        <f>S12-O12</f>
         <v>42</v>
       </c>
-      <c r="AA34" s="98">
-        <f t="shared" ref="AA34:AC34" si="77">AA11-Z11</f>
+      <c r="Y37" s="81">
+        <f t="shared" ref="Y37:AA37" si="23">Y12-X12</f>
+        <v>101</v>
+      </c>
+      <c r="Z37" s="81">
+        <f t="shared" si="23"/>
+        <v>90</v>
+      </c>
+      <c r="AA37" s="81">
+        <f>AA12-Z12</f>
         <v>89</v>
       </c>
-      <c r="AB34" s="98">
-        <f t="shared" si="77"/>
+      <c r="AB37" s="81">
+        <f>AB12-AA12</f>
         <v>44</v>
       </c>
-      <c r="AC34" s="98">
-        <f>AC11-AB11</f>
+      <c r="AC37" s="81">
+        <f>AC12-AB12</f>
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
-      <c r="A35" s="3" t="s">
+    <row r="38" spans="1:29">
+      <c r="A38" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="N35" s="25">
-        <f t="shared" ref="N35:Q35" si="78">N11/M11-1</f>
+      <c r="N38" s="25">
+        <f>N12/M12-1</f>
         <v>5.5452865064695711E-3</v>
       </c>
-      <c r="O35" s="25">
-        <f t="shared" si="78"/>
+      <c r="O38" s="25">
+        <f>O12/N12-1</f>
         <v>8.5784313725489891E-3</v>
       </c>
-      <c r="P35" s="25">
-        <f t="shared" si="78"/>
+      <c r="P38" s="25">
+        <f>P12/O12-1</f>
         <v>5.4678007290400732E-3</v>
       </c>
-      <c r="Q35" s="25">
-        <f t="shared" ref="Q35:R35" si="79">Q11/P11-1</f>
+      <c r="Q38" s="25">
+        <f>Q12/P12-1</f>
         <v>9.6676737160121817E-3</v>
       </c>
-      <c r="R35" s="25">
-        <f>R11/Q11-1</f>
+      <c r="R38" s="25">
+        <f>R12/Q12-1</f>
         <v>3.5906642728904536E-3</v>
       </c>
-      <c r="S35" s="25">
-        <f t="shared" ref="S35" si="80">S11/R11-1</f>
+      <c r="S38" s="25">
+        <f>S12/R12-1</f>
         <v>6.5593321407275695E-3</v>
       </c>
-      <c r="Z35" s="63" t="s">
+      <c r="X38" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AA35" s="63" t="s">
+      <c r="Y38" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AB35" s="63" t="s">
+      <c r="Z38" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AC35" s="63" t="s">
+      <c r="AA38" s="63" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="36" spans="1:29" s="101" customFormat="1">
-      <c r="A36" s="101" t="s">
+      <c r="AB38" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC38" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" s="84" customFormat="1">
+      <c r="A39" s="106" t="s">
         <v>203</v>
       </c>
-      <c r="B36" s="102"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="102"/>
-      <c r="N36" s="98">
-        <f t="shared" ref="N36:S36" si="81">N11-M11</f>
+      <c r="B39" s="85"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="N39" s="81">
+        <f>N12-M12</f>
         <v>9</v>
       </c>
-      <c r="O36" s="98">
-        <f t="shared" si="81"/>
+      <c r="O39" s="81">
+        <f>O12-N12</f>
         <v>14</v>
       </c>
-      <c r="P36" s="98">
-        <f t="shared" si="81"/>
+      <c r="P39" s="81">
+        <f>P12-O12</f>
         <v>9</v>
       </c>
-      <c r="Q36" s="98">
-        <f t="shared" si="81"/>
+      <c r="Q39" s="81">
+        <f>Q12-P12</f>
         <v>16</v>
       </c>
-      <c r="R36" s="98">
-        <f t="shared" si="81"/>
+      <c r="R39" s="81">
+        <f>R12-Q12</f>
         <v>6</v>
       </c>
-      <c r="S36" s="98">
-        <f>S11-R11</f>
+      <c r="S39" s="81">
+        <f>S12-R12</f>
         <v>11</v>
       </c>
-      <c r="Z36" s="63" t="s">
+      <c r="X39" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AA36" s="63" t="s">
+      <c r="Y39" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AB36" s="63" t="s">
+      <c r="Z39" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AC36" s="63" t="s">
+      <c r="AA39" s="63" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="37" spans="1:29">
-      <c r="AC37" s="25"/>
-    </row>
-    <row r="38" spans="1:29" s="2" customFormat="1" ht="13">
-      <c r="A38" s="2" t="s">
+      <c r="AB39" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC39" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29">
+      <c r="AC40" s="25"/>
+    </row>
+    <row r="41" spans="1:29" s="2" customFormat="1" ht="13">
+      <c r="A41" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="I38" s="34">
-        <f t="shared" ref="I38" si="82">I19/E19-1</f>
+      <c r="I41" s="34">
+        <f t="shared" ref="I41" si="24">I21/E21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
-      <c r="M38" s="34">
-        <f t="shared" ref="M38" si="83">M19/I19-1</f>
+      <c r="M41" s="34">
+        <f t="shared" ref="M41" si="25">M21/I21-1</f>
         <v>-0.16863905325443784</v>
       </c>
-      <c r="Q38" s="34">
-        <f t="shared" ref="Q38" si="84">Q19/M19-1</f>
+      <c r="Q41" s="34">
+        <f t="shared" ref="Q41" si="26">Q21/M21-1</f>
         <v>0.15658362989323837</v>
       </c>
-      <c r="R38" s="34">
-        <f>R19/N19-1</f>
+      <c r="R41" s="34">
+        <f>R21/N21-1</f>
         <v>0.15808823529411775</v>
       </c>
-      <c r="S38" s="34">
-        <f t="shared" ref="S38" si="85">S19/O19-1</f>
+      <c r="S41" s="34">
+        <f t="shared" ref="S41" si="27">S21/O21-1</f>
         <v>1.9607843137254832E-2</v>
       </c>
-      <c r="AA38" s="34">
-        <f t="shared" ref="AA38:AB38" si="86">AA19/Z19-1</f>
+      <c r="Y41" s="34">
+        <f t="shared" ref="Y41" si="28">Y21/X21-1</f>
+        <v>-3.3333333333333326E-2</v>
+      </c>
+      <c r="Z41" s="34">
+        <f t="shared" ref="Z41" si="29">Z21/Y21-1</f>
+        <v>-0.15402298850574714</v>
+      </c>
+      <c r="AA41" s="34">
+        <f t="shared" ref="AA41" si="30">AA21/Z21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
-      <c r="AB38" s="34">
-        <f>AB19/AA19-1</f>
+      <c r="AB41" s="34">
+        <f>AB21/AA21-1</f>
         <v>-0.16863905325443784</v>
       </c>
-      <c r="AC38" s="34">
-        <f>AC19/AB19-1</f>
+      <c r="AC41" s="34">
+        <f>AC21/AB21-1</f>
         <v>0.15658362989323837</v>
       </c>
     </row>
-    <row r="39" spans="1:29" s="103" customFormat="1" ht="13">
-      <c r="A39" s="103" t="s">
+    <row r="42" spans="1:29" s="86" customFormat="1" ht="13">
+      <c r="A42" s="107" t="s">
         <v>215</v>
       </c>
-      <c r="I39" s="103">
-        <f>I19-E19</f>
+      <c r="I42" s="86">
+        <f>I21-E21</f>
         <v>-30</v>
       </c>
-      <c r="M39" s="103">
-        <f>M19-I19</f>
+      <c r="M42" s="86">
+        <f>M21-I21</f>
         <v>-57</v>
       </c>
-      <c r="Q39" s="103">
-        <f t="shared" ref="Q39:R39" si="87">Q19-M19</f>
+      <c r="Q42" s="86">
+        <f t="shared" ref="Q42:R42" si="31">Q21-M21</f>
         <v>44</v>
       </c>
-      <c r="R39" s="103">
-        <f t="shared" si="87"/>
+      <c r="R42" s="86">
+        <f t="shared" si="31"/>
         <v>43</v>
       </c>
-      <c r="S39" s="103">
-        <f>S19-O19</f>
+      <c r="S42" s="86">
+        <f>S21-O21</f>
         <v>6</v>
       </c>
-      <c r="AA39" s="103">
-        <f t="shared" ref="AA39:AC39" si="88">AA19-Z19</f>
+      <c r="Y42" s="86">
+        <f t="shared" ref="Y42" si="32">Y21-X21</f>
+        <v>-15</v>
+      </c>
+      <c r="Z42" s="86">
+        <f t="shared" ref="Z42" si="33">Z21-Y21</f>
+        <v>-67</v>
+      </c>
+      <c r="AA42" s="86">
+        <f t="shared" ref="AA42:AB42" si="34">AA21-Z21</f>
         <v>-30</v>
       </c>
-      <c r="AB39" s="103">
-        <f t="shared" si="88"/>
+      <c r="AB42" s="86">
+        <f t="shared" si="34"/>
         <v>-57</v>
       </c>
-      <c r="AC39" s="103">
-        <f>AC19-AB19</f>
+      <c r="AC42" s="86">
+        <f>AC21-AB21</f>
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
-      <c r="A40" s="3" t="s">
+    <row r="43" spans="1:29">
+      <c r="A43" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="N40" s="25">
-        <f t="shared" ref="N40:Q40" si="89">N19/M19-1</f>
+      <c r="N43" s="25">
+        <f t="shared" ref="N43:P43" si="35">N21/M21-1</f>
         <v>-3.2028469750889688E-2</v>
       </c>
-      <c r="O40" s="25">
-        <f t="shared" si="89"/>
+      <c r="O43" s="25">
+        <f t="shared" si="35"/>
         <v>0.125</v>
       </c>
-      <c r="P40" s="25">
-        <f t="shared" si="89"/>
+      <c r="P43" s="25">
+        <f t="shared" si="35"/>
         <v>2.2875816993463971E-2</v>
       </c>
-      <c r="Q40" s="25">
-        <f t="shared" ref="Q40:R40" si="90">Q19/P19-1</f>
+      <c r="Q43" s="25">
+        <f t="shared" ref="Q43" si="36">Q21/P21-1</f>
         <v>3.833865814696491E-2</v>
       </c>
-      <c r="R40" s="25">
-        <f>R19/Q19-1</f>
+      <c r="R43" s="25">
+        <f>R21/Q21-1</f>
         <v>-3.0769230769230771E-2</v>
       </c>
-      <c r="S40" s="25">
-        <f t="shared" ref="S40" si="91">S19/R19-1</f>
+      <c r="S43" s="25">
+        <f t="shared" ref="S43" si="37">S21/R21-1</f>
         <v>-9.52380952380949E-3</v>
       </c>
-      <c r="Z40" s="63" t="s">
+      <c r="X43" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AA40" s="63" t="s">
+      <c r="Y43" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AB40" s="63" t="s">
+      <c r="Z43" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AC40" s="63" t="s">
+      <c r="AA43" s="63" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="41" spans="1:29" s="101" customFormat="1">
-      <c r="A41" s="101" t="s">
+      <c r="AB43" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC43" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" s="84" customFormat="1">
+      <c r="A44" s="106" t="s">
         <v>216</v>
       </c>
-      <c r="B41" s="102"/>
-      <c r="C41" s="102"/>
-      <c r="D41" s="102"/>
-      <c r="N41" s="98">
-        <f t="shared" ref="N41:S41" si="92">N19-M19</f>
+      <c r="B44" s="85"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+      <c r="N44" s="81">
+        <f t="shared" ref="N44:R44" si="38">N21-M21</f>
         <v>-9</v>
       </c>
-      <c r="O41" s="98">
-        <f t="shared" si="92"/>
+      <c r="O44" s="81">
+        <f t="shared" si="38"/>
         <v>34</v>
       </c>
-      <c r="P41" s="98">
-        <f t="shared" si="92"/>
+      <c r="P44" s="81">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
-      <c r="Q41" s="98">
-        <f t="shared" si="92"/>
+      <c r="Q44" s="81">
+        <f t="shared" si="38"/>
         <v>12</v>
       </c>
-      <c r="R41" s="98">
-        <f t="shared" si="92"/>
+      <c r="R44" s="81">
+        <f t="shared" si="38"/>
         <v>-10</v>
       </c>
-      <c r="S41" s="98">
-        <f>S19-R19</f>
+      <c r="S44" s="81">
+        <f>S21-R21</f>
         <v>-3</v>
       </c>
-      <c r="Z41" s="63" t="s">
+      <c r="X44" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AA41" s="63" t="s">
+      <c r="Y44" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AB41" s="63" t="s">
+      <c r="Z44" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AC41" s="63" t="s">
+      <c r="AA44" s="63" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="44" spans="1:29">
-      <c r="N44" s="93"/>
-    </row>
-    <row r="46" spans="1:29">
-      <c r="N46" s="92"/>
+      <c r="AB44" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC44" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
+      <c r="N47" s="76"/>
+    </row>
+    <row r="49" spans="14:14">
+      <c r="N49" s="75"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18088,7 +18628,10 @@
     <hyperlink ref="I2" r:id="rId11" xr:uid="{998E2907-64B9-7A44-8D65-8083912D2D62}"/>
     <hyperlink ref="E2" r:id="rId12" xr:uid="{5D689E99-05ED-E34E-9D87-28B9F22988C9}"/>
     <hyperlink ref="Z2" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
+    <hyperlink ref="Y2" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
+    <hyperlink ref="X2" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more info, data & due diligence to main in $ERJ
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929A0A14-DD45-6942-AD41-707219E3F48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BD20DC-C224-E749-9831-81B7CB188F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="252">
   <si>
     <t>$ERJ</t>
   </si>
@@ -831,6 +831,105 @@
   </si>
   <si>
     <t>FY16</t>
+  </si>
+  <si>
+    <t>A220 vs E2</t>
+  </si>
+  <si>
+    <t>A220-300</t>
+  </si>
+  <si>
+    <t>E195-E2</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>38.7m</t>
+  </si>
+  <si>
+    <t>6,297km</t>
+  </si>
+  <si>
+    <t>21,508kg</t>
+  </si>
+  <si>
+    <t>$91.5m</t>
+  </si>
+  <si>
+    <t>160 seats</t>
+  </si>
+  <si>
+    <t>146 seats</t>
+  </si>
+  <si>
+    <t>41.5m</t>
+  </si>
+  <si>
+    <t>4,815km</t>
+  </si>
+  <si>
+    <t>13,690kg</t>
+  </si>
+  <si>
+    <t>$60.4m</t>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>2-3 seating</t>
+  </si>
+  <si>
+    <t>2-2 seating</t>
+  </si>
+  <si>
+    <t>CSeries/A220 enters service with Swiss International Airline to primarily compete with larger E-Jet E2 variants</t>
+  </si>
+  <si>
+    <t>E195-E2 lands at London City Airport (LCY) for the first time, making it the largest aircraft cleared to operate from the airport</t>
+  </si>
+  <si>
+    <t>As of July 2022, Embraer aircraft account for 85% of all LCY operations on routes as diverse as EDI &amp; Mykonos</t>
+  </si>
+  <si>
+    <t>LCY Cert</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Airbus confirmed there are no plans to certify the larger, higher capacity A220-300 for LCY steep approach operations</t>
+  </si>
+  <si>
+    <t>Quick Links</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>SimpleFlying</t>
+  </si>
+  <si>
+    <t>Embraer announced the opening of 1,000 job vacancies in Brazil focusing on production rate recovery, services &amp; support,</t>
+  </si>
+  <si>
+    <t>growth, product development &amp; new business</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1291,10 +1390,10 @@
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1306,28 +1405,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1340,6 +1427,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6096,10 +6223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AB44"/>
+  <dimension ref="A2:AC53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -6107,18 +6234,18 @@
     <col min="1" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" ht="15">
+    <row r="2" spans="1:29" ht="15">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:29">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:29">
       <c r="B5" s="93" t="s">
         <v>2</v>
       </c>
@@ -6138,18 +6265,18 @@
       <c r="P5" s="94"/>
       <c r="Q5" s="94"/>
       <c r="R5" s="95"/>
-      <c r="U5" s="93" t="s">
+      <c r="T5" s="93" t="s">
         <v>133</v>
       </c>
+      <c r="U5" s="94"/>
       <c r="V5" s="94"/>
-      <c r="W5" s="94"/>
-      <c r="X5" s="95"/>
-      <c r="AA5" s="91" t="s">
+      <c r="W5" s="95"/>
+      <c r="AA5" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="92"/>
-    </row>
-    <row r="6" spans="1:28">
+      <c r="AB5" s="105"/>
+    </row>
+    <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
@@ -6173,18 +6300,18 @@
       <c r="P6" s="37"/>
       <c r="Q6" s="37"/>
       <c r="R6" s="38"/>
-      <c r="U6" s="41" t="s">
+      <c r="T6" s="41" t="s">
         <v>148</v>
       </c>
+      <c r="U6" s="37"/>
       <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-      <c r="X6" s="38"/>
+      <c r="W6" s="38"/>
       <c r="AA6" s="70" t="s">
         <v>206</v>
       </c>
       <c r="AB6" s="38"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:29">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
@@ -6209,18 +6336,18 @@
       <c r="P7" s="37"/>
       <c r="Q7" s="37"/>
       <c r="R7" s="38"/>
-      <c r="U7" s="46" t="s">
+      <c r="T7" s="46" t="s">
         <v>84</v>
       </c>
+      <c r="U7" s="37"/>
       <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
-      <c r="X7" s="38"/>
+      <c r="W7" s="38"/>
       <c r="AA7" s="70" t="s">
         <v>207</v>
       </c>
       <c r="AB7" s="38"/>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:29">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
@@ -6243,18 +6370,18 @@
       <c r="P8" s="37"/>
       <c r="Q8" s="37"/>
       <c r="R8" s="38"/>
-      <c r="U8" s="45" t="s">
+      <c r="T8" s="45" t="s">
         <v>137</v>
       </c>
+      <c r="U8" s="37"/>
       <c r="V8" s="37"/>
-      <c r="W8" s="37"/>
-      <c r="X8" s="38"/>
+      <c r="W8" s="38"/>
       <c r="AA8" s="71" t="s">
         <v>208</v>
       </c>
       <c r="AB8" s="36"/>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:29">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
@@ -6278,14 +6405,14 @@
       <c r="P9" s="37"/>
       <c r="Q9" s="37"/>
       <c r="R9" s="38"/>
-      <c r="U9" s="47" t="s">
+      <c r="T9" s="47" t="s">
         <v>151</v>
       </c>
+      <c r="U9" s="37"/>
       <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
-      <c r="X9" s="38"/>
-    </row>
-    <row r="10" spans="1:28">
+      <c r="W9" s="38"/>
+    </row>
+    <row r="10" spans="1:29">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
@@ -6313,14 +6440,14 @@
       <c r="P10" s="37"/>
       <c r="Q10" s="37"/>
       <c r="R10" s="38"/>
-      <c r="U10" s="47" t="s">
+      <c r="T10" s="47" t="s">
         <v>152</v>
       </c>
+      <c r="U10" s="37"/>
       <c r="V10" s="37"/>
-      <c r="W10" s="37"/>
-      <c r="X10" s="38"/>
-    </row>
-    <row r="11" spans="1:28">
+      <c r="W10" s="38"/>
+    </row>
+    <row r="11" spans="1:29">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -6346,14 +6473,14 @@
       <c r="P11" s="37"/>
       <c r="Q11" s="37"/>
       <c r="R11" s="38"/>
-      <c r="U11" s="47" t="s">
+      <c r="T11" s="47" t="s">
         <v>153</v>
       </c>
+      <c r="U11" s="37"/>
       <c r="V11" s="37"/>
-      <c r="W11" s="37"/>
-      <c r="X11" s="38"/>
-    </row>
-    <row r="12" spans="1:28">
+      <c r="W11" s="38"/>
+    </row>
+    <row r="12" spans="1:29">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
@@ -6374,12 +6501,19 @@
       <c r="P12" s="37"/>
       <c r="Q12" s="37"/>
       <c r="R12" s="38"/>
-      <c r="U12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="37"/>
       <c r="V12" s="37"/>
-      <c r="W12" s="37"/>
-      <c r="X12" s="38"/>
-    </row>
-    <row r="13" spans="1:28">
+      <c r="W12" s="38"/>
+      <c r="Y12" s="93" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z12" s="94"/>
+      <c r="AA12" s="94"/>
+      <c r="AB12" s="94"/>
+      <c r="AC12" s="95"/>
+    </row>
+    <row r="13" spans="1:29">
       <c r="G13" s="10"/>
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
@@ -6392,14 +6526,23 @@
       <c r="P13" s="37"/>
       <c r="Q13" s="37"/>
       <c r="R13" s="38"/>
-      <c r="U13" s="45" t="s">
+      <c r="T13" s="45" t="s">
         <v>138</v>
       </c>
+      <c r="U13" s="37"/>
       <c r="V13" s="37"/>
-      <c r="W13" s="37"/>
-      <c r="X13" s="38"/>
-    </row>
-    <row r="14" spans="1:28">
+      <c r="W13" s="38"/>
+      <c r="Y13" s="111"/>
+      <c r="Z13" s="112" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA13" s="112"/>
+      <c r="AB13" s="112" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC13" s="113"/>
+    </row>
+    <row r="14" spans="1:29">
       <c r="G14" s="9">
         <v>44805</v>
       </c>
@@ -6416,14 +6559,25 @@
       <c r="P14" s="37"/>
       <c r="Q14" s="37"/>
       <c r="R14" s="38"/>
-      <c r="U14" s="47" t="s">
+      <c r="T14" s="47" t="s">
         <v>154</v>
       </c>
+      <c r="U14" s="37"/>
       <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-      <c r="X14" s="38"/>
-    </row>
-    <row r="15" spans="1:28">
+      <c r="W14" s="38"/>
+      <c r="Y14" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z14" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA14" s="98"/>
+      <c r="AB14" s="98" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC14" s="99"/>
+    </row>
+    <row r="15" spans="1:29">
       <c r="B15" s="93" t="s">
         <v>14</v>
       </c>
@@ -6441,14 +6595,25 @@
       <c r="P15" s="37"/>
       <c r="Q15" s="37"/>
       <c r="R15" s="38"/>
-      <c r="U15" s="47" t="s">
+      <c r="T15" s="47" t="s">
         <v>155</v>
       </c>
+      <c r="U15" s="37"/>
       <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="38"/>
-    </row>
-    <row r="16" spans="1:28">
+      <c r="W15" s="38"/>
+      <c r="Y15" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z15" s="98" t="s">
+        <v>227</v>
+      </c>
+      <c r="AA15" s="98"/>
+      <c r="AB15" s="98" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC15" s="99"/>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" s="14" t="s">
         <v>16</v>
       </c>
@@ -6471,14 +6636,25 @@
       <c r="P16" s="37"/>
       <c r="Q16" s="37"/>
       <c r="R16" s="38"/>
-      <c r="U16" s="47" t="s">
+      <c r="T16" s="47" t="s">
         <v>156</v>
       </c>
+      <c r="U16" s="37"/>
       <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="38"/>
-    </row>
-    <row r="17" spans="2:24">
+      <c r="W16" s="38"/>
+      <c r="Y16" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z16" s="98" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA16" s="98"/>
+      <c r="AB16" s="98" t="s">
+        <v>234</v>
+      </c>
+      <c r="AC16" s="99"/>
+    </row>
+    <row r="17" spans="2:29">
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
@@ -6502,12 +6678,23 @@
       <c r="P17" s="60"/>
       <c r="Q17" s="60"/>
       <c r="R17" s="38"/>
-      <c r="U17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="37"/>
       <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="38"/>
-    </row>
-    <row r="18" spans="2:24">
+      <c r="W17" s="38"/>
+      <c r="Y17" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z17" s="98" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA17" s="98"/>
+      <c r="AB17" s="98" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC17" s="99"/>
+    </row>
+    <row r="18" spans="2:29">
       <c r="B18" s="16"/>
       <c r="C18" s="98"/>
       <c r="D18" s="99"/>
@@ -6525,17 +6712,28 @@
       <c r="P18" s="60"/>
       <c r="Q18" s="60"/>
       <c r="R18" s="38"/>
-      <c r="U18" s="46" t="s">
+      <c r="T18" s="46" t="s">
         <v>139</v>
       </c>
+      <c r="U18" s="37"/>
       <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="38"/>
-    </row>
-    <row r="19" spans="2:24">
+      <c r="W18" s="38"/>
+      <c r="Y18" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z18" s="98" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA18" s="98"/>
+      <c r="AB18" s="98" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC18" s="99"/>
+    </row>
+    <row r="19" spans="2:29">
       <c r="B19" s="17"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="101"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="109"/>
       <c r="G19" s="10"/>
       <c r="H19" s="8" t="s">
         <v>193</v>
@@ -6550,14 +6748,25 @@
       <c r="P19" s="60"/>
       <c r="Q19" s="60"/>
       <c r="R19" s="38"/>
-      <c r="U19" s="45" t="s">
+      <c r="T19" s="45" t="s">
         <v>142</v>
       </c>
+      <c r="U19" s="37"/>
       <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
-      <c r="X19" s="38"/>
-    </row>
-    <row r="20" spans="2:24">
+      <c r="W19" s="38"/>
+      <c r="Y19" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z19" s="98" t="s">
+        <v>238</v>
+      </c>
+      <c r="AA19" s="98"/>
+      <c r="AB19" s="98" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC19" s="99"/>
+    </row>
+    <row r="20" spans="2:29">
       <c r="G20" s="10"/>
       <c r="H20" s="8" t="s">
         <v>191</v>
@@ -6574,14 +6783,25 @@
       <c r="R20" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="U20" s="45" t="s">
+      <c r="T20" s="45" t="s">
         <v>141</v>
       </c>
+      <c r="U20" s="37"/>
       <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="38"/>
-    </row>
-    <row r="21" spans="2:24">
+      <c r="W20" s="38"/>
+      <c r="Y20" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z20" s="98" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA20" s="98"/>
+      <c r="AB20" s="98" t="s">
+        <v>245</v>
+      </c>
+      <c r="AC20" s="99"/>
+    </row>
+    <row r="21" spans="2:29">
       <c r="G21" s="10"/>
       <c r="H21" s="60"/>
       <c r="I21" s="60"/>
@@ -6594,14 +6814,19 @@
       <c r="P21" s="60"/>
       <c r="Q21" s="60"/>
       <c r="R21" s="38"/>
-      <c r="U21" s="45" t="s">
+      <c r="T21" s="45" t="s">
         <v>140</v>
       </c>
+      <c r="U21" s="37"/>
       <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="38"/>
-    </row>
-    <row r="22" spans="2:24">
+      <c r="W21" s="38"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="60"/>
+      <c r="AA21" s="60"/>
+      <c r="AB21" s="60"/>
+      <c r="AC21" s="38"/>
+    </row>
+    <row r="22" spans="2:29">
       <c r="B22" s="93" t="s">
         <v>20</v>
       </c>
@@ -6619,14 +6844,19 @@
       <c r="P22" s="60"/>
       <c r="Q22" s="60"/>
       <c r="R22" s="38"/>
-      <c r="U22" s="45" t="s">
+      <c r="T22" s="45" t="s">
         <v>157</v>
       </c>
+      <c r="U22" s="37"/>
       <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="38"/>
-    </row>
-    <row r="23" spans="2:24">
+      <c r="W22" s="38"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="35"/>
+      <c r="AA22" s="35"/>
+      <c r="AB22" s="35"/>
+      <c r="AC22" s="36"/>
+    </row>
+    <row r="23" spans="2:29">
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
@@ -6650,12 +6880,12 @@
       <c r="P23" s="60"/>
       <c r="Q23" s="60"/>
       <c r="R23" s="38"/>
-      <c r="U23" s="42"/>
+      <c r="T23" s="42"/>
+      <c r="U23" s="37"/>
       <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="38"/>
-    </row>
-    <row r="24" spans="2:24">
+      <c r="W23" s="38"/>
+    </row>
+    <row r="24" spans="2:29">
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
@@ -6677,14 +6907,14 @@
       <c r="P24" s="60"/>
       <c r="Q24" s="60"/>
       <c r="R24" s="38"/>
-      <c r="U24" s="46" t="s">
+      <c r="T24" s="46" t="s">
         <v>143</v>
       </c>
+      <c r="U24" s="37"/>
       <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="38"/>
-    </row>
-    <row r="25" spans="2:24">
+      <c r="W24" s="38"/>
+    </row>
+    <row r="25" spans="2:29">
       <c r="B25" s="10"/>
       <c r="C25" s="98"/>
       <c r="D25" s="99"/>
@@ -6702,22 +6932,22 @@
       <c r="P25" s="60"/>
       <c r="Q25" s="60"/>
       <c r="R25" s="38"/>
-      <c r="U25" s="45" t="s">
+      <c r="T25" s="45" t="s">
         <v>144</v>
       </c>
+      <c r="U25" s="37"/>
       <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
-      <c r="X25" s="38"/>
-    </row>
-    <row r="26" spans="2:24">
+      <c r="W25" s="38"/>
+    </row>
+    <row r="26" spans="2:29">
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="96">
+      <c r="C26" s="106">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="97"/>
+      <c r="D26" s="107"/>
       <c r="G26" s="10"/>
       <c r="H26" s="60"/>
       <c r="I26" s="60"/>
@@ -6730,22 +6960,22 @@
       <c r="P26" s="60"/>
       <c r="Q26" s="60"/>
       <c r="R26" s="38"/>
-      <c r="U26" s="45" t="s">
+      <c r="T26" s="45" t="s">
         <v>145</v>
       </c>
+      <c r="U26" s="37"/>
       <c r="V26" s="37"/>
-      <c r="W26" s="37"/>
-      <c r="X26" s="38"/>
-    </row>
-    <row r="27" spans="2:24">
+      <c r="W26" s="38"/>
+    </row>
+    <row r="27" spans="2:29">
       <c r="B27" s="10"/>
       <c r="C27" s="98"/>
       <c r="D27" s="99"/>
       <c r="G27" s="9">
-        <v>43922</v>
-      </c>
-      <c r="H27" s="37" t="s">
-        <v>164</v>
+        <v>44743</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="I27" s="37"/>
       <c r="J27" s="37"/>
@@ -6757,14 +6987,14 @@
       <c r="P27" s="37"/>
       <c r="Q27" s="37"/>
       <c r="R27" s="38"/>
-      <c r="U27" s="45" t="s">
+      <c r="T27" s="45" t="s">
         <v>146</v>
       </c>
+      <c r="U27" s="37"/>
       <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="38"/>
-    </row>
-    <row r="28" spans="2:24">
+      <c r="W27" s="38"/>
+    </row>
+    <row r="28" spans="2:29">
       <c r="B28" s="10" t="s">
         <v>23</v>
       </c>
@@ -6776,131 +7006,135 @@
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="37"/>
+        <v>242</v>
+      </c>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
       <c r="R28" s="38"/>
-      <c r="U28" s="45" t="s">
+      <c r="T28" s="45" t="s">
         <v>147</v>
       </c>
+      <c r="U28" s="37"/>
       <c r="V28" s="37"/>
-      <c r="W28" s="37"/>
-      <c r="X28" s="38"/>
-    </row>
-    <row r="29" spans="2:24">
+      <c r="W28" s="38"/>
+    </row>
+    <row r="29" spans="2:29">
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="104" t="s">
+      <c r="C29" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="105"/>
+      <c r="D29" s="101"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="51" t="s">
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="38"/>
+      <c r="T29" s="42"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="38"/>
+    </row>
+    <row r="30" spans="2:29">
+      <c r="G30" s="9">
+        <v>44682</v>
+      </c>
+      <c r="H30" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="38"/>
+      <c r="T30" s="42"/>
+      <c r="U30" s="37"/>
+      <c r="V30" s="37"/>
+      <c r="W30" s="38"/>
+    </row>
+    <row r="31" spans="2:29">
+      <c r="G31" s="10"/>
+      <c r="H31" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="U29" s="42"/>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="38"/>
-    </row>
-    <row r="30" spans="2:24">
-      <c r="G30" s="10"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="37"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="37"/>
-      <c r="Q30" s="37"/>
-      <c r="R30" s="38"/>
-      <c r="U30" s="42"/>
-      <c r="V30" s="37"/>
-      <c r="W30" s="37"/>
-      <c r="X30" s="38"/>
-    </row>
-    <row r="31" spans="2:24">
-      <c r="G31" s="10"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="37"/>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="38"/>
-      <c r="U31" s="46" t="s">
+      <c r="T31" s="46" t="s">
         <v>149</v>
       </c>
+      <c r="U31" s="37"/>
       <c r="V31" s="37"/>
-      <c r="W31" s="37"/>
-      <c r="X31" s="38"/>
-    </row>
-    <row r="32" spans="2:24">
+      <c r="W31" s="38"/>
+    </row>
+    <row r="32" spans="2:29">
       <c r="B32" s="93" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="94"/>
       <c r="D32" s="95"/>
-      <c r="G32" s="9">
-        <v>43770</v>
-      </c>
-      <c r="H32" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="37"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="60"/>
       <c r="R32" s="38"/>
-      <c r="U32" s="45" t="s">
+      <c r="T32" s="45" t="s">
         <v>150</v>
       </c>
+      <c r="U32" s="37"/>
       <c r="V32" s="37"/>
-      <c r="W32" s="37"/>
-      <c r="X32" s="38"/>
-    </row>
-    <row r="33" spans="2:24">
+      <c r="W32" s="38"/>
+    </row>
+    <row r="33" spans="2:23">
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="106">
+      <c r="C33" s="102">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="107"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="50" t="s">
-        <v>168</v>
+      <c r="D33" s="103"/>
+      <c r="G33" s="9">
+        <v>43922</v>
+      </c>
+      <c r="H33" s="37" t="s">
+        <v>164</v>
       </c>
       <c r="I33" s="37"/>
       <c r="J33" s="37"/>
@@ -6912,22 +7146,24 @@
       <c r="P33" s="37"/>
       <c r="Q33" s="37"/>
       <c r="R33" s="38"/>
-      <c r="U33" s="42"/>
+      <c r="T33" s="42"/>
+      <c r="U33" s="37"/>
       <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="38"/>
-    </row>
-    <row r="34" spans="2:24">
+      <c r="W33" s="38"/>
+    </row>
+    <row r="34" spans="2:23">
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="106">
+      <c r="C34" s="102">
         <f>C6/'Financial Model'!AC9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="107"/>
+      <c r="D34" s="103"/>
       <c r="G34" s="10"/>
-      <c r="H34" s="37"/>
+      <c r="H34" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="I34" s="37"/>
       <c r="J34" s="37"/>
       <c r="K34" s="37"/>
@@ -6938,22 +7174,22 @@
       <c r="P34" s="37"/>
       <c r="Q34" s="37"/>
       <c r="R34" s="38"/>
-      <c r="U34" s="43"/>
+      <c r="T34" s="43"/>
+      <c r="U34" s="35"/>
       <c r="V34" s="35"/>
-      <c r="W34" s="35"/>
-      <c r="X34" s="36"/>
-    </row>
-    <row r="35" spans="2:24">
+      <c r="W34" s="36"/>
+    </row>
+    <row r="35" spans="2:23">
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="102">
+      <c r="C35" s="96">
         <f>C6/'Financial Model'!AC26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="103"/>
+      <c r="D35" s="97"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="60"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="37"/>
       <c r="J35" s="37"/>
       <c r="K35" s="37"/>
@@ -6962,18 +7198,14 @@
       <c r="N35" s="37"/>
       <c r="O35" s="37"/>
       <c r="P35" s="37"/>
-      <c r="Q35" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="R35" s="38"/>
-    </row>
-    <row r="36" spans="2:24">
-      <c r="G36" s="9">
-        <v>43586</v>
-      </c>
-      <c r="H36" s="60" t="s">
-        <v>166</v>
-      </c>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23">
+      <c r="G36" s="10"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="37"/>
       <c r="J36" s="37"/>
       <c r="K36" s="37"/>
@@ -6985,9 +7217,13 @@
       <c r="Q36" s="37"/>
       <c r="R36" s="38"/>
     </row>
-    <row r="37" spans="2:24">
-      <c r="G37" s="10"/>
-      <c r="H37" s="37"/>
+    <row r="37" spans="2:23">
+      <c r="G37" s="9">
+        <v>43770</v>
+      </c>
+      <c r="H37" s="37" t="s">
+        <v>167</v>
+      </c>
       <c r="I37" s="37"/>
       <c r="J37" s="37"/>
       <c r="K37" s="37"/>
@@ -6998,16 +7234,23 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="U37" s="93" t="s">
+      <c r="T37" s="93" t="s">
         <v>158</v>
       </c>
+      <c r="U37" s="94"/>
       <c r="V37" s="94"/>
-      <c r="W37" s="94"/>
-      <c r="X37" s="95"/>
-    </row>
-    <row r="38" spans="2:24">
+      <c r="W37" s="95"/>
+    </row>
+    <row r="38" spans="2:23">
+      <c r="B38" s="93" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38" s="94"/>
+      <c r="D38" s="95"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="37"/>
+      <c r="H38" s="50" t="s">
+        <v>168</v>
+      </c>
       <c r="I38" s="37"/>
       <c r="J38" s="37"/>
       <c r="K38" s="37"/>
@@ -7018,14 +7261,21 @@
       <c r="P38" s="37"/>
       <c r="Q38" s="37"/>
       <c r="R38" s="38"/>
-      <c r="U38" s="42" t="s">
+      <c r="T38" s="42" t="s">
         <v>159</v>
       </c>
+      <c r="U38" s="37"/>
       <c r="V38" s="37"/>
-      <c r="W38" s="37"/>
-      <c r="X38" s="38"/>
-    </row>
-    <row r="39" spans="2:24">
+      <c r="W38" s="38"/>
+    </row>
+    <row r="39" spans="2:23">
+      <c r="B39" s="114" t="s">
+        <v>248</v>
+      </c>
+      <c r="C39" s="115"/>
+      <c r="D39" s="51" t="s">
+        <v>31</v>
+      </c>
       <c r="G39" s="10"/>
       <c r="H39" s="37"/>
       <c r="I39" s="37"/>
@@ -7038,16 +7288,27 @@
       <c r="P39" s="37"/>
       <c r="Q39" s="37"/>
       <c r="R39" s="38"/>
-      <c r="U39" s="44" t="s">
+      <c r="T39" s="44" t="s">
         <v>160</v>
       </c>
+      <c r="U39" s="37"/>
       <c r="V39" s="37"/>
-      <c r="W39" s="37"/>
-      <c r="X39" s="38"/>
-    </row>
-    <row r="40" spans="2:24">
-      <c r="G40" s="10"/>
-      <c r="H40" s="37"/>
+      <c r="W39" s="38"/>
+    </row>
+    <row r="40" spans="2:23">
+      <c r="B40" s="114" t="s">
+        <v>249</v>
+      </c>
+      <c r="C40" s="115"/>
+      <c r="D40" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="9">
+        <v>43739</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>246</v>
+      </c>
       <c r="I40" s="37"/>
       <c r="J40" s="37"/>
       <c r="K40" s="37"/>
@@ -7056,22 +7317,25 @@
       <c r="N40" s="37"/>
       <c r="O40" s="37"/>
       <c r="P40" s="37"/>
-      <c r="Q40" s="37"/>
+      <c r="Q40" s="37" t="s">
+        <v>179</v>
+      </c>
       <c r="R40" s="38"/>
-      <c r="U40" s="44" t="s">
+      <c r="T40" s="44" t="s">
         <v>161</v>
       </c>
+      <c r="U40" s="37"/>
       <c r="V40" s="37"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="38"/>
-    </row>
-    <row r="41" spans="2:24">
-      <c r="G41" s="9">
-        <v>43282</v>
-      </c>
-      <c r="H41" s="37" t="s">
-        <v>162</v>
-      </c>
+      <c r="W40" s="38"/>
+    </row>
+    <row r="41" spans="2:23">
+      <c r="B41" s="114"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="60"/>
       <c r="I41" s="37"/>
       <c r="J41" s="37"/>
       <c r="K41" s="37"/>
@@ -7082,16 +7346,19 @@
       <c r="P41" s="37"/>
       <c r="Q41" s="37"/>
       <c r="R41" s="38"/>
-      <c r="U41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="60"/>
       <c r="V41" s="60"/>
-      <c r="W41" s="60"/>
-      <c r="X41" s="38"/>
-    </row>
-    <row r="42" spans="2:24">
+      <c r="W41" s="38"/>
+    </row>
+    <row r="42" spans="2:23">
+      <c r="B42" s="114"/>
+      <c r="C42" s="115"/>
+      <c r="D42" s="91" t="s">
+        <v>31</v>
+      </c>
       <c r="G42" s="10"/>
-      <c r="H42" s="8" t="s">
-        <v>163</v>
-      </c>
+      <c r="H42" s="37"/>
       <c r="I42" s="37"/>
       <c r="J42" s="37"/>
       <c r="K42" s="37"/>
@@ -7102,54 +7369,227 @@
       <c r="P42" s="37"/>
       <c r="Q42" s="37"/>
       <c r="R42" s="38"/>
-      <c r="U42" s="61" t="s">
+      <c r="T42" s="61" t="s">
         <v>199</v>
       </c>
+      <c r="U42" s="60"/>
       <c r="V42" s="60"/>
-      <c r="W42" s="60"/>
-      <c r="X42" s="38"/>
-    </row>
-    <row r="43" spans="2:24">
-      <c r="G43" s="11"/>
-      <c r="H43" s="54" t="s">
+      <c r="W42" s="38"/>
+    </row>
+    <row r="43" spans="2:23">
+      <c r="B43" s="116"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="10"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="37"/>
+      <c r="N43" s="37"/>
+      <c r="O43" s="37"/>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="38"/>
+      <c r="T43" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="U43" s="60"/>
+      <c r="V43" s="60"/>
+      <c r="W43" s="38"/>
+    </row>
+    <row r="44" spans="2:23">
+      <c r="G44" s="9">
+        <v>43586</v>
+      </c>
+      <c r="H44" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
+      <c r="O44" s="37"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="38"/>
+      <c r="T44" s="43"/>
+      <c r="U44" s="35"/>
+      <c r="V44" s="35"/>
+      <c r="W44" s="62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23">
+      <c r="G45" s="10"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="38"/>
+    </row>
+    <row r="46" spans="2:23">
+      <c r="G46" s="9">
+        <v>43282</v>
+      </c>
+      <c r="H46" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="37"/>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="38"/>
+    </row>
+    <row r="47" spans="2:23">
+      <c r="G47" s="10"/>
+      <c r="H47" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="38"/>
+    </row>
+    <row r="48" spans="2:23">
+      <c r="G48" s="10"/>
+      <c r="H48" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="36"/>
-      <c r="U43" s="61" t="s">
-        <v>200</v>
-      </c>
-      <c r="V43" s="60"/>
-      <c r="W43" s="60"/>
-      <c r="X43" s="38"/>
-    </row>
-    <row r="44" spans="2:24">
-      <c r="U44" s="43"/>
-      <c r="V44" s="35"/>
-      <c r="W44" s="35"/>
-      <c r="X44" s="62" t="s">
-        <v>31</v>
-      </c>
+      <c r="I48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="60"/>
+      <c r="L48" s="60"/>
+      <c r="M48" s="60"/>
+      <c r="N48" s="60"/>
+      <c r="O48" s="60"/>
+      <c r="P48" s="60"/>
+      <c r="Q48" s="60"/>
+      <c r="R48" s="38"/>
+    </row>
+    <row r="49" spans="7:18">
+      <c r="G49" s="10"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="60"/>
+      <c r="L49" s="60"/>
+      <c r="M49" s="60"/>
+      <c r="N49" s="60"/>
+      <c r="O49" s="60"/>
+      <c r="P49" s="60"/>
+      <c r="Q49" s="60"/>
+      <c r="R49" s="38"/>
+    </row>
+    <row r="50" spans="7:18">
+      <c r="G50" s="10"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="60"/>
+      <c r="L50" s="60"/>
+      <c r="M50" s="60"/>
+      <c r="N50" s="60"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="60"/>
+      <c r="Q50" s="60"/>
+      <c r="R50" s="38"/>
+    </row>
+    <row r="51" spans="7:18">
+      <c r="G51" s="10"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="60"/>
+      <c r="L51" s="60"/>
+      <c r="M51" s="60"/>
+      <c r="N51" s="60"/>
+      <c r="O51" s="60"/>
+      <c r="P51" s="60"/>
+      <c r="Q51" s="60"/>
+      <c r="R51" s="38"/>
+    </row>
+    <row r="52" spans="7:18">
+      <c r="G52" s="10"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="60"/>
+      <c r="J52" s="60"/>
+      <c r="K52" s="60"/>
+      <c r="L52" s="60"/>
+      <c r="M52" s="60"/>
+      <c r="N52" s="60"/>
+      <c r="O52" s="60"/>
+      <c r="P52" s="60"/>
+      <c r="Q52" s="60"/>
+      <c r="R52" s="38"/>
+    </row>
+    <row r="53" spans="7:18">
+      <c r="G53" s="110">
+        <v>42552</v>
+      </c>
+      <c r="H53" s="54" t="s">
+        <v>240</v>
+      </c>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="35"/>
+      <c r="P53" s="35"/>
+      <c r="Q53" s="35"/>
+      <c r="R53" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+  <mergeCells count="44">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
     <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="T5:W5"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="G5:R5"/>
@@ -7162,21 +7602,35 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
     <hyperlink ref="H10" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C29:D29" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R29" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="R35" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
     <hyperlink ref="H14" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
     <hyperlink ref="H17" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
     <hyperlink ref="R20" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
     <hyperlink ref="H23" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
-    <hyperlink ref="X44" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
+    <hyperlink ref="W44" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
+    <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
+    <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
+    <hyperlink ref="H27" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H40" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="D40" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
+    <hyperlink ref="D39" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
+    <hyperlink ref="R31" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId10"/>
-  <drawing r:id="rId11"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId17"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -7185,10 +7639,10 @@
   <dimension ref="B1:AM141"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="I96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB44" sqref="AB44"/>
+      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -9788,7 +10242,7 @@
         <v>0.2289724212385906</v>
       </c>
       <c r="X36" s="25">
-        <f t="shared" ref="X36:Z36" si="48">X11/X9</f>
+        <f t="shared" ref="X36:Y36" si="48">X11/X9</f>
         <v>0.19892239646160034</v>
       </c>
       <c r="Y36" s="25">
@@ -9889,7 +10343,7 @@
         <v>6.5462753950338556E-2</v>
       </c>
       <c r="X37" s="25">
-        <f t="shared" ref="X37:Z37" si="59">X18/X9</f>
+        <f t="shared" ref="X37:Y37" si="59">X18/X9</f>
         <v>3.3132287897064766E-2</v>
       </c>
       <c r="Y37" s="25">
@@ -9990,7 +10444,7 @@
         <v>7.2725488271665487E-2</v>
       </c>
       <c r="X38" s="25">
-        <f t="shared" ref="X38:Z38" si="70">X23/X9</f>
+        <f t="shared" ref="X38:Y38" si="70">X23/X9</f>
         <v>2.6988339364696447E-2</v>
       </c>
       <c r="Y38" s="25">
@@ -10091,7 +10545,7 @@
         <v>-0.49696969696969745</v>
       </c>
       <c r="X39" s="25">
-        <f t="shared" ref="X39:Z39" si="80">X22/X21</f>
+        <f t="shared" ref="X39:Y39" si="80">X22/X21</f>
         <v>-5.4682589566310433E-2</v>
       </c>
       <c r="Y39" s="25">
@@ -10197,7 +10651,7 @@
         <v>32</v>
       </c>
       <c r="X43" s="2">
-        <f t="shared" ref="X43:Z43" si="90">X44+X52</f>
+        <f t="shared" ref="X43:Y43" si="90">X44+X52</f>
         <v>225</v>
       </c>
       <c r="Y43" s="2">
@@ -10298,7 +10752,7 @@
         <v>11</v>
       </c>
       <c r="X44" s="40">
-        <f t="shared" ref="X44:Z44" si="96">SUM(X45:X50)</f>
+        <f t="shared" ref="X44:Y44" si="96">SUM(X45:X50)</f>
         <v>108</v>
       </c>
       <c r="Y44" s="40">
@@ -10864,7 +11318,7 @@
         <v>21</v>
       </c>
       <c r="X52" s="40">
-        <f t="shared" ref="X52:Z52" si="104">X53+X54+X55</f>
+        <f t="shared" ref="X52:Y52" si="104">X53+X54+X55</f>
         <v>117</v>
       </c>
       <c r="Y52" s="40">
@@ -13697,7 +14151,7 @@
         <v>12.3</v>
       </c>
       <c r="X90" s="27">
-        <f t="shared" ref="X90:Y91" si="126">G90</f>
+        <f t="shared" ref="X90:X91" si="126">G90</f>
         <v>0</v>
       </c>
       <c r="Y90" s="27">
@@ -14278,7 +14732,7 @@
         <v>68.400000000000006</v>
       </c>
       <c r="AA97" s="27">
-        <f t="shared" ref="Z97:AA115" si="134">J97</f>
+        <f t="shared" ref="AA97:AA115" si="134">J97</f>
         <v>63.8</v>
       </c>
       <c r="AB97" s="27">
@@ -15025,7 +15479,7 @@
         <v>3809.6</v>
       </c>
       <c r="Z106" s="26">
-        <f>F106</f>
+        <f t="shared" ref="Z106:Z115" si="139">F106</f>
         <v>3468.4</v>
       </c>
       <c r="AA106" s="26">
@@ -15106,7 +15560,7 @@
         <v>346.5</v>
       </c>
       <c r="Z107" s="26">
-        <f>F107</f>
+        <f t="shared" si="139"/>
         <v>17.399999999999999</v>
       </c>
       <c r="AA107" s="26">
@@ -15187,7 +15641,7 @@
         <v>21.5</v>
       </c>
       <c r="Z108" s="27">
-        <f>F108</f>
+        <f t="shared" si="139"/>
         <v>28.6</v>
       </c>
       <c r="AA108" s="27">
@@ -15195,11 +15649,11 @@
         <v>18</v>
       </c>
       <c r="AB108" s="27">
-        <f t="shared" ref="AB108:AB115" si="139">N108</f>
+        <f t="shared" ref="AB108:AB115" si="140">N108</f>
         <v>42.3</v>
       </c>
       <c r="AC108" s="27">
-        <f t="shared" ref="AC108:AC115" si="140">R108</f>
+        <f t="shared" ref="AC108:AC115" si="141">R108</f>
         <v>57.6</v>
       </c>
     </row>
@@ -15268,7 +15722,7 @@
         <v>104.1</v>
       </c>
       <c r="Z109" s="27">
-        <f>F109</f>
+        <f t="shared" si="139"/>
         <v>198.2</v>
       </c>
       <c r="AA109" s="27">
@@ -15276,11 +15730,11 @@
         <v>257.8</v>
       </c>
       <c r="AB109" s="27">
-        <f t="shared" si="139"/>
+        <f t="shared" si="140"/>
         <v>262.39999999999998</v>
       </c>
       <c r="AC109" s="27">
-        <f t="shared" si="140"/>
+        <f t="shared" si="141"/>
         <v>308.7</v>
       </c>
     </row>
@@ -15349,7 +15803,7 @@
         <v>0.1</v>
       </c>
       <c r="Z110" s="27">
-        <f>F110</f>
+        <f t="shared" si="139"/>
         <v>0</v>
       </c>
       <c r="AA110" s="27">
@@ -15357,11 +15811,11 @@
         <v>0</v>
       </c>
       <c r="AB110" s="27">
-        <f t="shared" si="139"/>
+        <f t="shared" si="140"/>
         <v>8.6999999999999993</v>
       </c>
       <c r="AC110" s="27">
-        <f t="shared" si="140"/>
+        <f t="shared" si="141"/>
         <v>3</v>
       </c>
     </row>
@@ -15430,7 +15884,7 @@
         <v>70.2</v>
       </c>
       <c r="Z111" s="27">
-        <f>F111</f>
+        <f t="shared" si="139"/>
         <v>58.2</v>
       </c>
       <c r="AA111" s="27">
@@ -15438,11 +15892,11 @@
         <v>13.4</v>
       </c>
       <c r="AB111" s="27">
-        <f t="shared" si="139"/>
+        <f t="shared" si="140"/>
         <v>11.8</v>
       </c>
       <c r="AC111" s="27">
-        <f t="shared" si="140"/>
+        <f t="shared" si="141"/>
         <v>10</v>
       </c>
     </row>
@@ -15511,7 +15965,7 @@
         <v>251.3</v>
       </c>
       <c r="Z112" s="27">
-        <f>F112</f>
+        <f t="shared" si="139"/>
         <v>254</v>
       </c>
       <c r="AA112" s="27">
@@ -15519,11 +15973,11 @@
         <v>301</v>
       </c>
       <c r="AB112" s="27">
-        <f t="shared" si="139"/>
+        <f t="shared" si="140"/>
         <v>474.7</v>
       </c>
       <c r="AC112" s="27">
-        <f t="shared" si="140"/>
+        <f t="shared" si="141"/>
         <v>505.8</v>
       </c>
     </row>
@@ -15592,7 +16046,7 @@
         <v>134.6</v>
       </c>
       <c r="Z113" s="27">
-        <f>F113</f>
+        <f t="shared" si="139"/>
         <v>101.1</v>
       </c>
       <c r="AA113" s="27">
@@ -15600,11 +16054,11 @@
         <v>109.6</v>
       </c>
       <c r="AB113" s="27">
-        <f t="shared" si="139"/>
+        <f t="shared" si="140"/>
         <v>82.6</v>
       </c>
       <c r="AC113" s="27">
-        <f t="shared" si="140"/>
+        <f t="shared" si="141"/>
         <v>2.9</v>
       </c>
     </row>
@@ -15673,7 +16127,7 @@
         <v>97.5</v>
       </c>
       <c r="Z114" s="27">
-        <f>F114</f>
+        <f t="shared" si="139"/>
         <v>73.2</v>
       </c>
       <c r="AA114" s="27">
@@ -15681,11 +16135,11 @@
         <v>63.7</v>
       </c>
       <c r="AB114" s="27">
-        <f t="shared" si="139"/>
+        <f t="shared" si="140"/>
         <v>57.3</v>
       </c>
       <c r="AC114" s="27">
-        <f t="shared" si="140"/>
+        <f t="shared" si="141"/>
         <v>37.700000000000003</v>
       </c>
     </row>
@@ -15754,7 +16208,7 @@
         <v>136.19999999999999</v>
       </c>
       <c r="Z115" s="27">
-        <f>F115</f>
+        <f t="shared" si="139"/>
         <v>125.5</v>
       </c>
       <c r="AA115" s="27">
@@ -15762,11 +16216,11 @@
         <v>125.2</v>
       </c>
       <c r="AB115" s="27">
-        <f t="shared" si="139"/>
+        <f t="shared" si="140"/>
         <v>114.2</v>
       </c>
       <c r="AC115" s="27">
-        <f t="shared" si="140"/>
+        <f t="shared" si="141"/>
         <v>120.5</v>
       </c>
     </row>
@@ -15775,91 +16229,91 @@
         <v>118</v>
       </c>
       <c r="C116" s="27">
-        <f t="shared" ref="C116:T116" si="141">SUM(C105:C115)+C104</f>
+        <f t="shared" ref="C116:T116" si="142">SUM(C105:C115)+C104</f>
         <v>7811.2000000000007</v>
       </c>
       <c r="D116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7821</v>
       </c>
       <c r="E116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7824.7999999999993</v>
       </c>
       <c r="F116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7353.2</v>
       </c>
       <c r="G116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7293.7999999999993</v>
       </c>
       <c r="H116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7363.3</v>
       </c>
       <c r="I116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7260.1999999999989</v>
       </c>
       <c r="J116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>6957.9</v>
       </c>
       <c r="K116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7571.6999999999989</v>
       </c>
       <c r="L116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7345.1</v>
       </c>
       <c r="M116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7574.5</v>
       </c>
       <c r="N116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7608.5</v>
       </c>
       <c r="O116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7513.7</v>
       </c>
       <c r="P116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7455.6400000000012</v>
       </c>
       <c r="Q116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7574.5</v>
       </c>
       <c r="R116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7379.9999999999991</v>
       </c>
       <c r="S116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>7111.5000000000009</v>
       </c>
       <c r="T116" s="27">
-        <f t="shared" si="141"/>
+        <f t="shared" si="142"/>
         <v>6826.0999999999995</v>
       </c>
       <c r="X116" s="27">
-        <f t="shared" ref="X116:Y116" si="142">SUM(X105:X115)+X104</f>
+        <f t="shared" ref="X116:Y116" si="143">SUM(X105:X115)+X104</f>
         <v>7731.9000000000005</v>
       </c>
       <c r="Y116" s="27">
-        <f t="shared" si="142"/>
+        <f t="shared" si="143"/>
         <v>7763.7000000000007</v>
       </c>
       <c r="Z116" s="27">
-        <f t="shared" ref="Z116:AA116" si="143">SUM(Z105:Z115)+Z104</f>
+        <f t="shared" ref="Z116:AA116" si="144">SUM(Z105:Z115)+Z104</f>
         <v>7353.2</v>
       </c>
       <c r="AA116" s="27">
-        <f t="shared" si="143"/>
+        <f t="shared" si="144"/>
         <v>6957.9</v>
       </c>
       <c r="AB116" s="27">
@@ -15951,7 +16405,7 @@
         <v>3940.1</v>
       </c>
       <c r="AA118" s="27">
-        <f t="shared" ref="AA118" si="144">J118</f>
+        <f t="shared" ref="AA118" si="145">J118</f>
         <v>3614.6</v>
       </c>
       <c r="AB118" s="27">
@@ -15968,83 +16422,83 @@
         <v>120</v>
       </c>
       <c r="C119" s="27">
-        <f t="shared" ref="C119:D119" si="145">C118+C116</f>
+        <f t="shared" ref="C119:D119" si="146">C118+C116</f>
         <v>11995.1</v>
       </c>
       <c r="D119" s="27">
-        <f t="shared" si="145"/>
+        <f t="shared" si="146"/>
         <v>11811.1</v>
       </c>
       <c r="E119" s="27">
-        <f t="shared" ref="E119:K119" si="146">E118+E116</f>
+        <f t="shared" ref="E119:K119" si="147">E118+E116</f>
         <v>11794.5</v>
       </c>
       <c r="F119" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="147"/>
         <v>11293.3</v>
       </c>
       <c r="G119" s="27">
-        <f t="shared" ref="G119" si="147">G118+G116</f>
+        <f t="shared" ref="G119" si="148">G118+G116</f>
         <v>11185.5</v>
       </c>
       <c r="H119" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="147"/>
         <v>11273.4</v>
       </c>
       <c r="I119" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="147"/>
         <v>11062.5</v>
       </c>
       <c r="J119" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="147"/>
         <v>10572.5</v>
       </c>
       <c r="K119" s="27">
-        <f t="shared" si="146"/>
+        <f t="shared" si="147"/>
         <v>10856.099999999999</v>
       </c>
       <c r="L119" s="27">
-        <f t="shared" ref="L119:T119" si="148">L118+L116</f>
+        <f t="shared" ref="L119:T119" si="149">L118+L116</f>
         <v>10325.400000000001</v>
       </c>
       <c r="M119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>10382.700000000001</v>
       </c>
       <c r="N119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>10516</v>
       </c>
       <c r="O119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>10308.1</v>
       </c>
       <c r="P119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>10341.34</v>
       </c>
       <c r="Q119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>10382.700000000001</v>
       </c>
       <c r="R119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>10155</v>
       </c>
       <c r="S119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>9868.4000000000015</v>
       </c>
       <c r="T119" s="27">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>9698.7999999999993</v>
       </c>
       <c r="X119" s="27">
-        <f t="shared" ref="X119:Y119" si="149">X118+X116</f>
+        <f t="shared" ref="X119:Y119" si="150">X118+X116</f>
         <v>11673.1</v>
       </c>
       <c r="Y119" s="27">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>11945.7</v>
       </c>
       <c r="Z119" s="27">
@@ -16082,67 +16536,67 @@
         <v>121</v>
       </c>
       <c r="C121" s="27">
-        <f t="shared" ref="C121:D121" si="150">C87-C116</f>
+        <f t="shared" ref="C121:D121" si="151">C87-C116</f>
         <v>4183.8999999999978</v>
       </c>
       <c r="D121" s="27">
-        <f t="shared" si="150"/>
+        <f t="shared" si="151"/>
         <v>3990.0999999999985</v>
       </c>
       <c r="E121" s="27">
-        <f t="shared" ref="E121" si="151">E87-E116</f>
+        <f t="shared" ref="E121" si="152">E87-E116</f>
         <v>3969.7000000000007</v>
       </c>
       <c r="F121" s="27">
-        <f t="shared" ref="F121:G121" si="152">F87-F116</f>
+        <f t="shared" ref="F121:G121" si="153">F87-F116</f>
         <v>3940.2</v>
       </c>
       <c r="G121" s="27">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>3891.8000000000011</v>
       </c>
       <c r="H121" s="27">
-        <f t="shared" ref="H121:I121" si="153">H87-H116</f>
+        <f t="shared" ref="H121:I121" si="154">H87-H116</f>
         <v>3910.0999999999995</v>
       </c>
       <c r="I121" s="27">
-        <f t="shared" si="153"/>
+        <f t="shared" si="154"/>
         <v>3802.3000000000011</v>
       </c>
       <c r="J121" s="27">
-        <f t="shared" ref="J121:K121" si="154">J87-J116</f>
+        <f t="shared" ref="J121:K121" si="155">J87-J116</f>
         <v>3614.6000000000004</v>
       </c>
       <c r="K121" s="27">
-        <f t="shared" si="154"/>
+        <f t="shared" si="155"/>
         <v>3284.3999999999996</v>
       </c>
       <c r="L121" s="27">
-        <f t="shared" ref="L121:O121" si="155">L87-L116</f>
+        <f t="shared" ref="L121:O121" si="156">L87-L116</f>
         <v>2980.3000000000011</v>
       </c>
       <c r="M121" s="27">
-        <f t="shared" ref="M121" si="156">M87-M116</f>
+        <f t="shared" ref="M121" si="157">M87-M116</f>
         <v>2808.2000000000007</v>
       </c>
       <c r="N121" s="27">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>2907.5</v>
       </c>
       <c r="O121" s="27">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>2794.4000000000005</v>
       </c>
       <c r="P121" s="27">
-        <f t="shared" ref="P121:Q121" si="157">P87-P116</f>
+        <f t="shared" ref="P121:Q121" si="158">P87-P116</f>
         <v>2885.659999999998</v>
       </c>
       <c r="Q121" s="27">
-        <f t="shared" si="157"/>
+        <f t="shared" si="158"/>
         <v>2808.2000000000007</v>
       </c>
       <c r="R121" s="27">
-        <f t="shared" ref="R121" si="158">R87-R116</f>
+        <f t="shared" ref="R121" si="159">R87-R116</f>
         <v>2775.0000000000009</v>
       </c>
       <c r="S121" s="27">
@@ -16154,23 +16608,23 @@
         <v>2872.7</v>
       </c>
       <c r="X121" s="27">
-        <f t="shared" ref="X121:Z121" si="159">X87-X116</f>
+        <f t="shared" ref="X121:Z121" si="160">X87-X116</f>
         <v>3932.699999999998</v>
       </c>
       <c r="Y121" s="27">
-        <f t="shared" si="159"/>
+        <f t="shared" si="160"/>
         <v>4172.5</v>
       </c>
       <c r="Z121" s="27">
-        <f t="shared" si="159"/>
+        <f t="shared" si="160"/>
         <v>3940.2</v>
       </c>
       <c r="AA121" s="27">
-        <f t="shared" ref="AA121:AB121" si="160">AA87-AA116</f>
+        <f t="shared" ref="AA121:AB121" si="161">AA87-AA116</f>
         <v>3614.6000000000004</v>
       </c>
       <c r="AB121" s="27">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>2907.5</v>
       </c>
       <c r="AC121" s="27">
@@ -16183,67 +16637,67 @@
         <v>122</v>
       </c>
       <c r="C122" s="3">
-        <f t="shared" ref="C122:D122" si="161">C121/C27</f>
+        <f t="shared" ref="C122:D122" si="162">C121/C27</f>
         <v>5.705577526251191</v>
       </c>
       <c r="D122" s="3">
-        <f t="shared" si="161"/>
+        <f t="shared" si="162"/>
         <v>5.4398091342876596</v>
       </c>
       <c r="E122" s="3">
-        <f t="shared" ref="E122" si="162">E121/E27</f>
+        <f t="shared" ref="E122" si="163">E121/E27</f>
         <v>5.4097846824747897</v>
       </c>
       <c r="F122" s="3">
-        <f t="shared" ref="F122:G122" si="163">F121/F27</f>
+        <f t="shared" ref="F122:G122" si="164">F121/F27</f>
         <v>5.3673886391499792</v>
       </c>
       <c r="G122" s="3">
-        <f t="shared" si="163"/>
+        <f t="shared" si="164"/>
         <v>5.2899279597662101</v>
       </c>
       <c r="H122" s="3">
-        <f t="shared" ref="H122:I122" si="164">H121/H27</f>
+        <f t="shared" ref="H122:I122" si="165">H121/H27</f>
         <v>5.3140799130198415</v>
       </c>
       <c r="I122" s="3">
-        <f t="shared" si="164"/>
+        <f t="shared" si="165"/>
         <v>5.1675727099755386</v>
       </c>
       <c r="J122" s="3">
-        <f t="shared" ref="J122:K122" si="165">J121/J27</f>
+        <f t="shared" ref="J122:K122" si="166">J121/J27</f>
         <v>4.911808669656204</v>
       </c>
       <c r="K122" s="3">
-        <f t="shared" si="165"/>
+        <f t="shared" si="166"/>
         <v>4.4618937644341798</v>
       </c>
       <c r="L122" s="3">
-        <f t="shared" ref="L122:M122" si="166">L121/L27</f>
+        <f t="shared" ref="L122:M122" si="167">L121/L27</f>
         <v>4.0482205922303738</v>
       </c>
       <c r="M122" s="3">
-        <f t="shared" si="166"/>
+        <f t="shared" si="167"/>
         <v>3.8144525944036953</v>
       </c>
       <c r="N122" s="3">
-        <f t="shared" ref="N122:Q122" si="167">N121/N27</f>
+        <f t="shared" ref="N122:Q122" si="168">N121/N27</f>
         <v>3.9493344199945666</v>
       </c>
       <c r="O122" s="3">
-        <f t="shared" ref="O122" si="168">O121/O27</f>
+        <f t="shared" ref="O122" si="169">O121/O27</f>
         <v>3.8019047619047628</v>
       </c>
       <c r="P122" s="3">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>3.9271366358192683</v>
       </c>
       <c r="Q122" s="3">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>3.821720195971694</v>
       </c>
       <c r="R122" s="3">
-        <f t="shared" ref="R122" si="169">R121/R27</f>
+        <f t="shared" ref="R122" si="170">R121/R27</f>
         <v>3.7770518579011854</v>
       </c>
       <c r="S122" s="3">
@@ -16255,23 +16709,23 @@
         <v>3.9105635720119789</v>
       </c>
       <c r="X122" s="3">
-        <f t="shared" ref="X122:Z122" si="170">X121/X27</f>
+        <f t="shared" ref="X122:Z122" si="171">X121/X27</f>
         <v>5.3462479608482845</v>
       </c>
       <c r="Y122" s="3">
-        <f t="shared" si="170"/>
+        <f t="shared" si="171"/>
         <v>5.6822824458668126</v>
       </c>
       <c r="Z122" s="3">
-        <f t="shared" si="170"/>
+        <f t="shared" si="171"/>
         <v>5.3673886391499792</v>
       </c>
       <c r="AA122" s="3">
-        <f t="shared" ref="AA122:AB122" si="171">AA121/AA27</f>
+        <f t="shared" ref="AA122:AB122" si="172">AA121/AA27</f>
         <v>4.911808669656204</v>
       </c>
       <c r="AB122" s="3">
-        <f t="shared" si="171"/>
+        <f t="shared" si="172"/>
         <v>3.9493344199945666</v>
       </c>
       <c r="AC122" s="3">
@@ -16292,71 +16746,71 @@
         <v>6</v>
       </c>
       <c r="C124" s="52">
-        <f t="shared" ref="C124:D124" si="172">C61+C62+C74+C76</f>
+        <f t="shared" ref="C124:D124" si="173">C61+C62+C74+C76</f>
         <v>3435.7999999999997</v>
       </c>
       <c r="D124" s="52">
-        <f t="shared" si="172"/>
+        <f t="shared" si="173"/>
         <v>3346.5</v>
       </c>
       <c r="E124" s="52">
-        <f t="shared" ref="E124" si="173">E61+E62+E74+E76</f>
+        <f t="shared" ref="E124" si="174">E61+E62+E74+E76</f>
         <v>3147.6</v>
       </c>
       <c r="F124" s="52">
-        <f t="shared" ref="F124:G124" si="174">F61+F62+F74+F76</f>
+        <f t="shared" ref="F124:G124" si="175">F61+F62+F74+F76</f>
         <v>3211.9</v>
       </c>
       <c r="G124" s="52">
-        <f t="shared" si="174"/>
+        <f t="shared" si="175"/>
         <v>2485.4999999999995</v>
       </c>
       <c r="H124" s="52">
-        <f t="shared" ref="H124:I124" si="175">H61+H62+H74+H76</f>
+        <f t="shared" ref="H124:I124" si="176">H61+H62+H74+H76</f>
         <v>2480.8999999999996</v>
       </c>
       <c r="I124" s="52">
-        <f t="shared" si="175"/>
+        <f t="shared" si="176"/>
         <v>2177.2000000000003</v>
       </c>
       <c r="J124" s="52">
-        <f t="shared" ref="J124:K124" si="176">J61+J62+J74+J76</f>
+        <f t="shared" ref="J124:K124" si="177">J61+J62+J74+J76</f>
         <v>2780.6</v>
       </c>
       <c r="K124" s="52">
-        <f t="shared" si="176"/>
+        <f t="shared" si="177"/>
         <v>2501.1</v>
       </c>
       <c r="L124" s="52">
-        <f t="shared" ref="L124:O124" si="177">L61+L62+L74+L76</f>
+        <f t="shared" ref="L124:O124" si="178">L61+L62+L74+L76</f>
         <v>1998.9</v>
       </c>
       <c r="M124" s="52">
-        <f t="shared" ref="M124" si="178">M61+M62+M74+M76</f>
+        <f t="shared" ref="M124" si="179">M61+M62+M74+M76</f>
         <v>2503.6999999999998</v>
       </c>
       <c r="N124" s="52">
-        <f t="shared" si="177"/>
+        <f t="shared" si="178"/>
         <v>2753.6</v>
       </c>
       <c r="O124" s="52">
-        <f t="shared" si="177"/>
+        <f t="shared" si="178"/>
         <v>2463.4</v>
       </c>
       <c r="P124" s="52">
-        <f t="shared" ref="P124:Q124" si="179">P61+P62+P74+P76</f>
+        <f t="shared" ref="P124:Q124" si="180">P61+P62+P74+P76</f>
         <v>2514.3000000000002</v>
       </c>
       <c r="Q124" s="52">
-        <f t="shared" si="179"/>
+        <f t="shared" si="180"/>
         <v>2503.6999999999998</v>
       </c>
       <c r="R124" s="52">
-        <f t="shared" ref="R124" si="180">R61+R62+R74+R76</f>
+        <f t="shared" ref="R124" si="181">R61+R62+R74+R76</f>
         <v>2634.7</v>
       </c>
       <c r="S124" s="52">
-        <f t="shared" ref="S124" si="181">S61+S62+S74+S76</f>
+        <f t="shared" ref="S124" si="182">S61+S62+S74+S76</f>
         <v>2104.1999999999998</v>
       </c>
       <c r="T124" s="52">
@@ -16364,23 +16818,23 @@
         <v>1968.2</v>
       </c>
       <c r="X124" s="52">
-        <f t="shared" ref="X124:Z124" si="182">X61+X62+X74+X76</f>
+        <f t="shared" ref="X124:Z124" si="183">X61+X62+X74+X76</f>
         <v>3196.2999999999997</v>
       </c>
       <c r="Y124" s="52">
-        <f t="shared" si="182"/>
+        <f t="shared" si="183"/>
         <v>3892.5</v>
       </c>
       <c r="Z124" s="52">
-        <f t="shared" si="182"/>
+        <f t="shared" si="183"/>
         <v>3211.9</v>
       </c>
       <c r="AA124" s="52">
-        <f t="shared" ref="AA124:AB124" si="183">AA61+AA62+AA74+AA76</f>
+        <f t="shared" ref="AA124:AB124" si="184">AA61+AA62+AA74+AA76</f>
         <v>2780.6</v>
       </c>
       <c r="AB124" s="52">
-        <f t="shared" si="183"/>
+        <f t="shared" si="184"/>
         <v>2753.6</v>
       </c>
       <c r="AC124" s="52">
@@ -16393,39 +16847,39 @@
         <v>7</v>
       </c>
       <c r="C125" s="52">
-        <f t="shared" ref="C125:D125" si="184">C92+C96+C106+C93+C107</f>
+        <f t="shared" ref="C125:D125" si="185">C92+C96+C106+C93+C107</f>
         <v>4559.1000000000004</v>
       </c>
       <c r="D125" s="52">
-        <f t="shared" si="184"/>
+        <f t="shared" si="185"/>
         <v>4452.8</v>
       </c>
       <c r="E125" s="52">
-        <f t="shared" ref="E125" si="185">E92+E96+E106+E93+E107</f>
+        <f t="shared" ref="E125" si="186">E92+E96+E106+E93+E107</f>
         <v>4399.8</v>
       </c>
       <c r="F125" s="52">
-        <f t="shared" ref="F125:G125" si="186">F92+F96+F106+F93+F107</f>
+        <f t="shared" ref="F125:G125" si="187">F92+F96+F106+F93+F107</f>
         <v>3997.2000000000003</v>
       </c>
       <c r="G125" s="52">
-        <f t="shared" si="186"/>
+        <f t="shared" si="187"/>
         <v>3928.3</v>
       </c>
       <c r="H125" s="52">
-        <f t="shared" ref="H125:I125" si="187">H92+H96+H106+H93+H107</f>
+        <f t="shared" ref="H125:I125" si="188">H92+H96+H106+H93+H107</f>
         <v>3879.5</v>
       </c>
       <c r="I125" s="52">
-        <f t="shared" si="187"/>
+        <f t="shared" si="188"/>
         <v>3811.6</v>
       </c>
       <c r="J125" s="52">
-        <f t="shared" ref="J125:K125" si="188">J92+J96+J106+J93+J107</f>
+        <f t="shared" ref="J125:K125" si="189">J92+J96+J106+J93+J107</f>
         <v>3414.4</v>
       </c>
       <c r="K125" s="52">
-        <f t="shared" si="188"/>
+        <f t="shared" si="189"/>
         <v>3862.2</v>
       </c>
       <c r="L125" s="52">
@@ -16433,7 +16887,7 @@
         <v>3826.3999999999996</v>
       </c>
       <c r="M125" s="52">
-        <f t="shared" ref="M125" si="189">M92+M96+M106+M93+M107</f>
+        <f t="shared" ref="M125" si="190">M92+M96+M106+M93+M107</f>
         <v>4310.1000000000004</v>
       </c>
       <c r="N125" s="52">
@@ -16441,51 +16895,51 @@
         <v>4449.2</v>
       </c>
       <c r="O125" s="52">
-        <f t="shared" ref="O125" si="190">O92+O96+O106+O93+O107</f>
+        <f t="shared" ref="O125" si="191">O92+O96+O106+O93+O107</f>
         <v>4380</v>
       </c>
       <c r="P125" s="52">
-        <f t="shared" ref="P125:T125" si="191">P92+P96+P106+P93+P107</f>
+        <f t="shared" ref="P125:T125" si="192">P92+P96+P106+P93+P107</f>
         <v>4334.0999999999995</v>
       </c>
       <c r="Q125" s="52">
-        <f t="shared" si="191"/>
+        <f t="shared" si="192"/>
         <v>4310.1000000000004</v>
       </c>
       <c r="R125" s="52">
-        <f t="shared" si="191"/>
+        <f t="shared" si="192"/>
         <v>4029.7999999999997</v>
       </c>
       <c r="S125" s="52">
-        <f t="shared" si="191"/>
+        <f t="shared" si="192"/>
         <v>3559</v>
       </c>
       <c r="T125" s="52">
-        <f t="shared" si="191"/>
+        <f t="shared" si="192"/>
         <v>3173.8999999999996</v>
       </c>
       <c r="X125" s="52">
-        <f t="shared" ref="X125:Y125" si="192">X92+X96+X106+X93+X107</f>
+        <f t="shared" ref="X125:Y125" si="193">X92+X96+X106+X93+X107</f>
         <v>4142.2000000000007</v>
       </c>
       <c r="Y125" s="52">
-        <f t="shared" si="192"/>
+        <f t="shared" si="193"/>
         <v>4571.4000000000005</v>
       </c>
       <c r="Z125" s="52">
-        <f t="shared" ref="Z125:AA125" si="193">Z92+Z96+Z106+Z93+Z107</f>
+        <f t="shared" ref="Z125:AA125" si="194">Z92+Z96+Z106+Z93+Z107</f>
         <v>3997.2000000000003</v>
       </c>
       <c r="AA125" s="52">
-        <f t="shared" si="193"/>
+        <f t="shared" si="194"/>
         <v>3414.4</v>
       </c>
       <c r="AB125" s="52">
-        <f t="shared" ref="AB125:AC125" si="194">AB92+AB96+AB106+AB93+AB107</f>
+        <f t="shared" ref="AB125:AC125" si="195">AB92+AB96+AB106+AB93+AB107</f>
         <v>4449.2</v>
       </c>
       <c r="AC125" s="52">
-        <f t="shared" si="194"/>
+        <f t="shared" si="195"/>
         <v>4029.7999999999997</v>
       </c>
     </row>
@@ -16494,67 +16948,67 @@
         <v>8</v>
       </c>
       <c r="C126" s="27">
-        <f t="shared" ref="C126:D126" si="195">C124-C125</f>
+        <f t="shared" ref="C126:D126" si="196">C124-C125</f>
         <v>-1123.3000000000006</v>
       </c>
       <c r="D126" s="27">
-        <f t="shared" si="195"/>
+        <f t="shared" si="196"/>
         <v>-1106.3000000000002</v>
       </c>
       <c r="E126" s="27">
-        <f t="shared" ref="E126" si="196">E124-E125</f>
+        <f t="shared" ref="E126" si="197">E124-E125</f>
         <v>-1252.2000000000003</v>
       </c>
       <c r="F126" s="27">
-        <f t="shared" ref="F126:G126" si="197">F124-F125</f>
+        <f t="shared" ref="F126:G126" si="198">F124-F125</f>
         <v>-785.30000000000018</v>
       </c>
       <c r="G126" s="27">
-        <f t="shared" si="197"/>
+        <f t="shared" si="198"/>
         <v>-1442.8000000000006</v>
       </c>
       <c r="H126" s="27">
-        <f t="shared" ref="H126:I126" si="198">H124-H125</f>
+        <f t="shared" ref="H126:I126" si="199">H124-H125</f>
         <v>-1398.6000000000004</v>
       </c>
       <c r="I126" s="27">
-        <f t="shared" si="198"/>
+        <f t="shared" si="199"/>
         <v>-1634.3999999999996</v>
       </c>
       <c r="J126" s="27">
-        <f t="shared" ref="J126:K126" si="199">J124-J125</f>
+        <f t="shared" ref="J126:K126" si="200">J124-J125</f>
         <v>-633.80000000000018</v>
       </c>
       <c r="K126" s="27">
-        <f t="shared" si="199"/>
+        <f t="shared" si="200"/>
         <v>-1361.1</v>
       </c>
       <c r="L126" s="27">
-        <f t="shared" ref="L126:M126" si="200">L124-L125</f>
+        <f t="shared" ref="L126:M126" si="201">L124-L125</f>
         <v>-1827.4999999999995</v>
       </c>
       <c r="M126" s="27">
-        <f t="shared" si="200"/>
-        <v>-1806.4000000000005</v>
-      </c>
-      <c r="N126" s="27">
-        <f t="shared" ref="N126:R126" si="201">N124-N125</f>
-        <v>-1695.6</v>
-      </c>
-      <c r="O126" s="27">
-        <f t="shared" ref="O126" si="202">O124-O125</f>
-        <v>-1916.6</v>
-      </c>
-      <c r="P126" s="27">
-        <f t="shared" si="201"/>
-        <v>-1819.7999999999993</v>
-      </c>
-      <c r="Q126" s="27">
         <f t="shared" si="201"/>
         <v>-1806.4000000000005</v>
       </c>
+      <c r="N126" s="27">
+        <f t="shared" ref="N126:R126" si="202">N124-N125</f>
+        <v>-1695.6</v>
+      </c>
+      <c r="O126" s="27">
+        <f t="shared" ref="O126" si="203">O124-O125</f>
+        <v>-1916.6</v>
+      </c>
+      <c r="P126" s="27">
+        <f t="shared" si="202"/>
+        <v>-1819.7999999999993</v>
+      </c>
+      <c r="Q126" s="27">
+        <f t="shared" si="202"/>
+        <v>-1806.4000000000005</v>
+      </c>
       <c r="R126" s="27">
-        <f t="shared" si="201"/>
+        <f t="shared" si="202"/>
         <v>-1395.1</v>
       </c>
       <c r="S126" s="27">
@@ -16566,23 +17020,23 @@
         <v>-1205.6999999999996</v>
       </c>
       <c r="X126" s="27">
-        <f t="shared" ref="X126:Z126" si="203">X124-X125</f>
+        <f t="shared" ref="X126:Z126" si="204">X124-X125</f>
         <v>-945.900000000001</v>
       </c>
       <c r="Y126" s="27">
-        <f t="shared" si="203"/>
+        <f t="shared" si="204"/>
         <v>-678.90000000000055</v>
       </c>
       <c r="Z126" s="27">
-        <f t="shared" si="203"/>
+        <f t="shared" si="204"/>
         <v>-785.30000000000018</v>
       </c>
       <c r="AA126" s="27">
-        <f t="shared" ref="AA126:AB126" si="204">AA124-AA125</f>
+        <f t="shared" ref="AA126:AB126" si="205">AA124-AA125</f>
         <v>-633.80000000000018</v>
       </c>
       <c r="AB126" s="27">
-        <f t="shared" si="204"/>
+        <f t="shared" si="205"/>
         <v>-1695.6</v>
       </c>
       <c r="AC126" s="27">
@@ -16607,55 +17061,55 @@
         <v>186</v>
       </c>
       <c r="G128" s="34">
-        <f t="shared" ref="G128" si="205">G68/C68-1</f>
+        <f t="shared" ref="G128" si="206">G68/C68-1</f>
         <v>0.20714400903080143</v>
       </c>
       <c r="H128" s="34">
-        <f t="shared" ref="H128" si="206">H68/D68-1</f>
+        <f t="shared" ref="H128" si="207">H68/D68-1</f>
         <v>0.18512820512820527</v>
       </c>
       <c r="I128" s="34">
-        <f t="shared" ref="I128" si="207">I68/E68-1</f>
+        <f t="shared" ref="I128" si="208">I68/E68-1</f>
         <v>0.10459366489895361</v>
       </c>
       <c r="J128" s="34">
-        <f t="shared" ref="J128:L128" si="208">J68/F68-1</f>
+        <f t="shared" ref="J128:L128" si="209">J68/F68-1</f>
         <v>-4.9062624650977216E-2</v>
       </c>
       <c r="K128" s="34">
-        <f t="shared" ref="K128" si="209">K68/G68-1</f>
+        <f t="shared" ref="K128" si="210">K68/G68-1</f>
         <v>-2.3011154899472142E-2</v>
       </c>
       <c r="L128" s="34">
-        <f t="shared" si="208"/>
+        <f t="shared" si="209"/>
         <v>4.1440601804080712E-2</v>
       </c>
       <c r="M128" s="34">
-        <f t="shared" ref="M128" si="210">M68/I68-1</f>
+        <f t="shared" ref="M128" si="211">M68/I68-1</f>
         <v>-0.25227884646576049</v>
       </c>
       <c r="N128" s="34">
-        <f t="shared" ref="N128" si="211">N68/J68-1</f>
+        <f t="shared" ref="N128" si="212">N68/J68-1</f>
         <v>2.2609060402684511E-2</v>
       </c>
       <c r="O128" s="34">
-        <f t="shared" ref="O128" si="212">O68/K68-1</f>
+        <f t="shared" ref="O128" si="213">O68/K68-1</f>
         <v>-0.15109561412504702</v>
       </c>
       <c r="P128" s="34">
-        <f t="shared" ref="P128:S128" si="213">P68/L68-1</f>
+        <f t="shared" ref="P128:S128" si="214">P68/L68-1</f>
         <v>-0.26009971874200977</v>
       </c>
       <c r="Q128" s="34">
-        <f t="shared" si="213"/>
+        <f t="shared" si="214"/>
         <v>0</v>
       </c>
       <c r="R128" s="34">
-        <f t="shared" si="213"/>
+        <f t="shared" si="214"/>
         <v>-0.18536445301283899</v>
       </c>
       <c r="S128" s="34">
-        <f t="shared" si="213"/>
+        <f t="shared" si="214"/>
         <v>-0.10490073692264323</v>
       </c>
       <c r="T128" s="34">
@@ -16666,19 +17120,19 @@
         <v>186</v>
       </c>
       <c r="Y128" s="34">
-        <f t="shared" ref="Y128" si="214">Y68/X68-1</f>
+        <f t="shared" ref="Y128" si="215">Y68/X68-1</f>
         <v>-0.13928056401217759</v>
       </c>
       <c r="Z128" s="34">
-        <f t="shared" ref="Z128" si="215">Z68/Y68-1</f>
+        <f t="shared" ref="Z128" si="216">Z68/Y68-1</f>
         <v>0.16675198957509196</v>
       </c>
       <c r="AA128" s="34">
-        <f t="shared" ref="AA128" si="216">AA68/Z68-1</f>
+        <f t="shared" ref="AA128" si="217">AA68/Z68-1</f>
         <v>-4.9062624650977216E-2</v>
       </c>
       <c r="AB128" s="34">
-        <f t="shared" ref="AB128" si="217">AB68/AA68-1</f>
+        <f t="shared" ref="AB128" si="218">AB68/AA68-1</f>
         <v>2.2609060402684511E-2</v>
       </c>
       <c r="AC128" s="34">
@@ -16694,55 +17148,55 @@
         <v>186</v>
       </c>
       <c r="D129" s="25">
-        <f t="shared" ref="D129" si="218">D68/C68-1</f>
+        <f t="shared" ref="D129" si="219">D68/C68-1</f>
         <v>2.2012578616352085E-2</v>
       </c>
       <c r="E129" s="25">
-        <f t="shared" ref="E129" si="219">E68/D68-1</f>
+        <f t="shared" ref="E129" si="220">E68/D68-1</f>
         <v>0.10090729783037489</v>
       </c>
       <c r="F129" s="25">
-        <f t="shared" ref="F129" si="220">F68/E68-1</f>
+        <f t="shared" ref="F129" si="221">F68/E68-1</f>
         <v>-0.10169127132005162</v>
       </c>
       <c r="G129" s="25">
-        <f t="shared" ref="G129" si="221">G68/F68-1</f>
+        <f t="shared" ref="G129" si="222">G68/F68-1</f>
         <v>0.19433585959313904</v>
       </c>
       <c r="H129" s="25">
-        <f t="shared" ref="H129" si="222">H68/G68-1</f>
+        <f t="shared" ref="H129" si="223">H68/G68-1</f>
         <v>3.3731881637835137E-3</v>
       </c>
       <c r="I129" s="25">
-        <f t="shared" ref="I129" si="223">I68/H68-1</f>
+        <f t="shared" ref="I129" si="224">I68/H68-1</f>
         <v>2.6095929168192145E-2</v>
       </c>
       <c r="J129" s="25">
-        <f t="shared" ref="J129" si="224">J68/I68-1</f>
+        <f t="shared" ref="J129" si="225">J68/I68-1</f>
         <v>-0.22665196094332885</v>
       </c>
       <c r="K129" s="25">
-        <f t="shared" ref="K129:P129" si="225">K68/J68-1</f>
+        <f t="shared" ref="K129:P129" si="226">K68/J68-1</f>
         <v>0.22705536912751678</v>
       </c>
       <c r="L129" s="25">
-        <f t="shared" si="225"/>
+        <f t="shared" si="226"/>
         <v>6.9565514648070259E-2</v>
       </c>
       <c r="M129" s="25">
-        <f t="shared" si="225"/>
+        <f t="shared" si="226"/>
         <v>-0.26329583226796216</v>
       </c>
       <c r="N129" s="25">
-        <f t="shared" si="225"/>
+        <f t="shared" si="226"/>
         <v>5.7657266811279806E-2</v>
       </c>
       <c r="O129" s="25">
-        <f t="shared" si="225"/>
+        <f t="shared" si="226"/>
         <v>1.862258501169034E-2</v>
       </c>
       <c r="P129" s="25">
-        <f t="shared" si="225"/>
+        <f t="shared" si="226"/>
         <v>-6.7772721781500511E-2</v>
       </c>
       <c r="Q129" s="25">
@@ -16750,11 +17204,11 @@
         <v>-4.3196544276458138E-3</v>
       </c>
       <c r="R129" s="25">
-        <f t="shared" ref="R129:S129" si="226">R68/Q68-1</f>
+        <f t="shared" ref="R129:S129" si="227">R68/Q68-1</f>
         <v>-0.13839479392624732</v>
       </c>
       <c r="S129" s="25">
-        <f t="shared" si="226"/>
+        <f t="shared" si="227"/>
         <v>0.11923464249748239</v>
       </c>
       <c r="T129" s="25">
@@ -16800,55 +17254,55 @@
         <v>186</v>
       </c>
       <c r="G131" s="25">
-        <f t="shared" ref="G131" si="227">G68/SUM(D9:G9)</f>
+        <f t="shared" ref="G131" si="228">G68/SUM(D9:G9)</f>
         <v>0.60651852452042865</v>
       </c>
       <c r="H131" s="25">
-        <f t="shared" ref="H131" si="228">H68/SUM(E9:H9)</f>
+        <f t="shared" ref="H131" si="229">H68/SUM(E9:H9)</f>
         <v>0.59386427879578574</v>
       </c>
       <c r="I131" s="25">
-        <f t="shared" ref="I131" si="229">I68/SUM(F9:I9)</f>
+        <f t="shared" ref="I131" si="230">I68/SUM(F9:I9)</f>
         <v>0.60740463430012614</v>
       </c>
       <c r="J131" s="25">
-        <f t="shared" ref="J131" si="230">J68/SUM(G9:J9)</f>
+        <f t="shared" ref="J131" si="231">J68/SUM(G9:J9)</f>
         <v>0.43642221652692853</v>
       </c>
       <c r="K131" s="25">
-        <f t="shared" ref="K131" si="231">K68/SUM(H9:K9)</f>
+        <f t="shared" ref="K131" si="232">K68/SUM(H9:K9)</f>
         <v>0.55475906013540421</v>
       </c>
       <c r="L131" s="25">
-        <f t="shared" ref="L131" si="232">L68/SUM(I9:L9)</f>
+        <f t="shared" ref="L131" si="233">L68/SUM(I9:L9)</f>
         <v>0.70602039895297419</v>
       </c>
       <c r="M131" s="25">
-        <f t="shared" ref="M131" si="233">M68/SUM(J9:M9)</f>
+        <f t="shared" ref="M131" si="234">M68/SUM(J9:M9)</f>
         <v>0.57414003537001523</v>
       </c>
       <c r="N131" s="25">
-        <f t="shared" ref="N131" si="234">N68/SUM(K9:N9)</f>
+        <f t="shared" ref="N131" si="235">N68/SUM(K9:N9)</f>
         <v>0.64646919996817898</v>
       </c>
       <c r="O131" s="25">
-        <f t="shared" ref="O131" si="235">O68/SUM(L9:O9)</f>
+        <f t="shared" ref="O131" si="236">O68/SUM(L9:O9)</f>
         <v>0.62954418698980885</v>
       </c>
       <c r="P131" s="25">
-        <f t="shared" ref="P131:S131" si="236">P68/SUM(M9:P9)</f>
+        <f t="shared" ref="P131:S131" si="237">P68/SUM(M9:P9)</f>
         <v>0.51014786575288118</v>
       </c>
       <c r="Q131" s="25">
-        <f t="shared" si="236"/>
+        <f t="shared" si="237"/>
         <v>0.48656407658370798</v>
       </c>
       <c r="R131" s="25">
-        <f t="shared" si="236"/>
+        <f t="shared" si="237"/>
         <v>0.47317259125131039</v>
       </c>
       <c r="S131" s="25">
-        <f t="shared" si="236"/>
+        <f t="shared" si="237"/>
         <v>0.55698105642978857</v>
       </c>
       <c r="T131" s="25">
@@ -16856,23 +17310,23 @@
         <v>0.61685399051350787</v>
       </c>
       <c r="X131" s="25">
-        <f t="shared" ref="X131:Y131" si="237">X68/X9</f>
+        <f t="shared" ref="X131:Y131" si="238">X68/X9</f>
         <v>0.40151186168073988</v>
       </c>
       <c r="Y131" s="25">
-        <f t="shared" si="237"/>
+        <f t="shared" si="238"/>
         <v>0.36797218844724533</v>
       </c>
       <c r="Z131" s="25">
-        <f t="shared" ref="Z131:AB131" si="238">Z68/Z9</f>
+        <f t="shared" ref="Z131:AB131" si="239">Z68/Z9</f>
         <v>0.49437005777839121</v>
       </c>
       <c r="AA131" s="25">
-        <f t="shared" si="238"/>
+        <f t="shared" si="239"/>
         <v>0.43642221652692853</v>
       </c>
       <c r="AB131" s="25">
-        <f t="shared" si="238"/>
+        <f t="shared" si="239"/>
         <v>0.64646919996817909</v>
       </c>
       <c r="AC131" s="25">
@@ -16966,95 +17420,95 @@
         <v>178</v>
       </c>
       <c r="C134" s="27">
-        <f t="shared" ref="C134:G134" si="239">C133*C27</f>
+        <f t="shared" ref="C134:G134" si="240">C133*C27</f>
         <v>19065.8</v>
       </c>
       <c r="D134" s="27">
-        <f t="shared" si="239"/>
+        <f t="shared" si="240"/>
         <v>18264.149999999998</v>
       </c>
       <c r="E134" s="27">
-        <f t="shared" si="239"/>
+        <f t="shared" si="240"/>
         <v>14375.142</v>
       </c>
       <c r="F134" s="27">
-        <f t="shared" si="239"/>
+        <f t="shared" si="240"/>
         <v>16245.633</v>
       </c>
       <c r="G134" s="27">
-        <f t="shared" si="239"/>
+        <f t="shared" si="240"/>
         <v>13985.657000000003</v>
       </c>
       <c r="H134" s="27">
-        <f t="shared" ref="H134:I134" si="240">H133*H27</f>
+        <f t="shared" ref="H134:I134" si="241">H133*H27</f>
         <v>14877.875999999998</v>
       </c>
       <c r="I134" s="27">
-        <f t="shared" si="240"/>
+        <f t="shared" si="241"/>
         <v>12692.55</v>
       </c>
       <c r="J134" s="27">
-        <f t="shared" ref="J134:K134" si="241">J133*J27</f>
+        <f t="shared" ref="J134:K134" si="242">J133*J27</f>
         <v>14342.690999999999</v>
       </c>
       <c r="K134" s="27">
-        <f t="shared" si="241"/>
+        <f t="shared" si="242"/>
         <v>5314.6419999999998</v>
       </c>
       <c r="L134" s="27">
-        <f t="shared" ref="L134" si="242">L133*L27</f>
+        <f t="shared" ref="L134" si="243">L133*L27</f>
         <v>4402.4760000000006</v>
       </c>
       <c r="M134" s="27">
-        <f t="shared" ref="M134:T134" si="243">M133*M27</f>
+        <f t="shared" ref="M134:T134" si="244">M133*M27</f>
         <v>3246.6420000000003</v>
       </c>
       <c r="N134" s="27">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>5013.5219999999999</v>
       </c>
       <c r="O134" s="27">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>7320.6</v>
       </c>
       <c r="P134" s="27">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>11124.871999999999</v>
       </c>
       <c r="Q134" s="27">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>12491.599999999999</v>
       </c>
       <c r="R134" s="27">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>10212.330000000002</v>
       </c>
       <c r="S134" s="27">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>9263.3060000000005</v>
       </c>
       <c r="T134" s="27">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>6449.7879999999996</v>
       </c>
       <c r="X134" s="27">
-        <f t="shared" ref="X134:Z134" si="244">X133*X27</f>
+        <f t="shared" ref="X134:Z134" si="245">X133*X27</f>
         <v>14160.300000000001</v>
       </c>
       <c r="Y134" s="27">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>17571.798999999999</v>
       </c>
       <c r="Z134" s="27">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>16245.633</v>
       </c>
       <c r="AA134" s="27">
-        <f t="shared" ref="AA134:AB134" si="245">AA133*AA27</f>
+        <f t="shared" ref="AA134:AB134" si="246">AA133*AA27</f>
         <v>14342.690999999999</v>
       </c>
       <c r="AB134" s="27">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>5013.5219999999999</v>
       </c>
       <c r="AC134" s="27">
@@ -17067,95 +17521,95 @@
         <v>9</v>
       </c>
       <c r="C135" s="27">
-        <f t="shared" ref="C135:G135" si="246">C134-C126</f>
+        <f t="shared" ref="C135:G135" si="247">C134-C126</f>
         <v>20189.099999999999</v>
       </c>
       <c r="D135" s="27">
-        <f t="shared" si="246"/>
+        <f t="shared" si="247"/>
         <v>19370.449999999997</v>
       </c>
       <c r="E135" s="27">
-        <f t="shared" si="246"/>
+        <f t="shared" si="247"/>
         <v>15627.342000000001</v>
       </c>
       <c r="F135" s="27">
-        <f t="shared" si="246"/>
+        <f t="shared" si="247"/>
         <v>17030.933000000001</v>
       </c>
       <c r="G135" s="27">
-        <f t="shared" si="246"/>
+        <f t="shared" si="247"/>
         <v>15428.457000000004</v>
       </c>
       <c r="H135" s="27">
-        <f t="shared" ref="H135:I135" si="247">H134-H126</f>
+        <f t="shared" ref="H135:I135" si="248">H134-H126</f>
         <v>16276.475999999999</v>
       </c>
       <c r="I135" s="27">
-        <f t="shared" si="247"/>
+        <f t="shared" si="248"/>
         <v>14326.949999999999</v>
       </c>
       <c r="J135" s="27">
-        <f t="shared" ref="J135:K135" si="248">J134-J126</f>
+        <f t="shared" ref="J135:K135" si="249">J134-J126</f>
         <v>14976.490999999998</v>
       </c>
       <c r="K135" s="27">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>6675.7420000000002</v>
       </c>
       <c r="L135" s="27">
-        <f t="shared" ref="L135" si="249">L134-L126</f>
+        <f t="shared" ref="L135" si="250">L134-L126</f>
         <v>6229.9760000000006</v>
       </c>
       <c r="M135" s="27">
-        <f t="shared" ref="M135:T135" si="250">M134-M126</f>
+        <f t="shared" ref="M135:T135" si="251">M134-M126</f>
         <v>5053.0420000000013</v>
       </c>
       <c r="N135" s="27">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>6709.1219999999994</v>
       </c>
       <c r="O135" s="27">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>9237.2000000000007</v>
       </c>
       <c r="P135" s="27">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>12944.671999999999</v>
       </c>
       <c r="Q135" s="27">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>14298</v>
       </c>
       <c r="R135" s="27">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>11607.430000000002</v>
       </c>
       <c r="S135" s="27">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>10718.106</v>
       </c>
       <c r="T135" s="27">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>7655.4879999999994</v>
       </c>
       <c r="X135" s="27">
-        <f t="shared" ref="X135:Z135" si="251">X134-X126</f>
+        <f t="shared" ref="X135:Z135" si="252">X134-X126</f>
         <v>15106.200000000003</v>
       </c>
       <c r="Y135" s="27">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>18250.699000000001</v>
       </c>
       <c r="Z135" s="27">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>17030.933000000001</v>
       </c>
       <c r="AA135" s="27">
-        <f t="shared" ref="AA135:AB135" si="252">AA134-AA126</f>
+        <f t="shared" ref="AA135:AB135" si="253">AA134-AA126</f>
         <v>14976.490999999998</v>
       </c>
       <c r="AB135" s="27">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>6709.1219999999994</v>
       </c>
       <c r="AC135" s="27">
@@ -17168,39 +17622,39 @@
         <v>26</v>
       </c>
       <c r="C137" s="57">
-        <f t="shared" ref="C137:G137" si="253">C133/C122</f>
+        <f t="shared" ref="C137:G137" si="254">C133/C122</f>
         <v>4.5569444776404806</v>
       </c>
       <c r="D137" s="57">
-        <f t="shared" si="253"/>
+        <f t="shared" si="254"/>
         <v>4.5773664820430584</v>
       </c>
       <c r="E137" s="57">
-        <f t="shared" si="253"/>
+        <f t="shared" si="254"/>
         <v>3.6212162128120506</v>
       </c>
       <c r="F137" s="57">
-        <f t="shared" si="253"/>
+        <f t="shared" si="254"/>
         <v>4.1230478148317342</v>
       </c>
       <c r="G137" s="57">
-        <f t="shared" si="253"/>
+        <f t="shared" si="254"/>
         <v>3.5936217174572174</v>
       </c>
       <c r="H137" s="57">
-        <f t="shared" ref="H137:I137" si="254">H133/H122</f>
+        <f t="shared" ref="H137:I137" si="255">H133/H122</f>
         <v>3.8049860617375519</v>
       </c>
       <c r="I137" s="57">
-        <f t="shared" si="254"/>
+        <f t="shared" si="255"/>
         <v>3.3381242931909623</v>
       </c>
       <c r="J137" s="57">
-        <f t="shared" ref="J137:K137" si="255">J133/J122</f>
+        <f t="shared" ref="J137:K137" si="256">J133/J122</f>
         <v>3.9679884357881914</v>
       </c>
       <c r="K137" s="57">
-        <f t="shared" si="255"/>
+        <f t="shared" si="256"/>
         <v>1.6181469979296066</v>
       </c>
       <c r="L137" s="57">
@@ -17216,7 +17670,7 @@
         <v>1.7243411865864144</v>
       </c>
       <c r="O137" s="57">
-        <f t="shared" ref="O137" si="256">O133/O122</f>
+        <f t="shared" ref="O137" si="257">O133/O122</f>
         <v>2.6197394789579156</v>
       </c>
       <c r="P137" s="57">
@@ -17240,19 +17694,19 @@
         <v>2.2452006822849584</v>
       </c>
       <c r="X137" s="57">
-        <f t="shared" ref="X137:Z137" si="257">X133/X122</f>
+        <f t="shared" ref="X137:Y137" si="258">X133/X122</f>
         <v>3.6006560378366026</v>
       </c>
       <c r="Y137" s="57">
-        <f t="shared" si="257"/>
+        <f t="shared" si="258"/>
         <v>4.2113358897543431</v>
       </c>
       <c r="Z137" s="57">
-        <f t="shared" ref="Z137:AA137" si="258">Z133/Z122</f>
+        <f t="shared" ref="Z137:AA137" si="259">Z133/Z122</f>
         <v>4.1230478148317342</v>
       </c>
       <c r="AA137" s="57">
-        <f t="shared" si="258"/>
+        <f t="shared" si="259"/>
         <v>3.9679884357881914</v>
       </c>
       <c r="AB137" s="57">
@@ -17284,51 +17738,51 @@
         <v>186</v>
       </c>
       <c r="H138" s="74">
-        <f t="shared" ref="H138" si="259">H133/SUM(E9:H9)</f>
+        <f t="shared" ref="H138" si="260">H133/SUM(E9:H9)</f>
         <v>3.9969163256834486E-3</v>
       </c>
       <c r="I138" s="74">
-        <f t="shared" ref="I138" si="260">I133/SUM(F9:I9)</f>
+        <f t="shared" ref="I138" si="261">I133/SUM(F9:I9)</f>
         <v>3.3988808322824725E-3</v>
       </c>
       <c r="J138" s="74">
-        <f t="shared" ref="J138" si="261">J133/SUM(G9:J9)</f>
+        <f t="shared" ref="J138" si="262">J133/SUM(G9:J9)</f>
         <v>3.5678980705158708E-3</v>
       </c>
       <c r="K138" s="74">
-        <f t="shared" ref="K138" si="262">K133/SUM(H9:K9)</f>
+        <f t="shared" ref="K138" si="263">K133/SUM(H9:K9)</f>
         <v>1.3692135555934837E-3</v>
       </c>
       <c r="L138" s="74">
-        <f t="shared" ref="L138" si="263">L133/SUM(I9:L9)</f>
+        <f t="shared" ref="L138" si="264">L133/SUM(I9:L9)</f>
         <v>1.3493997653217802E-3</v>
       </c>
       <c r="M138" s="74">
-        <f t="shared" ref="M138" si="264">M133/SUM(J9:M9)</f>
+        <f t="shared" ref="M138" si="265">M133/SUM(J9:M9)</f>
         <v>1.0984631479313523E-3</v>
       </c>
       <c r="N138" s="74">
-        <f t="shared" ref="N138" si="265">N133/SUM(K9:N9)</f>
+        <f t="shared" ref="N138" si="266">N133/SUM(K9:N9)</f>
         <v>1.8058391450770329E-3</v>
       </c>
       <c r="O138" s="74">
-        <f t="shared" ref="O138" si="266">O133/SUM(L9:O9)</f>
+        <f t="shared" ref="O138" si="267">O133/SUM(L9:O9)</f>
         <v>2.5249708462201492E-3</v>
       </c>
       <c r="P138" s="74">
-        <f t="shared" ref="P138:S138" si="267">P133/SUM(M9:P9)</f>
+        <f t="shared" ref="P138:S138" si="268">P133/SUM(M9:P9)</f>
         <v>3.3363450053989726E-3</v>
       </c>
       <c r="Q138" s="74">
-        <f t="shared" si="267"/>
+        <f t="shared" si="268"/>
         <v>3.5885419964958943E-3</v>
       </c>
       <c r="R138" s="74">
-        <f t="shared" si="267"/>
+        <f t="shared" si="268"/>
         <v>3.3117316306108839E-3</v>
       </c>
       <c r="S138" s="74">
-        <f t="shared" si="267"/>
+        <f t="shared" si="268"/>
         <v>3.1597674651698908E-3</v>
       </c>
       <c r="T138" s="74">
@@ -17336,23 +17790,23 @@
         <v>2.2633532687151986E-3</v>
       </c>
       <c r="X138" s="57">
-        <f t="shared" ref="X138:Z138" si="268">X134/X9</f>
+        <f t="shared" ref="X138:Z138" si="269">X134/X9</f>
         <v>2.2774909529553682</v>
       </c>
       <c r="Y138" s="57">
-        <f t="shared" si="268"/>
+        <f t="shared" si="269"/>
         <v>3.0092303872039454</v>
       </c>
       <c r="Z138" s="57">
-        <f t="shared" si="268"/>
+        <f t="shared" si="269"/>
         <v>3.2035718088777578</v>
       </c>
       <c r="AA138" s="57">
-        <f t="shared" ref="AA138:AB138" si="269">AA134/AA9</f>
+        <f t="shared" ref="AA138:AB138" si="270">AA134/AA9</f>
         <v>2.6256161900926296</v>
       </c>
       <c r="AB138" s="57">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>1.3294587786057119</v>
       </c>
       <c r="AC138" s="57">
@@ -17380,51 +17834,51 @@
         <v>186</v>
       </c>
       <c r="H139" s="57">
-        <f t="shared" ref="H139" si="270">H133/SUM(E26:H26)</f>
+        <f t="shared" ref="H139" si="271">H133/SUM(E26:H26)</f>
         <v>-328.9104111728746</v>
       </c>
       <c r="I139" s="57">
-        <f t="shared" ref="I139" si="271">I133/SUM(F26:I26)</f>
+        <f t="shared" ref="I139" si="272">I133/SUM(F26:I26)</f>
         <v>-115.49206732790152</v>
       </c>
       <c r="J139" s="57">
-        <f t="shared" ref="J139" si="272">J133/SUM(G26:J26)</f>
+        <f t="shared" ref="J139" si="273">J133/SUM(G26:J26)</f>
         <v>-44.49814940755099</v>
       </c>
       <c r="K139" s="57">
-        <f t="shared" ref="K139" si="273">K133/SUM(H26:K26)</f>
+        <f t="shared" ref="K139" si="274">K133/SUM(H26:K26)</f>
         <v>-9.2931914725575346</v>
       </c>
       <c r="L139" s="57">
-        <f t="shared" ref="L139" si="274">L133/SUM(I26:L26)</f>
+        <f t="shared" ref="L139" si="275">L133/SUM(I26:L26)</f>
         <v>-4.921897835209367</v>
       </c>
       <c r="M139" s="57">
-        <f t="shared" ref="M139" si="275">M133/SUM(J26:M26)</f>
+        <f t="shared" ref="M139" si="276">M133/SUM(J26:M26)</f>
         <v>-3.4596705334508839</v>
       </c>
       <c r="N139" s="57">
-        <f t="shared" ref="N139" si="276">N133/SUM(K26:N26)</f>
+        <f t="shared" ref="N139" si="277">N133/SUM(K26:N26)</f>
         <v>-6.8505742659676452</v>
       </c>
       <c r="O139" s="57">
-        <f t="shared" ref="O139" si="277">O133/SUM(L26:O26)</f>
+        <f t="shared" ref="O139" si="278">O133/SUM(L26:O26)</f>
         <v>-13.844238952468716</v>
       </c>
       <c r="P139" s="57">
-        <f t="shared" ref="P139:S139" si="278">P133/SUM(M26:P26)</f>
+        <f t="shared" ref="P139:S139" si="279">P133/SUM(M26:P26)</f>
         <v>-88.265429889576552</v>
       </c>
       <c r="Q139" s="57">
-        <f t="shared" si="278"/>
+        <f t="shared" si="279"/>
         <v>-249.48613055071797</v>
       </c>
       <c r="R139" s="57">
-        <f t="shared" si="278"/>
+        <f t="shared" si="279"/>
         <v>-228.62115367889854</v>
       </c>
       <c r="S139" s="57">
-        <f t="shared" si="278"/>
+        <f t="shared" si="279"/>
         <v>697.1161832155442</v>
       </c>
       <c r="T139" s="57">
@@ -17432,19 +17886,19 @@
         <v>-16621.554193892349</v>
       </c>
       <c r="X139" s="57">
-        <f t="shared" ref="X139:Z139" si="279">X133/X26</f>
+        <f t="shared" ref="X139:Y139" si="280">X133/X26</f>
         <v>85.25165562913908</v>
       </c>
       <c r="Y139" s="57">
-        <f t="shared" si="279"/>
+        <f t="shared" si="280"/>
         <v>71.19853727714748</v>
       </c>
       <c r="Z139" s="57">
-        <f t="shared" ref="Z139:AA139" si="280">Z133/Z26</f>
+        <f t="shared" ref="Z139:AA139" si="281">Z133/Z26</f>
         <v>-91.165168350168358</v>
       </c>
       <c r="AA139" s="57">
-        <f t="shared" si="280"/>
+        <f t="shared" si="281"/>
         <v>-44.501058020477807</v>
       </c>
       <c r="AB139" s="57">
@@ -17464,67 +17918,67 @@
         <v>186</v>
       </c>
       <c r="D141" s="25">
-        <f t="shared" ref="D141:S141" si="281">D15:D15/D9</f>
+        <f t="shared" ref="D141:S141" si="282">D15:D15/D9</f>
         <v>8.0382013529645847E-3</v>
       </c>
       <c r="E141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>7.5045285948417148E-3</v>
       </c>
       <c r="F141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>1.0308671065032988E-2</v>
       </c>
       <c r="G141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>1.1296003886797037E-2</v>
       </c>
       <c r="H141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>8.5587872633640389E-3</v>
       </c>
       <c r="I141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>9.8673018033344686E-3</v>
       </c>
       <c r="J141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>8.057553956834532E-3</v>
       </c>
       <c r="K141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>9.1511517828968131E-3</v>
       </c>
       <c r="L141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>1.1913626209977662E-2</v>
       </c>
       <c r="M141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>9.3581125609595358E-3</v>
       </c>
       <c r="N141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>5.7021831215379598E-3</v>
       </c>
       <c r="O141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>1.0405053883314754E-2</v>
       </c>
       <c r="P141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>8.2264484741264941E-3</v>
       </c>
       <c r="Q141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>1.0750443586264482E-2</v>
       </c>
       <c r="R141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>1.1526934603857682E-2</v>
       </c>
       <c r="S141" s="25">
-        <f t="shared" si="281"/>
+        <f t="shared" si="282"/>
         <v>2.8956565152271591E-2</v>
       </c>
       <c r="T141" s="25">
@@ -17532,27 +17986,27 @@
         <v>2.4438119540681126E-2</v>
       </c>
       <c r="X141" s="25">
-        <f t="shared" ref="X141:Z141" si="282">X15:X15/X9</f>
+        <f t="shared" ref="X141:Z141" si="283">X15:X15/X9</f>
         <v>7.6558102131081629E-3</v>
       </c>
       <c r="Y141" s="25">
-        <f t="shared" si="282"/>
+        <f t="shared" si="283"/>
         <v>8.4256674601407705E-3</v>
       </c>
       <c r="Z141" s="25">
-        <f t="shared" si="282"/>
+        <f t="shared" si="283"/>
         <v>9.0907298219321253E-3</v>
       </c>
       <c r="AA141" s="25">
-        <f t="shared" ref="AA141:AC141" si="283">AA15:AA15/AA9</f>
+        <f t="shared" ref="AA141:AC141" si="284">AA15:AA15/AA9</f>
         <v>9.043312708234174E-3</v>
       </c>
       <c r="AB141" s="25">
-        <f t="shared" si="283"/>
+        <f t="shared" si="284"/>
         <v>7.9022036010713056E-3</v>
       </c>
       <c r="AC141" s="25">
-        <f t="shared" si="283"/>
+        <f t="shared" si="284"/>
         <v>1.0244925188220719E-2</v>
       </c>
     </row>
@@ -17591,8 +18045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -17613,7 +18067,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add order, backlog data for QX18,19 $ERJ
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BD20DC-C224-E749-9831-81B7CB188F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1A5337-6A71-49DC-8DA1-62DB1006BDFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="3" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -132,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="253">
   <si>
     <t>$ERJ</t>
   </si>
@@ -931,6 +921,9 @@
   <si>
     <t>growth, product development &amp; new business</t>
   </si>
+  <si>
+    <t>(Projected)</t>
+  </si>
 </sst>
 </file>
 
@@ -943,7 +936,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.0000\x"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1070,22 +1063,33 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i/>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1113,6 +1117,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF323232"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1374,9 +1384,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1396,6 +1404,28 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,28 +1435,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1447,27 +1459,51 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="3" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1496,7 +1532,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1974,7 +2010,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6225,13 +6261,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y39" sqref="Y39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="3"/>
+    <col min="1" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:29" ht="15">
@@ -6246,31 +6282,31 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="95"/>
-      <c r="G5" s="93" t="s">
+      <c r="C5" s="100"/>
+      <c r="D5" s="101"/>
+      <c r="G5" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
-      <c r="M5" s="94"/>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="94"/>
-      <c r="R5" s="95"/>
-      <c r="T5" s="93" t="s">
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="100"/>
+      <c r="P5" s="100"/>
+      <c r="Q5" s="100"/>
+      <c r="R5" s="101"/>
+      <c r="T5" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="94"/>
-      <c r="V5" s="94"/>
-      <c r="W5" s="95"/>
+      <c r="U5" s="100"/>
+      <c r="V5" s="100"/>
+      <c r="W5" s="101"/>
       <c r="AA5" s="104" t="s">
         <v>205</v>
       </c>
@@ -6505,13 +6541,13 @@
       <c r="U12" s="37"/>
       <c r="V12" s="37"/>
       <c r="W12" s="38"/>
-      <c r="Y12" s="93" t="s">
+      <c r="Y12" s="99" t="s">
         <v>219</v>
       </c>
-      <c r="Z12" s="94"/>
-      <c r="AA12" s="94"/>
-      <c r="AB12" s="94"/>
-      <c r="AC12" s="95"/>
+      <c r="Z12" s="100"/>
+      <c r="AA12" s="100"/>
+      <c r="AB12" s="100"/>
+      <c r="AC12" s="101"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="10"/>
@@ -6532,15 +6568,15 @@
       <c r="U13" s="37"/>
       <c r="V13" s="37"/>
       <c r="W13" s="38"/>
-      <c r="Y13" s="111"/>
-      <c r="Z13" s="112" t="s">
+      <c r="Y13" s="92"/>
+      <c r="Z13" s="102" t="s">
         <v>220</v>
       </c>
-      <c r="AA13" s="112"/>
-      <c r="AB13" s="112" t="s">
+      <c r="AA13" s="102"/>
+      <c r="AB13" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="AC13" s="113"/>
+      <c r="AC13" s="103"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="9">
@@ -6568,21 +6604,21 @@
       <c r="Y14" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="Z14" s="98" t="s">
+      <c r="Z14" s="97" t="s">
         <v>231</v>
       </c>
-      <c r="AA14" s="98"/>
-      <c r="AB14" s="98" t="s">
+      <c r="AA14" s="97"/>
+      <c r="AB14" s="97" t="s">
         <v>232</v>
       </c>
-      <c r="AC14" s="99"/>
+      <c r="AC14" s="98"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="95"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="101"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -6604,14 +6640,14 @@
       <c r="Y15" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="Z15" s="98" t="s">
+      <c r="Z15" s="97" t="s">
         <v>227</v>
       </c>
-      <c r="AA15" s="98"/>
-      <c r="AB15" s="98" t="s">
+      <c r="AA15" s="97"/>
+      <c r="AB15" s="97" t="s">
         <v>233</v>
       </c>
-      <c r="AC15" s="99"/>
+      <c r="AC15" s="98"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="14" t="s">
@@ -6620,10 +6656,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="99"/>
+      <c r="D16" s="98"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -6645,23 +6681,23 @@
       <c r="Y16" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="Z16" s="98" t="s">
+      <c r="Z16" s="97" t="s">
         <v>228</v>
       </c>
-      <c r="AA16" s="98"/>
-      <c r="AB16" s="98" t="s">
+      <c r="AA16" s="97"/>
+      <c r="AB16" s="97" t="s">
         <v>234</v>
       </c>
-      <c r="AC16" s="99"/>
+      <c r="AC16" s="98"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="98" t="s">
+      <c r="C17" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="99"/>
+      <c r="D17" s="98"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
@@ -6685,19 +6721,19 @@
       <c r="Y17" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="Z17" s="98" t="s">
+      <c r="Z17" s="97" t="s">
         <v>229</v>
       </c>
-      <c r="AA17" s="98"/>
-      <c r="AB17" s="98" t="s">
+      <c r="AA17" s="97"/>
+      <c r="AB17" s="97" t="s">
         <v>235</v>
       </c>
-      <c r="AC17" s="99"/>
+      <c r="AC17" s="98"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="16"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="98"/>
       <c r="G18" s="10"/>
       <c r="H18" s="8" t="s">
         <v>192</v>
@@ -6721,14 +6757,14 @@
       <c r="Y18" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="Z18" s="98" t="s">
+      <c r="Z18" s="97" t="s">
         <v>230</v>
       </c>
-      <c r="AA18" s="98"/>
-      <c r="AB18" s="98" t="s">
+      <c r="AA18" s="97"/>
+      <c r="AB18" s="97" t="s">
         <v>236</v>
       </c>
-      <c r="AC18" s="99"/>
+      <c r="AC18" s="98"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="17"/>
@@ -6757,14 +6793,14 @@
       <c r="Y19" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="Z19" s="98" t="s">
+      <c r="Z19" s="97" t="s">
         <v>238</v>
       </c>
-      <c r="AA19" s="98"/>
-      <c r="AB19" s="98" t="s">
+      <c r="AA19" s="97"/>
+      <c r="AB19" s="97" t="s">
         <v>239</v>
       </c>
-      <c r="AC19" s="99"/>
+      <c r="AC19" s="98"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="10"/>
@@ -6792,14 +6828,14 @@
       <c r="Y20" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="Z20" s="98" t="s">
+      <c r="Z20" s="97" t="s">
         <v>244</v>
       </c>
-      <c r="AA20" s="98"/>
-      <c r="AB20" s="98" t="s">
+      <c r="AA20" s="97"/>
+      <c r="AB20" s="97" t="s">
         <v>245</v>
       </c>
-      <c r="AC20" s="99"/>
+      <c r="AC20" s="98"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="10"/>
@@ -6827,11 +6863,11 @@
       <c r="AC21" s="38"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="95"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="101"/>
       <c r="G22" s="10"/>
       <c r="H22" s="60"/>
       <c r="I22" s="60"/>
@@ -6860,10 +6896,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C23" s="97" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="99"/>
+      <c r="D23" s="98"/>
       <c r="G23" s="9">
         <v>44743</v>
       </c>
@@ -6889,10 +6925,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="98">
+      <c r="C24" s="97">
         <v>1969</v>
       </c>
-      <c r="D24" s="99"/>
+      <c r="D24" s="98"/>
       <c r="G24" s="10"/>
       <c r="H24" s="8" t="s">
         <v>197</v>
@@ -6916,8 +6952,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="10"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="99"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="98"/>
       <c r="G25" s="10"/>
       <c r="H25" s="50" t="s">
         <v>198</v>
@@ -6969,8 +7005,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="10"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="99"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="98"/>
       <c r="G27" s="9">
         <v>44743</v>
       </c>
@@ -7029,10 +7065,10 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="100" t="s">
+      <c r="C29" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="101"/>
+      <c r="D29" s="113"/>
       <c r="G29" s="10"/>
       <c r="H29" s="60"/>
       <c r="I29" s="60"/>
@@ -7097,11 +7133,11 @@
       <c r="W31" s="38"/>
     </row>
     <row r="32" spans="2:29">
-      <c r="B32" s="93" t="s">
+      <c r="B32" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="94"/>
-      <c r="D32" s="95"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="101"/>
       <c r="G32" s="10"/>
       <c r="H32" s="60"/>
       <c r="I32" s="60"/>
@@ -7125,11 +7161,11 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="102">
+      <c r="C33" s="114">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="103"/>
+      <c r="D33" s="115"/>
       <c r="G33" s="9">
         <v>43922</v>
       </c>
@@ -7155,11 +7191,11 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="102">
+      <c r="C34" s="114">
         <f>C6/'Financial Model'!AC9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="103"/>
+      <c r="D34" s="115"/>
       <c r="G34" s="10"/>
       <c r="H34" s="8" t="s">
         <v>169</v>
@@ -7183,11 +7219,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="96">
+      <c r="C35" s="110">
         <f>C6/'Financial Model'!AC26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="97"/>
+      <c r="D35" s="111"/>
       <c r="G35" s="10"/>
       <c r="H35" s="37"/>
       <c r="I35" s="37"/>
@@ -7234,19 +7270,19 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="T37" s="93" t="s">
+      <c r="T37" s="99" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="94"/>
-      <c r="V37" s="94"/>
-      <c r="W37" s="95"/>
+      <c r="U37" s="100"/>
+      <c r="V37" s="100"/>
+      <c r="W37" s="101"/>
     </row>
     <row r="38" spans="2:23">
-      <c r="B38" s="93" t="s">
+      <c r="B38" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C38" s="94"/>
-      <c r="D38" s="95"/>
+      <c r="C38" s="100"/>
+      <c r="D38" s="101"/>
       <c r="G38" s="10"/>
       <c r="H38" s="50" t="s">
         <v>168</v>
@@ -7269,10 +7305,10 @@
       <c r="W38" s="38"/>
     </row>
     <row r="39" spans="2:23">
-      <c r="B39" s="114" t="s">
+      <c r="B39" s="93" t="s">
         <v>248</v>
       </c>
-      <c r="C39" s="115"/>
+      <c r="C39" s="94"/>
       <c r="D39" s="51" t="s">
         <v>31</v>
       </c>
@@ -7296,10 +7332,10 @@
       <c r="W39" s="38"/>
     </row>
     <row r="40" spans="2:23">
-      <c r="B40" s="114" t="s">
+      <c r="B40" s="93" t="s">
         <v>249</v>
       </c>
-      <c r="C40" s="115"/>
+      <c r="C40" s="94"/>
       <c r="D40" s="51" t="s">
         <v>31</v>
       </c>
@@ -7329,9 +7365,9 @@
       <c r="W40" s="38"/>
     </row>
     <row r="41" spans="2:23">
-      <c r="B41" s="114"/>
-      <c r="C41" s="115"/>
-      <c r="D41" s="91" t="s">
+      <c r="B41" s="93"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="89" t="s">
         <v>31</v>
       </c>
       <c r="G41" s="10"/>
@@ -7352,9 +7388,9 @@
       <c r="W41" s="38"/>
     </row>
     <row r="42" spans="2:23">
-      <c r="B42" s="114"/>
-      <c r="C42" s="115"/>
-      <c r="D42" s="91" t="s">
+      <c r="B42" s="93"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="89" t="s">
         <v>31</v>
       </c>
       <c r="G42" s="10"/>
@@ -7377,9 +7413,9 @@
       <c r="W42" s="38"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="116"/>
-      <c r="C43" s="117"/>
-      <c r="D43" s="92" t="s">
+      <c r="B43" s="95"/>
+      <c r="C43" s="96"/>
+      <c r="D43" s="90" t="s">
         <v>31</v>
       </c>
       <c r="G43" s="10"/>
@@ -7546,7 +7582,7 @@
       <c r="R52" s="38"/>
     </row>
     <row r="53" spans="7:18">
-      <c r="G53" s="110">
+      <c r="G53" s="91">
         <v>42552</v>
       </c>
       <c r="H53" s="54" t="s">
@@ -7565,29 +7601,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="C26:D26"/>
@@ -7602,6 +7615,24 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="B38:D38"/>
     <mergeCell ref="T37:W37"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C27:D27"/>
@@ -7609,6 +7640,11 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -7642,16 +7678,16 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
+      <selection pane="bottomRight" activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="19" width="9.1640625" style="3"/>
-    <col min="20" max="20" width="9.1640625" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="9.1640625" style="3"/>
+    <col min="2" max="2" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="9.140625" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:39" s="15" customFormat="1">
@@ -18046,12 +18082,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+      <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="72"/>
+    <col min="1" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18061,135 +18097,146 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258CA0E5-563F-4C1F-B583-AD76D8E7BBD2}">
-  <dimension ref="A2:AG49"/>
+  <dimension ref="A1:AG49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41:B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="3"/>
+    <col min="1" max="1" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="9.140625" style="123"/>
+    <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" s="2" customFormat="1" ht="13">
-      <c r="B2" s="15" t="s">
+    <row r="1" spans="1:33" s="2" customFormat="1">
+      <c r="B1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="O1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="S1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T1" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="X2" s="80">
+      <c r="X1" s="80">
         <v>2016</v>
       </c>
-      <c r="Y2" s="80">
+      <c r="Y1" s="80">
         <v>2017</v>
       </c>
-      <c r="Z2" s="80">
+      <c r="Z1" s="80">
         <v>2018</v>
       </c>
-      <c r="AA2" s="80">
-        <f>Z2+1</f>
+      <c r="AA1" s="80">
+        <f>Z1+1</f>
         <v>2019</v>
       </c>
-      <c r="AB2" s="80">
-        <f t="shared" ref="AB2:AG2" si="0">AA2+1</f>
+      <c r="AB1" s="80">
+        <f t="shared" ref="AB1:AG1" si="0">AA1+1</f>
         <v>2020</v>
       </c>
-      <c r="AC2" s="80">
+      <c r="AC1" s="80">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD1" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE1" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AF1" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AG1" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="77" customFormat="1" ht="13">
+    <row r="2" spans="1:33" s="126" customFormat="1">
+      <c r="A2" s="124"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="T2" s="127" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" s="77" customFormat="1">
       <c r="A3" s="77" t="s">
         <v>210</v>
       </c>
       <c r="B3" s="77">
         <f t="shared" ref="B3" si="1">SUM(B4:B10)</f>
-        <v>0</v>
+        <v>1835</v>
       </c>
       <c r="C3" s="77">
         <f t="shared" ref="C3" si="2">SUM(C4:C10)</f>
-        <v>0</v>
+        <v>1802</v>
       </c>
       <c r="D3" s="77">
         <f t="shared" ref="D3" si="3">SUM(D4:D10)</f>
-        <v>0</v>
+        <v>1708</v>
       </c>
       <c r="E3" s="77">
         <f t="shared" ref="E3" si="4">SUM(E4:E10)</f>
@@ -18197,15 +18244,15 @@
       </c>
       <c r="F3" s="77">
         <f t="shared" ref="F3" si="5">SUM(F4:F10)</f>
-        <v>0</v>
+        <v>1860</v>
       </c>
       <c r="G3" s="77">
         <f t="shared" ref="G3" si="6">SUM(G4:G10)</f>
-        <v>0</v>
+        <v>1890</v>
       </c>
       <c r="H3" s="77">
         <f t="shared" ref="H3" si="7">SUM(H4:H10)</f>
-        <v>0</v>
+        <v>1889</v>
       </c>
       <c r="I3" s="77">
         <f t="shared" ref="I3" si="8">SUM(I4:I10)</f>
@@ -18213,15 +18260,15 @@
       </c>
       <c r="J3" s="77">
         <f t="shared" ref="J3" si="9">SUM(J4:J10)</f>
-        <v>0</v>
+        <v>1902</v>
       </c>
       <c r="K3" s="77">
         <f t="shared" ref="K3" si="10">SUM(K4:K10)</f>
-        <v>0</v>
+        <v>1902</v>
       </c>
       <c r="L3" s="77">
         <f t="shared" ref="L3" si="11">SUM(L4:L10)</f>
-        <v>0</v>
+        <v>1902</v>
       </c>
       <c r="M3" s="77">
         <f t="shared" ref="M3:Q3" si="12">SUM(M4:M10)</f>
@@ -18251,6 +18298,7 @@
         <f t="shared" ref="S3" si="14">SUM(S4:S10)</f>
         <v>2000</v>
       </c>
+      <c r="T3" s="120"/>
       <c r="X3" s="77">
         <f t="shared" ref="X3:Z3" si="15">SUM(X4:X10)</f>
         <v>1749</v>
@@ -18276,16 +18324,43 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="4" spans="1:33" s="78" customFormat="1">
       <c r="A4" s="79" t="s">
         <v>201</v>
       </c>
+      <c r="B4" s="78">
+        <v>191</v>
+      </c>
+      <c r="C4" s="78">
+        <v>191</v>
+      </c>
+      <c r="D4" s="78">
+        <v>191</v>
+      </c>
       <c r="E4" s="78">
         <v>191</v>
       </c>
+      <c r="F4" s="78">
+        <v>191</v>
+      </c>
+      <c r="G4" s="78">
+        <v>191</v>
+      </c>
+      <c r="H4" s="78">
+        <v>191</v>
+      </c>
       <c r="I4" s="78">
         <v>191</v>
       </c>
+      <c r="J4" s="78">
+        <v>191</v>
+      </c>
+      <c r="K4" s="78">
+        <v>191</v>
+      </c>
+      <c r="L4" s="78">
+        <v>191</v>
+      </c>
       <c r="M4" s="78">
         <v>191</v>
       </c>
@@ -18307,6 +18382,7 @@
       <c r="S4" s="78">
         <v>191</v>
       </c>
+      <c r="T4" s="121"/>
       <c r="X4" s="78">
         <v>193</v>
       </c>
@@ -18326,16 +18402,43 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="5" spans="1:33" s="78" customFormat="1">
       <c r="A5" s="79" t="s">
         <v>85</v>
       </c>
+      <c r="B5" s="78">
+        <v>603</v>
+      </c>
+      <c r="C5" s="78">
+        <v>622</v>
+      </c>
+      <c r="D5" s="78">
+        <v>647</v>
+      </c>
       <c r="E5" s="78">
         <v>771</v>
       </c>
+      <c r="F5" s="78">
+        <v>773</v>
+      </c>
+      <c r="G5" s="78">
+        <v>793</v>
+      </c>
+      <c r="H5" s="78">
+        <v>793</v>
+      </c>
       <c r="I5" s="78">
         <v>815</v>
       </c>
+      <c r="J5" s="78">
+        <v>800</v>
+      </c>
+      <c r="K5" s="78">
+        <v>798</v>
+      </c>
+      <c r="L5" s="78">
+        <v>798</v>
+      </c>
       <c r="M5" s="78">
         <v>798</v>
       </c>
@@ -18357,6 +18460,7 @@
       <c r="S5" s="78">
         <v>848</v>
       </c>
+      <c r="T5" s="121"/>
       <c r="X5" s="78">
         <v>525</v>
       </c>
@@ -18376,16 +18480,43 @@
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="6" spans="1:33" s="78" customFormat="1">
       <c r="A6" s="79" t="s">
         <v>185</v>
       </c>
+      <c r="B6" s="78">
+        <v>592</v>
+      </c>
+      <c r="C6" s="78">
+        <v>587</v>
+      </c>
+      <c r="D6" s="78">
+        <v>563</v>
+      </c>
       <c r="E6" s="78">
         <v>566</v>
       </c>
+      <c r="F6" s="78">
+        <v>566</v>
+      </c>
+      <c r="G6" s="78">
+        <v>566</v>
+      </c>
+      <c r="H6" s="78">
+        <v>565</v>
+      </c>
       <c r="I6" s="78">
         <v>568</v>
       </c>
+      <c r="J6" s="78">
+        <v>568</v>
+      </c>
+      <c r="K6" s="78">
+        <v>568</v>
+      </c>
+      <c r="L6" s="78">
+        <v>568</v>
+      </c>
       <c r="M6" s="78">
         <v>568</v>
       </c>
@@ -18407,6 +18538,7 @@
       <c r="S6" s="78">
         <v>568</v>
       </c>
+      <c r="T6" s="121"/>
       <c r="X6" s="78">
         <v>590</v>
       </c>
@@ -18426,16 +18558,43 @@
         <v>568</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="7" spans="1:33" s="78" customFormat="1">
       <c r="A7" s="79" t="s">
         <v>188</v>
       </c>
+      <c r="B7" s="78">
+        <v>169</v>
+      </c>
+      <c r="C7" s="78">
+        <v>172</v>
+      </c>
+      <c r="D7" s="78">
+        <v>172</v>
+      </c>
       <c r="E7" s="78">
         <v>172</v>
       </c>
+      <c r="F7" s="78">
+        <v>172</v>
+      </c>
+      <c r="G7" s="78">
+        <v>172</v>
+      </c>
+      <c r="H7" s="78">
+        <v>172</v>
+      </c>
       <c r="I7" s="78">
         <v>172</v>
       </c>
+      <c r="J7" s="78">
+        <v>172</v>
+      </c>
+      <c r="K7" s="78">
+        <v>172</v>
+      </c>
+      <c r="L7" s="78">
+        <v>172</v>
+      </c>
       <c r="M7" s="78">
         <v>172</v>
       </c>
@@ -18457,6 +18616,7 @@
       <c r="S7" s="78">
         <v>172</v>
       </c>
+      <c r="T7" s="121"/>
       <c r="X7" s="78">
         <v>166</v>
       </c>
@@ -18476,10 +18636,19 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="8" spans="1:33" s="78" customFormat="1">
       <c r="A8" s="79" t="s">
         <v>217</v>
       </c>
+      <c r="B8" s="78">
+        <v>100</v>
+      </c>
+      <c r="C8" s="78">
+        <v>100</v>
+      </c>
+      <c r="D8" s="78">
+        <v>0</v>
+      </c>
       <c r="E8" s="78">
         <v>0</v>
       </c>
@@ -18525,6 +18694,7 @@
       <c r="S8" s="78">
         <v>0</v>
       </c>
+      <c r="T8" s="121"/>
       <c r="X8" s="78">
         <v>100</v>
       </c>
@@ -18544,16 +18714,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="9" spans="1:33" s="78" customFormat="1">
       <c r="A9" s="79" t="s">
         <v>180</v>
       </c>
+      <c r="B9" s="78">
+        <v>74</v>
+      </c>
+      <c r="C9" s="78">
+        <v>50</v>
+      </c>
+      <c r="D9" s="78">
+        <v>62</v>
+      </c>
       <c r="E9" s="78">
         <v>47</v>
       </c>
+      <c r="F9" s="78">
+        <v>46</v>
+      </c>
+      <c r="G9" s="78">
+        <v>44</v>
+      </c>
+      <c r="H9" s="78">
+        <v>44</v>
+      </c>
       <c r="I9" s="78">
         <v>27</v>
       </c>
+      <c r="J9" s="78">
+        <v>27</v>
+      </c>
+      <c r="K9" s="78">
+        <v>25</v>
+      </c>
+      <c r="L9" s="78">
+        <v>22</v>
+      </c>
       <c r="M9" s="78">
         <v>22</v>
       </c>
@@ -18575,6 +18772,7 @@
       <c r="S9" s="78">
         <v>20</v>
       </c>
+      <c r="T9" s="121"/>
       <c r="X9" s="78">
         <v>85</v>
       </c>
@@ -18594,16 +18792,43 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="10" spans="1:33" s="78" customFormat="1">
       <c r="A10" s="79" t="s">
         <v>86</v>
       </c>
+      <c r="B10" s="78">
+        <v>106</v>
+      </c>
+      <c r="C10" s="78">
+        <v>80</v>
+      </c>
+      <c r="D10" s="78">
+        <v>73</v>
+      </c>
       <c r="E10" s="78">
         <v>111</v>
       </c>
+      <c r="F10" s="78">
+        <v>112</v>
+      </c>
+      <c r="G10" s="78">
+        <v>124</v>
+      </c>
+      <c r="H10" s="78">
+        <v>124</v>
+      </c>
       <c r="I10" s="78">
         <v>144</v>
       </c>
+      <c r="J10" s="78">
+        <v>144</v>
+      </c>
+      <c r="K10" s="78">
+        <v>148</v>
+      </c>
+      <c r="L10" s="78">
+        <v>151</v>
+      </c>
       <c r="M10" s="78">
         <v>153</v>
       </c>
@@ -18625,6 +18850,10 @@
       <c r="S10" s="78">
         <v>201</v>
       </c>
+      <c r="T10" s="121">
+        <f>S10+6</f>
+        <v>207</v>
+      </c>
       <c r="X10" s="78">
         <v>90</v>
       </c>
@@ -18644,22 +18873,24 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="78" customFormat="1" ht="13"/>
-    <row r="12" spans="1:33" s="77" customFormat="1" ht="13">
+    <row r="11" spans="1:33" s="78" customFormat="1">
+      <c r="T11" s="121"/>
+    </row>
+    <row r="12" spans="1:33" s="77" customFormat="1">
       <c r="A12" s="77" t="s">
         <v>212</v>
       </c>
       <c r="B12" s="77">
         <f t="shared" ref="B12:S12" si="19">SUM(B13:B19)</f>
-        <v>0</v>
+        <v>1414</v>
       </c>
       <c r="C12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1442</v>
       </c>
       <c r="D12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1457</v>
       </c>
       <c r="E12" s="77">
         <f t="shared" si="19"/>
@@ -18667,15 +18898,15 @@
       </c>
       <c r="F12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1501</v>
       </c>
       <c r="G12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1527</v>
       </c>
       <c r="H12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1544</v>
       </c>
       <c r="I12" s="77">
         <f t="shared" si="19"/>
@@ -18683,15 +18914,15 @@
       </c>
       <c r="J12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1584</v>
       </c>
       <c r="K12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1588</v>
       </c>
       <c r="L12" s="77">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1595</v>
       </c>
       <c r="M12" s="77">
         <f t="shared" si="19"/>
@@ -18721,6 +18952,7 @@
         <f t="shared" si="19"/>
         <v>1688</v>
       </c>
+      <c r="T12" s="120"/>
       <c r="X12" s="77">
         <f t="shared" ref="X12:AC12" si="20">SUM(X13:X19)</f>
         <v>1299</v>
@@ -18746,16 +18978,43 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="13" spans="1:33" s="78" customFormat="1">
       <c r="A13" s="79" t="s">
         <v>201</v>
       </c>
+      <c r="B13" s="78">
+        <v>190</v>
+      </c>
+      <c r="C13" s="78">
+        <v>191</v>
+      </c>
+      <c r="D13" s="78">
+        <v>191</v>
+      </c>
       <c r="E13" s="78">
         <v>191</v>
       </c>
+      <c r="F13" s="78">
+        <v>191</v>
+      </c>
+      <c r="G13" s="78">
+        <v>191</v>
+      </c>
+      <c r="H13" s="78">
+        <v>191</v>
+      </c>
       <c r="I13" s="78">
         <v>191</v>
       </c>
+      <c r="J13" s="78">
+        <v>191</v>
+      </c>
+      <c r="K13" s="78">
+        <v>191</v>
+      </c>
+      <c r="L13" s="78">
+        <v>191</v>
+      </c>
       <c r="M13" s="78">
         <v>191</v>
       </c>
@@ -18777,6 +19036,7 @@
       <c r="S13" s="78">
         <v>191</v>
       </c>
+      <c r="T13" s="121"/>
       <c r="X13" s="78">
         <v>190</v>
       </c>
@@ -18796,16 +19056,43 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="14" spans="1:33" s="78" customFormat="1">
       <c r="A14" s="79" t="s">
         <v>85</v>
       </c>
+      <c r="B14" s="78">
+        <v>511</v>
+      </c>
+      <c r="C14" s="78">
+        <v>531</v>
+      </c>
+      <c r="D14" s="78">
+        <v>544</v>
+      </c>
       <c r="E14" s="78">
         <v>567</v>
       </c>
+      <c r="F14" s="78">
+        <v>577</v>
+      </c>
+      <c r="G14" s="78">
+        <v>599</v>
+      </c>
+      <c r="H14" s="78">
+        <v>612</v>
+      </c>
       <c r="I14" s="78">
         <v>634</v>
       </c>
+      <c r="J14" s="78">
+        <v>637</v>
+      </c>
+      <c r="K14" s="78">
+        <v>639</v>
+      </c>
+      <c r="L14" s="78">
+        <v>645</v>
+      </c>
       <c r="M14" s="78">
         <v>666</v>
       </c>
@@ -18827,6 +19114,7 @@
       <c r="S14" s="78">
         <v>705</v>
       </c>
+      <c r="T14" s="121"/>
       <c r="X14" s="78">
         <v>421</v>
       </c>
@@ -18846,16 +19134,43 @@
         <v>693</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="15" spans="1:33" s="78" customFormat="1">
       <c r="A15" s="79" t="s">
         <v>185</v>
       </c>
+      <c r="B15" s="78">
+        <v>549</v>
+      </c>
+      <c r="C15" s="78">
+        <v>551</v>
+      </c>
+      <c r="D15" s="78">
+        <v>553</v>
+      </c>
       <c r="E15" s="78">
         <v>559</v>
       </c>
+      <c r="F15" s="78">
+        <v>559</v>
+      </c>
+      <c r="G15" s="78">
+        <v>560</v>
+      </c>
+      <c r="H15" s="78">
+        <v>562</v>
+      </c>
       <c r="I15" s="78">
         <v>564</v>
       </c>
+      <c r="J15" s="78">
+        <v>564</v>
+      </c>
+      <c r="K15" s="78">
+        <v>564</v>
+      </c>
+      <c r="L15" s="78">
+        <v>565</v>
+      </c>
       <c r="M15" s="78">
         <v>565</v>
       </c>
@@ -18877,6 +19192,7 @@
       <c r="S15" s="78">
         <v>565</v>
       </c>
+      <c r="T15" s="121"/>
       <c r="X15" s="78">
         <v>534</v>
       </c>
@@ -18896,16 +19212,43 @@
         <v>565</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="78" customFormat="1" ht="13">
+    <row r="16" spans="1:33" s="78" customFormat="1">
       <c r="A16" s="79" t="s">
         <v>188</v>
       </c>
+      <c r="B16" s="78">
+        <v>164</v>
+      </c>
+      <c r="C16" s="78">
+        <v>166</v>
+      </c>
+      <c r="D16" s="78">
+        <v>166</v>
+      </c>
       <c r="E16" s="78">
         <v>169</v>
       </c>
+      <c r="F16" s="78">
+        <v>169</v>
+      </c>
+      <c r="G16" s="78">
+        <v>171</v>
+      </c>
+      <c r="H16" s="78">
+        <v>171</v>
+      </c>
       <c r="I16" s="78">
         <v>172</v>
       </c>
+      <c r="J16" s="78">
+        <v>172</v>
+      </c>
+      <c r="K16" s="78">
+        <v>172</v>
+      </c>
+      <c r="L16" s="78">
+        <v>172</v>
+      </c>
       <c r="M16" s="78">
         <v>172</v>
       </c>
@@ -18927,6 +19270,7 @@
       <c r="S16" s="78">
         <v>172</v>
       </c>
+      <c r="T16" s="121"/>
       <c r="X16" s="78">
         <v>154</v>
       </c>
@@ -18946,10 +19290,19 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="17" spans="1:29" s="78" customFormat="1">
       <c r="A17" s="79" t="s">
         <v>217</v>
       </c>
+      <c r="B17" s="78">
+        <v>0</v>
+      </c>
+      <c r="C17" s="78">
+        <v>0</v>
+      </c>
+      <c r="D17" s="78">
+        <v>0</v>
+      </c>
       <c r="E17" s="78">
         <v>0</v>
       </c>
@@ -18995,6 +19348,7 @@
       <c r="S17" s="78">
         <v>0</v>
       </c>
+      <c r="T17" s="121"/>
       <c r="X17" s="78">
         <v>0</v>
       </c>
@@ -19014,16 +19368,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="18" spans="1:29" s="78" customFormat="1">
       <c r="A18" s="79" t="s">
         <v>180</v>
       </c>
+      <c r="B18" s="78">
+        <v>0</v>
+      </c>
+      <c r="C18" s="78">
+        <v>3</v>
+      </c>
+      <c r="D18" s="78">
+        <v>3</v>
+      </c>
       <c r="E18" s="78">
         <v>4</v>
       </c>
+      <c r="F18" s="78">
+        <v>5</v>
+      </c>
+      <c r="G18" s="78">
+        <v>6</v>
+      </c>
+      <c r="H18" s="78">
+        <v>7</v>
+      </c>
       <c r="I18" s="78">
         <v>11</v>
       </c>
+      <c r="J18" s="78">
+        <v>12</v>
+      </c>
+      <c r="K18" s="78">
+        <v>14</v>
+      </c>
+      <c r="L18" s="78">
+        <v>14</v>
+      </c>
       <c r="M18" s="78">
         <v>15</v>
       </c>
@@ -19045,6 +19426,7 @@
       <c r="S18" s="78">
         <v>17</v>
       </c>
+      <c r="T18" s="121"/>
       <c r="X18" s="78">
         <v>0</v>
       </c>
@@ -19064,16 +19446,43 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="19" spans="1:29" s="78" customFormat="1">
       <c r="A19" s="79" t="s">
         <v>86</v>
       </c>
+      <c r="B19" s="78">
+        <v>0</v>
+      </c>
+      <c r="C19" s="78">
+        <v>0</v>
+      </c>
+      <c r="D19" s="78">
+        <v>0</v>
+      </c>
       <c r="E19" s="78">
         <v>0</v>
+      </c>
+      <c r="F19" s="78">
+        <v>0</v>
+      </c>
+      <c r="G19" s="78">
+        <v>0</v>
+      </c>
+      <c r="H19" s="78">
+        <v>1</v>
       </c>
       <c r="I19" s="78">
         <v>7</v>
       </c>
+      <c r="J19" s="78">
+        <v>8</v>
+      </c>
+      <c r="K19" s="78">
+        <v>8</v>
+      </c>
+      <c r="L19" s="78">
+        <v>8</v>
+      </c>
       <c r="M19" s="78">
         <v>14</v>
       </c>
@@ -19095,6 +19504,7 @@
       <c r="S19" s="78">
         <v>38</v>
       </c>
+      <c r="T19" s="121"/>
       <c r="X19" s="78">
         <v>0</v>
       </c>
@@ -19114,24 +19524,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="20" spans="1:29" s="78" customFormat="1">
       <c r="A20" s="79"/>
-    </row>
-    <row r="21" spans="1:29" s="77" customFormat="1" ht="13">
+      <c r="T20" s="121"/>
+    </row>
+    <row r="21" spans="1:29" s="77" customFormat="1">
       <c r="A21" s="77" t="s">
         <v>211</v>
       </c>
       <c r="B21" s="77">
         <f t="shared" ref="B21:S21" si="21">SUM(B22:B28)</f>
-        <v>0</v>
+        <v>421</v>
       </c>
       <c r="C21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="D21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="E21" s="77">
         <f t="shared" si="21"/>
@@ -19139,15 +19550,15 @@
       </c>
       <c r="F21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>359</v>
       </c>
       <c r="G21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>363</v>
       </c>
       <c r="H21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="I21" s="77">
         <f t="shared" si="21"/>
@@ -19155,15 +19566,15 @@
       </c>
       <c r="J21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>318</v>
       </c>
       <c r="K21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>314</v>
       </c>
       <c r="L21" s="77">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="M21" s="77">
         <f t="shared" si="21"/>
@@ -19193,6 +19604,7 @@
         <f t="shared" si="21"/>
         <v>312</v>
       </c>
+      <c r="T21" s="120"/>
       <c r="X21" s="77">
         <f t="shared" ref="X21:AC21" si="22">SUM(X22:X28)</f>
         <v>450</v>
@@ -19218,16 +19630,43 @@
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="22" spans="1:29" s="78" customFormat="1">
       <c r="A22" s="79" t="s">
         <v>201</v>
       </c>
+      <c r="B22" s="78">
+        <v>1</v>
+      </c>
+      <c r="C22" s="78">
+        <v>0</v>
+      </c>
+      <c r="D22" s="78">
+        <v>0</v>
+      </c>
       <c r="E22" s="78">
         <v>0</v>
       </c>
+      <c r="F22" s="78">
+        <v>0</v>
+      </c>
+      <c r="G22" s="78">
+        <v>0</v>
+      </c>
+      <c r="H22" s="78">
+        <v>0</v>
+      </c>
       <c r="I22" s="78">
         <v>0</v>
       </c>
+      <c r="J22" s="78">
+        <v>0</v>
+      </c>
+      <c r="K22" s="78">
+        <v>0</v>
+      </c>
+      <c r="L22" s="78">
+        <v>0</v>
+      </c>
       <c r="M22" s="78">
         <v>0</v>
       </c>
@@ -19249,6 +19688,7 @@
       <c r="S22" s="78">
         <v>0</v>
       </c>
+      <c r="T22" s="121"/>
       <c r="X22" s="78">
         <v>3</v>
       </c>
@@ -19268,16 +19708,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="23" spans="1:29" s="78" customFormat="1">
       <c r="A23" s="79" t="s">
         <v>85</v>
       </c>
+      <c r="B23" s="78">
+        <v>92</v>
+      </c>
+      <c r="C23" s="78">
+        <v>91</v>
+      </c>
+      <c r="D23" s="78">
+        <v>103</v>
+      </c>
       <c r="E23" s="78">
         <v>204</v>
       </c>
+      <c r="F23" s="78">
+        <v>196</v>
+      </c>
+      <c r="G23" s="78">
+        <v>194</v>
+      </c>
+      <c r="H23" s="78">
+        <v>181</v>
+      </c>
       <c r="I23" s="78">
         <v>181</v>
       </c>
+      <c r="J23" s="78">
+        <v>163</v>
+      </c>
+      <c r="K23" s="78">
+        <v>159</v>
+      </c>
+      <c r="L23" s="78">
+        <v>153</v>
+      </c>
       <c r="M23" s="78">
         <v>132</v>
       </c>
@@ -19299,6 +19766,7 @@
       <c r="S23" s="78">
         <v>143</v>
       </c>
+      <c r="T23" s="121"/>
       <c r="X23" s="78">
         <v>104</v>
       </c>
@@ -19318,16 +19786,43 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="24" spans="1:29" s="78" customFormat="1">
       <c r="A24" s="79" t="s">
         <v>185</v>
       </c>
+      <c r="B24" s="78">
+        <v>43</v>
+      </c>
+      <c r="C24" s="78">
+        <v>36</v>
+      </c>
+      <c r="D24" s="78">
+        <v>10</v>
+      </c>
       <c r="E24" s="78">
         <v>7</v>
       </c>
+      <c r="F24" s="78">
+        <v>7</v>
+      </c>
+      <c r="G24" s="78">
+        <v>6</v>
+      </c>
+      <c r="H24" s="78">
+        <v>3</v>
+      </c>
       <c r="I24" s="78">
         <v>4</v>
       </c>
+      <c r="J24" s="78">
+        <v>4</v>
+      </c>
+      <c r="K24" s="78">
+        <v>4</v>
+      </c>
+      <c r="L24" s="78">
+        <v>3</v>
+      </c>
       <c r="M24" s="78">
         <v>3</v>
       </c>
@@ -19349,6 +19844,7 @@
       <c r="S24" s="78">
         <v>3</v>
       </c>
+      <c r="T24" s="121"/>
       <c r="X24" s="78">
         <v>56</v>
       </c>
@@ -19368,16 +19864,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="25" spans="1:29" s="78" customFormat="1">
       <c r="A25" s="79" t="s">
         <v>188</v>
       </c>
+      <c r="B25" s="78">
+        <v>5</v>
+      </c>
+      <c r="C25" s="78">
+        <v>6</v>
+      </c>
+      <c r="D25" s="78">
+        <v>6</v>
+      </c>
       <c r="E25" s="78">
         <v>3</v>
       </c>
+      <c r="F25" s="78">
+        <v>3</v>
+      </c>
+      <c r="G25" s="78">
+        <v>1</v>
+      </c>
+      <c r="H25" s="78">
+        <v>1</v>
+      </c>
       <c r="I25" s="78">
         <v>0</v>
       </c>
+      <c r="J25" s="78">
+        <v>0</v>
+      </c>
+      <c r="K25" s="78">
+        <v>0</v>
+      </c>
+      <c r="L25" s="78">
+        <v>0</v>
+      </c>
       <c r="M25" s="78">
         <v>0</v>
       </c>
@@ -19399,6 +19922,7 @@
       <c r="S25" s="78">
         <v>0</v>
       </c>
+      <c r="T25" s="121"/>
       <c r="X25" s="78">
         <v>12</v>
       </c>
@@ -19418,10 +19942,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="26" spans="1:29" s="78" customFormat="1">
       <c r="A26" s="79" t="s">
         <v>217</v>
       </c>
+      <c r="B26" s="78">
+        <v>100</v>
+      </c>
+      <c r="C26" s="78">
+        <v>100</v>
+      </c>
+      <c r="D26" s="78">
+        <v>0</v>
+      </c>
       <c r="E26" s="78">
         <v>0</v>
       </c>
@@ -19467,6 +20000,7 @@
       <c r="S26" s="78">
         <v>0</v>
       </c>
+      <c r="T26" s="121"/>
       <c r="X26" s="78">
         <v>100</v>
       </c>
@@ -19486,16 +20020,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="27" spans="1:29" s="78" customFormat="1">
       <c r="A27" s="79" t="s">
         <v>180</v>
       </c>
+      <c r="B27" s="78">
+        <v>74</v>
+      </c>
+      <c r="C27" s="78">
+        <v>47</v>
+      </c>
+      <c r="D27" s="78">
+        <v>59</v>
+      </c>
       <c r="E27" s="78">
         <v>43</v>
       </c>
+      <c r="F27" s="78">
+        <v>41</v>
+      </c>
+      <c r="G27" s="78">
+        <v>38</v>
+      </c>
+      <c r="H27" s="78">
+        <v>37</v>
+      </c>
       <c r="I27" s="78">
         <v>16</v>
       </c>
+      <c r="J27" s="78">
+        <v>15</v>
+      </c>
+      <c r="K27" s="78">
+        <v>11</v>
+      </c>
+      <c r="L27" s="78">
+        <v>8</v>
+      </c>
       <c r="M27" s="78">
         <v>7</v>
       </c>
@@ -19517,6 +20078,7 @@
       <c r="S27" s="78">
         <v>3</v>
       </c>
+      <c r="T27" s="121"/>
       <c r="X27" s="78">
         <v>85</v>
       </c>
@@ -19536,16 +20098,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="78" customFormat="1" ht="13">
+    <row r="28" spans="1:29" s="78" customFormat="1">
       <c r="A28" s="79" t="s">
         <v>86</v>
       </c>
+      <c r="B28" s="78">
+        <v>106</v>
+      </c>
+      <c r="C28" s="78">
+        <v>80</v>
+      </c>
+      <c r="D28" s="78">
+        <v>73</v>
+      </c>
       <c r="E28" s="78">
         <v>111</v>
       </c>
+      <c r="F28" s="78">
+        <v>112</v>
+      </c>
+      <c r="G28" s="78">
+        <v>124</v>
+      </c>
+      <c r="H28" s="78">
+        <v>123</v>
+      </c>
       <c r="I28" s="78">
         <v>137</v>
       </c>
+      <c r="J28" s="78">
+        <v>136</v>
+      </c>
+      <c r="K28" s="78">
+        <v>140</v>
+      </c>
+      <c r="L28" s="78">
+        <v>143</v>
+      </c>
       <c r="M28" s="78">
         <v>139</v>
       </c>
@@ -19567,6 +20156,10 @@
       <c r="S28" s="78">
         <v>163</v>
       </c>
+      <c r="T28" s="121">
+        <f>S28+6</f>
+        <v>169</v>
+      </c>
       <c r="X28" s="78">
         <v>90</v>
       </c>
@@ -19586,18 +20179,66 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="2" customFormat="1" ht="13">
+    <row r="31" spans="1:29" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>213</v>
       </c>
+      <c r="B31" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="34">
+        <f t="shared" ref="F31" si="23">F3/B3-1</f>
+        <v>1.3623978201634968E-2</v>
+      </c>
+      <c r="G31" s="34">
+        <f t="shared" ref="G31" si="24">G3/C3-1</f>
+        <v>4.8834628190898899E-2</v>
+      </c>
+      <c r="H31" s="34">
+        <f t="shared" ref="H31" si="25">H3/D3-1</f>
+        <v>0.10597189695550346</v>
+      </c>
       <c r="I31" s="34">
-        <f>I3/E3-1</f>
+        <f t="shared" ref="I31:L31" si="26">I3/E3-1</f>
         <v>3.1754574811625469E-2</v>
+      </c>
+      <c r="J31" s="34">
+        <f t="shared" si="26"/>
+        <v>2.2580645161290214E-2</v>
+      </c>
+      <c r="K31" s="34">
+        <f t="shared" si="26"/>
+        <v>6.3492063492063266E-3</v>
+      </c>
+      <c r="L31" s="34">
+        <f t="shared" si="26"/>
+        <v>6.8819481206987554E-3</v>
       </c>
       <c r="M31" s="34">
         <f>M3/I3-1</f>
         <v>-6.7814293166406081E-3</v>
       </c>
+      <c r="N31" s="34">
+        <f t="shared" ref="N31" si="27">N3/J3-1</f>
+        <v>1.051524710830698E-3</v>
+      </c>
+      <c r="O31" s="34">
+        <f t="shared" ref="O31" si="28">O3/K3-1</f>
+        <v>2.6288117770767672E-2</v>
+      </c>
+      <c r="P31" s="34">
+        <f t="shared" ref="P31" si="29">P3/L3-1</f>
+        <v>3.4700315457413256E-2</v>
+      </c>
       <c r="Q31" s="34">
         <f>Q3/M3-1</f>
         <v>4.8319327731092487E-2</v>
@@ -19610,12 +20251,13 @@
         <f>S3/O3-1</f>
         <v>2.4590163934426146E-2</v>
       </c>
+      <c r="T31" s="122"/>
       <c r="Y31" s="34">
-        <f t="shared" ref="Y31:Z31" si="23">Y3/X3-1</f>
+        <f t="shared" ref="Y31:Z31" si="30">Y3/X3-1</f>
         <v>4.9170954831332159E-2</v>
       </c>
       <c r="Z31" s="34">
-        <f t="shared" si="23"/>
+        <f t="shared" si="30"/>
         <v>1.2534059945504161E-2</v>
       </c>
       <c r="AA31" s="34">
@@ -19631,18 +20273,66 @@
         <v>4.8319327731092487E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="81" customFormat="1" ht="13">
-      <c r="A32" s="87" t="s">
+    <row r="32" spans="1:29" s="81" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A32" s="85" t="s">
         <v>213</v>
       </c>
+      <c r="B32" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" s="81">
+        <f t="shared" ref="F32" si="31">F3-B3</f>
+        <v>25</v>
+      </c>
+      <c r="G32" s="81">
+        <f t="shared" ref="G32" si="32">G3-C3</f>
+        <v>88</v>
+      </c>
+      <c r="H32" s="81">
+        <f t="shared" ref="H32" si="33">H3-D3</f>
+        <v>181</v>
+      </c>
       <c r="I32" s="81">
-        <f>I3-E3</f>
+        <f t="shared" ref="I32:L32" si="34">I3-E3</f>
         <v>59</v>
+      </c>
+      <c r="J32" s="81">
+        <f t="shared" si="34"/>
+        <v>42</v>
+      </c>
+      <c r="K32" s="81">
+        <f t="shared" si="34"/>
+        <v>12</v>
+      </c>
+      <c r="L32" s="81">
+        <f t="shared" si="34"/>
+        <v>13</v>
       </c>
       <c r="M32" s="81">
         <f>M3-I3</f>
         <v>-13</v>
       </c>
+      <c r="N32" s="81">
+        <f t="shared" ref="N32" si="35">N3-J3</f>
+        <v>2</v>
+      </c>
+      <c r="O32" s="81">
+        <f t="shared" ref="O32" si="36">O3-K3</f>
+        <v>50</v>
+      </c>
+      <c r="P32" s="81">
+        <f t="shared" ref="P32" si="37">P3-L3</f>
+        <v>66</v>
+      </c>
       <c r="Q32" s="81">
         <f>Q3-M3</f>
         <v>92</v>
@@ -19655,12 +20345,13 @@
         <f>S3-O3</f>
         <v>48</v>
       </c>
+      <c r="T32" s="116"/>
       <c r="Y32" s="81">
-        <f t="shared" ref="Y32:Z32" si="24">Y3-X3</f>
+        <f t="shared" ref="Y32:Z32" si="38">Y3-X3</f>
         <v>86</v>
       </c>
       <c r="Z32" s="81">
-        <f t="shared" si="24"/>
+        <f t="shared" si="38"/>
         <v>23</v>
       </c>
       <c r="AA32" s="81">
@@ -19676,32 +20367,79 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:29" ht="12.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>214</v>
       </c>
+      <c r="B33" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="25">
+        <f t="shared" ref="C33" si="39">C3/B3-1</f>
+        <v>-1.7983651226158082E-2</v>
+      </c>
+      <c r="D33" s="25">
+        <f t="shared" ref="D33" si="40">D3/C3-1</f>
+        <v>-5.2164261931187617E-2</v>
+      </c>
+      <c r="E33" s="25">
+        <f t="shared" ref="E33" si="41">E3/D3-1</f>
+        <v>8.7822014051522235E-2</v>
+      </c>
+      <c r="F33" s="25">
+        <f t="shared" ref="F33" si="42">F3/E3-1</f>
+        <v>1.0764262648008671E-3</v>
+      </c>
+      <c r="G33" s="25">
+        <f t="shared" ref="G33" si="43">G3/F3-1</f>
+        <v>1.6129032258064502E-2</v>
+      </c>
+      <c r="H33" s="25">
+        <f t="shared" ref="H33" si="44">H3/G3-1</f>
+        <v>-5.2910052910049021E-4</v>
+      </c>
+      <c r="I33" s="25">
+        <f t="shared" ref="I33" si="45">I3/H3-1</f>
+        <v>1.4822657490735747E-2</v>
+      </c>
+      <c r="J33" s="25">
+        <f t="shared" ref="J33" si="46">J3/I3-1</f>
+        <v>-7.8247261345852914E-3</v>
+      </c>
+      <c r="K33" s="25">
+        <f t="shared" ref="K33" si="47">K3/J3-1</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="25">
+        <f t="shared" ref="L33" si="48">L3/K3-1</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="25">
+        <f t="shared" ref="M33" si="49">M3/L3-1</f>
+        <v>1.051524710830698E-3</v>
+      </c>
       <c r="N33" s="25">
-        <f t="shared" ref="N33:S33" si="25">N3/M3-1</f>
+        <f t="shared" ref="N33" si="50">N3/M3-1</f>
         <v>0</v>
       </c>
       <c r="O33" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="O33" si="51">O3/N3-1</f>
         <v>2.5210084033613356E-2</v>
       </c>
       <c r="P33" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="N33:S33" si="52">P3/O3-1</f>
         <v>8.1967213114753079E-3</v>
       </c>
       <c r="Q33" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="52"/>
         <v>1.4227642276422703E-2</v>
       </c>
       <c r="R33" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="52"/>
         <v>-2.0040080160320661E-3</v>
       </c>
       <c r="S33" s="25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="52"/>
         <v>4.0160642570281624E-3</v>
       </c>
       <c r="X33" s="63" t="s">
@@ -19723,37 +20461,82 @@
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="1:29" s="82" customFormat="1">
-      <c r="A34" s="88" t="s">
+    <row r="34" spans="1:29" s="82" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A34" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="83"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
+      <c r="B34" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="81">
+        <f t="shared" ref="C34" si="53">C3-B3</f>
+        <v>-33</v>
+      </c>
+      <c r="D34" s="81">
+        <f t="shared" ref="D34" si="54">D3-C3</f>
+        <v>-94</v>
+      </c>
+      <c r="E34" s="81">
+        <f t="shared" ref="E34" si="55">E3-D3</f>
+        <v>150</v>
+      </c>
+      <c r="F34" s="81">
+        <f t="shared" ref="F34" si="56">F3-E3</f>
+        <v>2</v>
+      </c>
+      <c r="G34" s="81">
+        <f t="shared" ref="G34" si="57">G3-F3</f>
+        <v>30</v>
+      </c>
+      <c r="H34" s="81">
+        <f t="shared" ref="H34" si="58">H3-G3</f>
+        <v>-1</v>
+      </c>
+      <c r="I34" s="81">
+        <f t="shared" ref="I34" si="59">I3-H3</f>
+        <v>28</v>
+      </c>
+      <c r="J34" s="81">
+        <f t="shared" ref="J34" si="60">J3-I3</f>
+        <v>-15</v>
+      </c>
+      <c r="K34" s="81">
+        <f t="shared" ref="K34" si="61">K3-J3</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="81">
+        <f t="shared" ref="L34" si="62">L3-K3</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="81">
+        <f t="shared" ref="M34" si="63">M3-L3</f>
+        <v>2</v>
+      </c>
       <c r="N34" s="81">
-        <f t="shared" ref="N34:S34" si="26">N3-M3</f>
+        <f t="shared" ref="N34" si="64">N3-M3</f>
         <v>0</v>
       </c>
       <c r="O34" s="81">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="O34" si="65">O3-N3</f>
         <v>48</v>
       </c>
       <c r="P34" s="81">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="N34:S34" si="66">P3-O3</f>
         <v>16</v>
       </c>
       <c r="Q34" s="81">
-        <f t="shared" si="26"/>
+        <f t="shared" si="66"/>
         <v>28</v>
       </c>
       <c r="R34" s="81">
-        <f t="shared" si="26"/>
+        <f t="shared" si="66"/>
         <v>-4</v>
       </c>
       <c r="S34" s="81">
-        <f t="shared" si="26"/>
+        <f t="shared" si="66"/>
         <v>8</v>
       </c>
+      <c r="T34" s="117"/>
       <c r="X34" s="63" t="s">
         <v>186</v>
       </c>
@@ -19773,21 +20556,69 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" ht="12.75" customHeight="1">
       <c r="AC35" s="25"/>
     </row>
-    <row r="36" spans="1:29" s="2" customFormat="1" ht="13">
+    <row r="36" spans="1:29" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="B36" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="F36" s="34">
+        <f t="shared" ref="F36" si="67">F12/B12-1</f>
+        <v>6.1527581329561487E-2</v>
+      </c>
+      <c r="G36" s="34">
+        <f t="shared" ref="G36" si="68">G12/C12-1</f>
+        <v>5.8945908460471541E-2</v>
+      </c>
+      <c r="H36" s="34">
+        <f t="shared" ref="H36" si="69">H12/D12-1</f>
+        <v>5.9711736444749475E-2</v>
+      </c>
       <c r="I36" s="34">
-        <f>I12/E12-1</f>
+        <f t="shared" ref="I36:L36" si="70">I12/E12-1</f>
         <v>5.9731543624160999E-2</v>
+      </c>
+      <c r="J36" s="34">
+        <f t="shared" si="70"/>
+        <v>5.5296469020652994E-2</v>
+      </c>
+      <c r="K36" s="34">
+        <f t="shared" si="70"/>
+        <v>3.9947609692206898E-2</v>
+      </c>
+      <c r="L36" s="34">
+        <f t="shared" si="70"/>
+        <v>3.303108808290145E-2</v>
       </c>
       <c r="M36" s="34">
         <f>M12/I12-1</f>
         <v>2.7865737808739688E-2</v>
       </c>
+      <c r="N36" s="34">
+        <f t="shared" ref="N36" si="71">N12/J12-1</f>
+        <v>3.0303030303030276E-2</v>
+      </c>
+      <c r="O36" s="34">
+        <f t="shared" ref="O36" si="72">O12/K12-1</f>
+        <v>3.6523929471032668E-2</v>
+      </c>
+      <c r="P36" s="34">
+        <f t="shared" ref="P36" si="73">P12/L12-1</f>
+        <v>3.7617554858934144E-2</v>
+      </c>
       <c r="Q36" s="34">
         <f>Q12/M12-1</f>
         <v>2.9574861367837268E-2</v>
@@ -19800,12 +20631,13 @@
         <f>S12/O12-1</f>
         <v>2.5516403402187082E-2</v>
       </c>
+      <c r="T36" s="122"/>
       <c r="Y36" s="34">
-        <f t="shared" ref="Y36:Z36" si="27">Y12/X12-1</f>
+        <f t="shared" ref="Y36:Z36" si="74">Y12/X12-1</f>
         <v>7.7752117013087041E-2</v>
       </c>
       <c r="Z36" s="34">
-        <f t="shared" si="27"/>
+        <f t="shared" si="74"/>
         <v>6.4285714285714279E-2</v>
       </c>
       <c r="AA36" s="34">
@@ -19821,18 +20653,66 @@
         <v>2.9574861367837268E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:29" s="81" customFormat="1" ht="13">
-      <c r="A37" s="87" t="s">
+    <row r="37" spans="1:29" s="81" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A37" s="85" t="s">
         <v>202</v>
       </c>
+      <c r="B37" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E37" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="F37" s="81">
+        <f t="shared" ref="F37" si="75">F12-B12</f>
+        <v>87</v>
+      </c>
+      <c r="G37" s="81">
+        <f t="shared" ref="G37" si="76">G12-C12</f>
+        <v>85</v>
+      </c>
+      <c r="H37" s="81">
+        <f t="shared" ref="H37" si="77">H12-D12</f>
+        <v>87</v>
+      </c>
       <c r="I37" s="81">
-        <f>I12-E12</f>
+        <f t="shared" ref="I37:L37" si="78">I12-E12</f>
         <v>89</v>
+      </c>
+      <c r="J37" s="81">
+        <f t="shared" si="78"/>
+        <v>83</v>
+      </c>
+      <c r="K37" s="81">
+        <f t="shared" si="78"/>
+        <v>61</v>
+      </c>
+      <c r="L37" s="81">
+        <f t="shared" si="78"/>
+        <v>51</v>
       </c>
       <c r="M37" s="81">
         <f>M12-I12</f>
         <v>44</v>
       </c>
+      <c r="N37" s="81">
+        <f t="shared" ref="N37" si="79">N12-J12</f>
+        <v>48</v>
+      </c>
+      <c r="O37" s="81">
+        <f t="shared" ref="O37" si="80">O12-K12</f>
+        <v>58</v>
+      </c>
+      <c r="P37" s="81">
+        <f t="shared" ref="P37" si="81">P12-L12</f>
+        <v>60</v>
+      </c>
       <c r="Q37" s="81">
         <f>Q12-M12</f>
         <v>48</v>
@@ -19845,12 +20725,13 @@
         <f>S12-O12</f>
         <v>42</v>
       </c>
+      <c r="T37" s="116"/>
       <c r="Y37" s="81">
-        <f t="shared" ref="Y37:Z37" si="28">Y12-X12</f>
+        <f t="shared" ref="Y37:Z37" si="82">Y12-X12</f>
         <v>101</v>
       </c>
       <c r="Z37" s="81">
-        <f t="shared" si="28"/>
+        <f t="shared" si="82"/>
         <v>90</v>
       </c>
       <c r="AA37" s="81">
@@ -19866,32 +20747,79 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:29" ht="12.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>203</v>
       </c>
+      <c r="B38" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" s="25">
+        <f t="shared" ref="C38" si="83">C12/B12-1</f>
+        <v>1.980198019801982E-2</v>
+      </c>
+      <c r="D38" s="25">
+        <f t="shared" ref="D38" si="84">D12/C12-1</f>
+        <v>1.0402219140083213E-2</v>
+      </c>
+      <c r="E38" s="25">
+        <f t="shared" ref="E38" si="85">E12/D12-1</f>
+        <v>2.2649279341111939E-2</v>
+      </c>
+      <c r="F38" s="25">
+        <f t="shared" ref="F38" si="86">F12/E12-1</f>
+        <v>7.382550335570448E-3</v>
+      </c>
+      <c r="G38" s="25">
+        <f t="shared" ref="G38" si="87">G12/F12-1</f>
+        <v>1.7321785476348994E-2</v>
+      </c>
+      <c r="H38" s="25">
+        <f t="shared" ref="H38" si="88">H12/G12-1</f>
+        <v>1.1132940406024971E-2</v>
+      </c>
+      <c r="I38" s="25">
+        <f t="shared" ref="I38" si="89">I12/H12-1</f>
+        <v>2.26683937823835E-2</v>
+      </c>
+      <c r="J38" s="25">
+        <f t="shared" ref="J38" si="90">J12/I12-1</f>
+        <v>3.1665611146294292E-3</v>
+      </c>
+      <c r="K38" s="25">
+        <f t="shared" ref="K38" si="91">K12/J12-1</f>
+        <v>2.525252525252597E-3</v>
+      </c>
+      <c r="L38" s="25">
+        <f t="shared" ref="L38" si="92">L12/K12-1</f>
+        <v>4.4080604534004753E-3</v>
+      </c>
+      <c r="M38" s="25">
+        <f t="shared" ref="M38" si="93">M12/L12-1</f>
+        <v>1.7554858934169193E-2</v>
+      </c>
       <c r="N38" s="25">
-        <f t="shared" ref="N38:S38" si="29">N12/M12-1</f>
+        <f t="shared" ref="N38" si="94">N12/M12-1</f>
         <v>5.5452865064695711E-3</v>
       </c>
       <c r="O38" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="O38" si="95">O12/N12-1</f>
         <v>8.5784313725489891E-3</v>
       </c>
       <c r="P38" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="N38:S38" si="96">P12/O12-1</f>
         <v>5.4678007290400732E-3</v>
       </c>
       <c r="Q38" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="96"/>
         <v>9.6676737160121817E-3</v>
       </c>
       <c r="R38" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="96"/>
         <v>3.5906642728904536E-3</v>
       </c>
       <c r="S38" s="25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="96"/>
         <v>6.5593321407275695E-3</v>
       </c>
       <c r="X38" s="63" t="s">
@@ -19913,37 +20841,82 @@
         <v>186</v>
       </c>
     </row>
-    <row r="39" spans="1:29" s="84" customFormat="1">
-      <c r="A39" s="89" t="s">
+    <row r="39" spans="1:29" s="83" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A39" s="87" t="s">
         <v>203</v>
       </c>
-      <c r="B39" s="85"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
+      <c r="B39" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="81">
+        <f t="shared" ref="C39" si="97">C12-B12</f>
+        <v>28</v>
+      </c>
+      <c r="D39" s="81">
+        <f t="shared" ref="D39" si="98">D12-C12</f>
+        <v>15</v>
+      </c>
+      <c r="E39" s="81">
+        <f t="shared" ref="E39" si="99">E12-D12</f>
+        <v>33</v>
+      </c>
+      <c r="F39" s="81">
+        <f t="shared" ref="F39" si="100">F12-E12</f>
+        <v>11</v>
+      </c>
+      <c r="G39" s="81">
+        <f t="shared" ref="G39" si="101">G12-F12</f>
+        <v>26</v>
+      </c>
+      <c r="H39" s="81">
+        <f t="shared" ref="H39" si="102">H12-G12</f>
+        <v>17</v>
+      </c>
+      <c r="I39" s="81">
+        <f t="shared" ref="I39" si="103">I12-H12</f>
+        <v>35</v>
+      </c>
+      <c r="J39" s="81">
+        <f t="shared" ref="J39" si="104">J12-I12</f>
+        <v>5</v>
+      </c>
+      <c r="K39" s="81">
+        <f t="shared" ref="K39" si="105">K12-J12</f>
+        <v>4</v>
+      </c>
+      <c r="L39" s="81">
+        <f t="shared" ref="L39" si="106">L12-K12</f>
+        <v>7</v>
+      </c>
+      <c r="M39" s="81">
+        <f t="shared" ref="M39" si="107">M12-L12</f>
+        <v>28</v>
+      </c>
       <c r="N39" s="81">
-        <f t="shared" ref="N39:S39" si="30">N12-M12</f>
+        <f t="shared" ref="N39" si="108">N12-M12</f>
         <v>9</v>
       </c>
       <c r="O39" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="O39" si="109">O12-N12</f>
         <v>14</v>
       </c>
       <c r="P39" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="N39:S39" si="110">P12-O12</f>
         <v>9</v>
       </c>
       <c r="Q39" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="110"/>
         <v>16</v>
       </c>
       <c r="R39" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="110"/>
         <v>6</v>
       </c>
       <c r="S39" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="110"/>
         <v>11</v>
       </c>
+      <c r="T39" s="117"/>
       <c r="X39" s="63" t="s">
         <v>186</v>
       </c>
@@ -19963,23 +20936,71 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:29" ht="12.75" customHeight="1">
       <c r="AC40" s="25"/>
     </row>
-    <row r="41" spans="1:29" s="2" customFormat="1" ht="13">
+    <row r="41" spans="1:29" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>215</v>
       </c>
+      <c r="B41" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="D41" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="E41" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" s="34">
+        <f t="shared" ref="F41" si="111">F21/B21-1</f>
+        <v>-0.14726840855106893</v>
+      </c>
+      <c r="G41" s="34">
+        <f t="shared" ref="G41" si="112">G21/C21-1</f>
+        <v>8.3333333333333037E-3</v>
+      </c>
+      <c r="H41" s="34">
+        <f t="shared" ref="H41" si="113">H21/D21-1</f>
+        <v>0.3745019920318724</v>
+      </c>
       <c r="I41" s="34">
-        <f t="shared" ref="I41" si="31">I21/E21-1</f>
+        <f t="shared" ref="I41" si="114">I21/E21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
+      <c r="J41" s="34">
+        <f t="shared" ref="J41" si="115">J21/F21-1</f>
+        <v>-0.11420612813370479</v>
+      </c>
+      <c r="K41" s="34">
+        <f t="shared" ref="K41" si="116">K21/G21-1</f>
+        <v>-0.13498622589531684</v>
+      </c>
+      <c r="L41" s="34">
+        <f t="shared" ref="L41" si="117">L21/H21-1</f>
+        <v>-0.11014492753623184</v>
+      </c>
       <c r="M41" s="34">
-        <f t="shared" ref="M41" si="32">M21/I21-1</f>
+        <f t="shared" ref="M41" si="118">M21/I21-1</f>
         <v>-0.16863905325443784</v>
       </c>
+      <c r="N41" s="34">
+        <f t="shared" ref="N41" si="119">N21/J21-1</f>
+        <v>-0.14465408805031443</v>
+      </c>
+      <c r="O41" s="34">
+        <f t="shared" ref="O41" si="120">O21/K21-1</f>
+        <v>-2.5477707006369421E-2</v>
+      </c>
+      <c r="P41" s="34">
+        <f t="shared" ref="P41" si="121">P21/L21-1</f>
+        <v>1.9543973941368087E-2</v>
+      </c>
       <c r="Q41" s="34">
-        <f t="shared" ref="Q41" si="33">Q21/M21-1</f>
+        <f t="shared" ref="Q41" si="122">Q21/M21-1</f>
         <v>0.15658362989323837</v>
       </c>
       <c r="R41" s="34">
@@ -19987,19 +21008,20 @@
         <v>0.15808823529411775</v>
       </c>
       <c r="S41" s="34">
-        <f t="shared" ref="S41" si="34">S21/O21-1</f>
+        <f t="shared" ref="S41" si="123">S21/O21-1</f>
         <v>1.9607843137254832E-2</v>
       </c>
+      <c r="T41" s="122"/>
       <c r="Y41" s="34">
-        <f t="shared" ref="Y41" si="35">Y21/X21-1</f>
+        <f t="shared" ref="Y41" si="124">Y21/X21-1</f>
         <v>-3.3333333333333326E-2</v>
       </c>
       <c r="Z41" s="34">
-        <f t="shared" ref="Z41" si="36">Z21/Y21-1</f>
+        <f t="shared" ref="Z41" si="125">Z21/Y21-1</f>
         <v>-0.15402298850574714</v>
       </c>
       <c r="AA41" s="34">
-        <f t="shared" ref="AA41" si="37">AA21/Z21-1</f>
+        <f t="shared" ref="AA41" si="126">AA21/Z21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
       <c r="AB41" s="34">
@@ -20011,69 +21033,165 @@
         <v>0.15658362989323837</v>
       </c>
     </row>
-    <row r="42" spans="1:29" s="86" customFormat="1" ht="13">
-      <c r="A42" s="90" t="s">
+    <row r="42" spans="1:29" s="84" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A42" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="I42" s="86">
-        <f>I21-E21</f>
+      <c r="B42" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E42" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="F42" s="84">
+        <f t="shared" ref="F42" si="127">F21-B21</f>
+        <v>-62</v>
+      </c>
+      <c r="G42" s="84">
+        <f t="shared" ref="G42" si="128">G21-C21</f>
+        <v>3</v>
+      </c>
+      <c r="H42" s="84">
+        <f t="shared" ref="H42" si="129">H21-D21</f>
+        <v>94</v>
+      </c>
+      <c r="I42" s="84">
+        <f t="shared" ref="I42:L42" si="130">I21-E21</f>
         <v>-30</v>
       </c>
-      <c r="M42" s="86">
+      <c r="J42" s="84">
+        <f t="shared" si="130"/>
+        <v>-41</v>
+      </c>
+      <c r="K42" s="84">
+        <f t="shared" si="130"/>
+        <v>-49</v>
+      </c>
+      <c r="L42" s="84">
+        <f t="shared" si="130"/>
+        <v>-38</v>
+      </c>
+      <c r="M42" s="84">
         <f>M21-I21</f>
         <v>-57</v>
       </c>
-      <c r="Q42" s="86">
-        <f t="shared" ref="Q42:R42" si="38">Q21-M21</f>
+      <c r="N42" s="84">
+        <f t="shared" ref="N42" si="131">N21-J21</f>
+        <v>-46</v>
+      </c>
+      <c r="O42" s="84">
+        <f t="shared" ref="O42" si="132">O21-K21</f>
+        <v>-8</v>
+      </c>
+      <c r="P42" s="84">
+        <f t="shared" ref="P42" si="133">P21-L21</f>
+        <v>6</v>
+      </c>
+      <c r="Q42" s="84">
+        <f t="shared" ref="Q42:R42" si="134">Q21-M21</f>
         <v>44</v>
       </c>
-      <c r="R42" s="86">
-        <f t="shared" si="38"/>
+      <c r="R42" s="84">
+        <f t="shared" si="134"/>
         <v>43</v>
       </c>
-      <c r="S42" s="86">
+      <c r="S42" s="84">
         <f>S21-O21</f>
         <v>6</v>
       </c>
-      <c r="Y42" s="86">
-        <f t="shared" ref="Y42" si="39">Y21-X21</f>
+      <c r="T42" s="118"/>
+      <c r="Y42" s="84">
+        <f t="shared" ref="Y42" si="135">Y21-X21</f>
         <v>-15</v>
       </c>
-      <c r="Z42" s="86">
-        <f t="shared" ref="Z42" si="40">Z21-Y21</f>
+      <c r="Z42" s="84">
+        <f t="shared" ref="Z42" si="136">Z21-Y21</f>
         <v>-67</v>
       </c>
-      <c r="AA42" s="86">
-        <f t="shared" ref="AA42:AB42" si="41">AA21-Z21</f>
+      <c r="AA42" s="84">
+        <f t="shared" ref="AA42:AB42" si="137">AA21-Z21</f>
         <v>-30</v>
       </c>
-      <c r="AB42" s="86">
-        <f t="shared" si="41"/>
+      <c r="AB42" s="84">
+        <f t="shared" si="137"/>
         <v>-57</v>
       </c>
-      <c r="AC42" s="86">
+      <c r="AC42" s="84">
         <f>AC21-AB21</f>
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:29" ht="12.75" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>216</v>
       </c>
+      <c r="B43" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" s="25">
+        <f t="shared" ref="C43" si="138">C21/B21-1</f>
+        <v>-0.14489311163895491</v>
+      </c>
+      <c r="D43" s="25">
+        <f t="shared" ref="D43" si="139">D21/C21-1</f>
+        <v>-0.30277777777777781</v>
+      </c>
+      <c r="E43" s="25">
+        <f t="shared" ref="E43" si="140">E21/D21-1</f>
+        <v>0.46613545816733071</v>
+      </c>
+      <c r="F43" s="25">
+        <f t="shared" ref="F43" si="141">F21/E21-1</f>
+        <v>-2.4456521739130488E-2</v>
+      </c>
+      <c r="G43" s="25">
+        <f t="shared" ref="G43" si="142">G21/F21-1</f>
+        <v>1.1142061281337101E-2</v>
+      </c>
+      <c r="H43" s="25">
+        <f t="shared" ref="H43" si="143">H21/G21-1</f>
+        <v>-4.9586776859504078E-2</v>
+      </c>
+      <c r="I43" s="25">
+        <f t="shared" ref="I43" si="144">I21/H21-1</f>
+        <v>-2.0289855072463725E-2</v>
+      </c>
+      <c r="J43" s="25">
+        <f t="shared" ref="J43" si="145">J21/I21-1</f>
+        <v>-5.9171597633136064E-2</v>
+      </c>
+      <c r="K43" s="25">
+        <f t="shared" ref="K43" si="146">K21/J21-1</f>
+        <v>-1.2578616352201255E-2</v>
+      </c>
+      <c r="L43" s="25">
+        <f t="shared" ref="L43" si="147">L21/K21-1</f>
+        <v>-2.2292993630573243E-2</v>
+      </c>
+      <c r="M43" s="25">
+        <f t="shared" ref="M43" si="148">M21/L21-1</f>
+        <v>-8.4690553745928376E-2</v>
+      </c>
       <c r="N43" s="25">
-        <f t="shared" ref="N43:P43" si="42">N21/M21-1</f>
+        <f t="shared" ref="N43" si="149">N21/M21-1</f>
         <v>-3.2028469750889688E-2</v>
       </c>
       <c r="O43" s="25">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="O43" si="150">O21/N21-1</f>
         <v>0.125</v>
       </c>
       <c r="P43" s="25">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="N43:P43" si="151">P21/O21-1</f>
         <v>2.2875816993463971E-2</v>
       </c>
       <c r="Q43" s="25">
-        <f t="shared" ref="Q43" si="43">Q21/P21-1</f>
+        <f t="shared" ref="Q43" si="152">Q21/P21-1</f>
         <v>3.833865814696491E-2</v>
       </c>
       <c r="R43" s="25">
@@ -20081,7 +21199,7 @@
         <v>-3.0769230769230771E-2</v>
       </c>
       <c r="S43" s="25">
-        <f t="shared" ref="S43" si="44">S21/R21-1</f>
+        <f t="shared" ref="S43" si="153">S21/R21-1</f>
         <v>-9.52380952380949E-3</v>
       </c>
       <c r="X43" s="63" t="s">
@@ -20103,37 +21221,82 @@
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:29" s="84" customFormat="1">
-      <c r="A44" s="89" t="s">
+    <row r="44" spans="1:29" s="83" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A44" s="87" t="s">
         <v>216</v>
       </c>
-      <c r="B44" s="85"/>
-      <c r="C44" s="85"/>
-      <c r="D44" s="85"/>
+      <c r="B44" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="81">
+        <f t="shared" ref="C44" si="154">C21-B21</f>
+        <v>-61</v>
+      </c>
+      <c r="D44" s="81">
+        <f t="shared" ref="D44" si="155">D21-C21</f>
+        <v>-109</v>
+      </c>
+      <c r="E44" s="81">
+        <f t="shared" ref="E44" si="156">E21-D21</f>
+        <v>117</v>
+      </c>
+      <c r="F44" s="81">
+        <f t="shared" ref="F44" si="157">F21-E21</f>
+        <v>-9</v>
+      </c>
+      <c r="G44" s="81">
+        <f t="shared" ref="G44" si="158">G21-F21</f>
+        <v>4</v>
+      </c>
+      <c r="H44" s="81">
+        <f t="shared" ref="H44" si="159">H21-G21</f>
+        <v>-18</v>
+      </c>
+      <c r="I44" s="81">
+        <f t="shared" ref="I44" si="160">I21-H21</f>
+        <v>-7</v>
+      </c>
+      <c r="J44" s="81">
+        <f t="shared" ref="J44" si="161">J21-I21</f>
+        <v>-20</v>
+      </c>
+      <c r="K44" s="81">
+        <f t="shared" ref="K44" si="162">K21-J21</f>
+        <v>-4</v>
+      </c>
+      <c r="L44" s="81">
+        <f t="shared" ref="L44" si="163">L21-K21</f>
+        <v>-7</v>
+      </c>
+      <c r="M44" s="81">
+        <f t="shared" ref="M44" si="164">M21-L21</f>
+        <v>-26</v>
+      </c>
       <c r="N44" s="81">
-        <f t="shared" ref="N44:R44" si="45">N21-M21</f>
+        <f t="shared" ref="N44" si="165">N21-M21</f>
         <v>-9</v>
       </c>
       <c r="O44" s="81">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="O44" si="166">O21-N21</f>
         <v>34</v>
       </c>
       <c r="P44" s="81">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="N44:R44" si="167">P21-O21</f>
         <v>7</v>
       </c>
       <c r="Q44" s="81">
-        <f t="shared" si="45"/>
+        <f t="shared" si="167"/>
         <v>12</v>
       </c>
       <c r="R44" s="81">
-        <f t="shared" si="45"/>
+        <f t="shared" si="167"/>
         <v>-10</v>
       </c>
       <c r="S44" s="81">
         <f>S21-R21</f>
         <v>-3</v>
       </c>
+      <c r="T44" s="117"/>
       <c r="X44" s="63" t="s">
         <v>186</v>
       </c>
@@ -20153,31 +21316,41 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:29" ht="12.75" customHeight="1">
       <c r="N47" s="76"/>
     </row>
-    <row r="49" spans="14:14">
+    <row r="49" spans="14:14" ht="12.75" customHeight="1">
       <c r="N49" s="75"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" xr:uid="{3579012F-D250-C14B-8084-0358505A2D9B}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{77A3087C-239B-E34B-8F51-3E2EA54A463A}"/>
-    <hyperlink ref="P2" r:id="rId3" xr:uid="{614FFF93-232C-A94F-8FDC-F25E6D371847}"/>
-    <hyperlink ref="N2" r:id="rId4" xr:uid="{9287A329-D88E-784B-8BDF-1EDA927EB785}"/>
-    <hyperlink ref="S2" r:id="rId5" xr:uid="{6AF4C14B-B6A4-FE47-B0D3-A570A390AD5C}"/>
-    <hyperlink ref="O2" r:id="rId6" xr:uid="{0A17F8BF-EADB-DE42-994D-117A4F2CB3FE}"/>
-    <hyperlink ref="AC2" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
-    <hyperlink ref="M2" r:id="rId8" xr:uid="{F1748A46-ECC6-544E-9D30-C00CF38C6CF7}"/>
-    <hyperlink ref="AB2" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
-    <hyperlink ref="AA2" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
-    <hyperlink ref="I2" r:id="rId11" xr:uid="{998E2907-64B9-7A44-8D65-8083912D2D62}"/>
-    <hyperlink ref="E2" r:id="rId12" xr:uid="{5D689E99-05ED-E34E-9D87-28B9F22988C9}"/>
-    <hyperlink ref="Z2" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
-    <hyperlink ref="Y2" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
-    <hyperlink ref="X2" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
+    <hyperlink ref="R1" r:id="rId1" xr:uid="{3579012F-D250-C14B-8084-0358505A2D9B}"/>
+    <hyperlink ref="Q1" r:id="rId2" xr:uid="{77A3087C-239B-E34B-8F51-3E2EA54A463A}"/>
+    <hyperlink ref="P1" r:id="rId3" xr:uid="{614FFF93-232C-A94F-8FDC-F25E6D371847}"/>
+    <hyperlink ref="N1" r:id="rId4" xr:uid="{9287A329-D88E-784B-8BDF-1EDA927EB785}"/>
+    <hyperlink ref="S1" r:id="rId5" xr:uid="{6AF4C14B-B6A4-FE47-B0D3-A570A390AD5C}"/>
+    <hyperlink ref="O1" r:id="rId6" xr:uid="{0A17F8BF-EADB-DE42-994D-117A4F2CB3FE}"/>
+    <hyperlink ref="AC1" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
+    <hyperlink ref="M1" r:id="rId8" xr:uid="{F1748A46-ECC6-544E-9D30-C00CF38C6CF7}"/>
+    <hyperlink ref="AB1" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
+    <hyperlink ref="AA1" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
+    <hyperlink ref="I1" r:id="rId11" xr:uid="{998E2907-64B9-7A44-8D65-8083912D2D62}"/>
+    <hyperlink ref="E1" r:id="rId12" xr:uid="{5D689E99-05ED-E34E-9D87-28B9F22988C9}"/>
+    <hyperlink ref="Z1" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
+    <hyperlink ref="Y1" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
+    <hyperlink ref="X1" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
+    <hyperlink ref="L1" r:id="rId16" xr:uid="{E0D344DF-ECD3-4969-946B-75165895949D}"/>
+    <hyperlink ref="K1" r:id="rId17" xr:uid="{34FDBE06-551B-4817-B842-42B3C369DE44}"/>
+    <hyperlink ref="J1" r:id="rId18" xr:uid="{8672DEA7-6978-4CBC-A339-3D96580B25F6}"/>
+    <hyperlink ref="H1" r:id="rId19" xr:uid="{17B363D6-A0A5-40EB-B7DB-DDC426C51A14}"/>
+    <hyperlink ref="G1" r:id="rId20" xr:uid="{31E18C39-D30F-4CE8-9CC8-617FD1B8BCF2}"/>
+    <hyperlink ref="F1" r:id="rId21" xr:uid="{C604ED82-58BF-4FA7-9129-2334C1DCA7D7}"/>
+    <hyperlink ref="D1" r:id="rId22" xr:uid="{9AA615B1-70E4-40CE-8BD9-FA369F45AAE7}"/>
+    <hyperlink ref="C1" r:id="rId23" xr:uid="{B190BD40-76B4-4C45-B1D6-B5043307E3B6}"/>
+    <hyperlink ref="B1" r:id="rId24" xr:uid="{2E883042-0703-4781-AC08-6A8AD2EAD4EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId16"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add key event re. $300m revolving credit facility
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FC0ECB-AA15-4B4A-9E34-D4180A2C7992}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12445F0-8CAF-4307-9548-A7F465B79E5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="256">
   <si>
     <t>$ERJ</t>
   </si>
@@ -929,6 +929,9 @@
   </si>
   <si>
     <t>FY14</t>
+  </si>
+  <si>
+    <t>Embraer closes $650m syndicated credit facility to regain access to financial resources for 3 years @ fixed rates</t>
   </si>
 </sst>
 </file>
@@ -6265,10 +6268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC53"/>
+  <dimension ref="A2:AC56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -6330,17 +6333,17 @@
         <v>44835</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
+        <v>255</v>
+      </c>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
       <c r="R6" s="38"/>
       <c r="T6" s="41" t="s">
         <v>148</v>
@@ -6365,18 +6368,16 @@
         <v>Q222</v>
       </c>
       <c r="G7" s="10"/>
-      <c r="H7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
       <c r="R7" s="38"/>
       <c r="T7" s="46" t="s">
         <v>84</v>
@@ -6399,18 +6400,16 @@
       </c>
       <c r="D8" s="18"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
       <c r="R8" s="38"/>
       <c r="T8" s="45" t="s">
         <v>137</v>
@@ -6435,8 +6434,12 @@
         <f>$C$28</f>
         <v>Q222</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="37"/>
+      <c r="G9" s="9">
+        <v>44835</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="I9" s="37"/>
       <c r="J9" s="37"/>
       <c r="K9" s="37"/>
@@ -6466,11 +6469,9 @@
         <f>$C$28</f>
         <v>Q222</v>
       </c>
-      <c r="G10" s="9">
-        <v>44835</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>29</v>
+      <c r="G10" s="10"/>
+      <c r="H10" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="I10" s="37"/>
       <c r="J10" s="37"/>
@@ -6503,7 +6504,7 @@
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="8" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="37"/>
@@ -6556,8 +6557,12 @@
       <c r="AC12" s="111"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="G13" s="10"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="9">
+        <v>44835</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="I13" s="37"/>
       <c r="J13" s="37"/>
       <c r="K13" s="37"/>
@@ -6585,11 +6590,9 @@
       <c r="AC13" s="119"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="G14" s="9">
-        <v>44805</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>187</v>
+      <c r="G14" s="10"/>
+      <c r="H14" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="I14" s="37"/>
       <c r="J14" s="37"/>
@@ -6708,17 +6711,17 @@
         <v>44805</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="60"/>
+        <v>187</v>
+      </c>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
       <c r="R17" s="38"/>
       <c r="T17" s="42"/>
       <c r="U17" s="37"/>
@@ -6741,18 +6744,16 @@
       <c r="C18" s="114"/>
       <c r="D18" s="115"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
       <c r="R18" s="38"/>
       <c r="T18" s="46" t="s">
         <v>139</v>
@@ -6777,18 +6778,16 @@
       <c r="C19" s="116"/>
       <c r="D19" s="117"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="60"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
       <c r="R19" s="38"/>
       <c r="T19" s="45" t="s">
         <v>142</v>
@@ -6809,9 +6808,11 @@
       <c r="AC19" s="115"/>
     </row>
     <row r="20" spans="2:29">
-      <c r="G20" s="10"/>
-      <c r="H20" s="8" t="s">
-        <v>191</v>
+      <c r="G20" s="9">
+        <v>44805</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="I20" s="60"/>
       <c r="J20" s="60"/>
@@ -6822,9 +6823,7 @@
       <c r="O20" s="60"/>
       <c r="P20" s="60"/>
       <c r="Q20" s="60"/>
-      <c r="R20" s="51" t="s">
-        <v>194</v>
-      </c>
+      <c r="R20" s="38"/>
       <c r="T20" s="45" t="s">
         <v>141</v>
       </c>
@@ -6845,7 +6844,9 @@
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="10"/>
-      <c r="H21" s="60"/>
+      <c r="H21" s="8" t="s">
+        <v>192</v>
+      </c>
       <c r="I21" s="60"/>
       <c r="J21" s="60"/>
       <c r="K21" s="60"/>
@@ -6875,7 +6876,9 @@
       <c r="C22" s="110"/>
       <c r="D22" s="111"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="60"/>
+      <c r="H22" s="8" t="s">
+        <v>193</v>
+      </c>
       <c r="I22" s="60"/>
       <c r="J22" s="60"/>
       <c r="K22" s="60"/>
@@ -6906,11 +6909,9 @@
         <v>132</v>
       </c>
       <c r="D23" s="115"/>
-      <c r="G23" s="9">
-        <v>44743</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>196</v>
+      <c r="G23" s="10"/>
+      <c r="H23" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="I23" s="60"/>
       <c r="J23" s="60"/>
@@ -6921,7 +6922,9 @@
       <c r="O23" s="60"/>
       <c r="P23" s="60"/>
       <c r="Q23" s="60"/>
-      <c r="R23" s="38"/>
+      <c r="R23" s="51" t="s">
+        <v>194</v>
+      </c>
       <c r="T23" s="42"/>
       <c r="U23" s="37"/>
       <c r="V23" s="37"/>
@@ -6936,9 +6939,7 @@
       </c>
       <c r="D24" s="115"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="8" t="s">
-        <v>197</v>
-      </c>
+      <c r="H24" s="60"/>
       <c r="I24" s="60"/>
       <c r="J24" s="60"/>
       <c r="K24" s="60"/>
@@ -6961,9 +6962,7 @@
       <c r="C25" s="114"/>
       <c r="D25" s="115"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="50" t="s">
-        <v>198</v>
-      </c>
+      <c r="H25" s="60"/>
       <c r="I25" s="60"/>
       <c r="J25" s="60"/>
       <c r="K25" s="60"/>
@@ -6990,8 +6989,12 @@
         <v>2392.9</v>
       </c>
       <c r="D26" s="113"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="60"/>
+      <c r="G26" s="9">
+        <v>44743</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>196</v>
+      </c>
       <c r="I26" s="60"/>
       <c r="J26" s="60"/>
       <c r="K26" s="60"/>
@@ -7013,21 +7016,19 @@
       <c r="B27" s="10"/>
       <c r="C27" s="114"/>
       <c r="D27" s="115"/>
-      <c r="G27" s="9">
-        <v>44743</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
       <c r="R27" s="38"/>
       <c r="T27" s="45" t="s">
         <v>146</v>
@@ -7047,8 +7048,8 @@
         <v>44777</v>
       </c>
       <c r="G28" s="10"/>
-      <c r="H28" s="8" t="s">
-        <v>242</v>
+      <c r="H28" s="50" t="s">
+        <v>198</v>
       </c>
       <c r="I28" s="60"/>
       <c r="J28" s="60"/>
@@ -7094,20 +7095,20 @@
     </row>
     <row r="30" spans="2:29">
       <c r="G30" s="9">
-        <v>44682</v>
-      </c>
-      <c r="H30" s="60" t="s">
-        <v>250</v>
-      </c>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
+        <v>44743</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="37"/>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="37"/>
       <c r="R30" s="38"/>
       <c r="T30" s="42"/>
       <c r="U30" s="37"/>
@@ -7117,7 +7118,7 @@
     <row r="31" spans="2:29">
       <c r="G31" s="10"/>
       <c r="H31" s="8" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="I31" s="60"/>
       <c r="J31" s="60"/>
@@ -7128,9 +7129,7 @@
       <c r="O31" s="60"/>
       <c r="P31" s="60"/>
       <c r="Q31" s="60"/>
-      <c r="R31" s="51" t="s">
-        <v>31</v>
-      </c>
+      <c r="R31" s="38"/>
       <c r="T31" s="46" t="s">
         <v>149</v>
       </c>
@@ -7173,20 +7172,20 @@
       </c>
       <c r="D33" s="125"/>
       <c r="G33" s="9">
-        <v>43922</v>
-      </c>
-      <c r="H33" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
+        <v>44682</v>
+      </c>
+      <c r="H33" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
       <c r="R33" s="38"/>
       <c r="T33" s="42"/>
       <c r="U33" s="37"/>
@@ -7204,18 +7203,20 @@
       <c r="D34" s="125"/>
       <c r="G34" s="10"/>
       <c r="H34" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="37"/>
-      <c r="R34" s="38"/>
+        <v>251</v>
+      </c>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="51" t="s">
+        <v>31</v>
+      </c>
       <c r="T34" s="43"/>
       <c r="U34" s="35"/>
       <c r="V34" s="35"/>
@@ -7231,23 +7232,25 @@
       </c>
       <c r="D35" s="121"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="37"/>
-      <c r="Q35" s="37"/>
-      <c r="R35" s="51" t="s">
-        <v>31</v>
-      </c>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="38"/>
     </row>
     <row r="36" spans="2:23">
-      <c r="G36" s="10"/>
-      <c r="H36" s="37"/>
+      <c r="G36" s="9">
+        <v>43922</v>
+      </c>
+      <c r="H36" s="37" t="s">
+        <v>164</v>
+      </c>
       <c r="I36" s="37"/>
       <c r="J36" s="37"/>
       <c r="K36" s="37"/>
@@ -7260,11 +7263,9 @@
       <c r="R36" s="38"/>
     </row>
     <row r="37" spans="2:23">
-      <c r="G37" s="9">
-        <v>43770</v>
-      </c>
-      <c r="H37" s="37" t="s">
-        <v>167</v>
+      <c r="G37" s="10"/>
+      <c r="H37" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="I37" s="37"/>
       <c r="J37" s="37"/>
@@ -7290,9 +7291,7 @@
       <c r="C38" s="110"/>
       <c r="D38" s="111"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="50" t="s">
-        <v>168</v>
-      </c>
+      <c r="H38" s="37"/>
       <c r="I38" s="37"/>
       <c r="J38" s="37"/>
       <c r="K38" s="37"/>
@@ -7302,7 +7301,9 @@
       <c r="O38" s="37"/>
       <c r="P38" s="37"/>
       <c r="Q38" s="37"/>
-      <c r="R38" s="38"/>
+      <c r="R38" s="51" t="s">
+        <v>31</v>
+      </c>
       <c r="T38" s="42" t="s">
         <v>159</v>
       </c>
@@ -7346,10 +7347,10 @@
         <v>31</v>
       </c>
       <c r="G40" s="9">
-        <v>43739</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>246</v>
+        <v>43770</v>
+      </c>
+      <c r="H40" s="37" t="s">
+        <v>167</v>
       </c>
       <c r="I40" s="37"/>
       <c r="J40" s="37"/>
@@ -7359,9 +7360,7 @@
       <c r="N40" s="37"/>
       <c r="O40" s="37"/>
       <c r="P40" s="37"/>
-      <c r="Q40" s="37" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q40" s="37"/>
       <c r="R40" s="38"/>
       <c r="T40" s="44" t="s">
         <v>161</v>
@@ -7377,7 +7376,9 @@
         <v>31</v>
       </c>
       <c r="G41" s="10"/>
-      <c r="H41" s="60"/>
+      <c r="H41" s="50" t="s">
+        <v>168</v>
+      </c>
       <c r="I41" s="37"/>
       <c r="J41" s="37"/>
       <c r="K41" s="37"/>
@@ -7424,8 +7425,12 @@
       <c r="D43" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="37"/>
+      <c r="G43" s="9">
+        <v>43739</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>246</v>
+      </c>
       <c r="I43" s="37"/>
       <c r="J43" s="37"/>
       <c r="K43" s="37"/>
@@ -7434,7 +7439,9 @@
       <c r="N43" s="37"/>
       <c r="O43" s="37"/>
       <c r="P43" s="37"/>
-      <c r="Q43" s="37"/>
+      <c r="Q43" s="37" t="s">
+        <v>179</v>
+      </c>
       <c r="R43" s="38"/>
       <c r="T43" s="61" t="s">
         <v>200</v>
@@ -7444,12 +7451,8 @@
       <c r="W43" s="38"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="G44" s="9">
-        <v>43586</v>
-      </c>
-      <c r="H44" s="60" t="s">
-        <v>166</v>
-      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="60"/>
       <c r="I44" s="37"/>
       <c r="J44" s="37"/>
       <c r="K44" s="37"/>
@@ -7482,12 +7485,8 @@
       <c r="R45" s="38"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="G46" s="9">
-        <v>43282</v>
-      </c>
-      <c r="H46" s="37" t="s">
-        <v>162</v>
-      </c>
+      <c r="G46" s="10"/>
+      <c r="H46" s="37"/>
       <c r="I46" s="37"/>
       <c r="J46" s="37"/>
       <c r="K46" s="37"/>
@@ -7500,9 +7499,11 @@
       <c r="R46" s="38"/>
     </row>
     <row r="47" spans="2:23">
-      <c r="G47" s="10"/>
-      <c r="H47" s="8" t="s">
-        <v>163</v>
+      <c r="G47" s="9">
+        <v>43586</v>
+      </c>
+      <c r="H47" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="I47" s="37"/>
       <c r="J47" s="37"/>
@@ -7517,51 +7518,57 @@
     </row>
     <row r="48" spans="2:23">
       <c r="G48" s="10"/>
-      <c r="H48" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="I48" s="60"/>
-      <c r="J48" s="60"/>
-      <c r="K48" s="60"/>
-      <c r="L48" s="60"/>
-      <c r="M48" s="60"/>
-      <c r="N48" s="60"/>
-      <c r="O48" s="60"/>
-      <c r="P48" s="60"/>
-      <c r="Q48" s="60"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
       <c r="R48" s="38"/>
     </row>
     <row r="49" spans="7:18">
-      <c r="G49" s="10"/>
-      <c r="H49" s="60"/>
-      <c r="I49" s="60"/>
-      <c r="J49" s="60"/>
-      <c r="K49" s="60"/>
-      <c r="L49" s="60"/>
-      <c r="M49" s="60"/>
-      <c r="N49" s="60"/>
-      <c r="O49" s="60"/>
-      <c r="P49" s="60"/>
-      <c r="Q49" s="60"/>
+      <c r="G49" s="9">
+        <v>43282</v>
+      </c>
+      <c r="H49" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
       <c r="R49" s="38"/>
     </row>
     <row r="50" spans="7:18">
       <c r="G50" s="10"/>
-      <c r="H50" s="60"/>
-      <c r="I50" s="60"/>
-      <c r="J50" s="60"/>
-      <c r="K50" s="60"/>
-      <c r="L50" s="60"/>
-      <c r="M50" s="60"/>
-      <c r="N50" s="60"/>
-      <c r="O50" s="60"/>
-      <c r="P50" s="60"/>
-      <c r="Q50" s="60"/>
+      <c r="H50" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
       <c r="R50" s="38"/>
     </row>
     <row r="51" spans="7:18">
       <c r="G51" s="10"/>
-      <c r="H51" s="60"/>
+      <c r="H51" s="8" t="s">
+        <v>165</v>
+      </c>
       <c r="I51" s="60"/>
       <c r="J51" s="60"/>
       <c r="K51" s="60"/>
@@ -7588,22 +7595,64 @@
       <c r="R52" s="38"/>
     </row>
     <row r="53" spans="7:18">
-      <c r="G53" s="91">
+      <c r="G53" s="10"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="60"/>
+      <c r="L53" s="60"/>
+      <c r="M53" s="60"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="60"/>
+      <c r="P53" s="60"/>
+      <c r="Q53" s="60"/>
+      <c r="R53" s="38"/>
+    </row>
+    <row r="54" spans="7:18">
+      <c r="G54" s="10"/>
+      <c r="H54" s="60"/>
+      <c r="I54" s="60"/>
+      <c r="J54" s="60"/>
+      <c r="K54" s="60"/>
+      <c r="L54" s="60"/>
+      <c r="M54" s="60"/>
+      <c r="N54" s="60"/>
+      <c r="O54" s="60"/>
+      <c r="P54" s="60"/>
+      <c r="Q54" s="60"/>
+      <c r="R54" s="38"/>
+    </row>
+    <row r="55" spans="7:18">
+      <c r="G55" s="10"/>
+      <c r="H55" s="60"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="60"/>
+      <c r="K55" s="60"/>
+      <c r="L55" s="60"/>
+      <c r="M55" s="60"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="60"/>
+      <c r="P55" s="60"/>
+      <c r="Q55" s="60"/>
+      <c r="R55" s="38"/>
+    </row>
+    <row r="56" spans="7:18">
+      <c r="G56" s="91">
         <v>42552</v>
       </c>
-      <c r="H53" s="54" t="s">
+      <c r="H56" s="54" t="s">
         <v>240</v>
       </c>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35"/>
-      <c r="O53" s="35"/>
-      <c r="P53" s="35"/>
-      <c r="Q53" s="35"/>
-      <c r="R53" s="36"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="35"/>
+      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
+      <c r="O56" s="35"/>
+      <c r="P56" s="35"/>
+      <c r="Q56" s="35"/>
+      <c r="R56" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -7653,26 +7702,27 @@
     <mergeCell ref="AB13:AC13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H10" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H13" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C29:D29" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R35" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H14" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H17" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R20" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H23" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="R38" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H17" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H20" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R23" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H26" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
     <hyperlink ref="W44" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
     <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
     <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
-    <hyperlink ref="H27" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H40" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="H30" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H43" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
     <hyperlink ref="D40" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D39" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
-    <hyperlink ref="R31" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="R34" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H6" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId17"/>
-  <drawing r:id="rId18"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -7680,11 +7730,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
   <dimension ref="B1:AO141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -8510,6 +8560,7 @@
       <c r="T10" s="27">
         <v>785.6</v>
       </c>
+      <c r="V10" s="27"/>
       <c r="X10" s="27">
         <v>5038.3</v>
       </c>
@@ -8611,6 +8662,7 @@
         <f t="shared" si="1"/>
         <v>233.29999999999995</v>
       </c>
+      <c r="V11" s="26"/>
       <c r="X11" s="26">
         <f t="shared" ref="X11:AC11" si="2">X9-X10</f>
         <v>1250.5</v>
@@ -8785,6 +8837,7 @@
       <c r="T13" s="27">
         <v>67.400000000000006</v>
       </c>
+      <c r="V13" s="25"/>
       <c r="X13" s="27">
         <v>419.9</v>
       </c>
@@ -10475,7 +10528,7 @@
         <v>0.2289724212385906</v>
       </c>
       <c r="X36" s="25">
-        <f t="shared" ref="X36:Z36" si="52">X11/X9</f>
+        <f t="shared" ref="X36:Y36" si="52">X11/X9</f>
         <v>0.19884556672179113</v>
       </c>
       <c r="Y36" s="25">
@@ -10584,7 +10637,7 @@
         <v>6.5462753950338556E-2</v>
       </c>
       <c r="X37" s="25">
-        <f t="shared" ref="X37:Z37" si="64">X18/X9</f>
+        <f t="shared" ref="X37:Y37" si="64">X18/X9</f>
         <v>8.6391680447780173E-2</v>
       </c>
       <c r="Y37" s="25">
@@ -10693,7 +10746,7 @@
         <v>7.2725488271665487E-2</v>
       </c>
       <c r="X38" s="25">
-        <f t="shared" ref="X38:Z38" si="76">X23/X9</f>
+        <f t="shared" ref="X38:Y38" si="76">X23/X9</f>
         <v>5.5288767332400457E-2</v>
       </c>
       <c r="Y38" s="25">
@@ -10802,7 +10855,7 @@
         <v>-0.49696969696969745</v>
       </c>
       <c r="X39" s="25">
-        <f t="shared" ref="X39:Z39" si="87">X22/X21</f>
+        <f t="shared" ref="X39:Y39" si="87">X22/X21</f>
         <v>0.30998213931335583</v>
       </c>
       <c r="Y39" s="25">
@@ -10916,7 +10969,7 @@
         <v>32</v>
       </c>
       <c r="X43" s="2">
-        <f t="shared" ref="X43:Z43" si="98">X44+X52</f>
+        <f t="shared" ref="X43:Y43" si="98">X44+X52</f>
         <v>208</v>
       </c>
       <c r="Y43" s="2">
@@ -11025,7 +11078,7 @@
         <v>11</v>
       </c>
       <c r="X44" s="40">
-        <f t="shared" ref="X44:Z44" si="105">SUM(X45:X50)</f>
+        <f t="shared" ref="X44:Y44" si="105">SUM(X45:X50)</f>
         <v>92</v>
       </c>
       <c r="Y44" s="40">
@@ -11635,7 +11688,7 @@
         <v>21</v>
       </c>
       <c r="X52" s="40">
-        <f t="shared" ref="X52:Z52" si="114">X53+X54+X55</f>
+        <f t="shared" ref="X52:Y52" si="114">X53+X54+X55</f>
         <v>116</v>
       </c>
       <c r="Y52" s="40">
@@ -17323,7 +17376,7 @@
         <v>2872.7</v>
       </c>
       <c r="X121" s="27">
-        <f t="shared" ref="X121:Z121" si="173">X87-X116</f>
+        <f t="shared" ref="X121:Y121" si="173">X87-X116</f>
         <v>3864.8</v>
       </c>
       <c r="Y121" s="27">
@@ -17432,7 +17485,7 @@
         <v>3.9105635720119789</v>
       </c>
       <c r="X122" s="3">
-        <f t="shared" ref="X122:Z122" si="185">X121/X27</f>
+        <f t="shared" ref="X122:Y122" si="185">X121/X27</f>
         <v>5.2675480441597387</v>
       </c>
       <c r="Y122" s="3">
@@ -17549,7 +17602,7 @@
         <v>1968.2</v>
       </c>
       <c r="X124" s="52">
-        <f t="shared" ref="X124:Z124" si="198">X61+X62+X74+X76</f>
+        <f t="shared" ref="X124:Y124" si="198">X61+X62+X74+X76</f>
         <v>2482.1</v>
       </c>
       <c r="Y124" s="52">
@@ -17658,7 +17711,7 @@
         <v>3173.8999999999996</v>
       </c>
       <c r="X125" s="52">
-        <f t="shared" ref="X125:Z125" si="209">X92+X96+X106+X93+X107</f>
+        <f t="shared" ref="X125:Y125" si="209">X92+X96+X106+X93+X107</f>
         <v>2923.5</v>
       </c>
       <c r="Y125" s="52">
@@ -17767,7 +17820,7 @@
         <v>-1205.6999999999996</v>
       </c>
       <c r="X126" s="27">
-        <f t="shared" ref="X126:Z126" si="221">X124-X125</f>
+        <f t="shared" ref="X126:Y126" si="221">X124-X125</f>
         <v>-441.40000000000009</v>
       </c>
       <c r="Y126" s="27">
@@ -18275,7 +18328,7 @@
         <v>6449.7879999999996</v>
       </c>
       <c r="X134" s="27">
-        <f t="shared" ref="X134:Z134" si="265">X133*X27</f>
+        <f t="shared" ref="X134:Y134" si="265">X133*X27</f>
         <v>27044.182000000001</v>
       </c>
       <c r="Y134" s="27">
@@ -18384,7 +18437,7 @@
         <v>7655.4879999999994</v>
       </c>
       <c r="X135" s="27">
-        <f t="shared" ref="X135:Z135" si="273">X134-X126</f>
+        <f t="shared" ref="X135:Y135" si="273">X134-X126</f>
         <v>27485.582000000002</v>
       </c>
       <c r="Y135" s="27">
@@ -18493,7 +18546,7 @@
         <v>2.2452006822849584</v>
       </c>
       <c r="X137" s="57">
-        <f t="shared" ref="X137:Z137" si="280">X133/X122</f>
+        <f t="shared" ref="X137:Y137" si="280">X133/X122</f>
         <v>6.9975631339267226</v>
       </c>
       <c r="Y137" s="57">
@@ -18597,7 +18650,7 @@
         <v>2.2633532687151986E-3</v>
       </c>
       <c r="X138" s="57">
-        <f t="shared" ref="X138:Z138" si="292">X134/X9</f>
+        <f t="shared" ref="X138:Y138" si="292">X134/X9</f>
         <v>4.3003724080905741</v>
       </c>
       <c r="Y138" s="57">
@@ -18701,7 +18754,7 @@
         <v>-16621.554193892349</v>
       </c>
       <c r="X139" s="57">
-        <f t="shared" ref="X139:Z139" si="304">X133/X26</f>
+        <f t="shared" ref="X139:Y139" si="304">X133/X26</f>
         <v>80.801260830594572</v>
       </c>
       <c r="Y139" s="57">
@@ -18877,7 +18930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
@@ -18896,10 +18949,10 @@
   <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X32" sqref="X32"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -21727,7 +21780,7 @@
         <v>186</v>
       </c>
       <c r="X37" s="81">
-        <f t="shared" ref="W37:X37" si="88">X12-W12</f>
+        <f t="shared" ref="X37" si="88">X12-W12</f>
         <v>91</v>
       </c>
       <c r="Y37" s="81">

</xml_diff>

<commit_message>
Calculate ROE, ROA, ROTB & Buffet Return
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12445F0-8CAF-4307-9548-A7F465B79E5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201AF951-7909-4F54-9E1C-2D2E9A8CCD60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="261">
   <si>
     <t>$ERJ</t>
   </si>
@@ -932,6 +932,21 @@
   </si>
   <si>
     <t>Embraer closes $650m syndicated credit facility to regain access to financial resources for 3 years @ fixed rates</t>
+  </si>
+  <si>
+    <t>TTM Cash Flow</t>
+  </si>
+  <si>
+    <t>ROE (Return on Equity)</t>
+  </si>
+  <si>
+    <t>ROA (Return on Assets)</t>
+  </si>
+  <si>
+    <t>ROTB (Return on Tangible Book)</t>
+  </si>
+  <si>
+    <t>Buffet Return</t>
   </si>
 </sst>
 </file>
@@ -1445,10 +1460,22 @@
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1458,30 +1485,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1502,16 +1505,28 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6270,8 +6285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y31" sqref="Y31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -6291,35 +6306,35 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="111"/>
-      <c r="G5" s="109" t="s">
+      <c r="C5" s="114"/>
+      <c r="D5" s="115"/>
+      <c r="G5" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="110"/>
-      <c r="N5" s="110"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="111"/>
-      <c r="T5" s="109" t="s">
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114"/>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="114"/>
+      <c r="Q5" s="114"/>
+      <c r="R5" s="115"/>
+      <c r="T5" s="113" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="111"/>
-      <c r="AA5" s="107" t="s">
+      <c r="U5" s="114"/>
+      <c r="V5" s="114"/>
+      <c r="W5" s="115"/>
+      <c r="AA5" s="122" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="108"/>
+      <c r="AB5" s="123"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -6548,13 +6563,13 @@
       <c r="U12" s="37"/>
       <c r="V12" s="37"/>
       <c r="W12" s="38"/>
-      <c r="Y12" s="109" t="s">
+      <c r="Y12" s="113" t="s">
         <v>219</v>
       </c>
-      <c r="Z12" s="110"/>
-      <c r="AA12" s="110"/>
-      <c r="AB12" s="110"/>
-      <c r="AC12" s="111"/>
+      <c r="Z12" s="114"/>
+      <c r="AA12" s="114"/>
+      <c r="AB12" s="114"/>
+      <c r="AC12" s="115"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9">
@@ -6580,14 +6595,14 @@
       <c r="V13" s="37"/>
       <c r="W13" s="38"/>
       <c r="Y13" s="92"/>
-      <c r="Z13" s="118" t="s">
+      <c r="Z13" s="128" t="s">
         <v>220</v>
       </c>
-      <c r="AA13" s="118"/>
-      <c r="AB13" s="118" t="s">
+      <c r="AA13" s="128"/>
+      <c r="AB13" s="128" t="s">
         <v>221</v>
       </c>
-      <c r="AC13" s="119"/>
+      <c r="AC13" s="129"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="10"/>
@@ -6613,21 +6628,21 @@
       <c r="Y14" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="Z14" s="114" t="s">
+      <c r="Z14" s="111" t="s">
         <v>231</v>
       </c>
-      <c r="AA14" s="114"/>
-      <c r="AB14" s="114" t="s">
+      <c r="AA14" s="111"/>
+      <c r="AB14" s="111" t="s">
         <v>232</v>
       </c>
-      <c r="AC14" s="115"/>
+      <c r="AC14" s="112"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="110"/>
-      <c r="D15" s="111"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="115"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -6649,14 +6664,14 @@
       <c r="Y15" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="Z15" s="114" t="s">
+      <c r="Z15" s="111" t="s">
         <v>227</v>
       </c>
-      <c r="AA15" s="114"/>
-      <c r="AB15" s="114" t="s">
+      <c r="AA15" s="111"/>
+      <c r="AB15" s="111" t="s">
         <v>233</v>
       </c>
-      <c r="AC15" s="115"/>
+      <c r="AC15" s="112"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="14" t="s">
@@ -6665,10 +6680,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="111" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="115"/>
+      <c r="D16" s="112"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -6690,23 +6705,23 @@
       <c r="Y16" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="Z16" s="114" t="s">
+      <c r="Z16" s="111" t="s">
         <v>228</v>
       </c>
-      <c r="AA16" s="114"/>
-      <c r="AB16" s="114" t="s">
+      <c r="AA16" s="111"/>
+      <c r="AB16" s="111" t="s">
         <v>234</v>
       </c>
-      <c r="AC16" s="115"/>
+      <c r="AC16" s="112"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="114" t="s">
+      <c r="C17" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="115"/>
+      <c r="D17" s="112"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
@@ -6730,19 +6745,19 @@
       <c r="Y17" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="Z17" s="114" t="s">
+      <c r="Z17" s="111" t="s">
         <v>229</v>
       </c>
-      <c r="AA17" s="114"/>
-      <c r="AB17" s="114" t="s">
+      <c r="AA17" s="111"/>
+      <c r="AB17" s="111" t="s">
         <v>235</v>
       </c>
-      <c r="AC17" s="115"/>
+      <c r="AC17" s="112"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="16"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="115"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="112"/>
       <c r="G18" s="10"/>
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
@@ -6764,19 +6779,19 @@
       <c r="Y18" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="Z18" s="114" t="s">
+      <c r="Z18" s="111" t="s">
         <v>230</v>
       </c>
-      <c r="AA18" s="114"/>
-      <c r="AB18" s="114" t="s">
+      <c r="AA18" s="111"/>
+      <c r="AB18" s="111" t="s">
         <v>236</v>
       </c>
-      <c r="AC18" s="115"/>
+      <c r="AC18" s="112"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="17"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="117"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="127"/>
       <c r="G19" s="10"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
@@ -6798,14 +6813,14 @@
       <c r="Y19" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="Z19" s="114" t="s">
+      <c r="Z19" s="111" t="s">
         <v>238</v>
       </c>
-      <c r="AA19" s="114"/>
-      <c r="AB19" s="114" t="s">
+      <c r="AA19" s="111"/>
+      <c r="AB19" s="111" t="s">
         <v>239</v>
       </c>
-      <c r="AC19" s="115"/>
+      <c r="AC19" s="112"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9">
@@ -6833,14 +6848,14 @@
       <c r="Y20" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="Z20" s="114" t="s">
+      <c r="Z20" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="AA20" s="114"/>
-      <c r="AB20" s="114" t="s">
+      <c r="AA20" s="111"/>
+      <c r="AB20" s="111" t="s">
         <v>245</v>
       </c>
-      <c r="AC20" s="115"/>
+      <c r="AC20" s="112"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="10"/>
@@ -6870,11 +6885,11 @@
       <c r="AC21" s="38"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="110"/>
-      <c r="D22" s="111"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="115"/>
       <c r="G22" s="10"/>
       <c r="H22" s="8" t="s">
         <v>193</v>
@@ -6905,10 +6920,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="114" t="s">
+      <c r="C23" s="111" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="115"/>
+      <c r="D23" s="112"/>
       <c r="G23" s="10"/>
       <c r="H23" s="8" t="s">
         <v>191</v>
@@ -6934,10 +6949,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="114">
+      <c r="C24" s="111">
         <v>1969</v>
       </c>
-      <c r="D24" s="115"/>
+      <c r="D24" s="112"/>
       <c r="G24" s="10"/>
       <c r="H24" s="60"/>
       <c r="I24" s="60"/>
@@ -6959,8 +6974,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="10"/>
-      <c r="C25" s="114"/>
-      <c r="D25" s="115"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="112"/>
       <c r="G25" s="10"/>
       <c r="H25" s="60"/>
       <c r="I25" s="60"/>
@@ -6984,11 +6999,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="112">
+      <c r="C26" s="124">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="113"/>
+      <c r="D26" s="125"/>
       <c r="G26" s="9">
         <v>44743</v>
       </c>
@@ -7014,8 +7029,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="10"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="115"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="112"/>
       <c r="G27" s="10"/>
       <c r="H27" s="8" t="s">
         <v>197</v>
@@ -7072,10 +7087,10 @@
       <c r="B29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="122" t="s">
+      <c r="C29" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="123"/>
+      <c r="D29" s="119"/>
       <c r="G29" s="10"/>
       <c r="H29" s="60"/>
       <c r="I29" s="60"/>
@@ -7138,11 +7153,11 @@
       <c r="W31" s="38"/>
     </row>
     <row r="32" spans="2:29">
-      <c r="B32" s="109" t="s">
+      <c r="B32" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="110"/>
-      <c r="D32" s="111"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="115"/>
       <c r="G32" s="10"/>
       <c r="H32" s="60"/>
       <c r="I32" s="60"/>
@@ -7166,11 +7181,11 @@
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="124">
+      <c r="C33" s="120">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D33" s="125"/>
+      <c r="D33" s="121"/>
       <c r="G33" s="9">
         <v>44682</v>
       </c>
@@ -7196,11 +7211,11 @@
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="124">
+      <c r="C34" s="120">
         <f>C6/'Financial Model'!AE9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D34" s="125"/>
+      <c r="D34" s="121"/>
       <c r="G34" s="10"/>
       <c r="H34" s="8" t="s">
         <v>251</v>
@@ -7226,11 +7241,11 @@
       <c r="B35" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="120">
+      <c r="C35" s="116">
         <f>C6/'Financial Model'!AE26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D35" s="121"/>
+      <c r="D35" s="117"/>
       <c r="G35" s="10"/>
       <c r="H35" s="60"/>
       <c r="I35" s="60"/>
@@ -7277,19 +7292,19 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="T37" s="109" t="s">
+      <c r="T37" s="113" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="110"/>
-      <c r="V37" s="110"/>
-      <c r="W37" s="111"/>
+      <c r="U37" s="114"/>
+      <c r="V37" s="114"/>
+      <c r="W37" s="115"/>
     </row>
     <row r="38" spans="2:23">
-      <c r="B38" s="109" t="s">
+      <c r="B38" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="C38" s="110"/>
-      <c r="D38" s="111"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="115"/>
       <c r="G38" s="10"/>
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
@@ -7312,10 +7327,10 @@
       <c r="W38" s="38"/>
     </row>
     <row r="39" spans="2:23">
-      <c r="B39" s="126" t="s">
+      <c r="B39" s="107" t="s">
         <v>248</v>
       </c>
-      <c r="C39" s="127"/>
+      <c r="C39" s="108"/>
       <c r="D39" s="51" t="s">
         <v>31</v>
       </c>
@@ -7339,10 +7354,10 @@
       <c r="W39" s="38"/>
     </row>
     <row r="40" spans="2:23">
-      <c r="B40" s="126" t="s">
+      <c r="B40" s="107" t="s">
         <v>249</v>
       </c>
-      <c r="C40" s="127"/>
+      <c r="C40" s="108"/>
       <c r="D40" s="51" t="s">
         <v>31</v>
       </c>
@@ -7370,8 +7385,8 @@
       <c r="W40" s="38"/>
     </row>
     <row r="41" spans="2:23">
-      <c r="B41" s="126"/>
-      <c r="C41" s="127"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="108"/>
       <c r="D41" s="89" t="s">
         <v>31</v>
       </c>
@@ -7395,8 +7410,8 @@
       <c r="W41" s="38"/>
     </row>
     <row r="42" spans="2:23">
-      <c r="B42" s="126"/>
-      <c r="C42" s="127"/>
+      <c r="B42" s="107"/>
+      <c r="C42" s="108"/>
       <c r="D42" s="89" t="s">
         <v>31</v>
       </c>
@@ -7420,8 +7435,8 @@
       <c r="W42" s="38"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="128"/>
-      <c r="C43" s="129"/>
+      <c r="B43" s="109"/>
+      <c r="C43" s="110"/>
       <c r="D43" s="90" t="s">
         <v>31</v>
       </c>
@@ -7656,34 +7671,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="C26:D26"/>
@@ -7700,6 +7687,34 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H9" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -7728,13 +7743,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
-  <dimension ref="B1:AO141"/>
+  <dimension ref="B1:AO147"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="E121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -18892,6 +18907,564 @@
       <c r="AE141" s="25">
         <f t="shared" si="309"/>
         <v>1.0244925188220719E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="2:31">
+      <c r="C142" s="14"/>
+      <c r="D142" s="25"/>
+      <c r="E142" s="25"/>
+      <c r="F142" s="25"/>
+      <c r="G142" s="25"/>
+      <c r="H142" s="25"/>
+      <c r="I142" s="25"/>
+      <c r="J142" s="25"/>
+      <c r="K142" s="25"/>
+      <c r="L142" s="25"/>
+      <c r="M142" s="25"/>
+      <c r="N142" s="25"/>
+      <c r="O142" s="25"/>
+      <c r="P142" s="25"/>
+      <c r="Q142" s="25"/>
+      <c r="R142" s="25"/>
+      <c r="S142" s="25"/>
+      <c r="T142" s="25"/>
+      <c r="X142" s="25"/>
+      <c r="Y142" s="25"/>
+      <c r="Z142" s="25"/>
+      <c r="AA142" s="25"/>
+      <c r="AB142" s="25"/>
+      <c r="AC142" s="25"/>
+      <c r="AD142" s="25"/>
+      <c r="AE142" s="25"/>
+    </row>
+    <row r="143" spans="2:31" s="2" customFormat="1">
+      <c r="B143" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C143" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D143" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E143" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F143" s="26">
+        <f t="shared" ref="F143:S143" si="310">SUM(C23:F23)</f>
+        <v>-166.40000000000032</v>
+      </c>
+      <c r="G143" s="26">
+        <f t="shared" si="310"/>
+        <v>-172.70000000000024</v>
+      </c>
+      <c r="H143" s="26">
+        <f t="shared" si="310"/>
+        <v>-38.800000000000068</v>
+      </c>
+      <c r="I143" s="26">
+        <f t="shared" si="310"/>
+        <v>-103.50000000000016</v>
+      </c>
+      <c r="J143" s="26">
+        <f t="shared" si="310"/>
+        <v>-316.50000000000011</v>
+      </c>
+      <c r="K143" s="26">
+        <f t="shared" si="310"/>
+        <v>-565.90000000000009</v>
+      </c>
+      <c r="L143" s="26">
+        <f t="shared" si="310"/>
+        <v>-887.70000000000027</v>
+      </c>
+      <c r="M143" s="26">
+        <f t="shared" si="310"/>
+        <v>-931.90000000000009</v>
+      </c>
+      <c r="N143" s="26">
+        <f t="shared" si="310"/>
+        <v>-728.19999999999993</v>
+      </c>
+      <c r="O143" s="26">
+        <f t="shared" si="310"/>
+        <v>-527.5999999999998</v>
+      </c>
+      <c r="P143" s="26">
+        <f t="shared" si="310"/>
+        <v>-125.79999999999983</v>
+      </c>
+      <c r="Q143" s="26">
+        <f t="shared" si="310"/>
+        <v>-51.999999999999829</v>
+      </c>
+      <c r="R143" s="26">
+        <f t="shared" si="310"/>
+        <v>-43.5</v>
+      </c>
+      <c r="S143" s="26">
+        <f t="shared" si="310"/>
+        <v>15.800000000000026</v>
+      </c>
+      <c r="T143" s="26">
+        <f>SUM(Q23:T23)</f>
+        <v>0.69999999999996021</v>
+      </c>
+      <c r="X143" s="26">
+        <f t="shared" ref="X143:AE143" si="311">X23</f>
+        <v>347.7</v>
+      </c>
+      <c r="Y143" s="26">
+        <f t="shared" si="311"/>
+        <v>80.800000000000153</v>
+      </c>
+      <c r="Z143" s="26">
+        <f t="shared" si="311"/>
+        <v>167.80000000000015</v>
+      </c>
+      <c r="AA143" s="26">
+        <f t="shared" si="311"/>
+        <v>262.80000000000047</v>
+      </c>
+      <c r="AB143" s="26">
+        <f t="shared" si="311"/>
+        <v>-171.20000000000002</v>
+      </c>
+      <c r="AC143" s="26">
+        <f t="shared" si="311"/>
+        <v>-316.5</v>
+      </c>
+      <c r="AD143" s="26">
+        <f t="shared" si="311"/>
+        <v>-728.30000000000007</v>
+      </c>
+      <c r="AE143" s="26">
+        <f>AE23</f>
+        <v>-43.500000000000142</v>
+      </c>
+    </row>
+    <row r="144" spans="2:31">
+      <c r="B144" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C144" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D144" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E144" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F144" s="25">
+        <f t="shared" ref="F144:S144" si="312">SUM(C23:F23)/F118</f>
+        <v>-4.223243064896838E-2</v>
+      </c>
+      <c r="G144" s="25">
+        <f t="shared" si="312"/>
+        <v>-4.4376493563224366E-2</v>
+      </c>
+      <c r="H144" s="25">
+        <f t="shared" si="312"/>
+        <v>-9.9230198716145548E-3</v>
+      </c>
+      <c r="I144" s="25">
+        <f t="shared" si="312"/>
+        <v>-2.72203666202036E-2</v>
+      </c>
+      <c r="J144" s="25">
+        <f t="shared" si="312"/>
+        <v>-8.7561555912134159E-2</v>
+      </c>
+      <c r="K144" s="25">
+        <f t="shared" si="312"/>
+        <v>-0.1722993545244185</v>
+      </c>
+      <c r="L144" s="25">
+        <f t="shared" si="312"/>
+        <v>-0.29785592054491167</v>
+      </c>
+      <c r="M144" s="25">
+        <f t="shared" si="312"/>
+        <v>-0.3318495833630084</v>
+      </c>
+      <c r="N144" s="25">
+        <f t="shared" si="312"/>
+        <v>-0.25045571797076521</v>
+      </c>
+      <c r="O144" s="25">
+        <f t="shared" si="312"/>
+        <v>-0.18880618379616368</v>
+      </c>
+      <c r="P144" s="25">
+        <f t="shared" si="312"/>
+        <v>-4.3594275219184193E-2</v>
+      </c>
+      <c r="Q144" s="25">
+        <f t="shared" si="312"/>
+        <v>-1.8517199629655947E-2</v>
+      </c>
+      <c r="R144" s="25">
+        <f t="shared" si="312"/>
+        <v>-1.5675675675675675E-2</v>
+      </c>
+      <c r="S144" s="25">
+        <f t="shared" si="312"/>
+        <v>5.7310747578802369E-3</v>
+      </c>
+      <c r="T144" s="25">
+        <f>SUM(Q23:T23)/T118</f>
+        <v>2.4367319942909468E-4</v>
+      </c>
+      <c r="X144" s="25">
+        <f t="shared" ref="X144:AE144" si="313">X23/X118</f>
+        <v>8.996584558062512E-2</v>
+      </c>
+      <c r="Y144" s="25">
+        <f t="shared" si="313"/>
+        <v>2.1021411660639529E-2</v>
+      </c>
+      <c r="Z144" s="25">
+        <f t="shared" si="313"/>
+        <v>4.2575865218715155E-2</v>
+      </c>
+      <c r="AA144" s="25">
+        <f t="shared" si="313"/>
+        <v>6.2840746054519475E-2</v>
+      </c>
+      <c r="AB144" s="25">
+        <f t="shared" si="313"/>
+        <v>-4.3450673840765466E-2</v>
+      </c>
+      <c r="AC144" s="25">
+        <f t="shared" si="313"/>
+        <v>-8.7561555912134131E-2</v>
+      </c>
+      <c r="AD144" s="25">
+        <f t="shared" si="313"/>
+        <v>-0.25049011177987962</v>
+      </c>
+      <c r="AE144" s="25">
+        <f>AE23/AE118</f>
+        <v>-1.5675675675675727E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="2:31">
+      <c r="B145" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C145" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D145" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E145" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F145" s="25">
+        <f t="shared" ref="F145:T145" si="314">F143/F87</f>
+        <v>-1.473426957337917E-2</v>
+      </c>
+      <c r="G145" s="25">
+        <f t="shared" si="314"/>
+        <v>-1.5439493634673172E-2</v>
+      </c>
+      <c r="H145" s="25">
+        <f t="shared" si="314"/>
+        <v>-3.4417300903010688E-3</v>
+      </c>
+      <c r="I145" s="25">
+        <f t="shared" si="314"/>
+        <v>-9.355932203389844E-3</v>
+      </c>
+      <c r="J145" s="25">
+        <f t="shared" si="314"/>
+        <v>-2.9936155119413582E-2</v>
+      </c>
+      <c r="K145" s="25">
+        <f t="shared" si="314"/>
+        <v>-5.2127375392636413E-2</v>
+      </c>
+      <c r="L145" s="25">
+        <f t="shared" si="314"/>
+        <v>-8.5972456272880485E-2</v>
+      </c>
+      <c r="M145" s="25">
+        <f t="shared" si="314"/>
+        <v>-8.9755073343157368E-2</v>
+      </c>
+      <c r="N145" s="25">
+        <f t="shared" si="314"/>
+        <v>-6.9246861924686182E-2</v>
+      </c>
+      <c r="O145" s="25">
+        <f t="shared" si="314"/>
+        <v>-5.1183050222640428E-2</v>
+      </c>
+      <c r="P145" s="25">
+        <f t="shared" si="314"/>
+        <v>-1.2164814868536822E-2</v>
+      </c>
+      <c r="Q145" s="25">
+        <f t="shared" si="314"/>
+        <v>-5.0083311662669468E-3</v>
+      </c>
+      <c r="R145" s="25">
+        <f t="shared" si="314"/>
+        <v>-4.2836041358936486E-3</v>
+      </c>
+      <c r="S145" s="25">
+        <f t="shared" si="314"/>
+        <v>1.6010700822828448E-3</v>
+      </c>
+      <c r="T145" s="25">
+        <f>T143/T87</f>
+        <v>7.2173877180678044E-5</v>
+      </c>
+      <c r="X145" s="25">
+        <f t="shared" ref="X145:AE145" si="315">X143/X87</f>
+        <v>3.3397368168283544E-2</v>
+      </c>
+      <c r="Y145" s="25">
+        <f t="shared" si="315"/>
+        <v>6.9240327349072497E-3</v>
+      </c>
+      <c r="Z145" s="25">
+        <f t="shared" si="315"/>
+        <v>1.4385405414673471E-2</v>
+      </c>
+      <c r="AA145" s="25">
+        <f t="shared" si="315"/>
+        <v>2.2017057354937121E-2</v>
+      </c>
+      <c r="AB145" s="25">
+        <f t="shared" si="315"/>
+        <v>-1.5159296580303542E-2</v>
+      </c>
+      <c r="AC145" s="25">
+        <f t="shared" si="315"/>
+        <v>-2.9936155119413572E-2</v>
+      </c>
+      <c r="AD145" s="25">
+        <f t="shared" si="315"/>
+        <v>-6.9256371243818948E-2</v>
+      </c>
+      <c r="AE145" s="25">
+        <f>AE143/AE87</f>
+        <v>-4.2836041358936625E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="2:31">
+      <c r="B146" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C146" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D146" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E146" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F146" s="25">
+        <f t="shared" ref="F146:T146" si="316">F143/(F121-F85)</f>
+        <v>-8.1512687371411943E-2</v>
+      </c>
+      <c r="G146" s="25">
+        <f t="shared" si="316"/>
+        <v>-8.8970171552212735E-2</v>
+      </c>
+      <c r="H146" s="25">
+        <f t="shared" si="316"/>
+        <v>-2.0297133291483617E-2</v>
+      </c>
+      <c r="I146" s="25">
+        <f t="shared" si="316"/>
+        <v>-5.8800136348142303E-2</v>
+      </c>
+      <c r="J146" s="25">
+        <f t="shared" si="316"/>
+        <v>-0.20250815791157464</v>
+      </c>
+      <c r="K146" s="25">
+        <f t="shared" si="316"/>
+        <v>-0.46602981141398353</v>
+      </c>
+      <c r="L146" s="25">
+        <f t="shared" si="316"/>
+        <v>-0.88074213711677685</v>
+      </c>
+      <c r="M146" s="25">
+        <f t="shared" si="316"/>
+        <v>-1.3460927343637141</v>
+      </c>
+      <c r="N146" s="25">
+        <f t="shared" si="316"/>
+        <v>-0.87534559442240634</v>
+      </c>
+      <c r="O146" s="25">
+        <f t="shared" si="316"/>
+        <v>-0.73779890924346181</v>
+      </c>
+      <c r="P146" s="25">
+        <f t="shared" si="316"/>
+        <v>-0.15965277425250027</v>
+      </c>
+      <c r="Q146" s="25">
+        <f t="shared" si="316"/>
+        <v>-7.5111945688285109E-2</v>
+      </c>
+      <c r="R146" s="25">
+        <f t="shared" si="316"/>
+        <v>-7.7457264957264849E-2</v>
+      </c>
+      <c r="S146" s="25">
+        <f t="shared" si="316"/>
+        <v>2.9845107669059432E-2</v>
+      </c>
+      <c r="T146" s="25">
+        <f>T143/(T121-T85)</f>
+        <v>1.0913626442157166E-3</v>
+      </c>
+      <c r="X146" s="25">
+        <f t="shared" ref="X146:AE146" si="317">X143/(X121-X85)</f>
+        <v>0.1335304735204885</v>
+      </c>
+      <c r="Y146" s="25">
+        <f t="shared" si="317"/>
+        <v>3.3137841939055952E-2</v>
+      </c>
+      <c r="Z146" s="25">
+        <f t="shared" si="317"/>
+        <v>7.398262863189467E-2</v>
+      </c>
+      <c r="AA146" s="25">
+        <f t="shared" si="317"/>
+        <v>0.11475481420025348</v>
+      </c>
+      <c r="AB146" s="25">
+        <f t="shared" si="317"/>
+        <v>-8.3864014891740973E-2</v>
+      </c>
+      <c r="AC146" s="25">
+        <f t="shared" si="317"/>
+        <v>-0.20250815791157456</v>
+      </c>
+      <c r="AD146" s="25">
+        <f t="shared" si="317"/>
+        <v>-0.87546580117802619</v>
+      </c>
+      <c r="AE146" s="25">
+        <f>AE143/(AE121-AE85)</f>
+        <v>-7.7457264957265098E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:31">
+      <c r="B147" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C147" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D147" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="E147" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F147" s="25">
+        <f t="shared" ref="F147:T147" si="318">F143/(F63+F67+F69+F68+F70+F70+F77+F78+F79+F80+F81+F82+F83+F84+F86)</f>
+        <v>-2.7305546439120493E-2</v>
+      </c>
+      <c r="G147" s="25">
+        <f t="shared" si="318"/>
+        <v>-2.5833956619296966E-2</v>
+      </c>
+      <c r="H147" s="25">
+        <f t="shared" si="318"/>
+        <v>-5.7692593638945591E-3</v>
+      </c>
+      <c r="I147" s="25">
+        <f t="shared" si="318"/>
+        <v>-1.5152846099789202E-2</v>
+      </c>
+      <c r="J147" s="25">
+        <f t="shared" si="318"/>
+        <v>-5.7190871144359542E-2</v>
+      </c>
+      <c r="K147" s="25">
+        <f t="shared" si="318"/>
+        <v>-9.3356649124832977E-2</v>
+      </c>
+      <c r="L147" s="25">
+        <f t="shared" si="318"/>
+        <v>-0.14483129935391248</v>
+      </c>
+      <c r="M147" s="25">
+        <f t="shared" si="318"/>
+        <v>-0.16481262048352582</v>
+      </c>
+      <c r="N147" s="25">
+        <f t="shared" si="318"/>
+        <v>-0.13265808026524328</v>
+      </c>
+      <c r="O147" s="25">
+        <f t="shared" si="318"/>
+        <v>-9.4657145932756787E-2</v>
+      </c>
+      <c r="P147" s="25">
+        <f t="shared" si="318"/>
+        <v>-2.2775414139585379E-2</v>
+      </c>
+      <c r="Q147" s="25">
+        <f t="shared" si="318"/>
+        <v>-9.196540685849677E-3</v>
+      </c>
+      <c r="R147" s="25">
+        <f t="shared" si="318"/>
+        <v>-8.9263728145776901E-3</v>
+      </c>
+      <c r="S147" s="25">
+        <f t="shared" si="318"/>
+        <v>3.1154490781820023E-3</v>
+      </c>
+      <c r="T147" s="25">
+        <f>T143/(T63+T67+T69+T68+T70+T70+T77+T78+T79+T80+T81+T82+T83+T84+T86)</f>
+        <v>1.3257073595696376E-4</v>
+      </c>
+      <c r="X147" s="25">
+        <f t="shared" ref="X147:AE147" si="319">X143/(X63+X67+X69+X68+X70+X70+X77+X78+X79+X80+X81+X82+X83+X84+X86)</f>
+        <v>5.3721242834850053E-2</v>
+      </c>
+      <c r="Y147" s="25">
+        <f t="shared" si="319"/>
+        <v>1.2784001012594165E-2</v>
+      </c>
+      <c r="Z147" s="25">
+        <f t="shared" si="319"/>
+        <v>2.6713364642203318E-2</v>
+      </c>
+      <c r="AA147" s="25">
+        <f t="shared" si="319"/>
+        <v>4.6196846379665028E-2</v>
+      </c>
+      <c r="AB147" s="25">
+        <f t="shared" si="319"/>
+        <v>-2.8093206432556611E-2</v>
+      </c>
+      <c r="AC147" s="25">
+        <f t="shared" si="319"/>
+        <v>-5.7190871144359522E-2</v>
+      </c>
+      <c r="AD147" s="25">
+        <f t="shared" si="319"/>
+        <v>-0.13267629752427451</v>
+      </c>
+      <c r="AE147" s="25">
+        <f>AE143/(AE63+AE67+AE69+AE68+AE70+AE70+AE77+AE78+AE79+AE80+AE81+AE82+AE83+AE84+AE86)</f>
+        <v>-8.9263728145777196E-3</v>
       </c>
     </row>
   </sheetData>
@@ -18931,7 +19504,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U39" sqref="U39"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Q322 order/backlog data entry
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A35293-6C4A-4B90-A520-3AA4E2D23249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C8BC68-7BF1-40CE-9878-B4A37F2111CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="263">
   <si>
     <t>$ERJ</t>
   </si>
@@ -922,9 +922,6 @@
     <t>growth, product development &amp; new business</t>
   </si>
   <si>
-    <t>(Projected)</t>
-  </si>
-  <si>
     <t>FY15</t>
   </si>
   <si>
@@ -970,7 +967,7 @@
     <numFmt numFmtId="168" formatCode="0.0000\x"/>
     <numFmt numFmtId="169" formatCode="mmmm\ yyyy;"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1115,15 +1112,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1151,12 +1141,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF323232"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1254,7 +1238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1442,16 +1426,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1461,31 +1435,22 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1495,6 +1460,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1524,28 +1507,16 @@
     <xf numFmtId="169" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4956,6 +4927,789 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Commercial A/C Order &amp; Backlog Q/Q</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Firm Orders</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Order &amp; Backlog'!$B$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Q322</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Order &amp; Backlog'!$B$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1708</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1858</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1860</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1890</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1889</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1917</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1902</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1904</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1904</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E782-4B71-B90E-043B17166DDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Delivered</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Order &amp; Backlog'!$B$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Q322</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Order &amp; Backlog'!$B$12:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1414</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1442</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1457</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1490</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1579</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1584</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1588</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1646</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1655</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1671</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1677</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1688</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E782-4B71-B90E-043B17166DDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Firm Order Backlog</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Order &amp; Backlog'!$B$1:$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Q118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Q320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Q420</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Q121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Q221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q321</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Q421</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Q222</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Q322</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Order &amp; Backlog'!$B$21:$T$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>297</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E782-4B71-B90E-043B17166DDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
+        <c:axId val="912516495"/>
+        <c:axId val="847870127"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="912516495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="847870127"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="847870127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="912516495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5037,6 +5791,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6723,6 +7517,555 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -7010,6 +8353,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C969349-039C-4A3D-B56F-FBAB1264D415}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7017,16 +8398,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7041,8 +8422,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14147800" y="12700"/>
-          <a:ext cx="0" cy="10464800"/>
+          <a:off x="13173075" y="3175"/>
+          <a:ext cx="0" cy="9617075"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7067,13 +8448,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7417,8 +8798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -7438,35 +8819,35 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="115"/>
-      <c r="G5" s="113" t="s">
+      <c r="C5" s="103"/>
+      <c r="D5" s="104"/>
+      <c r="G5" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114"/>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="115"/>
-      <c r="T5" s="113" t="s">
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="104"/>
+      <c r="T5" s="102" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="114"/>
-      <c r="V5" s="114"/>
-      <c r="W5" s="115"/>
-      <c r="AA5" s="127" t="s">
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="104"/>
+      <c r="AA5" s="100" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="128"/>
+      <c r="AB5" s="101"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -7480,7 +8861,7 @@
         <v>44835</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
@@ -7695,13 +9076,13 @@
       <c r="U12" s="37"/>
       <c r="V12" s="37"/>
       <c r="W12" s="38"/>
-      <c r="Y12" s="113" t="s">
+      <c r="Y12" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="Z12" s="114"/>
-      <c r="AA12" s="114"/>
-      <c r="AB12" s="114"/>
-      <c r="AC12" s="115"/>
+      <c r="Z12" s="103"/>
+      <c r="AA12" s="103"/>
+      <c r="AB12" s="103"/>
+      <c r="AC12" s="104"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9">
@@ -7727,14 +9108,14 @@
       <c r="V13" s="37"/>
       <c r="W13" s="38"/>
       <c r="Y13" s="92"/>
-      <c r="Z13" s="125" t="s">
+      <c r="Z13" s="109" t="s">
         <v>220</v>
       </c>
-      <c r="AA13" s="125"/>
-      <c r="AB13" s="125" t="s">
+      <c r="AA13" s="109"/>
+      <c r="AB13" s="109" t="s">
         <v>221</v>
       </c>
-      <c r="AC13" s="126"/>
+      <c r="AC13" s="110"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="10"/>
@@ -7760,21 +9141,21 @@
       <c r="Y14" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="Z14" s="111" t="s">
+      <c r="Z14" s="98" t="s">
         <v>231</v>
       </c>
-      <c r="AA14" s="111"/>
-      <c r="AB14" s="111" t="s">
+      <c r="AA14" s="98"/>
+      <c r="AB14" s="98" t="s">
         <v>232</v>
       </c>
-      <c r="AC14" s="112"/>
+      <c r="AC14" s="99"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="113" t="s">
+      <c r="B15" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="115"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="104"/>
       <c r="G15" s="10"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
@@ -7796,14 +9177,14 @@
       <c r="Y15" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="Z15" s="111" t="s">
+      <c r="Z15" s="98" t="s">
         <v>227</v>
       </c>
-      <c r="AA15" s="111"/>
-      <c r="AB15" s="111" t="s">
+      <c r="AA15" s="98"/>
+      <c r="AB15" s="98" t="s">
         <v>233</v>
       </c>
-      <c r="AC15" s="112"/>
+      <c r="AC15" s="99"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="14" t="s">
@@ -7812,10 +9193,10 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="111" t="s">
+      <c r="C16" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="112"/>
+      <c r="D16" s="99"/>
       <c r="G16" s="10"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
@@ -7837,23 +9218,23 @@
       <c r="Y16" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="Z16" s="111" t="s">
+      <c r="Z16" s="98" t="s">
         <v>228</v>
       </c>
-      <c r="AA16" s="111"/>
-      <c r="AB16" s="111" t="s">
+      <c r="AA16" s="98"/>
+      <c r="AB16" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="AC16" s="112"/>
+      <c r="AC16" s="99"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="112"/>
+      <c r="D17" s="99"/>
       <c r="G17" s="9">
         <v>44805</v>
       </c>
@@ -7877,19 +9258,19 @@
       <c r="Y17" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="Z17" s="111" t="s">
+      <c r="Z17" s="98" t="s">
         <v>229</v>
       </c>
-      <c r="AA17" s="111"/>
-      <c r="AB17" s="111" t="s">
+      <c r="AA17" s="98"/>
+      <c r="AB17" s="98" t="s">
         <v>235</v>
       </c>
-      <c r="AC17" s="112"/>
+      <c r="AC17" s="99"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="16"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="112"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="99"/>
       <c r="G18" s="10"/>
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
@@ -7911,19 +9292,19 @@
       <c r="Y18" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="Z18" s="111" t="s">
+      <c r="Z18" s="98" t="s">
         <v>230</v>
       </c>
-      <c r="AA18" s="111"/>
-      <c r="AB18" s="111" t="s">
+      <c r="AA18" s="98"/>
+      <c r="AB18" s="98" t="s">
         <v>236</v>
       </c>
-      <c r="AC18" s="112"/>
+      <c r="AC18" s="99"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="17"/>
-      <c r="C19" s="131"/>
-      <c r="D19" s="132"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="108"/>
       <c r="G19" s="10"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
@@ -7945,14 +9326,14 @@
       <c r="Y19" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="Z19" s="111" t="s">
+      <c r="Z19" s="98" t="s">
         <v>238</v>
       </c>
-      <c r="AA19" s="111"/>
-      <c r="AB19" s="111" t="s">
+      <c r="AA19" s="98"/>
+      <c r="AB19" s="98" t="s">
         <v>239</v>
       </c>
-      <c r="AC19" s="112"/>
+      <c r="AC19" s="99"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9">
@@ -7980,14 +9361,14 @@
       <c r="Y20" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="Z20" s="111" t="s">
+      <c r="Z20" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="AA20" s="111"/>
-      <c r="AB20" s="111" t="s">
+      <c r="AA20" s="98"/>
+      <c r="AB20" s="98" t="s">
         <v>245</v>
       </c>
-      <c r="AC20" s="112"/>
+      <c r="AC20" s="99"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="10"/>
@@ -8017,11 +9398,11 @@
       <c r="AC21" s="38"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="113" t="s">
+      <c r="B22" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="114"/>
-      <c r="D22" s="115"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="104"/>
       <c r="G22" s="10"/>
       <c r="H22" s="8" t="s">
         <v>193</v>
@@ -8052,10 +9433,10 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="111" t="s">
+      <c r="C23" s="98" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="112"/>
+      <c r="D23" s="99"/>
       <c r="G23" s="10"/>
       <c r="H23" s="8" t="s">
         <v>191</v>
@@ -8081,10 +9462,10 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="111">
+      <c r="C24" s="98">
         <v>1969</v>
       </c>
-      <c r="D24" s="112"/>
+      <c r="D24" s="99"/>
       <c r="G24" s="10"/>
       <c r="H24" s="60"/>
       <c r="I24" s="60"/>
@@ -8106,8 +9487,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="10"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="112"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="99"/>
       <c r="G25" s="10"/>
       <c r="H25" s="60"/>
       <c r="I25" s="60"/>
@@ -8131,11 +9512,11 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="129">
+      <c r="C26" s="105">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="130"/>
+      <c r="D26" s="106"/>
       <c r="G26" s="9">
         <v>44743</v>
       </c>
@@ -8161,8 +9542,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="10"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="112"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="99"/>
       <c r="G27" s="10"/>
       <c r="H27" s="8" t="s">
         <v>197</v>
@@ -8186,10 +9567,10 @@
     </row>
     <row r="28" spans="2:29">
       <c r="B28" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="C28" s="111"/>
-      <c r="D28" s="112"/>
+        <v>260</v>
+      </c>
+      <c r="C28" s="98"/>
+      <c r="D28" s="99"/>
       <c r="G28" s="10"/>
       <c r="H28" s="50" t="s">
         <v>198</v>
@@ -8213,13 +9594,13 @@
     </row>
     <row r="29" spans="2:29">
       <c r="B29" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="C29" s="122">
+        <v>261</v>
+      </c>
+      <c r="C29" s="117">
         <f>'Order &amp; Backlog'!S21</f>
         <v>312</v>
       </c>
-      <c r="D29" s="112"/>
+      <c r="D29" s="99"/>
       <c r="G29" s="10"/>
       <c r="H29" s="60"/>
       <c r="I29" s="60"/>
@@ -8241,11 +9622,11 @@
       <c r="B30" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="111">
+      <c r="C30" s="98">
         <f>'Financial Model'!T43</f>
         <v>32</v>
       </c>
-      <c r="D30" s="112"/>
+      <c r="D30" s="99"/>
       <c r="G30" s="9">
         <v>44743</v>
       </c>
@@ -8269,12 +9650,12 @@
     </row>
     <row r="31" spans="2:29">
       <c r="B31" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C31" s="123">
+        <v>262</v>
+      </c>
+      <c r="C31" s="118">
         <v>36708</v>
       </c>
-      <c r="D31" s="124"/>
+      <c r="D31" s="119"/>
       <c r="G31" s="10"/>
       <c r="H31" s="8" t="s">
         <v>242</v>
@@ -8298,8 +9679,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="10"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="112"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="99"/>
       <c r="G32" s="10"/>
       <c r="H32" s="60"/>
       <c r="I32" s="60"/>
@@ -8354,10 +9735,10 @@
       <c r="B34" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="118" t="s">
+      <c r="C34" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="119"/>
+      <c r="D34" s="114"/>
       <c r="G34" s="10"/>
       <c r="H34" s="8" t="s">
         <v>251</v>
@@ -8412,11 +9793,11 @@
       <c r="R36" s="38"/>
     </row>
     <row r="37" spans="2:23">
-      <c r="B37" s="113" t="s">
+      <c r="B37" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="114"/>
-      <c r="D37" s="115"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="104"/>
       <c r="G37" s="10"/>
       <c r="H37" s="8" t="s">
         <v>169</v>
@@ -8431,22 +9812,22 @@
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
       <c r="R37" s="38"/>
-      <c r="T37" s="113" t="s">
+      <c r="T37" s="102" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="114"/>
-      <c r="V37" s="114"/>
-      <c r="W37" s="115"/>
+      <c r="U37" s="103"/>
+      <c r="V37" s="103"/>
+      <c r="W37" s="104"/>
     </row>
     <row r="38" spans="2:23">
       <c r="B38" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="120">
+      <c r="C38" s="115">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D38" s="121"/>
+      <c r="D38" s="116"/>
       <c r="G38" s="10"/>
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
@@ -8472,11 +9853,11 @@
       <c r="B39" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="120">
+      <c r="C39" s="115">
         <f>C6/'Financial Model'!AE9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D39" s="121"/>
+      <c r="D39" s="116"/>
       <c r="G39" s="10"/>
       <c r="H39" s="37"/>
       <c r="I39" s="37"/>
@@ -8500,11 +9881,11 @@
       <c r="B40" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="116">
+      <c r="C40" s="111">
         <f>C6/'Financial Model'!AE26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D40" s="117"/>
+      <c r="D40" s="112"/>
       <c r="G40" s="9">
         <v>43770</v>
       </c>
@@ -8569,11 +9950,11 @@
       <c r="W42" s="38"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="113" t="s">
+      <c r="B43" s="102" t="s">
         <v>247</v>
       </c>
-      <c r="C43" s="114"/>
-      <c r="D43" s="115"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="104"/>
       <c r="G43" s="9">
         <v>43739</v>
       </c>
@@ -8600,10 +9981,10 @@
       <c r="W43" s="38"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="107" t="s">
+      <c r="B44" s="120" t="s">
         <v>248</v>
       </c>
-      <c r="C44" s="108"/>
+      <c r="C44" s="121"/>
       <c r="D44" s="51" t="s">
         <v>31</v>
       </c>
@@ -8627,10 +10008,10 @@
       </c>
     </row>
     <row r="45" spans="2:23">
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="120" t="s">
         <v>249</v>
       </c>
-      <c r="C45" s="108"/>
+      <c r="C45" s="121"/>
       <c r="D45" s="51" t="s">
         <v>31</v>
       </c>
@@ -8648,8 +10029,8 @@
       <c r="R45" s="38"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="B46" s="107"/>
-      <c r="C46" s="108"/>
+      <c r="B46" s="120"/>
+      <c r="C46" s="121"/>
       <c r="D46" s="89" t="s">
         <v>31</v>
       </c>
@@ -8667,8 +10048,8 @@
       <c r="R46" s="38"/>
     </row>
     <row r="47" spans="2:23">
-      <c r="B47" s="107"/>
-      <c r="C47" s="108"/>
+      <c r="B47" s="120"/>
+      <c r="C47" s="121"/>
       <c r="D47" s="89" t="s">
         <v>31</v>
       </c>
@@ -8690,8 +10071,8 @@
       <c r="R47" s="38"/>
     </row>
     <row r="48" spans="2:23">
-      <c r="B48" s="109"/>
-      <c r="C48" s="110"/>
+      <c r="B48" s="122"/>
+      <c r="C48" s="123"/>
       <c r="D48" s="90" t="s">
         <v>31</v>
       </c>
@@ -8834,6 +10215,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="T5:W5"/>
@@ -8850,39 +10264,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H9" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -8917,7 +10298,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M33" sqref="M33"/>
+      <selection pane="bottomRight" activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -8994,10 +10375,10 @@
         <v>76</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y1" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>218</v>
@@ -9660,6 +11041,10 @@
       <c r="T9" s="26">
         <v>1018.9</v>
       </c>
+      <c r="U9" s="26">
+        <f>T9*1.2</f>
+        <v>1222.6799999999998</v>
+      </c>
       <c r="X9" s="26">
         <v>6288.8</v>
       </c>
@@ -11490,6 +12875,10 @@
       <c r="T31" s="25">
         <f>T9/S9-1</f>
         <v>0.69562323181893837</v>
+      </c>
+      <c r="U31" s="25">
+        <f>U9/T9-1</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="X31" s="63" t="s">
         <v>186</v>
@@ -20107,7 +21496,7 @@
     </row>
     <row r="143" spans="2:31" s="2" customFormat="1">
       <c r="B143" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C143" s="14" t="s">
         <v>186</v>
@@ -20213,7 +21602,7 @@
     </row>
     <row r="144" spans="2:31">
       <c r="B144" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C144" s="14" t="s">
         <v>186</v>
@@ -20319,7 +21708,7 @@
     </row>
     <row r="145" spans="2:31">
       <c r="B145" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C145" s="14" t="s">
         <v>186</v>
@@ -20425,7 +21814,7 @@
     </row>
     <row r="146" spans="2:31">
       <c r="B146" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C146" s="14" t="s">
         <v>186</v>
@@ -20531,7 +21920,7 @@
     </row>
     <row r="147" spans="2:31">
       <c r="B147" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C147" s="14" t="s">
         <v>186</v>
@@ -20671,8 +22060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -20687,24 +22076,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258CA0E5-563F-4C1F-B583-AD76D8E7BBD2}">
-  <dimension ref="A1:AH49"/>
+  <dimension ref="A1:AI49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F54" sqref="F54"/>
+      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="19" width="9.140625" style="3"/>
-    <col min="20" max="20" width="9.140625" style="100"/>
-    <col min="21" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1">
+    <row r="1" spans="1:35" s="2" customFormat="1">
       <c r="B1" s="24" t="s">
         <v>32</v>
       </c>
@@ -20759,66 +22146,62 @@
       <c r="S1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="96" t="s">
+      <c r="T1" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="U1" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="W1" s="80">
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="X1" s="80">
         <v>2014</v>
       </c>
-      <c r="X1" s="80">
+      <c r="Y1" s="80">
         <v>2015</v>
       </c>
-      <c r="Y1" s="80">
+      <c r="Z1" s="80">
         <v>2016</v>
       </c>
-      <c r="Z1" s="80">
+      <c r="AA1" s="80">
         <v>2017</v>
       </c>
-      <c r="AA1" s="80">
+      <c r="AB1" s="80">
         <v>2018</v>
       </c>
-      <c r="AB1" s="80">
-        <f>AA1+1</f>
+      <c r="AC1" s="80">
+        <f>AB1+1</f>
         <v>2019</v>
       </c>
-      <c r="AC1" s="80">
-        <f t="shared" ref="AC1:AH1" si="0">AB1+1</f>
+      <c r="AD1" s="80">
+        <f t="shared" ref="AD1:AI1" si="0">AC1+1</f>
         <v>2020</v>
       </c>
-      <c r="AD1" s="80">
+      <c r="AE1" s="80">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="AE1" s="2">
+      <c r="AF1" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="AF1" s="2">
+      <c r="AG1" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="AG1" s="2">
+      <c r="AH1" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="AH1" s="2">
+      <c r="AI1" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="103" customFormat="1">
-      <c r="A2" s="101"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="T2" s="104" t="s">
-        <v>252</v>
-      </c>
+    <row r="2" spans="1:35" s="95" customFormat="1">
+      <c r="A2" s="93"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
     </row>
-    <row r="3" spans="1:34" s="77" customFormat="1">
+    <row r="3" spans="1:35" s="77" customFormat="1">
       <c r="A3" s="77" t="s">
         <v>210</v>
       </c>
@@ -20891,44 +22274,47 @@
         <v>1992</v>
       </c>
       <c r="S3" s="77">
-        <f t="shared" ref="S3" si="14">SUM(S4:S10)</f>
+        <f t="shared" ref="S3:T3" si="14">SUM(S4:S10)</f>
         <v>2000</v>
       </c>
-      <c r="T3" s="97"/>
-      <c r="W3" s="77">
-        <f t="shared" ref="W3:AA3" si="15">SUM(W4:W10)</f>
+      <c r="T3" s="77">
+        <f t="shared" si="14"/>
+        <v>1995</v>
+      </c>
+      <c r="X3" s="77">
+        <f t="shared" ref="X3:AB3" si="15">SUM(X4:X10)</f>
         <v>1549</v>
       </c>
-      <c r="X3" s="77">
+      <c r="Y3" s="77">
         <f t="shared" si="15"/>
         <v>1704</v>
       </c>
-      <c r="Y3" s="77">
+      <c r="Z3" s="77">
         <f t="shared" si="15"/>
         <v>1749</v>
       </c>
-      <c r="Z3" s="77">
+      <c r="AA3" s="77">
         <f t="shared" si="15"/>
         <v>1835</v>
       </c>
-      <c r="AA3" s="77">
+      <c r="AB3" s="77">
         <f t="shared" si="15"/>
         <v>1858</v>
       </c>
-      <c r="AB3" s="77">
-        <f t="shared" ref="AB3" si="16">SUM(AB4:AB10)</f>
+      <c r="AC3" s="77">
+        <f t="shared" ref="AC3" si="16">SUM(AC4:AC10)</f>
         <v>1917</v>
       </c>
-      <c r="AC3" s="77">
-        <f t="shared" ref="AC3" si="17">SUM(AC4:AC10)</f>
+      <c r="AD3" s="77">
+        <f t="shared" ref="AD3" si="17">SUM(AD4:AD10)</f>
         <v>1904</v>
       </c>
-      <c r="AD3" s="77">
-        <f t="shared" ref="AD3" si="18">SUM(AD4:AD10)</f>
+      <c r="AE3" s="77">
+        <f t="shared" ref="AE3" si="18">SUM(AE4:AE10)</f>
         <v>1996</v>
       </c>
     </row>
-    <row r="4" spans="1:34" s="78" customFormat="1">
+    <row r="4" spans="1:35" s="78" customFormat="1">
       <c r="A4" s="79" t="s">
         <v>201</v>
       </c>
@@ -20986,9 +22372,8 @@
       <c r="S4" s="78">
         <v>191</v>
       </c>
-      <c r="T4" s="98"/>
-      <c r="W4" s="78">
-        <v>193</v>
+      <c r="T4" s="78">
+        <v>191</v>
       </c>
       <c r="X4" s="78">
         <v>193</v>
@@ -20997,7 +22382,7 @@
         <v>193</v>
       </c>
       <c r="Z4" s="78">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AA4" s="78">
         <v>191</v>
@@ -21011,8 +22396,11 @@
       <c r="AD4" s="78">
         <v>191</v>
       </c>
+      <c r="AE4" s="78">
+        <v>191</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" s="78" customFormat="1">
+    <row r="5" spans="1:35" s="78" customFormat="1">
       <c r="A5" s="79" t="s">
         <v>85</v>
       </c>
@@ -21070,33 +22458,35 @@
       <c r="S5" s="78">
         <v>848</v>
       </c>
-      <c r="T5" s="98"/>
-      <c r="W5" s="78">
+      <c r="T5" s="78">
+        <v>817</v>
+      </c>
+      <c r="X5" s="78">
         <v>421</v>
       </c>
-      <c r="X5" s="78">
+      <c r="Y5" s="78">
         <v>500</v>
       </c>
-      <c r="Y5" s="78">
+      <c r="Z5" s="78">
         <v>525</v>
       </c>
-      <c r="Z5" s="78">
+      <c r="AA5" s="78">
         <v>603</v>
       </c>
-      <c r="AA5" s="78">
+      <c r="AB5" s="78">
         <v>771</v>
       </c>
-      <c r="AB5" s="78">
+      <c r="AC5" s="78">
         <v>815</v>
       </c>
-      <c r="AC5" s="78">
+      <c r="AD5" s="78">
         <v>798</v>
       </c>
-      <c r="AD5" s="78">
+      <c r="AE5" s="78">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="78" customFormat="1">
+    <row r="6" spans="1:35" s="78" customFormat="1">
       <c r="A6" s="79" t="s">
         <v>185</v>
       </c>
@@ -21154,24 +22544,23 @@
       <c r="S6" s="78">
         <v>568</v>
       </c>
-      <c r="T6" s="98"/>
-      <c r="W6" s="78">
+      <c r="T6" s="78">
+        <v>568</v>
+      </c>
+      <c r="X6" s="78">
         <v>580</v>
       </c>
-      <c r="X6" s="78">
+      <c r="Y6" s="78">
         <v>578</v>
       </c>
-      <c r="Y6" s="78">
+      <c r="Z6" s="78">
         <v>590</v>
       </c>
-      <c r="Z6" s="78">
+      <c r="AA6" s="78">
         <v>592</v>
       </c>
-      <c r="AA6" s="78">
+      <c r="AB6" s="78">
         <v>566</v>
-      </c>
-      <c r="AB6" s="78">
-        <v>568</v>
       </c>
       <c r="AC6" s="78">
         <v>568</v>
@@ -21179,8 +22568,11 @@
       <c r="AD6" s="78">
         <v>568</v>
       </c>
+      <c r="AE6" s="78">
+        <v>568</v>
+      </c>
     </row>
-    <row r="7" spans="1:34" s="78" customFormat="1">
+    <row r="7" spans="1:35" s="78" customFormat="1">
       <c r="A7" s="79" t="s">
         <v>188</v>
       </c>
@@ -21238,21 +22630,20 @@
       <c r="S7" s="78">
         <v>172</v>
       </c>
-      <c r="T7" s="98"/>
-      <c r="W7" s="78">
+      <c r="T7" s="78">
+        <v>172</v>
+      </c>
+      <c r="X7" s="78">
         <v>145</v>
-      </c>
-      <c r="X7" s="78">
-        <v>166</v>
       </c>
       <c r="Y7" s="78">
         <v>166</v>
       </c>
       <c r="Z7" s="78">
+        <v>166</v>
+      </c>
+      <c r="AA7" s="78">
         <v>169</v>
-      </c>
-      <c r="AA7" s="78">
-        <v>172</v>
       </c>
       <c r="AB7" s="78">
         <v>172</v>
@@ -21263,8 +22654,11 @@
       <c r="AD7" s="78">
         <v>172</v>
       </c>
+      <c r="AE7" s="78">
+        <v>172</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" s="78" customFormat="1">
+    <row r="8" spans="1:35" s="78" customFormat="1">
       <c r="A8" s="79" t="s">
         <v>217</v>
       </c>
@@ -21322,9 +22716,8 @@
       <c r="S8" s="78">
         <v>0</v>
       </c>
-      <c r="T8" s="98"/>
-      <c r="W8" s="78">
-        <v>100</v>
+      <c r="T8" s="78">
+        <v>0</v>
       </c>
       <c r="X8" s="78">
         <v>100</v>
@@ -21336,7 +22729,7 @@
         <v>100</v>
       </c>
       <c r="AA8" s="78">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AB8" s="78">
         <v>0</v>
@@ -21347,8 +22740,11 @@
       <c r="AD8" s="78">
         <v>0</v>
       </c>
+      <c r="AE8" s="78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" s="78" customFormat="1">
+    <row r="9" spans="1:35" s="78" customFormat="1">
       <c r="A9" s="79" t="s">
         <v>180</v>
       </c>
@@ -21406,33 +22802,35 @@
       <c r="S9" s="78">
         <v>20</v>
       </c>
-      <c r="T9" s="98"/>
-      <c r="W9" s="78">
+      <c r="T9" s="78">
+        <v>20</v>
+      </c>
+      <c r="X9" s="78">
         <v>60</v>
       </c>
-      <c r="X9" s="78">
+      <c r="Y9" s="78">
         <v>77</v>
       </c>
-      <c r="Y9" s="78">
+      <c r="Z9" s="78">
         <v>85</v>
       </c>
-      <c r="Z9" s="78">
+      <c r="AA9" s="78">
         <v>74</v>
       </c>
-      <c r="AA9" s="78">
+      <c r="AB9" s="78">
         <v>47</v>
       </c>
-      <c r="AB9" s="78">
+      <c r="AC9" s="78">
         <v>27</v>
-      </c>
-      <c r="AC9" s="78">
-        <v>22</v>
       </c>
       <c r="AD9" s="78">
         <v>22</v>
       </c>
+      <c r="AE9" s="78">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:34" s="78" customFormat="1">
+    <row r="10" spans="1:35" s="78" customFormat="1">
       <c r="A10" s="79" t="s">
         <v>86</v>
       </c>
@@ -21490,39 +22888,36 @@
       <c r="S10" s="78">
         <v>201</v>
       </c>
-      <c r="T10" s="98">
-        <f>S10+6</f>
-        <v>207</v>
-      </c>
-      <c r="W10" s="78">
+      <c r="T10" s="78">
+        <v>227</v>
+      </c>
+      <c r="X10" s="78">
         <v>50</v>
-      </c>
-      <c r="X10" s="78">
-        <v>90</v>
       </c>
       <c r="Y10" s="78">
         <v>90</v>
       </c>
       <c r="Z10" s="78">
+        <v>90</v>
+      </c>
+      <c r="AA10" s="78">
         <v>106</v>
       </c>
-      <c r="AA10" s="78">
+      <c r="AB10" s="78">
         <v>111</v>
       </c>
-      <c r="AB10" s="78">
+      <c r="AC10" s="78">
         <v>144</v>
       </c>
-      <c r="AC10" s="78">
+      <c r="AD10" s="78">
         <v>153</v>
       </c>
-      <c r="AD10" s="78">
+      <c r="AE10" s="78">
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:34" s="78" customFormat="1">
-      <c r="T11" s="98"/>
-    </row>
-    <row r="12" spans="1:34" s="77" customFormat="1">
+    <row r="11" spans="1:35" s="78" customFormat="1"/>
+    <row r="12" spans="1:35" s="77" customFormat="1">
       <c r="A12" s="77" t="s">
         <v>212</v>
       </c>
@@ -21598,41 +22993,44 @@
         <f t="shared" si="19"/>
         <v>1688</v>
       </c>
-      <c r="T12" s="97"/>
-      <c r="W12" s="77">
-        <f t="shared" ref="W12:AD12" si="20">SUM(W13:W19)</f>
+      <c r="T12" s="77">
+        <f>SUM(T13:T19)</f>
+        <v>1698</v>
+      </c>
+      <c r="X12" s="77">
+        <f t="shared" ref="X12:AE12" si="20">SUM(X13:X19)</f>
         <v>1090</v>
       </c>
-      <c r="X12" s="77">
+      <c r="Y12" s="77">
         <f t="shared" si="20"/>
         <v>1181</v>
       </c>
-      <c r="Y12" s="77">
+      <c r="Z12" s="77">
         <f t="shared" si="20"/>
         <v>1299</v>
       </c>
-      <c r="Z12" s="77">
+      <c r="AA12" s="77">
         <f t="shared" si="20"/>
         <v>1400</v>
       </c>
-      <c r="AA12" s="77">
+      <c r="AB12" s="77">
         <f t="shared" si="20"/>
         <v>1490</v>
       </c>
-      <c r="AB12" s="77">
+      <c r="AC12" s="77">
         <f t="shared" si="20"/>
         <v>1579</v>
       </c>
-      <c r="AC12" s="77">
+      <c r="AD12" s="77">
         <f t="shared" si="20"/>
         <v>1623</v>
       </c>
-      <c r="AD12" s="77">
+      <c r="AE12" s="77">
         <f t="shared" si="20"/>
         <v>1671</v>
       </c>
     </row>
-    <row r="13" spans="1:34" s="78" customFormat="1">
+    <row r="13" spans="1:35" s="78" customFormat="1">
       <c r="A13" s="79" t="s">
         <v>201</v>
       </c>
@@ -21690,12 +23088,11 @@
       <c r="S13" s="78">
         <v>191</v>
       </c>
-      <c r="T13" s="98"/>
-      <c r="W13" s="78">
+      <c r="T13" s="78">
+        <v>191</v>
+      </c>
+      <c r="X13" s="78">
         <v>188</v>
-      </c>
-      <c r="X13" s="78">
-        <v>190</v>
       </c>
       <c r="Y13" s="78">
         <v>190</v>
@@ -21704,7 +23101,7 @@
         <v>190</v>
       </c>
       <c r="AA13" s="78">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AB13" s="78">
         <v>191</v>
@@ -21715,8 +23112,11 @@
       <c r="AD13" s="78">
         <v>191</v>
       </c>
+      <c r="AE13" s="78">
+        <v>191</v>
+      </c>
     </row>
-    <row r="14" spans="1:34" s="78" customFormat="1">
+    <row r="14" spans="1:35" s="78" customFormat="1">
       <c r="A14" s="79" t="s">
         <v>85</v>
       </c>
@@ -21774,33 +23174,35 @@
       <c r="S14" s="78">
         <v>705</v>
       </c>
-      <c r="T14" s="98"/>
-      <c r="W14" s="78">
+      <c r="T14" s="78">
+        <v>714</v>
+      </c>
+      <c r="X14" s="78">
         <v>249</v>
       </c>
-      <c r="X14" s="78">
+      <c r="Y14" s="78">
         <v>331</v>
       </c>
-      <c r="Y14" s="78">
+      <c r="Z14" s="78">
         <v>421</v>
       </c>
-      <c r="Z14" s="78">
+      <c r="AA14" s="78">
         <v>500</v>
       </c>
-      <c r="AA14" s="78">
+      <c r="AB14" s="78">
         <v>567</v>
       </c>
-      <c r="AB14" s="78">
+      <c r="AC14" s="78">
         <v>634</v>
       </c>
-      <c r="AC14" s="78">
+      <c r="AD14" s="78">
         <v>666</v>
       </c>
-      <c r="AD14" s="78">
+      <c r="AE14" s="78">
         <v>693</v>
       </c>
     </row>
-    <row r="15" spans="1:34" s="78" customFormat="1">
+    <row r="15" spans="1:35" s="78" customFormat="1">
       <c r="A15" s="79" t="s">
         <v>185</v>
       </c>
@@ -21858,33 +23260,35 @@
       <c r="S15" s="78">
         <v>565</v>
       </c>
-      <c r="T15" s="98"/>
-      <c r="W15" s="78">
+      <c r="T15" s="78">
+        <v>565</v>
+      </c>
+      <c r="X15" s="78">
         <v>515</v>
       </c>
-      <c r="X15" s="78">
+      <c r="Y15" s="78">
         <v>523</v>
       </c>
-      <c r="Y15" s="78">
+      <c r="Z15" s="78">
         <v>534</v>
       </c>
-      <c r="Z15" s="78">
+      <c r="AA15" s="78">
         <v>546</v>
       </c>
-      <c r="AA15" s="78">
+      <c r="AB15" s="78">
         <v>559</v>
       </c>
-      <c r="AB15" s="78">
+      <c r="AC15" s="78">
         <v>564</v>
-      </c>
-      <c r="AC15" s="78">
-        <v>565</v>
       </c>
       <c r="AD15" s="78">
         <v>565</v>
       </c>
+      <c r="AE15" s="78">
+        <v>565</v>
+      </c>
     </row>
-    <row r="16" spans="1:34" s="78" customFormat="1">
+    <row r="16" spans="1:35" s="78" customFormat="1">
       <c r="A16" s="79" t="s">
         <v>188</v>
       </c>
@@ -21942,24 +23346,23 @@
       <c r="S16" s="78">
         <v>172</v>
       </c>
-      <c r="T16" s="98"/>
-      <c r="W16" s="78">
+      <c r="T16" s="78">
+        <v>172</v>
+      </c>
+      <c r="X16" s="78">
         <v>138</v>
       </c>
-      <c r="X16" s="78">
+      <c r="Y16" s="78">
         <v>137</v>
       </c>
-      <c r="Y16" s="78">
+      <c r="Z16" s="78">
         <v>154</v>
       </c>
-      <c r="Z16" s="78">
+      <c r="AA16" s="78">
         <v>164</v>
       </c>
-      <c r="AA16" s="78">
+      <c r="AB16" s="78">
         <v>169</v>
-      </c>
-      <c r="AB16" s="78">
-        <v>172</v>
       </c>
       <c r="AC16" s="78">
         <v>172</v>
@@ -21967,8 +23370,11 @@
       <c r="AD16" s="78">
         <v>172</v>
       </c>
+      <c r="AE16" s="78">
+        <v>172</v>
+      </c>
     </row>
-    <row r="17" spans="1:30" s="78" customFormat="1">
+    <row r="17" spans="1:31" s="78" customFormat="1">
       <c r="A17" s="79" t="s">
         <v>217</v>
       </c>
@@ -22026,8 +23432,7 @@
       <c r="S17" s="78">
         <v>0</v>
       </c>
-      <c r="T17" s="98"/>
-      <c r="W17" s="78">
+      <c r="T17" s="78">
         <v>0</v>
       </c>
       <c r="X17" s="78">
@@ -22051,8 +23456,11 @@
       <c r="AD17" s="78">
         <v>0</v>
       </c>
+      <c r="AE17" s="78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:30" s="78" customFormat="1">
+    <row r="18" spans="1:31" s="78" customFormat="1">
       <c r="A18" s="79" t="s">
         <v>180</v>
       </c>
@@ -22110,9 +23518,8 @@
       <c r="S18" s="78">
         <v>17</v>
       </c>
-      <c r="T18" s="98"/>
-      <c r="W18" s="78">
-        <v>0</v>
+      <c r="T18" s="78">
+        <v>17</v>
       </c>
       <c r="X18" s="78">
         <v>0</v>
@@ -22124,19 +23531,22 @@
         <v>0</v>
       </c>
       <c r="AA18" s="78">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="78">
         <v>4</v>
       </c>
-      <c r="AB18" s="78">
+      <c r="AC18" s="78">
         <v>11</v>
       </c>
-      <c r="AC18" s="78">
+      <c r="AD18" s="78">
         <v>15</v>
       </c>
-      <c r="AD18" s="78">
+      <c r="AE18" s="78">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="78" customFormat="1">
+    <row r="19" spans="1:31" s="78" customFormat="1">
       <c r="A19" s="79" t="s">
         <v>86</v>
       </c>
@@ -22194,9 +23604,8 @@
       <c r="S19" s="78">
         <v>38</v>
       </c>
-      <c r="T19" s="98"/>
-      <c r="W19" s="78">
-        <v>0</v>
+      <c r="T19" s="78">
+        <v>39</v>
       </c>
       <c r="X19" s="78">
         <v>0</v>
@@ -22211,25 +23620,27 @@
         <v>0</v>
       </c>
       <c r="AB19" s="78">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="78">
         <v>7</v>
       </c>
-      <c r="AC19" s="78">
+      <c r="AD19" s="78">
         <v>14</v>
       </c>
-      <c r="AD19" s="78">
+      <c r="AE19" s="78">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="78" customFormat="1">
+    <row r="20" spans="1:31" s="78" customFormat="1">
       <c r="A20" s="79"/>
-      <c r="T20" s="98"/>
     </row>
-    <row r="21" spans="1:30" s="77" customFormat="1">
+    <row r="21" spans="1:31" s="77" customFormat="1">
       <c r="A21" s="77" t="s">
         <v>211</v>
       </c>
       <c r="B21" s="77">
-        <f t="shared" ref="B21:S21" si="21">SUM(B22:B28)</f>
+        <f t="shared" ref="B21:T21" si="21">SUM(B22:B28)</f>
         <v>421</v>
       </c>
       <c r="C21" s="77">
@@ -22300,41 +23711,44 @@
         <f t="shared" si="21"/>
         <v>312</v>
       </c>
-      <c r="T21" s="97"/>
-      <c r="W21" s="77">
-        <f t="shared" ref="W21:AD21" si="22">SUM(W22:W28)</f>
+      <c r="T21" s="77">
+        <f t="shared" si="21"/>
+        <v>297</v>
+      </c>
+      <c r="X21" s="77">
+        <f t="shared" ref="X21:AE21" si="22">SUM(X22:X28)</f>
         <v>459</v>
       </c>
-      <c r="X21" s="77">
+      <c r="Y21" s="77">
         <f t="shared" si="22"/>
         <v>513</v>
       </c>
-      <c r="Y21" s="77">
+      <c r="Z21" s="77">
         <f t="shared" si="22"/>
         <v>450</v>
       </c>
-      <c r="Z21" s="77">
+      <c r="AA21" s="77">
         <f t="shared" si="22"/>
         <v>435</v>
       </c>
-      <c r="AA21" s="77">
+      <c r="AB21" s="77">
         <f t="shared" si="22"/>
         <v>368</v>
       </c>
-      <c r="AB21" s="77">
+      <c r="AC21" s="77">
         <f t="shared" si="22"/>
         <v>338</v>
       </c>
-      <c r="AC21" s="77">
+      <c r="AD21" s="77">
         <f t="shared" si="22"/>
         <v>281</v>
       </c>
-      <c r="AD21" s="77">
+      <c r="AE21" s="77">
         <f t="shared" si="22"/>
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="78" customFormat="1">
+    <row r="22" spans="1:31" s="78" customFormat="1">
       <c r="A22" s="79" t="s">
         <v>201</v>
       </c>
@@ -22392,22 +23806,21 @@
       <c r="S22" s="78">
         <v>0</v>
       </c>
-      <c r="T22" s="98"/>
-      <c r="W22" s="78">
+      <c r="T22" s="78">
+        <v>0</v>
+      </c>
+      <c r="X22" s="78">
         <v>5</v>
-      </c>
-      <c r="X22" s="78">
-        <v>3</v>
       </c>
       <c r="Y22" s="78">
         <v>3</v>
       </c>
       <c r="Z22" s="78">
+        <v>3</v>
+      </c>
+      <c r="AA22" s="78">
         <v>1</v>
       </c>
-      <c r="AA22" s="78">
-        <v>0</v>
-      </c>
       <c r="AB22" s="78">
         <v>0</v>
       </c>
@@ -22417,8 +23830,11 @@
       <c r="AD22" s="78">
         <v>0</v>
       </c>
+      <c r="AE22" s="78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:30" s="78" customFormat="1">
+    <row r="23" spans="1:31" s="78" customFormat="1">
       <c r="A23" s="79" t="s">
         <v>85</v>
       </c>
@@ -22476,33 +23892,35 @@
       <c r="S23" s="78">
         <v>143</v>
       </c>
-      <c r="T23" s="98"/>
-      <c r="W23" s="78">
+      <c r="T23" s="78">
+        <v>103</v>
+      </c>
+      <c r="X23" s="78">
         <v>172</v>
       </c>
-      <c r="X23" s="78">
+      <c r="Y23" s="78">
         <v>169</v>
       </c>
-      <c r="Y23" s="78">
+      <c r="Z23" s="78">
         <v>104</v>
       </c>
-      <c r="Z23" s="78">
+      <c r="AA23" s="78">
         <v>103</v>
       </c>
-      <c r="AA23" s="78">
+      <c r="AB23" s="78">
         <v>204</v>
       </c>
-      <c r="AB23" s="78">
+      <c r="AC23" s="78">
         <v>181</v>
       </c>
-      <c r="AC23" s="78">
+      <c r="AD23" s="78">
         <v>132</v>
       </c>
-      <c r="AD23" s="78">
+      <c r="AE23" s="78">
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="78" customFormat="1">
+    <row r="24" spans="1:31" s="78" customFormat="1">
       <c r="A24" s="79" t="s">
         <v>185</v>
       </c>
@@ -22560,33 +23978,35 @@
       <c r="S24" s="78">
         <v>3</v>
       </c>
-      <c r="T24" s="98"/>
-      <c r="W24" s="78">
+      <c r="T24" s="78">
+        <v>3</v>
+      </c>
+      <c r="X24" s="78">
         <v>65</v>
       </c>
-      <c r="X24" s="78">
+      <c r="Y24" s="78">
         <v>55</v>
       </c>
-      <c r="Y24" s="78">
+      <c r="Z24" s="78">
         <v>56</v>
       </c>
-      <c r="Z24" s="78">
+      <c r="AA24" s="78">
         <v>46</v>
       </c>
-      <c r="AA24" s="78">
+      <c r="AB24" s="78">
         <v>7</v>
       </c>
-      <c r="AB24" s="78">
+      <c r="AC24" s="78">
         <v>4</v>
-      </c>
-      <c r="AC24" s="78">
-        <v>3</v>
       </c>
       <c r="AD24" s="78">
         <v>3</v>
       </c>
+      <c r="AE24" s="78">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="1:30" s="78" customFormat="1">
+    <row r="25" spans="1:31" s="78" customFormat="1">
       <c r="A25" s="79" t="s">
         <v>188</v>
       </c>
@@ -22644,33 +24064,35 @@
       <c r="S25" s="78">
         <v>0</v>
       </c>
-      <c r="T25" s="98"/>
-      <c r="W25" s="78">
+      <c r="T25" s="78">
+        <v>0</v>
+      </c>
+      <c r="X25" s="78">
         <v>7</v>
       </c>
-      <c r="X25" s="78">
+      <c r="Y25" s="78">
         <v>19</v>
       </c>
-      <c r="Y25" s="78">
+      <c r="Z25" s="78">
         <v>12</v>
       </c>
-      <c r="Z25" s="78">
+      <c r="AA25" s="78">
         <v>5</v>
       </c>
-      <c r="AA25" s="78">
+      <c r="AB25" s="78">
         <v>3</v>
       </c>
-      <c r="AB25" s="78">
-        <v>0</v>
-      </c>
       <c r="AC25" s="78">
         <v>0</v>
       </c>
       <c r="AD25" s="78">
         <v>0</v>
       </c>
+      <c r="AE25" s="78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:30" s="78" customFormat="1">
+    <row r="26" spans="1:31" s="78" customFormat="1">
       <c r="A26" s="79" t="s">
         <v>217</v>
       </c>
@@ -22728,9 +24150,8 @@
       <c r="S26" s="78">
         <v>0</v>
       </c>
-      <c r="T26" s="98"/>
-      <c r="W26" s="78">
-        <v>100</v>
+      <c r="T26" s="78">
+        <v>0</v>
       </c>
       <c r="X26" s="78">
         <v>100</v>
@@ -22742,7 +24163,7 @@
         <v>100</v>
       </c>
       <c r="AA26" s="78">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AB26" s="78">
         <v>0</v>
@@ -22753,8 +24174,11 @@
       <c r="AD26" s="78">
         <v>0</v>
       </c>
+      <c r="AE26" s="78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:30" s="78" customFormat="1">
+    <row r="27" spans="1:31" s="78" customFormat="1">
       <c r="A27" s="79" t="s">
         <v>180</v>
       </c>
@@ -22812,33 +24236,35 @@
       <c r="S27" s="78">
         <v>3</v>
       </c>
-      <c r="T27" s="98"/>
-      <c r="W27" s="78">
+      <c r="T27" s="78">
+        <v>3</v>
+      </c>
+      <c r="X27" s="78">
         <v>60</v>
       </c>
-      <c r="X27" s="78">
+      <c r="Y27" s="78">
         <v>77</v>
       </c>
-      <c r="Y27" s="78">
+      <c r="Z27" s="78">
         <v>85</v>
       </c>
-      <c r="Z27" s="78">
+      <c r="AA27" s="78">
         <v>74</v>
       </c>
-      <c r="AA27" s="78">
+      <c r="AB27" s="78">
         <v>43</v>
       </c>
-      <c r="AB27" s="78">
+      <c r="AC27" s="78">
         <v>16</v>
       </c>
-      <c r="AC27" s="78">
+      <c r="AD27" s="78">
         <v>7</v>
       </c>
-      <c r="AD27" s="78">
+      <c r="AE27" s="78">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="78" customFormat="1">
+    <row r="28" spans="1:31" s="78" customFormat="1">
       <c r="A28" s="79" t="s">
         <v>86</v>
       </c>
@@ -22896,49 +24322,48 @@
       <c r="S28" s="78">
         <v>163</v>
       </c>
-      <c r="T28" s="98">
-        <f>S28+6</f>
-        <v>169</v>
-      </c>
-      <c r="W28" s="78">
+      <c r="T28" s="78">
+        <v>188</v>
+      </c>
+      <c r="X28" s="78">
         <v>50</v>
-      </c>
-      <c r="X28" s="78">
-        <v>90</v>
       </c>
       <c r="Y28" s="78">
         <v>90</v>
       </c>
       <c r="Z28" s="78">
+        <v>90</v>
+      </c>
+      <c r="AA28" s="78">
         <v>106</v>
       </c>
-      <c r="AA28" s="78">
+      <c r="AB28" s="78">
         <v>111</v>
       </c>
-      <c r="AB28" s="78">
+      <c r="AC28" s="78">
         <v>137</v>
       </c>
-      <c r="AC28" s="78">
+      <c r="AD28" s="78">
         <v>139</v>
       </c>
-      <c r="AD28" s="78">
+      <c r="AE28" s="78">
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="31" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B31" s="105" t="s">
+      <c r="B31" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="105" t="s">
+      <c r="C31" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="105" t="s">
+      <c r="D31" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="E31" s="105" t="s">
+      <c r="E31" s="96" t="s">
         <v>186</v>
       </c>
       <c r="F31" s="34">
@@ -22997,53 +24422,56 @@
         <f>S3/O3-1</f>
         <v>2.4590163934426146E-2</v>
       </c>
-      <c r="T31" s="99"/>
-      <c r="W31" s="63" t="s">
+      <c r="T31" s="34">
+        <f>T3/P3-1</f>
+        <v>1.3719512195121908E-2</v>
+      </c>
+      <c r="X31" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="X31" s="34">
-        <f t="shared" ref="X31" si="30">X3/W3-1</f>
+      <c r="Y31" s="34">
+        <f t="shared" ref="Y31" si="30">Y3/X3-1</f>
         <v>0.1000645577792123</v>
       </c>
-      <c r="Y31" s="34">
-        <f t="shared" ref="Y31" si="31">Y3/X3-1</f>
+      <c r="Z31" s="34">
+        <f t="shared" ref="Z31" si="31">Z3/Y3-1</f>
         <v>2.6408450704225261E-2</v>
       </c>
-      <c r="Z31" s="34">
-        <f t="shared" ref="Z31:AA31" si="32">Z3/Y3-1</f>
+      <c r="AA31" s="34">
+        <f t="shared" ref="AA31:AB31" si="32">AA3/Z3-1</f>
         <v>4.9170954831332159E-2</v>
       </c>
-      <c r="AA31" s="34">
+      <c r="AB31" s="34">
         <f t="shared" si="32"/>
         <v>1.2534059945504161E-2</v>
       </c>
-      <c r="AB31" s="34">
-        <f>AB3/AA3-1</f>
-        <v>3.1754574811625469E-2</v>
-      </c>
       <c r="AC31" s="34">
         <f>AC3/AB3-1</f>
-        <v>-6.7814293166406081E-3</v>
+        <v>3.1754574811625469E-2</v>
       </c>
       <c r="AD31" s="34">
         <f>AD3/AC3-1</f>
+        <v>-6.7814293166406081E-3</v>
+      </c>
+      <c r="AE31" s="34">
+        <f>AE3/AD3-1</f>
         <v>4.8319327731092487E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="81" customFormat="1" ht="12.75" customHeight="1">
+    <row r="32" spans="1:31" s="81" customFormat="1" ht="12.75" customHeight="1">
       <c r="A32" s="85" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="105" t="s">
+      <c r="B32" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="106" t="s">
+      <c r="C32" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="D32" s="106" t="s">
+      <c r="D32" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="E32" s="106" t="s">
+      <c r="E32" s="97" t="s">
         <v>186</v>
       </c>
       <c r="F32" s="81">
@@ -23102,44 +24530,47 @@
         <f>S3-O3</f>
         <v>48</v>
       </c>
-      <c r="T32" s="93"/>
-      <c r="W32" s="63" t="s">
+      <c r="T32" s="81">
+        <f>T3-P3</f>
+        <v>27</v>
+      </c>
+      <c r="X32" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="X32" s="81">
-        <f t="shared" ref="X32" si="40">X3-W3</f>
+      <c r="Y32" s="81">
+        <f t="shared" ref="Y32" si="40">Y3-X3</f>
         <v>155</v>
       </c>
-      <c r="Y32" s="81">
-        <f t="shared" ref="Y32" si="41">Y3-X3</f>
+      <c r="Z32" s="81">
+        <f t="shared" ref="Z32" si="41">Z3-Y3</f>
         <v>45</v>
       </c>
-      <c r="Z32" s="81">
-        <f t="shared" ref="Z32:AA32" si="42">Z3-Y3</f>
+      <c r="AA32" s="81">
+        <f t="shared" ref="AA32:AB32" si="42">AA3-Z3</f>
         <v>86</v>
       </c>
-      <c r="AA32" s="81">
+      <c r="AB32" s="81">
         <f t="shared" si="42"/>
         <v>23</v>
       </c>
-      <c r="AB32" s="81">
-        <f>AB3-AA3</f>
-        <v>59</v>
-      </c>
       <c r="AC32" s="81">
         <f>AC3-AB3</f>
-        <v>-13</v>
+        <v>59</v>
       </c>
       <c r="AD32" s="81">
         <f>AD3-AC3</f>
+        <v>-13</v>
+      </c>
+      <c r="AE32" s="81">
+        <f>AE3-AD3</f>
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:30" ht="12.75" customHeight="1">
+    <row r="33" spans="1:31" ht="12.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B33" s="105" t="s">
+      <c r="B33" s="96" t="s">
         <v>186</v>
       </c>
       <c r="C33" s="25">
@@ -23195,7 +24626,7 @@
         <v>2.5210084033613356E-2</v>
       </c>
       <c r="P33" s="25">
-        <f t="shared" ref="P33:S33" si="56">P3/O3-1</f>
+        <f t="shared" ref="P33:T33" si="56">P3/O3-1</f>
         <v>8.1967213114753079E-3</v>
       </c>
       <c r="Q33" s="25">
@@ -23210,8 +24641,9 @@
         <f t="shared" si="56"/>
         <v>4.0160642570281624E-3</v>
       </c>
-      <c r="W33" s="63" t="s">
-        <v>186</v>
+      <c r="T33" s="25">
+        <f t="shared" si="56"/>
+        <v>-2.4999999999999467E-3</v>
       </c>
       <c r="X33" s="63" t="s">
         <v>186</v>
@@ -23234,12 +24666,15 @@
       <c r="AD33" s="63" t="s">
         <v>186</v>
       </c>
+      <c r="AE33" s="63" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="34" spans="1:30" s="82" customFormat="1" ht="12.75" customHeight="1">
+    <row r="34" spans="1:31" s="82" customFormat="1" ht="12.75" customHeight="1">
       <c r="A34" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="105" t="s">
+      <c r="B34" s="96" t="s">
         <v>186</v>
       </c>
       <c r="C34" s="81">
@@ -23295,7 +24730,7 @@
         <v>48</v>
       </c>
       <c r="P34" s="81">
-        <f t="shared" ref="P34:S34" si="70">P3-O3</f>
+        <f t="shared" ref="P34:T34" si="70">P3-O3</f>
         <v>16</v>
       </c>
       <c r="Q34" s="81">
@@ -23310,9 +24745,9 @@
         <f t="shared" si="70"/>
         <v>8</v>
       </c>
-      <c r="T34" s="94"/>
-      <c r="W34" s="63" t="s">
-        <v>186</v>
+      <c r="T34" s="81">
+        <f t="shared" si="70"/>
+        <v>-5</v>
       </c>
       <c r="X34" s="63" t="s">
         <v>186</v>
@@ -23335,24 +24770,27 @@
       <c r="AD34" s="63" t="s">
         <v>186</v>
       </c>
+      <c r="AE34" s="63" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="35" spans="1:30" ht="12.75" customHeight="1">
-      <c r="AD35" s="25"/>
+    <row r="35" spans="1:31" ht="12.75" customHeight="1">
+      <c r="AE35" s="25"/>
     </row>
-    <row r="36" spans="1:30" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="36" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B36" s="105" t="s">
+      <c r="B36" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="105" t="s">
+      <c r="C36" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="D36" s="105" t="s">
+      <c r="D36" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="E36" s="105" t="s">
+      <c r="E36" s="96" t="s">
         <v>186</v>
       </c>
       <c r="F36" s="34">
@@ -23411,53 +24849,56 @@
         <f>S12/O12-1</f>
         <v>2.5516403402187082E-2</v>
       </c>
-      <c r="T36" s="99"/>
-      <c r="W36" s="63" t="s">
+      <c r="T36" s="34">
+        <f>T12/P12-1</f>
+        <v>2.5981873111782461E-2</v>
+      </c>
+      <c r="X36" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="X36" s="34">
-        <f t="shared" ref="X36" si="78">X12/W12-1</f>
+      <c r="Y36" s="34">
+        <f t="shared" ref="Y36" si="78">Y12/X12-1</f>
         <v>8.3486238532110013E-2</v>
       </c>
-      <c r="Y36" s="34">
-        <f t="shared" ref="Y36" si="79">Y12/X12-1</f>
+      <c r="Z36" s="34">
+        <f t="shared" ref="Z36" si="79">Z12/Y12-1</f>
         <v>9.9915325994919479E-2</v>
       </c>
-      <c r="Z36" s="34">
-        <f t="shared" ref="Z36:AA36" si="80">Z12/Y12-1</f>
+      <c r="AA36" s="34">
+        <f t="shared" ref="AA36:AB36" si="80">AA12/Z12-1</f>
         <v>7.7752117013087041E-2</v>
       </c>
-      <c r="AA36" s="34">
+      <c r="AB36" s="34">
         <f t="shared" si="80"/>
         <v>6.4285714285714279E-2</v>
       </c>
-      <c r="AB36" s="34">
-        <f>AB12/AA12-1</f>
-        <v>5.9731543624160999E-2</v>
-      </c>
       <c r="AC36" s="34">
         <f>AC12/AB12-1</f>
-        <v>2.7865737808739688E-2</v>
+        <v>5.9731543624160999E-2</v>
       </c>
       <c r="AD36" s="34">
         <f>AD12/AC12-1</f>
+        <v>2.7865737808739688E-2</v>
+      </c>
+      <c r="AE36" s="34">
+        <f>AE12/AD12-1</f>
         <v>2.9574861367837268E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:30" s="81" customFormat="1" ht="12.75" customHeight="1">
+    <row r="37" spans="1:31" s="81" customFormat="1" ht="12.75" customHeight="1">
       <c r="A37" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="105" t="s">
+      <c r="B37" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C37" s="106" t="s">
+      <c r="C37" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="D37" s="106" t="s">
+      <c r="D37" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="E37" s="106" t="s">
+      <c r="E37" s="97" t="s">
         <v>186</v>
       </c>
       <c r="F37" s="81">
@@ -23516,44 +24957,47 @@
         <f>S12-O12</f>
         <v>42</v>
       </c>
-      <c r="T37" s="93"/>
-      <c r="W37" s="63" t="s">
+      <c r="T37" s="81">
+        <f>T12-P12</f>
+        <v>43</v>
+      </c>
+      <c r="X37" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="X37" s="81">
-        <f t="shared" ref="X37" si="88">X12-W12</f>
+      <c r="Y37" s="81">
+        <f t="shared" ref="Y37" si="88">Y12-X12</f>
         <v>91</v>
       </c>
-      <c r="Y37" s="81">
-        <f t="shared" ref="Y37" si="89">Y12-X12</f>
+      <c r="Z37" s="81">
+        <f t="shared" ref="Z37" si="89">Z12-Y12</f>
         <v>118</v>
       </c>
-      <c r="Z37" s="81">
-        <f t="shared" ref="Z37:AA37" si="90">Z12-Y12</f>
+      <c r="AA37" s="81">
+        <f t="shared" ref="AA37:AB37" si="90">AA12-Z12</f>
         <v>101</v>
       </c>
-      <c r="AA37" s="81">
+      <c r="AB37" s="81">
         <f t="shared" si="90"/>
         <v>90</v>
       </c>
-      <c r="AB37" s="81">
-        <f>AB12-AA12</f>
-        <v>89</v>
-      </c>
       <c r="AC37" s="81">
         <f>AC12-AB12</f>
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="AD37" s="81">
         <f>AD12-AC12</f>
+        <v>44</v>
+      </c>
+      <c r="AE37" s="81">
+        <f>AE12-AD12</f>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:30" ht="12.75" customHeight="1">
+    <row r="38" spans="1:31" ht="12.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B38" s="105" t="s">
+      <c r="B38" s="96" t="s">
         <v>186</v>
       </c>
       <c r="C38" s="25">
@@ -23609,7 +25053,7 @@
         <v>8.5784313725489891E-3</v>
       </c>
       <c r="P38" s="25">
-        <f t="shared" ref="P38:S38" si="104">P12/O12-1</f>
+        <f t="shared" ref="P38:T38" si="104">P12/O12-1</f>
         <v>5.4678007290400732E-3</v>
       </c>
       <c r="Q38" s="25">
@@ -23624,8 +25068,9 @@
         <f t="shared" si="104"/>
         <v>6.5593321407275695E-3</v>
       </c>
-      <c r="W38" s="63" t="s">
-        <v>186</v>
+      <c r="T38" s="25">
+        <f t="shared" si="104"/>
+        <v>5.924170616113722E-3</v>
       </c>
       <c r="X38" s="63" t="s">
         <v>186</v>
@@ -23648,12 +25093,15 @@
       <c r="AD38" s="63" t="s">
         <v>186</v>
       </c>
+      <c r="AE38" s="63" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="39" spans="1:30" s="83" customFormat="1" ht="12.75" customHeight="1">
+    <row r="39" spans="1:31" s="83" customFormat="1" ht="12.75" customHeight="1">
       <c r="A39" s="87" t="s">
         <v>203</v>
       </c>
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="96" t="s">
         <v>186</v>
       </c>
       <c r="C39" s="81">
@@ -23709,7 +25157,7 @@
         <v>14</v>
       </c>
       <c r="P39" s="81">
-        <f t="shared" ref="P39:S39" si="118">P12-O12</f>
+        <f t="shared" ref="P39:T39" si="118">P12-O12</f>
         <v>9</v>
       </c>
       <c r="Q39" s="81">
@@ -23724,9 +25172,9 @@
         <f t="shared" si="118"/>
         <v>11</v>
       </c>
-      <c r="T39" s="94"/>
-      <c r="W39" s="63" t="s">
-        <v>186</v>
+      <c r="T39" s="81">
+        <f t="shared" si="118"/>
+        <v>10</v>
       </c>
       <c r="X39" s="63" t="s">
         <v>186</v>
@@ -23749,24 +25197,27 @@
       <c r="AD39" s="63" t="s">
         <v>186</v>
       </c>
+      <c r="AE39" s="63" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="40" spans="1:30" ht="12.75" customHeight="1">
-      <c r="AD40" s="25"/>
+    <row r="40" spans="1:31" ht="12.75" customHeight="1">
+      <c r="AE40" s="25"/>
     </row>
-    <row r="41" spans="1:30" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="41" spans="1:31" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B41" s="105" t="s">
+      <c r="B41" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C41" s="105" t="s">
+      <c r="C41" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="D41" s="105" t="s">
+      <c r="D41" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="E41" s="105" t="s">
+      <c r="E41" s="96" t="s">
         <v>186</v>
       </c>
       <c r="F41" s="34">
@@ -23822,56 +25273,59 @@
         <v>0.15808823529411775</v>
       </c>
       <c r="S41" s="34">
-        <f t="shared" ref="S41" si="131">S21/O21-1</f>
+        <f t="shared" ref="S41:T41" si="131">S21/O21-1</f>
         <v>1.9607843137254832E-2</v>
       </c>
-      <c r="T41" s="99"/>
-      <c r="W41" s="63" t="s">
+      <c r="T41" s="34">
+        <f t="shared" si="131"/>
+        <v>-5.1118210862619806E-2</v>
+      </c>
+      <c r="X41" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="X41" s="34">
-        <f t="shared" ref="X41" si="132">X21/W21-1</f>
+      <c r="Y41" s="34">
+        <f t="shared" ref="Y41" si="132">Y21/X21-1</f>
         <v>0.11764705882352944</v>
       </c>
-      <c r="Y41" s="34">
-        <f t="shared" ref="Y41" si="133">Y21/X21-1</f>
+      <c r="Z41" s="34">
+        <f t="shared" ref="Z41" si="133">Z21/Y21-1</f>
         <v>-0.1228070175438597</v>
       </c>
-      <c r="Z41" s="34">
-        <f t="shared" ref="Z41" si="134">Z21/Y21-1</f>
+      <c r="AA41" s="34">
+        <f t="shared" ref="AA41" si="134">AA21/Z21-1</f>
         <v>-3.3333333333333326E-2</v>
       </c>
-      <c r="AA41" s="34">
-        <f t="shared" ref="AA41" si="135">AA21/Z21-1</f>
+      <c r="AB41" s="34">
+        <f t="shared" ref="AB41" si="135">AB21/AA21-1</f>
         <v>-0.15402298850574714</v>
       </c>
-      <c r="AB41" s="34">
-        <f t="shared" ref="AB41" si="136">AB21/AA21-1</f>
+      <c r="AC41" s="34">
+        <f t="shared" ref="AC41" si="136">AC21/AB21-1</f>
         <v>-8.1521739130434812E-2</v>
-      </c>
-      <c r="AC41" s="34">
-        <f>AC21/AB21-1</f>
-        <v>-0.16863905325443784</v>
       </c>
       <c r="AD41" s="34">
         <f>AD21/AC21-1</f>
+        <v>-0.16863905325443784</v>
+      </c>
+      <c r="AE41" s="34">
+        <f>AE21/AD21-1</f>
         <v>0.15658362989323837</v>
       </c>
     </row>
-    <row r="42" spans="1:30" s="84" customFormat="1" ht="12.75" customHeight="1">
+    <row r="42" spans="1:31" s="84" customFormat="1" ht="12.75" customHeight="1">
       <c r="A42" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="B42" s="105" t="s">
+      <c r="B42" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C42" s="106" t="s">
+      <c r="C42" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="D42" s="106" t="s">
+      <c r="D42" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="E42" s="106" t="s">
+      <c r="E42" s="97" t="s">
         <v>186</v>
       </c>
       <c r="F42" s="84">
@@ -23930,44 +25384,47 @@
         <f>S21-O21</f>
         <v>6</v>
       </c>
-      <c r="T42" s="95"/>
-      <c r="W42" s="63" t="s">
+      <c r="T42" s="84">
+        <f>T21-P21</f>
+        <v>-16</v>
+      </c>
+      <c r="X42" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="X42" s="84">
-        <f t="shared" ref="X42" si="145">X21-W21</f>
+      <c r="Y42" s="84">
+        <f t="shared" ref="Y42" si="145">Y21-X21</f>
         <v>54</v>
       </c>
-      <c r="Y42" s="84">
-        <f t="shared" ref="Y42" si="146">Y21-X21</f>
+      <c r="Z42" s="84">
+        <f t="shared" ref="Z42" si="146">Z21-Y21</f>
         <v>-63</v>
       </c>
-      <c r="Z42" s="84">
-        <f t="shared" ref="Z42" si="147">Z21-Y21</f>
+      <c r="AA42" s="84">
+        <f t="shared" ref="AA42" si="147">AA21-Z21</f>
         <v>-15</v>
       </c>
-      <c r="AA42" s="84">
-        <f t="shared" ref="AA42" si="148">AA21-Z21</f>
+      <c r="AB42" s="84">
+        <f t="shared" ref="AB42" si="148">AB21-AA21</f>
         <v>-67</v>
       </c>
-      <c r="AB42" s="84">
-        <f t="shared" ref="AB42:AC42" si="149">AB21-AA21</f>
+      <c r="AC42" s="84">
+        <f t="shared" ref="AC42:AD42" si="149">AC21-AB21</f>
         <v>-30</v>
       </c>
-      <c r="AC42" s="84">
+      <c r="AD42" s="84">
         <f t="shared" si="149"/>
         <v>-57</v>
       </c>
-      <c r="AD42" s="84">
-        <f>AD21-AC21</f>
+      <c r="AE42" s="84">
+        <f>AE21-AD21</f>
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:30" ht="12.75" customHeight="1">
+    <row r="43" spans="1:31" ht="12.75" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="96" t="s">
         <v>186</v>
       </c>
       <c r="C43" s="25">
@@ -24035,11 +25492,12 @@
         <v>-3.0769230769230771E-2</v>
       </c>
       <c r="S43" s="25">
-        <f t="shared" ref="S43" si="165">S21/R21-1</f>
+        <f t="shared" ref="S43:T43" si="165">S21/R21-1</f>
         <v>-9.52380952380949E-3</v>
       </c>
-      <c r="W43" s="63" t="s">
-        <v>186</v>
+      <c r="T43" s="25">
+        <f t="shared" si="165"/>
+        <v>-4.8076923076923128E-2</v>
       </c>
       <c r="X43" s="63" t="s">
         <v>186</v>
@@ -24062,12 +25520,15 @@
       <c r="AD43" s="63" t="s">
         <v>186</v>
       </c>
+      <c r="AE43" s="63" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="44" spans="1:30" s="83" customFormat="1" ht="12.75" customHeight="1">
+    <row r="44" spans="1:31" s="83" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" s="87" t="s">
         <v>216</v>
       </c>
-      <c r="B44" s="105" t="s">
+      <c r="B44" s="96" t="s">
         <v>186</v>
       </c>
       <c r="C44" s="81">
@@ -24138,9 +25599,9 @@
         <f>S21-R21</f>
         <v>-3</v>
       </c>
-      <c r="T44" s="94"/>
-      <c r="W44" s="63" t="s">
-        <v>186</v>
+      <c r="T44" s="81">
+        <f>T21-S21</f>
+        <v>-15</v>
       </c>
       <c r="X44" s="63" t="s">
         <v>186</v>
@@ -24163,8 +25624,11 @@
       <c r="AD44" s="63" t="s">
         <v>186</v>
       </c>
+      <c r="AE44" s="63" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="47" spans="1:30" ht="12.75" customHeight="1">
+    <row r="47" spans="1:31" ht="12.75" customHeight="1">
       <c r="N47" s="76"/>
     </row>
     <row r="49" spans="14:14" ht="12.75" customHeight="1">
@@ -24178,15 +25642,15 @@
     <hyperlink ref="N1" r:id="rId4" xr:uid="{9287A329-D88E-784B-8BDF-1EDA927EB785}"/>
     <hyperlink ref="S1" r:id="rId5" xr:uid="{6AF4C14B-B6A4-FE47-B0D3-A570A390AD5C}"/>
     <hyperlink ref="O1" r:id="rId6" xr:uid="{0A17F8BF-EADB-DE42-994D-117A4F2CB3FE}"/>
-    <hyperlink ref="AD1" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
+    <hyperlink ref="AE1" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
     <hyperlink ref="M1" r:id="rId8" xr:uid="{F1748A46-ECC6-544E-9D30-C00CF38C6CF7}"/>
-    <hyperlink ref="AC1" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
-    <hyperlink ref="AB1" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
+    <hyperlink ref="AD1" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
+    <hyperlink ref="AC1" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
     <hyperlink ref="I1" r:id="rId11" xr:uid="{998E2907-64B9-7A44-8D65-8083912D2D62}"/>
     <hyperlink ref="E1" r:id="rId12" xr:uid="{5D689E99-05ED-E34E-9D87-28B9F22988C9}"/>
-    <hyperlink ref="AA1" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
-    <hyperlink ref="Z1" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
-    <hyperlink ref="Y1" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
+    <hyperlink ref="AB1" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
+    <hyperlink ref="AA1" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
+    <hyperlink ref="Z1" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
     <hyperlink ref="L1" r:id="rId16" xr:uid="{E0D344DF-ECD3-4969-946B-75165895949D}"/>
     <hyperlink ref="K1" r:id="rId17" xr:uid="{34FDBE06-551B-4817-B842-42B3C369DE44}"/>
     <hyperlink ref="J1" r:id="rId18" xr:uid="{8672DEA7-6978-4CBC-A339-3D96580B25F6}"/>
@@ -24196,11 +25660,12 @@
     <hyperlink ref="D1" r:id="rId22" xr:uid="{9AA615B1-70E4-40CE-8BD9-FA369F45AAE7}"/>
     <hyperlink ref="C1" r:id="rId23" xr:uid="{B190BD40-76B4-4C45-B1D6-B5043307E3B6}"/>
     <hyperlink ref="B1" r:id="rId24" xr:uid="{2E883042-0703-4781-AC08-6A8AD2EAD4EB}"/>
-    <hyperlink ref="X1" r:id="rId25" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/93a33ec4-dc07-47b3-91c2-d84b2e56d699?origin=1" xr:uid="{CE32064C-B077-40F4-9C44-3F45FE0A2ECE}"/>
-    <hyperlink ref="W1" r:id="rId26" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a574642d-6cd1-4e80-a242-26ff2d0747f5?origin=1" xr:uid="{4A9206DD-D830-44D0-A5B0-DF41E9DD8391}"/>
+    <hyperlink ref="Y1" r:id="rId25" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/93a33ec4-dc07-47b3-91c2-d84b2e56d699?origin=1" xr:uid="{CE32064C-B077-40F4-9C44-3F45FE0A2ECE}"/>
+    <hyperlink ref="X1" r:id="rId26" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a574642d-6cd1-4e80-a242-26ff2d0747f5?origin=1" xr:uid="{4A9206DD-D830-44D0-A5B0-DF41E9DD8391}"/>
+    <hyperlink ref="T1" r:id="rId27" xr:uid="{F6F821CD-3C9C-4984-B9E1-54EA40AA851B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId27"/>
-  <drawing r:id="rId28"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId28"/>
+  <drawing r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add E190-E2 China news
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C8BC68-7BF1-40CE-9878-B4A37F2111CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B39FE1B-B5DE-4EDA-9424-5AEC715F081A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="264">
   <si>
     <t>$ERJ</t>
   </si>
@@ -953,6 +953,9 @@
   </si>
   <si>
     <t>IPO</t>
+  </si>
+  <si>
+    <t>Embraer E190-E2 is certified in China by CAAC after 5 years since launching process</t>
   </si>
 </sst>
 </file>
@@ -1441,16 +1444,22 @@
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1460,24 +1469,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1507,16 +1498,28 @@
     <xf numFmtId="169" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8796,10 +8799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC56"/>
+  <dimension ref="A2:AC55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U56" sqref="U56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -8819,35 +8822,35 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="104"/>
-      <c r="G5" s="102" t="s">
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
+      <c r="G5" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="104"/>
-      <c r="T5" s="102" t="s">
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="105"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="105"/>
+      <c r="Q5" s="105"/>
+      <c r="R5" s="106"/>
+      <c r="T5" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="104"/>
-      <c r="AA5" s="100" t="s">
+      <c r="U5" s="105"/>
+      <c r="V5" s="105"/>
+      <c r="W5" s="106"/>
+      <c r="AA5" s="118" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="101"/>
+      <c r="AB5" s="119"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -8858,10 +8861,10 @@
       </c>
       <c r="D6" s="18"/>
       <c r="G6" s="9">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
@@ -8927,8 +8930,12 @@
         <v>6941.9699999999993</v>
       </c>
       <c r="D8" s="18"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="60"/>
+      <c r="G8" s="9">
+        <v>44835</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>254</v>
+      </c>
       <c r="I8" s="60"/>
       <c r="J8" s="60"/>
       <c r="K8" s="60"/>
@@ -8962,21 +8969,17 @@
         <f>$C$33</f>
         <v>Q222</v>
       </c>
-      <c r="G9" s="9">
-        <v>44835</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
       <c r="R9" s="38"/>
       <c r="T9" s="47" t="s">
         <v>151</v>
@@ -8998,18 +9001,16 @@
         <v>Q222</v>
       </c>
       <c r="G10" s="10"/>
-      <c r="H10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="60"/>
       <c r="R10" s="38"/>
       <c r="T10" s="47" t="s">
         <v>152</v>
@@ -9030,9 +9031,11 @@
         <f>$C$33</f>
         <v>Q222</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="8" t="s">
-        <v>13</v>
+      <c r="G11" s="9">
+        <v>44835</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="I11" s="37"/>
       <c r="J11" s="37"/>
@@ -9061,7 +9064,9 @@
       </c>
       <c r="D12" s="19"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="37"/>
+      <c r="H12" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="I12" s="37"/>
       <c r="J12" s="37"/>
       <c r="K12" s="37"/>
@@ -9076,20 +9081,18 @@
       <c r="U12" s="37"/>
       <c r="V12" s="37"/>
       <c r="W12" s="38"/>
-      <c r="Y12" s="102" t="s">
+      <c r="Y12" s="104" t="s">
         <v>219</v>
       </c>
-      <c r="Z12" s="103"/>
-      <c r="AA12" s="103"/>
-      <c r="AB12" s="103"/>
-      <c r="AC12" s="104"/>
+      <c r="Z12" s="105"/>
+      <c r="AA12" s="105"/>
+      <c r="AB12" s="105"/>
+      <c r="AC12" s="106"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="G13" s="9">
-        <v>44835</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>29</v>
+      <c r="G13" s="10"/>
+      <c r="H13" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="I13" s="37"/>
       <c r="J13" s="37"/>
@@ -9108,20 +9111,18 @@
       <c r="V13" s="37"/>
       <c r="W13" s="38"/>
       <c r="Y13" s="92"/>
-      <c r="Z13" s="109" t="s">
+      <c r="Z13" s="116" t="s">
         <v>220</v>
       </c>
-      <c r="AA13" s="109"/>
-      <c r="AB13" s="109" t="s">
+      <c r="AA13" s="116"/>
+      <c r="AB13" s="116" t="s">
         <v>221</v>
       </c>
-      <c r="AC13" s="110"/>
+      <c r="AC13" s="117"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="10"/>
-      <c r="H14" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="H14" s="37"/>
       <c r="I14" s="37"/>
       <c r="J14" s="37"/>
       <c r="K14" s="37"/>
@@ -9141,23 +9142,27 @@
       <c r="Y14" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="Z14" s="98" t="s">
+      <c r="Z14" s="102" t="s">
         <v>231</v>
       </c>
-      <c r="AA14" s="98"/>
-      <c r="AB14" s="98" t="s">
+      <c r="AA14" s="102"/>
+      <c r="AB14" s="102" t="s">
         <v>232</v>
       </c>
-      <c r="AC14" s="99"/>
+      <c r="AC14" s="103"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="103"/>
-      <c r="D15" s="104"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="37"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
+      <c r="G15" s="9">
+        <v>44835</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="I15" s="37"/>
       <c r="J15" s="37"/>
       <c r="K15" s="37"/>
@@ -9177,14 +9182,14 @@
       <c r="Y15" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="Z15" s="98" t="s">
+      <c r="Z15" s="102" t="s">
         <v>227</v>
       </c>
-      <c r="AA15" s="98"/>
-      <c r="AB15" s="98" t="s">
+      <c r="AA15" s="102"/>
+      <c r="AB15" s="102" t="s">
         <v>233</v>
       </c>
-      <c r="AC15" s="99"/>
+      <c r="AC15" s="103"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="14" t="s">
@@ -9193,12 +9198,14 @@
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="99"/>
+      <c r="D16" s="103"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="37"/>
+      <c r="H16" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="I16" s="37"/>
       <c r="J16" s="37"/>
       <c r="K16" s="37"/>
@@ -9218,29 +9225,25 @@
       <c r="Y16" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="Z16" s="98" t="s">
+      <c r="Z16" s="102" t="s">
         <v>228</v>
       </c>
-      <c r="AA16" s="98"/>
-      <c r="AB16" s="98" t="s">
+      <c r="AA16" s="102"/>
+      <c r="AB16" s="102" t="s">
         <v>234</v>
       </c>
-      <c r="AC16" s="99"/>
+      <c r="AC16" s="103"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="98" t="s">
+      <c r="C17" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="99"/>
-      <c r="G17" s="9">
-        <v>44805</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>187</v>
-      </c>
+      <c r="D17" s="103"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="37"/>
       <c r="J17" s="37"/>
       <c r="K17" s="37"/>
@@ -9258,19 +9261,19 @@
       <c r="Y17" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="Z17" s="98" t="s">
+      <c r="Z17" s="102" t="s">
         <v>229</v>
       </c>
-      <c r="AA17" s="98"/>
-      <c r="AB17" s="98" t="s">
+      <c r="AA17" s="102"/>
+      <c r="AB17" s="102" t="s">
         <v>235</v>
       </c>
-      <c r="AC17" s="99"/>
+      <c r="AC17" s="103"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="16"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="103"/>
       <c r="G18" s="10"/>
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
@@ -9292,21 +9295,25 @@
       <c r="Y18" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="Z18" s="98" t="s">
+      <c r="Z18" s="102" t="s">
         <v>230</v>
       </c>
-      <c r="AA18" s="98"/>
-      <c r="AB18" s="98" t="s">
+      <c r="AA18" s="102"/>
+      <c r="AB18" s="102" t="s">
         <v>236</v>
       </c>
-      <c r="AC18" s="99"/>
+      <c r="AC18" s="103"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="17"/>
-      <c r="C19" s="107"/>
-      <c r="D19" s="108"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="37"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="123"/>
+      <c r="G19" s="9">
+        <v>44805</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>187</v>
+      </c>
       <c r="I19" s="37"/>
       <c r="J19" s="37"/>
       <c r="K19" s="37"/>
@@ -9326,31 +9333,27 @@
       <c r="Y19" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="Z19" s="98" t="s">
+      <c r="Z19" s="102" t="s">
         <v>238</v>
       </c>
-      <c r="AA19" s="98"/>
-      <c r="AB19" s="98" t="s">
+      <c r="AA19" s="102"/>
+      <c r="AB19" s="102" t="s">
         <v>239</v>
       </c>
-      <c r="AC19" s="99"/>
+      <c r="AC19" s="103"/>
     </row>
     <row r="20" spans="2:29">
-      <c r="G20" s="9">
-        <v>44805</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
       <c r="R20" s="38"/>
       <c r="T20" s="45" t="s">
         <v>141</v>
@@ -9361,29 +9364,27 @@
       <c r="Y20" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="Z20" s="98" t="s">
+      <c r="Z20" s="102" t="s">
         <v>244</v>
       </c>
-      <c r="AA20" s="98"/>
-      <c r="AB20" s="98" t="s">
+      <c r="AA20" s="102"/>
+      <c r="AB20" s="102" t="s">
         <v>245</v>
       </c>
-      <c r="AC20" s="99"/>
+      <c r="AC20" s="103"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="10"/>
-      <c r="H21" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
       <c r="R21" s="38"/>
       <c r="T21" s="45" t="s">
         <v>140</v>
@@ -9398,14 +9399,16 @@
       <c r="AC21" s="38"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="103"/>
-      <c r="D22" s="104"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="8" t="s">
-        <v>193</v>
+      <c r="C22" s="105"/>
+      <c r="D22" s="106"/>
+      <c r="G22" s="9">
+        <v>44805</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="I22" s="60"/>
       <c r="J22" s="60"/>
@@ -9433,13 +9436,13 @@
       <c r="B23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C23" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="99"/>
+      <c r="D23" s="103"/>
       <c r="G23" s="10"/>
       <c r="H23" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I23" s="60"/>
       <c r="J23" s="60"/>
@@ -9450,9 +9453,7 @@
       <c r="O23" s="60"/>
       <c r="P23" s="60"/>
       <c r="Q23" s="60"/>
-      <c r="R23" s="51" t="s">
-        <v>194</v>
-      </c>
+      <c r="R23" s="38"/>
       <c r="T23" s="42"/>
       <c r="U23" s="37"/>
       <c r="V23" s="37"/>
@@ -9462,12 +9463,14 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="98">
+      <c r="C24" s="102">
         <v>1969</v>
       </c>
-      <c r="D24" s="99"/>
+      <c r="D24" s="103"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="60"/>
+      <c r="H24" s="8" t="s">
+        <v>193</v>
+      </c>
       <c r="I24" s="60"/>
       <c r="J24" s="60"/>
       <c r="K24" s="60"/>
@@ -9487,10 +9490,12 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="10"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="99"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="103"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="60"/>
+      <c r="H25" s="8" t="s">
+        <v>191</v>
+      </c>
       <c r="I25" s="60"/>
       <c r="J25" s="60"/>
       <c r="K25" s="60"/>
@@ -9500,7 +9505,9 @@
       <c r="O25" s="60"/>
       <c r="P25" s="60"/>
       <c r="Q25" s="60"/>
-      <c r="R25" s="38"/>
+      <c r="R25" s="51" t="s">
+        <v>194</v>
+      </c>
       <c r="T25" s="45" t="s">
         <v>144</v>
       </c>
@@ -9512,17 +9519,13 @@
       <c r="B26" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="105">
+      <c r="C26" s="120">
         <f>'Financial Model'!T68</f>
         <v>2392.9</v>
       </c>
-      <c r="D26" s="106"/>
-      <c r="G26" s="9">
-        <v>44743</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>196</v>
-      </c>
+      <c r="D26" s="121"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="60"/>
       <c r="I26" s="60"/>
       <c r="J26" s="60"/>
       <c r="K26" s="60"/>
@@ -9542,12 +9545,10 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="10"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="99"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="103"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="8" t="s">
-        <v>197</v>
-      </c>
+      <c r="H27" s="60"/>
       <c r="I27" s="60"/>
       <c r="J27" s="60"/>
       <c r="K27" s="60"/>
@@ -9569,11 +9570,13 @@
       <c r="B28" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C28" s="98"/>
-      <c r="D28" s="99"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="50" t="s">
-        <v>198</v>
+      <c r="C28" s="102"/>
+      <c r="D28" s="103"/>
+      <c r="G28" s="9">
+        <v>44743</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="I28" s="60"/>
       <c r="J28" s="60"/>
@@ -9596,13 +9599,15 @@
       <c r="B29" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C29" s="117">
+      <c r="C29" s="113">
         <f>'Order &amp; Backlog'!S21</f>
         <v>312</v>
       </c>
-      <c r="D29" s="99"/>
+      <c r="D29" s="103"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="60"/>
+      <c r="H29" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="I29" s="60"/>
       <c r="J29" s="60"/>
       <c r="K29" s="60"/>
@@ -9622,26 +9627,24 @@
       <c r="B30" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="98">
+      <c r="C30" s="102">
         <f>'Financial Model'!T43</f>
         <v>32</v>
       </c>
-      <c r="D30" s="99"/>
-      <c r="G30" s="9">
-        <v>44743</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="37"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="37"/>
-      <c r="Q30" s="37"/>
+      <c r="D30" s="103"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
       <c r="R30" s="38"/>
       <c r="T30" s="42"/>
       <c r="U30" s="37"/>
@@ -9652,14 +9655,12 @@
       <c r="B31" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C31" s="118">
+      <c r="C31" s="114">
         <v>36708</v>
       </c>
-      <c r="D31" s="119"/>
+      <c r="D31" s="115"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="8" t="s">
-        <v>242</v>
-      </c>
+      <c r="H31" s="60"/>
       <c r="I31" s="60"/>
       <c r="J31" s="60"/>
       <c r="K31" s="60"/>
@@ -9679,19 +9680,23 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="10"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="99"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="60"/>
-      <c r="P32" s="60"/>
-      <c r="Q32" s="60"/>
+      <c r="C32" s="102"/>
+      <c r="D32" s="103"/>
+      <c r="G32" s="9">
+        <v>44743</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
       <c r="R32" s="38"/>
       <c r="T32" s="45" t="s">
         <v>150</v>
@@ -9710,11 +9715,9 @@
       <c r="D33" s="32">
         <v>44777</v>
       </c>
-      <c r="G33" s="9">
-        <v>44682</v>
-      </c>
-      <c r="H33" s="60" t="s">
-        <v>250</v>
+      <c r="G33" s="10"/>
+      <c r="H33" s="8" t="s">
+        <v>242</v>
       </c>
       <c r="I33" s="60"/>
       <c r="J33" s="60"/>
@@ -9735,14 +9738,12 @@
       <c r="B34" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="114"/>
+      <c r="D34" s="110"/>
       <c r="G34" s="10"/>
-      <c r="H34" s="8" t="s">
-        <v>251</v>
-      </c>
+      <c r="H34" s="60"/>
       <c r="I34" s="60"/>
       <c r="J34" s="60"/>
       <c r="K34" s="60"/>
@@ -9752,17 +9753,19 @@
       <c r="O34" s="60"/>
       <c r="P34" s="60"/>
       <c r="Q34" s="60"/>
-      <c r="R34" s="51" t="s">
-        <v>31</v>
-      </c>
+      <c r="R34" s="38"/>
       <c r="T34" s="43"/>
       <c r="U34" s="35"/>
       <c r="V34" s="35"/>
       <c r="W34" s="36"/>
     </row>
     <row r="35" spans="2:23">
-      <c r="G35" s="10"/>
-      <c r="H35" s="60"/>
+      <c r="G35" s="9">
+        <v>44682</v>
+      </c>
+      <c r="H35" s="60" t="s">
+        <v>250</v>
+      </c>
       <c r="I35" s="60"/>
       <c r="J35" s="60"/>
       <c r="K35" s="60"/>
@@ -9775,61 +9778,63 @@
       <c r="R35" s="38"/>
     </row>
     <row r="36" spans="2:23">
-      <c r="G36" s="9">
-        <v>43922</v>
-      </c>
-      <c r="H36" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="37"/>
-      <c r="R36" s="38"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="I36" s="60"/>
+      <c r="J36" s="60"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="51" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="37" spans="2:23">
-      <c r="B37" s="102" t="s">
+      <c r="B37" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="103"/>
-      <c r="D37" s="104"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="106"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="37"/>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="37"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
       <c r="R37" s="38"/>
-      <c r="T37" s="102" t="s">
+      <c r="T37" s="104" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="103"/>
-      <c r="V37" s="103"/>
-      <c r="W37" s="104"/>
+      <c r="U37" s="105"/>
+      <c r="V37" s="105"/>
+      <c r="W37" s="106"/>
     </row>
     <row r="38" spans="2:23">
       <c r="B38" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="115">
+      <c r="C38" s="111">
         <f>C6/'Financial Model'!T122</f>
         <v>2.4165314860584122</v>
       </c>
-      <c r="D38" s="116"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="37"/>
+      <c r="D38" s="112"/>
+      <c r="G38" s="9">
+        <v>43922</v>
+      </c>
+      <c r="H38" s="37" t="s">
+        <v>164</v>
+      </c>
       <c r="I38" s="37"/>
       <c r="J38" s="37"/>
       <c r="K38" s="37"/>
@@ -9839,9 +9844,7 @@
       <c r="O38" s="37"/>
       <c r="P38" s="37"/>
       <c r="Q38" s="37"/>
-      <c r="R38" s="51" t="s">
-        <v>31</v>
-      </c>
+      <c r="R38" s="38"/>
       <c r="T38" s="42" t="s">
         <v>159</v>
       </c>
@@ -9853,13 +9856,15 @@
       <c r="B39" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="115">
+      <c r="C39" s="111">
         <f>C6/'Financial Model'!AE9</f>
         <v>2.2515010006671113E-3</v>
       </c>
-      <c r="D39" s="116"/>
+      <c r="D39" s="112"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="37"/>
+      <c r="H39" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="I39" s="37"/>
       <c r="J39" s="37"/>
       <c r="K39" s="37"/>
@@ -9881,17 +9886,13 @@
       <c r="B40" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="111">
+      <c r="C40" s="107">
         <f>C6/'Financial Model'!AE26</f>
         <v>-155.32248322147649</v>
       </c>
-      <c r="D40" s="112"/>
-      <c r="G40" s="9">
-        <v>43770</v>
-      </c>
-      <c r="H40" s="37" t="s">
-        <v>167</v>
-      </c>
+      <c r="D40" s="108"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="37"/>
       <c r="I40" s="37"/>
       <c r="J40" s="37"/>
       <c r="K40" s="37"/>
@@ -9901,7 +9902,9 @@
       <c r="O40" s="37"/>
       <c r="P40" s="37"/>
       <c r="Q40" s="37"/>
-      <c r="R40" s="38"/>
+      <c r="R40" s="51" t="s">
+        <v>31</v>
+      </c>
       <c r="T40" s="44" t="s">
         <v>161</v>
       </c>
@@ -9911,9 +9914,7 @@
     </row>
     <row r="41" spans="2:23">
       <c r="G41" s="10"/>
-      <c r="H41" s="50" t="s">
-        <v>168</v>
-      </c>
+      <c r="H41" s="37"/>
       <c r="I41" s="37"/>
       <c r="J41" s="37"/>
       <c r="K41" s="37"/>
@@ -9930,8 +9931,12 @@
       <c r="W41" s="38"/>
     </row>
     <row r="42" spans="2:23">
-      <c r="G42" s="10"/>
-      <c r="H42" s="37"/>
+      <c r="G42" s="9">
+        <v>43770</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>167</v>
+      </c>
       <c r="I42" s="37"/>
       <c r="J42" s="37"/>
       <c r="K42" s="37"/>
@@ -9950,16 +9955,14 @@
       <c r="W42" s="38"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="102" t="s">
+      <c r="B43" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="C43" s="103"/>
-      <c r="D43" s="104"/>
-      <c r="G43" s="9">
-        <v>43739</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>246</v>
+      <c r="C43" s="105"/>
+      <c r="D43" s="106"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="50" t="s">
+        <v>168</v>
       </c>
       <c r="I43" s="37"/>
       <c r="J43" s="37"/>
@@ -9969,9 +9972,7 @@
       <c r="N43" s="37"/>
       <c r="O43" s="37"/>
       <c r="P43" s="37"/>
-      <c r="Q43" s="37" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q43" s="37"/>
       <c r="R43" s="38"/>
       <c r="T43" s="61" t="s">
         <v>200</v>
@@ -9981,15 +9982,15 @@
       <c r="W43" s="38"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="120" t="s">
+      <c r="B44" s="98" t="s">
         <v>248</v>
       </c>
-      <c r="C44" s="121"/>
+      <c r="C44" s="99"/>
       <c r="D44" s="51" t="s">
         <v>31</v>
       </c>
       <c r="G44" s="10"/>
-      <c r="H44" s="60"/>
+      <c r="H44" s="37"/>
       <c r="I44" s="37"/>
       <c r="J44" s="37"/>
       <c r="K44" s="37"/>
@@ -10008,15 +10009,19 @@
       </c>
     </row>
     <row r="45" spans="2:23">
-      <c r="B45" s="120" t="s">
+      <c r="B45" s="98" t="s">
         <v>249</v>
       </c>
-      <c r="C45" s="121"/>
+      <c r="C45" s="99"/>
       <c r="D45" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="G45" s="10"/>
-      <c r="H45" s="37"/>
+      <c r="G45" s="9">
+        <v>43739</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>246</v>
+      </c>
       <c r="I45" s="37"/>
       <c r="J45" s="37"/>
       <c r="K45" s="37"/>
@@ -10025,17 +10030,19 @@
       <c r="N45" s="37"/>
       <c r="O45" s="37"/>
       <c r="P45" s="37"/>
-      <c r="Q45" s="37"/>
+      <c r="Q45" s="37" t="s">
+        <v>179</v>
+      </c>
       <c r="R45" s="38"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="B46" s="120"/>
-      <c r="C46" s="121"/>
+      <c r="B46" s="98"/>
+      <c r="C46" s="99"/>
       <c r="D46" s="89" t="s">
         <v>31</v>
       </c>
       <c r="G46" s="10"/>
-      <c r="H46" s="37"/>
+      <c r="H46" s="60"/>
       <c r="I46" s="37"/>
       <c r="J46" s="37"/>
       <c r="K46" s="37"/>
@@ -10048,17 +10055,13 @@
       <c r="R46" s="38"/>
     </row>
     <row r="47" spans="2:23">
-      <c r="B47" s="120"/>
-      <c r="C47" s="121"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="99"/>
       <c r="D47" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="9">
-        <v>43586</v>
-      </c>
-      <c r="H47" s="60" t="s">
-        <v>166</v>
-      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="37"/>
       <c r="I47" s="37"/>
       <c r="J47" s="37"/>
       <c r="K47" s="37"/>
@@ -10071,8 +10074,8 @@
       <c r="R47" s="38"/>
     </row>
     <row r="48" spans="2:23">
-      <c r="B48" s="122"/>
-      <c r="C48" s="123"/>
+      <c r="B48" s="100"/>
+      <c r="C48" s="101"/>
       <c r="D48" s="90" t="s">
         <v>31</v>
       </c>
@@ -10091,10 +10094,10 @@
     </row>
     <row r="49" spans="7:18">
       <c r="G49" s="9">
-        <v>43282</v>
-      </c>
-      <c r="H49" s="37" t="s">
-        <v>162</v>
+        <v>43586</v>
+      </c>
+      <c r="H49" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="I49" s="37"/>
       <c r="J49" s="37"/>
@@ -10109,9 +10112,7 @@
     </row>
     <row r="50" spans="7:18">
       <c r="G50" s="10"/>
-      <c r="H50" s="8" t="s">
-        <v>163</v>
-      </c>
+      <c r="H50" s="37"/>
       <c r="I50" s="37"/>
       <c r="J50" s="37"/>
       <c r="K50" s="37"/>
@@ -10124,38 +10125,44 @@
       <c r="R50" s="38"/>
     </row>
     <row r="51" spans="7:18">
-      <c r="G51" s="10"/>
-      <c r="H51" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="I51" s="60"/>
-      <c r="J51" s="60"/>
-      <c r="K51" s="60"/>
-      <c r="L51" s="60"/>
-      <c r="M51" s="60"/>
-      <c r="N51" s="60"/>
-      <c r="O51" s="60"/>
-      <c r="P51" s="60"/>
-      <c r="Q51" s="60"/>
+      <c r="G51" s="9">
+        <v>43282</v>
+      </c>
+      <c r="H51" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
       <c r="R51" s="38"/>
     </row>
     <row r="52" spans="7:18">
       <c r="G52" s="10"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="60"/>
-      <c r="J52" s="60"/>
-      <c r="K52" s="60"/>
-      <c r="L52" s="60"/>
-      <c r="M52" s="60"/>
-      <c r="N52" s="60"/>
-      <c r="O52" s="60"/>
-      <c r="P52" s="60"/>
-      <c r="Q52" s="60"/>
+      <c r="H52" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
+      <c r="O52" s="37"/>
+      <c r="P52" s="37"/>
+      <c r="Q52" s="37"/>
       <c r="R52" s="38"/>
     </row>
     <row r="53" spans="7:18">
       <c r="G53" s="10"/>
-      <c r="H53" s="60"/>
+      <c r="H53" s="8" t="s">
+        <v>165</v>
+      </c>
       <c r="I53" s="60"/>
       <c r="J53" s="60"/>
       <c r="K53" s="60"/>
@@ -10182,44 +10189,53 @@
       <c r="R54" s="38"/>
     </row>
     <row r="55" spans="7:18">
-      <c r="G55" s="10"/>
-      <c r="H55" s="60"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-      <c r="K55" s="60"/>
-      <c r="L55" s="60"/>
-      <c r="M55" s="60"/>
-      <c r="N55" s="60"/>
-      <c r="O55" s="60"/>
-      <c r="P55" s="60"/>
-      <c r="Q55" s="60"/>
-      <c r="R55" s="38"/>
-    </row>
-    <row r="56" spans="7:18">
-      <c r="G56" s="91">
+      <c r="G55" s="91">
         <v>42552</v>
       </c>
-      <c r="H56" s="54" t="s">
+      <c r="H55" s="54" t="s">
         <v>240</v>
       </c>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
-      <c r="O56" s="35"/>
-      <c r="P56" s="35"/>
-      <c r="Q56" s="35"/>
-      <c r="R56" s="36"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="35"/>
+      <c r="Q55" s="35"/>
+      <c r="R55" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
     <mergeCell ref="Z19:AA19"/>
     <mergeCell ref="AB19:AC19"/>
     <mergeCell ref="Z20:AA20"/>
@@ -10236,57 +10252,35 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H9" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H13" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="H11" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H15" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C34:D34" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R38" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H17" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H20" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R23" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H26" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="R40" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H19" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H22" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R25" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H28" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
     <hyperlink ref="W44" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
     <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
     <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
-    <hyperlink ref="H30" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H43" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="H32" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H45" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
     <hyperlink ref="D45" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D44" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
-    <hyperlink ref="R34" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H6" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="R36" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H8" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H6" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId18"/>
-  <drawing r:id="rId19"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -22060,7 +22054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
$ERJ Q422 orders & backlog
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6032CFB1-D582-4914-994F-05EC516BA36A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCA53E8-C918-44BE-B07F-E28A2C502DBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="268">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1461,16 +1461,26 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1480,24 +1490,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1527,21 +1519,29 @@
     <xf numFmtId="169" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5115,9 +5115,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$T$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$U$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5174,16 +5174,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Q322</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Q422</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$3:$T$3</c:f>
+              <c:f>'Order &amp; Backlog'!$B$3:$U$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1835</c:v>
                 </c:pt>
@@ -5240,6 +5243,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5276,9 +5282,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$T$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$U$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5335,16 +5341,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Q322</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Q422</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$12:$T$12</c:f>
+              <c:f>'Order &amp; Backlog'!$B$12:$U$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1414</c:v>
                 </c:pt>
@@ -5401,6 +5410,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1698</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5437,9 +5449,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$T$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$U$1</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5496,16 +5508,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Q322</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Q422</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$21:$T$21</c:f>
+              <c:f>'Order &amp; Backlog'!$B$21:$U$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>421</c:v>
                 </c:pt>
@@ -5562,6 +5577,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8486,14 +8504,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -8510,7 +8528,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13173075" y="3175"/>
+          <a:off x="13763625" y="3175"/>
           <a:ext cx="0" cy="9617075"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -8886,8 +8904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X33" sqref="X33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -8907,35 +8925,35 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="103"/>
-      <c r="G5" s="101" t="s">
+      <c r="C5" s="106"/>
+      <c r="D5" s="107"/>
+      <c r="G5" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="102"/>
-      <c r="N5" s="102"/>
-      <c r="O5" s="102"/>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-      <c r="R5" s="103"/>
-      <c r="T5" s="101" t="s">
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="107"/>
+      <c r="T5" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="102"/>
-      <c r="V5" s="102"/>
-      <c r="W5" s="103"/>
-      <c r="AA5" s="99" t="s">
+      <c r="U5" s="106"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="107"/>
+      <c r="AA5" s="119" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="100"/>
+      <c r="AB5" s="120"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -8948,7 +8966,7 @@
       <c r="G6" s="8">
         <v>44927</v>
       </c>
-      <c r="H6" s="123" t="s">
+      <c r="H6" s="97" t="s">
         <v>266</v>
       </c>
       <c r="I6" s="35"/>
@@ -9165,13 +9183,13 @@
       <c r="U12" s="35"/>
       <c r="V12" s="35"/>
       <c r="W12" s="36"/>
-      <c r="Y12" s="101" t="s">
+      <c r="Y12" s="105" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="102"/>
-      <c r="AA12" s="102"/>
-      <c r="AB12" s="102"/>
-      <c r="AC12" s="103"/>
+      <c r="Z12" s="106"/>
+      <c r="AA12" s="106"/>
+      <c r="AB12" s="106"/>
+      <c r="AC12" s="107"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -9193,14 +9211,14 @@
       <c r="V13" s="35"/>
       <c r="W13" s="36"/>
       <c r="Y13" s="89"/>
-      <c r="Z13" s="108" t="s">
+      <c r="Z13" s="117" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="108"/>
-      <c r="AB13" s="108" t="s">
+      <c r="AA13" s="117"/>
+      <c r="AB13" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="109"/>
+      <c r="AC13" s="118"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="9"/>
@@ -9224,21 +9242,21 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="97" t="s">
+      <c r="Z14" s="103" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="97"/>
-      <c r="AB14" s="97" t="s">
+      <c r="AA14" s="103"/>
+      <c r="AB14" s="103" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="98"/>
+      <c r="AC14" s="104"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="103"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="107"/>
       <c r="G15" s="8">
         <v>44835</v>
       </c>
@@ -9264,14 +9282,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="97" t="s">
+      <c r="Z15" s="103" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="97"/>
-      <c r="AB15" s="97" t="s">
+      <c r="AA15" s="103"/>
+      <c r="AB15" s="103" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="98"/>
+      <c r="AC15" s="104"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9280,10 +9298,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="97" t="s">
+      <c r="C16" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="98"/>
+      <c r="D16" s="104"/>
       <c r="E16" s="3" t="s">
         <v>265</v>
       </c>
@@ -9310,23 +9328,23 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="97" t="s">
+      <c r="Z16" s="103" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="97"/>
-      <c r="AB16" s="97" t="s">
+      <c r="AA16" s="103"/>
+      <c r="AB16" s="103" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="98"/>
+      <c r="AC16" s="104"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="97" t="s">
+      <c r="C17" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="98"/>
+      <c r="D17" s="104"/>
       <c r="E17" s="3" t="s">
         <v>265</v>
       </c>
@@ -9351,19 +9369,19 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="97" t="s">
+      <c r="Z17" s="103" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="97"/>
-      <c r="AB17" s="97" t="s">
+      <c r="AA17" s="103"/>
+      <c r="AB17" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="98"/>
+      <c r="AC17" s="104"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="97"/>
-      <c r="D18" s="98"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="104"/>
       <c r="G18" s="9"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
@@ -9385,19 +9403,19 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="97" t="s">
+      <c r="Z18" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="97"/>
-      <c r="AB18" s="97" t="s">
+      <c r="AA18" s="103"/>
+      <c r="AB18" s="103" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="98"/>
+      <c r="AC18" s="104"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="106"/>
-      <c r="D19" s="107"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="124"/>
       <c r="G19" s="8">
         <v>44835</v>
       </c>
@@ -9423,14 +9441,14 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="97" t="s">
+      <c r="Z19" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="97"/>
-      <c r="AB19" s="97" t="s">
+      <c r="AA19" s="103"/>
+      <c r="AB19" s="103" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="98"/>
+      <c r="AC19" s="104"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9"/>
@@ -9456,14 +9474,14 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="97" t="s">
+      <c r="Z20" s="103" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="97"/>
-      <c r="AB20" s="97" t="s">
+      <c r="AA20" s="103"/>
+      <c r="AB20" s="103" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="98"/>
+      <c r="AC20" s="104"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -9491,11 +9509,11 @@
       <c r="AC21" s="36"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="103"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="107"/>
       <c r="G22" s="9"/>
       <c r="H22" s="35"/>
       <c r="I22" s="35"/>
@@ -9524,10 +9542,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="97" t="s">
+      <c r="C23" s="103" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="98"/>
+      <c r="D23" s="104"/>
       <c r="G23" s="8">
         <v>44805</v>
       </c>
@@ -9553,10 +9571,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="97">
+      <c r="C24" s="103">
         <v>1969</v>
       </c>
-      <c r="D24" s="98"/>
+      <c r="D24" s="104"/>
       <c r="G24" s="9"/>
       <c r="H24" s="35"/>
       <c r="I24" s="35"/>
@@ -9578,8 +9596,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="98"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="104"/>
       <c r="G25" s="9"/>
       <c r="H25" s="35"/>
       <c r="I25" s="35"/>
@@ -9603,11 +9621,11 @@
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="104">
+      <c r="C26" s="121">
         <f>'Financial Model'!U68</f>
         <v>2678.6</v>
       </c>
-      <c r="D26" s="105"/>
+      <c r="D26" s="122"/>
       <c r="G26" s="8">
         <v>44805</v>
       </c>
@@ -9633,8 +9651,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="98"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="104"/>
       <c r="G27" s="9"/>
       <c r="H27" s="7" t="s">
         <v>192</v>
@@ -9649,7 +9667,7 @@
       <c r="P27" s="35"/>
       <c r="Q27" s="35"/>
       <c r="R27" s="36"/>
-      <c r="T27" s="124" t="s">
+      <c r="T27" s="98" t="s">
         <v>267</v>
       </c>
       <c r="U27" s="35"/>
@@ -9660,8 +9678,8 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="97"/>
-      <c r="D28" s="98"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="104"/>
       <c r="G28" s="9"/>
       <c r="H28" s="7" t="s">
         <v>193</v>
@@ -9687,11 +9705,11 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="116">
+      <c r="C29" s="114">
         <f>'Order &amp; Backlog'!T21</f>
         <v>297</v>
       </c>
-      <c r="D29" s="98"/>
+      <c r="D29" s="104"/>
       <c r="G29" s="9"/>
       <c r="H29" s="7" t="s">
         <v>191</v>
@@ -9719,11 +9737,11 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="97">
+      <c r="C30" s="103">
         <f>'Financial Model'!T43</f>
         <v>32</v>
       </c>
-      <c r="D30" s="98"/>
+      <c r="D30" s="104"/>
       <c r="G30" s="9"/>
       <c r="H30" s="35"/>
       <c r="I30" s="35"/>
@@ -9745,10 +9763,10 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="117">
+      <c r="C31" s="115">
         <v>36708</v>
       </c>
-      <c r="D31" s="118"/>
+      <c r="D31" s="116"/>
       <c r="G31" s="9"/>
       <c r="H31" s="35"/>
       <c r="I31" s="35"/>
@@ -9770,8 +9788,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="98"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="104"/>
       <c r="G32" s="8">
         <v>44743</v>
       </c>
@@ -9829,10 +9847,10 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="112" t="s">
+      <c r="C34" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="113"/>
+      <c r="D34" s="111"/>
       <c r="G34" s="9"/>
       <c r="H34" s="48" t="s">
         <v>198</v>
@@ -9885,11 +9903,11 @@
       <c r="R36" s="36"/>
     </row>
     <row r="37" spans="2:23">
-      <c r="B37" s="101" t="s">
+      <c r="B37" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="102"/>
-      <c r="D37" s="103"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="107"/>
       <c r="G37" s="9"/>
       <c r="H37" s="7" t="s">
         <v>240</v>
@@ -9904,22 +9922,22 @@
       <c r="P37" s="35"/>
       <c r="Q37" s="35"/>
       <c r="R37" s="36"/>
-      <c r="T37" s="101" t="s">
+      <c r="T37" s="105" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="102"/>
-      <c r="V37" s="102"/>
-      <c r="W37" s="103"/>
+      <c r="U37" s="106"/>
+      <c r="V37" s="106"/>
+      <c r="W37" s="107"/>
     </row>
     <row r="38" spans="2:23">
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="114">
+      <c r="C38" s="112">
         <f>C6/'Financial Model'!U122</f>
         <v>3.4899664342886649</v>
       </c>
-      <c r="D38" s="115"/>
+      <c r="D38" s="113"/>
       <c r="G38" s="9"/>
       <c r="H38" s="35"/>
       <c r="I38" s="35"/>
@@ -9943,11 +9961,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="114">
+      <c r="C39" s="112">
         <f>C6/'Financial Model'!AE9</f>
         <v>3.0687124749833226E-3</v>
       </c>
-      <c r="D39" s="115"/>
+      <c r="D39" s="113"/>
       <c r="G39" s="8">
         <v>44682</v>
       </c>
@@ -9975,11 +9993,11 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="110">
+      <c r="C40" s="108">
         <f>C6/'Financial Model'!AE26</f>
         <v>-211.69879194630872</v>
       </c>
-      <c r="D40" s="111"/>
+      <c r="D40" s="109"/>
       <c r="G40" s="9"/>
       <c r="H40" s="7" t="s">
         <v>249</v>
@@ -10046,11 +10064,11 @@
       <c r="W42" s="36"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="101" t="s">
+      <c r="B43" s="105" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="102"/>
-      <c r="D43" s="103"/>
+      <c r="C43" s="106"/>
+      <c r="D43" s="107"/>
       <c r="G43" s="9"/>
       <c r="H43" s="7" t="s">
         <v>169</v>
@@ -10073,10 +10091,10 @@
       <c r="W43" s="36"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="119" t="s">
+      <c r="B44" s="99" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="120"/>
+      <c r="C44" s="100"/>
       <c r="D44" s="49" t="s">
         <v>31</v>
       </c>
@@ -10104,10 +10122,10 @@
       </c>
     </row>
     <row r="45" spans="2:23">
-      <c r="B45" s="119" t="s">
+      <c r="B45" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="120"/>
+      <c r="C45" s="100"/>
       <c r="D45" s="49" t="s">
         <v>31</v>
       </c>
@@ -10125,8 +10143,8 @@
       <c r="R45" s="36"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
+      <c r="B46" s="99"/>
+      <c r="C46" s="100"/>
       <c r="D46" s="86" t="s">
         <v>31</v>
       </c>
@@ -10148,8 +10166,8 @@
       <c r="R46" s="36"/>
     </row>
     <row r="47" spans="2:23">
-      <c r="B47" s="119"/>
-      <c r="C47" s="120"/>
+      <c r="B47" s="99"/>
+      <c r="C47" s="100"/>
       <c r="D47" s="86" t="s">
         <v>31</v>
       </c>
@@ -10169,8 +10187,8 @@
       <c r="R47" s="36"/>
     </row>
     <row r="48" spans="2:23">
-      <c r="B48" s="121"/>
-      <c r="C48" s="122"/>
+      <c r="B48" s="101"/>
+      <c r="C48" s="102"/>
       <c r="D48" s="87" t="s">
         <v>31</v>
       </c>
@@ -10365,11 +10383,34 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
     <mergeCell ref="Z19:AA19"/>
     <mergeCell ref="AB19:AC19"/>
     <mergeCell ref="Z20:AA20"/>
@@ -10386,34 +10427,11 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -10448,10 +10466,10 @@
   <dimension ref="B1:AO147"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C85" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="U138" sqref="U138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -22622,8 +22640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG34" sqref="AG34"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -22644,7 +22662,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -22711,7 +22729,9 @@
       <c r="T1" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="U1" s="23"/>
+      <c r="U1" s="23" t="s">
+        <v>76</v>
+      </c>
       <c r="V1" s="23"/>
       <c r="X1" s="77">
         <v>2014</v>
@@ -22836,12 +22856,16 @@
         <v>1992</v>
       </c>
       <c r="S3" s="74">
-        <f t="shared" ref="S3:T3" si="14">SUM(S4:S10)</f>
+        <f t="shared" ref="S3:U3" si="14">SUM(S4:S10)</f>
         <v>2000</v>
       </c>
       <c r="T3" s="74">
         <f t="shared" si="14"/>
         <v>1995</v>
+      </c>
+      <c r="U3" s="74">
+        <f t="shared" si="14"/>
+        <v>2019</v>
       </c>
       <c r="X3" s="74">
         <f t="shared" ref="X3:AB3" si="15">SUM(X4:X10)</f>
@@ -22937,6 +22961,9 @@
       <c r="T4" s="75">
         <v>191</v>
       </c>
+      <c r="U4" s="75">
+        <v>191</v>
+      </c>
       <c r="X4" s="75">
         <v>193</v>
       </c>
@@ -23023,6 +23050,9 @@
       <c r="T5" s="75">
         <v>817</v>
       </c>
+      <c r="U5" s="75">
+        <v>818</v>
+      </c>
       <c r="X5" s="75">
         <v>421</v>
       </c>
@@ -23109,6 +23139,9 @@
       <c r="T6" s="75">
         <v>568</v>
       </c>
+      <c r="U6" s="75">
+        <v>568</v>
+      </c>
       <c r="X6" s="75">
         <v>580</v>
       </c>
@@ -23195,6 +23228,9 @@
       <c r="T7" s="75">
         <v>172</v>
       </c>
+      <c r="U7" s="75">
+        <v>172</v>
+      </c>
       <c r="X7" s="75">
         <v>145</v>
       </c>
@@ -23281,6 +23317,9 @@
       <c r="T8" s="75">
         <v>0</v>
       </c>
+      <c r="U8" s="75">
+        <v>0</v>
+      </c>
       <c r="X8" s="75">
         <v>100</v>
       </c>
@@ -23367,6 +23406,9 @@
       <c r="T9" s="75">
         <v>20</v>
       </c>
+      <c r="U9" s="75">
+        <v>25</v>
+      </c>
       <c r="X9" s="75">
         <v>60</v>
       </c>
@@ -23452,6 +23494,9 @@
       </c>
       <c r="T10" s="75">
         <v>227</v>
+      </c>
+      <c r="U10" s="75">
+        <v>245</v>
       </c>
       <c r="X10" s="75">
         <v>50</v>
@@ -23559,6 +23604,10 @@
         <f>SUM(T13:T19)</f>
         <v>1698</v>
       </c>
+      <c r="U12" s="74">
+        <f>SUM(U13:U19)</f>
+        <v>1728</v>
+      </c>
       <c r="X12" s="74">
         <f t="shared" ref="X12:AE12" si="20">SUM(X13:X19)</f>
         <v>1090</v>
@@ -23653,6 +23702,9 @@
       <c r="T13" s="75">
         <v>191</v>
       </c>
+      <c r="U13" s="75">
+        <v>191</v>
+      </c>
       <c r="X13" s="75">
         <v>188</v>
       </c>
@@ -23739,6 +23791,9 @@
       <c r="T14" s="75">
         <v>714</v>
       </c>
+      <c r="U14" s="75">
+        <v>728</v>
+      </c>
       <c r="X14" s="75">
         <v>249</v>
       </c>
@@ -23825,6 +23880,9 @@
       <c r="T15" s="75">
         <v>565</v>
       </c>
+      <c r="U15" s="75">
+        <v>568</v>
+      </c>
       <c r="X15" s="75">
         <v>515</v>
       </c>
@@ -23911,6 +23969,9 @@
       <c r="T16" s="75">
         <v>172</v>
       </c>
+      <c r="U16" s="75">
+        <v>172</v>
+      </c>
       <c r="X16" s="75">
         <v>138</v>
       </c>
@@ -23997,6 +24058,9 @@
       <c r="T17" s="75">
         <v>0</v>
       </c>
+      <c r="U17" s="75">
+        <v>0</v>
+      </c>
       <c r="X17" s="75">
         <v>0</v>
       </c>
@@ -24083,6 +24147,9 @@
       <c r="T18" s="75">
         <v>17</v>
       </c>
+      <c r="U18" s="75">
+        <v>18</v>
+      </c>
       <c r="X18" s="75">
         <v>0</v>
       </c>
@@ -24168,6 +24235,9 @@
       </c>
       <c r="T19" s="75">
         <v>39</v>
+      </c>
+      <c r="U19" s="75">
+        <v>51</v>
       </c>
       <c r="X19" s="75">
         <v>0</v>
@@ -24202,7 +24272,7 @@
         <v>209</v>
       </c>
       <c r="B21" s="74">
-        <f t="shared" ref="B21:T21" si="21">SUM(B22:B28)</f>
+        <f t="shared" ref="B21:U21" si="21">SUM(B22:B28)</f>
         <v>421</v>
       </c>
       <c r="C21" s="74">
@@ -24276,6 +24346,10 @@
       <c r="T21" s="74">
         <f t="shared" si="21"/>
         <v>297</v>
+      </c>
+      <c r="U21" s="74">
+        <f t="shared" si="21"/>
+        <v>291</v>
       </c>
       <c r="X21" s="74">
         <f t="shared" ref="X21:AE21" si="22">SUM(X22:X28)</f>
@@ -24371,6 +24445,9 @@
       <c r="T22" s="75">
         <v>0</v>
       </c>
+      <c r="U22" s="75">
+        <v>0</v>
+      </c>
       <c r="X22" s="75">
         <v>5</v>
       </c>
@@ -24457,6 +24534,9 @@
       <c r="T23" s="75">
         <v>103</v>
       </c>
+      <c r="U23" s="75">
+        <v>90</v>
+      </c>
       <c r="X23" s="75">
         <v>172</v>
       </c>
@@ -24543,6 +24623,9 @@
       <c r="T24" s="75">
         <v>3</v>
       </c>
+      <c r="U24" s="75">
+        <v>0</v>
+      </c>
       <c r="X24" s="75">
         <v>65</v>
       </c>
@@ -24629,6 +24712,9 @@
       <c r="T25" s="75">
         <v>0</v>
       </c>
+      <c r="U25" s="75">
+        <v>0</v>
+      </c>
       <c r="X25" s="75">
         <v>7</v>
       </c>
@@ -24715,6 +24801,9 @@
       <c r="T26" s="75">
         <v>0</v>
       </c>
+      <c r="U26" s="75">
+        <v>0</v>
+      </c>
       <c r="X26" s="75">
         <v>100</v>
       </c>
@@ -24801,6 +24890,9 @@
       <c r="T27" s="75">
         <v>3</v>
       </c>
+      <c r="U27" s="75">
+        <v>7</v>
+      </c>
       <c r="X27" s="75">
         <v>60</v>
       </c>
@@ -24887,6 +24979,9 @@
       <c r="T28" s="75">
         <v>188</v>
       </c>
+      <c r="U28" s="75">
+        <v>194</v>
+      </c>
       <c r="X28" s="75">
         <v>50</v>
       </c>
@@ -24988,23 +25083,27 @@
         <f>T3/P3-1</f>
         <v>1.3719512195121908E-2</v>
       </c>
+      <c r="U31" s="32">
+        <f t="shared" ref="U31" si="30">U3/Q3-1</f>
+        <v>1.1523046092184464E-2</v>
+      </c>
       <c r="X31" s="60" t="s">
         <v>186</v>
       </c>
       <c r="Y31" s="32">
-        <f t="shared" ref="Y31" si="30">Y3/X3-1</f>
+        <f t="shared" ref="Y31" si="31">Y3/X3-1</f>
         <v>0.1000645577792123</v>
       </c>
       <c r="Z31" s="32">
-        <f t="shared" ref="Z31" si="31">Z3/Y3-1</f>
+        <f t="shared" ref="Z31" si="32">Z3/Y3-1</f>
         <v>2.6408450704225261E-2</v>
       </c>
       <c r="AA31" s="32">
-        <f t="shared" ref="AA31:AB31" si="32">AA3/Z3-1</f>
+        <f t="shared" ref="AA31:AB31" si="33">AA3/Z3-1</f>
         <v>4.9170954831332159E-2</v>
       </c>
       <c r="AB31" s="32">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.2534059945504161E-2</v>
       </c>
       <c r="AC31" s="32">
@@ -25037,31 +25136,31 @@
         <v>186</v>
       </c>
       <c r="F32" s="78">
-        <f t="shared" ref="F32" si="33">F3-B3</f>
+        <f t="shared" ref="F32" si="34">F3-B3</f>
         <v>25</v>
       </c>
       <c r="G32" s="78">
-        <f t="shared" ref="G32" si="34">G3-C3</f>
+        <f t="shared" ref="G32" si="35">G3-C3</f>
         <v>88</v>
       </c>
       <c r="H32" s="78">
-        <f t="shared" ref="H32" si="35">H3-D3</f>
+        <f t="shared" ref="H32" si="36">H3-D3</f>
         <v>181</v>
       </c>
       <c r="I32" s="78">
-        <f t="shared" ref="I32:L32" si="36">I3-E3</f>
+        <f t="shared" ref="I32:L32" si="37">I3-E3</f>
         <v>59</v>
       </c>
       <c r="J32" s="78">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>42</v>
       </c>
       <c r="K32" s="78">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>12</v>
       </c>
       <c r="L32" s="78">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>13</v>
       </c>
       <c r="M32" s="78">
@@ -25069,15 +25168,15 @@
         <v>-13</v>
       </c>
       <c r="N32" s="78">
-        <f t="shared" ref="N32" si="37">N3-J3</f>
+        <f t="shared" ref="N32" si="38">N3-J3</f>
         <v>2</v>
       </c>
       <c r="O32" s="78">
-        <f t="shared" ref="O32" si="38">O3-K3</f>
+        <f t="shared" ref="O32" si="39">O3-K3</f>
         <v>50</v>
       </c>
       <c r="P32" s="78">
-        <f t="shared" ref="P32" si="39">P3-L3</f>
+        <f t="shared" ref="P32" si="40">P3-L3</f>
         <v>66</v>
       </c>
       <c r="Q32" s="78">
@@ -25096,23 +25195,27 @@
         <f>T3-P3</f>
         <v>27</v>
       </c>
+      <c r="U32" s="78">
+        <f t="shared" ref="U32" si="41">U3-Q3</f>
+        <v>23</v>
+      </c>
       <c r="X32" s="60" t="s">
         <v>186</v>
       </c>
       <c r="Y32" s="78">
-        <f t="shared" ref="Y32" si="40">Y3-X3</f>
+        <f t="shared" ref="Y32" si="42">Y3-X3</f>
         <v>155</v>
       </c>
       <c r="Z32" s="78">
-        <f t="shared" ref="Z32" si="41">Z3-Y3</f>
+        <f t="shared" ref="Z32" si="43">Z3-Y3</f>
         <v>45</v>
       </c>
       <c r="AA32" s="78">
-        <f t="shared" ref="AA32:AB32" si="42">AA3-Z3</f>
+        <f t="shared" ref="AA32:AB32" si="44">AA3-Z3</f>
         <v>86</v>
       </c>
       <c r="AB32" s="78">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>23</v>
       </c>
       <c r="AC32" s="78">
@@ -25136,76 +25239,80 @@
         <v>186</v>
       </c>
       <c r="C33" s="24">
-        <f t="shared" ref="C33" si="43">C3/B3-1</f>
+        <f t="shared" ref="C33" si="45">C3/B3-1</f>
         <v>-1.7983651226158082E-2</v>
       </c>
       <c r="D33" s="24">
-        <f t="shared" ref="D33" si="44">D3/C3-1</f>
+        <f t="shared" ref="D33" si="46">D3/C3-1</f>
         <v>-5.2164261931187617E-2</v>
       </c>
       <c r="E33" s="24">
-        <f t="shared" ref="E33" si="45">E3/D3-1</f>
+        <f t="shared" ref="E33" si="47">E3/D3-1</f>
         <v>8.7822014051522235E-2</v>
       </c>
       <c r="F33" s="24">
-        <f t="shared" ref="F33" si="46">F3/E3-1</f>
+        <f t="shared" ref="F33" si="48">F3/E3-1</f>
         <v>1.0764262648008671E-3</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" ref="G33" si="47">G3/F3-1</f>
+        <f t="shared" ref="G33" si="49">G3/F3-1</f>
         <v>1.6129032258064502E-2</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" ref="H33" si="48">H3/G3-1</f>
+        <f t="shared" ref="H33" si="50">H3/G3-1</f>
         <v>-5.2910052910049021E-4</v>
       </c>
       <c r="I33" s="24">
-        <f t="shared" ref="I33" si="49">I3/H3-1</f>
+        <f t="shared" ref="I33" si="51">I3/H3-1</f>
         <v>1.4822657490735747E-2</v>
       </c>
       <c r="J33" s="24">
-        <f t="shared" ref="J33" si="50">J3/I3-1</f>
+        <f t="shared" ref="J33" si="52">J3/I3-1</f>
         <v>-7.8247261345852914E-3</v>
       </c>
       <c r="K33" s="24">
-        <f t="shared" ref="K33" si="51">K3/J3-1</f>
+        <f t="shared" ref="K33" si="53">K3/J3-1</f>
         <v>0</v>
       </c>
       <c r="L33" s="24">
-        <f t="shared" ref="L33" si="52">L3/K3-1</f>
+        <f t="shared" ref="L33" si="54">L3/K3-1</f>
         <v>0</v>
       </c>
       <c r="M33" s="24">
-        <f t="shared" ref="M33" si="53">M3/L3-1</f>
+        <f t="shared" ref="M33" si="55">M3/L3-1</f>
         <v>1.051524710830698E-3</v>
       </c>
       <c r="N33" s="24">
-        <f t="shared" ref="N33" si="54">N3/M3-1</f>
+        <f t="shared" ref="N33" si="56">N3/M3-1</f>
         <v>0</v>
       </c>
       <c r="O33" s="24">
-        <f t="shared" ref="O33" si="55">O3/N3-1</f>
+        <f t="shared" ref="O33" si="57">O3/N3-1</f>
         <v>2.5210084033613356E-2</v>
       </c>
       <c r="P33" s="24">
-        <f t="shared" ref="P33:T33" si="56">P3/O3-1</f>
+        <f t="shared" ref="P33:T33" si="58">P3/O3-1</f>
         <v>8.1967213114753079E-3</v>
       </c>
       <c r="Q33" s="24">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>1.4227642276422703E-2</v>
       </c>
       <c r="R33" s="24">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>-2.0040080160320661E-3</v>
       </c>
       <c r="S33" s="24">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>4.0160642570281624E-3</v>
       </c>
       <c r="T33" s="24">
-        <f t="shared" si="56"/>
+        <f t="shared" si="58"/>
         <v>-2.4999999999999467E-3</v>
+      </c>
+      <c r="U33" s="24">
+        <f t="shared" ref="U33" si="59">U3/T3-1</f>
+        <v>1.2030075187969835E-2</v>
       </c>
       <c r="X33" s="60" t="s">
         <v>186</v>
@@ -25240,76 +25347,80 @@
         <v>186</v>
       </c>
       <c r="C34" s="78">
-        <f t="shared" ref="C34" si="57">C3-B3</f>
+        <f t="shared" ref="C34" si="60">C3-B3</f>
         <v>-33</v>
       </c>
       <c r="D34" s="78">
-        <f t="shared" ref="D34" si="58">D3-C3</f>
+        <f t="shared" ref="D34" si="61">D3-C3</f>
         <v>-94</v>
       </c>
       <c r="E34" s="78">
-        <f t="shared" ref="E34" si="59">E3-D3</f>
+        <f t="shared" ref="E34" si="62">E3-D3</f>
         <v>150</v>
       </c>
       <c r="F34" s="78">
-        <f t="shared" ref="F34" si="60">F3-E3</f>
+        <f t="shared" ref="F34" si="63">F3-E3</f>
         <v>2</v>
       </c>
       <c r="G34" s="78">
-        <f t="shared" ref="G34" si="61">G3-F3</f>
+        <f t="shared" ref="G34" si="64">G3-F3</f>
         <v>30</v>
       </c>
       <c r="H34" s="78">
-        <f t="shared" ref="H34" si="62">H3-G3</f>
+        <f t="shared" ref="H34" si="65">H3-G3</f>
         <v>-1</v>
       </c>
       <c r="I34" s="78">
-        <f t="shared" ref="I34" si="63">I3-H3</f>
+        <f t="shared" ref="I34" si="66">I3-H3</f>
         <v>28</v>
       </c>
       <c r="J34" s="78">
-        <f t="shared" ref="J34" si="64">J3-I3</f>
+        <f t="shared" ref="J34" si="67">J3-I3</f>
         <v>-15</v>
       </c>
       <c r="K34" s="78">
-        <f t="shared" ref="K34" si="65">K3-J3</f>
+        <f t="shared" ref="K34" si="68">K3-J3</f>
         <v>0</v>
       </c>
       <c r="L34" s="78">
-        <f t="shared" ref="L34" si="66">L3-K3</f>
+        <f t="shared" ref="L34" si="69">L3-K3</f>
         <v>0</v>
       </c>
       <c r="M34" s="78">
-        <f t="shared" ref="M34" si="67">M3-L3</f>
+        <f t="shared" ref="M34" si="70">M3-L3</f>
         <v>2</v>
       </c>
       <c r="N34" s="78">
-        <f t="shared" ref="N34" si="68">N3-M3</f>
+        <f t="shared" ref="N34" si="71">N3-M3</f>
         <v>0</v>
       </c>
       <c r="O34" s="78">
-        <f t="shared" ref="O34" si="69">O3-N3</f>
+        <f t="shared" ref="O34" si="72">O3-N3</f>
         <v>48</v>
       </c>
       <c r="P34" s="78">
-        <f t="shared" ref="P34:T34" si="70">P3-O3</f>
+        <f t="shared" ref="P34:T34" si="73">P3-O3</f>
         <v>16</v>
       </c>
       <c r="Q34" s="78">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>28</v>
       </c>
       <c r="R34" s="78">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>-4</v>
       </c>
       <c r="S34" s="78">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>8</v>
       </c>
       <c r="T34" s="78">
-        <f t="shared" si="70"/>
+        <f t="shared" si="73"/>
         <v>-5</v>
+      </c>
+      <c r="U34" s="78">
+        <f t="shared" ref="U34" si="74">U3-T3</f>
+        <v>24</v>
       </c>
       <c r="X34" s="60" t="s">
         <v>186</v>
@@ -25356,31 +25467,31 @@
         <v>186</v>
       </c>
       <c r="F36" s="32">
-        <f t="shared" ref="F36" si="71">F12/B12-1</f>
+        <f t="shared" ref="F36" si="75">F12/B12-1</f>
         <v>6.1527581329561487E-2</v>
       </c>
       <c r="G36" s="32">
-        <f t="shared" ref="G36" si="72">G12/C12-1</f>
+        <f t="shared" ref="G36" si="76">G12/C12-1</f>
         <v>5.8945908460471541E-2</v>
       </c>
       <c r="H36" s="32">
-        <f t="shared" ref="H36" si="73">H12/D12-1</f>
+        <f t="shared" ref="H36" si="77">H12/D12-1</f>
         <v>5.9711736444749475E-2</v>
       </c>
       <c r="I36" s="32">
-        <f t="shared" ref="I36:L36" si="74">I12/E12-1</f>
+        <f t="shared" ref="I36:L36" si="78">I12/E12-1</f>
         <v>5.9731543624160999E-2</v>
       </c>
       <c r="J36" s="32">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>5.5296469020652994E-2</v>
       </c>
       <c r="K36" s="32">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>3.9947609692206898E-2</v>
       </c>
       <c r="L36" s="32">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>3.303108808290145E-2</v>
       </c>
       <c r="M36" s="32">
@@ -25388,15 +25499,15 @@
         <v>2.7865737808739688E-2</v>
       </c>
       <c r="N36" s="32">
-        <f t="shared" ref="N36" si="75">N12/J12-1</f>
+        <f t="shared" ref="N36" si="79">N12/J12-1</f>
         <v>3.0303030303030276E-2</v>
       </c>
       <c r="O36" s="32">
-        <f t="shared" ref="O36" si="76">O12/K12-1</f>
+        <f t="shared" ref="O36" si="80">O12/K12-1</f>
         <v>3.6523929471032668E-2</v>
       </c>
       <c r="P36" s="32">
-        <f t="shared" ref="P36" si="77">P12/L12-1</f>
+        <f t="shared" ref="P36" si="81">P12/L12-1</f>
         <v>3.7617554858934144E-2</v>
       </c>
       <c r="Q36" s="32">
@@ -25415,23 +25526,27 @@
         <f>T12/P12-1</f>
         <v>2.5981873111782461E-2</v>
       </c>
+      <c r="U36" s="32">
+        <f t="shared" ref="U36" si="82">U12/Q12-1</f>
+        <v>3.4111310592459532E-2</v>
+      </c>
       <c r="X36" s="60" t="s">
         <v>186</v>
       </c>
       <c r="Y36" s="32">
-        <f t="shared" ref="Y36" si="78">Y12/X12-1</f>
+        <f t="shared" ref="Y36" si="83">Y12/X12-1</f>
         <v>8.3486238532110013E-2</v>
       </c>
       <c r="Z36" s="32">
-        <f t="shared" ref="Z36" si="79">Z12/Y12-1</f>
+        <f t="shared" ref="Z36" si="84">Z12/Y12-1</f>
         <v>9.9915325994919479E-2</v>
       </c>
       <c r="AA36" s="32">
-        <f t="shared" ref="AA36:AB36" si="80">AA12/Z12-1</f>
+        <f t="shared" ref="AA36:AB36" si="85">AA12/Z12-1</f>
         <v>7.7752117013087041E-2</v>
       </c>
       <c r="AB36" s="32">
-        <f t="shared" si="80"/>
+        <f t="shared" si="85"/>
         <v>6.4285714285714279E-2</v>
       </c>
       <c r="AC36" s="32">
@@ -25464,31 +25579,31 @@
         <v>186</v>
       </c>
       <c r="F37" s="78">
-        <f t="shared" ref="F37" si="81">F12-B12</f>
+        <f t="shared" ref="F37" si="86">F12-B12</f>
         <v>87</v>
       </c>
       <c r="G37" s="78">
-        <f t="shared" ref="G37" si="82">G12-C12</f>
+        <f t="shared" ref="G37" si="87">G12-C12</f>
         <v>85</v>
       </c>
       <c r="H37" s="78">
-        <f t="shared" ref="H37" si="83">H12-D12</f>
+        <f t="shared" ref="H37" si="88">H12-D12</f>
         <v>87</v>
       </c>
       <c r="I37" s="78">
-        <f t="shared" ref="I37:L37" si="84">I12-E12</f>
+        <f t="shared" ref="I37:L37" si="89">I12-E12</f>
         <v>89</v>
       </c>
       <c r="J37" s="78">
-        <f t="shared" si="84"/>
+        <f t="shared" si="89"/>
         <v>83</v>
       </c>
       <c r="K37" s="78">
-        <f t="shared" si="84"/>
+        <f t="shared" si="89"/>
         <v>61</v>
       </c>
       <c r="L37" s="78">
-        <f t="shared" si="84"/>
+        <f t="shared" si="89"/>
         <v>51</v>
       </c>
       <c r="M37" s="78">
@@ -25496,15 +25611,15 @@
         <v>44</v>
       </c>
       <c r="N37" s="78">
-        <f t="shared" ref="N37" si="85">N12-J12</f>
+        <f t="shared" ref="N37" si="90">N12-J12</f>
         <v>48</v>
       </c>
       <c r="O37" s="78">
-        <f t="shared" ref="O37" si="86">O12-K12</f>
+        <f t="shared" ref="O37" si="91">O12-K12</f>
         <v>58</v>
       </c>
       <c r="P37" s="78">
-        <f t="shared" ref="P37" si="87">P12-L12</f>
+        <f t="shared" ref="P37" si="92">P12-L12</f>
         <v>60</v>
       </c>
       <c r="Q37" s="78">
@@ -25523,23 +25638,27 @@
         <f>T12-P12</f>
         <v>43</v>
       </c>
+      <c r="U37" s="78">
+        <f t="shared" ref="U37" si="93">U12-Q12</f>
+        <v>57</v>
+      </c>
       <c r="X37" s="60" t="s">
         <v>186</v>
       </c>
       <c r="Y37" s="78">
-        <f t="shared" ref="Y37" si="88">Y12-X12</f>
+        <f t="shared" ref="Y37" si="94">Y12-X12</f>
         <v>91</v>
       </c>
       <c r="Z37" s="78">
-        <f t="shared" ref="Z37" si="89">Z12-Y12</f>
+        <f t="shared" ref="Z37" si="95">Z12-Y12</f>
         <v>118</v>
       </c>
       <c r="AA37" s="78">
-        <f t="shared" ref="AA37:AB37" si="90">AA12-Z12</f>
+        <f t="shared" ref="AA37:AB37" si="96">AA12-Z12</f>
         <v>101</v>
       </c>
       <c r="AB37" s="78">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>90</v>
       </c>
       <c r="AC37" s="78">
@@ -25563,76 +25682,80 @@
         <v>186</v>
       </c>
       <c r="C38" s="24">
-        <f t="shared" ref="C38" si="91">C12/B12-1</f>
+        <f t="shared" ref="C38" si="97">C12/B12-1</f>
         <v>1.980198019801982E-2</v>
       </c>
       <c r="D38" s="24">
-        <f t="shared" ref="D38" si="92">D12/C12-1</f>
+        <f t="shared" ref="D38" si="98">D12/C12-1</f>
         <v>1.0402219140083213E-2</v>
       </c>
       <c r="E38" s="24">
-        <f t="shared" ref="E38" si="93">E12/D12-1</f>
+        <f t="shared" ref="E38" si="99">E12/D12-1</f>
         <v>2.2649279341111939E-2</v>
       </c>
       <c r="F38" s="24">
-        <f t="shared" ref="F38" si="94">F12/E12-1</f>
+        <f t="shared" ref="F38" si="100">F12/E12-1</f>
         <v>7.382550335570448E-3</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" ref="G38" si="95">G12/F12-1</f>
+        <f t="shared" ref="G38" si="101">G12/F12-1</f>
         <v>1.7321785476348994E-2</v>
       </c>
       <c r="H38" s="24">
-        <f t="shared" ref="H38" si="96">H12/G12-1</f>
+        <f t="shared" ref="H38" si="102">H12/G12-1</f>
         <v>1.1132940406024971E-2</v>
       </c>
       <c r="I38" s="24">
-        <f t="shared" ref="I38" si="97">I12/H12-1</f>
+        <f t="shared" ref="I38" si="103">I12/H12-1</f>
         <v>2.26683937823835E-2</v>
       </c>
       <c r="J38" s="24">
-        <f t="shared" ref="J38" si="98">J12/I12-1</f>
+        <f t="shared" ref="J38" si="104">J12/I12-1</f>
         <v>3.1665611146294292E-3</v>
       </c>
       <c r="K38" s="24">
-        <f t="shared" ref="K38" si="99">K12/J12-1</f>
+        <f t="shared" ref="K38" si="105">K12/J12-1</f>
         <v>2.525252525252597E-3</v>
       </c>
       <c r="L38" s="24">
-        <f t="shared" ref="L38" si="100">L12/K12-1</f>
+        <f t="shared" ref="L38" si="106">L12/K12-1</f>
         <v>4.4080604534004753E-3</v>
       </c>
       <c r="M38" s="24">
-        <f t="shared" ref="M38" si="101">M12/L12-1</f>
+        <f t="shared" ref="M38" si="107">M12/L12-1</f>
         <v>1.7554858934169193E-2</v>
       </c>
       <c r="N38" s="24">
-        <f t="shared" ref="N38" si="102">N12/M12-1</f>
+        <f t="shared" ref="N38" si="108">N12/M12-1</f>
         <v>5.5452865064695711E-3</v>
       </c>
       <c r="O38" s="24">
-        <f t="shared" ref="O38" si="103">O12/N12-1</f>
+        <f t="shared" ref="O38" si="109">O12/N12-1</f>
         <v>8.5784313725489891E-3</v>
       </c>
       <c r="P38" s="24">
-        <f t="shared" ref="P38:T38" si="104">P12/O12-1</f>
+        <f t="shared" ref="P38:T38" si="110">P12/O12-1</f>
         <v>5.4678007290400732E-3</v>
       </c>
       <c r="Q38" s="24">
-        <f t="shared" si="104"/>
+        <f t="shared" si="110"/>
         <v>9.6676737160121817E-3</v>
       </c>
       <c r="R38" s="24">
-        <f t="shared" si="104"/>
+        <f t="shared" si="110"/>
         <v>3.5906642728904536E-3</v>
       </c>
       <c r="S38" s="24">
-        <f t="shared" si="104"/>
+        <f t="shared" si="110"/>
         <v>6.5593321407275695E-3</v>
       </c>
       <c r="T38" s="24">
-        <f t="shared" si="104"/>
+        <f t="shared" si="110"/>
         <v>5.924170616113722E-3</v>
+      </c>
+      <c r="U38" s="24">
+        <f t="shared" ref="U38" si="111">U12/T12-1</f>
+        <v>1.7667844522968101E-2</v>
       </c>
       <c r="X38" s="60" t="s">
         <v>186</v>
@@ -25667,76 +25790,80 @@
         <v>186</v>
       </c>
       <c r="C39" s="78">
-        <f t="shared" ref="C39" si="105">C12-B12</f>
+        <f t="shared" ref="C39" si="112">C12-B12</f>
         <v>28</v>
       </c>
       <c r="D39" s="78">
-        <f t="shared" ref="D39" si="106">D12-C12</f>
+        <f t="shared" ref="D39" si="113">D12-C12</f>
         <v>15</v>
       </c>
       <c r="E39" s="78">
-        <f t="shared" ref="E39" si="107">E12-D12</f>
+        <f t="shared" ref="E39" si="114">E12-D12</f>
         <v>33</v>
       </c>
       <c r="F39" s="78">
-        <f t="shared" ref="F39" si="108">F12-E12</f>
+        <f t="shared" ref="F39" si="115">F12-E12</f>
         <v>11</v>
       </c>
       <c r="G39" s="78">
-        <f t="shared" ref="G39" si="109">G12-F12</f>
+        <f t="shared" ref="G39" si="116">G12-F12</f>
         <v>26</v>
       </c>
       <c r="H39" s="78">
-        <f t="shared" ref="H39" si="110">H12-G12</f>
+        <f t="shared" ref="H39" si="117">H12-G12</f>
         <v>17</v>
       </c>
       <c r="I39" s="78">
-        <f t="shared" ref="I39" si="111">I12-H12</f>
+        <f t="shared" ref="I39" si="118">I12-H12</f>
         <v>35</v>
       </c>
       <c r="J39" s="78">
-        <f t="shared" ref="J39" si="112">J12-I12</f>
+        <f t="shared" ref="J39" si="119">J12-I12</f>
         <v>5</v>
       </c>
       <c r="K39" s="78">
-        <f t="shared" ref="K39" si="113">K12-J12</f>
+        <f t="shared" ref="K39" si="120">K12-J12</f>
         <v>4</v>
       </c>
       <c r="L39" s="78">
-        <f t="shared" ref="L39" si="114">L12-K12</f>
+        <f t="shared" ref="L39" si="121">L12-K12</f>
         <v>7</v>
       </c>
       <c r="M39" s="78">
-        <f t="shared" ref="M39" si="115">M12-L12</f>
+        <f t="shared" ref="M39" si="122">M12-L12</f>
         <v>28</v>
       </c>
       <c r="N39" s="78">
-        <f t="shared" ref="N39" si="116">N12-M12</f>
+        <f t="shared" ref="N39" si="123">N12-M12</f>
         <v>9</v>
       </c>
       <c r="O39" s="78">
-        <f t="shared" ref="O39" si="117">O12-N12</f>
+        <f t="shared" ref="O39" si="124">O12-N12</f>
         <v>14</v>
       </c>
       <c r="P39" s="78">
-        <f t="shared" ref="P39:T39" si="118">P12-O12</f>
+        <f t="shared" ref="P39:T39" si="125">P12-O12</f>
         <v>9</v>
       </c>
       <c r="Q39" s="78">
-        <f t="shared" si="118"/>
+        <f t="shared" si="125"/>
         <v>16</v>
       </c>
       <c r="R39" s="78">
-        <f t="shared" si="118"/>
+        <f t="shared" si="125"/>
         <v>6</v>
       </c>
       <c r="S39" s="78">
-        <f t="shared" si="118"/>
+        <f t="shared" si="125"/>
         <v>11</v>
       </c>
       <c r="T39" s="78">
-        <f t="shared" si="118"/>
+        <f t="shared" si="125"/>
         <v>10</v>
+      </c>
+      <c r="U39" s="78">
+        <f t="shared" ref="U39" si="126">U12-T12</f>
+        <v>30</v>
       </c>
       <c r="X39" s="60" t="s">
         <v>186</v>
@@ -25783,51 +25910,51 @@
         <v>186</v>
       </c>
       <c r="F41" s="32">
-        <f t="shared" ref="F41" si="119">F21/B21-1</f>
+        <f t="shared" ref="F41" si="127">F21/B21-1</f>
         <v>-0.14726840855106893</v>
       </c>
       <c r="G41" s="32">
-        <f t="shared" ref="G41" si="120">G21/C21-1</f>
+        <f t="shared" ref="G41" si="128">G21/C21-1</f>
         <v>8.3333333333333037E-3</v>
       </c>
       <c r="H41" s="32">
-        <f t="shared" ref="H41" si="121">H21/D21-1</f>
+        <f t="shared" ref="H41" si="129">H21/D21-1</f>
         <v>0.3745019920318724</v>
       </c>
       <c r="I41" s="32">
-        <f t="shared" ref="I41" si="122">I21/E21-1</f>
+        <f t="shared" ref="I41" si="130">I21/E21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
       <c r="J41" s="32">
-        <f t="shared" ref="J41" si="123">J21/F21-1</f>
+        <f t="shared" ref="J41" si="131">J21/F21-1</f>
         <v>-0.11420612813370479</v>
       </c>
       <c r="K41" s="32">
-        <f t="shared" ref="K41" si="124">K21/G21-1</f>
+        <f t="shared" ref="K41" si="132">K21/G21-1</f>
         <v>-0.13498622589531684</v>
       </c>
       <c r="L41" s="32">
-        <f t="shared" ref="L41" si="125">L21/H21-1</f>
+        <f t="shared" ref="L41" si="133">L21/H21-1</f>
         <v>-0.11014492753623184</v>
       </c>
       <c r="M41" s="32">
-        <f t="shared" ref="M41" si="126">M21/I21-1</f>
+        <f t="shared" ref="M41" si="134">M21/I21-1</f>
         <v>-0.16863905325443784</v>
       </c>
       <c r="N41" s="32">
-        <f t="shared" ref="N41" si="127">N21/J21-1</f>
+        <f t="shared" ref="N41" si="135">N21/J21-1</f>
         <v>-0.14465408805031443</v>
       </c>
       <c r="O41" s="32">
-        <f t="shared" ref="O41" si="128">O21/K21-1</f>
+        <f t="shared" ref="O41" si="136">O21/K21-1</f>
         <v>-2.5477707006369421E-2</v>
       </c>
       <c r="P41" s="32">
-        <f t="shared" ref="P41" si="129">P21/L21-1</f>
+        <f t="shared" ref="P41" si="137">P21/L21-1</f>
         <v>1.9543973941368087E-2</v>
       </c>
       <c r="Q41" s="32">
-        <f t="shared" ref="Q41" si="130">Q21/M21-1</f>
+        <f t="shared" ref="Q41" si="138">Q21/M21-1</f>
         <v>0.15658362989323837</v>
       </c>
       <c r="R41" s="32">
@@ -25835,34 +25962,38 @@
         <v>0.15808823529411775</v>
       </c>
       <c r="S41" s="32">
-        <f t="shared" ref="S41:T41" si="131">S21/O21-1</f>
+        <f t="shared" ref="S41:T41" si="139">S21/O21-1</f>
         <v>1.9607843137254832E-2</v>
       </c>
       <c r="T41" s="32">
-        <f t="shared" si="131"/>
+        <f t="shared" si="139"/>
         <v>-5.1118210862619806E-2</v>
+      </c>
+      <c r="U41" s="32">
+        <f t="shared" ref="U41" si="140">U21/Q21-1</f>
+        <v>-0.10461538461538467</v>
       </c>
       <c r="X41" s="60" t="s">
         <v>186</v>
       </c>
       <c r="Y41" s="32">
-        <f t="shared" ref="Y41" si="132">Y21/X21-1</f>
+        <f t="shared" ref="Y41" si="141">Y21/X21-1</f>
         <v>0.11764705882352944</v>
       </c>
       <c r="Z41" s="32">
-        <f t="shared" ref="Z41" si="133">Z21/Y21-1</f>
+        <f t="shared" ref="Z41" si="142">Z21/Y21-1</f>
         <v>-0.1228070175438597</v>
       </c>
       <c r="AA41" s="32">
-        <f t="shared" ref="AA41" si="134">AA21/Z21-1</f>
+        <f t="shared" ref="AA41" si="143">AA21/Z21-1</f>
         <v>-3.3333333333333326E-2</v>
       </c>
       <c r="AB41" s="32">
-        <f t="shared" ref="AB41" si="135">AB21/AA21-1</f>
+        <f t="shared" ref="AB41" si="144">AB21/AA21-1</f>
         <v>-0.15402298850574714</v>
       </c>
       <c r="AC41" s="32">
-        <f t="shared" ref="AC41" si="136">AC21/AB21-1</f>
+        <f t="shared" ref="AC41" si="145">AC21/AB21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
       <c r="AD41" s="32">
@@ -25891,31 +26022,31 @@
         <v>186</v>
       </c>
       <c r="F42" s="81">
-        <f t="shared" ref="F42" si="137">F21-B21</f>
+        <f t="shared" ref="F42" si="146">F21-B21</f>
         <v>-62</v>
       </c>
       <c r="G42" s="81">
-        <f t="shared" ref="G42" si="138">G21-C21</f>
+        <f t="shared" ref="G42" si="147">G21-C21</f>
         <v>3</v>
       </c>
       <c r="H42" s="81">
-        <f t="shared" ref="H42" si="139">H21-D21</f>
+        <f t="shared" ref="H42" si="148">H21-D21</f>
         <v>94</v>
       </c>
       <c r="I42" s="81">
-        <f t="shared" ref="I42:L42" si="140">I21-E21</f>
+        <f t="shared" ref="I42:L42" si="149">I21-E21</f>
         <v>-30</v>
       </c>
       <c r="J42" s="81">
-        <f t="shared" si="140"/>
+        <f t="shared" si="149"/>
         <v>-41</v>
       </c>
       <c r="K42" s="81">
-        <f t="shared" si="140"/>
+        <f t="shared" si="149"/>
         <v>-49</v>
       </c>
       <c r="L42" s="81">
-        <f t="shared" si="140"/>
+        <f t="shared" si="149"/>
         <v>-38</v>
       </c>
       <c r="M42" s="81">
@@ -25923,23 +26054,23 @@
         <v>-57</v>
       </c>
       <c r="N42" s="81">
-        <f t="shared" ref="N42" si="141">N21-J21</f>
+        <f t="shared" ref="N42" si="150">N21-J21</f>
         <v>-46</v>
       </c>
       <c r="O42" s="81">
-        <f t="shared" ref="O42" si="142">O21-K21</f>
+        <f t="shared" ref="O42" si="151">O21-K21</f>
         <v>-8</v>
       </c>
       <c r="P42" s="81">
-        <f t="shared" ref="P42" si="143">P21-L21</f>
+        <f t="shared" ref="P42" si="152">P21-L21</f>
         <v>6</v>
       </c>
       <c r="Q42" s="81">
-        <f t="shared" ref="Q42:R42" si="144">Q21-M21</f>
+        <f t="shared" ref="Q42:R42" si="153">Q21-M21</f>
         <v>44</v>
       </c>
       <c r="R42" s="81">
-        <f t="shared" si="144"/>
+        <f t="shared" si="153"/>
         <v>43</v>
       </c>
       <c r="S42" s="81">
@@ -25950,31 +26081,35 @@
         <f>T21-P21</f>
         <v>-16</v>
       </c>
+      <c r="U42" s="81">
+        <f t="shared" ref="U42" si="154">U21-Q21</f>
+        <v>-34</v>
+      </c>
       <c r="X42" s="60" t="s">
         <v>186</v>
       </c>
       <c r="Y42" s="81">
-        <f t="shared" ref="Y42" si="145">Y21-X21</f>
+        <f t="shared" ref="Y42" si="155">Y21-X21</f>
         <v>54</v>
       </c>
       <c r="Z42" s="81">
-        <f t="shared" ref="Z42" si="146">Z21-Y21</f>
+        <f t="shared" ref="Z42" si="156">Z21-Y21</f>
         <v>-63</v>
       </c>
       <c r="AA42" s="81">
-        <f t="shared" ref="AA42" si="147">AA21-Z21</f>
+        <f t="shared" ref="AA42" si="157">AA21-Z21</f>
         <v>-15</v>
       </c>
       <c r="AB42" s="81">
-        <f t="shared" ref="AB42" si="148">AB21-AA21</f>
+        <f t="shared" ref="AB42" si="158">AB21-AA21</f>
         <v>-67</v>
       </c>
       <c r="AC42" s="81">
-        <f t="shared" ref="AC42:AD42" si="149">AC21-AB21</f>
+        <f t="shared" ref="AC42:AD42" si="159">AC21-AB21</f>
         <v>-30</v>
       </c>
       <c r="AD42" s="81">
-        <f t="shared" si="149"/>
+        <f t="shared" si="159"/>
         <v>-57</v>
       </c>
       <c r="AE42" s="81">
@@ -25990,63 +26125,63 @@
         <v>186</v>
       </c>
       <c r="C43" s="24">
-        <f t="shared" ref="C43" si="150">C21/B21-1</f>
+        <f t="shared" ref="C43" si="160">C21/B21-1</f>
         <v>-0.14489311163895491</v>
       </c>
       <c r="D43" s="24">
-        <f t="shared" ref="D43" si="151">D21/C21-1</f>
+        <f t="shared" ref="D43" si="161">D21/C21-1</f>
         <v>-0.30277777777777781</v>
       </c>
       <c r="E43" s="24">
-        <f t="shared" ref="E43" si="152">E21/D21-1</f>
+        <f t="shared" ref="E43" si="162">E21/D21-1</f>
         <v>0.46613545816733071</v>
       </c>
       <c r="F43" s="24">
-        <f t="shared" ref="F43" si="153">F21/E21-1</f>
+        <f t="shared" ref="F43" si="163">F21/E21-1</f>
         <v>-2.4456521739130488E-2</v>
       </c>
       <c r="G43" s="24">
-        <f t="shared" ref="G43" si="154">G21/F21-1</f>
+        <f t="shared" ref="G43" si="164">G21/F21-1</f>
         <v>1.1142061281337101E-2</v>
       </c>
       <c r="H43" s="24">
-        <f t="shared" ref="H43" si="155">H21/G21-1</f>
+        <f t="shared" ref="H43" si="165">H21/G21-1</f>
         <v>-4.9586776859504078E-2</v>
       </c>
       <c r="I43" s="24">
-        <f t="shared" ref="I43" si="156">I21/H21-1</f>
+        <f t="shared" ref="I43" si="166">I21/H21-1</f>
         <v>-2.0289855072463725E-2</v>
       </c>
       <c r="J43" s="24">
-        <f t="shared" ref="J43" si="157">J21/I21-1</f>
+        <f t="shared" ref="J43" si="167">J21/I21-1</f>
         <v>-5.9171597633136064E-2</v>
       </c>
       <c r="K43" s="24">
-        <f t="shared" ref="K43" si="158">K21/J21-1</f>
+        <f t="shared" ref="K43" si="168">K21/J21-1</f>
         <v>-1.2578616352201255E-2</v>
       </c>
       <c r="L43" s="24">
-        <f t="shared" ref="L43" si="159">L21/K21-1</f>
+        <f t="shared" ref="L43" si="169">L21/K21-1</f>
         <v>-2.2292993630573243E-2</v>
       </c>
       <c r="M43" s="24">
-        <f t="shared" ref="M43" si="160">M21/L21-1</f>
+        <f t="shared" ref="M43" si="170">M21/L21-1</f>
         <v>-8.4690553745928376E-2</v>
       </c>
       <c r="N43" s="24">
-        <f t="shared" ref="N43" si="161">N21/M21-1</f>
+        <f t="shared" ref="N43" si="171">N21/M21-1</f>
         <v>-3.2028469750889688E-2</v>
       </c>
       <c r="O43" s="24">
-        <f t="shared" ref="O43" si="162">O21/N21-1</f>
+        <f t="shared" ref="O43" si="172">O21/N21-1</f>
         <v>0.125</v>
       </c>
       <c r="P43" s="24">
-        <f t="shared" ref="P43" si="163">P21/O21-1</f>
+        <f t="shared" ref="P43" si="173">P21/O21-1</f>
         <v>2.2875816993463971E-2</v>
       </c>
       <c r="Q43" s="24">
-        <f t="shared" ref="Q43" si="164">Q21/P21-1</f>
+        <f t="shared" ref="Q43" si="174">Q21/P21-1</f>
         <v>3.833865814696491E-2</v>
       </c>
       <c r="R43" s="24">
@@ -26054,12 +26189,16 @@
         <v>-3.0769230769230771E-2</v>
       </c>
       <c r="S43" s="24">
-        <f t="shared" ref="S43:T43" si="165">S21/R21-1</f>
+        <f t="shared" ref="S43:T43" si="175">S21/R21-1</f>
         <v>-9.52380952380949E-3</v>
       </c>
       <c r="T43" s="24">
-        <f t="shared" si="165"/>
+        <f t="shared" si="175"/>
         <v>-4.8076923076923128E-2</v>
+      </c>
+      <c r="U43" s="24">
+        <f t="shared" ref="U43" si="176">U21/T21-1</f>
+        <v>-2.0202020202020221E-2</v>
       </c>
       <c r="X43" s="60" t="s">
         <v>186</v>
@@ -26094,67 +26233,67 @@
         <v>186</v>
       </c>
       <c r="C44" s="78">
-        <f t="shared" ref="C44" si="166">C21-B21</f>
+        <f t="shared" ref="C44" si="177">C21-B21</f>
         <v>-61</v>
       </c>
       <c r="D44" s="78">
-        <f t="shared" ref="D44" si="167">D21-C21</f>
+        <f t="shared" ref="D44" si="178">D21-C21</f>
         <v>-109</v>
       </c>
       <c r="E44" s="78">
-        <f t="shared" ref="E44" si="168">E21-D21</f>
+        <f t="shared" ref="E44" si="179">E21-D21</f>
         <v>117</v>
       </c>
       <c r="F44" s="78">
-        <f t="shared" ref="F44" si="169">F21-E21</f>
+        <f t="shared" ref="F44" si="180">F21-E21</f>
         <v>-9</v>
       </c>
       <c r="G44" s="78">
-        <f t="shared" ref="G44" si="170">G21-F21</f>
+        <f t="shared" ref="G44" si="181">G21-F21</f>
         <v>4</v>
       </c>
       <c r="H44" s="78">
-        <f t="shared" ref="H44" si="171">H21-G21</f>
+        <f t="shared" ref="H44" si="182">H21-G21</f>
         <v>-18</v>
       </c>
       <c r="I44" s="78">
-        <f t="shared" ref="I44" si="172">I21-H21</f>
+        <f t="shared" ref="I44" si="183">I21-H21</f>
         <v>-7</v>
       </c>
       <c r="J44" s="78">
-        <f t="shared" ref="J44" si="173">J21-I21</f>
+        <f t="shared" ref="J44" si="184">J21-I21</f>
         <v>-20</v>
       </c>
       <c r="K44" s="78">
-        <f t="shared" ref="K44" si="174">K21-J21</f>
+        <f t="shared" ref="K44" si="185">K21-J21</f>
         <v>-4</v>
       </c>
       <c r="L44" s="78">
-        <f t="shared" ref="L44" si="175">L21-K21</f>
+        <f t="shared" ref="L44" si="186">L21-K21</f>
         <v>-7</v>
       </c>
       <c r="M44" s="78">
-        <f t="shared" ref="M44" si="176">M21-L21</f>
+        <f t="shared" ref="M44" si="187">M21-L21</f>
         <v>-26</v>
       </c>
       <c r="N44" s="78">
-        <f t="shared" ref="N44" si="177">N21-M21</f>
+        <f t="shared" ref="N44" si="188">N21-M21</f>
         <v>-9</v>
       </c>
       <c r="O44" s="78">
-        <f t="shared" ref="O44" si="178">O21-N21</f>
+        <f t="shared" ref="O44" si="189">O21-N21</f>
         <v>34</v>
       </c>
       <c r="P44" s="78">
-        <f t="shared" ref="P44:R44" si="179">P21-O21</f>
+        <f t="shared" ref="P44:R44" si="190">P21-O21</f>
         <v>7</v>
       </c>
       <c r="Q44" s="78">
-        <f t="shared" si="179"/>
+        <f t="shared" si="190"/>
         <v>12</v>
       </c>
       <c r="R44" s="78">
-        <f t="shared" si="179"/>
+        <f t="shared" si="190"/>
         <v>-10</v>
       </c>
       <c r="S44" s="78">
@@ -26164,6 +26303,10 @@
       <c r="T44" s="78">
         <f>T21-S21</f>
         <v>-15</v>
+      </c>
+      <c r="U44" s="78">
+        <f t="shared" ref="U44" si="191">U21-T21</f>
+        <v>-6</v>
       </c>
       <c r="X44" s="60" t="s">
         <v>186</v>
@@ -26195,111 +26338,115 @@
         <v>262</v>
       </c>
       <c r="B46" s="24">
-        <f t="shared" ref="B46:S46" si="180">B12/B3</f>
+        <f t="shared" ref="B46:S46" si="192">B12/B3</f>
         <v>0.77057220708446872</v>
       </c>
       <c r="C46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.80022197558268593</v>
       </c>
       <c r="D46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.85304449648711944</v>
       </c>
       <c r="E46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.80193756727664156</v>
       </c>
       <c r="F46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.80698924731182797</v>
       </c>
       <c r="G46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.80793650793650795</v>
       </c>
       <c r="H46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.81736368448914765</v>
       </c>
       <c r="I46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.82368283776734486</v>
       </c>
       <c r="J46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.83280757097791802</v>
       </c>
       <c r="K46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.83491062039957942</v>
       </c>
       <c r="L46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.83859095688748686</v>
       </c>
       <c r="M46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.85241596638655459</v>
       </c>
       <c r="N46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="O46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.84323770491803274</v>
       </c>
       <c r="P46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.84095528455284552</v>
       </c>
       <c r="Q46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.83717434869739482</v>
       </c>
       <c r="R46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.8418674698795181</v>
       </c>
       <c r="S46" s="24">
-        <f t="shared" si="180"/>
+        <f t="shared" si="192"/>
         <v>0.84399999999999997</v>
       </c>
       <c r="T46" s="24">
         <f>T12/T3</f>
         <v>0.85112781954887218</v>
       </c>
+      <c r="U46" s="24">
+        <f t="shared" ref="U46" si="193">U12/U3</f>
+        <v>0.85586924219910843</v>
+      </c>
       <c r="X46" s="24">
-        <f t="shared" ref="X46:AE46" si="181">X12/X3</f>
+        <f t="shared" ref="X46:AE46" si="194">X12/X3</f>
         <v>0.70367979341510656</v>
       </c>
       <c r="Y46" s="24">
-        <f t="shared" si="181"/>
+        <f t="shared" si="194"/>
         <v>0.693075117370892</v>
       </c>
       <c r="Z46" s="24">
-        <f t="shared" si="181"/>
+        <f t="shared" si="194"/>
         <v>0.74271012006861059</v>
       </c>
       <c r="AA46" s="24">
-        <f t="shared" si="181"/>
+        <f t="shared" si="194"/>
         <v>0.76294277929155319</v>
       </c>
       <c r="AB46" s="24">
-        <f t="shared" si="181"/>
+        <f t="shared" si="194"/>
         <v>0.80193756727664156</v>
       </c>
       <c r="AC46" s="24">
-        <f t="shared" si="181"/>
+        <f t="shared" si="194"/>
         <v>0.82368283776734486</v>
       </c>
       <c r="AD46" s="24">
-        <f t="shared" si="181"/>
+        <f t="shared" si="194"/>
         <v>0.85241596638655459</v>
       </c>
       <c r="AE46" s="24">
-        <f t="shared" si="181"/>
+        <f t="shared" si="194"/>
         <v>0.83717434869739482</v>
       </c>
     </row>
@@ -26338,9 +26485,10 @@
     <hyperlink ref="Y1" r:id="rId25" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/93a33ec4-dc07-47b3-91c2-d84b2e56d699?origin=1" xr:uid="{CE32064C-B077-40F4-9C44-3F45FE0A2ECE}"/>
     <hyperlink ref="X1" r:id="rId26" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a574642d-6cd1-4e80-a242-26ff2d0747f5?origin=1" xr:uid="{4A9206DD-D830-44D0-A5B0-DF41E9DD8391}"/>
     <hyperlink ref="T1" r:id="rId27" xr:uid="{F6F821CD-3C9C-4984-B9E1-54EA40AA851B}"/>
+    <hyperlink ref="U1" r:id="rId28" xr:uid="{8A371147-4AFA-4AEF-811C-DCBC2CB2AA7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId28"/>
-  <drawing r:id="rId29"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId29"/>
+  <drawing r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
£TEG latest interim results & other updates
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCA53E8-C918-44BE-B07F-E28A2C502DBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8641C22E-8C62-432F-BFD9-B4A97C9A1ED7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1465,22 +1465,16 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1490,6 +1484,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1519,28 +1531,16 @@
     <xf numFmtId="169" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8904,8 +8904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC59"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -8925,42 +8925,42 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
-      <c r="G5" s="105" t="s">
+      <c r="C5" s="104"/>
+      <c r="D5" s="105"/>
+      <c r="G5" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="T5" s="105" t="s">
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="104"/>
+      <c r="R5" s="105"/>
+      <c r="T5" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="107"/>
-      <c r="AA5" s="119" t="s">
+      <c r="U5" s="104"/>
+      <c r="V5" s="104"/>
+      <c r="W5" s="105"/>
+      <c r="AA5" s="101" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="120"/>
+      <c r="AB5" s="102"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>12.88</v>
+        <v>14.02</v>
       </c>
       <c r="D6" s="17"/>
       <c r="G6" s="8">
@@ -9029,7 +9029,7 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>9461.648000000001</v>
+        <v>10299.092000000001</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
@@ -9160,7 +9160,7 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>10834.848000000002</v>
+        <v>11672.292000000001</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
@@ -9183,13 +9183,13 @@
       <c r="U12" s="35"/>
       <c r="V12" s="35"/>
       <c r="W12" s="36"/>
-      <c r="Y12" s="105" t="s">
+      <c r="Y12" s="103" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="107"/>
+      <c r="Z12" s="104"/>
+      <c r="AA12" s="104"/>
+      <c r="AB12" s="104"/>
+      <c r="AC12" s="105"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -9211,14 +9211,14 @@
       <c r="V13" s="35"/>
       <c r="W13" s="36"/>
       <c r="Y13" s="89"/>
-      <c r="Z13" s="117" t="s">
+      <c r="Z13" s="110" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="117"/>
-      <c r="AB13" s="117" t="s">
+      <c r="AA13" s="110"/>
+      <c r="AB13" s="110" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="118"/>
+      <c r="AC13" s="111"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="9"/>
@@ -9242,21 +9242,21 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="103" t="s">
+      <c r="Z14" s="99" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="103"/>
-      <c r="AB14" s="103" t="s">
+      <c r="AA14" s="99"/>
+      <c r="AB14" s="99" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="104"/>
+      <c r="AC14" s="100"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="107"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="105"/>
       <c r="G15" s="8">
         <v>44835</v>
       </c>
@@ -9282,14 +9282,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="103" t="s">
+      <c r="Z15" s="99" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="103"/>
-      <c r="AB15" s="103" t="s">
+      <c r="AA15" s="99"/>
+      <c r="AB15" s="99" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="104"/>
+      <c r="AC15" s="100"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9298,10 +9298,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="103" t="s">
+      <c r="C16" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="104"/>
+      <c r="D16" s="100"/>
       <c r="E16" s="3" t="s">
         <v>265</v>
       </c>
@@ -9328,23 +9328,23 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="103" t="s">
+      <c r="Z16" s="99" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="103"/>
-      <c r="AB16" s="103" t="s">
+      <c r="AA16" s="99"/>
+      <c r="AB16" s="99" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="104"/>
+      <c r="AC16" s="100"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="103" t="s">
+      <c r="C17" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="104"/>
+      <c r="D17" s="100"/>
       <c r="E17" s="3" t="s">
         <v>265</v>
       </c>
@@ -9369,19 +9369,19 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="103" t="s">
+      <c r="Z17" s="99" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="103"/>
-      <c r="AB17" s="103" t="s">
+      <c r="AA17" s="99"/>
+      <c r="AB17" s="99" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="104"/>
+      <c r="AC17" s="100"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="103"/>
-      <c r="D18" s="104"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="100"/>
       <c r="G18" s="9"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
@@ -9403,19 +9403,19 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="103" t="s">
+      <c r="Z18" s="99" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="103"/>
-      <c r="AB18" s="103" t="s">
+      <c r="AA18" s="99"/>
+      <c r="AB18" s="99" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="104"/>
+      <c r="AC18" s="100"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="124"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="109"/>
       <c r="G19" s="8">
         <v>44835</v>
       </c>
@@ -9441,14 +9441,14 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="103" t="s">
+      <c r="Z19" s="99" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="103"/>
-      <c r="AB19" s="103" t="s">
+      <c r="AA19" s="99"/>
+      <c r="AB19" s="99" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="104"/>
+      <c r="AC19" s="100"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9"/>
@@ -9474,14 +9474,14 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="103" t="s">
+      <c r="Z20" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="103"/>
-      <c r="AB20" s="103" t="s">
+      <c r="AA20" s="99"/>
+      <c r="AB20" s="99" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="104"/>
+      <c r="AC20" s="100"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -9509,11 +9509,11 @@
       <c r="AC21" s="36"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="105"/>
       <c r="G22" s="9"/>
       <c r="H22" s="35"/>
       <c r="I22" s="35"/>
@@ -9542,10 +9542,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="103" t="s">
+      <c r="C23" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="104"/>
+      <c r="D23" s="100"/>
       <c r="G23" s="8">
         <v>44805</v>
       </c>
@@ -9571,10 +9571,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="103">
+      <c r="C24" s="99">
         <v>1969</v>
       </c>
-      <c r="D24" s="104"/>
+      <c r="D24" s="100"/>
       <c r="G24" s="9"/>
       <c r="H24" s="35"/>
       <c r="I24" s="35"/>
@@ -9596,8 +9596,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="103"/>
-      <c r="D25" s="104"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="100"/>
       <c r="G25" s="9"/>
       <c r="H25" s="35"/>
       <c r="I25" s="35"/>
@@ -9621,11 +9621,11 @@
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="121">
+      <c r="C26" s="106">
         <f>'Financial Model'!U68</f>
         <v>2678.6</v>
       </c>
-      <c r="D26" s="122"/>
+      <c r="D26" s="107"/>
       <c r="G26" s="8">
         <v>44805</v>
       </c>
@@ -9651,8 +9651,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="103"/>
-      <c r="D27" s="104"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="100"/>
       <c r="G27" s="9"/>
       <c r="H27" s="7" t="s">
         <v>192</v>
@@ -9678,8 +9678,8 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="104"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="100"/>
       <c r="G28" s="9"/>
       <c r="H28" s="7" t="s">
         <v>193</v>
@@ -9705,11 +9705,11 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="114">
-        <f>'Order &amp; Backlog'!T21</f>
-        <v>297</v>
-      </c>
-      <c r="D29" s="104"/>
+      <c r="C29" s="118">
+        <f>'Order &amp; Backlog'!U21</f>
+        <v>291</v>
+      </c>
+      <c r="D29" s="100"/>
       <c r="G29" s="9"/>
       <c r="H29" s="7" t="s">
         <v>191</v>
@@ -9737,11 +9737,11 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="103">
+      <c r="C30" s="99">
         <f>'Financial Model'!T43</f>
         <v>32</v>
       </c>
-      <c r="D30" s="104"/>
+      <c r="D30" s="100"/>
       <c r="G30" s="9"/>
       <c r="H30" s="35"/>
       <c r="I30" s="35"/>
@@ -9763,10 +9763,10 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="115">
+      <c r="C31" s="119">
         <v>36708</v>
       </c>
-      <c r="D31" s="116"/>
+      <c r="D31" s="120"/>
       <c r="G31" s="9"/>
       <c r="H31" s="35"/>
       <c r="I31" s="35"/>
@@ -9788,8 +9788,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="103"/>
-      <c r="D32" s="104"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="100"/>
       <c r="G32" s="8">
         <v>44743</v>
       </c>
@@ -9847,10 +9847,10 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="110" t="s">
+      <c r="C34" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="111"/>
+      <c r="D34" s="115"/>
       <c r="G34" s="9"/>
       <c r="H34" s="48" t="s">
         <v>198</v>
@@ -9903,11 +9903,11 @@
       <c r="R36" s="36"/>
     </row>
     <row r="37" spans="2:23">
-      <c r="B37" s="105" t="s">
+      <c r="B37" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107"/>
+      <c r="C37" s="104"/>
+      <c r="D37" s="105"/>
       <c r="G37" s="9"/>
       <c r="H37" s="7" t="s">
         <v>240</v>
@@ -9922,22 +9922,22 @@
       <c r="P37" s="35"/>
       <c r="Q37" s="35"/>
       <c r="R37" s="36"/>
-      <c r="T37" s="105" t="s">
+      <c r="T37" s="103" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="107"/>
+      <c r="U37" s="104"/>
+      <c r="V37" s="104"/>
+      <c r="W37" s="105"/>
     </row>
     <row r="38" spans="2:23">
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="112">
+      <c r="C38" s="116">
         <f>C6/'Financial Model'!U122</f>
-        <v>3.4899664342886649</v>
-      </c>
-      <c r="D38" s="113"/>
+        <v>3.7988609789384378</v>
+      </c>
+      <c r="D38" s="117"/>
       <c r="G38" s="9"/>
       <c r="H38" s="35"/>
       <c r="I38" s="35"/>
@@ -9961,11 +9961,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="112">
+      <c r="C39" s="116">
         <f>C6/'Financial Model'!AE9</f>
-        <v>3.0687124749833226E-3</v>
-      </c>
-      <c r="D39" s="113"/>
+        <v>3.3403221195082437E-3</v>
+      </c>
+      <c r="D39" s="117"/>
       <c r="G39" s="8">
         <v>44682</v>
       </c>
@@ -9993,11 +9993,11 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="108">
+      <c r="C40" s="112">
         <f>C6/'Financial Model'!AE26</f>
-        <v>-211.69879194630872</v>
-      </c>
-      <c r="D40" s="109"/>
+        <v>-230.43610738255032</v>
+      </c>
+      <c r="D40" s="113"/>
       <c r="G40" s="9"/>
       <c r="H40" s="7" t="s">
         <v>249</v>
@@ -10064,11 +10064,11 @@
       <c r="W42" s="36"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="106"/>
-      <c r="D43" s="107"/>
+      <c r="C43" s="104"/>
+      <c r="D43" s="105"/>
       <c r="G43" s="9"/>
       <c r="H43" s="7" t="s">
         <v>169</v>
@@ -10091,10 +10091,10 @@
       <c r="W43" s="36"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="99" t="s">
+      <c r="B44" s="121" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="100"/>
+      <c r="C44" s="122"/>
       <c r="D44" s="49" t="s">
         <v>31</v>
       </c>
@@ -10122,10 +10122,10 @@
       </c>
     </row>
     <row r="45" spans="2:23">
-      <c r="B45" s="99" t="s">
+      <c r="B45" s="121" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="100"/>
+      <c r="C45" s="122"/>
       <c r="D45" s="49" t="s">
         <v>31</v>
       </c>
@@ -10143,8 +10143,8 @@
       <c r="R45" s="36"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="B46" s="99"/>
-      <c r="C46" s="100"/>
+      <c r="B46" s="121"/>
+      <c r="C46" s="122"/>
       <c r="D46" s="86" t="s">
         <v>31</v>
       </c>
@@ -10166,8 +10166,8 @@
       <c r="R46" s="36"/>
     </row>
     <row r="47" spans="2:23">
-      <c r="B47" s="99"/>
-      <c r="C47" s="100"/>
+      <c r="B47" s="121"/>
+      <c r="C47" s="122"/>
       <c r="D47" s="86" t="s">
         <v>31</v>
       </c>
@@ -10187,8 +10187,8 @@
       <c r="R47" s="36"/>
     </row>
     <row r="48" spans="2:23">
-      <c r="B48" s="101"/>
-      <c r="C48" s="102"/>
+      <c r="B48" s="123"/>
+      <c r="C48" s="124"/>
       <c r="D48" s="87" t="s">
         <v>31</v>
       </c>
@@ -10383,6 +10383,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="T5:W5"/>
@@ -10399,39 +10432,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -10465,11 +10465,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
   <dimension ref="B1:AO147"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="I91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U138" sqref="U138"/>
+      <selection pane="bottomRight" activeCell="AE122" sqref="AE122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -22640,7 +22640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
£SDRY March pilot data + other misc updates
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3E02C6-EC24-4FEF-B3A1-47730B1AFA39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740E48A0-DD1C-4B43-977C-67D7F429BD75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -979,10 +979,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0\x"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0000\x"/>
-    <numFmt numFmtId="169" formatCode="mmmm\ yyyy;"/>
+    <numFmt numFmtId="165" formatCode="0.0\x"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000\x"/>
+    <numFmt numFmtId="168" formatCode="mmmm\ yyyy;"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1378,11 +1378,11 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -1410,7 +1410,7 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1466,22 +1466,20 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1491,45 +1489,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1544,10 +1503,51 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8993,8 +8993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9039,17 +9039,17 @@
       <c r="U5" s="105"/>
       <c r="V5" s="105"/>
       <c r="W5" s="106"/>
-      <c r="AA5" s="118" t="s">
+      <c r="AA5" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="119"/>
+      <c r="AB5" s="103"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
       <c r="D6" s="17"/>
       <c r="G6" s="8">
@@ -9118,7 +9118,7 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>10653.150000000001</v>
+        <v>12122.550000000001</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
@@ -9249,7 +9249,7 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>10652.006189451024</v>
+        <v>12121.406189451023</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
@@ -9300,14 +9300,14 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="116" t="s">
+      <c r="Z13" s="111" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="116"/>
-      <c r="AB13" s="116" t="s">
+      <c r="AA13" s="111"/>
+      <c r="AB13" s="111" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="117"/>
+      <c r="AC13" s="112"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="9"/>
@@ -9331,14 +9331,14 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="102" t="s">
+      <c r="Z14" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="102"/>
-      <c r="AB14" s="102" t="s">
+      <c r="AA14" s="100"/>
+      <c r="AB14" s="100" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="103"/>
+      <c r="AC14" s="101"/>
     </row>
     <row r="15" spans="1:29">
       <c r="B15" s="104" t="s">
@@ -9371,14 +9371,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="102" t="s">
+      <c r="Z15" s="100" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="102"/>
-      <c r="AB15" s="102" t="s">
+      <c r="AA15" s="100"/>
+      <c r="AB15" s="100" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="103"/>
+      <c r="AC15" s="101"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9387,10 +9387,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="102" t="s">
+      <c r="C16" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="103"/>
+      <c r="D16" s="101"/>
       <c r="E16" s="3" t="s">
         <v>265</v>
       </c>
@@ -9417,23 +9417,23 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="102" t="s">
+      <c r="Z16" s="100" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="102"/>
-      <c r="AB16" s="102" t="s">
+      <c r="AA16" s="100"/>
+      <c r="AB16" s="100" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="103"/>
+      <c r="AC16" s="101"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="102" t="s">
+      <c r="C17" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="103"/>
+      <c r="D17" s="101"/>
       <c r="E17" s="3" t="s">
         <v>265</v>
       </c>
@@ -9458,19 +9458,19 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="102" t="s">
+      <c r="Z17" s="100" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="102"/>
-      <c r="AB17" s="102" t="s">
+      <c r="AA17" s="100"/>
+      <c r="AB17" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="103"/>
+      <c r="AC17" s="101"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="102"/>
-      <c r="D18" s="103"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="101"/>
       <c r="G18" s="9"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
@@ -9492,19 +9492,19 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="102" t="s">
+      <c r="Z18" s="100" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="102"/>
-      <c r="AB18" s="102" t="s">
+      <c r="AA18" s="100"/>
+      <c r="AB18" s="100" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="103"/>
+      <c r="AC18" s="101"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="123"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="110"/>
       <c r="G19" s="8">
         <v>44835</v>
       </c>
@@ -9530,14 +9530,14 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="102" t="s">
+      <c r="Z19" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="102"/>
-      <c r="AB19" s="102" t="s">
+      <c r="AA19" s="100"/>
+      <c r="AB19" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="103"/>
+      <c r="AC19" s="101"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9"/>
@@ -9563,14 +9563,14 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="102" t="s">
+      <c r="Z20" s="100" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="102"/>
-      <c r="AB20" s="102" t="s">
+      <c r="AA20" s="100"/>
+      <c r="AB20" s="100" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="103"/>
+      <c r="AC20" s="101"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -9631,10 +9631,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="102" t="s">
+      <c r="C23" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="103"/>
+      <c r="D23" s="101"/>
       <c r="G23" s="8">
         <v>44805</v>
       </c>
@@ -9660,10 +9660,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="102">
+      <c r="C24" s="100">
         <v>1969</v>
       </c>
-      <c r="D24" s="103"/>
+      <c r="D24" s="101"/>
       <c r="G24" s="9"/>
       <c r="H24" s="34"/>
       <c r="I24" s="34"/>
@@ -9685,8 +9685,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="103"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="101"/>
       <c r="G25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -9710,11 +9710,11 @@
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="120">
+      <c r="C26" s="107">
         <f>'Financial Model'!V68</f>
         <v>2329</v>
       </c>
-      <c r="D26" s="121"/>
+      <c r="D26" s="108"/>
       <c r="G26" s="8">
         <v>44805</v>
       </c>
@@ -9740,8 +9740,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="103"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="101"/>
       <c r="G27" s="9"/>
       <c r="H27" s="7" t="s">
         <v>192</v>
@@ -9767,8 +9767,8 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="102"/>
-      <c r="D28" s="103"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="101"/>
       <c r="G28" s="9"/>
       <c r="H28" s="7" t="s">
         <v>193</v>
@@ -9794,11 +9794,11 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="113">
+      <c r="C29" s="119">
         <f>'Order &amp; Backlog'!U21</f>
         <v>291</v>
       </c>
-      <c r="D29" s="103"/>
+      <c r="D29" s="101"/>
       <c r="G29" s="9"/>
       <c r="H29" s="7" t="s">
         <v>191</v>
@@ -9826,11 +9826,11 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="102">
+      <c r="C30" s="100">
         <f>'Financial Model'!V43</f>
         <v>80</v>
       </c>
-      <c r="D30" s="103"/>
+      <c r="D30" s="101"/>
       <c r="G30" s="9"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
@@ -9852,10 +9852,10 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="114">
+      <c r="C31" s="120">
         <v>36708</v>
       </c>
-      <c r="D31" s="115"/>
+      <c r="D31" s="121"/>
       <c r="G31" s="9"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -9877,8 +9877,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="102"/>
-      <c r="D32" s="103"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="101"/>
       <c r="G32" s="8">
         <v>44743</v>
       </c>
@@ -9935,10 +9935,10 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="109" t="s">
+      <c r="C34" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="110"/>
+      <c r="D34" s="116"/>
       <c r="G34" s="9"/>
       <c r="H34" s="47" t="s">
         <v>198</v>
@@ -10021,11 +10021,11 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="111">
+      <c r="C38" s="117">
         <f>C6/'Financial Model'!V123</f>
-        <v>3.7718276448095129</v>
-      </c>
-      <c r="D38" s="112"/>
+        <v>4.2920797337487562</v>
+      </c>
+      <c r="D38" s="118"/>
       <c r="G38" s="9"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -10049,11 +10049,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="111">
+      <c r="C39" s="117">
         <f>C8/'Financial Model'!AG9</f>
-        <v>2.3463020879217695</v>
-      </c>
-      <c r="D39" s="112"/>
+        <v>2.6699299621178754</v>
+      </c>
+      <c r="D39" s="118"/>
       <c r="G39" s="8">
         <v>44682</v>
       </c>
@@ -10081,11 +10081,11 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="107">
+      <c r="C40" s="113">
         <f>C6/'Financial Model'!AG26</f>
-        <v>-57.452535059331176</v>
-      </c>
-      <c r="D40" s="108"/>
+        <v>-65.377022653721681</v>
+      </c>
+      <c r="D40" s="114"/>
       <c r="G40" s="9"/>
       <c r="H40" s="7" t="s">
         <v>249</v>
@@ -10179,10 +10179,10 @@
       <c r="W43" s="35"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="98" t="s">
+      <c r="B44" s="122" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="99"/>
+      <c r="C44" s="123"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
@@ -10210,10 +10210,10 @@
       </c>
     </row>
     <row r="45" spans="2:23">
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="122" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="99"/>
+      <c r="C45" s="123"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
@@ -10231,8 +10231,8 @@
       <c r="R45" s="35"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="B46" s="98"/>
-      <c r="C46" s="99"/>
+      <c r="B46" s="122"/>
+      <c r="C46" s="123"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
@@ -10254,8 +10254,8 @@
       <c r="R46" s="35"/>
     </row>
     <row r="47" spans="2:23">
-      <c r="B47" s="98"/>
-      <c r="C47" s="99"/>
+      <c r="B47" s="122"/>
+      <c r="C47" s="123"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
@@ -10275,8 +10275,8 @@
       <c r="R47" s="35"/>
     </row>
     <row r="48" spans="2:23">
-      <c r="B48" s="100"/>
-      <c r="C48" s="101"/>
+      <c r="B48" s="124"/>
+      <c r="C48" s="125"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
@@ -10471,6 +10471,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="T5:W5"/>
@@ -10487,39 +10520,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -10827,7 +10827,7 @@
       <c r="U3" s="22">
         <v>44879</v>
       </c>
-      <c r="V3" s="124">
+      <c r="V3" s="98">
         <v>44995</v>
       </c>
       <c r="Z3" s="22">
@@ -10842,7 +10842,7 @@
       <c r="AF3" s="22">
         <v>44629</v>
       </c>
-      <c r="AG3" s="124">
+      <c r="AG3" s="98">
         <f>V3</f>
         <v>44995</v>
       </c>
@@ -13000,123 +13000,123 @@
         <v>-18.100000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:33" s="125" customFormat="1">
-      <c r="B26" s="125" t="s">
+    <row r="26" spans="2:33" s="99" customFormat="1">
+      <c r="B26" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="125">
+      <c r="C26" s="99">
         <f>C24/C27</f>
         <v>-5.0456838947224879E-2</v>
       </c>
-      <c r="D26" s="125">
+      <c r="D26" s="99">
         <f>D24/D27</f>
         <v>-0.17246080436264485</v>
       </c>
-      <c r="E26" s="125">
+      <c r="E26" s="99">
         <f>E24/E27</f>
         <v>-1.7034614336331428E-2</v>
       </c>
-      <c r="F26" s="125">
+      <c r="F26" s="99">
         <f t="shared" ref="F26:M26" si="13">F24/F27</f>
         <v>3.5417518049312082E-3</v>
       </c>
-      <c r="G26" s="125">
+      <c r="G26" s="99">
         <f t="shared" si="13"/>
         <v>-5.7768112002174798E-2</v>
       </c>
-      <c r="H26" s="125">
+      <c r="H26" s="99">
         <f t="shared" si="13"/>
         <v>9.7852677357977719E-3</v>
       </c>
-      <c r="I26" s="125">
+      <c r="I26" s="99">
         <f t="shared" si="13"/>
         <v>-0.104919815167165</v>
       </c>
-      <c r="J26" s="125">
+      <c r="J26" s="99">
         <f t="shared" si="13"/>
         <v>-0.28509308329936134</v>
       </c>
-      <c r="K26" s="125">
+      <c r="K26" s="99">
         <f t="shared" si="13"/>
         <v>-0.39668523298464881</v>
       </c>
-      <c r="L26" s="125">
+      <c r="L26" s="99">
         <f t="shared" si="13"/>
         <v>-0.42828035859820701</v>
       </c>
-      <c r="M26" s="125">
+      <c r="M26" s="99">
         <f t="shared" si="13"/>
         <v>-0.16462917685411571</v>
       </c>
-      <c r="N26" s="125">
+      <c r="N26" s="99">
         <f t="shared" ref="N26:V26" si="14">N24/N27</f>
         <v>-4.4824775876120618E-3</v>
       </c>
-      <c r="O26" s="125">
+      <c r="O26" s="99">
         <f t="shared" si="14"/>
         <v>-0.12204081632653062</v>
       </c>
-      <c r="P26" s="125">
+      <c r="P26" s="99">
         <f t="shared" si="14"/>
         <v>0.11962438758845946</v>
       </c>
-      <c r="Q26" s="125">
+      <c r="Q26" s="99">
         <f t="shared" si="14"/>
         <v>-6.1241154055525319E-2</v>
       </c>
-      <c r="R26" s="125">
+      <c r="R26" s="99">
         <f t="shared" si="14"/>
         <v>2.8583095140873828E-3</v>
       </c>
-      <c r="S26" s="125">
+      <c r="S26" s="99">
         <f t="shared" si="14"/>
         <v>-4.3152736182956709E-2</v>
       </c>
-      <c r="T26" s="125">
+      <c r="T26" s="99">
         <f t="shared" si="14"/>
         <v>0.10100735093928669</v>
       </c>
-      <c r="U26" s="125">
+      <c r="U26" s="99">
         <f t="shared" si="14"/>
         <v>-4.111080860332153E-2</v>
       </c>
-      <c r="V26" s="125">
+      <c r="V26" s="99">
         <f t="shared" si="14"/>
         <v>3.1169184701238598E-2</v>
       </c>
-      <c r="Y26" s="125">
+      <c r="Y26" s="99">
         <f t="shared" ref="Y26:AG26" si="15">Y24/Y27</f>
         <v>0.45618100040888643</v>
       </c>
-      <c r="Z26" s="125">
+      <c r="Z26" s="99">
         <f t="shared" si="15"/>
         <v>9.4768556559846617E-2</v>
       </c>
-      <c r="AA26" s="125">
+      <c r="AA26" s="99">
         <f t="shared" si="15"/>
         <v>0.22580206634040237</v>
       </c>
-      <c r="AB26" s="125">
+      <c r="AB26" s="99">
         <f t="shared" si="15"/>
         <v>0.33610241045894051</v>
       </c>
-      <c r="AC26" s="125">
+      <c r="AC26" s="99">
         <f t="shared" si="15"/>
         <v>-0.24274621986105432</v>
       </c>
-      <c r="AD26" s="125">
+      <c r="AD26" s="99">
         <f t="shared" si="15"/>
         <v>-0.43796711509715996</v>
       </c>
-      <c r="AE26" s="125">
+      <c r="AE26" s="99">
         <f t="shared" si="15"/>
         <v>-0.99415919587068724</v>
       </c>
-      <c r="AF26" s="125">
+      <c r="AF26" s="99">
         <f t="shared" si="15"/>
         <v>-6.0841159657002861E-2</v>
       </c>
-      <c r="AG26" s="125">
+      <c r="AG26" s="99">
         <f t="shared" si="15"/>
         <v>-0.25238224884290772</v>
       </c>
@@ -23714,7 +23714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
$ERJ Q223 orders & deliveries
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B813A9A-43FA-439C-A6D6-C619495496D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649F17E3-FDB4-4187-A372-B8230F677FF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="271">
   <si>
     <t>$ERJ</t>
   </si>
@@ -975,6 +975,9 @@
   <si>
     <t>Q123</t>
   </si>
+  <si>
+    <t>Q223</t>
+  </si>
 </sst>
 </file>
 
@@ -1480,16 +1483,22 @@
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1499,24 +1508,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1546,16 +1537,28 @@
     <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5301,9 +5304,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$V$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5366,16 +5369,19 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Q123</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Q223</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$3:$V$3</c:f>
+              <c:f>'Order &amp; Backlog'!$B$3:$W$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>1835</c:v>
                 </c:pt>
@@ -5438,6 +5444,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5474,9 +5483,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$V$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5539,16 +5548,19 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Q123</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Q223</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$12:$V$12</c:f>
+              <c:f>'Order &amp; Backlog'!$B$12:$W$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>1414</c:v>
                 </c:pt>
@@ -5611,6 +5623,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1735</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5647,9 +5662,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$V$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$W$1</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5712,16 +5727,19 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Q123</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Q223</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$21:$V$21</c:f>
+              <c:f>'Order &amp; Backlog'!$B$21:$W$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>421</c:v>
                 </c:pt>
@@ -5784,6 +5802,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8708,13 +8729,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -8758,13 +8779,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>32</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -9109,7 +9130,7 @@
   <dimension ref="A2:AC61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19:AA19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9129,42 +9150,42 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
-      <c r="G5" s="105" t="s">
+      <c r="C5" s="108"/>
+      <c r="D5" s="109"/>
+      <c r="G5" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="T5" s="105" t="s">
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="109"/>
+      <c r="T5" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="107"/>
-      <c r="AA5" s="103" t="s">
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="109"/>
+      <c r="AA5" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="104"/>
+      <c r="AB5" s="122"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>13.5</v>
+        <v>15.5</v>
       </c>
       <c r="D6" s="17"/>
       <c r="G6" s="8">
@@ -9233,7 +9254,7 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>9917.1</v>
+        <v>11386.300000000001</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
@@ -9364,7 +9385,7 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>11115</v>
+        <v>12584.2</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
@@ -9387,13 +9408,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="105" t="s">
+      <c r="Y12" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="107"/>
+      <c r="Z12" s="108"/>
+      <c r="AA12" s="108"/>
+      <c r="AB12" s="108"/>
+      <c r="AC12" s="109"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -9415,14 +9436,14 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="112" t="s">
+      <c r="Z13" s="119" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="112"/>
-      <c r="AB13" s="112" t="s">
+      <c r="AA13" s="119"/>
+      <c r="AB13" s="119" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="113"/>
+      <c r="AC13" s="120"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
@@ -9450,21 +9471,21 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="101" t="s">
+      <c r="Z14" s="105" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="101"/>
-      <c r="AB14" s="101" t="s">
+      <c r="AA14" s="105"/>
+      <c r="AB14" s="105" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="102"/>
+      <c r="AC14" s="106"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="107"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -9486,14 +9507,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="101" t="s">
+      <c r="Z15" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="101"/>
-      <c r="AB15" s="101" t="s">
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="105" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="102"/>
+      <c r="AC15" s="106"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9502,10 +9523,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="101" t="s">
+      <c r="C16" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="102"/>
+      <c r="D16" s="106"/>
       <c r="G16" s="9"/>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
@@ -9527,23 +9548,23 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="101" t="s">
+      <c r="Z16" s="105" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="101"/>
-      <c r="AB16" s="101" t="s">
+      <c r="AA16" s="105"/>
+      <c r="AB16" s="105" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="102"/>
+      <c r="AC16" s="106"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="102"/>
+      <c r="D17" s="106"/>
       <c r="G17" s="8">
         <v>44835</v>
       </c>
@@ -9567,19 +9588,19 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="101" t="s">
+      <c r="Z17" s="105" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="101"/>
-      <c r="AB17" s="101" t="s">
+      <c r="AA17" s="105"/>
+      <c r="AB17" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="102"/>
+      <c r="AC17" s="106"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
       <c r="G18" s="9"/>
       <c r="H18" s="7" t="s">
         <v>12</v>
@@ -9603,19 +9624,19 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="101" t="s">
+      <c r="Z18" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="101"/>
-      <c r="AB18" s="101" t="s">
+      <c r="AA18" s="105"/>
+      <c r="AB18" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="102"/>
+      <c r="AC18" s="106"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="126"/>
       <c r="G19" s="9"/>
       <c r="H19" s="7" t="s">
         <v>13</v>
@@ -9639,14 +9660,14 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="101" t="s">
+      <c r="Z19" s="105" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="101"/>
-      <c r="AB19" s="101" t="s">
+      <c r="AA19" s="105"/>
+      <c r="AB19" s="105" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="102"/>
+      <c r="AC19" s="106"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9"/>
@@ -9670,14 +9691,14 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="101" t="s">
+      <c r="Z20" s="105" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="101"/>
-      <c r="AB20" s="101" t="s">
+      <c r="AA20" s="105"/>
+      <c r="AB20" s="105" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="102"/>
+      <c r="AC20" s="106"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="8">
@@ -9709,11 +9730,11 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="109"/>
       <c r="G22" s="9"/>
       <c r="H22" s="7" t="s">
         <v>30</v>
@@ -9744,10 +9765,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="102"/>
+      <c r="D23" s="106"/>
       <c r="G23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -9769,10 +9790,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="101">
+      <c r="C24" s="105">
         <v>1969</v>
       </c>
-      <c r="D24" s="102"/>
+      <c r="D24" s="106"/>
       <c r="G24" s="9"/>
       <c r="H24" s="34"/>
       <c r="I24" s="34"/>
@@ -9794,8 +9815,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="102"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="106"/>
       <c r="G25" s="8">
         <v>44805</v>
       </c>
@@ -9823,11 +9844,11 @@
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="108">
+      <c r="C26" s="123">
         <f>'Financial Model'!V68</f>
         <v>2329</v>
       </c>
-      <c r="D26" s="109"/>
+      <c r="D26" s="124"/>
       <c r="G26" s="9"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
@@ -9849,8 +9870,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="102"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="106"/>
       <c r="G27" s="9"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -9874,8 +9895,8 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="102"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="106"/>
       <c r="G28" s="8">
         <v>44805</v>
       </c>
@@ -9903,11 +9924,11 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="120">
+      <c r="C29" s="116">
         <f>'Order &amp; Backlog'!V21</f>
         <v>281</v>
       </c>
-      <c r="D29" s="102"/>
+      <c r="D29" s="106"/>
       <c r="G29" s="9"/>
       <c r="H29" s="7" t="s">
         <v>192</v>
@@ -9933,11 +9954,11 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="101">
+      <c r="C30" s="105">
         <f>'Financial Model'!W43</f>
         <v>15</v>
       </c>
-      <c r="D30" s="102"/>
+      <c r="D30" s="106"/>
       <c r="G30" s="9"/>
       <c r="H30" s="7" t="s">
         <v>193</v>
@@ -9961,10 +9982,10 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="121">
+      <c r="C31" s="117">
         <v>36708</v>
       </c>
-      <c r="D31" s="122"/>
+      <c r="D31" s="118"/>
       <c r="G31" s="9"/>
       <c r="H31" s="7" t="s">
         <v>191</v>
@@ -9990,8 +10011,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="102"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="106"/>
       <c r="G32" s="9"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
@@ -10042,10 +10063,10 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="116" t="s">
+      <c r="C34" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="117"/>
+      <c r="D34" s="113"/>
       <c r="G34" s="8">
         <v>44743</v>
       </c>
@@ -10100,11 +10121,11 @@
       <c r="R36" s="35"/>
     </row>
     <row r="37" spans="2:23">
-      <c r="B37" s="105" t="s">
+      <c r="B37" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107"/>
+      <c r="C37" s="108"/>
+      <c r="D37" s="109"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -10117,22 +10138,22 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="105" t="s">
+      <c r="T37" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="107"/>
+      <c r="U37" s="108"/>
+      <c r="V37" s="108"/>
+      <c r="W37" s="109"/>
     </row>
     <row r="38" spans="2:23">
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="118">
+      <c r="C38" s="114">
         <f>C6/'Financial Model'!W123</f>
-        <v>3.5775974025974029</v>
-      </c>
-      <c r="D38" s="119"/>
+        <v>4.1076118326118332</v>
+      </c>
+      <c r="D38" s="115"/>
       <c r="G38" s="8">
         <v>44743</v>
       </c>
@@ -10160,11 +10181,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="118">
+      <c r="C39" s="114">
         <f>C8/SUM('Financial Model'!T9:W9)</f>
-        <v>2.1298698509514198</v>
-      </c>
-      <c r="D39" s="119"/>
+        <v>2.445406125166445</v>
+      </c>
+      <c r="D39" s="115"/>
       <c r="G39" s="9"/>
       <c r="H39" s="7" t="s">
         <v>240</v>
@@ -10190,11 +10211,11 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="114">
+      <c r="C40" s="110">
         <f>C6/SUM('Financial Model'!T26:W26)</f>
-        <v>-2540.815509028399</v>
-      </c>
-      <c r="D40" s="115"/>
+        <v>-2917.2326214770505</v>
+      </c>
+      <c r="D40" s="111"/>
       <c r="G40" s="9"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
@@ -10261,11 +10282,11 @@
       <c r="W42" s="35"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="107" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="106"/>
-      <c r="D43" s="107"/>
+      <c r="C43" s="108"/>
+      <c r="D43" s="109"/>
       <c r="G43" s="9"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -10286,10 +10307,10 @@
       <c r="W43" s="35"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="123" t="s">
+      <c r="B44" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="124"/>
+      <c r="C44" s="102"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
@@ -10319,10 +10340,10 @@
       </c>
     </row>
     <row r="45" spans="2:23">
-      <c r="B45" s="123" t="s">
+      <c r="B45" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="124"/>
+      <c r="C45" s="102"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
@@ -10342,8 +10363,8 @@
       <c r="R45" s="35"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="B46" s="123"/>
-      <c r="C46" s="124"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="102"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
@@ -10363,8 +10384,8 @@
       </c>
     </row>
     <row r="47" spans="2:23">
-      <c r="B47" s="123"/>
-      <c r="C47" s="124"/>
+      <c r="B47" s="101"/>
+      <c r="C47" s="102"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
@@ -10382,8 +10403,8 @@
       <c r="R47" s="35"/>
     </row>
     <row r="48" spans="2:23">
-      <c r="B48" s="125"/>
-      <c r="C48" s="126"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="104"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
@@ -10612,11 +10633,34 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
     <mergeCell ref="Z19:AA19"/>
     <mergeCell ref="AB19:AC19"/>
     <mergeCell ref="Z20:AA20"/>
@@ -10633,34 +10677,11 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H17" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -10696,10 +10717,10 @@
   <dimension ref="B1:AQ148"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="L101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W142" sqref="W142"/>
+      <selection pane="bottomRight" activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -24278,8 +24299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE34" sqref="AE34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -24294,13 +24315,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258CA0E5-563F-4C1F-B583-AD76D8E7BBD2}">
-  <dimension ref="A1:AJ49"/>
+  <dimension ref="A1:AK49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R23" sqref="R23"/>
+      <selection pane="bottomRight" activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -24309,7 +24330,7 @@
     <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="2" customFormat="1">
+    <row r="1" spans="1:37" s="2" customFormat="1">
       <c r="B1" s="23" t="s">
         <v>32</v>
       </c>
@@ -24373,57 +24394,60 @@
       <c r="V1" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="Y1" s="76">
+      <c r="W1" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="Z1" s="76">
         <v>2014</v>
       </c>
-      <c r="Z1" s="76">
+      <c r="AA1" s="76">
         <v>2015</v>
       </c>
-      <c r="AA1" s="76">
+      <c r="AB1" s="76">
         <v>2016</v>
       </c>
-      <c r="AB1" s="76">
+      <c r="AC1" s="76">
         <v>2017</v>
       </c>
-      <c r="AC1" s="76">
+      <c r="AD1" s="76">
         <v>2018</v>
       </c>
-      <c r="AD1" s="76">
-        <f>AC1+1</f>
+      <c r="AE1" s="76">
+        <f>AD1+1</f>
         <v>2019</v>
       </c>
-      <c r="AE1" s="76">
-        <f t="shared" ref="AE1:AJ1" si="0">AD1+1</f>
+      <c r="AF1" s="76">
+        <f t="shared" ref="AF1:AK1" si="0">AE1+1</f>
         <v>2020</v>
       </c>
-      <c r="AF1" s="76">
+      <c r="AG1" s="76">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="AG1" s="2">
+      <c r="AH1" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="AH1" s="2">
+      <c r="AI1" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="AI1" s="2">
+      <c r="AJ1" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="AJ1" s="2">
+      <c r="AK1" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="91" customFormat="1">
+    <row r="2" spans="1:37" s="91" customFormat="1">
       <c r="A2" s="89"/>
       <c r="B2" s="90"/>
       <c r="C2" s="90"/>
       <c r="D2" s="90"/>
     </row>
-    <row r="3" spans="1:36" s="73" customFormat="1">
+    <row r="3" spans="1:37" s="73" customFormat="1">
       <c r="A3" s="73" t="s">
         <v>208</v>
       </c>
@@ -24496,7 +24520,7 @@
         <v>1992</v>
       </c>
       <c r="S3" s="73">
-        <f t="shared" ref="S3:V3" si="14">SUM(S4:S10)</f>
+        <f t="shared" ref="S3:W3" si="14">SUM(S4:S10)</f>
         <v>2000</v>
       </c>
       <c r="T3" s="73">
@@ -24511,40 +24535,44 @@
         <f t="shared" si="14"/>
         <v>2016</v>
       </c>
-      <c r="Y3" s="73">
-        <f t="shared" ref="Y3:AC3" si="15">SUM(Y4:Y10)</f>
+      <c r="W3" s="73">
+        <f t="shared" si="14"/>
+        <v>2023</v>
+      </c>
+      <c r="Z3" s="73">
+        <f t="shared" ref="Z3:AD3" si="15">SUM(Z4:Z10)</f>
         <v>1549</v>
       </c>
-      <c r="Z3" s="73">
+      <c r="AA3" s="73">
         <f t="shared" si="15"/>
         <v>1704</v>
       </c>
-      <c r="AA3" s="73">
+      <c r="AB3" s="73">
         <f t="shared" si="15"/>
         <v>1749</v>
       </c>
-      <c r="AB3" s="73">
+      <c r="AC3" s="73">
         <f t="shared" si="15"/>
         <v>1835</v>
       </c>
-      <c r="AC3" s="73">
+      <c r="AD3" s="73">
         <f t="shared" si="15"/>
         <v>1858</v>
       </c>
-      <c r="AD3" s="73">
-        <f t="shared" ref="AD3" si="16">SUM(AD4:AD10)</f>
+      <c r="AE3" s="73">
+        <f t="shared" ref="AE3" si="16">SUM(AE4:AE10)</f>
         <v>1917</v>
       </c>
-      <c r="AE3" s="73">
-        <f t="shared" ref="AE3" si="17">SUM(AE4:AE10)</f>
+      <c r="AF3" s="73">
+        <f t="shared" ref="AF3" si="17">SUM(AF4:AF10)</f>
         <v>1904</v>
       </c>
-      <c r="AF3" s="73">
-        <f t="shared" ref="AF3" si="18">SUM(AF4:AF10)</f>
+      <c r="AG3" s="73">
+        <f t="shared" ref="AG3" si="18">SUM(AG4:AG10)</f>
         <v>1996</v>
       </c>
     </row>
-    <row r="4" spans="1:36" s="74" customFormat="1">
+    <row r="4" spans="1:37" s="74" customFormat="1">
       <c r="A4" s="75" t="s">
         <v>201</v>
       </c>
@@ -24611,8 +24639,8 @@
       <c r="V4" s="74">
         <v>191</v>
       </c>
-      <c r="Y4" s="74">
-        <v>193</v>
+      <c r="W4" s="74">
+        <v>191</v>
       </c>
       <c r="Z4" s="74">
         <v>193</v>
@@ -24621,7 +24649,7 @@
         <v>193</v>
       </c>
       <c r="AB4" s="74">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AC4" s="74">
         <v>191</v>
@@ -24635,8 +24663,11 @@
       <c r="AF4" s="74">
         <v>191</v>
       </c>
+      <c r="AG4" s="74">
+        <v>191</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" s="74" customFormat="1">
+    <row r="5" spans="1:37" s="74" customFormat="1">
       <c r="A5" s="75" t="s">
         <v>85</v>
       </c>
@@ -24703,32 +24734,35 @@
       <c r="V5" s="74">
         <v>815</v>
       </c>
-      <c r="Y5" s="74">
+      <c r="W5" s="74">
+        <v>822</v>
+      </c>
+      <c r="Z5" s="74">
         <v>421</v>
       </c>
-      <c r="Z5" s="74">
+      <c r="AA5" s="74">
         <v>500</v>
       </c>
-      <c r="AA5" s="74">
+      <c r="AB5" s="74">
         <v>525</v>
       </c>
-      <c r="AB5" s="74">
+      <c r="AC5" s="74">
         <v>603</v>
       </c>
-      <c r="AC5" s="74">
+      <c r="AD5" s="74">
         <v>771</v>
       </c>
-      <c r="AD5" s="74">
+      <c r="AE5" s="74">
         <v>815</v>
       </c>
-      <c r="AE5" s="74">
+      <c r="AF5" s="74">
         <v>798</v>
       </c>
-      <c r="AF5" s="74">
+      <c r="AG5" s="74">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:36" s="74" customFormat="1">
+    <row r="6" spans="1:37" s="74" customFormat="1">
       <c r="A6" s="75" t="s">
         <v>185</v>
       </c>
@@ -24795,23 +24829,23 @@
       <c r="V6" s="74">
         <v>568</v>
       </c>
-      <c r="Y6" s="74">
+      <c r="W6" s="74">
+        <v>568</v>
+      </c>
+      <c r="Z6" s="74">
         <v>580</v>
       </c>
-      <c r="Z6" s="74">
+      <c r="AA6" s="74">
         <v>578</v>
       </c>
-      <c r="AA6" s="74">
+      <c r="AB6" s="74">
         <v>590</v>
       </c>
-      <c r="AB6" s="74">
+      <c r="AC6" s="74">
         <v>592</v>
       </c>
-      <c r="AC6" s="74">
+      <c r="AD6" s="74">
         <v>566</v>
-      </c>
-      <c r="AD6" s="74">
-        <v>568</v>
       </c>
       <c r="AE6" s="74">
         <v>568</v>
@@ -24819,8 +24853,11 @@
       <c r="AF6" s="74">
         <v>568</v>
       </c>
+      <c r="AG6" s="74">
+        <v>568</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" s="74" customFormat="1">
+    <row r="7" spans="1:37" s="74" customFormat="1">
       <c r="A7" s="75" t="s">
         <v>188</v>
       </c>
@@ -24887,20 +24924,20 @@
       <c r="V7" s="74">
         <v>172</v>
       </c>
-      <c r="Y7" s="74">
+      <c r="W7" s="74">
+        <v>172</v>
+      </c>
+      <c r="Z7" s="74">
         <v>145</v>
-      </c>
-      <c r="Z7" s="74">
-        <v>166</v>
       </c>
       <c r="AA7" s="74">
         <v>166</v>
       </c>
       <c r="AB7" s="74">
+        <v>166</v>
+      </c>
+      <c r="AC7" s="74">
         <v>169</v>
-      </c>
-      <c r="AC7" s="74">
-        <v>172</v>
       </c>
       <c r="AD7" s="74">
         <v>172</v>
@@ -24911,8 +24948,11 @@
       <c r="AF7" s="74">
         <v>172</v>
       </c>
+      <c r="AG7" s="74">
+        <v>172</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" s="74" customFormat="1">
+    <row r="8" spans="1:37" s="74" customFormat="1">
       <c r="A8" s="75" t="s">
         <v>215</v>
       </c>
@@ -24979,8 +25019,8 @@
       <c r="V8" s="74">
         <v>0</v>
       </c>
-      <c r="Y8" s="74">
-        <v>100</v>
+      <c r="W8" s="74">
+        <v>0</v>
       </c>
       <c r="Z8" s="74">
         <v>100</v>
@@ -24992,7 +25032,7 @@
         <v>100</v>
       </c>
       <c r="AC8" s="74">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AD8" s="74">
         <v>0</v>
@@ -25003,8 +25043,11 @@
       <c r="AF8" s="74">
         <v>0</v>
       </c>
+      <c r="AG8" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" s="74" customFormat="1">
+    <row r="9" spans="1:37" s="74" customFormat="1">
       <c r="A9" s="75" t="s">
         <v>180</v>
       </c>
@@ -25071,32 +25114,35 @@
       <c r="V9" s="74">
         <v>25</v>
       </c>
-      <c r="Y9" s="74">
+      <c r="W9" s="74">
+        <v>34</v>
+      </c>
+      <c r="Z9" s="74">
         <v>60</v>
       </c>
-      <c r="Z9" s="74">
+      <c r="AA9" s="74">
         <v>77</v>
       </c>
-      <c r="AA9" s="74">
+      <c r="AB9" s="74">
         <v>85</v>
       </c>
-      <c r="AB9" s="74">
+      <c r="AC9" s="74">
         <v>74</v>
       </c>
-      <c r="AC9" s="74">
+      <c r="AD9" s="74">
         <v>47</v>
       </c>
-      <c r="AD9" s="74">
+      <c r="AE9" s="74">
         <v>27</v>
-      </c>
-      <c r="AE9" s="74">
-        <v>22</v>
       </c>
       <c r="AF9" s="74">
         <v>22</v>
       </c>
+      <c r="AG9" s="74">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" s="74" customFormat="1">
+    <row r="10" spans="1:37" s="74" customFormat="1">
       <c r="A10" s="75" t="s">
         <v>86</v>
       </c>
@@ -25163,33 +25209,36 @@
       <c r="V10" s="74">
         <v>245</v>
       </c>
-      <c r="Y10" s="74">
+      <c r="W10" s="74">
+        <v>236</v>
+      </c>
+      <c r="Z10" s="74">
         <v>50</v>
-      </c>
-      <c r="Z10" s="74">
-        <v>90</v>
       </c>
       <c r="AA10" s="74">
         <v>90</v>
       </c>
       <c r="AB10" s="74">
+        <v>90</v>
+      </c>
+      <c r="AC10" s="74">
         <v>106</v>
       </c>
-      <c r="AC10" s="74">
+      <c r="AD10" s="74">
         <v>111</v>
       </c>
-      <c r="AD10" s="74">
+      <c r="AE10" s="74">
         <v>144</v>
       </c>
-      <c r="AE10" s="74">
+      <c r="AF10" s="74">
         <v>153</v>
       </c>
-      <c r="AF10" s="74">
+      <c r="AG10" s="74">
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:36" s="74" customFormat="1"/>
-    <row r="12" spans="1:36" s="73" customFormat="1">
+    <row r="11" spans="1:37" s="74" customFormat="1"/>
+    <row r="12" spans="1:37" s="73" customFormat="1">
       <c r="A12" s="73" t="s">
         <v>210</v>
       </c>
@@ -25277,40 +25326,44 @@
         <f>SUM(V13:V19)</f>
         <v>1735</v>
       </c>
-      <c r="Y12" s="73">
-        <f t="shared" ref="Y12:AF12" si="20">SUM(Y13:Y19)</f>
+      <c r="W12" s="73">
+        <f>SUM(W13:W19)</f>
+        <v>1752</v>
+      </c>
+      <c r="Z12" s="73">
+        <f t="shared" ref="Z12:AG12" si="20">SUM(Z13:Z19)</f>
         <v>1090</v>
       </c>
-      <c r="Z12" s="73">
+      <c r="AA12" s="73">
         <f t="shared" si="20"/>
         <v>1181</v>
       </c>
-      <c r="AA12" s="73">
+      <c r="AB12" s="73">
         <f t="shared" si="20"/>
         <v>1299</v>
       </c>
-      <c r="AB12" s="73">
+      <c r="AC12" s="73">
         <f t="shared" si="20"/>
         <v>1400</v>
       </c>
-      <c r="AC12" s="73">
+      <c r="AD12" s="73">
         <f t="shared" si="20"/>
         <v>1490</v>
       </c>
-      <c r="AD12" s="73">
+      <c r="AE12" s="73">
         <f t="shared" si="20"/>
         <v>1579</v>
       </c>
-      <c r="AE12" s="73">
+      <c r="AF12" s="73">
         <f t="shared" si="20"/>
         <v>1623</v>
       </c>
-      <c r="AF12" s="73">
+      <c r="AG12" s="73">
         <f t="shared" si="20"/>
         <v>1671</v>
       </c>
     </row>
-    <row r="13" spans="1:36" s="74" customFormat="1">
+    <row r="13" spans="1:37" s="74" customFormat="1">
       <c r="A13" s="75" t="s">
         <v>201</v>
       </c>
@@ -25377,11 +25430,11 @@
       <c r="V13" s="74">
         <v>191</v>
       </c>
-      <c r="Y13" s="74">
+      <c r="W13" s="74">
+        <v>191</v>
+      </c>
+      <c r="Z13" s="74">
         <v>188</v>
-      </c>
-      <c r="Z13" s="74">
-        <v>190</v>
       </c>
       <c r="AA13" s="74">
         <v>190</v>
@@ -25390,7 +25443,7 @@
         <v>190</v>
       </c>
       <c r="AC13" s="74">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AD13" s="74">
         <v>191</v>
@@ -25401,8 +25454,11 @@
       <c r="AF13" s="74">
         <v>191</v>
       </c>
+      <c r="AG13" s="74">
+        <v>191</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" s="74" customFormat="1">
+    <row r="14" spans="1:37" s="74" customFormat="1">
       <c r="A14" s="75" t="s">
         <v>85</v>
       </c>
@@ -25469,32 +25525,35 @@
       <c r="V14" s="74">
         <v>730</v>
       </c>
-      <c r="Y14" s="74">
+      <c r="W14" s="74">
+        <v>740</v>
+      </c>
+      <c r="Z14" s="74">
         <v>249</v>
       </c>
-      <c r="Z14" s="74">
+      <c r="AA14" s="74">
         <v>331</v>
       </c>
-      <c r="AA14" s="74">
+      <c r="AB14" s="74">
         <v>421</v>
       </c>
-      <c r="AB14" s="74">
+      <c r="AC14" s="74">
         <v>500</v>
       </c>
-      <c r="AC14" s="74">
+      <c r="AD14" s="74">
         <v>567</v>
       </c>
-      <c r="AD14" s="74">
+      <c r="AE14" s="74">
         <v>634</v>
       </c>
-      <c r="AE14" s="74">
+      <c r="AF14" s="74">
         <v>666</v>
       </c>
-      <c r="AF14" s="74">
+      <c r="AG14" s="74">
         <v>693</v>
       </c>
     </row>
-    <row r="15" spans="1:36" s="74" customFormat="1">
+    <row r="15" spans="1:37" s="74" customFormat="1">
       <c r="A15" s="75" t="s">
         <v>185</v>
       </c>
@@ -25561,32 +25620,35 @@
       <c r="V15" s="74">
         <v>568</v>
       </c>
-      <c r="Y15" s="74">
+      <c r="W15" s="74">
+        <v>568</v>
+      </c>
+      <c r="Z15" s="74">
         <v>515</v>
       </c>
-      <c r="Z15" s="74">
+      <c r="AA15" s="74">
         <v>523</v>
       </c>
-      <c r="AA15" s="74">
+      <c r="AB15" s="74">
         <v>534</v>
       </c>
-      <c r="AB15" s="74">
+      <c r="AC15" s="74">
         <v>546</v>
       </c>
-      <c r="AC15" s="74">
+      <c r="AD15" s="74">
         <v>559</v>
       </c>
-      <c r="AD15" s="74">
+      <c r="AE15" s="74">
         <v>564</v>
-      </c>
-      <c r="AE15" s="74">
-        <v>565</v>
       </c>
       <c r="AF15" s="74">
         <v>565</v>
       </c>
+      <c r="AG15" s="74">
+        <v>565</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" s="74" customFormat="1">
+    <row r="16" spans="1:37" s="74" customFormat="1">
       <c r="A16" s="75" t="s">
         <v>188</v>
       </c>
@@ -25653,23 +25715,23 @@
       <c r="V16" s="74">
         <v>172</v>
       </c>
-      <c r="Y16" s="74">
+      <c r="W16" s="74">
+        <v>172</v>
+      </c>
+      <c r="Z16" s="74">
         <v>138</v>
       </c>
-      <c r="Z16" s="74">
+      <c r="AA16" s="74">
         <v>137</v>
       </c>
-      <c r="AA16" s="74">
+      <c r="AB16" s="74">
         <v>154</v>
       </c>
-      <c r="AB16" s="74">
+      <c r="AC16" s="74">
         <v>164</v>
       </c>
-      <c r="AC16" s="74">
+      <c r="AD16" s="74">
         <v>169</v>
-      </c>
-      <c r="AD16" s="74">
-        <v>172</v>
       </c>
       <c r="AE16" s="74">
         <v>172</v>
@@ -25677,8 +25739,11 @@
       <c r="AF16" s="74">
         <v>172</v>
       </c>
+      <c r="AG16" s="74">
+        <v>172</v>
+      </c>
     </row>
-    <row r="17" spans="1:32" s="74" customFormat="1">
+    <row r="17" spans="1:33" s="74" customFormat="1">
       <c r="A17" s="75" t="s">
         <v>215</v>
       </c>
@@ -25745,7 +25810,7 @@
       <c r="V17" s="74">
         <v>0</v>
       </c>
-      <c r="Y17" s="74">
+      <c r="W17" s="74">
         <v>0</v>
       </c>
       <c r="Z17" s="74">
@@ -25769,8 +25834,11 @@
       <c r="AF17" s="74">
         <v>0</v>
       </c>
+      <c r="AG17" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" s="74" customFormat="1">
+    <row r="18" spans="1:33" s="74" customFormat="1">
       <c r="A18" s="75" t="s">
         <v>180</v>
       </c>
@@ -25837,8 +25905,8 @@
       <c r="V18" s="74">
         <v>18</v>
       </c>
-      <c r="Y18" s="74">
-        <v>0</v>
+      <c r="W18" s="74">
+        <v>18</v>
       </c>
       <c r="Z18" s="74">
         <v>0</v>
@@ -25850,19 +25918,22 @@
         <v>0</v>
       </c>
       <c r="AC18" s="74">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="74">
         <v>4</v>
       </c>
-      <c r="AD18" s="74">
+      <c r="AE18" s="74">
         <v>11</v>
       </c>
-      <c r="AE18" s="74">
+      <c r="AF18" s="74">
         <v>15</v>
       </c>
-      <c r="AF18" s="74">
+      <c r="AG18" s="74">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:32" s="74" customFormat="1">
+    <row r="19" spans="1:33" s="74" customFormat="1">
       <c r="A19" s="75" t="s">
         <v>86</v>
       </c>
@@ -25929,8 +26000,8 @@
       <c r="V19" s="74">
         <v>56</v>
       </c>
-      <c r="Y19" s="74">
-        <v>0</v>
+      <c r="W19" s="74">
+        <v>63</v>
       </c>
       <c r="Z19" s="74">
         <v>0</v>
@@ -25945,24 +26016,27 @@
         <v>0</v>
       </c>
       <c r="AD19" s="74">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="74">
         <v>7</v>
       </c>
-      <c r="AE19" s="74">
+      <c r="AF19" s="74">
         <v>14</v>
       </c>
-      <c r="AF19" s="74">
+      <c r="AG19" s="74">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:32" s="74" customFormat="1">
+    <row r="20" spans="1:33" s="74" customFormat="1">
       <c r="A20" s="75"/>
     </row>
-    <row r="21" spans="1:32" s="73" customFormat="1">
+    <row r="21" spans="1:33" s="73" customFormat="1">
       <c r="A21" s="73" t="s">
         <v>209</v>
       </c>
       <c r="B21" s="73">
-        <f t="shared" ref="B21:V21" si="21">SUM(B22:B28)</f>
+        <f t="shared" ref="B21:W21" si="21">SUM(B22:B28)</f>
         <v>421</v>
       </c>
       <c r="C21" s="73">
@@ -26045,40 +26119,44 @@
         <f t="shared" si="21"/>
         <v>281</v>
       </c>
-      <c r="Y21" s="73">
-        <f t="shared" ref="Y21:AF21" si="22">SUM(Y22:Y28)</f>
+      <c r="W21" s="73">
+        <f t="shared" si="21"/>
+        <v>271</v>
+      </c>
+      <c r="Z21" s="73">
+        <f t="shared" ref="Z21:AG21" si="22">SUM(Z22:Z28)</f>
         <v>459</v>
       </c>
-      <c r="Z21" s="73">
+      <c r="AA21" s="73">
         <f t="shared" si="22"/>
         <v>513</v>
       </c>
-      <c r="AA21" s="73">
+      <c r="AB21" s="73">
         <f t="shared" si="22"/>
         <v>450</v>
       </c>
-      <c r="AB21" s="73">
+      <c r="AC21" s="73">
         <f t="shared" si="22"/>
         <v>435</v>
       </c>
-      <c r="AC21" s="73">
+      <c r="AD21" s="73">
         <f t="shared" si="22"/>
         <v>368</v>
       </c>
-      <c r="AD21" s="73">
+      <c r="AE21" s="73">
         <f t="shared" si="22"/>
         <v>338</v>
       </c>
-      <c r="AE21" s="73">
+      <c r="AF21" s="73">
         <f t="shared" si="22"/>
         <v>281</v>
       </c>
-      <c r="AF21" s="73">
+      <c r="AG21" s="73">
         <f t="shared" si="22"/>
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="1:32" s="74" customFormat="1">
+    <row r="22" spans="1:33" s="74" customFormat="1">
       <c r="A22" s="75" t="s">
         <v>201</v>
       </c>
@@ -26145,21 +26223,18 @@
       <c r="V22" s="74">
         <v>0</v>
       </c>
-      <c r="Y22" s="74">
+      <c r="Z22" s="74">
         <v>5</v>
-      </c>
-      <c r="Z22" s="74">
-        <v>3</v>
       </c>
       <c r="AA22" s="74">
         <v>3</v>
       </c>
       <c r="AB22" s="74">
+        <v>3</v>
+      </c>
+      <c r="AC22" s="74">
         <v>1</v>
       </c>
-      <c r="AC22" s="74">
-        <v>0</v>
-      </c>
       <c r="AD22" s="74">
         <v>0</v>
       </c>
@@ -26169,8 +26244,11 @@
       <c r="AF22" s="74">
         <v>0</v>
       </c>
+      <c r="AG22" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" s="74" customFormat="1">
+    <row r="23" spans="1:33" s="74" customFormat="1">
       <c r="A23" s="75" t="s">
         <v>85</v>
       </c>
@@ -26237,32 +26315,35 @@
       <c r="V23" s="74">
         <v>85</v>
       </c>
-      <c r="Y23" s="74">
+      <c r="W23" s="74">
+        <v>82</v>
+      </c>
+      <c r="Z23" s="74">
         <v>172</v>
       </c>
-      <c r="Z23" s="74">
+      <c r="AA23" s="74">
         <v>169</v>
       </c>
-      <c r="AA23" s="74">
+      <c r="AB23" s="74">
         <v>104</v>
       </c>
-      <c r="AB23" s="74">
+      <c r="AC23" s="74">
         <v>103</v>
       </c>
-      <c r="AC23" s="74">
+      <c r="AD23" s="74">
         <v>204</v>
       </c>
-      <c r="AD23" s="74">
+      <c r="AE23" s="74">
         <v>181</v>
       </c>
-      <c r="AE23" s="74">
+      <c r="AF23" s="74">
         <v>132</v>
       </c>
-      <c r="AF23" s="74">
+      <c r="AG23" s="74">
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:32" s="74" customFormat="1">
+    <row r="24" spans="1:33" s="74" customFormat="1">
       <c r="A24" s="75" t="s">
         <v>185</v>
       </c>
@@ -26329,32 +26410,32 @@
       <c r="V24" s="74">
         <v>0</v>
       </c>
-      <c r="Y24" s="74">
+      <c r="Z24" s="74">
         <v>65</v>
       </c>
-      <c r="Z24" s="74">
+      <c r="AA24" s="74">
         <v>55</v>
       </c>
-      <c r="AA24" s="74">
+      <c r="AB24" s="74">
         <v>56</v>
       </c>
-      <c r="AB24" s="74">
+      <c r="AC24" s="74">
         <v>46</v>
       </c>
-      <c r="AC24" s="74">
+      <c r="AD24" s="74">
         <v>7</v>
       </c>
-      <c r="AD24" s="74">
+      <c r="AE24" s="74">
         <v>4</v>
-      </c>
-      <c r="AE24" s="74">
-        <v>3</v>
       </c>
       <c r="AF24" s="74">
         <v>3</v>
       </c>
+      <c r="AG24" s="74">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="1:32" s="74" customFormat="1">
+    <row r="25" spans="1:33" s="74" customFormat="1">
       <c r="A25" s="75" t="s">
         <v>188</v>
       </c>
@@ -26421,32 +26502,35 @@
       <c r="V25" s="74">
         <v>0</v>
       </c>
-      <c r="Y25" s="74">
+      <c r="W25" s="74">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="74">
         <v>7</v>
       </c>
-      <c r="Z25" s="74">
+      <c r="AA25" s="74">
         <v>19</v>
       </c>
-      <c r="AA25" s="74">
+      <c r="AB25" s="74">
         <v>12</v>
       </c>
-      <c r="AB25" s="74">
+      <c r="AC25" s="74">
         <v>5</v>
       </c>
-      <c r="AC25" s="74">
+      <c r="AD25" s="74">
         <v>3</v>
       </c>
-      <c r="AD25" s="74">
-        <v>0</v>
-      </c>
       <c r="AE25" s="74">
         <v>0</v>
       </c>
       <c r="AF25" s="74">
         <v>0</v>
       </c>
+      <c r="AG25" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:32" s="74" customFormat="1">
+    <row r="26" spans="1:33" s="74" customFormat="1">
       <c r="A26" s="75" t="s">
         <v>215</v>
       </c>
@@ -26513,8 +26597,8 @@
       <c r="V26" s="74">
         <v>0</v>
       </c>
-      <c r="Y26" s="74">
-        <v>100</v>
+      <c r="W26" s="74">
+        <v>0</v>
       </c>
       <c r="Z26" s="74">
         <v>100</v>
@@ -26526,7 +26610,7 @@
         <v>100</v>
       </c>
       <c r="AC26" s="74">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AD26" s="74">
         <v>0</v>
@@ -26537,8 +26621,11 @@
       <c r="AF26" s="74">
         <v>0</v>
       </c>
+      <c r="AG26" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:32" s="74" customFormat="1">
+    <row r="27" spans="1:33" s="74" customFormat="1">
       <c r="A27" s="75" t="s">
         <v>180</v>
       </c>
@@ -26605,32 +26692,35 @@
       <c r="V27" s="74">
         <v>7</v>
       </c>
-      <c r="Y27" s="74">
+      <c r="W27" s="74">
+        <v>16</v>
+      </c>
+      <c r="Z27" s="74">
         <v>60</v>
       </c>
-      <c r="Z27" s="74">
+      <c r="AA27" s="74">
         <v>77</v>
       </c>
-      <c r="AA27" s="74">
+      <c r="AB27" s="74">
         <v>85</v>
       </c>
-      <c r="AB27" s="74">
+      <c r="AC27" s="74">
         <v>74</v>
       </c>
-      <c r="AC27" s="74">
+      <c r="AD27" s="74">
         <v>43</v>
       </c>
-      <c r="AD27" s="74">
+      <c r="AE27" s="74">
         <v>16</v>
       </c>
-      <c r="AE27" s="74">
+      <c r="AF27" s="74">
         <v>7</v>
       </c>
-      <c r="AF27" s="74">
+      <c r="AG27" s="74">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:32" s="74" customFormat="1">
+    <row r="28" spans="1:33" s="74" customFormat="1">
       <c r="A28" s="75" t="s">
         <v>86</v>
       </c>
@@ -26697,32 +26787,35 @@
       <c r="V28" s="74">
         <v>189</v>
       </c>
-      <c r="Y28" s="74">
+      <c r="W28" s="74">
+        <v>173</v>
+      </c>
+      <c r="Z28" s="74">
         <v>50</v>
-      </c>
-      <c r="Z28" s="74">
-        <v>90</v>
       </c>
       <c r="AA28" s="74">
         <v>90</v>
       </c>
       <c r="AB28" s="74">
+        <v>90</v>
+      </c>
+      <c r="AC28" s="74">
         <v>106</v>
       </c>
-      <c r="AC28" s="74">
+      <c r="AD28" s="74">
         <v>111</v>
       </c>
-      <c r="AD28" s="74">
+      <c r="AE28" s="74">
         <v>137</v>
       </c>
-      <c r="AE28" s="74">
+      <c r="AF28" s="74">
         <v>139</v>
       </c>
-      <c r="AF28" s="74">
+      <c r="AG28" s="74">
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="31" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>211</v>
       </c>
@@ -26806,39 +26899,43 @@
         <f t="shared" ref="V31" si="31">V3/R3-1</f>
         <v>1.2048192771084265E-2</v>
       </c>
-      <c r="Y31" s="59" t="s">
+      <c r="W31" s="31">
+        <f t="shared" ref="W31" si="32">W3/S3-1</f>
+        <v>1.1500000000000066E-2</v>
+      </c>
+      <c r="Z31" s="59" t="s">
         <v>186</v>
-      </c>
-      <c r="Z31" s="31">
-        <f t="shared" ref="Z31" si="32">Z3/Y3-1</f>
-        <v>0.1000645577792123</v>
       </c>
       <c r="AA31" s="31">
         <f t="shared" ref="AA31" si="33">AA3/Z3-1</f>
+        <v>0.1000645577792123</v>
+      </c>
+      <c r="AB31" s="31">
+        <f t="shared" ref="AB31" si="34">AB3/AA3-1</f>
         <v>2.6408450704225261E-2</v>
       </c>
-      <c r="AB31" s="31">
-        <f t="shared" ref="AB31:AC31" si="34">AB3/AA3-1</f>
+      <c r="AC31" s="31">
+        <f t="shared" ref="AC31:AD31" si="35">AC3/AB3-1</f>
         <v>4.9170954831332159E-2</v>
       </c>
-      <c r="AC31" s="31">
-        <f t="shared" si="34"/>
+      <c r="AD31" s="31">
+        <f t="shared" si="35"/>
         <v>1.2534059945504161E-2</v>
-      </c>
-      <c r="AD31" s="31">
-        <f>AD3/AC3-1</f>
-        <v>3.1754574811625469E-2</v>
       </c>
       <c r="AE31" s="31">
         <f>AE3/AD3-1</f>
-        <v>-6.7814293166406081E-3</v>
+        <v>3.1754574811625469E-2</v>
       </c>
       <c r="AF31" s="31">
         <f>AF3/AE3-1</f>
+        <v>-6.7814293166406081E-3</v>
+      </c>
+      <c r="AG31" s="31">
+        <f>AG3/AF3-1</f>
         <v>4.8319327731092487E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:32" s="77" customFormat="1" ht="12.75" customHeight="1">
+    <row r="32" spans="1:33" s="77" customFormat="1" ht="12.75" customHeight="1">
       <c r="A32" s="81" t="s">
         <v>211</v>
       </c>
@@ -26855,31 +26952,31 @@
         <v>186</v>
       </c>
       <c r="F32" s="77">
-        <f t="shared" ref="F32" si="35">F3-B3</f>
+        <f t="shared" ref="F32" si="36">F3-B3</f>
         <v>25</v>
       </c>
       <c r="G32" s="77">
-        <f t="shared" ref="G32" si="36">G3-C3</f>
+        <f t="shared" ref="G32" si="37">G3-C3</f>
         <v>88</v>
       </c>
       <c r="H32" s="77">
-        <f t="shared" ref="H32" si="37">H3-D3</f>
+        <f t="shared" ref="H32" si="38">H3-D3</f>
         <v>181</v>
       </c>
       <c r="I32" s="77">
-        <f t="shared" ref="I32:L32" si="38">I3-E3</f>
+        <f t="shared" ref="I32:L32" si="39">I3-E3</f>
         <v>59</v>
       </c>
       <c r="J32" s="77">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>42</v>
       </c>
       <c r="K32" s="77">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>12</v>
       </c>
       <c r="L32" s="77">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>13</v>
       </c>
       <c r="M32" s="77">
@@ -26887,15 +26984,15 @@
         <v>-13</v>
       </c>
       <c r="N32" s="77">
-        <f t="shared" ref="N32" si="39">N3-J3</f>
+        <f t="shared" ref="N32" si="40">N3-J3</f>
         <v>2</v>
       </c>
       <c r="O32" s="77">
-        <f t="shared" ref="O32" si="40">O3-K3</f>
+        <f t="shared" ref="O32" si="41">O3-K3</f>
         <v>50</v>
       </c>
       <c r="P32" s="77">
-        <f t="shared" ref="P32" si="41">P3-L3</f>
+        <f t="shared" ref="P32" si="42">P3-L3</f>
         <v>66</v>
       </c>
       <c r="Q32" s="77">
@@ -26915,46 +27012,50 @@
         <v>27</v>
       </c>
       <c r="U32" s="77">
-        <f t="shared" ref="U32" si="42">U3-Q3</f>
+        <f t="shared" ref="U32" si="43">U3-Q3</f>
         <v>23</v>
       </c>
       <c r="V32" s="77">
-        <f t="shared" ref="V32" si="43">V3-R3</f>
+        <f t="shared" ref="V32" si="44">V3-R3</f>
         <v>24</v>
       </c>
-      <c r="Y32" s="59" t="s">
+      <c r="W32" s="77">
+        <f t="shared" ref="W32" si="45">W3-S3</f>
+        <v>23</v>
+      </c>
+      <c r="Z32" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="Z32" s="77">
-        <f t="shared" ref="Z32" si="44">Z3-Y3</f>
+      <c r="AA32" s="77">
+        <f t="shared" ref="AA32" si="46">AA3-Z3</f>
         <v>155</v>
       </c>
-      <c r="AA32" s="77">
-        <f t="shared" ref="AA32" si="45">AA3-Z3</f>
+      <c r="AB32" s="77">
+        <f t="shared" ref="AB32" si="47">AB3-AA3</f>
         <v>45</v>
       </c>
-      <c r="AB32" s="77">
-        <f t="shared" ref="AB32:AC32" si="46">AB3-AA3</f>
+      <c r="AC32" s="77">
+        <f t="shared" ref="AC32:AD32" si="48">AC3-AB3</f>
         <v>86</v>
       </c>
-      <c r="AC32" s="77">
-        <f t="shared" si="46"/>
+      <c r="AD32" s="77">
+        <f t="shared" si="48"/>
         <v>23</v>
-      </c>
-      <c r="AD32" s="77">
-        <f>AD3-AC3</f>
-        <v>59</v>
       </c>
       <c r="AE32" s="77">
         <f>AE3-AD3</f>
-        <v>-13</v>
+        <v>59</v>
       </c>
       <c r="AF32" s="77">
         <f>AF3-AE3</f>
+        <v>-13</v>
+      </c>
+      <c r="AG32" s="77">
+        <f>AG3-AF3</f>
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="12.75" customHeight="1">
+    <row r="33" spans="1:33" ht="12.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>212</v>
       </c>
@@ -26962,87 +27063,88 @@
         <v>186</v>
       </c>
       <c r="C33" s="24">
-        <f t="shared" ref="C33" si="47">C3/B3-1</f>
+        <f t="shared" ref="C33" si="49">C3/B3-1</f>
         <v>-1.7983651226158082E-2</v>
       </c>
       <c r="D33" s="24">
-        <f t="shared" ref="D33" si="48">D3/C3-1</f>
+        <f t="shared" ref="D33" si="50">D3/C3-1</f>
         <v>-5.2164261931187617E-2</v>
       </c>
       <c r="E33" s="24">
-        <f t="shared" ref="E33" si="49">E3/D3-1</f>
+        <f t="shared" ref="E33" si="51">E3/D3-1</f>
         <v>8.7822014051522235E-2</v>
       </c>
       <c r="F33" s="24">
-        <f t="shared" ref="F33" si="50">F3/E3-1</f>
+        <f t="shared" ref="F33" si="52">F3/E3-1</f>
         <v>1.0764262648008671E-3</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" ref="G33" si="51">G3/F3-1</f>
+        <f t="shared" ref="G33" si="53">G3/F3-1</f>
         <v>1.6129032258064502E-2</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" ref="H33" si="52">H3/G3-1</f>
+        <f t="shared" ref="H33" si="54">H3/G3-1</f>
         <v>-5.2910052910049021E-4</v>
       </c>
       <c r="I33" s="24">
-        <f t="shared" ref="I33" si="53">I3/H3-1</f>
+        <f t="shared" ref="I33" si="55">I3/H3-1</f>
         <v>1.4822657490735747E-2</v>
       </c>
       <c r="J33" s="24">
-        <f t="shared" ref="J33" si="54">J3/I3-1</f>
+        <f t="shared" ref="J33" si="56">J3/I3-1</f>
         <v>-7.8247261345852914E-3</v>
       </c>
       <c r="K33" s="24">
-        <f t="shared" ref="K33" si="55">K3/J3-1</f>
+        <f t="shared" ref="K33" si="57">K3/J3-1</f>
         <v>0</v>
       </c>
       <c r="L33" s="24">
-        <f t="shared" ref="L33" si="56">L3/K3-1</f>
+        <f t="shared" ref="L33" si="58">L3/K3-1</f>
         <v>0</v>
       </c>
       <c r="M33" s="24">
-        <f t="shared" ref="M33" si="57">M3/L3-1</f>
+        <f t="shared" ref="M33" si="59">M3/L3-1</f>
         <v>1.051524710830698E-3</v>
       </c>
       <c r="N33" s="24">
-        <f t="shared" ref="N33" si="58">N3/M3-1</f>
+        <f t="shared" ref="N33" si="60">N3/M3-1</f>
         <v>0</v>
       </c>
       <c r="O33" s="24">
-        <f t="shared" ref="O33" si="59">O3/N3-1</f>
+        <f t="shared" ref="O33" si="61">O3/N3-1</f>
         <v>2.5210084033613356E-2</v>
       </c>
       <c r="P33" s="24">
-        <f t="shared" ref="P33:T33" si="60">P3/O3-1</f>
+        <f t="shared" ref="P33:T33" si="62">P3/O3-1</f>
         <v>8.1967213114753079E-3</v>
       </c>
       <c r="Q33" s="24">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>1.4227642276422703E-2</v>
       </c>
       <c r="R33" s="24">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>-2.0040080160320661E-3</v>
       </c>
       <c r="S33" s="24">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>4.0160642570281624E-3</v>
       </c>
       <c r="T33" s="24">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>-2.4999999999999467E-3</v>
       </c>
       <c r="U33" s="24">
-        <f t="shared" ref="U33" si="61">U3/T3-1</f>
+        <f t="shared" ref="U33" si="63">U3/T3-1</f>
         <v>1.2030075187969835E-2</v>
       </c>
       <c r="V33" s="24">
-        <f t="shared" ref="V33" si="62">V3/U3-1</f>
+        <f t="shared" ref="V33" si="64">V3/U3-1</f>
         <v>-1.4858841010401136E-3</v>
       </c>
-      <c r="Y33" s="59" t="s">
-        <v>186</v>
+      <c r="W33" s="24">
+        <f t="shared" ref="W33" si="65">W3/V3-1</f>
+        <v>3.4722222222223209E-3</v>
       </c>
       <c r="Z33" s="59" t="s">
         <v>186</v>
@@ -27065,8 +27167,11 @@
       <c r="AF33" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AG33" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="34" spans="1:32" s="78" customFormat="1" ht="12.75" customHeight="1">
+    <row r="34" spans="1:33" s="78" customFormat="1" ht="12.75" customHeight="1">
       <c r="A34" s="82" t="s">
         <v>212</v>
       </c>
@@ -27074,87 +27179,88 @@
         <v>186</v>
       </c>
       <c r="C34" s="77">
-        <f t="shared" ref="C34" si="63">C3-B3</f>
+        <f t="shared" ref="C34" si="66">C3-B3</f>
         <v>-33</v>
       </c>
       <c r="D34" s="77">
-        <f t="shared" ref="D34" si="64">D3-C3</f>
+        <f t="shared" ref="D34" si="67">D3-C3</f>
         <v>-94</v>
       </c>
       <c r="E34" s="77">
-        <f t="shared" ref="E34" si="65">E3-D3</f>
+        <f t="shared" ref="E34" si="68">E3-D3</f>
         <v>150</v>
       </c>
       <c r="F34" s="77">
-        <f t="shared" ref="F34" si="66">F3-E3</f>
+        <f t="shared" ref="F34" si="69">F3-E3</f>
         <v>2</v>
       </c>
       <c r="G34" s="77">
-        <f t="shared" ref="G34" si="67">G3-F3</f>
+        <f t="shared" ref="G34" si="70">G3-F3</f>
         <v>30</v>
       </c>
       <c r="H34" s="77">
-        <f t="shared" ref="H34" si="68">H3-G3</f>
+        <f t="shared" ref="H34" si="71">H3-G3</f>
         <v>-1</v>
       </c>
       <c r="I34" s="77">
-        <f t="shared" ref="I34" si="69">I3-H3</f>
+        <f t="shared" ref="I34" si="72">I3-H3</f>
         <v>28</v>
       </c>
       <c r="J34" s="77">
-        <f t="shared" ref="J34" si="70">J3-I3</f>
+        <f t="shared" ref="J34" si="73">J3-I3</f>
         <v>-15</v>
       </c>
       <c r="K34" s="77">
-        <f t="shared" ref="K34" si="71">K3-J3</f>
+        <f t="shared" ref="K34" si="74">K3-J3</f>
         <v>0</v>
       </c>
       <c r="L34" s="77">
-        <f t="shared" ref="L34" si="72">L3-K3</f>
+        <f t="shared" ref="L34" si="75">L3-K3</f>
         <v>0</v>
       </c>
       <c r="M34" s="77">
-        <f t="shared" ref="M34" si="73">M3-L3</f>
+        <f t="shared" ref="M34" si="76">M3-L3</f>
         <v>2</v>
       </c>
       <c r="N34" s="77">
-        <f t="shared" ref="N34" si="74">N3-M3</f>
+        <f t="shared" ref="N34" si="77">N3-M3</f>
         <v>0</v>
       </c>
       <c r="O34" s="77">
-        <f t="shared" ref="O34" si="75">O3-N3</f>
+        <f t="shared" ref="O34" si="78">O3-N3</f>
         <v>48</v>
       </c>
       <c r="P34" s="77">
-        <f t="shared" ref="P34:T34" si="76">P3-O3</f>
+        <f t="shared" ref="P34:T34" si="79">P3-O3</f>
         <v>16</v>
       </c>
       <c r="Q34" s="77">
-        <f t="shared" si="76"/>
+        <f t="shared" si="79"/>
         <v>28</v>
       </c>
       <c r="R34" s="77">
-        <f t="shared" si="76"/>
+        <f t="shared" si="79"/>
         <v>-4</v>
       </c>
       <c r="S34" s="77">
-        <f t="shared" si="76"/>
+        <f t="shared" si="79"/>
         <v>8</v>
       </c>
       <c r="T34" s="77">
-        <f t="shared" si="76"/>
+        <f t="shared" si="79"/>
         <v>-5</v>
       </c>
       <c r="U34" s="77">
-        <f t="shared" ref="U34" si="77">U3-T3</f>
+        <f t="shared" ref="U34" si="80">U3-T3</f>
         <v>24</v>
       </c>
       <c r="V34" s="77">
-        <f t="shared" ref="V34" si="78">V3-U3</f>
+        <f t="shared" ref="V34" si="81">V3-U3</f>
         <v>-3</v>
       </c>
-      <c r="Y34" s="59" t="s">
-        <v>186</v>
+      <c r="W34" s="77">
+        <f t="shared" ref="W34" si="82">W3-V3</f>
+        <v>7</v>
       </c>
       <c r="Z34" s="59" t="s">
         <v>186</v>
@@ -27177,11 +27283,14 @@
       <c r="AF34" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AG34" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="35" spans="1:32" ht="12.75" customHeight="1">
-      <c r="AF35" s="24"/>
+    <row r="35" spans="1:33" ht="12.75" customHeight="1">
+      <c r="AG35" s="24"/>
     </row>
-    <row r="36" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="36" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
@@ -27198,31 +27307,31 @@
         <v>186</v>
       </c>
       <c r="F36" s="31">
-        <f t="shared" ref="F36" si="79">F12/B12-1</f>
+        <f t="shared" ref="F36" si="83">F12/B12-1</f>
         <v>6.1527581329561487E-2</v>
       </c>
       <c r="G36" s="31">
-        <f t="shared" ref="G36" si="80">G12/C12-1</f>
+        <f t="shared" ref="G36" si="84">G12/C12-1</f>
         <v>5.8945908460471541E-2</v>
       </c>
       <c r="H36" s="31">
-        <f t="shared" ref="H36" si="81">H12/D12-1</f>
+        <f t="shared" ref="H36" si="85">H12/D12-1</f>
         <v>5.9711736444749475E-2</v>
       </c>
       <c r="I36" s="31">
-        <f t="shared" ref="I36:L36" si="82">I12/E12-1</f>
+        <f t="shared" ref="I36:L36" si="86">I12/E12-1</f>
         <v>5.9731543624160999E-2</v>
       </c>
       <c r="J36" s="31">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>5.5296469020652994E-2</v>
       </c>
       <c r="K36" s="31">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>3.9947609692206898E-2</v>
       </c>
       <c r="L36" s="31">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>3.303108808290145E-2</v>
       </c>
       <c r="M36" s="31">
@@ -27230,15 +27339,15 @@
         <v>2.7865737808739688E-2</v>
       </c>
       <c r="N36" s="31">
-        <f t="shared" ref="N36" si="83">N12/J12-1</f>
+        <f t="shared" ref="N36" si="87">N12/J12-1</f>
         <v>3.0303030303030276E-2</v>
       </c>
       <c r="O36" s="31">
-        <f t="shared" ref="O36" si="84">O12/K12-1</f>
+        <f t="shared" ref="O36" si="88">O12/K12-1</f>
         <v>3.6523929471032668E-2</v>
       </c>
       <c r="P36" s="31">
-        <f t="shared" ref="P36" si="85">P12/L12-1</f>
+        <f t="shared" ref="P36" si="89">P12/L12-1</f>
         <v>3.7617554858934144E-2</v>
       </c>
       <c r="Q36" s="31">
@@ -27258,46 +27367,50 @@
         <v>2.5981873111782461E-2</v>
       </c>
       <c r="U36" s="31">
-        <f t="shared" ref="U36" si="86">U12/Q12-1</f>
+        <f t="shared" ref="U36" si="90">U12/Q12-1</f>
         <v>3.4111310592459532E-2</v>
       </c>
       <c r="V36" s="31">
-        <f t="shared" ref="V36" si="87">V12/R12-1</f>
+        <f t="shared" ref="V36" si="91">V12/R12-1</f>
         <v>3.4585569469290478E-2</v>
       </c>
-      <c r="Y36" s="59" t="s">
+      <c r="W36" s="31">
+        <f t="shared" ref="W36" si="92">W12/S12-1</f>
+        <v>3.7914691943127909E-2</v>
+      </c>
+      <c r="Z36" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="Z36" s="31">
-        <f t="shared" ref="Z36" si="88">Z12/Y12-1</f>
+      <c r="AA36" s="31">
+        <f t="shared" ref="AA36" si="93">AA12/Z12-1</f>
         <v>8.3486238532110013E-2</v>
       </c>
-      <c r="AA36" s="31">
-        <f t="shared" ref="AA36" si="89">AA12/Z12-1</f>
+      <c r="AB36" s="31">
+        <f t="shared" ref="AB36" si="94">AB12/AA12-1</f>
         <v>9.9915325994919479E-2</v>
       </c>
-      <c r="AB36" s="31">
-        <f t="shared" ref="AB36:AC36" si="90">AB12/AA12-1</f>
+      <c r="AC36" s="31">
+        <f t="shared" ref="AC36:AD36" si="95">AC12/AB12-1</f>
         <v>7.7752117013087041E-2</v>
       </c>
-      <c r="AC36" s="31">
-        <f t="shared" si="90"/>
+      <c r="AD36" s="31">
+        <f t="shared" si="95"/>
         <v>6.4285714285714279E-2</v>
-      </c>
-      <c r="AD36" s="31">
-        <f>AD12/AC12-1</f>
-        <v>5.9731543624160999E-2</v>
       </c>
       <c r="AE36" s="31">
         <f>AE12/AD12-1</f>
-        <v>2.7865737808739688E-2</v>
+        <v>5.9731543624160999E-2</v>
       </c>
       <c r="AF36" s="31">
         <f>AF12/AE12-1</f>
+        <v>2.7865737808739688E-2</v>
+      </c>
+      <c r="AG36" s="31">
+        <f>AG12/AF12-1</f>
         <v>2.9574861367837268E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:32" s="77" customFormat="1" ht="12.75" customHeight="1">
+    <row r="37" spans="1:33" s="77" customFormat="1" ht="12.75" customHeight="1">
       <c r="A37" s="81" t="s">
         <v>202</v>
       </c>
@@ -27314,31 +27427,31 @@
         <v>186</v>
       </c>
       <c r="F37" s="77">
-        <f t="shared" ref="F37" si="91">F12-B12</f>
+        <f t="shared" ref="F37" si="96">F12-B12</f>
         <v>87</v>
       </c>
       <c r="G37" s="77">
-        <f t="shared" ref="G37" si="92">G12-C12</f>
+        <f t="shared" ref="G37" si="97">G12-C12</f>
         <v>85</v>
       </c>
       <c r="H37" s="77">
-        <f t="shared" ref="H37" si="93">H12-D12</f>
+        <f t="shared" ref="H37" si="98">H12-D12</f>
         <v>87</v>
       </c>
       <c r="I37" s="77">
-        <f t="shared" ref="I37:L37" si="94">I12-E12</f>
+        <f t="shared" ref="I37:L37" si="99">I12-E12</f>
         <v>89</v>
       </c>
       <c r="J37" s="77">
-        <f t="shared" si="94"/>
+        <f t="shared" si="99"/>
         <v>83</v>
       </c>
       <c r="K37" s="77">
-        <f t="shared" si="94"/>
+        <f t="shared" si="99"/>
         <v>61</v>
       </c>
       <c r="L37" s="77">
-        <f t="shared" si="94"/>
+        <f t="shared" si="99"/>
         <v>51</v>
       </c>
       <c r="M37" s="77">
@@ -27346,15 +27459,15 @@
         <v>44</v>
       </c>
       <c r="N37" s="77">
-        <f t="shared" ref="N37" si="95">N12-J12</f>
+        <f t="shared" ref="N37" si="100">N12-J12</f>
         <v>48</v>
       </c>
       <c r="O37" s="77">
-        <f t="shared" ref="O37" si="96">O12-K12</f>
+        <f t="shared" ref="O37" si="101">O12-K12</f>
         <v>58</v>
       </c>
       <c r="P37" s="77">
-        <f t="shared" ref="P37" si="97">P12-L12</f>
+        <f t="shared" ref="P37" si="102">P12-L12</f>
         <v>60</v>
       </c>
       <c r="Q37" s="77">
@@ -27374,46 +27487,50 @@
         <v>43</v>
       </c>
       <c r="U37" s="77">
-        <f t="shared" ref="U37" si="98">U12-Q12</f>
+        <f t="shared" ref="U37" si="103">U12-Q12</f>
         <v>57</v>
       </c>
       <c r="V37" s="77">
-        <f t="shared" ref="V37" si="99">V12-R12</f>
+        <f t="shared" ref="V37" si="104">V12-R12</f>
         <v>58</v>
       </c>
-      <c r="Y37" s="59" t="s">
+      <c r="W37" s="77">
+        <f t="shared" ref="W37" si="105">W12-S12</f>
+        <v>64</v>
+      </c>
+      <c r="Z37" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="Z37" s="77">
-        <f t="shared" ref="Z37" si="100">Z12-Y12</f>
+      <c r="AA37" s="77">
+        <f t="shared" ref="AA37" si="106">AA12-Z12</f>
         <v>91</v>
       </c>
-      <c r="AA37" s="77">
-        <f t="shared" ref="AA37" si="101">AA12-Z12</f>
+      <c r="AB37" s="77">
+        <f t="shared" ref="AB37" si="107">AB12-AA12</f>
         <v>118</v>
       </c>
-      <c r="AB37" s="77">
-        <f t="shared" ref="AB37:AC37" si="102">AB12-AA12</f>
+      <c r="AC37" s="77">
+        <f t="shared" ref="AC37:AD37" si="108">AC12-AB12</f>
         <v>101</v>
       </c>
-      <c r="AC37" s="77">
-        <f t="shared" si="102"/>
+      <c r="AD37" s="77">
+        <f t="shared" si="108"/>
         <v>90</v>
-      </c>
-      <c r="AD37" s="77">
-        <f>AD12-AC12</f>
-        <v>89</v>
       </c>
       <c r="AE37" s="77">
         <f>AE12-AD12</f>
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="AF37" s="77">
         <f>AF12-AE12</f>
+        <v>44</v>
+      </c>
+      <c r="AG37" s="77">
+        <f>AG12-AF12</f>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:32" ht="12.75" customHeight="1">
+    <row r="38" spans="1:33" ht="12.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>203</v>
       </c>
@@ -27421,87 +27538,88 @@
         <v>186</v>
       </c>
       <c r="C38" s="24">
-        <f t="shared" ref="C38" si="103">C12/B12-1</f>
+        <f t="shared" ref="C38" si="109">C12/B12-1</f>
         <v>1.980198019801982E-2</v>
       </c>
       <c r="D38" s="24">
-        <f t="shared" ref="D38" si="104">D12/C12-1</f>
+        <f t="shared" ref="D38" si="110">D12/C12-1</f>
         <v>1.0402219140083213E-2</v>
       </c>
       <c r="E38" s="24">
-        <f t="shared" ref="E38" si="105">E12/D12-1</f>
+        <f t="shared" ref="E38" si="111">E12/D12-1</f>
         <v>2.2649279341111939E-2</v>
       </c>
       <c r="F38" s="24">
-        <f t="shared" ref="F38" si="106">F12/E12-1</f>
+        <f t="shared" ref="F38" si="112">F12/E12-1</f>
         <v>7.382550335570448E-3</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" ref="G38" si="107">G12/F12-1</f>
+        <f t="shared" ref="G38" si="113">G12/F12-1</f>
         <v>1.7321785476348994E-2</v>
       </c>
       <c r="H38" s="24">
-        <f t="shared" ref="H38" si="108">H12/G12-1</f>
+        <f t="shared" ref="H38" si="114">H12/G12-1</f>
         <v>1.1132940406024971E-2</v>
       </c>
       <c r="I38" s="24">
-        <f t="shared" ref="I38" si="109">I12/H12-1</f>
+        <f t="shared" ref="I38" si="115">I12/H12-1</f>
         <v>2.26683937823835E-2</v>
       </c>
       <c r="J38" s="24">
-        <f t="shared" ref="J38" si="110">J12/I12-1</f>
+        <f t="shared" ref="J38" si="116">J12/I12-1</f>
         <v>3.1665611146294292E-3</v>
       </c>
       <c r="K38" s="24">
-        <f t="shared" ref="K38" si="111">K12/J12-1</f>
+        <f t="shared" ref="K38" si="117">K12/J12-1</f>
         <v>2.525252525252597E-3</v>
       </c>
       <c r="L38" s="24">
-        <f t="shared" ref="L38" si="112">L12/K12-1</f>
+        <f t="shared" ref="L38" si="118">L12/K12-1</f>
         <v>4.4080604534004753E-3</v>
       </c>
       <c r="M38" s="24">
-        <f t="shared" ref="M38" si="113">M12/L12-1</f>
+        <f t="shared" ref="M38" si="119">M12/L12-1</f>
         <v>1.7554858934169193E-2</v>
       </c>
       <c r="N38" s="24">
-        <f t="shared" ref="N38" si="114">N12/M12-1</f>
+        <f t="shared" ref="N38" si="120">N12/M12-1</f>
         <v>5.5452865064695711E-3</v>
       </c>
       <c r="O38" s="24">
-        <f t="shared" ref="O38" si="115">O12/N12-1</f>
+        <f t="shared" ref="O38" si="121">O12/N12-1</f>
         <v>8.5784313725489891E-3</v>
       </c>
       <c r="P38" s="24">
-        <f t="shared" ref="P38:T38" si="116">P12/O12-1</f>
+        <f t="shared" ref="P38:T38" si="122">P12/O12-1</f>
         <v>5.4678007290400732E-3</v>
       </c>
       <c r="Q38" s="24">
-        <f t="shared" si="116"/>
+        <f t="shared" si="122"/>
         <v>9.6676737160121817E-3</v>
       </c>
       <c r="R38" s="24">
-        <f t="shared" si="116"/>
+        <f t="shared" si="122"/>
         <v>3.5906642728904536E-3</v>
       </c>
       <c r="S38" s="24">
-        <f t="shared" si="116"/>
+        <f t="shared" si="122"/>
         <v>6.5593321407275695E-3</v>
       </c>
       <c r="T38" s="24">
-        <f t="shared" si="116"/>
+        <f t="shared" si="122"/>
         <v>5.924170616113722E-3</v>
       </c>
       <c r="U38" s="24">
-        <f t="shared" ref="U38" si="117">U12/T12-1</f>
+        <f t="shared" ref="U38" si="123">U12/T12-1</f>
         <v>1.7667844522968101E-2</v>
       </c>
       <c r="V38" s="24">
-        <f t="shared" ref="V38" si="118">V12/U12-1</f>
+        <f t="shared" ref="V38" si="124">V12/U12-1</f>
         <v>4.050925925925819E-3</v>
       </c>
-      <c r="Y38" s="59" t="s">
-        <v>186</v>
+      <c r="W38" s="24">
+        <f t="shared" ref="W38" si="125">W12/V12-1</f>
+        <v>9.7982708933717078E-3</v>
       </c>
       <c r="Z38" s="59" t="s">
         <v>186</v>
@@ -27524,8 +27642,11 @@
       <c r="AF38" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AG38" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="39" spans="1:32" s="79" customFormat="1" ht="12.75" customHeight="1">
+    <row r="39" spans="1:33" s="79" customFormat="1" ht="12.75" customHeight="1">
       <c r="A39" s="83" t="s">
         <v>203</v>
       </c>
@@ -27533,87 +27654,88 @@
         <v>186</v>
       </c>
       <c r="C39" s="77">
-        <f t="shared" ref="C39" si="119">C12-B12</f>
+        <f t="shared" ref="C39" si="126">C12-B12</f>
         <v>28</v>
       </c>
       <c r="D39" s="77">
-        <f t="shared" ref="D39" si="120">D12-C12</f>
+        <f t="shared" ref="D39" si="127">D12-C12</f>
         <v>15</v>
       </c>
       <c r="E39" s="77">
-        <f t="shared" ref="E39" si="121">E12-D12</f>
+        <f t="shared" ref="E39" si="128">E12-D12</f>
         <v>33</v>
       </c>
       <c r="F39" s="77">
-        <f t="shared" ref="F39" si="122">F12-E12</f>
+        <f t="shared" ref="F39" si="129">F12-E12</f>
         <v>11</v>
       </c>
       <c r="G39" s="77">
-        <f t="shared" ref="G39" si="123">G12-F12</f>
+        <f t="shared" ref="G39" si="130">G12-F12</f>
         <v>26</v>
       </c>
       <c r="H39" s="77">
-        <f t="shared" ref="H39" si="124">H12-G12</f>
+        <f t="shared" ref="H39" si="131">H12-G12</f>
         <v>17</v>
       </c>
       <c r="I39" s="77">
-        <f t="shared" ref="I39" si="125">I12-H12</f>
+        <f t="shared" ref="I39" si="132">I12-H12</f>
         <v>35</v>
       </c>
       <c r="J39" s="77">
-        <f t="shared" ref="J39" si="126">J12-I12</f>
+        <f t="shared" ref="J39" si="133">J12-I12</f>
         <v>5</v>
       </c>
       <c r="K39" s="77">
-        <f t="shared" ref="K39" si="127">K12-J12</f>
+        <f t="shared" ref="K39" si="134">K12-J12</f>
         <v>4</v>
       </c>
       <c r="L39" s="77">
-        <f t="shared" ref="L39" si="128">L12-K12</f>
+        <f t="shared" ref="L39" si="135">L12-K12</f>
         <v>7</v>
       </c>
       <c r="M39" s="77">
-        <f t="shared" ref="M39" si="129">M12-L12</f>
+        <f t="shared" ref="M39" si="136">M12-L12</f>
         <v>28</v>
       </c>
       <c r="N39" s="77">
-        <f t="shared" ref="N39" si="130">N12-M12</f>
+        <f t="shared" ref="N39" si="137">N12-M12</f>
         <v>9</v>
       </c>
       <c r="O39" s="77">
-        <f t="shared" ref="O39" si="131">O12-N12</f>
+        <f t="shared" ref="O39" si="138">O12-N12</f>
         <v>14</v>
       </c>
       <c r="P39" s="77">
-        <f t="shared" ref="P39:T39" si="132">P12-O12</f>
+        <f t="shared" ref="P39:T39" si="139">P12-O12</f>
         <v>9</v>
       </c>
       <c r="Q39" s="77">
-        <f t="shared" si="132"/>
+        <f t="shared" si="139"/>
         <v>16</v>
       </c>
       <c r="R39" s="77">
-        <f t="shared" si="132"/>
+        <f t="shared" si="139"/>
         <v>6</v>
       </c>
       <c r="S39" s="77">
-        <f t="shared" si="132"/>
+        <f t="shared" si="139"/>
         <v>11</v>
       </c>
       <c r="T39" s="77">
-        <f t="shared" si="132"/>
+        <f t="shared" si="139"/>
         <v>10</v>
       </c>
       <c r="U39" s="77">
-        <f t="shared" ref="U39" si="133">U12-T12</f>
+        <f t="shared" ref="U39" si="140">U12-T12</f>
         <v>30</v>
       </c>
       <c r="V39" s="77">
-        <f t="shared" ref="V39" si="134">V12-U12</f>
+        <f t="shared" ref="V39" si="141">V12-U12</f>
         <v>7</v>
       </c>
-      <c r="Y39" s="59" t="s">
-        <v>186</v>
+      <c r="W39" s="77">
+        <f t="shared" ref="W39" si="142">W12-V12</f>
+        <v>17</v>
       </c>
       <c r="Z39" s="59" t="s">
         <v>186</v>
@@ -27636,11 +27758,14 @@
       <c r="AF39" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AG39" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="40" spans="1:32" ht="12.75" customHeight="1">
-      <c r="AF40" s="24"/>
+    <row r="40" spans="1:33" ht="12.75" customHeight="1">
+      <c r="AG40" s="24"/>
     </row>
-    <row r="41" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="41" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>213</v>
       </c>
@@ -27657,51 +27782,51 @@
         <v>186</v>
       </c>
       <c r="F41" s="31">
-        <f t="shared" ref="F41" si="135">F21/B21-1</f>
+        <f t="shared" ref="F41" si="143">F21/B21-1</f>
         <v>-0.14726840855106893</v>
       </c>
       <c r="G41" s="31">
-        <f t="shared" ref="G41" si="136">G21/C21-1</f>
+        <f t="shared" ref="G41" si="144">G21/C21-1</f>
         <v>8.3333333333333037E-3</v>
       </c>
       <c r="H41" s="31">
-        <f t="shared" ref="H41" si="137">H21/D21-1</f>
+        <f t="shared" ref="H41" si="145">H21/D21-1</f>
         <v>0.3745019920318724</v>
       </c>
       <c r="I41" s="31">
-        <f t="shared" ref="I41" si="138">I21/E21-1</f>
+        <f t="shared" ref="I41" si="146">I21/E21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
       <c r="J41" s="31">
-        <f t="shared" ref="J41" si="139">J21/F21-1</f>
+        <f t="shared" ref="J41" si="147">J21/F21-1</f>
         <v>-0.11420612813370479</v>
       </c>
       <c r="K41" s="31">
-        <f t="shared" ref="K41" si="140">K21/G21-1</f>
+        <f t="shared" ref="K41" si="148">K21/G21-1</f>
         <v>-0.13498622589531684</v>
       </c>
       <c r="L41" s="31">
-        <f t="shared" ref="L41" si="141">L21/H21-1</f>
+        <f t="shared" ref="L41" si="149">L21/H21-1</f>
         <v>-0.11014492753623184</v>
       </c>
       <c r="M41" s="31">
-        <f t="shared" ref="M41" si="142">M21/I21-1</f>
+        <f t="shared" ref="M41" si="150">M21/I21-1</f>
         <v>-0.16863905325443784</v>
       </c>
       <c r="N41" s="31">
-        <f t="shared" ref="N41" si="143">N21/J21-1</f>
+        <f t="shared" ref="N41" si="151">N21/J21-1</f>
         <v>-0.14465408805031443</v>
       </c>
       <c r="O41" s="31">
-        <f t="shared" ref="O41" si="144">O21/K21-1</f>
+        <f t="shared" ref="O41" si="152">O21/K21-1</f>
         <v>-2.5477707006369421E-2</v>
       </c>
       <c r="P41" s="31">
-        <f t="shared" ref="P41" si="145">P21/L21-1</f>
+        <f t="shared" ref="P41" si="153">P21/L21-1</f>
         <v>1.9543973941368087E-2</v>
       </c>
       <c r="Q41" s="31">
-        <f t="shared" ref="Q41" si="146">Q21/M21-1</f>
+        <f t="shared" ref="Q41" si="154">Q21/M21-1</f>
         <v>0.15658362989323837</v>
       </c>
       <c r="R41" s="31">
@@ -27709,54 +27834,58 @@
         <v>0.15808823529411775</v>
       </c>
       <c r="S41" s="31">
-        <f t="shared" ref="S41:T41" si="147">S21/O21-1</f>
+        <f t="shared" ref="S41:T41" si="155">S21/O21-1</f>
         <v>1.9607843137254832E-2</v>
       </c>
       <c r="T41" s="31">
-        <f t="shared" si="147"/>
+        <f t="shared" si="155"/>
         <v>-5.1118210862619806E-2</v>
       </c>
       <c r="U41" s="31">
-        <f t="shared" ref="U41" si="148">U21/Q21-1</f>
+        <f t="shared" ref="U41" si="156">U21/Q21-1</f>
         <v>-0.10461538461538467</v>
       </c>
       <c r="V41" s="31">
-        <f t="shared" ref="V41" si="149">V21/R21-1</f>
+        <f t="shared" ref="V41" si="157">V21/R21-1</f>
         <v>-0.10793650793650789</v>
       </c>
-      <c r="Y41" s="59" t="s">
+      <c r="W41" s="31">
+        <f t="shared" ref="W41" si="158">W21/S21-1</f>
+        <v>-0.13141025641025639</v>
+      </c>
+      <c r="Z41" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="Z41" s="31">
-        <f t="shared" ref="Z41" si="150">Z21/Y21-1</f>
+      <c r="AA41" s="31">
+        <f t="shared" ref="AA41" si="159">AA21/Z21-1</f>
         <v>0.11764705882352944</v>
       </c>
-      <c r="AA41" s="31">
-        <f t="shared" ref="AA41" si="151">AA21/Z21-1</f>
+      <c r="AB41" s="31">
+        <f t="shared" ref="AB41" si="160">AB21/AA21-1</f>
         <v>-0.1228070175438597</v>
       </c>
-      <c r="AB41" s="31">
-        <f t="shared" ref="AB41" si="152">AB21/AA21-1</f>
+      <c r="AC41" s="31">
+        <f t="shared" ref="AC41" si="161">AC21/AB21-1</f>
         <v>-3.3333333333333326E-2</v>
       </c>
-      <c r="AC41" s="31">
-        <f t="shared" ref="AC41" si="153">AC21/AB21-1</f>
+      <c r="AD41" s="31">
+        <f t="shared" ref="AD41" si="162">AD21/AC21-1</f>
         <v>-0.15402298850574714</v>
       </c>
-      <c r="AD41" s="31">
-        <f t="shared" ref="AD41" si="154">AD21/AC21-1</f>
+      <c r="AE41" s="31">
+        <f t="shared" ref="AE41" si="163">AE21/AD21-1</f>
         <v>-8.1521739130434812E-2</v>
-      </c>
-      <c r="AE41" s="31">
-        <f>AE21/AD21-1</f>
-        <v>-0.16863905325443784</v>
       </c>
       <c r="AF41" s="31">
         <f>AF21/AE21-1</f>
+        <v>-0.16863905325443784</v>
+      </c>
+      <c r="AG41" s="31">
+        <f>AG21/AF21-1</f>
         <v>0.15658362989323837</v>
       </c>
     </row>
-    <row r="42" spans="1:32" s="80" customFormat="1" ht="12.75" customHeight="1">
+    <row r="42" spans="1:33" s="80" customFormat="1" ht="12.75" customHeight="1">
       <c r="A42" s="84" t="s">
         <v>213</v>
       </c>
@@ -27773,31 +27902,31 @@
         <v>186</v>
       </c>
       <c r="F42" s="80">
-        <f t="shared" ref="F42" si="155">F21-B21</f>
+        <f t="shared" ref="F42" si="164">F21-B21</f>
         <v>-62</v>
       </c>
       <c r="G42" s="80">
-        <f t="shared" ref="G42" si="156">G21-C21</f>
+        <f t="shared" ref="G42" si="165">G21-C21</f>
         <v>3</v>
       </c>
       <c r="H42" s="80">
-        <f t="shared" ref="H42" si="157">H21-D21</f>
+        <f t="shared" ref="H42" si="166">H21-D21</f>
         <v>94</v>
       </c>
       <c r="I42" s="80">
-        <f t="shared" ref="I42:L42" si="158">I21-E21</f>
+        <f t="shared" ref="I42:L42" si="167">I21-E21</f>
         <v>-30</v>
       </c>
       <c r="J42" s="80">
-        <f t="shared" si="158"/>
+        <f t="shared" si="167"/>
         <v>-41</v>
       </c>
       <c r="K42" s="80">
-        <f t="shared" si="158"/>
+        <f t="shared" si="167"/>
         <v>-49</v>
       </c>
       <c r="L42" s="80">
-        <f t="shared" si="158"/>
+        <f t="shared" si="167"/>
         <v>-38</v>
       </c>
       <c r="M42" s="80">
@@ -27805,23 +27934,23 @@
         <v>-57</v>
       </c>
       <c r="N42" s="80">
-        <f t="shared" ref="N42" si="159">N21-J21</f>
+        <f t="shared" ref="N42" si="168">N21-J21</f>
         <v>-46</v>
       </c>
       <c r="O42" s="80">
-        <f t="shared" ref="O42" si="160">O21-K21</f>
+        <f t="shared" ref="O42" si="169">O21-K21</f>
         <v>-8</v>
       </c>
       <c r="P42" s="80">
-        <f t="shared" ref="P42" si="161">P21-L21</f>
+        <f t="shared" ref="P42" si="170">P21-L21</f>
         <v>6</v>
       </c>
       <c r="Q42" s="80">
-        <f t="shared" ref="Q42:R42" si="162">Q21-M21</f>
+        <f t="shared" ref="Q42:R42" si="171">Q21-M21</f>
         <v>44</v>
       </c>
       <c r="R42" s="80">
-        <f t="shared" si="162"/>
+        <f t="shared" si="171"/>
         <v>43</v>
       </c>
       <c r="S42" s="80">
@@ -27833,46 +27962,50 @@
         <v>-16</v>
       </c>
       <c r="U42" s="80">
-        <f t="shared" ref="U42" si="163">U21-Q21</f>
+        <f t="shared" ref="U42" si="172">U21-Q21</f>
         <v>-34</v>
       </c>
       <c r="V42" s="80">
-        <f t="shared" ref="V42" si="164">V21-R21</f>
+        <f t="shared" ref="V42" si="173">V21-R21</f>
         <v>-34</v>
       </c>
-      <c r="Y42" s="59" t="s">
+      <c r="W42" s="80">
+        <f t="shared" ref="W42" si="174">W21-S21</f>
+        <v>-41</v>
+      </c>
+      <c r="Z42" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="Z42" s="80">
-        <f t="shared" ref="Z42" si="165">Z21-Y21</f>
+      <c r="AA42" s="80">
+        <f t="shared" ref="AA42" si="175">AA21-Z21</f>
         <v>54</v>
       </c>
-      <c r="AA42" s="80">
-        <f t="shared" ref="AA42" si="166">AA21-Z21</f>
+      <c r="AB42" s="80">
+        <f t="shared" ref="AB42" si="176">AB21-AA21</f>
         <v>-63</v>
       </c>
-      <c r="AB42" s="80">
-        <f t="shared" ref="AB42" si="167">AB21-AA21</f>
+      <c r="AC42" s="80">
+        <f t="shared" ref="AC42" si="177">AC21-AB21</f>
         <v>-15</v>
       </c>
-      <c r="AC42" s="80">
-        <f t="shared" ref="AC42" si="168">AC21-AB21</f>
+      <c r="AD42" s="80">
+        <f t="shared" ref="AD42" si="178">AD21-AC21</f>
         <v>-67</v>
       </c>
-      <c r="AD42" s="80">
-        <f t="shared" ref="AD42:AE42" si="169">AD21-AC21</f>
+      <c r="AE42" s="80">
+        <f t="shared" ref="AE42:AF42" si="179">AE21-AD21</f>
         <v>-30</v>
       </c>
-      <c r="AE42" s="80">
-        <f t="shared" si="169"/>
+      <c r="AF42" s="80">
+        <f t="shared" si="179"/>
         <v>-57</v>
       </c>
-      <c r="AF42" s="80">
-        <f>AF21-AE21</f>
+      <c r="AG42" s="80">
+        <f>AG21-AF21</f>
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:32" ht="12.75" customHeight="1">
+    <row r="43" spans="1:33" ht="12.75" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>214</v>
       </c>
@@ -27880,63 +28013,63 @@
         <v>186</v>
       </c>
       <c r="C43" s="24">
-        <f t="shared" ref="C43" si="170">C21/B21-1</f>
+        <f t="shared" ref="C43" si="180">C21/B21-1</f>
         <v>-0.14489311163895491</v>
       </c>
       <c r="D43" s="24">
-        <f t="shared" ref="D43" si="171">D21/C21-1</f>
+        <f t="shared" ref="D43" si="181">D21/C21-1</f>
         <v>-0.30277777777777781</v>
       </c>
       <c r="E43" s="24">
-        <f t="shared" ref="E43" si="172">E21/D21-1</f>
+        <f t="shared" ref="E43" si="182">E21/D21-1</f>
         <v>0.46613545816733071</v>
       </c>
       <c r="F43" s="24">
-        <f t="shared" ref="F43" si="173">F21/E21-1</f>
+        <f t="shared" ref="F43" si="183">F21/E21-1</f>
         <v>-2.4456521739130488E-2</v>
       </c>
       <c r="G43" s="24">
-        <f t="shared" ref="G43" si="174">G21/F21-1</f>
+        <f t="shared" ref="G43" si="184">G21/F21-1</f>
         <v>1.1142061281337101E-2</v>
       </c>
       <c r="H43" s="24">
-        <f t="shared" ref="H43" si="175">H21/G21-1</f>
+        <f t="shared" ref="H43" si="185">H21/G21-1</f>
         <v>-4.9586776859504078E-2</v>
       </c>
       <c r="I43" s="24">
-        <f t="shared" ref="I43" si="176">I21/H21-1</f>
+        <f t="shared" ref="I43" si="186">I21/H21-1</f>
         <v>-2.0289855072463725E-2</v>
       </c>
       <c r="J43" s="24">
-        <f t="shared" ref="J43" si="177">J21/I21-1</f>
+        <f t="shared" ref="J43" si="187">J21/I21-1</f>
         <v>-5.9171597633136064E-2</v>
       </c>
       <c r="K43" s="24">
-        <f t="shared" ref="K43" si="178">K21/J21-1</f>
+        <f t="shared" ref="K43" si="188">K21/J21-1</f>
         <v>-1.2578616352201255E-2</v>
       </c>
       <c r="L43" s="24">
-        <f t="shared" ref="L43" si="179">L21/K21-1</f>
+        <f t="shared" ref="L43" si="189">L21/K21-1</f>
         <v>-2.2292993630573243E-2</v>
       </c>
       <c r="M43" s="24">
-        <f t="shared" ref="M43" si="180">M21/L21-1</f>
+        <f t="shared" ref="M43" si="190">M21/L21-1</f>
         <v>-8.4690553745928376E-2</v>
       </c>
       <c r="N43" s="24">
-        <f t="shared" ref="N43" si="181">N21/M21-1</f>
+        <f t="shared" ref="N43" si="191">N21/M21-1</f>
         <v>-3.2028469750889688E-2</v>
       </c>
       <c r="O43" s="24">
-        <f t="shared" ref="O43" si="182">O21/N21-1</f>
+        <f t="shared" ref="O43" si="192">O21/N21-1</f>
         <v>0.125</v>
       </c>
       <c r="P43" s="24">
-        <f t="shared" ref="P43" si="183">P21/O21-1</f>
+        <f t="shared" ref="P43" si="193">P21/O21-1</f>
         <v>2.2875816993463971E-2</v>
       </c>
       <c r="Q43" s="24">
-        <f t="shared" ref="Q43" si="184">Q21/P21-1</f>
+        <f t="shared" ref="Q43" si="194">Q21/P21-1</f>
         <v>3.833865814696491E-2</v>
       </c>
       <c r="R43" s="24">
@@ -27944,23 +28077,24 @@
         <v>-3.0769230769230771E-2</v>
       </c>
       <c r="S43" s="24">
-        <f t="shared" ref="S43:T43" si="185">S21/R21-1</f>
+        <f t="shared" ref="S43:T43" si="195">S21/R21-1</f>
         <v>-9.52380952380949E-3</v>
       </c>
       <c r="T43" s="24">
-        <f t="shared" si="185"/>
+        <f t="shared" si="195"/>
         <v>-4.8076923076923128E-2</v>
       </c>
       <c r="U43" s="24">
-        <f t="shared" ref="U43" si="186">U21/T21-1</f>
+        <f t="shared" ref="U43" si="196">U21/T21-1</f>
         <v>-2.0202020202020221E-2</v>
       </c>
       <c r="V43" s="24">
-        <f t="shared" ref="V43" si="187">V21/U21-1</f>
+        <f t="shared" ref="V43" si="197">V21/U21-1</f>
         <v>-3.4364261168384869E-2</v>
       </c>
-      <c r="Y43" s="59" t="s">
-        <v>186</v>
+      <c r="W43" s="24">
+        <f t="shared" ref="W43" si="198">W21/V21-1</f>
+        <v>-3.5587188612099641E-2</v>
       </c>
       <c r="Z43" s="59" t="s">
         <v>186</v>
@@ -27983,8 +28117,11 @@
       <c r="AF43" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AG43" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="44" spans="1:32" s="79" customFormat="1" ht="12.75" customHeight="1">
+    <row r="44" spans="1:33" s="79" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" s="83" t="s">
         <v>214</v>
       </c>
@@ -27992,67 +28129,67 @@
         <v>186</v>
       </c>
       <c r="C44" s="77">
-        <f t="shared" ref="C44" si="188">C21-B21</f>
+        <f t="shared" ref="C44" si="199">C21-B21</f>
         <v>-61</v>
       </c>
       <c r="D44" s="77">
-        <f t="shared" ref="D44" si="189">D21-C21</f>
+        <f t="shared" ref="D44" si="200">D21-C21</f>
         <v>-109</v>
       </c>
       <c r="E44" s="77">
-        <f t="shared" ref="E44" si="190">E21-D21</f>
+        <f t="shared" ref="E44" si="201">E21-D21</f>
         <v>117</v>
       </c>
       <c r="F44" s="77">
-        <f t="shared" ref="F44" si="191">F21-E21</f>
+        <f t="shared" ref="F44" si="202">F21-E21</f>
         <v>-9</v>
       </c>
       <c r="G44" s="77">
-        <f t="shared" ref="G44" si="192">G21-F21</f>
+        <f t="shared" ref="G44" si="203">G21-F21</f>
         <v>4</v>
       </c>
       <c r="H44" s="77">
-        <f t="shared" ref="H44" si="193">H21-G21</f>
+        <f t="shared" ref="H44" si="204">H21-G21</f>
         <v>-18</v>
       </c>
       <c r="I44" s="77">
-        <f t="shared" ref="I44" si="194">I21-H21</f>
+        <f t="shared" ref="I44" si="205">I21-H21</f>
         <v>-7</v>
       </c>
       <c r="J44" s="77">
-        <f t="shared" ref="J44" si="195">J21-I21</f>
+        <f t="shared" ref="J44" si="206">J21-I21</f>
         <v>-20</v>
       </c>
       <c r="K44" s="77">
-        <f t="shared" ref="K44" si="196">K21-J21</f>
+        <f t="shared" ref="K44" si="207">K21-J21</f>
         <v>-4</v>
       </c>
       <c r="L44" s="77">
-        <f t="shared" ref="L44" si="197">L21-K21</f>
+        <f t="shared" ref="L44" si="208">L21-K21</f>
         <v>-7</v>
       </c>
       <c r="M44" s="77">
-        <f t="shared" ref="M44" si="198">M21-L21</f>
+        <f t="shared" ref="M44" si="209">M21-L21</f>
         <v>-26</v>
       </c>
       <c r="N44" s="77">
-        <f t="shared" ref="N44" si="199">N21-M21</f>
+        <f t="shared" ref="N44" si="210">N21-M21</f>
         <v>-9</v>
       </c>
       <c r="O44" s="77">
-        <f t="shared" ref="O44" si="200">O21-N21</f>
+        <f t="shared" ref="O44" si="211">O21-N21</f>
         <v>34</v>
       </c>
       <c r="P44" s="77">
-        <f t="shared" ref="P44:R44" si="201">P21-O21</f>
+        <f t="shared" ref="P44:R44" si="212">P21-O21</f>
         <v>7</v>
       </c>
       <c r="Q44" s="77">
-        <f t="shared" si="201"/>
+        <f t="shared" si="212"/>
         <v>12</v>
       </c>
       <c r="R44" s="77">
-        <f t="shared" si="201"/>
+        <f t="shared" si="212"/>
         <v>-10</v>
       </c>
       <c r="S44" s="77">
@@ -28064,15 +28201,16 @@
         <v>-15</v>
       </c>
       <c r="U44" s="77">
-        <f t="shared" ref="U44" si="202">U21-T21</f>
+        <f t="shared" ref="U44" si="213">U21-T21</f>
         <v>-6</v>
       </c>
       <c r="V44" s="77">
-        <f t="shared" ref="V44" si="203">V21-U21</f>
+        <f t="shared" ref="V44" si="214">V21-U21</f>
         <v>-10</v>
       </c>
-      <c r="Y44" s="59" t="s">
-        <v>186</v>
+      <c r="W44" s="77">
+        <f t="shared" ref="W44" si="215">W21-V21</f>
+        <v>-10</v>
       </c>
       <c r="Z44" s="59" t="s">
         <v>186</v>
@@ -28095,81 +28233,84 @@
       <c r="AF44" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AG44" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="46" spans="1:32" ht="12.75" customHeight="1">
+    <row r="46" spans="1:33" ht="12.75" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B46" s="24">
-        <f t="shared" ref="B46:S46" si="204">B12/B3</f>
+        <f t="shared" ref="B46:S46" si="216">B12/B3</f>
         <v>0.77057220708446872</v>
       </c>
       <c r="C46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.80022197558268593</v>
       </c>
       <c r="D46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.85304449648711944</v>
       </c>
       <c r="E46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.80193756727664156</v>
       </c>
       <c r="F46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.80698924731182797</v>
       </c>
       <c r="G46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.80793650793650795</v>
       </c>
       <c r="H46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.81736368448914765</v>
       </c>
       <c r="I46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.82368283776734486</v>
       </c>
       <c r="J46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.83280757097791802</v>
       </c>
       <c r="K46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.83491062039957942</v>
       </c>
       <c r="L46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.83859095688748686</v>
       </c>
       <c r="M46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.85241596638655459</v>
       </c>
       <c r="N46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="O46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.84323770491803274</v>
       </c>
       <c r="P46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.84095528455284552</v>
       </c>
       <c r="Q46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.83717434869739482</v>
       </c>
       <c r="R46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.8418674698795181</v>
       </c>
       <c r="S46" s="24">
-        <f t="shared" si="204"/>
+        <f t="shared" si="216"/>
         <v>0.84399999999999997</v>
       </c>
       <c r="T46" s="24">
@@ -28177,47 +28318,51 @@
         <v>0.85112781954887218</v>
       </c>
       <c r="U46" s="24">
-        <f t="shared" ref="U46:V46" si="205">U12/U3</f>
+        <f t="shared" ref="U46:W46" si="217">U12/U3</f>
         <v>0.85586924219910843</v>
       </c>
       <c r="V46" s="24">
-        <f t="shared" si="205"/>
+        <f t="shared" si="217"/>
         <v>0.86061507936507942</v>
       </c>
-      <c r="Y46" s="24">
-        <f t="shared" ref="Y46:AF46" si="206">Y12/Y3</f>
+      <c r="W46" s="24">
+        <f t="shared" si="217"/>
+        <v>0.86604053386060309</v>
+      </c>
+      <c r="Z46" s="24">
+        <f t="shared" ref="Z46:AG46" si="218">Z12/Z3</f>
         <v>0.70367979341510656</v>
       </c>
-      <c r="Z46" s="24">
-        <f t="shared" si="206"/>
+      <c r="AA46" s="24">
+        <f t="shared" si="218"/>
         <v>0.693075117370892</v>
       </c>
-      <c r="AA46" s="24">
-        <f t="shared" si="206"/>
+      <c r="AB46" s="24">
+        <f t="shared" si="218"/>
         <v>0.74271012006861059</v>
       </c>
-      <c r="AB46" s="24">
-        <f t="shared" si="206"/>
+      <c r="AC46" s="24">
+        <f t="shared" si="218"/>
         <v>0.76294277929155319</v>
       </c>
-      <c r="AC46" s="24">
-        <f t="shared" si="206"/>
+      <c r="AD46" s="24">
+        <f t="shared" si="218"/>
         <v>0.80193756727664156</v>
       </c>
-      <c r="AD46" s="24">
-        <f t="shared" si="206"/>
+      <c r="AE46" s="24">
+        <f t="shared" si="218"/>
         <v>0.82368283776734486</v>
       </c>
-      <c r="AE46" s="24">
-        <f t="shared" si="206"/>
+      <c r="AF46" s="24">
+        <f t="shared" si="218"/>
         <v>0.85241596638655459</v>
       </c>
-      <c r="AF46" s="24">
-        <f t="shared" si="206"/>
+      <c r="AG46" s="24">
+        <f t="shared" si="218"/>
         <v>0.83717434869739482</v>
       </c>
     </row>
-    <row r="47" spans="1:32" ht="12.75" customHeight="1">
+    <row r="47" spans="1:33" ht="12.75" customHeight="1">
       <c r="N47" s="72"/>
     </row>
     <row r="49" spans="14:14" ht="12.75" customHeight="1">
@@ -28231,15 +28376,15 @@
     <hyperlink ref="N1" r:id="rId4" xr:uid="{9287A329-D88E-784B-8BDF-1EDA927EB785}"/>
     <hyperlink ref="S1" r:id="rId5" xr:uid="{6AF4C14B-B6A4-FE47-B0D3-A570A390AD5C}"/>
     <hyperlink ref="O1" r:id="rId6" xr:uid="{0A17F8BF-EADB-DE42-994D-117A4F2CB3FE}"/>
-    <hyperlink ref="AF1" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
+    <hyperlink ref="AG1" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
     <hyperlink ref="M1" r:id="rId8" xr:uid="{F1748A46-ECC6-544E-9D30-C00CF38C6CF7}"/>
-    <hyperlink ref="AE1" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
-    <hyperlink ref="AD1" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
+    <hyperlink ref="AF1" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
+    <hyperlink ref="AE1" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
     <hyperlink ref="I1" r:id="rId11" xr:uid="{998E2907-64B9-7A44-8D65-8083912D2D62}"/>
     <hyperlink ref="E1" r:id="rId12" xr:uid="{5D689E99-05ED-E34E-9D87-28B9F22988C9}"/>
-    <hyperlink ref="AC1" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
-    <hyperlink ref="AB1" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
-    <hyperlink ref="AA1" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
+    <hyperlink ref="AD1" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
+    <hyperlink ref="AC1" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
+    <hyperlink ref="AB1" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
     <hyperlink ref="L1" r:id="rId16" xr:uid="{E0D344DF-ECD3-4969-946B-75165895949D}"/>
     <hyperlink ref="K1" r:id="rId17" xr:uid="{34FDBE06-551B-4817-B842-42B3C369DE44}"/>
     <hyperlink ref="J1" r:id="rId18" xr:uid="{8672DEA7-6978-4CBC-A339-3D96580B25F6}"/>
@@ -28249,14 +28394,15 @@
     <hyperlink ref="D1" r:id="rId22" xr:uid="{9AA615B1-70E4-40CE-8BD9-FA369F45AAE7}"/>
     <hyperlink ref="C1" r:id="rId23" xr:uid="{B190BD40-76B4-4C45-B1D6-B5043307E3B6}"/>
     <hyperlink ref="B1" r:id="rId24" xr:uid="{2E883042-0703-4781-AC08-6A8AD2EAD4EB}"/>
-    <hyperlink ref="Z1" r:id="rId25" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/93a33ec4-dc07-47b3-91c2-d84b2e56d699?origin=1" xr:uid="{CE32064C-B077-40F4-9C44-3F45FE0A2ECE}"/>
-    <hyperlink ref="Y1" r:id="rId26" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a574642d-6cd1-4e80-a242-26ff2d0747f5?origin=1" xr:uid="{4A9206DD-D830-44D0-A5B0-DF41E9DD8391}"/>
+    <hyperlink ref="AA1" r:id="rId25" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/93a33ec4-dc07-47b3-91c2-d84b2e56d699?origin=1" xr:uid="{CE32064C-B077-40F4-9C44-3F45FE0A2ECE}"/>
+    <hyperlink ref="Z1" r:id="rId26" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a574642d-6cd1-4e80-a242-26ff2d0747f5?origin=1" xr:uid="{4A9206DD-D830-44D0-A5B0-DF41E9DD8391}"/>
     <hyperlink ref="T1" r:id="rId27" xr:uid="{F6F821CD-3C9C-4984-B9E1-54EA40AA851B}"/>
     <hyperlink ref="U1" r:id="rId28" xr:uid="{8A371147-4AFA-4AEF-811C-DCBC2CB2AA7E}"/>
     <hyperlink ref="V1" r:id="rId29" xr:uid="{1B3B2092-CF63-4E8C-950C-B7238A4569EE}"/>
+    <hyperlink ref="W1" r:id="rId30" xr:uid="{B722A3C9-0371-455C-8877-C5E990ECEA22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId30"/>
-  <drawing r:id="rId31"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId31"/>
+  <drawing r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$ERJ Austrian Air Force C-390 deal
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5338A009-4B65-4A89-AE50-31A3D795DDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EED2CD-DDF6-42EA-A29D-E1E04BCB2667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="273">
   <si>
     <t>$ERJ</t>
   </si>
@@ -990,6 +990,9 @@
   <si>
     <t>Embraer launch A-29N Super Tucano in NATO configuration to meet needs of European nations</t>
   </si>
+  <si>
+    <t>Austiran Air Force to replace aging C-130 with 4 KC-390 Millenium through a deal involving the Netherlands</t>
+  </si>
 </sst>
 </file>
 
@@ -1495,16 +1498,22 @@
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1514,24 +1523,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1561,16 +1552,28 @@
     <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9226,10 +9229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC63"/>
+  <dimension ref="A2:AC65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9249,49 +9252,49 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
-      <c r="G5" s="105" t="s">
+      <c r="C5" s="108"/>
+      <c r="D5" s="109"/>
+      <c r="G5" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="T5" s="105" t="s">
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="109"/>
+      <c r="T5" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="107"/>
-      <c r="AA5" s="103" t="s">
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="109"/>
+      <c r="AA5" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="104"/>
+      <c r="AB5" s="122"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>14.59</v>
+        <v>14.93</v>
       </c>
       <c r="D6" s="17"/>
       <c r="G6" s="8">
-        <v>45017</v>
+        <v>45170</v>
       </c>
       <c r="H6" s="94" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
@@ -9353,14 +9356,14 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>10717.814</v>
+        <v>10967.578</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
         <v>45017</v>
       </c>
-      <c r="H8" s="100" t="s">
-        <v>268</v>
+      <c r="H8" s="94" t="s">
+        <v>271</v>
       </c>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
@@ -9425,10 +9428,10 @@
         <v>Q223</v>
       </c>
       <c r="G10" s="8">
-        <v>44927</v>
-      </c>
-      <c r="H10" s="96" t="s">
-        <v>265</v>
+        <v>45017</v>
+      </c>
+      <c r="H10" s="100" t="s">
+        <v>268</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -9484,14 +9487,14 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>12005.714</v>
+        <v>12255.477999999999</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
-        <v>44896</v>
-      </c>
-      <c r="H12" s="94" t="s">
-        <v>263</v>
+        <v>44927</v>
+      </c>
+      <c r="H12" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -9507,13 +9510,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="105" t="s">
+      <c r="Y12" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="107"/>
+      <c r="Z12" s="108"/>
+      <c r="AA12" s="108"/>
+      <c r="AB12" s="108"/>
+      <c r="AC12" s="109"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -9535,21 +9538,21 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="112" t="s">
+      <c r="Z13" s="119" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="112"/>
-      <c r="AB13" s="112" t="s">
+      <c r="AA13" s="119"/>
+      <c r="AB13" s="119" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="113"/>
+      <c r="AC13" s="120"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
-        <v>44866</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>261</v>
+        <v>44896</v>
+      </c>
+      <c r="H14" s="94" t="s">
+        <v>263</v>
       </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
@@ -9570,21 +9573,21 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="101" t="s">
+      <c r="Z14" s="105" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="101"/>
-      <c r="AB14" s="101" t="s">
+      <c r="AA14" s="105"/>
+      <c r="AB14" s="105" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="102"/>
+      <c r="AC14" s="106"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="107"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -9606,14 +9609,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="101" t="s">
+      <c r="Z15" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="101"/>
-      <c r="AB15" s="101" t="s">
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="105" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="102"/>
+      <c r="AC15" s="106"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9622,15 +9625,15 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="101" t="s">
+      <c r="C16" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="102"/>
+      <c r="D16" s="106"/>
       <c r="G16" s="8">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
@@ -9651,23 +9654,23 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="101" t="s">
+      <c r="Z16" s="105" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="101"/>
-      <c r="AB16" s="101" t="s">
+      <c r="AA16" s="105"/>
+      <c r="AB16" s="105" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="102"/>
+      <c r="AC16" s="106"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="102"/>
+      <c r="D17" s="106"/>
       <c r="G17" s="9"/>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
@@ -9687,21 +9690,25 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="101" t="s">
+      <c r="Z17" s="105" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="101"/>
-      <c r="AB17" s="101" t="s">
+      <c r="AA17" s="105"/>
+      <c r="AB17" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="102"/>
+      <c r="AC17" s="106"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
+      <c r="G18" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
@@ -9721,25 +9728,21 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="101" t="s">
+      <c r="Z18" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="101"/>
-      <c r="AB18" s="101" t="s">
+      <c r="AA18" s="105"/>
+      <c r="AB18" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="102"/>
+      <c r="AC18" s="106"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
-      <c r="G19" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="C19" s="125"/>
+      <c r="D19" s="126"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
@@ -9759,20 +9762,18 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="101" t="s">
+      <c r="Z19" s="105" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="101"/>
-      <c r="AB19" s="101" t="s">
+      <c r="AA19" s="105"/>
+      <c r="AB19" s="105" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="102"/>
+      <c r="AC19" s="106"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9"/>
-      <c r="H20" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="H20" s="34"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -9792,19 +9793,21 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="101" t="s">
+      <c r="Z20" s="105" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="101"/>
-      <c r="AB20" s="101" t="s">
+      <c r="AA20" s="105"/>
+      <c r="AB20" s="105" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="102"/>
+      <c r="AC20" s="106"/>
     </row>
     <row r="21" spans="2:29">
-      <c r="G21" s="9"/>
-      <c r="H21" s="7" t="s">
-        <v>13</v>
+      <c r="G21" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
@@ -9829,13 +9832,15 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="109"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="34"/>
+      <c r="H22" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
@@ -9862,15 +9867,13 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="102"/>
-      <c r="G23" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>29</v>
+      <c r="D23" s="106"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
@@ -9891,14 +9894,12 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="101">
+      <c r="C24" s="105">
         <v>1969</v>
       </c>
-      <c r="D24" s="102"/>
+      <c r="D24" s="106"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="H24" s="34"/>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
       <c r="K24" s="34"/>
@@ -9918,10 +9919,14 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="102"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="34"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="106"/>
+      <c r="G25" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
@@ -9943,13 +9948,15 @@
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="108">
+      <c r="C26" s="123">
         <f>'Financial Model'!V68</f>
         <v>2329</v>
       </c>
-      <c r="D26" s="109"/>
+      <c r="D26" s="124"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="34"/>
+      <c r="H26" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
@@ -9969,14 +9976,10 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="102"/>
-      <c r="G27" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>187</v>
-      </c>
+      <c r="C27" s="105"/>
+      <c r="D27" s="106"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
@@ -9998,8 +10001,8 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="102"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="106"/>
       <c r="G28" s="9"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
@@ -10023,13 +10026,17 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="120">
+      <c r="C29" s="116">
         <f>'Order &amp; Backlog'!W21</f>
         <v>271</v>
       </c>
-      <c r="D29" s="102"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="34"/>
+      <c r="D29" s="106"/>
+      <c r="G29" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="I29" s="34"/>
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
@@ -10051,17 +10058,13 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="101">
+      <c r="C30" s="105">
         <f>'Financial Model'!X43</f>
         <v>47</v>
       </c>
-      <c r="D30" s="102"/>
-      <c r="G30" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="D30" s="106"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
@@ -10081,14 +10084,12 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="121">
+      <c r="C31" s="117">
         <v>36708</v>
       </c>
-      <c r="D31" s="122"/>
+      <c r="D31" s="118"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
@@ -10108,11 +10109,13 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="102"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="7" t="s">
-        <v>193</v>
+      <c r="C32" s="105"/>
+      <c r="D32" s="106"/>
+      <c r="G32" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
@@ -10143,7 +10146,7 @@
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
@@ -10154,9 +10157,7 @@
       <c r="O33" s="34"/>
       <c r="P33" s="34"/>
       <c r="Q33" s="34"/>
-      <c r="R33" s="48" t="s">
-        <v>194</v>
-      </c>
+      <c r="R33" s="35"/>
       <c r="T33" s="39"/>
       <c r="U33" s="34"/>
       <c r="V33" s="34"/>
@@ -10166,12 +10167,14 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="116" t="s">
+      <c r="C34" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="117"/>
+      <c r="D34" s="113"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="34"/>
+      <c r="H34" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
       <c r="K34" s="34"/>
@@ -10189,7 +10192,9 @@
     </row>
     <row r="35" spans="2:23">
       <c r="G35" s="9"/>
-      <c r="H35" s="34"/>
+      <c r="H35" s="7" t="s">
+        <v>191</v>
+      </c>
       <c r="I35" s="34"/>
       <c r="J35" s="34"/>
       <c r="K35" s="34"/>
@@ -10199,15 +10204,13 @@
       <c r="O35" s="34"/>
       <c r="P35" s="34"/>
       <c r="Q35" s="34"/>
-      <c r="R35" s="35"/>
+      <c r="R35" s="48" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="36" spans="2:23">
-      <c r="G36" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>196</v>
-      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="34"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
@@ -10220,15 +10223,13 @@
       <c r="R36" s="35"/>
     </row>
     <row r="37" spans="2:23">
-      <c r="B37" s="105" t="s">
+      <c r="B37" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107"/>
+      <c r="C37" s="108"/>
+      <c r="D37" s="109"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="H37" s="34"/>
       <c r="I37" s="34"/>
       <c r="J37" s="34"/>
       <c r="K37" s="34"/>
@@ -10239,25 +10240,27 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="105" t="s">
+      <c r="T37" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="107"/>
+      <c r="U37" s="108"/>
+      <c r="V37" s="108"/>
+      <c r="W37" s="109"/>
     </row>
     <row r="38" spans="2:23">
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="118">
+      <c r="C38" s="114">
         <f>C6/'Financial Model'!X123</f>
-        <v>3.8874914762422921</v>
-      </c>
-      <c r="D38" s="119"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="47" t="s">
-        <v>198</v>
+        <v>3.9780841494377945</v>
+      </c>
+      <c r="D38" s="115"/>
+      <c r="G38" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -10280,13 +10283,15 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="118">
+      <c r="C39" s="114">
         <f>C8/SUM('Financial Model'!U9:X9)</f>
-        <v>2.1741751866277186</v>
-      </c>
-      <c r="D39" s="119"/>
+        <v>2.2248413664394677</v>
+      </c>
+      <c r="D39" s="115"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="34"/>
+      <c r="H39" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="I39" s="34"/>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -10308,16 +10313,14 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="114">
+      <c r="C40" s="110">
         <f>C6/SUM('Financial Model'!U26:X26)</f>
-        <v>-110.60339791771077</v>
-      </c>
-      <c r="D40" s="115"/>
-      <c r="G40" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>239</v>
+        <v>-113.18085886987126</v>
+      </c>
+      <c r="D40" s="111"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="47" t="s">
+        <v>198</v>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
@@ -10338,9 +10341,7 @@
     </row>
     <row r="41" spans="2:23">
       <c r="G41" s="9"/>
-      <c r="H41" s="7" t="s">
-        <v>240</v>
-      </c>
+      <c r="H41" s="34"/>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
@@ -10357,8 +10358,12 @@
       <c r="W41" s="35"/>
     </row>
     <row r="42" spans="2:23">
-      <c r="G42" s="9"/>
-      <c r="H42" s="34"/>
+      <c r="G42" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>239</v>
+      </c>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
       <c r="K42" s="34"/>
@@ -10377,16 +10382,14 @@
       <c r="W42" s="35"/>
     </row>
     <row r="43" spans="2:23">
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="107" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="106"/>
-      <c r="D43" s="107"/>
-      <c r="G43" s="8">
-        <v>44682</v>
-      </c>
-      <c r="H43" s="34" t="s">
-        <v>248</v>
+      <c r="C43" s="108"/>
+      <c r="D43" s="109"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
@@ -10406,17 +10409,15 @@
       <c r="W43" s="35"/>
     </row>
     <row r="44" spans="2:23">
-      <c r="B44" s="123" t="s">
+      <c r="B44" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="124"/>
+      <c r="C44" s="102"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
       <c r="G44" s="9"/>
-      <c r="H44" s="7" t="s">
-        <v>249</v>
-      </c>
+      <c r="H44" s="34"/>
       <c r="I44" s="34"/>
       <c r="J44" s="34"/>
       <c r="K44" s="34"/>
@@ -10426,9 +10427,7 @@
       <c r="O44" s="34"/>
       <c r="P44" s="34"/>
       <c r="Q44" s="34"/>
-      <c r="R44" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R44" s="35"/>
       <c r="T44" s="95" t="s">
         <v>264</v>
       </c>
@@ -10439,15 +10438,19 @@
       </c>
     </row>
     <row r="45" spans="2:23">
-      <c r="B45" s="123" t="s">
+      <c r="B45" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="124"/>
+      <c r="C45" s="102"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="34"/>
+      <c r="G45" s="8">
+        <v>44682</v>
+      </c>
+      <c r="H45" s="34" t="s">
+        <v>248</v>
+      </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
       <c r="K45" s="34"/>
@@ -10460,16 +10463,14 @@
       <c r="R45" s="35"/>
     </row>
     <row r="46" spans="2:23">
-      <c r="B46" s="123"/>
-      <c r="C46" s="124"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="102"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="8">
-        <v>43922</v>
-      </c>
-      <c r="H46" s="34" t="s">
-        <v>164</v>
+      <c r="G46" s="9"/>
+      <c r="H46" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
@@ -10480,18 +10481,18 @@
       <c r="O46" s="34"/>
       <c r="P46" s="34"/>
       <c r="Q46" s="34"/>
-      <c r="R46" s="35"/>
+      <c r="R46" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="47" spans="2:23">
-      <c r="B47" s="123"/>
-      <c r="C47" s="124"/>
+      <c r="B47" s="101"/>
+      <c r="C47" s="102"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
       <c r="G47" s="9"/>
-      <c r="H47" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="H47" s="34"/>
       <c r="I47" s="34"/>
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
@@ -10504,13 +10505,17 @@
       <c r="R47" s="35"/>
     </row>
     <row r="48" spans="2:23">
-      <c r="B48" s="125"/>
-      <c r="C48" s="126"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="104"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="34"/>
+      <c r="G48" s="8">
+        <v>43922</v>
+      </c>
+      <c r="H48" s="34" t="s">
+        <v>164</v>
+      </c>
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
@@ -10520,13 +10525,13 @@
       <c r="O48" s="34"/>
       <c r="P48" s="34"/>
       <c r="Q48" s="34"/>
-      <c r="R48" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R48" s="35"/>
     </row>
     <row r="49" spans="7:18">
       <c r="G49" s="9"/>
-      <c r="H49" s="34"/>
+      <c r="H49" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
@@ -10539,12 +10544,8 @@
       <c r="R49" s="35"/>
     </row>
     <row r="50" spans="7:18">
-      <c r="G50" s="8">
-        <v>43770</v>
-      </c>
-      <c r="H50" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="34"/>
       <c r="I50" s="34"/>
       <c r="J50" s="34"/>
       <c r="K50" s="34"/>
@@ -10554,13 +10555,13 @@
       <c r="O50" s="34"/>
       <c r="P50" s="34"/>
       <c r="Q50" s="34"/>
-      <c r="R50" s="35"/>
+      <c r="R50" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="51" spans="7:18">
       <c r="G51" s="9"/>
-      <c r="H51" s="47" t="s">
-        <v>168</v>
-      </c>
+      <c r="H51" s="34"/>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
@@ -10573,8 +10574,12 @@
       <c r="R51" s="35"/>
     </row>
     <row r="52" spans="7:18">
-      <c r="G52" s="9"/>
-      <c r="H52" s="34"/>
+      <c r="G52" s="8">
+        <v>43770</v>
+      </c>
+      <c r="H52" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
       <c r="K52" s="34"/>
@@ -10587,11 +10592,9 @@
       <c r="R52" s="35"/>
     </row>
     <row r="53" spans="7:18">
-      <c r="G53" s="8">
-        <v>43739</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>244</v>
+      <c r="G53" s="9"/>
+      <c r="H53" s="47" t="s">
+        <v>168</v>
       </c>
       <c r="I53" s="34"/>
       <c r="J53" s="34"/>
@@ -10601,9 +10604,7 @@
       <c r="N53" s="34"/>
       <c r="O53" s="34"/>
       <c r="P53" s="34"/>
-      <c r="Q53" s="34" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q53" s="34"/>
       <c r="R53" s="35"/>
     </row>
     <row r="54" spans="7:18">
@@ -10621,8 +10622,12 @@
       <c r="R54" s="35"/>
     </row>
     <row r="55" spans="7:18">
-      <c r="G55" s="9"/>
-      <c r="H55" s="34"/>
+      <c r="G55" s="8">
+        <v>43739</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>244</v>
+      </c>
       <c r="I55" s="34"/>
       <c r="J55" s="34"/>
       <c r="K55" s="34"/>
@@ -10631,7 +10636,9 @@
       <c r="N55" s="34"/>
       <c r="O55" s="34"/>
       <c r="P55" s="34"/>
-      <c r="Q55" s="34"/>
+      <c r="Q55" s="34" t="s">
+        <v>179</v>
+      </c>
       <c r="R55" s="35"/>
     </row>
     <row r="56" spans="7:18">
@@ -10649,12 +10656,8 @@
       <c r="R56" s="35"/>
     </row>
     <row r="57" spans="7:18">
-      <c r="G57" s="8">
-        <v>43586</v>
-      </c>
-      <c r="H57" s="34" t="s">
-        <v>166</v>
-      </c>
+      <c r="G57" s="9"/>
+      <c r="H57" s="34"/>
       <c r="I57" s="34"/>
       <c r="J57" s="34"/>
       <c r="K57" s="34"/>
@@ -10682,10 +10685,10 @@
     </row>
     <row r="59" spans="7:18">
       <c r="G59" s="8">
-        <v>43282</v>
+        <v>43586</v>
       </c>
       <c r="H59" s="34" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I59" s="34"/>
       <c r="J59" s="34"/>
@@ -10700,9 +10703,7 @@
     </row>
     <row r="60" spans="7:18">
       <c r="G60" s="9"/>
-      <c r="H60" s="7" t="s">
-        <v>163</v>
-      </c>
+      <c r="H60" s="34"/>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
       <c r="K60" s="34"/>
@@ -10715,9 +10716,11 @@
       <c r="R60" s="35"/>
     </row>
     <row r="61" spans="7:18">
-      <c r="G61" s="9"/>
-      <c r="H61" s="7" t="s">
-        <v>165</v>
+      <c r="G61" s="8">
+        <v>43282</v>
+      </c>
+      <c r="H61" s="34" t="s">
+        <v>162</v>
       </c>
       <c r="I61" s="34"/>
       <c r="J61" s="34"/>
@@ -10732,7 +10735,9 @@
     </row>
     <row r="62" spans="7:18">
       <c r="G62" s="9"/>
-      <c r="H62" s="34"/>
+      <c r="H62" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
       <c r="K62" s="34"/>
@@ -10745,30 +10750,83 @@
       <c r="R62" s="35"/>
     </row>
     <row r="63" spans="7:18">
-      <c r="G63" s="87">
+      <c r="G63" s="9"/>
+      <c r="H63" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I63" s="34"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="34"/>
+      <c r="L63" s="34"/>
+      <c r="M63" s="34"/>
+      <c r="N63" s="34"/>
+      <c r="O63" s="34"/>
+      <c r="P63" s="34"/>
+      <c r="Q63" s="34"/>
+      <c r="R63" s="35"/>
+    </row>
+    <row r="64" spans="7:18">
+      <c r="G64" s="9"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="34"/>
+      <c r="L64" s="34"/>
+      <c r="M64" s="34"/>
+      <c r="N64" s="34"/>
+      <c r="O64" s="34"/>
+      <c r="P64" s="34"/>
+      <c r="Q64" s="34"/>
+      <c r="R64" s="35"/>
+    </row>
+    <row r="65" spans="7:18">
+      <c r="G65" s="87">
         <v>42552</v>
       </c>
-      <c r="H63" s="51" t="s">
+      <c r="H65" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="I63" s="32"/>
-      <c r="J63" s="32"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="32"/>
-      <c r="N63" s="32"/>
-      <c r="O63" s="32"/>
-      <c r="P63" s="32"/>
-      <c r="Q63" s="32"/>
-      <c r="R63" s="33"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="32"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="32"/>
+      <c r="N65" s="32"/>
+      <c r="O65" s="32"/>
+      <c r="P65" s="32"/>
+      <c r="Q65" s="32"/>
+      <c r="R65" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
     <mergeCell ref="Z19:AA19"/>
     <mergeCell ref="AB19:AC19"/>
     <mergeCell ref="Z20:AA20"/>
@@ -10785,62 +10843,40 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H19" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H23" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="H21" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H25" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C34:D34" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R48" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H27" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H30" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R33" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H36" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="R50" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H29" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H32" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R35" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H38" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
     <hyperlink ref="W44" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
     <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
     <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
-    <hyperlink ref="H40" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H53" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="H42" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H55" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
     <hyperlink ref="D45" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D44" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
-    <hyperlink ref="R44" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H16" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
-    <hyperlink ref="H14" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
-    <hyperlink ref="H12" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
-    <hyperlink ref="H10" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
-    <hyperlink ref="H8" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
-    <hyperlink ref="H6" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="R46" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H16" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
+    <hyperlink ref="H14" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
+    <hyperlink ref="H12" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
+    <hyperlink ref="H10" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
+    <hyperlink ref="H8" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="H6" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId23"/>
-  <drawing r:id="rId24"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId24"/>
+  <drawing r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -10848,7 +10884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
   <dimension ref="B1:AR148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
$ERJ KC-390 potential buyers
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99319F1E-8883-48EC-9798-8ECD338E047C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7EA123-54C1-4684-B1D4-5A94099DB8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="297">
   <si>
     <t>$ERJ</t>
   </si>
@@ -993,6 +993,78 @@
   <si>
     <t>Austiran Air Force to replace aging C-130 with 4 KC-390 Millenium through a deal involving the Netherlands</t>
   </si>
+  <si>
+    <t>South Africa - 6 Aircraft</t>
+  </si>
+  <si>
+    <t>SAAF facing financial crisis which has grounded jets</t>
+  </si>
+  <si>
+    <t>Outdated C-130B but plans to rennovate</t>
+  </si>
+  <si>
+    <t>Angola - 4 Aircraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required to replace aging Soviet era a/c </t>
+  </si>
+  <si>
+    <t>South Korea - 12 Aircraft</t>
+  </si>
+  <si>
+    <t>Has plans to create an A/C slightly larger than KC-390</t>
+  </si>
+  <si>
+    <t>Embraer has announced partnership with SK firms</t>
+  </si>
+  <si>
+    <t>Egypt - 12 Aircraft</t>
+  </si>
+  <si>
+    <t>Has orders for 24 C-130H turboprops</t>
+  </si>
+  <si>
+    <t>Greece - 6 Aircraft</t>
+  </si>
+  <si>
+    <t>Greek Government in talks with Embraer</t>
+  </si>
+  <si>
+    <t>India - Up to 80 Aircraft</t>
+  </si>
+  <si>
+    <t>Plans for a purchase of up to 80 airframes</t>
+  </si>
+  <si>
+    <t>Stipulation of Indian based production &amp; tech</t>
+  </si>
+  <si>
+    <t>Czech Republic - 2 Aircraft</t>
+  </si>
+  <si>
+    <t>KC-390 Potential Buyers</t>
+  </si>
+  <si>
+    <t>Selected by Air Force commander as best choice</t>
+  </si>
+  <si>
+    <t>Rwanda - 2 Aircraft</t>
+  </si>
+  <si>
+    <t>Highlighted by Rwandan govt. as possible purchase</t>
+  </si>
+  <si>
+    <t>Sweden - 6 Aircraft</t>
+  </si>
+  <si>
+    <t>Brazilian defence minister travelling in October to</t>
+  </si>
+  <si>
+    <t>negotiate an agreement in exchange for Grippens</t>
+  </si>
+  <si>
+    <t>Potential for 490 orders as aging C130 retires</t>
+  </si>
 </sst>
 </file>
 
@@ -1005,7 +1077,7 @@
     <numFmt numFmtId="167" formatCode="0.0000\x"/>
     <numFmt numFmtId="168" formatCode="mmmm\ yyyy;"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1162,8 +1234,28 @@
       <color theme="10"/>
       <name val="Airal"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1191,6 +1283,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF323232"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1288,7 +1386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1498,16 +1596,22 @@
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1517,24 +1621,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1564,16 +1650,56 @@
     <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9231,8 +9357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="AD50" sqref="AD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9252,35 +9378,35 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
-      <c r="G5" s="105" t="s">
+      <c r="C5" s="108"/>
+      <c r="D5" s="109"/>
+      <c r="G5" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="T5" s="105" t="s">
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="109"/>
+      <c r="T5" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="107"/>
-      <c r="AA5" s="103" t="s">
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="109"/>
+      <c r="AA5" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="104"/>
+      <c r="AB5" s="122"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -9510,13 +9636,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="105" t="s">
+      <c r="Y12" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="107"/>
+      <c r="Z12" s="108"/>
+      <c r="AA12" s="108"/>
+      <c r="AB12" s="108"/>
+      <c r="AC12" s="109"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -9538,14 +9664,14 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="112" t="s">
+      <c r="Z13" s="119" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="112"/>
-      <c r="AB13" s="112" t="s">
+      <c r="AA13" s="119"/>
+      <c r="AB13" s="119" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="113"/>
+      <c r="AC13" s="120"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
@@ -9573,21 +9699,21 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="101" t="s">
+      <c r="Z14" s="105" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="101"/>
-      <c r="AB14" s="101" t="s">
+      <c r="AA14" s="105"/>
+      <c r="AB14" s="105" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="102"/>
+      <c r="AC14" s="106"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="107"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -9609,14 +9735,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="101" t="s">
+      <c r="Z15" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="101"/>
-      <c r="AB15" s="101" t="s">
+      <c r="AA15" s="105"/>
+      <c r="AB15" s="105" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="102"/>
+      <c r="AC15" s="106"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9625,10 +9751,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="101" t="s">
+      <c r="C16" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="102"/>
+      <c r="D16" s="106"/>
       <c r="G16" s="8">
         <v>44866</v>
       </c>
@@ -9654,23 +9780,23 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="101" t="s">
+      <c r="Z16" s="105" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="101"/>
-      <c r="AB16" s="101" t="s">
+      <c r="AA16" s="105"/>
+      <c r="AB16" s="105" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="102"/>
+      <c r="AC16" s="106"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="102"/>
+      <c r="D17" s="106"/>
       <c r="G17" s="9"/>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
@@ -9690,19 +9816,19 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="101" t="s">
+      <c r="Z17" s="105" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="101"/>
-      <c r="AB17" s="101" t="s">
+      <c r="AA17" s="105"/>
+      <c r="AB17" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="102"/>
+      <c r="AC17" s="106"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
       <c r="G18" s="8">
         <v>44835</v>
       </c>
@@ -9728,19 +9854,19 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="101" t="s">
+      <c r="Z18" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="101"/>
-      <c r="AB18" s="101" t="s">
+      <c r="AA18" s="105"/>
+      <c r="AB18" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="102"/>
+      <c r="AC18" s="106"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="126"/>
       <c r="G19" s="9"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -9762,14 +9888,14 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="101" t="s">
+      <c r="Z19" s="105" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="101"/>
-      <c r="AB19" s="101" t="s">
+      <c r="AA19" s="105"/>
+      <c r="AB19" s="105" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="102"/>
+      <c r="AC19" s="106"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9"/>
@@ -9793,14 +9919,14 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="101" t="s">
+      <c r="Z20" s="105" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="101"/>
-      <c r="AB20" s="101" t="s">
+      <c r="AA20" s="105"/>
+      <c r="AB20" s="105" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="102"/>
+      <c r="AC20" s="106"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="8">
@@ -9832,11 +9958,11 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="109"/>
       <c r="G22" s="9"/>
       <c r="H22" s="7" t="s">
         <v>12</v>
@@ -9867,10 +9993,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="102"/>
+      <c r="D23" s="106"/>
       <c r="G23" s="9"/>
       <c r="H23" s="7" t="s">
         <v>13</v>
@@ -9894,10 +10020,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="101">
+      <c r="C24" s="105">
         <v>1969</v>
       </c>
-      <c r="D24" s="102"/>
+      <c r="D24" s="106"/>
       <c r="G24" s="9"/>
       <c r="H24" s="34"/>
       <c r="I24" s="34"/>
@@ -9919,8 +10045,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="102"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="106"/>
       <c r="G25" s="8">
         <v>44835</v>
       </c>
@@ -9943,16 +10069,23 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
+      <c r="Y25" s="130" t="s">
+        <v>289</v>
+      </c>
+      <c r="Z25" s="131"/>
+      <c r="AA25" s="131"/>
+      <c r="AB25" s="131"/>
+      <c r="AC25" s="132"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="108">
+      <c r="C26" s="123">
         <f>'Financial Model'!V68</f>
         <v>2329</v>
       </c>
-      <c r="D26" s="109"/>
+      <c r="D26" s="124"/>
       <c r="G26" s="9"/>
       <c r="H26" s="7" t="s">
         <v>30</v>
@@ -9973,11 +10106,18 @@
       <c r="U26" s="34"/>
       <c r="V26" s="34"/>
       <c r="W26" s="35"/>
+      <c r="Y26" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z26" s="127"/>
+      <c r="AA26" s="127"/>
+      <c r="AB26" s="127"/>
+      <c r="AC26" s="35"/>
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="102"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="106"/>
       <c r="G27" s="9"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -9996,13 +10136,20 @@
       <c r="U27" s="34"/>
       <c r="V27" s="34"/>
       <c r="W27" s="35"/>
+      <c r="Y27" s="128" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z27" s="127"/>
+      <c r="AA27" s="127"/>
+      <c r="AB27" s="127"/>
+      <c r="AC27" s="35"/>
     </row>
     <row r="28" spans="2:29">
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="102"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="106"/>
       <c r="G28" s="9"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
@@ -10021,16 +10168,23 @@
       <c r="U28" s="34"/>
       <c r="V28" s="34"/>
       <c r="W28" s="35"/>
+      <c r="Y28" s="128" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z28" s="127"/>
+      <c r="AA28" s="127"/>
+      <c r="AB28" s="127"/>
+      <c r="AC28" s="35"/>
     </row>
     <row r="29" spans="2:29">
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="120">
+      <c r="C29" s="116">
         <f>'Order &amp; Backlog'!W21</f>
         <v>271</v>
       </c>
-      <c r="D29" s="102"/>
+      <c r="D29" s="106"/>
       <c r="G29" s="8">
         <v>44805</v>
       </c>
@@ -10053,16 +10207,21 @@
       <c r="U29" s="34"/>
       <c r="V29" s="34"/>
       <c r="W29" s="35"/>
+      <c r="Y29" s="39"/>
+      <c r="Z29" s="127"/>
+      <c r="AA29" s="127"/>
+      <c r="AB29" s="127"/>
+      <c r="AC29" s="35"/>
     </row>
     <row r="30" spans="2:29">
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="101">
+      <c r="C30" s="105">
         <f>'Financial Model'!X43</f>
         <v>47</v>
       </c>
-      <c r="D30" s="102"/>
+      <c r="D30" s="106"/>
       <c r="G30" s="9"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
@@ -10079,15 +10238,22 @@
       <c r="U30" s="34"/>
       <c r="V30" s="34"/>
       <c r="W30" s="35"/>
+      <c r="Y30" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z30" s="127"/>
+      <c r="AA30" s="127"/>
+      <c r="AB30" s="127"/>
+      <c r="AC30" s="35"/>
     </row>
     <row r="31" spans="2:29">
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="121">
+      <c r="C31" s="117">
         <v>36708</v>
       </c>
-      <c r="D31" s="122"/>
+      <c r="D31" s="118"/>
       <c r="G31" s="9"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -10106,11 +10272,18 @@
       <c r="U31" s="34"/>
       <c r="V31" s="34"/>
       <c r="W31" s="35"/>
+      <c r="Y31" s="129" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z31" s="127"/>
+      <c r="AA31" s="127"/>
+      <c r="AB31" s="127"/>
+      <c r="AC31" s="35"/>
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="102"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="106"/>
       <c r="G32" s="8">
         <v>44805</v>
       </c>
@@ -10133,8 +10306,13 @@
       <c r="U32" s="34"/>
       <c r="V32" s="34"/>
       <c r="W32" s="35"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="127"/>
+      <c r="AA32" s="127"/>
+      <c r="AB32" s="127"/>
+      <c r="AC32" s="35"/>
     </row>
-    <row r="33" spans="2:23">
+    <row r="33" spans="2:29">
       <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
@@ -10162,15 +10340,22 @@
       <c r="U33" s="34"/>
       <c r="V33" s="34"/>
       <c r="W33" s="35"/>
+      <c r="Y33" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z33" s="127"/>
+      <c r="AA33" s="127"/>
+      <c r="AB33" s="127"/>
+      <c r="AC33" s="35"/>
     </row>
-    <row r="34" spans="2:23">
+    <row r="34" spans="2:29">
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="116" t="s">
+      <c r="C34" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="117"/>
+      <c r="D34" s="113"/>
       <c r="G34" s="9"/>
       <c r="H34" s="7" t="s">
         <v>193</v>
@@ -10189,8 +10374,15 @@
       <c r="U34" s="32"/>
       <c r="V34" s="32"/>
       <c r="W34" s="33"/>
+      <c r="Y34" s="128" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z34" s="127"/>
+      <c r="AA34" s="127"/>
+      <c r="AB34" s="127"/>
+      <c r="AC34" s="35"/>
     </row>
-    <row r="35" spans="2:23">
+    <row r="35" spans="2:29">
       <c r="G35" s="9"/>
       <c r="H35" s="7" t="s">
         <v>191</v>
@@ -10207,8 +10399,15 @@
       <c r="R35" s="48" t="s">
         <v>194</v>
       </c>
+      <c r="Y35" s="129" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z35" s="127"/>
+      <c r="AA35" s="127"/>
+      <c r="AB35" s="127"/>
+      <c r="AC35" s="35"/>
     </row>
-    <row r="36" spans="2:23">
+    <row r="36" spans="2:29">
       <c r="G36" s="9"/>
       <c r="H36" s="34"/>
       <c r="I36" s="34"/>
@@ -10221,13 +10420,18 @@
       <c r="P36" s="34"/>
       <c r="Q36" s="34"/>
       <c r="R36" s="35"/>
+      <c r="Y36" s="39"/>
+      <c r="Z36" s="127"/>
+      <c r="AA36" s="127"/>
+      <c r="AB36" s="127"/>
+      <c r="AC36" s="35"/>
     </row>
-    <row r="37" spans="2:23">
-      <c r="B37" s="105" t="s">
+    <row r="37" spans="2:29">
+      <c r="B37" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107"/>
+      <c r="C37" s="108"/>
+      <c r="D37" s="109"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -10240,22 +10444,29 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="105" t="s">
+      <c r="T37" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="107"/>
+      <c r="U37" s="108"/>
+      <c r="V37" s="108"/>
+      <c r="W37" s="109"/>
+      <c r="Y37" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z37" s="127"/>
+      <c r="AA37" s="127"/>
+      <c r="AB37" s="127"/>
+      <c r="AC37" s="35"/>
     </row>
-    <row r="38" spans="2:23">
+    <row r="38" spans="2:29">
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="118">
+      <c r="C38" s="114">
         <f>C6/'Financial Model'!X123</f>
         <v>3.9780841494377945</v>
       </c>
-      <c r="D38" s="119"/>
+      <c r="D38" s="115"/>
       <c r="G38" s="8">
         <v>44743</v>
       </c>
@@ -10278,16 +10489,23 @@
       <c r="U38" s="34"/>
       <c r="V38" s="34"/>
       <c r="W38" s="35"/>
+      <c r="Y38" s="128" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z38" s="127"/>
+      <c r="AA38" s="127"/>
+      <c r="AB38" s="127"/>
+      <c r="AC38" s="35"/>
     </row>
-    <row r="39" spans="2:23">
+    <row r="39" spans="2:29">
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="118">
+      <c r="C39" s="114">
         <f>C8/SUM('Financial Model'!U9:X9)</f>
         <v>2.2248413664394677</v>
       </c>
-      <c r="D39" s="119"/>
+      <c r="D39" s="115"/>
       <c r="G39" s="9"/>
       <c r="H39" s="7" t="s">
         <v>197</v>
@@ -10308,16 +10526,21 @@
       <c r="U39" s="34"/>
       <c r="V39" s="34"/>
       <c r="W39" s="35"/>
+      <c r="Y39" s="39"/>
+      <c r="Z39" s="127"/>
+      <c r="AA39" s="127"/>
+      <c r="AB39" s="127"/>
+      <c r="AC39" s="35"/>
     </row>
-    <row r="40" spans="2:23">
+    <row r="40" spans="2:29">
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="114">
+      <c r="C40" s="110">
         <f>C6/SUM('Financial Model'!U26:X26)</f>
         <v>-113.18085886987126</v>
       </c>
-      <c r="D40" s="115"/>
+      <c r="D40" s="111"/>
       <c r="G40" s="9"/>
       <c r="H40" s="47" t="s">
         <v>198</v>
@@ -10338,8 +10561,15 @@
       <c r="U40" s="34"/>
       <c r="V40" s="34"/>
       <c r="W40" s="35"/>
+      <c r="Y40" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="Z40" s="127"/>
+      <c r="AA40" s="127"/>
+      <c r="AB40" s="127"/>
+      <c r="AC40" s="35"/>
     </row>
-    <row r="41" spans="2:23">
+    <row r="41" spans="2:29">
       <c r="G41" s="9"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -10356,8 +10586,15 @@
       <c r="U41" s="34"/>
       <c r="V41" s="34"/>
       <c r="W41" s="35"/>
+      <c r="Y41" s="129" t="s">
+        <v>284</v>
+      </c>
+      <c r="Z41" s="127"/>
+      <c r="AA41" s="127"/>
+      <c r="AB41" s="127"/>
+      <c r="AC41" s="35"/>
     </row>
-    <row r="42" spans="2:23">
+    <row r="42" spans="2:29">
       <c r="G42" s="8">
         <v>44743</v>
       </c>
@@ -10380,13 +10617,18 @@
       <c r="U42" s="34"/>
       <c r="V42" s="34"/>
       <c r="W42" s="35"/>
+      <c r="Y42" s="39"/>
+      <c r="Z42" s="127"/>
+      <c r="AA42" s="127"/>
+      <c r="AB42" s="127"/>
+      <c r="AC42" s="35"/>
     </row>
-    <row r="43" spans="2:23">
-      <c r="B43" s="105" t="s">
+    <row r="43" spans="2:29">
+      <c r="B43" s="107" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="106"/>
-      <c r="D43" s="107"/>
+      <c r="C43" s="108"/>
+      <c r="D43" s="109"/>
       <c r="G43" s="9"/>
       <c r="H43" s="7" t="s">
         <v>240</v>
@@ -10407,12 +10649,19 @@
       <c r="U43" s="34"/>
       <c r="V43" s="34"/>
       <c r="W43" s="35"/>
+      <c r="Y43" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z43" s="127"/>
+      <c r="AA43" s="127"/>
+      <c r="AB43" s="127"/>
+      <c r="AC43" s="35"/>
     </row>
-    <row r="44" spans="2:23">
-      <c r="B44" s="123" t="s">
+    <row r="44" spans="2:29">
+      <c r="B44" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="124"/>
+      <c r="C44" s="102"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
@@ -10436,12 +10685,19 @@
       <c r="W44" s="58" t="s">
         <v>31</v>
       </c>
+      <c r="Y44" s="129" t="s">
+        <v>286</v>
+      </c>
+      <c r="Z44" s="127"/>
+      <c r="AA44" s="127"/>
+      <c r="AB44" s="127"/>
+      <c r="AC44" s="35"/>
     </row>
-    <row r="45" spans="2:23">
-      <c r="B45" s="123" t="s">
+    <row r="45" spans="2:29">
+      <c r="B45" s="101" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="124"/>
+      <c r="C45" s="102"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
@@ -10461,10 +10717,17 @@
       <c r="P45" s="34"/>
       <c r="Q45" s="34"/>
       <c r="R45" s="35"/>
+      <c r="Y45" s="128" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z45" s="127"/>
+      <c r="AA45" s="127"/>
+      <c r="AB45" s="127"/>
+      <c r="AC45" s="35"/>
     </row>
-    <row r="46" spans="2:23">
-      <c r="B46" s="123"/>
-      <c r="C46" s="124"/>
+    <row r="46" spans="2:29">
+      <c r="B46" s="101"/>
+      <c r="C46" s="102"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
@@ -10484,10 +10747,15 @@
       <c r="R46" s="48" t="s">
         <v>31</v>
       </c>
+      <c r="Y46" s="39"/>
+      <c r="Z46" s="127"/>
+      <c r="AA46" s="127"/>
+      <c r="AB46" s="127"/>
+      <c r="AC46" s="35"/>
     </row>
-    <row r="47" spans="2:23">
-      <c r="B47" s="123"/>
-      <c r="C47" s="124"/>
+    <row r="47" spans="2:29">
+      <c r="B47" s="101"/>
+      <c r="C47" s="102"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
@@ -10503,10 +10771,17 @@
       <c r="P47" s="34"/>
       <c r="Q47" s="34"/>
       <c r="R47" s="35"/>
+      <c r="Y47" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="Z47" s="127"/>
+      <c r="AA47" s="127"/>
+      <c r="AB47" s="127"/>
+      <c r="AC47" s="35"/>
     </row>
-    <row r="48" spans="2:23">
-      <c r="B48" s="125"/>
-      <c r="C48" s="126"/>
+    <row r="48" spans="2:29">
+      <c r="B48" s="103"/>
+      <c r="C48" s="104"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
@@ -10526,8 +10801,15 @@
       <c r="P48" s="34"/>
       <c r="Q48" s="34"/>
       <c r="R48" s="35"/>
+      <c r="Y48" s="129" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z48" s="127"/>
+      <c r="AA48" s="127"/>
+      <c r="AB48" s="127"/>
+      <c r="AC48" s="35"/>
     </row>
-    <row r="49" spans="7:18">
+    <row r="49" spans="7:29">
       <c r="G49" s="9"/>
       <c r="H49" s="7" t="s">
         <v>169</v>
@@ -10542,8 +10824,13 @@
       <c r="P49" s="34"/>
       <c r="Q49" s="34"/>
       <c r="R49" s="35"/>
+      <c r="Y49" s="39"/>
+      <c r="Z49" s="127"/>
+      <c r="AA49" s="127"/>
+      <c r="AB49" s="127"/>
+      <c r="AC49" s="35"/>
     </row>
-    <row r="50" spans="7:18">
+    <row r="50" spans="7:29">
       <c r="G50" s="9"/>
       <c r="H50" s="34"/>
       <c r="I50" s="34"/>
@@ -10558,8 +10845,15 @@
       <c r="R50" s="48" t="s">
         <v>31</v>
       </c>
+      <c r="Y50" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="Z50" s="127"/>
+      <c r="AA50" s="127"/>
+      <c r="AB50" s="127"/>
+      <c r="AC50" s="35"/>
     </row>
-    <row r="51" spans="7:18">
+    <row r="51" spans="7:29">
       <c r="G51" s="9"/>
       <c r="H51" s="34"/>
       <c r="I51" s="34"/>
@@ -10572,8 +10866,15 @@
       <c r="P51" s="34"/>
       <c r="Q51" s="34"/>
       <c r="R51" s="35"/>
+      <c r="Y51" s="129" t="s">
+        <v>292</v>
+      </c>
+      <c r="Z51" s="127"/>
+      <c r="AA51" s="127"/>
+      <c r="AB51" s="127"/>
+      <c r="AC51" s="35"/>
     </row>
-    <row r="52" spans="7:18">
+    <row r="52" spans="7:29">
       <c r="G52" s="8">
         <v>43770</v>
       </c>
@@ -10590,8 +10891,13 @@
       <c r="P52" s="34"/>
       <c r="Q52" s="34"/>
       <c r="R52" s="35"/>
+      <c r="Y52" s="39"/>
+      <c r="Z52" s="127"/>
+      <c r="AA52" s="127"/>
+      <c r="AB52" s="127"/>
+      <c r="AC52" s="35"/>
     </row>
-    <row r="53" spans="7:18">
+    <row r="53" spans="7:29">
       <c r="G53" s="9"/>
       <c r="H53" s="47" t="s">
         <v>168</v>
@@ -10606,8 +10912,15 @@
       <c r="P53" s="34"/>
       <c r="Q53" s="34"/>
       <c r="R53" s="35"/>
+      <c r="Y53" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z53" s="127"/>
+      <c r="AA53" s="127"/>
+      <c r="AB53" s="127"/>
+      <c r="AC53" s="35"/>
     </row>
-    <row r="54" spans="7:18">
+    <row r="54" spans="7:29">
       <c r="G54" s="9"/>
       <c r="H54" s="34"/>
       <c r="I54" s="34"/>
@@ -10620,8 +10933,15 @@
       <c r="P54" s="34"/>
       <c r="Q54" s="34"/>
       <c r="R54" s="35"/>
+      <c r="Y54" s="129" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z54" s="127"/>
+      <c r="AA54" s="127"/>
+      <c r="AB54" s="127"/>
+      <c r="AC54" s="35"/>
     </row>
-    <row r="55" spans="7:18">
+    <row r="55" spans="7:29">
       <c r="G55" s="8">
         <v>43739</v>
       </c>
@@ -10640,8 +10960,15 @@
         <v>179</v>
       </c>
       <c r="R55" s="35"/>
+      <c r="Y55" s="129" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z55" s="127"/>
+      <c r="AA55" s="127"/>
+      <c r="AB55" s="127"/>
+      <c r="AC55" s="35"/>
     </row>
-    <row r="56" spans="7:18">
+    <row r="56" spans="7:29">
       <c r="G56" s="9"/>
       <c r="H56" s="34"/>
       <c r="I56" s="34"/>
@@ -10654,8 +10981,13 @@
       <c r="P56" s="34"/>
       <c r="Q56" s="34"/>
       <c r="R56" s="35"/>
+      <c r="Y56" s="39"/>
+      <c r="Z56" s="127"/>
+      <c r="AA56" s="127"/>
+      <c r="AB56" s="127"/>
+      <c r="AC56" s="35"/>
     </row>
-    <row r="57" spans="7:18">
+    <row r="57" spans="7:29">
       <c r="G57" s="9"/>
       <c r="H57" s="34"/>
       <c r="I57" s="34"/>
@@ -10668,8 +11000,13 @@
       <c r="P57" s="34"/>
       <c r="Q57" s="34"/>
       <c r="R57" s="35"/>
+      <c r="Y57" s="133"/>
+      <c r="Z57" s="134"/>
+      <c r="AA57" s="134"/>
+      <c r="AB57" s="134"/>
+      <c r="AC57" s="135"/>
     </row>
-    <row r="58" spans="7:18">
+    <row r="58" spans="7:29">
       <c r="G58" s="9"/>
       <c r="H58" s="34"/>
       <c r="I58" s="34"/>
@@ -10682,8 +11019,15 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
+      <c r="Y58" s="136" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z58" s="137"/>
+      <c r="AA58" s="137"/>
+      <c r="AB58" s="137"/>
+      <c r="AC58" s="138"/>
     </row>
-    <row r="59" spans="7:18">
+    <row r="59" spans="7:29">
       <c r="G59" s="8">
         <v>43586</v>
       </c>
@@ -10701,7 +11045,7 @@
       <c r="Q59" s="34"/>
       <c r="R59" s="35"/>
     </row>
-    <row r="60" spans="7:18">
+    <row r="60" spans="7:29">
       <c r="G60" s="9"/>
       <c r="H60" s="34"/>
       <c r="I60" s="34"/>
@@ -10715,7 +11059,7 @@
       <c r="Q60" s="34"/>
       <c r="R60" s="35"/>
     </row>
-    <row r="61" spans="7:18">
+    <row r="61" spans="7:29">
       <c r="G61" s="8">
         <v>43282</v>
       </c>
@@ -10733,7 +11077,7 @@
       <c r="Q61" s="34"/>
       <c r="R61" s="35"/>
     </row>
-    <row r="62" spans="7:18">
+    <row r="62" spans="7:29">
       <c r="G62" s="9"/>
       <c r="H62" s="7" t="s">
         <v>163</v>
@@ -10749,7 +11093,7 @@
       <c r="Q62" s="34"/>
       <c r="R62" s="35"/>
     </row>
-    <row r="63" spans="7:18">
+    <row r="63" spans="7:29">
       <c r="G63" s="9"/>
       <c r="H63" s="7" t="s">
         <v>165</v>
@@ -10765,7 +11109,7 @@
       <c r="Q63" s="34"/>
       <c r="R63" s="35"/>
     </row>
-    <row r="64" spans="7:18">
+    <row r="64" spans="7:29">
       <c r="G64" s="9"/>
       <c r="H64" s="34"/>
       <c r="I64" s="34"/>
@@ -10798,12 +11142,37 @@
       <c r="R65" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
+  <mergeCells count="51">
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="Y58:AC58"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
     <mergeCell ref="Z19:AA19"/>
     <mergeCell ref="AB19:AC19"/>
     <mergeCell ref="Z20:AA20"/>
@@ -10820,34 +11189,11 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H21" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -10873,10 +11219,11 @@
     <hyperlink ref="H10" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
     <hyperlink ref="H8" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
     <hyperlink ref="H6" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
+    <hyperlink ref="Y25:AC25" r:id="rId24" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId24"/>
-  <drawing r:id="rId25"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
£SDRY Trustpilot updates, news events
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125DD8E9-F140-448D-8FEF-EC3E89111097}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B953262-2694-4E39-931F-A723494CECFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -9505,7 +9505,7 @@
   <dimension ref="A2:AC71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -10293,7 +10293,10 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="113"/>
+      <c r="C28" s="132">
+        <f>+'Order &amp; Backlog'!$X$3</f>
+        <v>2058</v>
+      </c>
       <c r="D28" s="114"/>
       <c r="G28" s="9"/>
       <c r="H28" s="7" t="s">
@@ -11499,7 +11502,7 @@
   <dimension ref="B1:AS148"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="C135" sqref="C135:Y135"/>

</xml_diff>

<commit_message>
£SDRY Feb trustpilot, $ERJ Q423 orders/backlog/deliveries
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B953262-2694-4E39-931F-A723494CECFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D227E5A4-1DC7-4C21-8317-5B96F15936B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="305">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1073,6 +1073,12 @@
   </si>
   <si>
     <t>C390 millenium. cargo, firefighting?</t>
+  </si>
+  <si>
+    <t>Since?</t>
+  </si>
+  <si>
+    <t>Q423</t>
   </si>
 </sst>
 </file>
@@ -1621,34 +1627,25 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1658,24 +1655,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1705,21 +1684,48 @@
     <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5645,9 +5651,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$X$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$Y$1</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5716,16 +5722,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>Q323</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Q423</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$3:$X$3</c:f>
+              <c:f>'Order &amp; Backlog'!$B$3:$Y$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>1835</c:v>
                 </c:pt>
@@ -5794,6 +5803,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2090</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5838,9 +5850,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$X$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$Y$1</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -5909,16 +5921,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>Q323</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Q423</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$12:$X$12</c:f>
+              <c:f>'Order &amp; Backlog'!$B$12:$Y$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>1414</c:v>
                 </c:pt>
@@ -5987,6 +6002,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1767</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6031,9 +6049,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Order &amp; Backlog'!$B$1:$X$1</c:f>
+              <c:f>'Order &amp; Backlog'!$B$1:$Y$1</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>Q118</c:v>
                 </c:pt>
@@ -6102,16 +6120,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>Q323</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Q423</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Order &amp; Backlog'!$B$21:$X$21</c:f>
+              <c:f>'Order &amp; Backlog'!$B$21:$Y$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>421</c:v>
                 </c:pt>
@@ -6180,6 +6201,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9104,14 +9128,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -9128,7 +9152,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15592425" y="3175"/>
+          <a:off x="16211550" y="3175"/>
           <a:ext cx="0" cy="9617075"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -9154,13 +9178,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -9504,8 +9528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
   <dimension ref="A2:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9525,35 +9549,35 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="119"/>
-      <c r="G5" s="117" t="s">
+      <c r="C5" s="117"/>
+      <c r="D5" s="118"/>
+      <c r="G5" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="118"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="118"/>
-      <c r="R5" s="119"/>
-      <c r="T5" s="117" t="s">
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="118"/>
+      <c r="T5" s="116" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="118"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="119"/>
-      <c r="AA5" s="115" t="s">
+      <c r="U5" s="117"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="118"/>
+      <c r="AA5" s="136" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="116"/>
+      <c r="AB5" s="137"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -9779,13 +9803,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="117" t="s">
+      <c r="Y12" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="118"/>
-      <c r="AA12" s="118"/>
-      <c r="AB12" s="118"/>
-      <c r="AC12" s="119"/>
+      <c r="Z12" s="117"/>
+      <c r="AA12" s="117"/>
+      <c r="AB12" s="117"/>
+      <c r="AC12" s="118"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -9807,14 +9831,14 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="124" t="s">
+      <c r="Z13" s="128" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="124"/>
-      <c r="AB13" s="124" t="s">
+      <c r="AA13" s="128"/>
+      <c r="AB13" s="128" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="125"/>
+      <c r="AC13" s="129"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
@@ -9842,21 +9866,21 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="113" t="s">
+      <c r="Z14" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="113"/>
-      <c r="AB14" s="113" t="s">
+      <c r="AA14" s="114"/>
+      <c r="AB14" s="114" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="114"/>
+      <c r="AC14" s="115"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="118"/>
-      <c r="D15" s="119"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="118"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -9878,14 +9902,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="113" t="s">
+      <c r="Z15" s="114" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="113"/>
-      <c r="AB15" s="113" t="s">
+      <c r="AA15" s="114"/>
+      <c r="AB15" s="114" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="114"/>
+      <c r="AC15" s="115"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9894,10 +9918,13 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="113" t="s">
+      <c r="C16" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="114"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="3" t="s">
+        <v>303</v>
+      </c>
       <c r="G16" s="8">
         <v>45017</v>
       </c>
@@ -9923,23 +9950,26 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="113" t="s">
+      <c r="Z16" s="114" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="113"/>
-      <c r="AB16" s="113" t="s">
+      <c r="AA16" s="114"/>
+      <c r="AB16" s="114" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="114"/>
+      <c r="AC16" s="115"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="113" t="s">
+      <c r="C17" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="114"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="3" t="s">
+        <v>303</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
@@ -9959,19 +9989,19 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="113" t="s">
+      <c r="Z17" s="114" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="113"/>
-      <c r="AB17" s="113" t="s">
+      <c r="AA17" s="114"/>
+      <c r="AB17" s="114" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="114"/>
+      <c r="AC17" s="115"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="115"/>
       <c r="G18" s="8">
         <v>44927</v>
       </c>
@@ -9997,19 +10027,19 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="113" t="s">
+      <c r="Z18" s="114" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="113"/>
-      <c r="AB18" s="113" t="s">
+      <c r="AA18" s="114"/>
+      <c r="AB18" s="114" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="114"/>
+      <c r="AC18" s="115"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="123"/>
+      <c r="C19" s="140"/>
+      <c r="D19" s="141"/>
       <c r="G19" s="9"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -10031,14 +10061,14 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="113" t="s">
+      <c r="Z19" s="114" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="113"/>
-      <c r="AB19" s="113" t="s">
+      <c r="AA19" s="114"/>
+      <c r="AB19" s="114" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="114"/>
+      <c r="AC19" s="115"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="8">
@@ -10066,14 +10096,14 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="113" t="s">
+      <c r="Z20" s="114" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="113"/>
-      <c r="AB20" s="113" t="s">
+      <c r="AA20" s="114"/>
+      <c r="AB20" s="114" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="114"/>
+      <c r="AC20" s="115"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -10101,11 +10131,11 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="118"/>
-      <c r="D22" s="119"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
       <c r="G22" s="8">
         <v>44866</v>
       </c>
@@ -10138,10 +10168,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="113" t="s">
+      <c r="C23" s="114" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="114"/>
+      <c r="D23" s="115"/>
       <c r="G23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -10163,10 +10193,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="113">
+      <c r="C24" s="114">
         <v>1969</v>
       </c>
-      <c r="D24" s="114"/>
+      <c r="D24" s="115"/>
       <c r="G24" s="8">
         <v>44835</v>
       </c>
@@ -10192,8 +10222,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="114"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="115"/>
       <c r="G25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -10212,23 +10242,23 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="107" t="s">
+      <c r="Y25" s="130" t="s">
         <v>288</v>
       </c>
-      <c r="Z25" s="108"/>
-      <c r="AA25" s="108"/>
-      <c r="AB25" s="108"/>
-      <c r="AC25" s="109"/>
+      <c r="Z25" s="131"/>
+      <c r="AA25" s="131"/>
+      <c r="AB25" s="131"/>
+      <c r="AC25" s="132"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="120">
+      <c r="C26" s="138">
         <f>'Financial Model'!Y68</f>
         <v>3053.1</v>
       </c>
-      <c r="D26" s="121"/>
+      <c r="D26" s="139"/>
       <c r="G26" s="9"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
@@ -10257,8 +10287,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="113"/>
-      <c r="D27" s="114"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="115"/>
       <c r="G27" s="8">
         <v>44835</v>
       </c>
@@ -10293,11 +10323,11 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="132">
+      <c r="C28" s="125">
         <f>+'Order &amp; Backlog'!$X$3</f>
         <v>2058</v>
       </c>
-      <c r="D28" s="114"/>
+      <c r="D28" s="115"/>
       <c r="G28" s="9"/>
       <c r="H28" s="7" t="s">
         <v>12</v>
@@ -10330,11 +10360,11 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="132">
+      <c r="C29" s="125">
         <f>'Order &amp; Backlog'!X21</f>
         <v>291</v>
       </c>
-      <c r="D29" s="114"/>
+      <c r="D29" s="115"/>
       <c r="G29" s="9"/>
       <c r="H29" s="7" t="s">
         <v>13</v>
@@ -10365,11 +10395,11 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="113">
+      <c r="C30" s="114">
         <f>'Financial Model'!Y43</f>
         <v>43</v>
       </c>
-      <c r="D30" s="114"/>
+      <c r="D30" s="115"/>
       <c r="G30" s="9"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
@@ -10398,10 +10428,10 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="133">
+      <c r="C31" s="126">
         <v>36708</v>
       </c>
-      <c r="D31" s="134"/>
+      <c r="D31" s="127"/>
       <c r="G31" s="8">
         <v>44835</v>
       </c>
@@ -10434,8 +10464,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="115"/>
       <c r="G32" s="9"/>
       <c r="H32" s="7" t="s">
         <v>30</v>
@@ -10489,22 +10519,22 @@
       <c r="U33" s="34"/>
       <c r="V33" s="34"/>
       <c r="W33" s="35"/>
-      <c r="Y33" s="139" t="s">
+      <c r="Y33" s="107" t="s">
         <v>299</v>
       </c>
-      <c r="Z33" s="140"/>
-      <c r="AA33" s="140"/>
-      <c r="AB33" s="140"/>
-      <c r="AC33" s="141"/>
+      <c r="Z33" s="108"/>
+      <c r="AA33" s="108"/>
+      <c r="AB33" s="108"/>
+      <c r="AC33" s="109"/>
     </row>
     <row r="34" spans="2:29">
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="128" t="s">
+      <c r="C34" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="129"/>
+      <c r="D34" s="122"/>
       <c r="G34" s="9"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
@@ -10574,11 +10604,11 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="117" t="s">
+      <c r="B37" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="118"/>
-      <c r="D37" s="119"/>
+      <c r="C37" s="117"/>
+      <c r="D37" s="118"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -10591,12 +10621,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="117" t="s">
+      <c r="T37" s="116" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="118"/>
-      <c r="V37" s="118"/>
-      <c r="W37" s="119"/>
+      <c r="U37" s="117"/>
+      <c r="V37" s="117"/>
+      <c r="W37" s="118"/>
       <c r="Y37" s="39" t="s">
         <v>280</v>
       </c>
@@ -10609,11 +10639,11 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="130">
+      <c r="C38" s="123">
         <f>C6/'Financial Model'!Y123</f>
         <v>5.0530683931892986</v>
       </c>
-      <c r="D38" s="131"/>
+      <c r="D38" s="124"/>
       <c r="G38" s="8">
         <v>44805</v>
       </c>
@@ -10648,11 +10678,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="130">
+      <c r="C39" s="123">
         <f>C8/SUM('Financial Model'!X9:Y9)</f>
         <v>5.4823448597042734</v>
       </c>
-      <c r="D39" s="131"/>
+      <c r="D39" s="124"/>
       <c r="G39" s="9"/>
       <c r="H39" s="7" t="s">
         <v>192</v>
@@ -10683,11 +10713,11 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="126">
+      <c r="C40" s="119">
         <f>C6/SUM('Financial Model'!X26:Y26)</f>
         <v>334.74781990521325</v>
       </c>
-      <c r="D40" s="127"/>
+      <c r="D40" s="120"/>
       <c r="G40" s="9"/>
       <c r="H40" s="7" t="s">
         <v>193</v>
@@ -10767,11 +10797,11 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="117" t="s">
+      <c r="B43" s="116" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="118"/>
-      <c r="D43" s="119"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="118"/>
       <c r="G43" s="9"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -10799,10 +10829,10 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="135" t="s">
+      <c r="B44" s="110" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="136"/>
+      <c r="C44" s="111"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
@@ -10837,10 +10867,10 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="135" t="s">
+      <c r="B45" s="110" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="136"/>
+      <c r="C45" s="111"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
@@ -10873,8 +10903,8 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="135"/>
-      <c r="C46" s="136"/>
+      <c r="B46" s="110"/>
+      <c r="C46" s="111"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
@@ -10903,8 +10933,8 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="135"/>
-      <c r="C47" s="136"/>
+      <c r="B47" s="110"/>
+      <c r="C47" s="111"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
@@ -10935,8 +10965,8 @@
       <c r="AC47" s="35"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="137"/>
-      <c r="C48" s="138"/>
+      <c r="B48" s="112"/>
+      <c r="C48" s="113"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
@@ -11194,13 +11224,13 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
-      <c r="Y58" s="110" t="s">
+      <c r="Y58" s="133" t="s">
         <v>295</v>
       </c>
-      <c r="Z58" s="111"/>
-      <c r="AA58" s="111"/>
-      <c r="AB58" s="111"/>
-      <c r="AC58" s="112"/>
+      <c r="Z58" s="134"/>
+      <c r="AA58" s="134"/>
+      <c r="AB58" s="134"/>
+      <c r="AC58" s="135"/>
     </row>
     <row r="59" spans="7:29">
       <c r="G59" s="9"/>
@@ -11410,11 +11440,37 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="Y58:AC58"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
     <mergeCell ref="Z20:AA20"/>
     <mergeCell ref="AB20:AC20"/>
     <mergeCell ref="B43:D43"/>
@@ -11430,37 +11486,11 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Y25:AC25"/>
-    <mergeCell ref="Y58:AC58"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H27" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
@@ -11502,10 +11532,10 @@
   <dimension ref="B1:AS148"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="N14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C135" sqref="C135:Y135"/>
+      <selection pane="bottomRight" activeCell="W148" sqref="W148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -25938,8 +25968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -25954,13 +25984,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258CA0E5-563F-4C1F-B583-AD76D8E7BBD2}">
-  <dimension ref="A1:AK49"/>
+  <dimension ref="A1:AL49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V20" sqref="V20"/>
+      <selection pane="bottomRight" activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -25969,7 +25999,7 @@
     <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="2" customFormat="1">
+    <row r="1" spans="1:38" s="2" customFormat="1">
       <c r="B1" s="23" t="s">
         <v>32</v>
       </c>
@@ -26039,57 +26069,60 @@
       <c r="X1" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="Z1" s="76">
+      <c r="Y1" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="AA1" s="76">
         <v>2014</v>
       </c>
-      <c r="AA1" s="76">
+      <c r="AB1" s="76">
         <v>2015</v>
       </c>
-      <c r="AB1" s="76">
+      <c r="AC1" s="76">
         <v>2016</v>
       </c>
-      <c r="AC1" s="76">
+      <c r="AD1" s="76">
         <v>2017</v>
       </c>
-      <c r="AD1" s="76">
+      <c r="AE1" s="76">
         <v>2018</v>
       </c>
-      <c r="AE1" s="76">
-        <f>AD1+1</f>
+      <c r="AF1" s="76">
+        <f>AE1+1</f>
         <v>2019</v>
       </c>
-      <c r="AF1" s="76">
-        <f t="shared" ref="AF1:AK1" si="0">AE1+1</f>
+      <c r="AG1" s="76">
+        <f t="shared" ref="AG1:AL1" si="0">AF1+1</f>
         <v>2020</v>
       </c>
-      <c r="AG1" s="76">
+      <c r="AH1" s="76">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="AH1" s="2">
+      <c r="AI1" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="AI1" s="2">
+      <c r="AJ1" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="AJ1" s="2">
+      <c r="AK1" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="AK1" s="2">
+      <c r="AL1" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="91" customFormat="1">
+    <row r="2" spans="1:38" s="91" customFormat="1">
       <c r="A2" s="89"/>
       <c r="B2" s="90"/>
       <c r="C2" s="90"/>
       <c r="D2" s="90"/>
     </row>
-    <row r="3" spans="1:37" s="73" customFormat="1">
+    <row r="3" spans="1:38" s="73" customFormat="1">
       <c r="A3" s="73" t="s">
         <v>208</v>
       </c>
@@ -26162,7 +26195,7 @@
         <v>1992</v>
       </c>
       <c r="S3" s="73">
-        <f t="shared" ref="S3:X3" si="14">SUM(S4:S10)</f>
+        <f t="shared" ref="S3:Y3" si="14">SUM(S4:S10)</f>
         <v>2000</v>
       </c>
       <c r="T3" s="73">
@@ -26185,40 +26218,44 @@
         <f t="shared" si="14"/>
         <v>2058</v>
       </c>
-      <c r="Z3" s="73">
-        <f t="shared" ref="Z3:AD3" si="15">SUM(Z4:Z10)</f>
+      <c r="Y3" s="73">
+        <f t="shared" si="14"/>
+        <v>2090</v>
+      </c>
+      <c r="AA3" s="73">
+        <f t="shared" ref="AA3:AE3" si="15">SUM(AA4:AA10)</f>
         <v>1549</v>
       </c>
-      <c r="AA3" s="73">
+      <c r="AB3" s="73">
         <f t="shared" si="15"/>
         <v>1704</v>
       </c>
-      <c r="AB3" s="73">
+      <c r="AC3" s="73">
         <f t="shared" si="15"/>
         <v>1749</v>
       </c>
-      <c r="AC3" s="73">
+      <c r="AD3" s="73">
         <f t="shared" si="15"/>
         <v>1835</v>
       </c>
-      <c r="AD3" s="73">
+      <c r="AE3" s="73">
         <f t="shared" si="15"/>
         <v>1858</v>
       </c>
-      <c r="AE3" s="73">
-        <f t="shared" ref="AE3" si="16">SUM(AE4:AE10)</f>
+      <c r="AF3" s="73">
+        <f t="shared" ref="AF3" si="16">SUM(AF4:AF10)</f>
         <v>1917</v>
       </c>
-      <c r="AF3" s="73">
-        <f t="shared" ref="AF3" si="17">SUM(AF4:AF10)</f>
+      <c r="AG3" s="73">
+        <f t="shared" ref="AG3" si="17">SUM(AG4:AG10)</f>
         <v>1904</v>
       </c>
-      <c r="AG3" s="73">
-        <f t="shared" ref="AG3" si="18">SUM(AG4:AG10)</f>
+      <c r="AH3" s="73">
+        <f t="shared" ref="AH3" si="18">SUM(AH4:AH10)</f>
         <v>1996</v>
       </c>
     </row>
-    <row r="4" spans="1:37" s="74" customFormat="1">
+    <row r="4" spans="1:38" s="74" customFormat="1">
       <c r="A4" s="75" t="s">
         <v>201</v>
       </c>
@@ -26291,8 +26328,8 @@
       <c r="X4" s="74">
         <v>191</v>
       </c>
-      <c r="Z4" s="74">
-        <v>193</v>
+      <c r="Y4" s="74">
+        <v>191</v>
       </c>
       <c r="AA4" s="74">
         <v>193</v>
@@ -26301,7 +26338,7 @@
         <v>193</v>
       </c>
       <c r="AC4" s="74">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AD4" s="74">
         <v>191</v>
@@ -26315,8 +26352,11 @@
       <c r="AG4" s="74">
         <v>191</v>
       </c>
+      <c r="AH4" s="74">
+        <v>191</v>
+      </c>
     </row>
-    <row r="5" spans="1:37" s="74" customFormat="1">
+    <row r="5" spans="1:38" s="74" customFormat="1">
       <c r="A5" s="75" t="s">
         <v>85</v>
       </c>
@@ -26389,32 +26429,35 @@
       <c r="X5" s="74">
         <v>847</v>
       </c>
-      <c r="Z5" s="74">
+      <c r="Y5" s="74">
+        <v>853</v>
+      </c>
+      <c r="AA5" s="74">
         <v>421</v>
       </c>
-      <c r="AA5" s="74">
+      <c r="AB5" s="74">
         <v>500</v>
       </c>
-      <c r="AB5" s="74">
+      <c r="AC5" s="74">
         <v>525</v>
       </c>
-      <c r="AC5" s="74">
+      <c r="AD5" s="74">
         <v>603</v>
       </c>
-      <c r="AD5" s="74">
+      <c r="AE5" s="74">
         <v>771</v>
       </c>
-      <c r="AE5" s="74">
+      <c r="AF5" s="74">
         <v>815</v>
       </c>
-      <c r="AF5" s="74">
+      <c r="AG5" s="74">
         <v>798</v>
       </c>
-      <c r="AG5" s="74">
+      <c r="AH5" s="74">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:37" s="74" customFormat="1">
+    <row r="6" spans="1:38" s="74" customFormat="1">
       <c r="A6" s="75" t="s">
         <v>185</v>
       </c>
@@ -26487,23 +26530,23 @@
       <c r="X6" s="74">
         <v>568</v>
       </c>
-      <c r="Z6" s="74">
+      <c r="Y6" s="74">
+        <v>568</v>
+      </c>
+      <c r="AA6" s="74">
         <v>580</v>
       </c>
-      <c r="AA6" s="74">
+      <c r="AB6" s="74">
         <v>578</v>
       </c>
-      <c r="AB6" s="74">
+      <c r="AC6" s="74">
         <v>590</v>
       </c>
-      <c r="AC6" s="74">
+      <c r="AD6" s="74">
         <v>592</v>
       </c>
-      <c r="AD6" s="74">
+      <c r="AE6" s="74">
         <v>566</v>
-      </c>
-      <c r="AE6" s="74">
-        <v>568</v>
       </c>
       <c r="AF6" s="74">
         <v>568</v>
@@ -26511,8 +26554,11 @@
       <c r="AG6" s="74">
         <v>568</v>
       </c>
+      <c r="AH6" s="74">
+        <v>568</v>
+      </c>
     </row>
-    <row r="7" spans="1:37" s="74" customFormat="1">
+    <row r="7" spans="1:38" s="74" customFormat="1">
       <c r="A7" s="75" t="s">
         <v>188</v>
       </c>
@@ -26585,20 +26631,20 @@
       <c r="X7" s="74">
         <v>172</v>
       </c>
-      <c r="Z7" s="74">
+      <c r="Y7" s="74">
+        <v>172</v>
+      </c>
+      <c r="AA7" s="74">
         <v>145</v>
-      </c>
-      <c r="AA7" s="74">
-        <v>166</v>
       </c>
       <c r="AB7" s="74">
         <v>166</v>
       </c>
       <c r="AC7" s="74">
+        <v>166</v>
+      </c>
+      <c r="AD7" s="74">
         <v>169</v>
-      </c>
-      <c r="AD7" s="74">
-        <v>172</v>
       </c>
       <c r="AE7" s="74">
         <v>172</v>
@@ -26609,8 +26655,11 @@
       <c r="AG7" s="74">
         <v>172</v>
       </c>
+      <c r="AH7" s="74">
+        <v>172</v>
+      </c>
     </row>
-    <row r="8" spans="1:37" s="74" customFormat="1">
+    <row r="8" spans="1:38" s="74" customFormat="1">
       <c r="A8" s="75" t="s">
         <v>215</v>
       </c>
@@ -26683,8 +26732,8 @@
       <c r="X8" s="74">
         <v>0</v>
       </c>
-      <c r="Z8" s="74">
-        <v>100</v>
+      <c r="Y8" s="74">
+        <v>0</v>
       </c>
       <c r="AA8" s="74">
         <v>100</v>
@@ -26696,7 +26745,7 @@
         <v>100</v>
       </c>
       <c r="AD8" s="74">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AE8" s="74">
         <v>0</v>
@@ -26707,8 +26756,11 @@
       <c r="AG8" s="74">
         <v>0</v>
       </c>
+      <c r="AH8" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:37" s="74" customFormat="1">
+    <row r="9" spans="1:38" s="74" customFormat="1">
       <c r="A9" s="75" t="s">
         <v>180</v>
       </c>
@@ -26781,32 +26833,35 @@
       <c r="X9" s="74">
         <v>34</v>
       </c>
-      <c r="Z9" s="74">
+      <c r="Y9" s="74">
+        <v>35</v>
+      </c>
+      <c r="AA9" s="74">
         <v>60</v>
       </c>
-      <c r="AA9" s="74">
+      <c r="AB9" s="74">
         <v>77</v>
       </c>
-      <c r="AB9" s="74">
+      <c r="AC9" s="74">
         <v>85</v>
       </c>
-      <c r="AC9" s="74">
+      <c r="AD9" s="74">
         <v>74</v>
       </c>
-      <c r="AD9" s="74">
+      <c r="AE9" s="74">
         <v>47</v>
       </c>
-      <c r="AE9" s="74">
+      <c r="AF9" s="74">
         <v>27</v>
-      </c>
-      <c r="AF9" s="74">
-        <v>22</v>
       </c>
       <c r="AG9" s="74">
         <v>22</v>
       </c>
+      <c r="AH9" s="74">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:37" s="74" customFormat="1">
+    <row r="10" spans="1:38" s="74" customFormat="1">
       <c r="A10" s="75" t="s">
         <v>86</v>
       </c>
@@ -26879,33 +26934,36 @@
       <c r="X10" s="74">
         <v>246</v>
       </c>
-      <c r="Z10" s="74">
+      <c r="Y10" s="74">
+        <v>271</v>
+      </c>
+      <c r="AA10" s="74">
         <v>50</v>
-      </c>
-      <c r="AA10" s="74">
-        <v>90</v>
       </c>
       <c r="AB10" s="74">
         <v>90</v>
       </c>
       <c r="AC10" s="74">
+        <v>90</v>
+      </c>
+      <c r="AD10" s="74">
         <v>106</v>
       </c>
-      <c r="AD10" s="74">
+      <c r="AE10" s="74">
         <v>111</v>
       </c>
-      <c r="AE10" s="74">
+      <c r="AF10" s="74">
         <v>144</v>
       </c>
-      <c r="AF10" s="74">
+      <c r="AG10" s="74">
         <v>153</v>
       </c>
-      <c r="AG10" s="74">
+      <c r="AH10" s="74">
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:37" s="74" customFormat="1"/>
-    <row r="12" spans="1:37" s="73" customFormat="1">
+    <row r="11" spans="1:38" s="74" customFormat="1"/>
+    <row r="12" spans="1:38" s="73" customFormat="1">
       <c r="A12" s="73" t="s">
         <v>210</v>
       </c>
@@ -27001,40 +27059,44 @@
         <f>SUM(X13:X19)</f>
         <v>1767</v>
       </c>
-      <c r="Z12" s="73">
-        <f t="shared" ref="Z12:AG12" si="20">SUM(Z13:Z19)</f>
+      <c r="Y12" s="73">
+        <f>SUM(Y13:Y19)</f>
+        <v>1797</v>
+      </c>
+      <c r="AA12" s="73">
+        <f t="shared" ref="AA12:AH12" si="20">SUM(AA13:AA19)</f>
         <v>1090</v>
       </c>
-      <c r="AA12" s="73">
+      <c r="AB12" s="73">
         <f t="shared" si="20"/>
         <v>1181</v>
       </c>
-      <c r="AB12" s="73">
+      <c r="AC12" s="73">
         <f t="shared" si="20"/>
         <v>1299</v>
       </c>
-      <c r="AC12" s="73">
+      <c r="AD12" s="73">
         <f t="shared" si="20"/>
         <v>1400</v>
       </c>
-      <c r="AD12" s="73">
+      <c r="AE12" s="73">
         <f t="shared" si="20"/>
         <v>1490</v>
       </c>
-      <c r="AE12" s="73">
+      <c r="AF12" s="73">
         <f t="shared" si="20"/>
         <v>1579</v>
       </c>
-      <c r="AF12" s="73">
+      <c r="AG12" s="73">
         <f t="shared" si="20"/>
         <v>1623</v>
       </c>
-      <c r="AG12" s="73">
+      <c r="AH12" s="73">
         <f t="shared" si="20"/>
         <v>1671</v>
       </c>
     </row>
-    <row r="13" spans="1:37" s="74" customFormat="1">
+    <row r="13" spans="1:38" s="74" customFormat="1">
       <c r="A13" s="75" t="s">
         <v>201</v>
       </c>
@@ -27107,11 +27169,11 @@
       <c r="X13" s="74">
         <v>191</v>
       </c>
-      <c r="Z13" s="74">
+      <c r="Y13" s="74">
+        <v>191</v>
+      </c>
+      <c r="AA13" s="74">
         <v>188</v>
-      </c>
-      <c r="AA13" s="74">
-        <v>190</v>
       </c>
       <c r="AB13" s="74">
         <v>190</v>
@@ -27120,7 +27182,7 @@
         <v>190</v>
       </c>
       <c r="AD13" s="74">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AE13" s="74">
         <v>191</v>
@@ -27131,8 +27193,11 @@
       <c r="AG13" s="74">
         <v>191</v>
       </c>
+      <c r="AH13" s="74">
+        <v>191</v>
+      </c>
     </row>
-    <row r="14" spans="1:37" s="74" customFormat="1">
+    <row r="14" spans="1:38" s="74" customFormat="1">
       <c r="A14" s="75" t="s">
         <v>85</v>
       </c>
@@ -27205,32 +27270,36 @@
       <c r="X14" s="74">
         <v>746</v>
       </c>
-      <c r="Z14" s="74">
+      <c r="Y14" s="74">
+        <f>+X14+14</f>
+        <v>760</v>
+      </c>
+      <c r="AA14" s="74">
         <v>249</v>
       </c>
-      <c r="AA14" s="74">
+      <c r="AB14" s="74">
         <v>331</v>
       </c>
-      <c r="AB14" s="74">
+      <c r="AC14" s="74">
         <v>421</v>
       </c>
-      <c r="AC14" s="74">
+      <c r="AD14" s="74">
         <v>500</v>
       </c>
-      <c r="AD14" s="74">
+      <c r="AE14" s="74">
         <v>567</v>
       </c>
-      <c r="AE14" s="74">
+      <c r="AF14" s="74">
         <v>634</v>
       </c>
-      <c r="AF14" s="74">
+      <c r="AG14" s="74">
         <v>666</v>
       </c>
-      <c r="AG14" s="74">
+      <c r="AH14" s="74">
         <v>693</v>
       </c>
     </row>
-    <row r="15" spans="1:37" s="74" customFormat="1">
+    <row r="15" spans="1:38" s="74" customFormat="1">
       <c r="A15" s="75" t="s">
         <v>185</v>
       </c>
@@ -27303,32 +27372,36 @@
       <c r="X15" s="74">
         <v>568</v>
       </c>
-      <c r="Z15" s="74">
+      <c r="Y15" s="74">
+        <f>3+X15</f>
+        <v>571</v>
+      </c>
+      <c r="AA15" s="74">
         <v>515</v>
       </c>
-      <c r="AA15" s="74">
+      <c r="AB15" s="74">
         <v>523</v>
       </c>
-      <c r="AB15" s="74">
+      <c r="AC15" s="74">
         <v>534</v>
       </c>
-      <c r="AC15" s="74">
+      <c r="AD15" s="74">
         <v>546</v>
       </c>
-      <c r="AD15" s="74">
+      <c r="AE15" s="74">
         <v>559</v>
       </c>
-      <c r="AE15" s="74">
+      <c r="AF15" s="74">
         <v>564</v>
-      </c>
-      <c r="AF15" s="74">
-        <v>565</v>
       </c>
       <c r="AG15" s="74">
         <v>565</v>
       </c>
+      <c r="AH15" s="74">
+        <v>565</v>
+      </c>
     </row>
-    <row r="16" spans="1:37" s="74" customFormat="1">
+    <row r="16" spans="1:38" s="74" customFormat="1">
       <c r="A16" s="75" t="s">
         <v>188</v>
       </c>
@@ -27401,23 +27474,23 @@
       <c r="X16" s="74">
         <v>172</v>
       </c>
-      <c r="Z16" s="74">
+      <c r="Y16" s="74">
+        <v>172</v>
+      </c>
+      <c r="AA16" s="74">
         <v>138</v>
       </c>
-      <c r="AA16" s="74">
+      <c r="AB16" s="74">
         <v>137</v>
       </c>
-      <c r="AB16" s="74">
+      <c r="AC16" s="74">
         <v>154</v>
       </c>
-      <c r="AC16" s="74">
+      <c r="AD16" s="74">
         <v>164</v>
       </c>
-      <c r="AD16" s="74">
+      <c r="AE16" s="74">
         <v>169</v>
-      </c>
-      <c r="AE16" s="74">
-        <v>172</v>
       </c>
       <c r="AF16" s="74">
         <v>172</v>
@@ -27425,8 +27498,11 @@
       <c r="AG16" s="74">
         <v>172</v>
       </c>
+      <c r="AH16" s="74">
+        <v>172</v>
+      </c>
     </row>
-    <row r="17" spans="1:33" s="74" customFormat="1">
+    <row r="17" spans="1:34" s="74" customFormat="1">
       <c r="A17" s="75" t="s">
         <v>215</v>
       </c>
@@ -27499,7 +27575,7 @@
       <c r="X17" s="74">
         <v>0</v>
       </c>
-      <c r="Z17" s="74">
+      <c r="Y17" s="74">
         <v>0</v>
       </c>
       <c r="AA17" s="74">
@@ -27523,8 +27599,11 @@
       <c r="AG17" s="74">
         <v>0</v>
       </c>
+      <c r="AH17" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:33" s="74" customFormat="1">
+    <row r="18" spans="1:34" s="74" customFormat="1">
       <c r="A18" s="75" t="s">
         <v>180</v>
       </c>
@@ -27597,8 +27676,9 @@
       <c r="X18" s="74">
         <v>18</v>
       </c>
-      <c r="Z18" s="74">
-        <v>0</v>
+      <c r="Y18" s="74">
+        <f>1+X18</f>
+        <v>19</v>
       </c>
       <c r="AA18" s="74">
         <v>0</v>
@@ -27610,19 +27690,22 @@
         <v>0</v>
       </c>
       <c r="AD18" s="74">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="74">
         <v>4</v>
       </c>
-      <c r="AE18" s="74">
+      <c r="AF18" s="74">
         <v>11</v>
       </c>
-      <c r="AF18" s="74">
+      <c r="AG18" s="74">
         <v>15</v>
       </c>
-      <c r="AG18" s="74">
+      <c r="AH18" s="74">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:33" s="74" customFormat="1">
+    <row r="19" spans="1:34" s="74" customFormat="1">
       <c r="A19" s="75" t="s">
         <v>86</v>
       </c>
@@ -27695,8 +27778,9 @@
       <c r="X19" s="74">
         <v>72</v>
       </c>
-      <c r="Z19" s="74">
-        <v>0</v>
+      <c r="Y19" s="74">
+        <f>12+X19</f>
+        <v>84</v>
       </c>
       <c r="AA19" s="74">
         <v>0</v>
@@ -27711,24 +27795,27 @@
         <v>0</v>
       </c>
       <c r="AE19" s="74">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="74">
         <v>7</v>
       </c>
-      <c r="AF19" s="74">
+      <c r="AG19" s="74">
         <v>14</v>
       </c>
-      <c r="AG19" s="74">
+      <c r="AH19" s="74">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:33" s="74" customFormat="1">
+    <row r="20" spans="1:34" s="74" customFormat="1">
       <c r="A20" s="75"/>
     </row>
-    <row r="21" spans="1:33" s="73" customFormat="1">
+    <row r="21" spans="1:34" s="73" customFormat="1">
       <c r="A21" s="73" t="s">
         <v>209</v>
       </c>
       <c r="B21" s="73">
-        <f t="shared" ref="B21:X21" si="21">SUM(B22:B28)</f>
+        <f t="shared" ref="B21:Y21" si="21">SUM(B22:B28)</f>
         <v>421</v>
       </c>
       <c r="C21" s="73">
@@ -27819,40 +27906,44 @@
         <f t="shared" si="21"/>
         <v>291</v>
       </c>
-      <c r="Z21" s="73">
-        <f t="shared" ref="Z21:AG21" si="22">SUM(Z22:Z28)</f>
+      <c r="Y21" s="73">
+        <f t="shared" si="21"/>
+        <v>298</v>
+      </c>
+      <c r="AA21" s="73">
+        <f t="shared" ref="AA21:AH21" si="22">SUM(AA22:AA28)</f>
         <v>459</v>
       </c>
-      <c r="AA21" s="73">
+      <c r="AB21" s="73">
         <f t="shared" si="22"/>
         <v>513</v>
       </c>
-      <c r="AB21" s="73">
+      <c r="AC21" s="73">
         <f t="shared" si="22"/>
         <v>450</v>
       </c>
-      <c r="AC21" s="73">
+      <c r="AD21" s="73">
         <f t="shared" si="22"/>
         <v>435</v>
       </c>
-      <c r="AD21" s="73">
+      <c r="AE21" s="73">
         <f t="shared" si="22"/>
         <v>368</v>
       </c>
-      <c r="AE21" s="73">
+      <c r="AF21" s="73">
         <f t="shared" si="22"/>
         <v>338</v>
       </c>
-      <c r="AF21" s="73">
+      <c r="AG21" s="73">
         <f t="shared" si="22"/>
         <v>281</v>
       </c>
-      <c r="AG21" s="73">
+      <c r="AH21" s="73">
         <f t="shared" si="22"/>
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="1:33" s="74" customFormat="1">
+    <row r="22" spans="1:34" s="74" customFormat="1">
       <c r="A22" s="75" t="s">
         <v>201</v>
       </c>
@@ -27925,21 +28016,21 @@
       <c r="X22" s="74">
         <v>0</v>
       </c>
-      <c r="Z22" s="74">
+      <c r="Y22" s="74">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="74">
         <v>5</v>
-      </c>
-      <c r="AA22" s="74">
-        <v>3</v>
       </c>
       <c r="AB22" s="74">
         <v>3</v>
       </c>
       <c r="AC22" s="74">
+        <v>3</v>
+      </c>
+      <c r="AD22" s="74">
         <v>1</v>
       </c>
-      <c r="AD22" s="74">
-        <v>0</v>
-      </c>
       <c r="AE22" s="74">
         <v>0</v>
       </c>
@@ -27949,8 +28040,11 @@
       <c r="AG22" s="74">
         <v>0</v>
       </c>
+      <c r="AH22" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:33" s="74" customFormat="1">
+    <row r="23" spans="1:34" s="74" customFormat="1">
       <c r="A23" s="75" t="s">
         <v>85</v>
       </c>
@@ -28023,32 +28117,35 @@
       <c r="X23" s="74">
         <v>101</v>
       </c>
-      <c r="Z23" s="74">
+      <c r="Y23" s="74">
+        <v>182</v>
+      </c>
+      <c r="AA23" s="74">
         <v>172</v>
       </c>
-      <c r="AA23" s="74">
+      <c r="AB23" s="74">
         <v>169</v>
       </c>
-      <c r="AB23" s="74">
+      <c r="AC23" s="74">
         <v>104</v>
       </c>
-      <c r="AC23" s="74">
+      <c r="AD23" s="74">
         <v>103</v>
       </c>
-      <c r="AD23" s="74">
+      <c r="AE23" s="74">
         <v>204</v>
       </c>
-      <c r="AE23" s="74">
+      <c r="AF23" s="74">
         <v>181</v>
       </c>
-      <c r="AF23" s="74">
+      <c r="AG23" s="74">
         <v>132</v>
       </c>
-      <c r="AG23" s="74">
+      <c r="AH23" s="74">
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:33" s="74" customFormat="1">
+    <row r="24" spans="1:34" s="74" customFormat="1">
       <c r="A24" s="75" t="s">
         <v>185</v>
       </c>
@@ -28121,32 +28218,35 @@
       <c r="X24" s="74">
         <v>0</v>
       </c>
-      <c r="Z24" s="74">
+      <c r="Y24" s="74">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="74">
         <v>65</v>
       </c>
-      <c r="AA24" s="74">
+      <c r="AB24" s="74">
         <v>55</v>
       </c>
-      <c r="AB24" s="74">
+      <c r="AC24" s="74">
         <v>56</v>
       </c>
-      <c r="AC24" s="74">
+      <c r="AD24" s="74">
         <v>46</v>
       </c>
-      <c r="AD24" s="74">
+      <c r="AE24" s="74">
         <v>7</v>
       </c>
-      <c r="AE24" s="74">
+      <c r="AF24" s="74">
         <v>4</v>
-      </c>
-      <c r="AF24" s="74">
-        <v>3</v>
       </c>
       <c r="AG24" s="74">
         <v>3</v>
       </c>
+      <c r="AH24" s="74">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="1:33" s="74" customFormat="1">
+    <row r="25" spans="1:34" s="74" customFormat="1">
       <c r="A25" s="75" t="s">
         <v>188</v>
       </c>
@@ -28219,32 +28319,35 @@
       <c r="X25" s="74">
         <v>0</v>
       </c>
-      <c r="Z25" s="74">
+      <c r="Y25" s="74">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="74">
         <v>7</v>
       </c>
-      <c r="AA25" s="74">
+      <c r="AB25" s="74">
         <v>19</v>
       </c>
-      <c r="AB25" s="74">
+      <c r="AC25" s="74">
         <v>12</v>
       </c>
-      <c r="AC25" s="74">
+      <c r="AD25" s="74">
         <v>5</v>
       </c>
-      <c r="AD25" s="74">
+      <c r="AE25" s="74">
         <v>3</v>
       </c>
-      <c r="AE25" s="74">
-        <v>0</v>
-      </c>
       <c r="AF25" s="74">
         <v>0</v>
       </c>
       <c r="AG25" s="74">
         <v>0</v>
       </c>
+      <c r="AH25" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:33" s="74" customFormat="1">
+    <row r="26" spans="1:34" s="74" customFormat="1">
       <c r="A26" s="75" t="s">
         <v>215</v>
       </c>
@@ -28317,8 +28420,8 @@
       <c r="X26" s="74">
         <v>0</v>
       </c>
-      <c r="Z26" s="74">
-        <v>100</v>
+      <c r="Y26" s="74">
+        <v>0</v>
       </c>
       <c r="AA26" s="74">
         <v>100</v>
@@ -28330,7 +28433,7 @@
         <v>100</v>
       </c>
       <c r="AD26" s="74">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AE26" s="74">
         <v>0</v>
@@ -28341,8 +28444,11 @@
       <c r="AG26" s="74">
         <v>0</v>
       </c>
+      <c r="AH26" s="74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:33" s="74" customFormat="1">
+    <row r="27" spans="1:34" s="74" customFormat="1">
       <c r="A27" s="75" t="s">
         <v>180</v>
       </c>
@@ -28415,32 +28521,35 @@
       <c r="X27" s="74">
         <v>16</v>
       </c>
-      <c r="Z27" s="74">
+      <c r="Y27" s="74">
+        <v>16</v>
+      </c>
+      <c r="AA27" s="74">
         <v>60</v>
       </c>
-      <c r="AA27" s="74">
+      <c r="AB27" s="74">
         <v>77</v>
       </c>
-      <c r="AB27" s="74">
+      <c r="AC27" s="74">
         <v>85</v>
       </c>
-      <c r="AC27" s="74">
+      <c r="AD27" s="74">
         <v>74</v>
       </c>
-      <c r="AD27" s="74">
+      <c r="AE27" s="74">
         <v>43</v>
       </c>
-      <c r="AE27" s="74">
+      <c r="AF27" s="74">
         <v>16</v>
       </c>
-      <c r="AF27" s="74">
+      <c r="AG27" s="74">
         <v>7</v>
       </c>
-      <c r="AG27" s="74">
+      <c r="AH27" s="74">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:33" s="74" customFormat="1">
+    <row r="28" spans="1:34" s="74" customFormat="1">
       <c r="A28" s="75" t="s">
         <v>86</v>
       </c>
@@ -28513,32 +28622,35 @@
       <c r="X28" s="74">
         <v>174</v>
       </c>
-      <c r="Z28" s="74">
+      <c r="Y28" s="74">
+        <v>100</v>
+      </c>
+      <c r="AA28" s="74">
         <v>50</v>
-      </c>
-      <c r="AA28" s="74">
-        <v>90</v>
       </c>
       <c r="AB28" s="74">
         <v>90</v>
       </c>
       <c r="AC28" s="74">
+        <v>90</v>
+      </c>
+      <c r="AD28" s="74">
         <v>106</v>
       </c>
-      <c r="AD28" s="74">
+      <c r="AE28" s="74">
         <v>111</v>
       </c>
-      <c r="AE28" s="74">
+      <c r="AF28" s="74">
         <v>137</v>
       </c>
-      <c r="AF28" s="74">
+      <c r="AG28" s="74">
         <v>139</v>
       </c>
-      <c r="AG28" s="74">
+      <c r="AH28" s="74">
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="31" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>211</v>
       </c>
@@ -28630,39 +28742,43 @@
         <f t="shared" ref="X31" si="33">X3/T3-1</f>
         <v>3.1578947368421151E-2</v>
       </c>
-      <c r="Z31" s="59" t="s">
+      <c r="Y31" s="31">
+        <f t="shared" ref="Y31" si="34">Y3/U3-1</f>
+        <v>3.5165923724616244E-2</v>
+      </c>
+      <c r="AA31" s="59" t="s">
         <v>186</v>
-      </c>
-      <c r="AA31" s="31">
-        <f t="shared" ref="AA31" si="34">AA3/Z3-1</f>
-        <v>0.1000645577792123</v>
       </c>
       <c r="AB31" s="31">
         <f t="shared" ref="AB31" si="35">AB3/AA3-1</f>
+        <v>0.1000645577792123</v>
+      </c>
+      <c r="AC31" s="31">
+        <f t="shared" ref="AC31" si="36">AC3/AB3-1</f>
         <v>2.6408450704225261E-2</v>
       </c>
-      <c r="AC31" s="31">
-        <f t="shared" ref="AC31:AD31" si="36">AC3/AB3-1</f>
+      <c r="AD31" s="31">
+        <f t="shared" ref="AD31:AE31" si="37">AD3/AC3-1</f>
         <v>4.9170954831332159E-2</v>
       </c>
-      <c r="AD31" s="31">
-        <f t="shared" si="36"/>
+      <c r="AE31" s="31">
+        <f t="shared" si="37"/>
         <v>1.2534059945504161E-2</v>
-      </c>
-      <c r="AE31" s="31">
-        <f>AE3/AD3-1</f>
-        <v>3.1754574811625469E-2</v>
       </c>
       <c r="AF31" s="31">
         <f>AF3/AE3-1</f>
-        <v>-6.7814293166406081E-3</v>
+        <v>3.1754574811625469E-2</v>
       </c>
       <c r="AG31" s="31">
         <f>AG3/AF3-1</f>
+        <v>-6.7814293166406081E-3</v>
+      </c>
+      <c r="AH31" s="31">
+        <f>AH3/AG3-1</f>
         <v>4.8319327731092487E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:33" s="77" customFormat="1" ht="12.75" customHeight="1">
+    <row r="32" spans="1:34" s="77" customFormat="1" ht="12.75" customHeight="1">
       <c r="A32" s="81" t="s">
         <v>211</v>
       </c>
@@ -28679,31 +28795,31 @@
         <v>186</v>
       </c>
       <c r="F32" s="77">
-        <f t="shared" ref="F32" si="37">F3-B3</f>
+        <f t="shared" ref="F32" si="38">F3-B3</f>
         <v>25</v>
       </c>
       <c r="G32" s="77">
-        <f t="shared" ref="G32" si="38">G3-C3</f>
+        <f t="shared" ref="G32" si="39">G3-C3</f>
         <v>88</v>
       </c>
       <c r="H32" s="77">
-        <f t="shared" ref="H32" si="39">H3-D3</f>
+        <f t="shared" ref="H32" si="40">H3-D3</f>
         <v>181</v>
       </c>
       <c r="I32" s="77">
-        <f t="shared" ref="I32:L32" si="40">I3-E3</f>
+        <f t="shared" ref="I32:L32" si="41">I3-E3</f>
         <v>59</v>
       </c>
       <c r="J32" s="77">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>42</v>
       </c>
       <c r="K32" s="77">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>12</v>
       </c>
       <c r="L32" s="77">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>13</v>
       </c>
       <c r="M32" s="77">
@@ -28711,15 +28827,15 @@
         <v>-13</v>
       </c>
       <c r="N32" s="77">
-        <f t="shared" ref="N32" si="41">N3-J3</f>
+        <f t="shared" ref="N32" si="42">N3-J3</f>
         <v>2</v>
       </c>
       <c r="O32" s="77">
-        <f t="shared" ref="O32" si="42">O3-K3</f>
+        <f t="shared" ref="O32" si="43">O3-K3</f>
         <v>50</v>
       </c>
       <c r="P32" s="77">
-        <f t="shared" ref="P32" si="43">P3-L3</f>
+        <f t="shared" ref="P32" si="44">P3-L3</f>
         <v>66</v>
       </c>
       <c r="Q32" s="77">
@@ -28739,54 +28855,58 @@
         <v>27</v>
       </c>
       <c r="U32" s="77">
-        <f t="shared" ref="U32" si="44">U3-Q3</f>
+        <f t="shared" ref="U32" si="45">U3-Q3</f>
         <v>23</v>
       </c>
       <c r="V32" s="77">
-        <f t="shared" ref="V32" si="45">V3-R3</f>
+        <f t="shared" ref="V32" si="46">V3-R3</f>
         <v>24</v>
       </c>
       <c r="W32" s="77">
-        <f t="shared" ref="W32" si="46">W3-S3</f>
+        <f t="shared" ref="W32" si="47">W3-S3</f>
         <v>23</v>
       </c>
       <c r="X32" s="77">
-        <f t="shared" ref="X32" si="47">X3-T3</f>
+        <f t="shared" ref="X32" si="48">X3-T3</f>
         <v>63</v>
       </c>
-      <c r="Z32" s="59" t="s">
+      <c r="Y32" s="77">
+        <f t="shared" ref="Y32" si="49">Y3-U3</f>
+        <v>71</v>
+      </c>
+      <c r="AA32" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="AA32" s="77">
-        <f t="shared" ref="AA32" si="48">AA3-Z3</f>
+      <c r="AB32" s="77">
+        <f t="shared" ref="AB32" si="50">AB3-AA3</f>
         <v>155</v>
       </c>
-      <c r="AB32" s="77">
-        <f t="shared" ref="AB32" si="49">AB3-AA3</f>
+      <c r="AC32" s="77">
+        <f t="shared" ref="AC32" si="51">AC3-AB3</f>
         <v>45</v>
       </c>
-      <c r="AC32" s="77">
-        <f t="shared" ref="AC32:AD32" si="50">AC3-AB3</f>
+      <c r="AD32" s="77">
+        <f t="shared" ref="AD32:AE32" si="52">AD3-AC3</f>
         <v>86</v>
       </c>
-      <c r="AD32" s="77">
-        <f t="shared" si="50"/>
+      <c r="AE32" s="77">
+        <f t="shared" si="52"/>
         <v>23</v>
-      </c>
-      <c r="AE32" s="77">
-        <f>AE3-AD3</f>
-        <v>59</v>
       </c>
       <c r="AF32" s="77">
         <f>AF3-AE3</f>
-        <v>-13</v>
+        <v>59</v>
       </c>
       <c r="AG32" s="77">
         <f>AG3-AF3</f>
+        <v>-13</v>
+      </c>
+      <c r="AH32" s="77">
+        <f>AH3-AG3</f>
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="12.75" customHeight="1">
+    <row r="33" spans="1:34" ht="12.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>212</v>
       </c>
@@ -28794,95 +28914,96 @@
         <v>186</v>
       </c>
       <c r="C33" s="24">
-        <f t="shared" ref="C33" si="51">C3/B3-1</f>
+        <f t="shared" ref="C33" si="53">C3/B3-1</f>
         <v>-1.7983651226158082E-2</v>
       </c>
       <c r="D33" s="24">
-        <f t="shared" ref="D33" si="52">D3/C3-1</f>
+        <f t="shared" ref="D33" si="54">D3/C3-1</f>
         <v>-5.2164261931187617E-2</v>
       </c>
       <c r="E33" s="24">
-        <f t="shared" ref="E33" si="53">E3/D3-1</f>
+        <f t="shared" ref="E33" si="55">E3/D3-1</f>
         <v>8.7822014051522235E-2</v>
       </c>
       <c r="F33" s="24">
-        <f t="shared" ref="F33" si="54">F3/E3-1</f>
+        <f t="shared" ref="F33" si="56">F3/E3-1</f>
         <v>1.0764262648008671E-3</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" ref="G33" si="55">G3/F3-1</f>
+        <f t="shared" ref="G33" si="57">G3/F3-1</f>
         <v>1.6129032258064502E-2</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" ref="H33" si="56">H3/G3-1</f>
+        <f t="shared" ref="H33" si="58">H3/G3-1</f>
         <v>-5.2910052910049021E-4</v>
       </c>
       <c r="I33" s="24">
-        <f t="shared" ref="I33" si="57">I3/H3-1</f>
+        <f t="shared" ref="I33" si="59">I3/H3-1</f>
         <v>1.4822657490735747E-2</v>
       </c>
       <c r="J33" s="24">
-        <f t="shared" ref="J33" si="58">J3/I3-1</f>
+        <f t="shared" ref="J33" si="60">J3/I3-1</f>
         <v>-7.8247261345852914E-3</v>
       </c>
       <c r="K33" s="24">
-        <f t="shared" ref="K33" si="59">K3/J3-1</f>
+        <f t="shared" ref="K33" si="61">K3/J3-1</f>
         <v>0</v>
       </c>
       <c r="L33" s="24">
-        <f t="shared" ref="L33" si="60">L3/K3-1</f>
+        <f t="shared" ref="L33" si="62">L3/K3-1</f>
         <v>0</v>
       </c>
       <c r="M33" s="24">
-        <f t="shared" ref="M33" si="61">M3/L3-1</f>
+        <f t="shared" ref="M33" si="63">M3/L3-1</f>
         <v>1.051524710830698E-3</v>
       </c>
       <c r="N33" s="24">
-        <f t="shared" ref="N33" si="62">N3/M3-1</f>
+        <f t="shared" ref="N33" si="64">N3/M3-1</f>
         <v>0</v>
       </c>
       <c r="O33" s="24">
-        <f t="shared" ref="O33" si="63">O3/N3-1</f>
+        <f t="shared" ref="O33" si="65">O3/N3-1</f>
         <v>2.5210084033613356E-2</v>
       </c>
       <c r="P33" s="24">
-        <f t="shared" ref="P33:T33" si="64">P3/O3-1</f>
+        <f t="shared" ref="P33:T33" si="66">P3/O3-1</f>
         <v>8.1967213114753079E-3</v>
       </c>
       <c r="Q33" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>1.4227642276422703E-2</v>
       </c>
       <c r="R33" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>-2.0040080160320661E-3</v>
       </c>
       <c r="S33" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>4.0160642570281624E-3</v>
       </c>
       <c r="T33" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>-2.4999999999999467E-3</v>
       </c>
       <c r="U33" s="24">
-        <f t="shared" ref="U33" si="65">U3/T3-1</f>
+        <f t="shared" ref="U33" si="67">U3/T3-1</f>
         <v>1.2030075187969835E-2</v>
       </c>
       <c r="V33" s="24">
-        <f t="shared" ref="V33" si="66">V3/U3-1</f>
+        <f t="shared" ref="V33" si="68">V3/U3-1</f>
         <v>-1.4858841010401136E-3</v>
       </c>
       <c r="W33" s="24">
-        <f t="shared" ref="W33" si="67">W3/V3-1</f>
+        <f t="shared" ref="W33" si="69">W3/V3-1</f>
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="X33" s="24">
-        <f t="shared" ref="X33" si="68">X3/W3-1</f>
+        <f t="shared" ref="X33" si="70">X3/W3-1</f>
         <v>1.730103806228378E-2</v>
       </c>
-      <c r="Z33" s="59" t="s">
-        <v>186</v>
+      <c r="Y33" s="24">
+        <f t="shared" ref="Y33" si="71">Y3/X3-1</f>
+        <v>1.554907677356665E-2</v>
       </c>
       <c r="AA33" s="59" t="s">
         <v>186</v>
@@ -28905,8 +29026,11 @@
       <c r="AG33" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AH33" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="34" spans="1:33" s="78" customFormat="1" ht="12.75" customHeight="1">
+    <row r="34" spans="1:34" s="78" customFormat="1" ht="12.75" customHeight="1">
       <c r="A34" s="82" t="s">
         <v>212</v>
       </c>
@@ -28914,95 +29038,96 @@
         <v>186</v>
       </c>
       <c r="C34" s="77">
-        <f t="shared" ref="C34" si="69">C3-B3</f>
+        <f t="shared" ref="C34" si="72">C3-B3</f>
         <v>-33</v>
       </c>
       <c r="D34" s="77">
-        <f t="shared" ref="D34" si="70">D3-C3</f>
+        <f t="shared" ref="D34" si="73">D3-C3</f>
         <v>-94</v>
       </c>
       <c r="E34" s="77">
-        <f t="shared" ref="E34" si="71">E3-D3</f>
+        <f t="shared" ref="E34" si="74">E3-D3</f>
         <v>150</v>
       </c>
       <c r="F34" s="77">
-        <f t="shared" ref="F34" si="72">F3-E3</f>
+        <f t="shared" ref="F34" si="75">F3-E3</f>
         <v>2</v>
       </c>
       <c r="G34" s="77">
-        <f t="shared" ref="G34" si="73">G3-F3</f>
+        <f t="shared" ref="G34" si="76">G3-F3</f>
         <v>30</v>
       </c>
       <c r="H34" s="77">
-        <f t="shared" ref="H34" si="74">H3-G3</f>
+        <f t="shared" ref="H34" si="77">H3-G3</f>
         <v>-1</v>
       </c>
       <c r="I34" s="77">
-        <f t="shared" ref="I34" si="75">I3-H3</f>
+        <f t="shared" ref="I34" si="78">I3-H3</f>
         <v>28</v>
       </c>
       <c r="J34" s="77">
-        <f t="shared" ref="J34" si="76">J3-I3</f>
+        <f t="shared" ref="J34" si="79">J3-I3</f>
         <v>-15</v>
       </c>
       <c r="K34" s="77">
-        <f t="shared" ref="K34" si="77">K3-J3</f>
+        <f t="shared" ref="K34" si="80">K3-J3</f>
         <v>0</v>
       </c>
       <c r="L34" s="77">
-        <f t="shared" ref="L34" si="78">L3-K3</f>
+        <f t="shared" ref="L34" si="81">L3-K3</f>
         <v>0</v>
       </c>
       <c r="M34" s="77">
-        <f t="shared" ref="M34" si="79">M3-L3</f>
+        <f t="shared" ref="M34" si="82">M3-L3</f>
         <v>2</v>
       </c>
       <c r="N34" s="77">
-        <f t="shared" ref="N34" si="80">N3-M3</f>
+        <f t="shared" ref="N34" si="83">N3-M3</f>
         <v>0</v>
       </c>
       <c r="O34" s="77">
-        <f t="shared" ref="O34" si="81">O3-N3</f>
+        <f t="shared" ref="O34" si="84">O3-N3</f>
         <v>48</v>
       </c>
       <c r="P34" s="77">
-        <f t="shared" ref="P34:T34" si="82">P3-O3</f>
+        <f t="shared" ref="P34:T34" si="85">P3-O3</f>
         <v>16</v>
       </c>
       <c r="Q34" s="77">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>28</v>
       </c>
       <c r="R34" s="77">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>-4</v>
       </c>
       <c r="S34" s="77">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>8</v>
       </c>
       <c r="T34" s="77">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>-5</v>
       </c>
       <c r="U34" s="77">
-        <f t="shared" ref="U34" si="83">U3-T3</f>
+        <f t="shared" ref="U34" si="86">U3-T3</f>
         <v>24</v>
       </c>
       <c r="V34" s="77">
-        <f t="shared" ref="V34" si="84">V3-U3</f>
+        <f t="shared" ref="V34" si="87">V3-U3</f>
         <v>-3</v>
       </c>
       <c r="W34" s="77">
-        <f t="shared" ref="W34" si="85">W3-V3</f>
+        <f t="shared" ref="W34" si="88">W3-V3</f>
         <v>7</v>
       </c>
       <c r="X34" s="77">
-        <f t="shared" ref="X34" si="86">X3-W3</f>
+        <f t="shared" ref="X34" si="89">X3-W3</f>
         <v>35</v>
       </c>
-      <c r="Z34" s="59" t="s">
-        <v>186</v>
+      <c r="Y34" s="77">
+        <f t="shared" ref="Y34" si="90">Y3-X3</f>
+        <v>32</v>
       </c>
       <c r="AA34" s="59" t="s">
         <v>186</v>
@@ -29025,11 +29150,14 @@
       <c r="AG34" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AH34" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="35" spans="1:33" ht="12.75" customHeight="1">
-      <c r="AG35" s="24"/>
+    <row r="35" spans="1:34" ht="12.75" customHeight="1">
+      <c r="AH35" s="24"/>
     </row>
-    <row r="36" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="36" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
@@ -29046,31 +29174,31 @@
         <v>186</v>
       </c>
       <c r="F36" s="31">
-        <f t="shared" ref="F36" si="87">F12/B12-1</f>
+        <f t="shared" ref="F36" si="91">F12/B12-1</f>
         <v>6.1527581329561487E-2</v>
       </c>
       <c r="G36" s="31">
-        <f t="shared" ref="G36" si="88">G12/C12-1</f>
+        <f t="shared" ref="G36" si="92">G12/C12-1</f>
         <v>5.8945908460471541E-2</v>
       </c>
       <c r="H36" s="31">
-        <f t="shared" ref="H36" si="89">H12/D12-1</f>
+        <f t="shared" ref="H36" si="93">H12/D12-1</f>
         <v>5.9711736444749475E-2</v>
       </c>
       <c r="I36" s="31">
-        <f t="shared" ref="I36:L36" si="90">I12/E12-1</f>
+        <f t="shared" ref="I36:L36" si="94">I12/E12-1</f>
         <v>5.9731543624160999E-2</v>
       </c>
       <c r="J36" s="31">
-        <f t="shared" si="90"/>
+        <f t="shared" si="94"/>
         <v>5.5296469020652994E-2</v>
       </c>
       <c r="K36" s="31">
-        <f t="shared" si="90"/>
+        <f t="shared" si="94"/>
         <v>3.9947609692206898E-2</v>
       </c>
       <c r="L36" s="31">
-        <f t="shared" si="90"/>
+        <f t="shared" si="94"/>
         <v>3.303108808290145E-2</v>
       </c>
       <c r="M36" s="31">
@@ -29078,15 +29206,15 @@
         <v>2.7865737808739688E-2</v>
       </c>
       <c r="N36" s="31">
-        <f t="shared" ref="N36" si="91">N12/J12-1</f>
+        <f t="shared" ref="N36" si="95">N12/J12-1</f>
         <v>3.0303030303030276E-2</v>
       </c>
       <c r="O36" s="31">
-        <f t="shared" ref="O36" si="92">O12/K12-1</f>
+        <f t="shared" ref="O36" si="96">O12/K12-1</f>
         <v>3.6523929471032668E-2</v>
       </c>
       <c r="P36" s="31">
-        <f t="shared" ref="P36" si="93">P12/L12-1</f>
+        <f t="shared" ref="P36" si="97">P12/L12-1</f>
         <v>3.7617554858934144E-2</v>
       </c>
       <c r="Q36" s="31">
@@ -29106,54 +29234,58 @@
         <v>2.5981873111782461E-2</v>
       </c>
       <c r="U36" s="31">
-        <f t="shared" ref="U36" si="94">U12/Q12-1</f>
+        <f t="shared" ref="U36" si="98">U12/Q12-1</f>
         <v>3.4111310592459532E-2</v>
       </c>
       <c r="V36" s="31">
-        <f t="shared" ref="V36" si="95">V12/R12-1</f>
+        <f t="shared" ref="V36" si="99">V12/R12-1</f>
         <v>3.4585569469290478E-2</v>
       </c>
       <c r="W36" s="31">
-        <f t="shared" ref="W36" si="96">W12/S12-1</f>
+        <f t="shared" ref="W36" si="100">W12/S12-1</f>
         <v>3.7914691943127909E-2</v>
       </c>
       <c r="X36" s="31">
-        <f t="shared" ref="X36" si="97">X12/T12-1</f>
+        <f t="shared" ref="X36" si="101">X12/T12-1</f>
         <v>4.0636042402826922E-2</v>
       </c>
-      <c r="Z36" s="59" t="s">
+      <c r="Y36" s="31">
+        <f t="shared" ref="Y36" si="102">Y12/U12-1</f>
+        <v>3.993055555555558E-2</v>
+      </c>
+      <c r="AA36" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="AA36" s="31">
-        <f t="shared" ref="AA36" si="98">AA12/Z12-1</f>
+      <c r="AB36" s="31">
+        <f t="shared" ref="AB36" si="103">AB12/AA12-1</f>
         <v>8.3486238532110013E-2</v>
       </c>
-      <c r="AB36" s="31">
-        <f t="shared" ref="AB36" si="99">AB12/AA12-1</f>
+      <c r="AC36" s="31">
+        <f t="shared" ref="AC36" si="104">AC12/AB12-1</f>
         <v>9.9915325994919479E-2</v>
       </c>
-      <c r="AC36" s="31">
-        <f t="shared" ref="AC36:AD36" si="100">AC12/AB12-1</f>
+      <c r="AD36" s="31">
+        <f t="shared" ref="AD36:AE36" si="105">AD12/AC12-1</f>
         <v>7.7752117013087041E-2</v>
       </c>
-      <c r="AD36" s="31">
-        <f t="shared" si="100"/>
+      <c r="AE36" s="31">
+        <f t="shared" si="105"/>
         <v>6.4285714285714279E-2</v>
-      </c>
-      <c r="AE36" s="31">
-        <f>AE12/AD12-1</f>
-        <v>5.9731543624160999E-2</v>
       </c>
       <c r="AF36" s="31">
         <f>AF12/AE12-1</f>
-        <v>2.7865737808739688E-2</v>
+        <v>5.9731543624160999E-2</v>
       </c>
       <c r="AG36" s="31">
         <f>AG12/AF12-1</f>
+        <v>2.7865737808739688E-2</v>
+      </c>
+      <c r="AH36" s="31">
+        <f>AH12/AG12-1</f>
         <v>2.9574861367837268E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:33" s="77" customFormat="1" ht="12.75" customHeight="1">
+    <row r="37" spans="1:34" s="77" customFormat="1" ht="12.75" customHeight="1">
       <c r="A37" s="81" t="s">
         <v>202</v>
       </c>
@@ -29170,31 +29302,31 @@
         <v>186</v>
       </c>
       <c r="F37" s="77">
-        <f t="shared" ref="F37" si="101">F12-B12</f>
+        <f t="shared" ref="F37" si="106">F12-B12</f>
         <v>87</v>
       </c>
       <c r="G37" s="77">
-        <f t="shared" ref="G37" si="102">G12-C12</f>
+        <f t="shared" ref="G37" si="107">G12-C12</f>
         <v>85</v>
       </c>
       <c r="H37" s="77">
-        <f t="shared" ref="H37" si="103">H12-D12</f>
+        <f t="shared" ref="H37" si="108">H12-D12</f>
         <v>87</v>
       </c>
       <c r="I37" s="77">
-        <f t="shared" ref="I37:L37" si="104">I12-E12</f>
+        <f t="shared" ref="I37:L37" si="109">I12-E12</f>
         <v>89</v>
       </c>
       <c r="J37" s="77">
-        <f t="shared" si="104"/>
+        <f t="shared" si="109"/>
         <v>83</v>
       </c>
       <c r="K37" s="77">
-        <f t="shared" si="104"/>
+        <f t="shared" si="109"/>
         <v>61</v>
       </c>
       <c r="L37" s="77">
-        <f t="shared" si="104"/>
+        <f t="shared" si="109"/>
         <v>51</v>
       </c>
       <c r="M37" s="77">
@@ -29202,15 +29334,15 @@
         <v>44</v>
       </c>
       <c r="N37" s="77">
-        <f t="shared" ref="N37" si="105">N12-J12</f>
+        <f t="shared" ref="N37" si="110">N12-J12</f>
         <v>48</v>
       </c>
       <c r="O37" s="77">
-        <f t="shared" ref="O37" si="106">O12-K12</f>
+        <f t="shared" ref="O37" si="111">O12-K12</f>
         <v>58</v>
       </c>
       <c r="P37" s="77">
-        <f t="shared" ref="P37" si="107">P12-L12</f>
+        <f t="shared" ref="P37" si="112">P12-L12</f>
         <v>60</v>
       </c>
       <c r="Q37" s="77">
@@ -29230,54 +29362,58 @@
         <v>43</v>
       </c>
       <c r="U37" s="77">
-        <f t="shared" ref="U37" si="108">U12-Q12</f>
+        <f t="shared" ref="U37" si="113">U12-Q12</f>
         <v>57</v>
       </c>
       <c r="V37" s="77">
-        <f t="shared" ref="V37" si="109">V12-R12</f>
+        <f t="shared" ref="V37" si="114">V12-R12</f>
         <v>58</v>
       </c>
       <c r="W37" s="77">
-        <f t="shared" ref="W37" si="110">W12-S12</f>
+        <f t="shared" ref="W37" si="115">W12-S12</f>
         <v>64</v>
       </c>
       <c r="X37" s="77">
-        <f t="shared" ref="X37" si="111">X12-T12</f>
+        <f t="shared" ref="X37" si="116">X12-T12</f>
         <v>69</v>
       </c>
-      <c r="Z37" s="59" t="s">
+      <c r="Y37" s="77">
+        <f t="shared" ref="Y37" si="117">Y12-U12</f>
+        <v>69</v>
+      </c>
+      <c r="AA37" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="AA37" s="77">
-        <f t="shared" ref="AA37" si="112">AA12-Z12</f>
+      <c r="AB37" s="77">
+        <f t="shared" ref="AB37" si="118">AB12-AA12</f>
         <v>91</v>
       </c>
-      <c r="AB37" s="77">
-        <f t="shared" ref="AB37" si="113">AB12-AA12</f>
+      <c r="AC37" s="77">
+        <f t="shared" ref="AC37" si="119">AC12-AB12</f>
         <v>118</v>
       </c>
-      <c r="AC37" s="77">
-        <f t="shared" ref="AC37:AD37" si="114">AC12-AB12</f>
+      <c r="AD37" s="77">
+        <f t="shared" ref="AD37:AE37" si="120">AD12-AC12</f>
         <v>101</v>
       </c>
-      <c r="AD37" s="77">
-        <f t="shared" si="114"/>
+      <c r="AE37" s="77">
+        <f t="shared" si="120"/>
         <v>90</v>
-      </c>
-      <c r="AE37" s="77">
-        <f>AE12-AD12</f>
-        <v>89</v>
       </c>
       <c r="AF37" s="77">
         <f>AF12-AE12</f>
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="AG37" s="77">
         <f>AG12-AF12</f>
+        <v>44</v>
+      </c>
+      <c r="AH37" s="77">
+        <f>AH12-AG12</f>
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="12.75" customHeight="1">
+    <row r="38" spans="1:34" ht="12.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>203</v>
       </c>
@@ -29285,95 +29421,96 @@
         <v>186</v>
       </c>
       <c r="C38" s="24">
-        <f t="shared" ref="C38" si="115">C12/B12-1</f>
+        <f t="shared" ref="C38" si="121">C12/B12-1</f>
         <v>1.980198019801982E-2</v>
       </c>
       <c r="D38" s="24">
-        <f t="shared" ref="D38" si="116">D12/C12-1</f>
+        <f t="shared" ref="D38" si="122">D12/C12-1</f>
         <v>1.0402219140083213E-2</v>
       </c>
       <c r="E38" s="24">
-        <f t="shared" ref="E38" si="117">E12/D12-1</f>
+        <f t="shared" ref="E38" si="123">E12/D12-1</f>
         <v>2.2649279341111939E-2</v>
       </c>
       <c r="F38" s="24">
-        <f t="shared" ref="F38" si="118">F12/E12-1</f>
+        <f t="shared" ref="F38" si="124">F12/E12-1</f>
         <v>7.382550335570448E-3</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" ref="G38" si="119">G12/F12-1</f>
+        <f t="shared" ref="G38" si="125">G12/F12-1</f>
         <v>1.7321785476348994E-2</v>
       </c>
       <c r="H38" s="24">
-        <f t="shared" ref="H38" si="120">H12/G12-1</f>
+        <f t="shared" ref="H38" si="126">H12/G12-1</f>
         <v>1.1132940406024971E-2</v>
       </c>
       <c r="I38" s="24">
-        <f t="shared" ref="I38" si="121">I12/H12-1</f>
+        <f t="shared" ref="I38" si="127">I12/H12-1</f>
         <v>2.26683937823835E-2</v>
       </c>
       <c r="J38" s="24">
-        <f t="shared" ref="J38" si="122">J12/I12-1</f>
+        <f t="shared" ref="J38" si="128">J12/I12-1</f>
         <v>3.1665611146294292E-3</v>
       </c>
       <c r="K38" s="24">
-        <f t="shared" ref="K38" si="123">K12/J12-1</f>
+        <f t="shared" ref="K38" si="129">K12/J12-1</f>
         <v>2.525252525252597E-3</v>
       </c>
       <c r="L38" s="24">
-        <f t="shared" ref="L38" si="124">L12/K12-1</f>
+        <f t="shared" ref="L38" si="130">L12/K12-1</f>
         <v>4.4080604534004753E-3</v>
       </c>
       <c r="M38" s="24">
-        <f t="shared" ref="M38" si="125">M12/L12-1</f>
+        <f t="shared" ref="M38" si="131">M12/L12-1</f>
         <v>1.7554858934169193E-2</v>
       </c>
       <c r="N38" s="24">
-        <f t="shared" ref="N38" si="126">N12/M12-1</f>
+        <f t="shared" ref="N38" si="132">N12/M12-1</f>
         <v>5.5452865064695711E-3</v>
       </c>
       <c r="O38" s="24">
-        <f t="shared" ref="O38" si="127">O12/N12-1</f>
+        <f t="shared" ref="O38" si="133">O12/N12-1</f>
         <v>8.5784313725489891E-3</v>
       </c>
       <c r="P38" s="24">
-        <f t="shared" ref="P38:T38" si="128">P12/O12-1</f>
+        <f t="shared" ref="P38:T38" si="134">P12/O12-1</f>
         <v>5.4678007290400732E-3</v>
       </c>
       <c r="Q38" s="24">
-        <f t="shared" si="128"/>
+        <f t="shared" si="134"/>
         <v>9.6676737160121817E-3</v>
       </c>
       <c r="R38" s="24">
-        <f t="shared" si="128"/>
+        <f t="shared" si="134"/>
         <v>3.5906642728904536E-3</v>
       </c>
       <c r="S38" s="24">
-        <f t="shared" si="128"/>
+        <f t="shared" si="134"/>
         <v>6.5593321407275695E-3</v>
       </c>
       <c r="T38" s="24">
-        <f t="shared" si="128"/>
+        <f t="shared" si="134"/>
         <v>5.924170616113722E-3</v>
       </c>
       <c r="U38" s="24">
-        <f t="shared" ref="U38" si="129">U12/T12-1</f>
+        <f t="shared" ref="U38" si="135">U12/T12-1</f>
         <v>1.7667844522968101E-2</v>
       </c>
       <c r="V38" s="24">
-        <f t="shared" ref="V38" si="130">V12/U12-1</f>
+        <f t="shared" ref="V38" si="136">V12/U12-1</f>
         <v>4.050925925925819E-3</v>
       </c>
       <c r="W38" s="24">
-        <f t="shared" ref="W38" si="131">W12/V12-1</f>
+        <f t="shared" ref="W38" si="137">W12/V12-1</f>
         <v>9.7982708933717078E-3</v>
       </c>
       <c r="X38" s="24">
-        <f t="shared" ref="X38" si="132">X12/W12-1</f>
+        <f t="shared" ref="X38" si="138">X12/W12-1</f>
         <v>8.5616438356164171E-3</v>
       </c>
-      <c r="Z38" s="59" t="s">
-        <v>186</v>
+      <c r="Y38" s="24">
+        <f t="shared" ref="Y38" si="139">Y12/X12-1</f>
+        <v>1.6977928692699429E-2</v>
       </c>
       <c r="AA38" s="59" t="s">
         <v>186</v>
@@ -29396,8 +29533,11 @@
       <c r="AG38" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AH38" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="39" spans="1:33" s="79" customFormat="1" ht="12.75" customHeight="1">
+    <row r="39" spans="1:34" s="79" customFormat="1" ht="12.75" customHeight="1">
       <c r="A39" s="83" t="s">
         <v>203</v>
       </c>
@@ -29405,95 +29545,96 @@
         <v>186</v>
       </c>
       <c r="C39" s="77">
-        <f t="shared" ref="C39" si="133">C12-B12</f>
+        <f t="shared" ref="C39" si="140">C12-B12</f>
         <v>28</v>
       </c>
       <c r="D39" s="77">
-        <f t="shared" ref="D39" si="134">D12-C12</f>
+        <f t="shared" ref="D39" si="141">D12-C12</f>
         <v>15</v>
       </c>
       <c r="E39" s="77">
-        <f t="shared" ref="E39" si="135">E12-D12</f>
+        <f t="shared" ref="E39" si="142">E12-D12</f>
         <v>33</v>
       </c>
       <c r="F39" s="77">
-        <f t="shared" ref="F39" si="136">F12-E12</f>
+        <f t="shared" ref="F39" si="143">F12-E12</f>
         <v>11</v>
       </c>
       <c r="G39" s="77">
-        <f t="shared" ref="G39" si="137">G12-F12</f>
+        <f t="shared" ref="G39" si="144">G12-F12</f>
         <v>26</v>
       </c>
       <c r="H39" s="77">
-        <f t="shared" ref="H39" si="138">H12-G12</f>
+        <f t="shared" ref="H39" si="145">H12-G12</f>
         <v>17</v>
       </c>
       <c r="I39" s="77">
-        <f t="shared" ref="I39" si="139">I12-H12</f>
+        <f t="shared" ref="I39" si="146">I12-H12</f>
         <v>35</v>
       </c>
       <c r="J39" s="77">
-        <f t="shared" ref="J39" si="140">J12-I12</f>
+        <f t="shared" ref="J39" si="147">J12-I12</f>
         <v>5</v>
       </c>
       <c r="K39" s="77">
-        <f t="shared" ref="K39" si="141">K12-J12</f>
+        <f t="shared" ref="K39" si="148">K12-J12</f>
         <v>4</v>
       </c>
       <c r="L39" s="77">
-        <f t="shared" ref="L39" si="142">L12-K12</f>
+        <f t="shared" ref="L39" si="149">L12-K12</f>
         <v>7</v>
       </c>
       <c r="M39" s="77">
-        <f t="shared" ref="M39" si="143">M12-L12</f>
+        <f t="shared" ref="M39" si="150">M12-L12</f>
         <v>28</v>
       </c>
       <c r="N39" s="77">
-        <f t="shared" ref="N39" si="144">N12-M12</f>
+        <f t="shared" ref="N39" si="151">N12-M12</f>
         <v>9</v>
       </c>
       <c r="O39" s="77">
-        <f t="shared" ref="O39" si="145">O12-N12</f>
+        <f t="shared" ref="O39" si="152">O12-N12</f>
         <v>14</v>
       </c>
       <c r="P39" s="77">
-        <f t="shared" ref="P39:T39" si="146">P12-O12</f>
+        <f t="shared" ref="P39:T39" si="153">P12-O12</f>
         <v>9</v>
       </c>
       <c r="Q39" s="77">
-        <f t="shared" si="146"/>
+        <f t="shared" si="153"/>
         <v>16</v>
       </c>
       <c r="R39" s="77">
-        <f t="shared" si="146"/>
+        <f t="shared" si="153"/>
         <v>6</v>
       </c>
       <c r="S39" s="77">
-        <f t="shared" si="146"/>
+        <f t="shared" si="153"/>
         <v>11</v>
       </c>
       <c r="T39" s="77">
-        <f t="shared" si="146"/>
+        <f t="shared" si="153"/>
         <v>10</v>
       </c>
       <c r="U39" s="77">
-        <f t="shared" ref="U39" si="147">U12-T12</f>
+        <f t="shared" ref="U39" si="154">U12-T12</f>
         <v>30</v>
       </c>
       <c r="V39" s="77">
-        <f t="shared" ref="V39" si="148">V12-U12</f>
+        <f t="shared" ref="V39" si="155">V12-U12</f>
         <v>7</v>
       </c>
       <c r="W39" s="77">
-        <f t="shared" ref="W39" si="149">W12-V12</f>
+        <f t="shared" ref="W39" si="156">W12-V12</f>
         <v>17</v>
       </c>
       <c r="X39" s="77">
-        <f t="shared" ref="X39" si="150">X12-W12</f>
+        <f t="shared" ref="X39" si="157">X12-W12</f>
         <v>15</v>
       </c>
-      <c r="Z39" s="59" t="s">
-        <v>186</v>
+      <c r="Y39" s="77">
+        <f t="shared" ref="Y39" si="158">Y12-X12</f>
+        <v>30</v>
       </c>
       <c r="AA39" s="59" t="s">
         <v>186</v>
@@ -29516,11 +29657,14 @@
       <c r="AG39" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AH39" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="40" spans="1:33" ht="12.75" customHeight="1">
-      <c r="AG40" s="24"/>
+    <row r="40" spans="1:34" ht="12.75" customHeight="1">
+      <c r="AH40" s="24"/>
     </row>
-    <row r="41" spans="1:33" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="41" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>213</v>
       </c>
@@ -29537,51 +29681,51 @@
         <v>186</v>
       </c>
       <c r="F41" s="31">
-        <f t="shared" ref="F41" si="151">F21/B21-1</f>
+        <f t="shared" ref="F41" si="159">F21/B21-1</f>
         <v>-0.14726840855106893</v>
       </c>
       <c r="G41" s="31">
-        <f t="shared" ref="G41" si="152">G21/C21-1</f>
+        <f t="shared" ref="G41" si="160">G21/C21-1</f>
         <v>8.3333333333333037E-3</v>
       </c>
       <c r="H41" s="31">
-        <f t="shared" ref="H41" si="153">H21/D21-1</f>
+        <f t="shared" ref="H41" si="161">H21/D21-1</f>
         <v>0.3745019920318724</v>
       </c>
       <c r="I41" s="31">
-        <f t="shared" ref="I41" si="154">I21/E21-1</f>
+        <f t="shared" ref="I41" si="162">I21/E21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
       <c r="J41" s="31">
-        <f t="shared" ref="J41" si="155">J21/F21-1</f>
+        <f t="shared" ref="J41" si="163">J21/F21-1</f>
         <v>-0.11420612813370479</v>
       </c>
       <c r="K41" s="31">
-        <f t="shared" ref="K41" si="156">K21/G21-1</f>
+        <f t="shared" ref="K41" si="164">K21/G21-1</f>
         <v>-0.13498622589531684</v>
       </c>
       <c r="L41" s="31">
-        <f t="shared" ref="L41" si="157">L21/H21-1</f>
+        <f t="shared" ref="L41" si="165">L21/H21-1</f>
         <v>-0.11014492753623184</v>
       </c>
       <c r="M41" s="31">
-        <f t="shared" ref="M41" si="158">M21/I21-1</f>
+        <f t="shared" ref="M41" si="166">M21/I21-1</f>
         <v>-0.16863905325443784</v>
       </c>
       <c r="N41" s="31">
-        <f t="shared" ref="N41" si="159">N21/J21-1</f>
+        <f t="shared" ref="N41" si="167">N21/J21-1</f>
         <v>-0.14465408805031443</v>
       </c>
       <c r="O41" s="31">
-        <f t="shared" ref="O41" si="160">O21/K21-1</f>
+        <f t="shared" ref="O41" si="168">O21/K21-1</f>
         <v>-2.5477707006369421E-2</v>
       </c>
       <c r="P41" s="31">
-        <f t="shared" ref="P41" si="161">P21/L21-1</f>
+        <f t="shared" ref="P41" si="169">P21/L21-1</f>
         <v>1.9543973941368087E-2</v>
       </c>
       <c r="Q41" s="31">
-        <f t="shared" ref="Q41" si="162">Q21/M21-1</f>
+        <f t="shared" ref="Q41" si="170">Q21/M21-1</f>
         <v>0.15658362989323837</v>
       </c>
       <c r="R41" s="31">
@@ -29589,62 +29733,66 @@
         <v>0.15808823529411775</v>
       </c>
       <c r="S41" s="31">
-        <f t="shared" ref="S41:T41" si="163">S21/O21-1</f>
+        <f t="shared" ref="S41:T41" si="171">S21/O21-1</f>
         <v>1.9607843137254832E-2</v>
       </c>
       <c r="T41" s="31">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>-5.1118210862619806E-2</v>
       </c>
       <c r="U41" s="31">
-        <f t="shared" ref="U41" si="164">U21/Q21-1</f>
+        <f t="shared" ref="U41" si="172">U21/Q21-1</f>
         <v>-0.10461538461538467</v>
       </c>
       <c r="V41" s="31">
-        <f t="shared" ref="V41" si="165">V21/R21-1</f>
+        <f t="shared" ref="V41" si="173">V21/R21-1</f>
         <v>-0.10793650793650789</v>
       </c>
       <c r="W41" s="31">
-        <f t="shared" ref="W41" si="166">W21/S21-1</f>
+        <f t="shared" ref="W41" si="174">W21/S21-1</f>
         <v>-0.13141025641025639</v>
       </c>
       <c r="X41" s="31">
-        <f t="shared" ref="X41" si="167">X21/T21-1</f>
+        <f t="shared" ref="X41" si="175">X21/T21-1</f>
         <v>-2.0202020202020221E-2</v>
       </c>
-      <c r="Z41" s="59" t="s">
+      <c r="Y41" s="31">
+        <f t="shared" ref="Y41" si="176">Y21/U21-1</f>
+        <v>2.405498281786933E-2</v>
+      </c>
+      <c r="AA41" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="AA41" s="31">
-        <f t="shared" ref="AA41" si="168">AA21/Z21-1</f>
+      <c r="AB41" s="31">
+        <f t="shared" ref="AB41" si="177">AB21/AA21-1</f>
         <v>0.11764705882352944</v>
       </c>
-      <c r="AB41" s="31">
-        <f t="shared" ref="AB41" si="169">AB21/AA21-1</f>
+      <c r="AC41" s="31">
+        <f t="shared" ref="AC41" si="178">AC21/AB21-1</f>
         <v>-0.1228070175438597</v>
       </c>
-      <c r="AC41" s="31">
-        <f t="shared" ref="AC41" si="170">AC21/AB21-1</f>
+      <c r="AD41" s="31">
+        <f t="shared" ref="AD41" si="179">AD21/AC21-1</f>
         <v>-3.3333333333333326E-2</v>
       </c>
-      <c r="AD41" s="31">
-        <f t="shared" ref="AD41" si="171">AD21/AC21-1</f>
+      <c r="AE41" s="31">
+        <f t="shared" ref="AE41" si="180">AE21/AD21-1</f>
         <v>-0.15402298850574714</v>
       </c>
-      <c r="AE41" s="31">
-        <f t="shared" ref="AE41" si="172">AE21/AD21-1</f>
+      <c r="AF41" s="31">
+        <f t="shared" ref="AF41" si="181">AF21/AE21-1</f>
         <v>-8.1521739130434812E-2</v>
-      </c>
-      <c r="AF41" s="31">
-        <f>AF21/AE21-1</f>
-        <v>-0.16863905325443784</v>
       </c>
       <c r="AG41" s="31">
         <f>AG21/AF21-1</f>
+        <v>-0.16863905325443784</v>
+      </c>
+      <c r="AH41" s="31">
+        <f>AH21/AG21-1</f>
         <v>0.15658362989323837</v>
       </c>
     </row>
-    <row r="42" spans="1:33" s="80" customFormat="1" ht="12.75" customHeight="1">
+    <row r="42" spans="1:34" s="80" customFormat="1" ht="12.75" customHeight="1">
       <c r="A42" s="84" t="s">
         <v>213</v>
       </c>
@@ -29661,31 +29809,31 @@
         <v>186</v>
       </c>
       <c r="F42" s="80">
-        <f t="shared" ref="F42" si="173">F21-B21</f>
+        <f t="shared" ref="F42" si="182">F21-B21</f>
         <v>-62</v>
       </c>
       <c r="G42" s="80">
-        <f t="shared" ref="G42" si="174">G21-C21</f>
+        <f t="shared" ref="G42" si="183">G21-C21</f>
         <v>3</v>
       </c>
       <c r="H42" s="80">
-        <f t="shared" ref="H42" si="175">H21-D21</f>
+        <f t="shared" ref="H42" si="184">H21-D21</f>
         <v>94</v>
       </c>
       <c r="I42" s="80">
-        <f t="shared" ref="I42:L42" si="176">I21-E21</f>
+        <f t="shared" ref="I42:L42" si="185">I21-E21</f>
         <v>-30</v>
       </c>
       <c r="J42" s="80">
-        <f t="shared" si="176"/>
+        <f t="shared" si="185"/>
         <v>-41</v>
       </c>
       <c r="K42" s="80">
-        <f t="shared" si="176"/>
+        <f t="shared" si="185"/>
         <v>-49</v>
       </c>
       <c r="L42" s="80">
-        <f t="shared" si="176"/>
+        <f t="shared" si="185"/>
         <v>-38</v>
       </c>
       <c r="M42" s="80">
@@ -29693,23 +29841,23 @@
         <v>-57</v>
       </c>
       <c r="N42" s="80">
-        <f t="shared" ref="N42" si="177">N21-J21</f>
+        <f t="shared" ref="N42" si="186">N21-J21</f>
         <v>-46</v>
       </c>
       <c r="O42" s="80">
-        <f t="shared" ref="O42" si="178">O21-K21</f>
+        <f t="shared" ref="O42" si="187">O21-K21</f>
         <v>-8</v>
       </c>
       <c r="P42" s="80">
-        <f t="shared" ref="P42" si="179">P21-L21</f>
+        <f t="shared" ref="P42" si="188">P21-L21</f>
         <v>6</v>
       </c>
       <c r="Q42" s="80">
-        <f t="shared" ref="Q42:R42" si="180">Q21-M21</f>
+        <f t="shared" ref="Q42:R42" si="189">Q21-M21</f>
         <v>44</v>
       </c>
       <c r="R42" s="80">
-        <f t="shared" si="180"/>
+        <f t="shared" si="189"/>
         <v>43</v>
       </c>
       <c r="S42" s="80">
@@ -29721,54 +29869,58 @@
         <v>-16</v>
       </c>
       <c r="U42" s="80">
-        <f t="shared" ref="U42" si="181">U21-Q21</f>
+        <f t="shared" ref="U42" si="190">U21-Q21</f>
         <v>-34</v>
       </c>
       <c r="V42" s="80">
-        <f t="shared" ref="V42" si="182">V21-R21</f>
+        <f t="shared" ref="V42" si="191">V21-R21</f>
         <v>-34</v>
       </c>
       <c r="W42" s="80">
-        <f t="shared" ref="W42" si="183">W21-S21</f>
+        <f t="shared" ref="W42" si="192">W21-S21</f>
         <v>-41</v>
       </c>
       <c r="X42" s="80">
-        <f t="shared" ref="X42" si="184">X21-T21</f>
+        <f t="shared" ref="X42" si="193">X21-T21</f>
         <v>-6</v>
       </c>
-      <c r="Z42" s="59" t="s">
+      <c r="Y42" s="80">
+        <f t="shared" ref="Y42" si="194">Y21-U21</f>
+        <v>7</v>
+      </c>
+      <c r="AA42" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="AA42" s="80">
-        <f t="shared" ref="AA42" si="185">AA21-Z21</f>
+      <c r="AB42" s="80">
+        <f t="shared" ref="AB42" si="195">AB21-AA21</f>
         <v>54</v>
       </c>
-      <c r="AB42" s="80">
-        <f t="shared" ref="AB42" si="186">AB21-AA21</f>
+      <c r="AC42" s="80">
+        <f t="shared" ref="AC42" si="196">AC21-AB21</f>
         <v>-63</v>
       </c>
-      <c r="AC42" s="80">
-        <f t="shared" ref="AC42" si="187">AC21-AB21</f>
+      <c r="AD42" s="80">
+        <f t="shared" ref="AD42" si="197">AD21-AC21</f>
         <v>-15</v>
       </c>
-      <c r="AD42" s="80">
-        <f t="shared" ref="AD42" si="188">AD21-AC21</f>
+      <c r="AE42" s="80">
+        <f t="shared" ref="AE42" si="198">AE21-AD21</f>
         <v>-67</v>
       </c>
-      <c r="AE42" s="80">
-        <f t="shared" ref="AE42:AF42" si="189">AE21-AD21</f>
+      <c r="AF42" s="80">
+        <f t="shared" ref="AF42:AG42" si="199">AF21-AE21</f>
         <v>-30</v>
       </c>
-      <c r="AF42" s="80">
-        <f t="shared" si="189"/>
+      <c r="AG42" s="80">
+        <f t="shared" si="199"/>
         <v>-57</v>
       </c>
-      <c r="AG42" s="80">
-        <f>AG21-AF21</f>
+      <c r="AH42" s="80">
+        <f>AH21-AG21</f>
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="12.75" customHeight="1">
+    <row r="43" spans="1:34" ht="12.75" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>214</v>
       </c>
@@ -29776,63 +29928,63 @@
         <v>186</v>
       </c>
       <c r="C43" s="24">
-        <f t="shared" ref="C43" si="190">C21/B21-1</f>
+        <f t="shared" ref="C43" si="200">C21/B21-1</f>
         <v>-0.14489311163895491</v>
       </c>
       <c r="D43" s="24">
-        <f t="shared" ref="D43" si="191">D21/C21-1</f>
+        <f t="shared" ref="D43" si="201">D21/C21-1</f>
         <v>-0.30277777777777781</v>
       </c>
       <c r="E43" s="24">
-        <f t="shared" ref="E43" si="192">E21/D21-1</f>
+        <f t="shared" ref="E43" si="202">E21/D21-1</f>
         <v>0.46613545816733071</v>
       </c>
       <c r="F43" s="24">
-        <f t="shared" ref="F43" si="193">F21/E21-1</f>
+        <f t="shared" ref="F43" si="203">F21/E21-1</f>
         <v>-2.4456521739130488E-2</v>
       </c>
       <c r="G43" s="24">
-        <f t="shared" ref="G43" si="194">G21/F21-1</f>
+        <f t="shared" ref="G43" si="204">G21/F21-1</f>
         <v>1.1142061281337101E-2</v>
       </c>
       <c r="H43" s="24">
-        <f t="shared" ref="H43" si="195">H21/G21-1</f>
+        <f t="shared" ref="H43" si="205">H21/G21-1</f>
         <v>-4.9586776859504078E-2</v>
       </c>
       <c r="I43" s="24">
-        <f t="shared" ref="I43" si="196">I21/H21-1</f>
+        <f t="shared" ref="I43" si="206">I21/H21-1</f>
         <v>-2.0289855072463725E-2</v>
       </c>
       <c r="J43" s="24">
-        <f t="shared" ref="J43" si="197">J21/I21-1</f>
+        <f t="shared" ref="J43" si="207">J21/I21-1</f>
         <v>-5.9171597633136064E-2</v>
       </c>
       <c r="K43" s="24">
-        <f t="shared" ref="K43" si="198">K21/J21-1</f>
+        <f t="shared" ref="K43" si="208">K21/J21-1</f>
         <v>-1.2578616352201255E-2</v>
       </c>
       <c r="L43" s="24">
-        <f t="shared" ref="L43" si="199">L21/K21-1</f>
+        <f t="shared" ref="L43" si="209">L21/K21-1</f>
         <v>-2.2292993630573243E-2</v>
       </c>
       <c r="M43" s="24">
-        <f t="shared" ref="M43" si="200">M21/L21-1</f>
+        <f t="shared" ref="M43" si="210">M21/L21-1</f>
         <v>-8.4690553745928376E-2</v>
       </c>
       <c r="N43" s="24">
-        <f t="shared" ref="N43" si="201">N21/M21-1</f>
+        <f t="shared" ref="N43" si="211">N21/M21-1</f>
         <v>-3.2028469750889688E-2</v>
       </c>
       <c r="O43" s="24">
-        <f t="shared" ref="O43" si="202">O21/N21-1</f>
+        <f t="shared" ref="O43" si="212">O21/N21-1</f>
         <v>0.125</v>
       </c>
       <c r="P43" s="24">
-        <f t="shared" ref="P43" si="203">P21/O21-1</f>
+        <f t="shared" ref="P43" si="213">P21/O21-1</f>
         <v>2.2875816993463971E-2</v>
       </c>
       <c r="Q43" s="24">
-        <f t="shared" ref="Q43" si="204">Q21/P21-1</f>
+        <f t="shared" ref="Q43" si="214">Q21/P21-1</f>
         <v>3.833865814696491E-2</v>
       </c>
       <c r="R43" s="24">
@@ -29840,31 +29992,32 @@
         <v>-3.0769230769230771E-2</v>
       </c>
       <c r="S43" s="24">
-        <f t="shared" ref="S43:T43" si="205">S21/R21-1</f>
+        <f t="shared" ref="S43:T43" si="215">S21/R21-1</f>
         <v>-9.52380952380949E-3</v>
       </c>
       <c r="T43" s="24">
-        <f t="shared" si="205"/>
+        <f t="shared" si="215"/>
         <v>-4.8076923076923128E-2</v>
       </c>
       <c r="U43" s="24">
-        <f t="shared" ref="U43" si="206">U21/T21-1</f>
+        <f t="shared" ref="U43" si="216">U21/T21-1</f>
         <v>-2.0202020202020221E-2</v>
       </c>
       <c r="V43" s="24">
-        <f t="shared" ref="V43" si="207">V21/U21-1</f>
+        <f t="shared" ref="V43" si="217">V21/U21-1</f>
         <v>-3.4364261168384869E-2</v>
       </c>
       <c r="W43" s="24">
-        <f t="shared" ref="W43" si="208">W21/V21-1</f>
+        <f t="shared" ref="W43" si="218">W21/V21-1</f>
         <v>-3.5587188612099641E-2</v>
       </c>
       <c r="X43" s="24">
-        <f t="shared" ref="X43" si="209">X21/W21-1</f>
+        <f t="shared" ref="X43" si="219">X21/W21-1</f>
         <v>7.3800738007380184E-2</v>
       </c>
-      <c r="Z43" s="59" t="s">
-        <v>186</v>
+      <c r="Y43" s="24">
+        <f t="shared" ref="Y43" si="220">Y21/X21-1</f>
+        <v>2.405498281786933E-2</v>
       </c>
       <c r="AA43" s="59" t="s">
         <v>186</v>
@@ -29887,8 +30040,11 @@
       <c r="AG43" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AH43" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="44" spans="1:33" s="79" customFormat="1" ht="12.75" customHeight="1">
+    <row r="44" spans="1:34" s="79" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" s="83" t="s">
         <v>214</v>
       </c>
@@ -29896,67 +30052,67 @@
         <v>186</v>
       </c>
       <c r="C44" s="77">
-        <f t="shared" ref="C44" si="210">C21-B21</f>
+        <f t="shared" ref="C44" si="221">C21-B21</f>
         <v>-61</v>
       </c>
       <c r="D44" s="77">
-        <f t="shared" ref="D44" si="211">D21-C21</f>
+        <f t="shared" ref="D44" si="222">D21-C21</f>
         <v>-109</v>
       </c>
       <c r="E44" s="77">
-        <f t="shared" ref="E44" si="212">E21-D21</f>
+        <f t="shared" ref="E44" si="223">E21-D21</f>
         <v>117</v>
       </c>
       <c r="F44" s="77">
-        <f t="shared" ref="F44" si="213">F21-E21</f>
+        <f t="shared" ref="F44" si="224">F21-E21</f>
         <v>-9</v>
       </c>
       <c r="G44" s="77">
-        <f t="shared" ref="G44" si="214">G21-F21</f>
+        <f t="shared" ref="G44" si="225">G21-F21</f>
         <v>4</v>
       </c>
       <c r="H44" s="77">
-        <f t="shared" ref="H44" si="215">H21-G21</f>
+        <f t="shared" ref="H44" si="226">H21-G21</f>
         <v>-18</v>
       </c>
       <c r="I44" s="77">
-        <f t="shared" ref="I44" si="216">I21-H21</f>
+        <f t="shared" ref="I44" si="227">I21-H21</f>
         <v>-7</v>
       </c>
       <c r="J44" s="77">
-        <f t="shared" ref="J44" si="217">J21-I21</f>
+        <f t="shared" ref="J44" si="228">J21-I21</f>
         <v>-20</v>
       </c>
       <c r="K44" s="77">
-        <f t="shared" ref="K44" si="218">K21-J21</f>
+        <f t="shared" ref="K44" si="229">K21-J21</f>
         <v>-4</v>
       </c>
       <c r="L44" s="77">
-        <f t="shared" ref="L44" si="219">L21-K21</f>
+        <f t="shared" ref="L44" si="230">L21-K21</f>
         <v>-7</v>
       </c>
       <c r="M44" s="77">
-        <f t="shared" ref="M44" si="220">M21-L21</f>
+        <f t="shared" ref="M44" si="231">M21-L21</f>
         <v>-26</v>
       </c>
       <c r="N44" s="77">
-        <f t="shared" ref="N44" si="221">N21-M21</f>
+        <f t="shared" ref="N44" si="232">N21-M21</f>
         <v>-9</v>
       </c>
       <c r="O44" s="77">
-        <f t="shared" ref="O44" si="222">O21-N21</f>
+        <f t="shared" ref="O44" si="233">O21-N21</f>
         <v>34</v>
       </c>
       <c r="P44" s="77">
-        <f t="shared" ref="P44:R44" si="223">P21-O21</f>
+        <f t="shared" ref="P44:R44" si="234">P21-O21</f>
         <v>7</v>
       </c>
       <c r="Q44" s="77">
-        <f t="shared" si="223"/>
+        <f t="shared" si="234"/>
         <v>12</v>
       </c>
       <c r="R44" s="77">
-        <f t="shared" si="223"/>
+        <f t="shared" si="234"/>
         <v>-10</v>
       </c>
       <c r="S44" s="77">
@@ -29968,23 +30124,24 @@
         <v>-15</v>
       </c>
       <c r="U44" s="77">
-        <f t="shared" ref="U44" si="224">U21-T21</f>
+        <f t="shared" ref="U44" si="235">U21-T21</f>
         <v>-6</v>
       </c>
       <c r="V44" s="77">
-        <f t="shared" ref="V44" si="225">V21-U21</f>
+        <f t="shared" ref="V44" si="236">V21-U21</f>
         <v>-10</v>
       </c>
       <c r="W44" s="77">
-        <f t="shared" ref="W44" si="226">W21-V21</f>
+        <f t="shared" ref="W44" si="237">W21-V21</f>
         <v>-10</v>
       </c>
       <c r="X44" s="77">
-        <f t="shared" ref="X44" si="227">X21-W21</f>
+        <f t="shared" ref="X44" si="238">X21-W21</f>
         <v>20</v>
       </c>
-      <c r="Z44" s="59" t="s">
-        <v>186</v>
+      <c r="Y44" s="77">
+        <f t="shared" ref="Y44" si="239">Y21-X21</f>
+        <v>7</v>
       </c>
       <c r="AA44" s="59" t="s">
         <v>186</v>
@@ -30007,81 +30164,84 @@
       <c r="AG44" s="59" t="s">
         <v>186</v>
       </c>
+      <c r="AH44" s="59" t="s">
+        <v>186</v>
+      </c>
     </row>
-    <row r="46" spans="1:33" ht="12.75" customHeight="1">
+    <row r="46" spans="1:34" ht="12.75" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B46" s="24">
-        <f t="shared" ref="B46:S46" si="228">B12/B3</f>
+        <f t="shared" ref="B46:S46" si="240">B12/B3</f>
         <v>0.77057220708446872</v>
       </c>
       <c r="C46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.80022197558268593</v>
       </c>
       <c r="D46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.85304449648711944</v>
       </c>
       <c r="E46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.80193756727664156</v>
       </c>
       <c r="F46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.80698924731182797</v>
       </c>
       <c r="G46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.80793650793650795</v>
       </c>
       <c r="H46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.81736368448914765</v>
       </c>
       <c r="I46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.82368283776734486</v>
       </c>
       <c r="J46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.83280757097791802</v>
       </c>
       <c r="K46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.83491062039957942</v>
       </c>
       <c r="L46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.83859095688748686</v>
       </c>
       <c r="M46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.85241596638655459</v>
       </c>
       <c r="N46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="O46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.84323770491803274</v>
       </c>
       <c r="P46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.84095528455284552</v>
       </c>
       <c r="Q46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.83717434869739482</v>
       </c>
       <c r="R46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.8418674698795181</v>
       </c>
       <c r="S46" s="24">
-        <f t="shared" si="228"/>
+        <f t="shared" si="240"/>
         <v>0.84399999999999997</v>
       </c>
       <c r="T46" s="24">
@@ -30089,55 +30249,59 @@
         <v>0.85112781954887218</v>
       </c>
       <c r="U46" s="24">
-        <f t="shared" ref="U46:X46" si="229">U12/U3</f>
+        <f t="shared" ref="U46:Y46" si="241">U12/U3</f>
         <v>0.85586924219910843</v>
       </c>
       <c r="V46" s="24">
-        <f t="shared" si="229"/>
+        <f t="shared" si="241"/>
         <v>0.86061507936507942</v>
       </c>
       <c r="W46" s="24">
-        <f t="shared" si="229"/>
+        <f t="shared" si="241"/>
         <v>0.86604053386060309</v>
       </c>
       <c r="X46" s="24">
-        <f t="shared" si="229"/>
+        <f t="shared" si="241"/>
         <v>0.85860058309037901</v>
       </c>
-      <c r="Z46" s="24">
-        <f t="shared" ref="Z46:AG46" si="230">Z12/Z3</f>
+      <c r="Y46" s="24">
+        <f t="shared" si="241"/>
+        <v>0.85980861244019136</v>
+      </c>
+      <c r="AA46" s="24">
+        <f t="shared" ref="AA46:AH46" si="242">AA12/AA3</f>
         <v>0.70367979341510656</v>
       </c>
-      <c r="AA46" s="24">
-        <f t="shared" si="230"/>
+      <c r="AB46" s="24">
+        <f t="shared" si="242"/>
         <v>0.693075117370892</v>
       </c>
-      <c r="AB46" s="24">
-        <f t="shared" si="230"/>
+      <c r="AC46" s="24">
+        <f t="shared" si="242"/>
         <v>0.74271012006861059</v>
       </c>
-      <c r="AC46" s="24">
-        <f t="shared" si="230"/>
+      <c r="AD46" s="24">
+        <f t="shared" si="242"/>
         <v>0.76294277929155319</v>
       </c>
-      <c r="AD46" s="24">
-        <f t="shared" si="230"/>
+      <c r="AE46" s="24">
+        <f t="shared" si="242"/>
         <v>0.80193756727664156</v>
       </c>
-      <c r="AE46" s="24">
-        <f t="shared" si="230"/>
+      <c r="AF46" s="24">
+        <f t="shared" si="242"/>
         <v>0.82368283776734486</v>
       </c>
-      <c r="AF46" s="24">
-        <f t="shared" si="230"/>
+      <c r="AG46" s="24">
+        <f t="shared" si="242"/>
         <v>0.85241596638655459</v>
       </c>
-      <c r="AG46" s="24">
-        <f t="shared" si="230"/>
+      <c r="AH46" s="24">
+        <f t="shared" si="242"/>
         <v>0.83717434869739482</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="12.75" customHeight="1">
+    <row r="47" spans="1:34" ht="12.75" customHeight="1">
       <c r="N47" s="72"/>
     </row>
     <row r="49" spans="14:14" ht="12.75" customHeight="1">
@@ -30151,15 +30315,15 @@
     <hyperlink ref="N1" r:id="rId4" xr:uid="{9287A329-D88E-784B-8BDF-1EDA927EB785}"/>
     <hyperlink ref="S1" r:id="rId5" xr:uid="{6AF4C14B-B6A4-FE47-B0D3-A570A390AD5C}"/>
     <hyperlink ref="O1" r:id="rId6" xr:uid="{0A17F8BF-EADB-DE42-994D-117A4F2CB3FE}"/>
-    <hyperlink ref="AG1" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
+    <hyperlink ref="AH1" r:id="rId7" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/282b37b7-69b6-46c3-86f1-3d03bb11cc0e?origin=1" xr:uid="{9A635200-D40C-2C47-BF87-74A9C3DCF160}"/>
     <hyperlink ref="M1" r:id="rId8" xr:uid="{F1748A46-ECC6-544E-9D30-C00CF38C6CF7}"/>
-    <hyperlink ref="AF1" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
-    <hyperlink ref="AE1" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
+    <hyperlink ref="AG1" r:id="rId9" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/631b88c4-9ae6-429c-98d6-230db8273d60?origin=1" xr:uid="{D9538A1F-7DBB-FA44-9BE7-595A80C2AFB9}"/>
+    <hyperlink ref="AF1" r:id="rId10" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/2b63fed1-515f-4f82-a272-84c564557830?origin=1" xr:uid="{D1A1F548-67B5-7A4D-985A-0DFAFE22EBD5}"/>
     <hyperlink ref="I1" r:id="rId11" xr:uid="{998E2907-64B9-7A44-8D65-8083912D2D62}"/>
     <hyperlink ref="E1" r:id="rId12" xr:uid="{5D689E99-05ED-E34E-9D87-28B9F22988C9}"/>
-    <hyperlink ref="AD1" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
-    <hyperlink ref="AC1" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
-    <hyperlink ref="AB1" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
+    <hyperlink ref="AE1" r:id="rId13" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/38d6b5b1-73e3-4d7d-aca3-84a2d5bbf813?origin=1" xr:uid="{6F460F9A-C5E5-A44E-8E60-30FD06C106C2}"/>
+    <hyperlink ref="AD1" r:id="rId14" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/ed568644-a6d5-4205-a73d-0b3221ad8c90?origin=1" xr:uid="{753E2A88-CB41-C94C-B023-B46ED8394A35}"/>
+    <hyperlink ref="AC1" r:id="rId15" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/3dfd5b58-8699-43d1-850f-8f68d67c11ee?origin=1" xr:uid="{B50E4D75-D405-DD4B-9E35-C517F0E7814A}"/>
     <hyperlink ref="L1" r:id="rId16" xr:uid="{E0D344DF-ECD3-4969-946B-75165895949D}"/>
     <hyperlink ref="K1" r:id="rId17" xr:uid="{34FDBE06-551B-4817-B842-42B3C369DE44}"/>
     <hyperlink ref="J1" r:id="rId18" xr:uid="{8672DEA7-6978-4CBC-A339-3D96580B25F6}"/>
@@ -30169,16 +30333,17 @@
     <hyperlink ref="D1" r:id="rId22" xr:uid="{9AA615B1-70E4-40CE-8BD9-FA369F45AAE7}"/>
     <hyperlink ref="C1" r:id="rId23" xr:uid="{B190BD40-76B4-4C45-B1D6-B5043307E3B6}"/>
     <hyperlink ref="B1" r:id="rId24" xr:uid="{2E883042-0703-4781-AC08-6A8AD2EAD4EB}"/>
-    <hyperlink ref="AA1" r:id="rId25" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/93a33ec4-dc07-47b3-91c2-d84b2e56d699?origin=1" xr:uid="{CE32064C-B077-40F4-9C44-3F45FE0A2ECE}"/>
-    <hyperlink ref="Z1" r:id="rId26" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a574642d-6cd1-4e80-a242-26ff2d0747f5?origin=1" xr:uid="{4A9206DD-D830-44D0-A5B0-DF41E9DD8391}"/>
+    <hyperlink ref="AB1" r:id="rId25" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/93a33ec4-dc07-47b3-91c2-d84b2e56d699?origin=1" xr:uid="{CE32064C-B077-40F4-9C44-3F45FE0A2ECE}"/>
+    <hyperlink ref="AA1" r:id="rId26" display="https://api.mziq.com/mzfilemanager/v2/d/12a56b3a-7b37-4dba-b80a-f3358bf66b71/a574642d-6cd1-4e80-a242-26ff2d0747f5?origin=1" xr:uid="{4A9206DD-D830-44D0-A5B0-DF41E9DD8391}"/>
     <hyperlink ref="T1" r:id="rId27" xr:uid="{F6F821CD-3C9C-4984-B9E1-54EA40AA851B}"/>
     <hyperlink ref="U1" r:id="rId28" xr:uid="{8A371147-4AFA-4AEF-811C-DCBC2CB2AA7E}"/>
     <hyperlink ref="V1" r:id="rId29" xr:uid="{1B3B2092-CF63-4E8C-950C-B7238A4569EE}"/>
     <hyperlink ref="W1" r:id="rId30" xr:uid="{B722A3C9-0371-455C-8877-C5E990ECEA22}"/>
     <hyperlink ref="X1" r:id="rId31" xr:uid="{283E1A1A-52A4-4BB0-826A-A775C26A1BB9}"/>
+    <hyperlink ref="Y1" r:id="rId32" xr:uid="{BFADB3EB-4CC0-410D-8F60-5F3AFC3EA622}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId32"/>
-  <drawing r:id="rId33"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId33"/>
+  <drawing r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
$ERJ pre Q423 updates
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2BD900-8890-4A3C-8FAA-DE0871BC5806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9B8AEC-603E-4397-B3F1-1A1EA29F993B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="195" yWindow="2010" windowWidth="26610" windowHeight="12885" activeTab="1" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="307">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1091,6 +1091,9 @@
   </si>
   <si>
     <t>American Airlines place order for up to 90 Embraer E175 jets</t>
+  </si>
+  <si>
+    <t>E2 Jets are approved for ETOPS-120 flight operations allowing for longer flights over water or rural areas</t>
   </si>
 </sst>
 </file>
@@ -1641,10 +1644,37 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1656,33 +1686,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1690,12 +1693,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1716,25 +1713,31 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9537,10 +9540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC73"/>
+  <dimension ref="A2:AC75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9560,49 +9563,49 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="113"/>
-      <c r="G5" s="111" t="s">
+      <c r="C5" s="121"/>
+      <c r="D5" s="122"/>
+      <c r="G5" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="113"/>
-      <c r="T5" s="111" t="s">
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="122"/>
+      <c r="T5" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="113"/>
-      <c r="AA5" s="109" t="s">
+      <c r="U5" s="121"/>
+      <c r="V5" s="121"/>
+      <c r="W5" s="122"/>
+      <c r="AA5" s="132" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="110"/>
+      <c r="AB5" s="133"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>21.75</v>
+        <v>23.33</v>
       </c>
       <c r="D6" s="17"/>
       <c r="G6" s="8">
         <v>44986</v>
       </c>
       <c r="H6" s="94" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
@@ -9663,14 +9666,14 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>15977.550000000001</v>
+        <v>17138.218000000001</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
-        <v>45261</v>
+        <v>44986</v>
       </c>
       <c r="H8" s="94" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
@@ -9733,10 +9736,10 @@
         <v>300</v>
       </c>
       <c r="G10" s="8">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="H10" s="94" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -9791,14 +9794,14 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>17177.25</v>
+        <v>18337.918000000001</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="H12" s="94" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -9814,13 +9817,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="111" t="s">
+      <c r="Y12" s="120" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="112"/>
-      <c r="AA12" s="112"/>
-      <c r="AB12" s="112"/>
-      <c r="AC12" s="113"/>
+      <c r="Z12" s="121"/>
+      <c r="AA12" s="121"/>
+      <c r="AB12" s="121"/>
+      <c r="AC12" s="122"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -9842,21 +9845,21 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="126" t="s">
+      <c r="Z13" s="118" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="126"/>
-      <c r="AB13" s="126" t="s">
+      <c r="AA13" s="118"/>
+      <c r="AB13" s="118" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="127"/>
+      <c r="AC13" s="119"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="H14" s="94" t="s">
-        <v>272</v>
+        <v>298</v>
       </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
@@ -9877,21 +9880,21 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="116" t="s">
+      <c r="Z14" s="115" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="116"/>
-      <c r="AB14" s="116" t="s">
+      <c r="AA14" s="115"/>
+      <c r="AB14" s="115" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="117"/>
+      <c r="AC14" s="114"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="112"/>
-      <c r="D15" s="113"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="122"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -9913,14 +9916,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="116" t="s">
+      <c r="Z15" s="115" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="116"/>
-      <c r="AB15" s="116" t="s">
+      <c r="AA15" s="115"/>
+      <c r="AB15" s="115" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="117"/>
+      <c r="AC15" s="114"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -9929,18 +9932,18 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="117"/>
+      <c r="D16" s="114"/>
       <c r="E16" s="3" t="s">
         <v>303</v>
       </c>
       <c r="G16" s="8">
-        <v>45017</v>
+        <v>45170</v>
       </c>
       <c r="H16" s="94" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
@@ -9961,23 +9964,23 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="116" t="s">
+      <c r="Z16" s="115" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="116"/>
-      <c r="AB16" s="116" t="s">
+      <c r="AA16" s="115"/>
+      <c r="AB16" s="115" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="117"/>
+      <c r="AC16" s="114"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="117"/>
+      <c r="D17" s="114"/>
       <c r="E17" s="3" t="s">
         <v>303</v>
       </c>
@@ -10000,24 +10003,24 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="116" t="s">
+      <c r="Z17" s="115" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="116"/>
-      <c r="AB17" s="116" t="s">
+      <c r="AA17" s="115"/>
+      <c r="AB17" s="115" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="117"/>
+      <c r="AC17" s="114"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="117"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="114"/>
       <c r="G18" s="8">
         <v>45017</v>
       </c>
-      <c r="H18" s="100" t="s">
-        <v>268</v>
+      <c r="H18" s="94" t="s">
+        <v>271</v>
       </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
@@ -10038,19 +10041,19 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="116" t="s">
+      <c r="Z18" s="115" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="116"/>
-      <c r="AB18" s="116" t="s">
+      <c r="AA18" s="115"/>
+      <c r="AB18" s="115" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="117"/>
+      <c r="AC18" s="114"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="137"/>
       <c r="G19" s="9"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -10072,21 +10075,21 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="116" t="s">
+      <c r="Z19" s="115" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="116"/>
-      <c r="AB19" s="116" t="s">
+      <c r="AA19" s="115"/>
+      <c r="AB19" s="115" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="117"/>
+      <c r="AC19" s="114"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="8">
-        <v>44927</v>
-      </c>
-      <c r="H20" s="96" t="s">
-        <v>265</v>
+        <v>45017</v>
+      </c>
+      <c r="H20" s="100" t="s">
+        <v>268</v>
       </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
@@ -10107,14 +10110,14 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="116" t="s">
+      <c r="Z20" s="115" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="116"/>
-      <c r="AB20" s="116" t="s">
+      <c r="AA20" s="115"/>
+      <c r="AB20" s="115" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="117"/>
+      <c r="AC20" s="114"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -10142,16 +10145,16 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="112"/>
-      <c r="D22" s="113"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="122"/>
       <c r="G22" s="8">
-        <v>44896</v>
-      </c>
-      <c r="H22" s="94" t="s">
-        <v>263</v>
+        <v>44927</v>
+      </c>
+      <c r="H22" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
@@ -10179,10 +10182,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="115" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="117"/>
+      <c r="D23" s="114"/>
       <c r="G23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -10204,15 +10207,15 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="116">
+      <c r="C24" s="115">
         <v>1969</v>
       </c>
-      <c r="D24" s="117"/>
+      <c r="D24" s="114"/>
       <c r="G24" s="8">
-        <v>44866</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>261</v>
+        <v>44896</v>
+      </c>
+      <c r="H24" s="94" t="s">
+        <v>263</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
@@ -10233,8 +10236,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="117"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="114"/>
       <c r="G25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -10253,28 +10256,28 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="120" t="s">
+      <c r="Y25" s="138" t="s">
         <v>288</v>
       </c>
-      <c r="Z25" s="121"/>
-      <c r="AA25" s="121"/>
-      <c r="AB25" s="121"/>
-      <c r="AC25" s="122"/>
+      <c r="Z25" s="139"/>
+      <c r="AA25" s="139"/>
+      <c r="AB25" s="139"/>
+      <c r="AC25" s="140"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="114">
+      <c r="C26" s="134">
         <f>'Financial Model'!Y68</f>
         <v>3053.1</v>
       </c>
-      <c r="D26" s="115"/>
+      <c r="D26" s="135"/>
       <c r="G26" s="8">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
@@ -10302,8 +10305,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="117"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="114"/>
       <c r="G27" s="9"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -10334,13 +10337,17 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="134">
+      <c r="C28" s="113">
         <f>+'Order &amp; Backlog'!$X$3</f>
         <v>2058</v>
       </c>
-      <c r="D28" s="117"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="34"/>
+      <c r="D28" s="114"/>
+      <c r="G28" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="I28" s="34"/>
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
@@ -10369,17 +10376,13 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="134">
+      <c r="C29" s="113">
         <f>'Order &amp; Backlog'!X21</f>
         <v>291</v>
       </c>
-      <c r="D29" s="117"/>
-      <c r="G29" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D29" s="114"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
@@ -10406,15 +10409,13 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="116">
+      <c r="C30" s="115">
         <f>'Financial Model'!Y43</f>
         <v>43</v>
       </c>
-      <c r="D30" s="117"/>
+      <c r="D30" s="114"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
@@ -10441,13 +10442,15 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="135">
+      <c r="C31" s="116">
         <v>36708</v>
       </c>
-      <c r="D31" s="136"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="7" t="s">
-        <v>13</v>
+      <c r="D31" s="117"/>
+      <c r="G31" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
@@ -10475,10 +10478,12 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="116"/>
-      <c r="D32" s="117"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="114"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="34"/>
+      <c r="H32" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
       <c r="K32" s="34"/>
@@ -10512,11 +10517,9 @@
         <f>+'Financial Model'!Y3</f>
         <v>45236</v>
       </c>
-      <c r="G33" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>29</v>
+      <c r="G33" s="9"/>
+      <c r="H33" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
@@ -10544,14 +10547,12 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="130" t="s">
+      <c r="C34" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="131"/>
+      <c r="D34" s="129"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="H34" s="34"/>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
       <c r="K34" s="34"/>
@@ -10575,8 +10576,12 @@
       <c r="AC34" s="35"/>
     </row>
     <row r="35" spans="2:29">
-      <c r="G35" s="9"/>
-      <c r="H35" s="34"/>
+      <c r="G35" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="I35" s="34"/>
       <c r="J35" s="34"/>
       <c r="K35" s="34"/>
@@ -10597,7 +10602,9 @@
     </row>
     <row r="36" spans="2:29">
       <c r="G36" s="9"/>
-      <c r="H36" s="34"/>
+      <c r="H36" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
@@ -10615,17 +10622,13 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="111" t="s">
+      <c r="B37" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="112"/>
-      <c r="D37" s="113"/>
-      <c r="G37" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>187</v>
-      </c>
+      <c r="C37" s="121"/>
+      <c r="D37" s="122"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="34"/>
       <c r="I37" s="34"/>
       <c r="J37" s="34"/>
       <c r="K37" s="34"/>
@@ -10636,12 +10639,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="111" t="s">
+      <c r="T37" s="120" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="112"/>
-      <c r="V37" s="112"/>
-      <c r="W37" s="113"/>
+      <c r="U37" s="121"/>
+      <c r="V37" s="121"/>
+      <c r="W37" s="122"/>
       <c r="Y37" s="39" t="s">
         <v>280</v>
       </c>
@@ -10654,11 +10657,11 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="132">
+      <c r="C38" s="130">
         <f>C6/'Financial Model'!Y123</f>
-        <v>5.7152489626556031</v>
-      </c>
-      <c r="D38" s="133"/>
+        <v>6.1304256689082859</v>
+      </c>
+      <c r="D38" s="131"/>
       <c r="G38" s="9"/>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
@@ -10689,13 +10692,17 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="132">
+      <c r="C39" s="130">
         <f>C8/SUM('Financial Model'!X9:Y9)</f>
-        <v>6.2007800675282345</v>
-      </c>
-      <c r="D39" s="133"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="34"/>
+        <v>6.6512275391004003</v>
+      </c>
+      <c r="D39" s="131"/>
+      <c r="G39" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="I39" s="34"/>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -10722,17 +10729,13 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="128">
+      <c r="C40" s="126">
         <f>C6/SUM('Financial Model'!X26:Y26)</f>
-        <v>378.6149289099526</v>
-      </c>
-      <c r="D40" s="129"/>
-      <c r="G40" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>195</v>
-      </c>
+        <v>406.1189099526066</v>
+      </c>
+      <c r="D40" s="127"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="34"/>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
       <c r="K40" s="34"/>
@@ -10757,9 +10760,7 @@
     </row>
     <row r="41" spans="2:29">
       <c r="G41" s="9"/>
-      <c r="H41" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="H41" s="34"/>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
@@ -10783,9 +10784,11 @@
       <c r="AC41" s="35"/>
     </row>
     <row r="42" spans="2:29">
-      <c r="G42" s="9"/>
-      <c r="H42" s="7" t="s">
-        <v>193</v>
+      <c r="G42" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
@@ -10808,14 +10811,14 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="111" t="s">
+      <c r="B43" s="120" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="112"/>
-      <c r="D43" s="113"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="122"/>
       <c r="G43" s="9"/>
       <c r="H43" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
@@ -10826,9 +10829,7 @@
       <c r="O43" s="34"/>
       <c r="P43" s="34"/>
       <c r="Q43" s="34"/>
-      <c r="R43" s="48" t="s">
-        <v>194</v>
-      </c>
+      <c r="R43" s="35"/>
       <c r="T43" s="39" t="s">
         <v>159</v>
       </c>
@@ -10844,15 +10845,17 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="137" t="s">
+      <c r="B44" s="109" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="138"/>
+      <c r="C44" s="110"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
       <c r="G44" s="9"/>
-      <c r="H44" s="34"/>
+      <c r="H44" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="I44" s="34"/>
       <c r="J44" s="34"/>
       <c r="K44" s="34"/>
@@ -10878,15 +10881,17 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="137" t="s">
+      <c r="B45" s="109" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="138"/>
+      <c r="C45" s="110"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
       <c r="G45" s="9"/>
-      <c r="H45" s="34"/>
+      <c r="H45" s="7" t="s">
+        <v>191</v>
+      </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
       <c r="K45" s="34"/>
@@ -10896,7 +10901,9 @@
       <c r="O45" s="34"/>
       <c r="P45" s="34"/>
       <c r="Q45" s="34"/>
-      <c r="R45" s="35"/>
+      <c r="R45" s="48" t="s">
+        <v>194</v>
+      </c>
       <c r="T45" s="41" t="s">
         <v>161</v>
       </c>
@@ -10912,17 +10919,13 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="137"/>
-      <c r="C46" s="138"/>
+      <c r="B46" s="109"/>
+      <c r="C46" s="110"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>196</v>
-      </c>
+      <c r="G46" s="9"/>
+      <c r="H46" s="34"/>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
@@ -10944,15 +10947,13 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="137"/>
-      <c r="C47" s="138"/>
+      <c r="B47" s="109"/>
+      <c r="C47" s="110"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
       <c r="G47" s="9"/>
-      <c r="H47" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="H47" s="34"/>
       <c r="I47" s="34"/>
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
@@ -10978,14 +10979,16 @@
       <c r="AC47" s="35"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="139"/>
-      <c r="C48" s="140"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="112"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="47" t="s">
-        <v>198</v>
+      <c r="G48" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
@@ -11013,7 +11016,9 @@
     </row>
     <row r="49" spans="7:29">
       <c r="G49" s="9"/>
-      <c r="H49" s="34"/>
+      <c r="H49" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
@@ -11039,11 +11044,9 @@
       <c r="AC49" s="35"/>
     </row>
     <row r="50" spans="7:29">
-      <c r="G50" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>239</v>
+      <c r="G50" s="9"/>
+      <c r="H50" s="47" t="s">
+        <v>198</v>
       </c>
       <c r="I50" s="34"/>
       <c r="J50" s="34"/>
@@ -11065,9 +11068,7 @@
     </row>
     <row r="51" spans="7:29">
       <c r="G51" s="9"/>
-      <c r="H51" s="7" t="s">
-        <v>240</v>
-      </c>
+      <c r="H51" s="34"/>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
@@ -11087,8 +11088,12 @@
       <c r="AC51" s="35"/>
     </row>
     <row r="52" spans="7:29">
-      <c r="G52" s="9"/>
-      <c r="H52" s="34"/>
+      <c r="G52" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>239</v>
+      </c>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
       <c r="K52" s="34"/>
@@ -11106,11 +11111,9 @@
       <c r="AC52" s="35"/>
     </row>
     <row r="53" spans="7:29">
-      <c r="G53" s="8">
-        <v>44682</v>
-      </c>
-      <c r="H53" s="34" t="s">
-        <v>248</v>
+      <c r="G53" s="9"/>
+      <c r="H53" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="I53" s="34"/>
       <c r="J53" s="34"/>
@@ -11132,9 +11135,7 @@
     </row>
     <row r="54" spans="7:29">
       <c r="G54" s="9"/>
-      <c r="H54" s="7" t="s">
-        <v>249</v>
-      </c>
+      <c r="H54" s="34"/>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
       <c r="K54" s="34"/>
@@ -11144,9 +11145,7 @@
       <c r="O54" s="34"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="34"/>
-      <c r="R54" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R54" s="35"/>
       <c r="Y54" s="102" t="s">
         <v>293</v>
       </c>
@@ -11156,8 +11155,12 @@
       <c r="AC54" s="35"/>
     </row>
     <row r="55" spans="7:29">
-      <c r="G55" s="9"/>
-      <c r="H55" s="34"/>
+      <c r="G55" s="8">
+        <v>44682</v>
+      </c>
+      <c r="H55" s="34" t="s">
+        <v>248</v>
+      </c>
       <c r="I55" s="34"/>
       <c r="J55" s="34"/>
       <c r="K55" s="34"/>
@@ -11177,11 +11180,9 @@
       <c r="AC55" s="35"/>
     </row>
     <row r="56" spans="7:29">
-      <c r="G56" s="8">
-        <v>43922</v>
-      </c>
-      <c r="H56" s="34" t="s">
-        <v>164</v>
+      <c r="G56" s="9"/>
+      <c r="H56" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
@@ -11192,7 +11193,9 @@
       <c r="O56" s="34"/>
       <c r="P56" s="34"/>
       <c r="Q56" s="34"/>
-      <c r="R56" s="35"/>
+      <c r="R56" s="48" t="s">
+        <v>31</v>
+      </c>
       <c r="Y56" s="39"/>
       <c r="Z56" s="34"/>
       <c r="AA56" s="34"/>
@@ -11201,9 +11204,7 @@
     </row>
     <row r="57" spans="7:29">
       <c r="G57" s="9"/>
-      <c r="H57" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="H57" s="34"/>
       <c r="I57" s="34"/>
       <c r="J57" s="34"/>
       <c r="K57" s="34"/>
@@ -11221,8 +11222,12 @@
       <c r="AC57" s="105"/>
     </row>
     <row r="58" spans="7:29">
-      <c r="G58" s="9"/>
-      <c r="H58" s="34"/>
+      <c r="G58" s="8">
+        <v>43922</v>
+      </c>
+      <c r="H58" s="34" t="s">
+        <v>164</v>
+      </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
@@ -11232,9 +11237,7 @@
       <c r="O58" s="34"/>
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
-      <c r="R58" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R58" s="35"/>
       <c r="Y58" s="123" t="s">
         <v>295</v>
       </c>
@@ -11245,7 +11248,9 @@
     </row>
     <row r="59" spans="7:29">
       <c r="G59" s="9"/>
-      <c r="H59" s="34"/>
+      <c r="H59" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="I59" s="34"/>
       <c r="J59" s="34"/>
       <c r="K59" s="34"/>
@@ -11258,12 +11263,8 @@
       <c r="R59" s="35"/>
     </row>
     <row r="60" spans="7:29">
-      <c r="G60" s="8">
-        <v>43770</v>
-      </c>
-      <c r="H60" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="34"/>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
       <c r="K60" s="34"/>
@@ -11273,13 +11274,13 @@
       <c r="O60" s="34"/>
       <c r="P60" s="34"/>
       <c r="Q60" s="34"/>
-      <c r="R60" s="35"/>
+      <c r="R60" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="61" spans="7:29">
       <c r="G61" s="9"/>
-      <c r="H61" s="47" t="s">
-        <v>168</v>
-      </c>
+      <c r="H61" s="34"/>
       <c r="I61" s="34"/>
       <c r="J61" s="34"/>
       <c r="K61" s="34"/>
@@ -11292,8 +11293,12 @@
       <c r="R61" s="35"/>
     </row>
     <row r="62" spans="7:29">
-      <c r="G62" s="9"/>
-      <c r="H62" s="34"/>
+      <c r="G62" s="8">
+        <v>43770</v>
+      </c>
+      <c r="H62" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
       <c r="K62" s="34"/>
@@ -11306,11 +11311,9 @@
       <c r="R62" s="35"/>
     </row>
     <row r="63" spans="7:29">
-      <c r="G63" s="8">
-        <v>43739</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>244</v>
+      <c r="G63" s="9"/>
+      <c r="H63" s="47" t="s">
+        <v>168</v>
       </c>
       <c r="I63" s="34"/>
       <c r="J63" s="34"/>
@@ -11320,9 +11323,7 @@
       <c r="N63" s="34"/>
       <c r="O63" s="34"/>
       <c r="P63" s="34"/>
-      <c r="Q63" s="34" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q63" s="34"/>
       <c r="R63" s="35"/>
     </row>
     <row r="64" spans="7:29">
@@ -11340,8 +11341,12 @@
       <c r="R64" s="35"/>
     </row>
     <row r="65" spans="7:18">
-      <c r="G65" s="9"/>
-      <c r="H65" s="34"/>
+      <c r="G65" s="8">
+        <v>43739</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>244</v>
+      </c>
       <c r="I65" s="34"/>
       <c r="J65" s="34"/>
       <c r="K65" s="34"/>
@@ -11350,7 +11355,9 @@
       <c r="N65" s="34"/>
       <c r="O65" s="34"/>
       <c r="P65" s="34"/>
-      <c r="Q65" s="34"/>
+      <c r="Q65" s="34" t="s">
+        <v>179</v>
+      </c>
       <c r="R65" s="35"/>
     </row>
     <row r="66" spans="7:18">
@@ -11368,12 +11375,8 @@
       <c r="R66" s="35"/>
     </row>
     <row r="67" spans="7:18">
-      <c r="G67" s="8">
-        <v>43586</v>
-      </c>
-      <c r="H67" s="34" t="s">
-        <v>166</v>
-      </c>
+      <c r="G67" s="9"/>
+      <c r="H67" s="34"/>
       <c r="I67" s="34"/>
       <c r="J67" s="34"/>
       <c r="K67" s="34"/>
@@ -11401,10 +11404,10 @@
     </row>
     <row r="69" spans="7:18">
       <c r="G69" s="8">
-        <v>43282</v>
+        <v>43586</v>
       </c>
       <c r="H69" s="34" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I69" s="34"/>
       <c r="J69" s="34"/>
@@ -11419,9 +11422,7 @@
     </row>
     <row r="70" spans="7:18">
       <c r="G70" s="9"/>
-      <c r="H70" s="7" t="s">
-        <v>163</v>
-      </c>
+      <c r="H70" s="34"/>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>
       <c r="K70" s="34"/>
@@ -11434,9 +11435,11 @@
       <c r="R70" s="35"/>
     </row>
     <row r="71" spans="7:18">
-      <c r="G71" s="9"/>
-      <c r="H71" s="7" t="s">
-        <v>165</v>
+      <c r="G71" s="8">
+        <v>43282</v>
+      </c>
+      <c r="H71" s="34" t="s">
+        <v>162</v>
       </c>
       <c r="I71" s="34"/>
       <c r="J71" s="34"/>
@@ -11451,7 +11454,9 @@
     </row>
     <row r="72" spans="7:18">
       <c r="G72" s="9"/>
-      <c r="H72" s="34"/>
+      <c r="H72" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="I72" s="34"/>
       <c r="J72" s="34"/>
       <c r="K72" s="34"/>
@@ -11464,44 +11469,71 @@
       <c r="R72" s="35"/>
     </row>
     <row r="73" spans="7:18">
-      <c r="G73" s="87">
+      <c r="G73" s="9"/>
+      <c r="H73" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I73" s="34"/>
+      <c r="J73" s="34"/>
+      <c r="K73" s="34"/>
+      <c r="L73" s="34"/>
+      <c r="M73" s="34"/>
+      <c r="N73" s="34"/>
+      <c r="O73" s="34"/>
+      <c r="P73" s="34"/>
+      <c r="Q73" s="34"/>
+      <c r="R73" s="35"/>
+    </row>
+    <row r="74" spans="7:18">
+      <c r="G74" s="9"/>
+      <c r="H74" s="34"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="34"/>
+      <c r="K74" s="34"/>
+      <c r="L74" s="34"/>
+      <c r="M74" s="34"/>
+      <c r="N74" s="34"/>
+      <c r="O74" s="34"/>
+      <c r="P74" s="34"/>
+      <c r="Q74" s="34"/>
+      <c r="R74" s="35"/>
+    </row>
+    <row r="75" spans="7:18">
+      <c r="G75" s="87">
         <v>42552</v>
       </c>
-      <c r="H73" s="51" t="s">
+      <c r="H75" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="I73" s="32"/>
-      <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
-      <c r="M73" s="32"/>
-      <c r="N73" s="32"/>
-      <c r="O73" s="32"/>
-      <c r="P73" s="32"/>
-      <c r="Q73" s="32"/>
-      <c r="R73" s="33"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="32"/>
+      <c r="K75" s="32"/>
+      <c r="L75" s="32"/>
+      <c r="M75" s="32"/>
+      <c r="N75" s="32"/>
+      <c r="O75" s="32"/>
+      <c r="P75" s="32"/>
+      <c r="Q75" s="32"/>
+      <c r="R75" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Y25:AC25"/>
     <mergeCell ref="Y58:AC58"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="Z16:AA16"/>
@@ -11518,56 +11550,60 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H29" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H33" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="H31" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H35" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C34:D34" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R58" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H37" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H40" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R43" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H46" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="R60" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H39" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H42" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R45" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H48" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
     <hyperlink ref="W49" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
     <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
     <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
-    <hyperlink ref="H50" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H63" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="H52" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H65" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
     <hyperlink ref="D45" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D44" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
-    <hyperlink ref="R54" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H26" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
-    <hyperlink ref="H24" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
-    <hyperlink ref="H22" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
-    <hyperlink ref="H20" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
-    <hyperlink ref="H18" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
-    <hyperlink ref="H16" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
-    <hyperlink ref="H14" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
+    <hyperlink ref="R56" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H28" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H26" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
+    <hyperlink ref="H24" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
+    <hyperlink ref="H22" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
+    <hyperlink ref="H20" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
+    <hyperlink ref="H18" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="H16" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
     <hyperlink ref="Y25:AC25" r:id="rId24" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
-    <hyperlink ref="H8" r:id="rId25" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
-    <hyperlink ref="H10" r:id="rId26" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
-    <hyperlink ref="H12" r:id="rId27" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
-    <hyperlink ref="H6" r:id="rId28" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
+    <hyperlink ref="H10" r:id="rId25" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
+    <hyperlink ref="H12" r:id="rId26" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
+    <hyperlink ref="H14" r:id="rId27" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
+    <hyperlink ref="H8" r:id="rId28" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
+    <hyperlink ref="H6" r:id="rId29" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId29"/>
-  <drawing r:id="rId30"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId30"/>
+  <drawing r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -11575,11 +11611,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D70B2A-3077-4926-AE7B-39AF91889CD9}">
   <dimension ref="B1:AS148"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W148" sqref="W148"/>
+      <selection pane="bottomRight" activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -11664,6 +11700,9 @@
       <c r="Y1" s="23" t="s">
         <v>300</v>
       </c>
+      <c r="Z1" s="14" t="s">
+        <v>304</v>
+      </c>
       <c r="AB1" s="14" t="s">
         <v>251</v>
       </c>
@@ -12483,6 +12522,10 @@
         <f t="shared" si="1"/>
         <v>1284.4000000000001</v>
       </c>
+      <c r="Z9" s="25">
+        <f>AK9-SUM(W9:Y9)</f>
+        <v>1701.0399999999995</v>
+      </c>
       <c r="AB9" s="25">
         <v>6288.8</v>
       </c>
@@ -14031,6 +14074,10 @@
         <f t="shared" si="12"/>
         <v>64.300000000000125</v>
       </c>
+      <c r="Z23" s="25">
+        <f>Z9*0.02</f>
+        <v>34.020799999999994</v>
+      </c>
       <c r="AB23" s="25">
         <f t="shared" ref="AB23:AG23" si="13">AB21-AB22</f>
         <v>347.7</v>
@@ -14593,8 +14640,12 @@
         <v>0.26832858965551076</v>
       </c>
       <c r="Y30" s="31">
-        <f t="shared" ref="Y30" si="23">Y9/U9-1</f>
+        <f t="shared" ref="Y30:Z30" si="23">Y9/U9-1</f>
         <v>0.38256189451022604</v>
+      </c>
+      <c r="Z30" s="31">
+        <f t="shared" si="23"/>
+        <v>-0.14589274954810227</v>
       </c>
       <c r="AB30" s="59" t="s">
         <v>186</v>
@@ -14728,8 +14779,12 @@
         <v>0.80312543602623143</v>
       </c>
       <c r="Y31" s="24">
-        <f t="shared" ref="Y31" si="46">Y9/X9-1</f>
+        <f t="shared" ref="Y31:Z31" si="46">Y9/X9-1</f>
         <v>-6.113131625783419E-3</v>
+      </c>
+      <c r="Z31" s="24">
+        <f t="shared" si="46"/>
+        <v>0.32438492681407616</v>
       </c>
       <c r="AB31" s="59" t="s">
         <v>186</v>
@@ -26012,7 +26067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1F7BB5-1110-4DCF-A4D2-2BD3A135983C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
$ERJ LOT leasing news
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E7BD55-C4B9-4445-A0BC-6FA148BB4840}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C63C0AD-3429-4DE1-8ADF-9A1A4B852DD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="2010" windowWidth="26610" windowHeight="12885" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="312">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1122,6 +1122,9 @@
   <si>
     <t>WSJ claim that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade</t>
   </si>
+  <si>
+    <t>Polish LOT airline has reached a lease agreement for 3 E195-E2 units in anticipation of an order of up to 84 jets</t>
+  </si>
 </sst>
 </file>
 
@@ -1689,10 +1692,39 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1702,33 +1734,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1758,35 +1763,33 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9779,10 +9782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC80"/>
+  <dimension ref="A2:AC82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9802,35 +9805,35 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="113"/>
-      <c r="G5" s="111" t="s">
+      <c r="C5" s="123"/>
+      <c r="D5" s="124"/>
+      <c r="G5" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="113"/>
-      <c r="T5" s="111" t="s">
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="123"/>
+      <c r="O5" s="123"/>
+      <c r="P5" s="123"/>
+      <c r="Q5" s="123"/>
+      <c r="R5" s="124"/>
+      <c r="T5" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="113"/>
-      <c r="AA5" s="109" t="s">
+      <c r="U5" s="123"/>
+      <c r="V5" s="123"/>
+      <c r="W5" s="124"/>
+      <c r="AA5" s="134" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="110"/>
+      <c r="AB5" s="135"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -9878,7 +9881,7 @@
         <v>45413</v>
       </c>
       <c r="H7" s="94" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
@@ -9941,10 +9944,10 @@
         <v>308</v>
       </c>
       <c r="G9" s="8">
-        <v>44986</v>
+        <v>45413</v>
       </c>
       <c r="H9" s="94" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -10008,7 +10011,7 @@
         <v>44986</v>
       </c>
       <c r="H11" s="94" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -10052,20 +10055,20 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="111" t="s">
+      <c r="Y12" s="122" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="112"/>
-      <c r="AA12" s="112"/>
-      <c r="AB12" s="112"/>
-      <c r="AC12" s="113"/>
+      <c r="Z12" s="123"/>
+      <c r="AA12" s="123"/>
+      <c r="AB12" s="123"/>
+      <c r="AC12" s="124"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="8">
         <v>44986</v>
       </c>
       <c r="H13" s="94" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
@@ -10084,14 +10087,14 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="135" t="s">
+      <c r="Z13" s="120" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="135"/>
-      <c r="AB13" s="135" t="s">
+      <c r="AA13" s="120"/>
+      <c r="AB13" s="120" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="136"/>
+      <c r="AC13" s="121"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="9"/>
@@ -10115,26 +10118,26 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="116" t="s">
+      <c r="Z14" s="117" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="116"/>
-      <c r="AB14" s="116" t="s">
+      <c r="AA14" s="117"/>
+      <c r="AB14" s="117" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="117"/>
+      <c r="AC14" s="116"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="112"/>
-      <c r="D15" s="113"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="124"/>
       <c r="G15" s="8">
-        <v>45261</v>
+        <v>44986</v>
       </c>
       <c r="H15" s="94" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
@@ -10155,14 +10158,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="116" t="s">
+      <c r="Z15" s="117" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="116"/>
-      <c r="AB15" s="116" t="s">
+      <c r="AA15" s="117"/>
+      <c r="AB15" s="117" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="117"/>
+      <c r="AC15" s="116"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -10171,10 +10174,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="117"/>
+      <c r="D16" s="116"/>
       <c r="E16" s="3" t="s">
         <v>303</v>
       </c>
@@ -10199,31 +10202,31 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="116" t="s">
+      <c r="Z16" s="117" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="116"/>
-      <c r="AB16" s="116" t="s">
+      <c r="AA16" s="117"/>
+      <c r="AB16" s="117" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="117"/>
+      <c r="AC16" s="116"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="117"/>
+      <c r="D17" s="116"/>
       <c r="E17" s="3" t="s">
         <v>303</v>
       </c>
       <c r="G17" s="8">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="H17" s="94" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
@@ -10242,19 +10245,19 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="116" t="s">
+      <c r="Z17" s="117" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="116"/>
-      <c r="AB17" s="116" t="s">
+      <c r="AA17" s="117"/>
+      <c r="AB17" s="117" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="117"/>
+      <c r="AC17" s="116"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="117"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="116"/>
       <c r="G18" s="9"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
@@ -10276,24 +10279,24 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="116" t="s">
+      <c r="Z18" s="117" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="116"/>
-      <c r="AB18" s="116" t="s">
+      <c r="AA18" s="117"/>
+      <c r="AB18" s="117" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="117"/>
+      <c r="AC18" s="116"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="139"/>
       <c r="G19" s="8">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="H19" s="94" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
@@ -10314,14 +10317,14 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="116" t="s">
+      <c r="Z19" s="117" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="116"/>
-      <c r="AB19" s="116" t="s">
+      <c r="AA19" s="117"/>
+      <c r="AB19" s="117" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="117"/>
+      <c r="AC19" s="116"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="9"/>
@@ -10345,21 +10348,21 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="116" t="s">
+      <c r="Z20" s="117" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="116"/>
-      <c r="AB20" s="116" t="s">
+      <c r="AA20" s="117"/>
+      <c r="AB20" s="117" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="117"/>
+      <c r="AC20" s="116"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="8">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="H21" s="94" t="s">
-        <v>272</v>
+        <v>298</v>
       </c>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
@@ -10384,11 +10387,11 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="112"/>
-      <c r="D22" s="113"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="124"/>
       <c r="G22" s="9"/>
       <c r="H22" s="34"/>
       <c r="I22" s="34"/>
@@ -10417,15 +10420,15 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="117" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="117"/>
+      <c r="D23" s="116"/>
       <c r="G23" s="8">
-        <v>45017</v>
+        <v>45170</v>
       </c>
       <c r="H23" s="94" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
@@ -10446,10 +10449,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="116">
+      <c r="C24" s="117">
         <v>1969</v>
       </c>
-      <c r="D24" s="117"/>
+      <c r="D24" s="116"/>
       <c r="G24" s="9"/>
       <c r="H24" s="34"/>
       <c r="I24" s="34"/>
@@ -10471,13 +10474,13 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="117"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="116"/>
       <c r="G25" s="8">
         <v>45017</v>
       </c>
-      <c r="H25" s="100" t="s">
-        <v>268</v>
+      <c r="H25" s="94" t="s">
+        <v>271</v>
       </c>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
@@ -10495,23 +10498,23 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="120" t="s">
+      <c r="Y25" s="140" t="s">
         <v>288</v>
       </c>
-      <c r="Z25" s="121"/>
-      <c r="AA25" s="121"/>
-      <c r="AB25" s="121"/>
-      <c r="AC25" s="122"/>
+      <c r="Z25" s="141"/>
+      <c r="AA25" s="141"/>
+      <c r="AB25" s="141"/>
+      <c r="AC25" s="142"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="114">
+      <c r="C26" s="136">
         <f>'Financial Model'!Z68</f>
         <v>2636</v>
       </c>
-      <c r="D26" s="115"/>
+      <c r="D26" s="137"/>
       <c r="G26" s="9"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
@@ -10540,13 +10543,13 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="116"/>
       <c r="G27" s="8">
-        <v>44927</v>
-      </c>
-      <c r="H27" s="96" t="s">
-        <v>265</v>
+        <v>45017</v>
+      </c>
+      <c r="H27" s="100" t="s">
+        <v>268</v>
       </c>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
@@ -10576,11 +10579,11 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="132">
+      <c r="C28" s="115">
         <f>+'Order &amp; Backlog'!$Z$3</f>
         <v>2180</v>
       </c>
-      <c r="D28" s="117"/>
+      <c r="D28" s="116"/>
       <c r="G28" s="9"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
@@ -10611,16 +10614,16 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="132">
+      <c r="C29" s="115">
         <f>'Order &amp; Backlog'!Z21</f>
         <v>381</v>
       </c>
-      <c r="D29" s="117"/>
+      <c r="D29" s="116"/>
       <c r="G29" s="8">
-        <v>44896</v>
-      </c>
-      <c r="H29" s="94" t="s">
-        <v>263</v>
+        <v>44927</v>
+      </c>
+      <c r="H29" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="I29" s="34"/>
       <c r="J29" s="34"/>
@@ -10648,11 +10651,11 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="116">
+      <c r="C30" s="117">
         <f>'Financial Model'!AA43</f>
         <v>25</v>
       </c>
-      <c r="D30" s="117"/>
+      <c r="D30" s="116"/>
       <c r="G30" s="9"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
@@ -10681,15 +10684,15 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="139">
+      <c r="C31" s="118">
         <v>36708</v>
       </c>
-      <c r="D31" s="140"/>
+      <c r="D31" s="119"/>
       <c r="G31" s="8">
-        <v>44866</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>261</v>
+        <v>44896</v>
+      </c>
+      <c r="H31" s="94" t="s">
+        <v>263</v>
       </c>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
@@ -10717,8 +10720,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="116"/>
-      <c r="D32" s="117"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="116"/>
       <c r="G32" s="9"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
@@ -10754,10 +10757,10 @@
         <v>45419</v>
       </c>
       <c r="G33" s="8">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
@@ -10785,10 +10788,10 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="128" t="s">
+      <c r="C34" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="129"/>
+      <c r="D34" s="131"/>
       <c r="G34" s="9"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
@@ -10814,8 +10817,12 @@
       <c r="AC34" s="35"/>
     </row>
     <row r="35" spans="2:29">
-      <c r="G35" s="9"/>
-      <c r="H35" s="34"/>
+      <c r="G35" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="I35" s="34"/>
       <c r="J35" s="34"/>
       <c r="K35" s="34"/>
@@ -10835,12 +10842,8 @@
       <c r="AC35" s="35"/>
     </row>
     <row r="36" spans="2:29">
-      <c r="G36" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="34"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
@@ -10858,15 +10861,13 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="111" t="s">
+      <c r="B37" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="112"/>
-      <c r="D37" s="113"/>
+      <c r="C37" s="123"/>
+      <c r="D37" s="124"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="H37" s="34"/>
       <c r="I37" s="34"/>
       <c r="J37" s="34"/>
       <c r="K37" s="34"/>
@@ -10877,12 +10878,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="111" t="s">
+      <c r="T37" s="122" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="112"/>
-      <c r="V37" s="112"/>
-      <c r="W37" s="113"/>
+      <c r="U37" s="123"/>
+      <c r="V37" s="123"/>
+      <c r="W37" s="124"/>
       <c r="Y37" s="39" t="s">
         <v>280</v>
       </c>
@@ -10895,14 +10896,16 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="130">
+      <c r="C38" s="132">
         <f>C6/'Financial Model'!AA123</f>
         <v>6.2876718272359708</v>
       </c>
-      <c r="D38" s="131"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="7" t="s">
-        <v>13</v>
+      <c r="D38" s="133"/>
+      <c r="G38" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -10932,13 +10935,15 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="130">
+      <c r="C39" s="132">
         <f>+C8/SUM('Financial Model'!X4:AA4)</f>
         <v>10.347262400605832</v>
       </c>
-      <c r="D39" s="131"/>
+      <c r="D39" s="133"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="34"/>
+      <c r="H39" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="I39" s="34"/>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -10965,16 +10970,14 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="126">
+      <c r="C40" s="128">
         <f>C6/SUM('Financial Model'!X26:AA26)</f>
         <v>72.595764705882345</v>
       </c>
-      <c r="D40" s="127"/>
-      <c r="G40" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>29</v>
+      <c r="D40" s="129"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
@@ -11000,9 +11003,7 @@
     </row>
     <row r="41" spans="2:29">
       <c r="G41" s="9"/>
-      <c r="H41" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="H41" s="34"/>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
@@ -11026,8 +11027,12 @@
       <c r="AC41" s="35"/>
     </row>
     <row r="42" spans="2:29">
-      <c r="G42" s="9"/>
-      <c r="H42" s="34"/>
+      <c r="G42" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
       <c r="K42" s="34"/>
@@ -11049,13 +11054,15 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="111" t="s">
+      <c r="B43" s="122" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="112"/>
-      <c r="D43" s="113"/>
+      <c r="C43" s="123"/>
+      <c r="D43" s="124"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="34"/>
+      <c r="H43" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
       <c r="K43" s="34"/>
@@ -11081,19 +11088,15 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="133" t="s">
+      <c r="B44" s="111" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="134"/>
+      <c r="C44" s="112"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>187</v>
-      </c>
+      <c r="G44" s="9"/>
+      <c r="H44" s="34"/>
       <c r="I44" s="34"/>
       <c r="J44" s="34"/>
       <c r="K44" s="34"/>
@@ -11119,10 +11122,10 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="133" t="s">
+      <c r="B45" s="111" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="134"/>
+      <c r="C45" s="112"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
@@ -11153,13 +11156,17 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="133"/>
-      <c r="C46" s="134"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="112"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="34"/>
+      <c r="G46" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
@@ -11181,17 +11188,13 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="133"/>
-      <c r="C47" s="134"/>
+      <c r="B47" s="111"/>
+      <c r="C47" s="112"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="G47" s="9"/>
+      <c r="H47" s="34"/>
       <c r="I47" s="34"/>
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
@@ -11217,15 +11220,13 @@
       <c r="AC47" s="35"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="137"/>
-      <c r="C48" s="138"/>
+      <c r="B48" s="113"/>
+      <c r="C48" s="114"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="H48" s="34"/>
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
@@ -11251,9 +11252,11 @@
       <c r="AC48" s="35"/>
     </row>
     <row r="49" spans="7:29">
-      <c r="G49" s="9"/>
-      <c r="H49" s="7" t="s">
-        <v>193</v>
+      <c r="G49" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
@@ -11282,7 +11285,7 @@
     <row r="50" spans="7:29">
       <c r="G50" s="9"/>
       <c r="H50" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I50" s="34"/>
       <c r="J50" s="34"/>
@@ -11293,9 +11296,7 @@
       <c r="O50" s="34"/>
       <c r="P50" s="34"/>
       <c r="Q50" s="34"/>
-      <c r="R50" s="48" t="s">
-        <v>194</v>
-      </c>
+      <c r="R50" s="35"/>
       <c r="Y50" s="39" t="s">
         <v>290</v>
       </c>
@@ -11306,7 +11307,9 @@
     </row>
     <row r="51" spans="7:29">
       <c r="G51" s="9"/>
-      <c r="H51" s="34"/>
+      <c r="H51" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
@@ -11327,7 +11330,9 @@
     </row>
     <row r="52" spans="7:29">
       <c r="G52" s="9"/>
-      <c r="H52" s="34"/>
+      <c r="H52" s="7" t="s">
+        <v>191</v>
+      </c>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
       <c r="K52" s="34"/>
@@ -11337,7 +11342,9 @@
       <c r="O52" s="34"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="34"/>
-      <c r="R52" s="35"/>
+      <c r="R52" s="48" t="s">
+        <v>194</v>
+      </c>
       <c r="Y52" s="39"/>
       <c r="Z52" s="34"/>
       <c r="AA52" s="34"/>
@@ -11345,12 +11352,8 @@
       <c r="AC52" s="35"/>
     </row>
     <row r="53" spans="7:29">
-      <c r="G53" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>196</v>
-      </c>
+      <c r="G53" s="9"/>
+      <c r="H53" s="34"/>
       <c r="I53" s="34"/>
       <c r="J53" s="34"/>
       <c r="K53" s="34"/>
@@ -11371,9 +11374,7 @@
     </row>
     <row r="54" spans="7:29">
       <c r="G54" s="9"/>
-      <c r="H54" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="H54" s="34"/>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
       <c r="K54" s="34"/>
@@ -11393,9 +11394,11 @@
       <c r="AC54" s="35"/>
     </row>
     <row r="55" spans="7:29">
-      <c r="G55" s="9"/>
-      <c r="H55" s="47" t="s">
-        <v>198</v>
+      <c r="G55" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="I55" s="34"/>
       <c r="J55" s="34"/>
@@ -11417,7 +11420,9 @@
     </row>
     <row r="56" spans="7:29">
       <c r="G56" s="9"/>
-      <c r="H56" s="34"/>
+      <c r="H56" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
       <c r="K56" s="34"/>
@@ -11435,11 +11440,9 @@
       <c r="AC56" s="35"/>
     </row>
     <row r="57" spans="7:29">
-      <c r="G57" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>239</v>
+      <c r="G57" s="9"/>
+      <c r="H57" s="47" t="s">
+        <v>198</v>
       </c>
       <c r="I57" s="34"/>
       <c r="J57" s="34"/>
@@ -11459,9 +11462,7 @@
     </row>
     <row r="58" spans="7:29">
       <c r="G58" s="9"/>
-      <c r="H58" s="7" t="s">
-        <v>240</v>
-      </c>
+      <c r="H58" s="34"/>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
@@ -11472,17 +11473,21 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
-      <c r="Y58" s="123" t="s">
+      <c r="Y58" s="125" t="s">
         <v>295</v>
       </c>
-      <c r="Z58" s="124"/>
-      <c r="AA58" s="124"/>
-      <c r="AB58" s="124"/>
-      <c r="AC58" s="125"/>
+      <c r="Z58" s="126"/>
+      <c r="AA58" s="126"/>
+      <c r="AB58" s="126"/>
+      <c r="AC58" s="127"/>
     </row>
     <row r="59" spans="7:29">
-      <c r="G59" s="9"/>
-      <c r="H59" s="34"/>
+      <c r="G59" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>239</v>
+      </c>
       <c r="I59" s="34"/>
       <c r="J59" s="34"/>
       <c r="K59" s="34"/>
@@ -11495,11 +11500,9 @@
       <c r="R59" s="35"/>
     </row>
     <row r="60" spans="7:29">
-      <c r="G60" s="8">
-        <v>44682</v>
-      </c>
-      <c r="H60" s="34" t="s">
-        <v>248</v>
+      <c r="G60" s="9"/>
+      <c r="H60" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
@@ -11514,9 +11517,7 @@
     </row>
     <row r="61" spans="7:29">
       <c r="G61" s="9"/>
-      <c r="H61" s="7" t="s">
-        <v>249</v>
-      </c>
+      <c r="H61" s="34"/>
       <c r="I61" s="34"/>
       <c r="J61" s="34"/>
       <c r="K61" s="34"/>
@@ -11526,13 +11527,15 @@
       <c r="O61" s="34"/>
       <c r="P61" s="34"/>
       <c r="Q61" s="34"/>
-      <c r="R61" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R61" s="35"/>
     </row>
     <row r="62" spans="7:29">
-      <c r="G62" s="9"/>
-      <c r="H62" s="34"/>
+      <c r="G62" s="8">
+        <v>44682</v>
+      </c>
+      <c r="H62" s="34" t="s">
+        <v>248</v>
+      </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
       <c r="K62" s="34"/>
@@ -11545,11 +11548,9 @@
       <c r="R62" s="35"/>
     </row>
     <row r="63" spans="7:29">
-      <c r="G63" s="8">
-        <v>43922</v>
-      </c>
-      <c r="H63" s="34" t="s">
-        <v>164</v>
+      <c r="G63" s="9"/>
+      <c r="H63" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="I63" s="34"/>
       <c r="J63" s="34"/>
@@ -11560,13 +11561,13 @@
       <c r="O63" s="34"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="34"/>
-      <c r="R63" s="35"/>
+      <c r="R63" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="64" spans="7:29">
       <c r="G64" s="9"/>
-      <c r="H64" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="H64" s="34"/>
       <c r="I64" s="34"/>
       <c r="J64" s="34"/>
       <c r="K64" s="34"/>
@@ -11579,8 +11580,12 @@
       <c r="R64" s="35"/>
     </row>
     <row r="65" spans="7:18">
-      <c r="G65" s="9"/>
-      <c r="H65" s="34"/>
+      <c r="G65" s="8">
+        <v>43922</v>
+      </c>
+      <c r="H65" s="34" t="s">
+        <v>164</v>
+      </c>
       <c r="I65" s="34"/>
       <c r="J65" s="34"/>
       <c r="K65" s="34"/>
@@ -11590,13 +11595,13 @@
       <c r="O65" s="34"/>
       <c r="P65" s="34"/>
       <c r="Q65" s="34"/>
-      <c r="R65" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R65" s="35"/>
     </row>
     <row r="66" spans="7:18">
       <c r="G66" s="9"/>
-      <c r="H66" s="34"/>
+      <c r="H66" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="I66" s="34"/>
       <c r="J66" s="34"/>
       <c r="K66" s="34"/>
@@ -11609,12 +11614,8 @@
       <c r="R66" s="35"/>
     </row>
     <row r="67" spans="7:18">
-      <c r="G67" s="8">
-        <v>43770</v>
-      </c>
-      <c r="H67" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="G67" s="9"/>
+      <c r="H67" s="34"/>
       <c r="I67" s="34"/>
       <c r="J67" s="34"/>
       <c r="K67" s="34"/>
@@ -11624,13 +11625,13 @@
       <c r="O67" s="34"/>
       <c r="P67" s="34"/>
       <c r="Q67" s="34"/>
-      <c r="R67" s="35"/>
+      <c r="R67" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="68" spans="7:18">
       <c r="G68" s="9"/>
-      <c r="H68" s="47" t="s">
-        <v>168</v>
-      </c>
+      <c r="H68" s="34"/>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
       <c r="K68" s="34"/>
@@ -11643,8 +11644,12 @@
       <c r="R68" s="35"/>
     </row>
     <row r="69" spans="7:18">
-      <c r="G69" s="9"/>
-      <c r="H69" s="34"/>
+      <c r="G69" s="8">
+        <v>43770</v>
+      </c>
+      <c r="H69" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="I69" s="34"/>
       <c r="J69" s="34"/>
       <c r="K69" s="34"/>
@@ -11657,11 +11662,9 @@
       <c r="R69" s="35"/>
     </row>
     <row r="70" spans="7:18">
-      <c r="G70" s="8">
-        <v>43739</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>244</v>
+      <c r="G70" s="9"/>
+      <c r="H70" s="47" t="s">
+        <v>168</v>
       </c>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>
@@ -11671,9 +11674,7 @@
       <c r="N70" s="34"/>
       <c r="O70" s="34"/>
       <c r="P70" s="34"/>
-      <c r="Q70" s="34" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q70" s="34"/>
       <c r="R70" s="35"/>
     </row>
     <row r="71" spans="7:18">
@@ -11691,8 +11692,12 @@
       <c r="R71" s="35"/>
     </row>
     <row r="72" spans="7:18">
-      <c r="G72" s="9"/>
-      <c r="H72" s="34"/>
+      <c r="G72" s="8">
+        <v>43739</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>244</v>
+      </c>
       <c r="I72" s="34"/>
       <c r="J72" s="34"/>
       <c r="K72" s="34"/>
@@ -11701,7 +11706,9 @@
       <c r="N72" s="34"/>
       <c r="O72" s="34"/>
       <c r="P72" s="34"/>
-      <c r="Q72" s="34"/>
+      <c r="Q72" s="34" t="s">
+        <v>179</v>
+      </c>
       <c r="R72" s="35"/>
     </row>
     <row r="73" spans="7:18">
@@ -11719,12 +11726,8 @@
       <c r="R73" s="35"/>
     </row>
     <row r="74" spans="7:18">
-      <c r="G74" s="8">
-        <v>43586</v>
-      </c>
-      <c r="H74" s="34" t="s">
-        <v>166</v>
-      </c>
+      <c r="G74" s="9"/>
+      <c r="H74" s="34"/>
       <c r="I74" s="34"/>
       <c r="J74" s="34"/>
       <c r="K74" s="34"/>
@@ -11752,10 +11755,10 @@
     </row>
     <row r="76" spans="7:18">
       <c r="G76" s="8">
-        <v>43282</v>
+        <v>43586</v>
       </c>
       <c r="H76" s="34" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I76" s="34"/>
       <c r="J76" s="34"/>
@@ -11770,9 +11773,7 @@
     </row>
     <row r="77" spans="7:18">
       <c r="G77" s="9"/>
-      <c r="H77" s="7" t="s">
-        <v>163</v>
-      </c>
+      <c r="H77" s="34"/>
       <c r="I77" s="34"/>
       <c r="J77" s="34"/>
       <c r="K77" s="34"/>
@@ -11785,9 +11786,11 @@
       <c r="R77" s="35"/>
     </row>
     <row r="78" spans="7:18">
-      <c r="G78" s="9"/>
-      <c r="H78" s="7" t="s">
-        <v>165</v>
+      <c r="G78" s="8">
+        <v>43282</v>
+      </c>
+      <c r="H78" s="34" t="s">
+        <v>162</v>
       </c>
       <c r="I78" s="34"/>
       <c r="J78" s="34"/>
@@ -11802,7 +11805,9 @@
     </row>
     <row r="79" spans="7:18">
       <c r="G79" s="9"/>
-      <c r="H79" s="34"/>
+      <c r="H79" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="I79" s="34"/>
       <c r="J79" s="34"/>
       <c r="K79" s="34"/>
@@ -11815,44 +11820,71 @@
       <c r="R79" s="35"/>
     </row>
     <row r="80" spans="7:18">
-      <c r="G80" s="87">
+      <c r="G80" s="9"/>
+      <c r="H80" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I80" s="34"/>
+      <c r="J80" s="34"/>
+      <c r="K80" s="34"/>
+      <c r="L80" s="34"/>
+      <c r="M80" s="34"/>
+      <c r="N80" s="34"/>
+      <c r="O80" s="34"/>
+      <c r="P80" s="34"/>
+      <c r="Q80" s="34"/>
+      <c r="R80" s="35"/>
+    </row>
+    <row r="81" spans="7:18">
+      <c r="G81" s="9"/>
+      <c r="H81" s="34"/>
+      <c r="I81" s="34"/>
+      <c r="J81" s="34"/>
+      <c r="K81" s="34"/>
+      <c r="L81" s="34"/>
+      <c r="M81" s="34"/>
+      <c r="N81" s="34"/>
+      <c r="O81" s="34"/>
+      <c r="P81" s="34"/>
+      <c r="Q81" s="34"/>
+      <c r="R81" s="35"/>
+    </row>
+    <row r="82" spans="7:18">
+      <c r="G82" s="87">
         <v>42552</v>
       </c>
-      <c r="H80" s="51" t="s">
+      <c r="H82" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="I80" s="32"/>
-      <c r="J80" s="32"/>
-      <c r="K80" s="32"/>
-      <c r="L80" s="32"/>
-      <c r="M80" s="32"/>
-      <c r="N80" s="32"/>
-      <c r="O80" s="32"/>
-      <c r="P80" s="32"/>
-      <c r="Q80" s="32"/>
-      <c r="R80" s="33"/>
+      <c r="I82" s="32"/>
+      <c r="J82" s="32"/>
+      <c r="K82" s="32"/>
+      <c r="L82" s="32"/>
+      <c r="M82" s="32"/>
+      <c r="N82" s="32"/>
+      <c r="O82" s="32"/>
+      <c r="P82" s="32"/>
+      <c r="Q82" s="32"/>
+      <c r="R82" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Y25:AC25"/>
     <mergeCell ref="Y58:AC58"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="Z16:AA16"/>
@@ -11869,62 +11901,66 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H36" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H40" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="H38" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H42" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C34:D34" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R65" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H44" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H47" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R50" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H53" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="R67" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H46" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H49" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R52" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H55" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
     <hyperlink ref="W49" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
     <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
     <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
-    <hyperlink ref="H57" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H70" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="H59" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H72" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
     <hyperlink ref="D45" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D44" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
-    <hyperlink ref="R61" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H33" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
-    <hyperlink ref="H31" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
-    <hyperlink ref="H29" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
-    <hyperlink ref="H27" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
-    <hyperlink ref="H25" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
-    <hyperlink ref="H23" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
-    <hyperlink ref="H21" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
+    <hyperlink ref="R63" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H35" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H33" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
+    <hyperlink ref="H31" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
+    <hyperlink ref="H29" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
+    <hyperlink ref="H27" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
+    <hyperlink ref="H25" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="H23" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
     <hyperlink ref="Y25:AC25" r:id="rId24" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
-    <hyperlink ref="H15" r:id="rId25" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
-    <hyperlink ref="H17" r:id="rId26" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
-    <hyperlink ref="H19" r:id="rId27" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
-    <hyperlink ref="H13" r:id="rId28" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
-    <hyperlink ref="H11" r:id="rId29" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
-    <hyperlink ref="H9" r:id="rId30" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
-    <hyperlink ref="H7" r:id="rId31" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
+    <hyperlink ref="H17" r:id="rId25" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
+    <hyperlink ref="H19" r:id="rId26" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
+    <hyperlink ref="H21" r:id="rId27" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
+    <hyperlink ref="H15" r:id="rId28" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
+    <hyperlink ref="H13" r:id="rId29" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
+    <hyperlink ref="H11" r:id="rId30" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
+    <hyperlink ref="H9" r:id="rId31" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
+    <hyperlink ref="H7" r:id="rId32" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId32"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId33"/>
   <ignoredErrors>
     <ignoredError sqref="C39" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId33"/>
+  <drawing r:id="rId34"/>
 </worksheet>
 </file>
 
@@ -15025,113 +15061,113 @@
         <v>0.22325074870677919</v>
       </c>
     </row>
-    <row r="27" spans="2:39" s="141" customFormat="1">
-      <c r="B27" s="141" t="s">
+    <row r="27" spans="2:39" s="109" customFormat="1">
+      <c r="B27" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="141">
+      <c r="C27" s="109">
         <v>733.3</v>
       </c>
-      <c r="D27" s="141">
+      <c r="D27" s="109">
         <v>733.5</v>
       </c>
-      <c r="E27" s="141">
+      <c r="E27" s="109">
         <v>733.8</v>
       </c>
-      <c r="F27" s="141">
+      <c r="F27" s="109">
         <v>734.1</v>
       </c>
-      <c r="G27" s="141">
+      <c r="G27" s="109">
         <v>735.7</v>
       </c>
-      <c r="H27" s="141">
+      <c r="H27" s="109">
         <v>735.8</v>
       </c>
-      <c r="I27" s="141">
+      <c r="I27" s="109">
         <v>735.8</v>
       </c>
-      <c r="J27" s="141">
+      <c r="J27" s="109">
         <v>735.9</v>
       </c>
-      <c r="K27" s="141">
+      <c r="K27" s="109">
         <v>736.1</v>
       </c>
-      <c r="L27" s="141">
+      <c r="L27" s="109">
         <v>736.2</v>
       </c>
-      <c r="M27" s="141">
+      <c r="M27" s="109">
         <v>736.2</v>
       </c>
-      <c r="N27" s="141">
+      <c r="N27" s="109">
         <v>736.2</v>
       </c>
-      <c r="O27" s="142">
+      <c r="O27" s="110">
         <v>735</v>
       </c>
-      <c r="P27" s="142">
+      <c r="P27" s="110">
         <v>734.8</v>
       </c>
-      <c r="Q27" s="141">
+      <c r="Q27" s="109">
         <v>734.8</v>
       </c>
-      <c r="R27" s="141">
+      <c r="R27" s="109">
         <v>734.7</v>
       </c>
-      <c r="S27" s="141">
+      <c r="S27" s="109">
         <v>734.6</v>
       </c>
-      <c r="T27" s="141">
+      <c r="T27" s="109">
         <v>734.6</v>
       </c>
-      <c r="U27" s="141">
+      <c r="U27" s="109">
         <v>734.6</v>
       </c>
-      <c r="V27" s="141">
+      <c r="V27" s="109">
         <v>734.7</v>
       </c>
-      <c r="W27" s="141">
+      <c r="W27" s="109">
         <v>734.6</v>
       </c>
-      <c r="X27" s="141">
+      <c r="X27" s="109">
         <v>734.6</v>
       </c>
-      <c r="Y27" s="141">
+      <c r="Y27" s="109">
         <v>734.6</v>
       </c>
-      <c r="Z27" s="141">
+      <c r="Z27" s="109">
         <v>734.6</v>
       </c>
-      <c r="AA27" s="141">
+      <c r="AA27" s="109">
         <v>734.6</v>
       </c>
-      <c r="AD27" s="141">
+      <c r="AD27" s="109">
         <v>733.7</v>
       </c>
-      <c r="AE27" s="141">
+      <c r="AE27" s="109">
         <v>730.2</v>
       </c>
-      <c r="AF27" s="141">
+      <c r="AF27" s="109">
         <v>735.6</v>
       </c>
-      <c r="AG27" s="141">
+      <c r="AG27" s="109">
         <v>734.3</v>
       </c>
-      <c r="AH27" s="141">
+      <c r="AH27" s="109">
         <v>734.1</v>
       </c>
-      <c r="AI27" s="141">
+      <c r="AI27" s="109">
         <v>735.9</v>
       </c>
-      <c r="AJ27" s="141">
+      <c r="AJ27" s="109">
         <v>736.2</v>
       </c>
-      <c r="AK27" s="141">
+      <c r="AK27" s="109">
         <v>734.7</v>
       </c>
-      <c r="AL27" s="141">
+      <c r="AL27" s="109">
         <v>734.6</v>
       </c>
-      <c r="AM27" s="141">
+      <c r="AM27" s="109">
         <f>+Z27</f>
         <v>734.6</v>
       </c>

</xml_diff>

<commit_message>
$ERJ news updates for Farnborough Air Show 2024
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C63C0AD-3429-4DE1-8ADF-9A1A4B852DD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF18B226-DF26-4D16-8309-D29B9E228695}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="2010" windowWidth="26610" windowHeight="12885" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -33,6 +33,30 @@
     <author>me</author>
   </authors>
   <commentList>
+    <comment ref="AN9" authorId="0" shapeId="0" xr:uid="{A79935ED-AE6D-4D20-81AA-870E21775608}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>me:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Analysts consensus</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B27" authorId="0" shapeId="0" xr:uid="{3EBCC6D1-3BEF-4E43-B81B-09A647044702}">
       <text>
         <r>
@@ -146,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="314">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1125,6 +1149,12 @@
   <si>
     <t>Polish LOT airline has reached a lease agreement for 3 E195-E2 units in anticipation of an order of up to 84 jets</t>
   </si>
+  <si>
+    <t>Embraer announce first-in-class Automatic Takeoff Functionality for E2 series of regional airliners</t>
+  </si>
+  <si>
+    <t>Austria &amp; Netherlands sign for a joint deal of 9 C-390 Millenium A/C at the Farnborough Air Show 2024, deliver from 2027</t>
+  </si>
 </sst>
 </file>
 
@@ -1137,7 +1167,7 @@
     <numFmt numFmtId="167" formatCode="0.0000\x"/>
     <numFmt numFmtId="168" formatCode="mmmm\ yyyy;"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1326,8 +1356,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1373,6 +1416,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1470,7 +1519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1694,6 +1743,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9782,10 +9833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC82"/>
+  <dimension ref="A2:AC85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9805,46 +9856,50 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="124"/>
-      <c r="G5" s="122" t="s">
+      <c r="C5" s="125"/>
+      <c r="D5" s="126"/>
+      <c r="G5" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="123"/>
-      <c r="I5" s="123"/>
-      <c r="J5" s="123"/>
-      <c r="K5" s="123"/>
-      <c r="L5" s="123"/>
-      <c r="M5" s="123"/>
-      <c r="N5" s="123"/>
-      <c r="O5" s="123"/>
-      <c r="P5" s="123"/>
-      <c r="Q5" s="123"/>
-      <c r="R5" s="124"/>
-      <c r="T5" s="122" t="s">
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
+      <c r="O5" s="125"/>
+      <c r="P5" s="125"/>
+      <c r="Q5" s="125"/>
+      <c r="R5" s="126"/>
+      <c r="T5" s="124" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="123"/>
-      <c r="V5" s="123"/>
-      <c r="W5" s="124"/>
-      <c r="AA5" s="134" t="s">
+      <c r="U5" s="125"/>
+      <c r="V5" s="125"/>
+      <c r="W5" s="126"/>
+      <c r="AA5" s="136" t="s">
         <v>205</v>
       </c>
-      <c r="AB5" s="135"/>
+      <c r="AB5" s="137"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>26.04</v>
+        <v>29.98</v>
       </c>
       <c r="D6" s="17"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="8">
+        <v>45474</v>
+      </c>
+      <c r="H6" s="94" t="s">
+        <v>312</v>
+      </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
@@ -9871,18 +9926,14 @@
         <v>4</v>
       </c>
       <c r="C7" s="3">
-        <f>+'Financial Model'!Z27</f>
-        <v>734.6</v>
+        <f>+'Financial Model'!Z27/4</f>
+        <v>183.65</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="G7" s="8">
-        <v>45413</v>
-      </c>
-      <c r="H7" s="94" t="s">
-        <v>311</v>
-      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
@@ -9908,11 +9959,15 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>19128.984</v>
+        <v>5505.8270000000002</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="34"/>
+      <c r="G8" s="8">
+        <v>45474</v>
+      </c>
+      <c r="H8" s="94" t="s">
+        <v>313</v>
+      </c>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
@@ -9943,12 +9998,8 @@
       <c r="D9" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="G9" s="8">
-        <v>45413</v>
-      </c>
-      <c r="H9" s="94" t="s">
-        <v>310</v>
-      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
@@ -9977,8 +10028,12 @@
       <c r="D10" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="34"/>
+      <c r="G10" s="8">
+        <v>45413</v>
+      </c>
+      <c r="H10" s="94" t="s">
+        <v>311</v>
+      </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
@@ -10007,12 +10062,8 @@
       <c r="D11" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="G11" s="8">
-        <v>44986</v>
-      </c>
-      <c r="H11" s="94" t="s">
-        <v>307</v>
-      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
@@ -10036,11 +10087,15 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>20056.584000000003</v>
+        <v>6433.4270000000006</v>
       </c>
       <c r="D12" s="18"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="34"/>
+      <c r="G12" s="8">
+        <v>45413</v>
+      </c>
+      <c r="H12" s="94" t="s">
+        <v>310</v>
+      </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
@@ -10055,21 +10110,17 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="122" t="s">
+      <c r="Y12" s="124" t="s">
         <v>217</v>
       </c>
-      <c r="Z12" s="123"/>
-      <c r="AA12" s="123"/>
-      <c r="AB12" s="123"/>
-      <c r="AC12" s="124"/>
+      <c r="Z12" s="125"/>
+      <c r="AA12" s="125"/>
+      <c r="AB12" s="125"/>
+      <c r="AC12" s="126"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="G13" s="8">
-        <v>44986</v>
-      </c>
-      <c r="H13" s="94" t="s">
-        <v>306</v>
-      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
@@ -10087,18 +10138,22 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="88"/>
-      <c r="Z13" s="120" t="s">
+      <c r="Z13" s="122" t="s">
         <v>218</v>
       </c>
-      <c r="AA13" s="120"/>
-      <c r="AB13" s="120" t="s">
+      <c r="AA13" s="122"/>
+      <c r="AB13" s="122" t="s">
         <v>219</v>
       </c>
-      <c r="AC13" s="121"/>
+      <c r="AC13" s="123"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="G14" s="9"/>
-      <c r="H14" s="34"/>
+      <c r="G14" s="8">
+        <v>44986</v>
+      </c>
+      <c r="H14" s="94" t="s">
+        <v>307</v>
+      </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
@@ -10118,27 +10173,23 @@
       <c r="Y14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z14" s="117" t="s">
+      <c r="Z14" s="119" t="s">
         <v>229</v>
       </c>
-      <c r="AA14" s="117"/>
-      <c r="AB14" s="117" t="s">
+      <c r="AA14" s="119"/>
+      <c r="AB14" s="119" t="s">
         <v>230</v>
       </c>
-      <c r="AC14" s="116"/>
+      <c r="AC14" s="118"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="123"/>
-      <c r="D15" s="124"/>
-      <c r="G15" s="8">
-        <v>44986</v>
-      </c>
-      <c r="H15" s="94" t="s">
-        <v>305</v>
-      </c>
+      <c r="C15" s="125"/>
+      <c r="D15" s="126"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
@@ -10158,14 +10209,14 @@
       <c r="Y15" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z15" s="117" t="s">
+      <c r="Z15" s="119" t="s">
         <v>225</v>
       </c>
-      <c r="AA15" s="117"/>
-      <c r="AB15" s="117" t="s">
+      <c r="AA15" s="119"/>
+      <c r="AB15" s="119" t="s">
         <v>231</v>
       </c>
-      <c r="AC15" s="116"/>
+      <c r="AC15" s="118"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -10174,15 +10225,19 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="117" t="s">
+      <c r="C16" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="116"/>
+      <c r="D16" s="118"/>
       <c r="E16" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="34"/>
+      <c r="G16" s="8">
+        <v>44986</v>
+      </c>
+      <c r="H16" s="94" t="s">
+        <v>306</v>
+      </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -10202,32 +10257,28 @@
       <c r="Y16" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z16" s="117" t="s">
+      <c r="Z16" s="119" t="s">
         <v>226</v>
       </c>
-      <c r="AA16" s="117"/>
-      <c r="AB16" s="117" t="s">
+      <c r="AA16" s="119"/>
+      <c r="AB16" s="119" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="116"/>
+      <c r="AC16" s="118"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C17" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="116"/>
+      <c r="D17" s="118"/>
       <c r="E17" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="G17" s="8">
-        <v>45261</v>
-      </c>
-      <c r="H17" s="94" t="s">
-        <v>296</v>
-      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
@@ -10245,21 +10296,25 @@
       <c r="Y17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="Z17" s="117" t="s">
+      <c r="Z17" s="119" t="s">
         <v>227</v>
       </c>
-      <c r="AA17" s="117"/>
-      <c r="AB17" s="117" t="s">
+      <c r="AA17" s="119"/>
+      <c r="AB17" s="119" t="s">
         <v>233</v>
       </c>
-      <c r="AC17" s="116"/>
+      <c r="AC17" s="118"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="116"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="118"/>
+      <c r="G18" s="8">
+        <v>44986</v>
+      </c>
+      <c r="H18" s="94" t="s">
+        <v>305</v>
+      </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
@@ -10279,25 +10334,21 @@
       <c r="Y18" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="Z18" s="117" t="s">
+      <c r="Z18" s="119" t="s">
         <v>228</v>
       </c>
-      <c r="AA18" s="117"/>
-      <c r="AB18" s="117" t="s">
+      <c r="AA18" s="119"/>
+      <c r="AB18" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="AC18" s="116"/>
+      <c r="AC18" s="118"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="139"/>
-      <c r="G19" s="8">
-        <v>45231</v>
-      </c>
-      <c r="H19" s="94" t="s">
-        <v>297</v>
-      </c>
+      <c r="C19" s="140"/>
+      <c r="D19" s="141"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
@@ -10317,18 +10368,22 @@
       <c r="Y19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Z19" s="117" t="s">
+      <c r="Z19" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="AA19" s="117"/>
-      <c r="AB19" s="117" t="s">
+      <c r="AA19" s="119"/>
+      <c r="AB19" s="119" t="s">
         <v>237</v>
       </c>
-      <c r="AC19" s="116"/>
+      <c r="AC19" s="118"/>
     </row>
     <row r="20" spans="2:29">
-      <c r="G20" s="9"/>
-      <c r="H20" s="34"/>
+      <c r="G20" s="8">
+        <v>45261</v>
+      </c>
+      <c r="H20" s="94" t="s">
+        <v>296</v>
+      </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -10348,22 +10403,18 @@
       <c r="Y20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Z20" s="117" t="s">
+      <c r="Z20" s="119" t="s">
         <v>242</v>
       </c>
-      <c r="AA20" s="117"/>
-      <c r="AB20" s="117" t="s">
+      <c r="AA20" s="119"/>
+      <c r="AB20" s="119" t="s">
         <v>243</v>
       </c>
-      <c r="AC20" s="116"/>
+      <c r="AC20" s="118"/>
     </row>
     <row r="21" spans="2:29">
-      <c r="G21" s="8">
-        <v>45200</v>
-      </c>
-      <c r="H21" s="94" t="s">
-        <v>298</v>
-      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
@@ -10387,13 +10438,17 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="122" t="s">
+      <c r="B22" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="123"/>
-      <c r="D22" s="124"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="34"/>
+      <c r="C22" s="125"/>
+      <c r="D22" s="126"/>
+      <c r="G22" s="8">
+        <v>45231</v>
+      </c>
+      <c r="H22" s="94" t="s">
+        <v>297</v>
+      </c>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
@@ -10420,16 +10475,12 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="117" t="s">
+      <c r="C23" s="119" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="116"/>
-      <c r="G23" s="8">
-        <v>45170</v>
-      </c>
-      <c r="H23" s="94" t="s">
-        <v>272</v>
-      </c>
+      <c r="D23" s="118"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
       <c r="K23" s="34"/>
@@ -10449,12 +10500,16 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="117">
+      <c r="C24" s="119">
         <v>1969</v>
       </c>
-      <c r="D24" s="116"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="34"/>
+      <c r="D24" s="118"/>
+      <c r="G24" s="8">
+        <v>45200</v>
+      </c>
+      <c r="H24" s="94" t="s">
+        <v>298</v>
+      </c>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
       <c r="K24" s="34"/>
@@ -10474,14 +10529,10 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="116"/>
-      <c r="G25" s="8">
-        <v>45017</v>
-      </c>
-      <c r="H25" s="94" t="s">
-        <v>271</v>
-      </c>
+      <c r="C25" s="119"/>
+      <c r="D25" s="118"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
@@ -10498,25 +10549,29 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="140" t="s">
+      <c r="Y25" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="Z25" s="141"/>
-      <c r="AA25" s="141"/>
-      <c r="AB25" s="141"/>
-      <c r="AC25" s="142"/>
+      <c r="Z25" s="143"/>
+      <c r="AA25" s="143"/>
+      <c r="AB25" s="143"/>
+      <c r="AC25" s="144"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="136">
+      <c r="C26" s="138">
         <f>'Financial Model'!Z68</f>
         <v>2636</v>
       </c>
-      <c r="D26" s="137"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="34"/>
+      <c r="D26" s="139"/>
+      <c r="G26" s="8">
+        <v>45170</v>
+      </c>
+      <c r="H26" s="94" t="s">
+        <v>272</v>
+      </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
@@ -10543,14 +10598,10 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="116"/>
-      <c r="G27" s="8">
-        <v>45017</v>
-      </c>
-      <c r="H27" s="100" t="s">
-        <v>268</v>
-      </c>
+      <c r="C27" s="119"/>
+      <c r="D27" s="118"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
@@ -10579,13 +10630,17 @@
       <c r="B28" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="115">
+      <c r="C28" s="117">
         <f>+'Order &amp; Backlog'!$Z$3</f>
         <v>2180</v>
       </c>
-      <c r="D28" s="116"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="34"/>
+      <c r="D28" s="118"/>
+      <c r="G28" s="8">
+        <v>45017</v>
+      </c>
+      <c r="H28" s="94" t="s">
+        <v>271</v>
+      </c>
       <c r="I28" s="34"/>
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
@@ -10614,17 +10669,13 @@
       <c r="B29" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="115">
+      <c r="C29" s="117">
         <f>'Order &amp; Backlog'!Z21</f>
         <v>381</v>
       </c>
-      <c r="D29" s="116"/>
-      <c r="G29" s="8">
-        <v>44927</v>
-      </c>
-      <c r="H29" s="96" t="s">
-        <v>265</v>
-      </c>
+      <c r="D29" s="118"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
@@ -10651,13 +10702,17 @@
       <c r="B30" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="117">
+      <c r="C30" s="119">
         <f>'Financial Model'!AA43</f>
         <v>25</v>
       </c>
-      <c r="D30" s="116"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="34"/>
+      <c r="D30" s="118"/>
+      <c r="G30" s="8">
+        <v>45017</v>
+      </c>
+      <c r="H30" s="100" t="s">
+        <v>268</v>
+      </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
@@ -10684,16 +10739,12 @@
       <c r="B31" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="118">
+      <c r="C31" s="120">
         <v>36708</v>
       </c>
-      <c r="D31" s="119"/>
-      <c r="G31" s="8">
-        <v>44896</v>
-      </c>
-      <c r="H31" s="94" t="s">
-        <v>263</v>
-      </c>
+      <c r="D31" s="121"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
@@ -10720,10 +10771,14 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="116"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="34"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="118"/>
+      <c r="G32" s="8">
+        <v>44927</v>
+      </c>
+      <c r="H32" s="96" t="s">
+        <v>265</v>
+      </c>
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
       <c r="K32" s="34"/>
@@ -10756,12 +10811,8 @@
       <c r="D33" s="29">
         <v>45419</v>
       </c>
-      <c r="G33" s="8">
-        <v>44866</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>261</v>
-      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="34"/>
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
       <c r="K33" s="34"/>
@@ -10788,12 +10839,16 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="130" t="s">
+      <c r="C34" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="131"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="34"/>
+      <c r="D34" s="133"/>
+      <c r="G34" s="8">
+        <v>44896</v>
+      </c>
+      <c r="H34" s="94" t="s">
+        <v>263</v>
+      </c>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
       <c r="K34" s="34"/>
@@ -10817,12 +10872,8 @@
       <c r="AC34" s="35"/>
     </row>
     <row r="35" spans="2:29">
-      <c r="G35" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>252</v>
-      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="34"/>
       <c r="I35" s="34"/>
       <c r="J35" s="34"/>
       <c r="K35" s="34"/>
@@ -10842,8 +10893,12 @@
       <c r="AC35" s="35"/>
     </row>
     <row r="36" spans="2:29">
-      <c r="G36" s="9"/>
-      <c r="H36" s="34"/>
+      <c r="G36" s="8">
+        <v>44866</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>261</v>
+      </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
       <c r="K36" s="34"/>
@@ -10861,11 +10916,11 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="122" t="s">
+      <c r="B37" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="123"/>
-      <c r="D37" s="124"/>
+      <c r="C37" s="125"/>
+      <c r="D37" s="126"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -10878,12 +10933,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="122" t="s">
+      <c r="T37" s="124" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="123"/>
-      <c r="V37" s="123"/>
-      <c r="W37" s="124"/>
+      <c r="U37" s="125"/>
+      <c r="V37" s="125"/>
+      <c r="W37" s="126"/>
       <c r="Y37" s="39" t="s">
         <v>280</v>
       </c>
@@ -10896,16 +10951,16 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="132">
+      <c r="C38" s="134">
         <f>C6/'Financial Model'!AA123</f>
-        <v>6.2876718272359708</v>
-      </c>
-      <c r="D38" s="133"/>
+        <v>7.2390323110804307</v>
+      </c>
+      <c r="D38" s="135"/>
       <c r="G38" s="8">
         <v>44835</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>11</v>
+        <v>252</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -10935,15 +10990,13 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="132">
+      <c r="C39" s="134">
         <f>+C8/SUM('Financial Model'!X4:AA4)</f>
-        <v>10.347262400605832</v>
-      </c>
-      <c r="D39" s="133"/>
+        <v>2.9782155027857415</v>
+      </c>
+      <c r="D39" s="135"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="H39" s="34"/>
       <c r="I39" s="34"/>
       <c r="J39" s="34"/>
       <c r="K39" s="34"/>
@@ -10970,15 +11023,13 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="128">
+      <c r="C40" s="130">
         <f>C6/SUM('Financial Model'!X26:AA26)</f>
-        <v>72.595764705882345</v>
-      </c>
-      <c r="D40" s="129"/>
+        <v>83.579916508538901</v>
+      </c>
+      <c r="D40" s="131"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="H40" s="34"/>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
       <c r="K40" s="34"/>
@@ -11002,8 +11053,12 @@
       <c r="AC40" s="35"/>
     </row>
     <row r="41" spans="2:29">
-      <c r="G41" s="9"/>
-      <c r="H41" s="34"/>
+      <c r="G41" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
@@ -11027,11 +11082,9 @@
       <c r="AC41" s="35"/>
     </row>
     <row r="42" spans="2:29">
-      <c r="G42" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>29</v>
+      <c r="G42" s="9"/>
+      <c r="H42" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
@@ -11054,14 +11107,14 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="122" t="s">
+      <c r="B43" s="124" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="123"/>
-      <c r="D43" s="124"/>
+      <c r="C43" s="125"/>
+      <c r="D43" s="126"/>
       <c r="G43" s="9"/>
       <c r="H43" s="7" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
@@ -11088,10 +11141,10 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="111" t="s">
+      <c r="B44" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="C44" s="112"/>
+      <c r="C44" s="114"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
@@ -11122,15 +11175,19 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="111" t="s">
+      <c r="B45" s="113" t="s">
         <v>247</v>
       </c>
-      <c r="C45" s="112"/>
+      <c r="C45" s="114"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="34"/>
+      <c r="G45" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
       <c r="K45" s="34"/>
@@ -11156,16 +11213,14 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="111"/>
-      <c r="C46" s="112"/>
+      <c r="B46" s="113"/>
+      <c r="C46" s="114"/>
       <c r="D46" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>187</v>
+      <c r="G46" s="9"/>
+      <c r="H46" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
@@ -11188,8 +11243,8 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="111"/>
-      <c r="C47" s="112"/>
+      <c r="B47" s="113"/>
+      <c r="C47" s="114"/>
       <c r="D47" s="85" t="s">
         <v>31</v>
       </c>
@@ -11220,8 +11275,8 @@
       <c r="AC47" s="35"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="113"/>
-      <c r="C48" s="114"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="116"/>
       <c r="D48" s="86" t="s">
         <v>31</v>
       </c>
@@ -11256,7 +11311,7 @@
         <v>44805</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
@@ -11284,9 +11339,7 @@
     </row>
     <row r="50" spans="7:29">
       <c r="G50" s="9"/>
-      <c r="H50" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="H50" s="34"/>
       <c r="I50" s="34"/>
       <c r="J50" s="34"/>
       <c r="K50" s="34"/>
@@ -11307,9 +11360,7 @@
     </row>
     <row r="51" spans="7:29">
       <c r="G51" s="9"/>
-      <c r="H51" s="7" t="s">
-        <v>193</v>
-      </c>
+      <c r="H51" s="34"/>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
@@ -11329,9 +11380,11 @@
       <c r="AC51" s="35"/>
     </row>
     <row r="52" spans="7:29">
-      <c r="G52" s="9"/>
-      <c r="H52" s="7" t="s">
-        <v>191</v>
+      <c r="G52" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
@@ -11342,9 +11395,7 @@
       <c r="O52" s="34"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="34"/>
-      <c r="R52" s="48" t="s">
-        <v>194</v>
-      </c>
+      <c r="R52" s="35"/>
       <c r="Y52" s="39"/>
       <c r="Z52" s="34"/>
       <c r="AA52" s="34"/>
@@ -11353,7 +11404,9 @@
     </row>
     <row r="53" spans="7:29">
       <c r="G53" s="9"/>
-      <c r="H53" s="34"/>
+      <c r="H53" s="7" t="s">
+        <v>192</v>
+      </c>
       <c r="I53" s="34"/>
       <c r="J53" s="34"/>
       <c r="K53" s="34"/>
@@ -11374,7 +11427,9 @@
     </row>
     <row r="54" spans="7:29">
       <c r="G54" s="9"/>
-      <c r="H54" s="34"/>
+      <c r="H54" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
       <c r="K54" s="34"/>
@@ -11394,11 +11449,9 @@
       <c r="AC54" s="35"/>
     </row>
     <row r="55" spans="7:29">
-      <c r="G55" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>196</v>
+      <c r="G55" s="9"/>
+      <c r="H55" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="I55" s="34"/>
       <c r="J55" s="34"/>
@@ -11409,7 +11462,9 @@
       <c r="O55" s="34"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="34"/>
-      <c r="R55" s="35"/>
+      <c r="R55" s="48" t="s">
+        <v>194</v>
+      </c>
       <c r="Y55" s="102" t="s">
         <v>294</v>
       </c>
@@ -11420,9 +11475,7 @@
     </row>
     <row r="56" spans="7:29">
       <c r="G56" s="9"/>
-      <c r="H56" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="H56" s="34"/>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
       <c r="K56" s="34"/>
@@ -11441,9 +11494,7 @@
     </row>
     <row r="57" spans="7:29">
       <c r="G57" s="9"/>
-      <c r="H57" s="47" t="s">
-        <v>198</v>
-      </c>
+      <c r="H57" s="34"/>
       <c r="I57" s="34"/>
       <c r="J57" s="34"/>
       <c r="K57" s="34"/>
@@ -11461,8 +11512,12 @@
       <c r="AC57" s="105"/>
     </row>
     <row r="58" spans="7:29">
-      <c r="G58" s="9"/>
-      <c r="H58" s="34"/>
+      <c r="G58" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>196</v>
+      </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
@@ -11473,20 +11528,18 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
-      <c r="Y58" s="125" t="s">
+      <c r="Y58" s="127" t="s">
         <v>295</v>
       </c>
-      <c r="Z58" s="126"/>
-      <c r="AA58" s="126"/>
-      <c r="AB58" s="126"/>
-      <c r="AC58" s="127"/>
+      <c r="Z58" s="128"/>
+      <c r="AA58" s="128"/>
+      <c r="AB58" s="128"/>
+      <c r="AC58" s="129"/>
     </row>
     <row r="59" spans="7:29">
-      <c r="G59" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>239</v>
+      <c r="G59" s="9"/>
+      <c r="H59" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="I59" s="34"/>
       <c r="J59" s="34"/>
@@ -11501,8 +11554,8 @@
     </row>
     <row r="60" spans="7:29">
       <c r="G60" s="9"/>
-      <c r="H60" s="7" t="s">
-        <v>240</v>
+      <c r="H60" s="47" t="s">
+        <v>198</v>
       </c>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
@@ -11531,10 +11584,10 @@
     </row>
     <row r="62" spans="7:29">
       <c r="G62" s="8">
-        <v>44682</v>
-      </c>
-      <c r="H62" s="34" t="s">
-        <v>248</v>
+        <v>44743</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
@@ -11550,7 +11603,7 @@
     <row r="63" spans="7:29">
       <c r="G63" s="9"/>
       <c r="H63" s="7" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="I63" s="34"/>
       <c r="J63" s="34"/>
@@ -11561,9 +11614,7 @@
       <c r="O63" s="34"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="34"/>
-      <c r="R63" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R63" s="35"/>
     </row>
     <row r="64" spans="7:29">
       <c r="G64" s="9"/>
@@ -11581,10 +11632,10 @@
     </row>
     <row r="65" spans="7:18">
       <c r="G65" s="8">
-        <v>43922</v>
+        <v>44682</v>
       </c>
       <c r="H65" s="34" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="I65" s="34"/>
       <c r="J65" s="34"/>
@@ -11600,7 +11651,7 @@
     <row r="66" spans="7:18">
       <c r="G66" s="9"/>
       <c r="H66" s="7" t="s">
-        <v>169</v>
+        <v>249</v>
       </c>
       <c r="I66" s="34"/>
       <c r="J66" s="34"/>
@@ -11611,7 +11662,9 @@
       <c r="O66" s="34"/>
       <c r="P66" s="34"/>
       <c r="Q66" s="34"/>
-      <c r="R66" s="35"/>
+      <c r="R66" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="67" spans="7:18">
       <c r="G67" s="9"/>
@@ -11625,13 +11678,15 @@
       <c r="O67" s="34"/>
       <c r="P67" s="34"/>
       <c r="Q67" s="34"/>
-      <c r="R67" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R67" s="35"/>
     </row>
     <row r="68" spans="7:18">
-      <c r="G68" s="9"/>
-      <c r="H68" s="34"/>
+      <c r="G68" s="8">
+        <v>43922</v>
+      </c>
+      <c r="H68" s="34" t="s">
+        <v>164</v>
+      </c>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
       <c r="K68" s="34"/>
@@ -11644,11 +11699,9 @@
       <c r="R68" s="35"/>
     </row>
     <row r="69" spans="7:18">
-      <c r="G69" s="8">
-        <v>43770</v>
-      </c>
-      <c r="H69" s="34" t="s">
-        <v>167</v>
+      <c r="G69" s="9"/>
+      <c r="H69" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="I69" s="34"/>
       <c r="J69" s="34"/>
@@ -11663,9 +11716,7 @@
     </row>
     <row r="70" spans="7:18">
       <c r="G70" s="9"/>
-      <c r="H70" s="47" t="s">
-        <v>168</v>
-      </c>
+      <c r="H70" s="34"/>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>
       <c r="K70" s="34"/>
@@ -11675,7 +11726,9 @@
       <c r="O70" s="34"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="34"/>
-      <c r="R70" s="35"/>
+      <c r="R70" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="71" spans="7:18">
       <c r="G71" s="9"/>
@@ -11693,10 +11746,10 @@
     </row>
     <row r="72" spans="7:18">
       <c r="G72" s="8">
-        <v>43739</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>244</v>
+        <v>43770</v>
+      </c>
+      <c r="H72" s="34" t="s">
+        <v>167</v>
       </c>
       <c r="I72" s="34"/>
       <c r="J72" s="34"/>
@@ -11706,14 +11759,14 @@
       <c r="N72" s="34"/>
       <c r="O72" s="34"/>
       <c r="P72" s="34"/>
-      <c r="Q72" s="34" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q72" s="34"/>
       <c r="R72" s="35"/>
     </row>
     <row r="73" spans="7:18">
       <c r="G73" s="9"/>
-      <c r="H73" s="34"/>
+      <c r="H73" s="47" t="s">
+        <v>168</v>
+      </c>
       <c r="I73" s="34"/>
       <c r="J73" s="34"/>
       <c r="K73" s="34"/>
@@ -11740,8 +11793,12 @@
       <c r="R74" s="35"/>
     </row>
     <row r="75" spans="7:18">
-      <c r="G75" s="9"/>
-      <c r="H75" s="34"/>
+      <c r="G75" s="8">
+        <v>43739</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>244</v>
+      </c>
       <c r="I75" s="34"/>
       <c r="J75" s="34"/>
       <c r="K75" s="34"/>
@@ -11750,16 +11807,14 @@
       <c r="N75" s="34"/>
       <c r="O75" s="34"/>
       <c r="P75" s="34"/>
-      <c r="Q75" s="34"/>
+      <c r="Q75" s="34" t="s">
+        <v>179</v>
+      </c>
       <c r="R75" s="35"/>
     </row>
     <row r="76" spans="7:18">
-      <c r="G76" s="8">
-        <v>43586</v>
-      </c>
-      <c r="H76" s="34" t="s">
-        <v>166</v>
-      </c>
+      <c r="G76" s="9"/>
+      <c r="H76" s="34"/>
       <c r="I76" s="34"/>
       <c r="J76" s="34"/>
       <c r="K76" s="34"/>
@@ -11786,12 +11841,8 @@
       <c r="R77" s="35"/>
     </row>
     <row r="78" spans="7:18">
-      <c r="G78" s="8">
-        <v>43282</v>
-      </c>
-      <c r="H78" s="34" t="s">
-        <v>162</v>
-      </c>
+      <c r="G78" s="9"/>
+      <c r="H78" s="34"/>
       <c r="I78" s="34"/>
       <c r="J78" s="34"/>
       <c r="K78" s="34"/>
@@ -11804,9 +11855,11 @@
       <c r="R78" s="35"/>
     </row>
     <row r="79" spans="7:18">
-      <c r="G79" s="9"/>
-      <c r="H79" s="7" t="s">
-        <v>163</v>
+      <c r="G79" s="8">
+        <v>43586</v>
+      </c>
+      <c r="H79" s="34" t="s">
+        <v>166</v>
       </c>
       <c r="I79" s="34"/>
       <c r="J79" s="34"/>
@@ -11821,9 +11874,7 @@
     </row>
     <row r="80" spans="7:18">
       <c r="G80" s="9"/>
-      <c r="H80" s="7" t="s">
-        <v>165</v>
-      </c>
+      <c r="H80" s="34"/>
       <c r="I80" s="34"/>
       <c r="J80" s="34"/>
       <c r="K80" s="34"/>
@@ -11836,8 +11887,12 @@
       <c r="R80" s="35"/>
     </row>
     <row r="81" spans="7:18">
-      <c r="G81" s="9"/>
-      <c r="H81" s="34"/>
+      <c r="G81" s="8">
+        <v>43282</v>
+      </c>
+      <c r="H81" s="34" t="s">
+        <v>162</v>
+      </c>
       <c r="I81" s="34"/>
       <c r="J81" s="34"/>
       <c r="K81" s="34"/>
@@ -11850,22 +11905,68 @@
       <c r="R81" s="35"/>
     </row>
     <row r="82" spans="7:18">
-      <c r="G82" s="87">
+      <c r="G82" s="9"/>
+      <c r="H82" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I82" s="34"/>
+      <c r="J82" s="34"/>
+      <c r="K82" s="34"/>
+      <c r="L82" s="34"/>
+      <c r="M82" s="34"/>
+      <c r="N82" s="34"/>
+      <c r="O82" s="34"/>
+      <c r="P82" s="34"/>
+      <c r="Q82" s="34"/>
+      <c r="R82" s="35"/>
+    </row>
+    <row r="83" spans="7:18">
+      <c r="G83" s="9"/>
+      <c r="H83" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I83" s="34"/>
+      <c r="J83" s="34"/>
+      <c r="K83" s="34"/>
+      <c r="L83" s="34"/>
+      <c r="M83" s="34"/>
+      <c r="N83" s="34"/>
+      <c r="O83" s="34"/>
+      <c r="P83" s="34"/>
+      <c r="Q83" s="34"/>
+      <c r="R83" s="35"/>
+    </row>
+    <row r="84" spans="7:18">
+      <c r="G84" s="9"/>
+      <c r="H84" s="34"/>
+      <c r="I84" s="34"/>
+      <c r="J84" s="34"/>
+      <c r="K84" s="34"/>
+      <c r="L84" s="34"/>
+      <c r="M84" s="34"/>
+      <c r="N84" s="34"/>
+      <c r="O84" s="34"/>
+      <c r="P84" s="34"/>
+      <c r="Q84" s="34"/>
+      <c r="R84" s="35"/>
+    </row>
+    <row r="85" spans="7:18">
+      <c r="G85" s="87">
         <v>42552</v>
       </c>
-      <c r="H82" s="51" t="s">
+      <c r="H85" s="51" t="s">
         <v>238</v>
       </c>
-      <c r="I82" s="32"/>
-      <c r="J82" s="32"/>
-      <c r="K82" s="32"/>
-      <c r="L82" s="32"/>
-      <c r="M82" s="32"/>
-      <c r="N82" s="32"/>
-      <c r="O82" s="32"/>
-      <c r="P82" s="32"/>
-      <c r="Q82" s="32"/>
-      <c r="R82" s="33"/>
+      <c r="I85" s="32"/>
+      <c r="J85" s="32"/>
+      <c r="K85" s="32"/>
+      <c r="L85" s="32"/>
+      <c r="M85" s="32"/>
+      <c r="N85" s="32"/>
+      <c r="O85" s="32"/>
+      <c r="P85" s="32"/>
+      <c r="Q85" s="32"/>
+      <c r="R85" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="51">
@@ -11922,45 +12023,47 @@
     <mergeCell ref="C31:D31"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H38" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H42" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="H41" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H45" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
     <hyperlink ref="C34:D34" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R67" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H46" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H49" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R52" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H55" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="R70" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H49" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H52" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R55" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H58" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
     <hyperlink ref="W49" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
     <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
     <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
-    <hyperlink ref="H59" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H72" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="H62" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H75" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
     <hyperlink ref="D45" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D44" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
-    <hyperlink ref="R63" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H35" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
-    <hyperlink ref="H33" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
-    <hyperlink ref="H31" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
-    <hyperlink ref="H29" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
-    <hyperlink ref="H27" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
-    <hyperlink ref="H25" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
-    <hyperlink ref="H23" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
+    <hyperlink ref="R66" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H38" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H36" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
+    <hyperlink ref="H34" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
+    <hyperlink ref="H32" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
+    <hyperlink ref="H30" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
+    <hyperlink ref="H28" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="H26" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
     <hyperlink ref="Y25:AC25" r:id="rId24" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
-    <hyperlink ref="H17" r:id="rId25" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
-    <hyperlink ref="H19" r:id="rId26" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
-    <hyperlink ref="H21" r:id="rId27" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
-    <hyperlink ref="H15" r:id="rId28" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
-    <hyperlink ref="H13" r:id="rId29" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
-    <hyperlink ref="H11" r:id="rId30" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
-    <hyperlink ref="H9" r:id="rId31" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
-    <hyperlink ref="H7" r:id="rId32" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
+    <hyperlink ref="H20" r:id="rId25" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
+    <hyperlink ref="H22" r:id="rId26" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
+    <hyperlink ref="H24" r:id="rId27" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
+    <hyperlink ref="H18" r:id="rId28" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
+    <hyperlink ref="H16" r:id="rId29" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
+    <hyperlink ref="H14" r:id="rId30" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
+    <hyperlink ref="H12" r:id="rId31" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
+    <hyperlink ref="H10" r:id="rId32" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
+    <hyperlink ref="H8" r:id="rId33" xr:uid="{DE4DB842-01BE-405E-8254-AC1C82253C72}"/>
+    <hyperlink ref="H6" r:id="rId34" xr:uid="{645C2C50-2541-448D-9073-14E40D1DE986}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId33"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId35"/>
   <ignoredErrors>
     <ignoredError sqref="C39" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId34"/>
+  <drawing r:id="rId36"/>
 </worksheet>
 </file>
 
@@ -11969,10 +12072,10 @@
   <dimension ref="B1:AU148"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="AR21" sqref="AR21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -12994,6 +13097,10 @@
         <f>SUM(AM4:AM8)</f>
         <v>5268.5</v>
       </c>
+      <c r="AN9" s="111">
+        <f>+AM9*1.192</f>
+        <v>6280.0519999999997</v>
+      </c>
     </row>
     <row r="10" spans="2:47">
       <c r="B10" s="3" t="s">
@@ -13810,7 +13917,7 @@
         <v>-5.6000000000000014</v>
       </c>
     </row>
-    <row r="17" spans="2:39">
+    <row r="17" spans="2:40">
       <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
@@ -13922,7 +14029,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:39" s="2" customFormat="1">
+    <row r="18" spans="2:40" s="2" customFormat="1">
       <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
@@ -14067,7 +14174,7 @@
         <v>314.50000000000034</v>
       </c>
     </row>
-    <row r="19" spans="2:39">
+    <row r="19" spans="2:40">
       <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
@@ -14185,7 +14292,7 @@
         <v>-193.29999999999995</v>
       </c>
     </row>
-    <row r="20" spans="2:39">
+    <row r="20" spans="2:40">
       <c r="B20" s="3" t="s">
         <v>61</v>
       </c>
@@ -14296,7 +14403,7 @@
         <v>-0.49999999999999956</v>
       </c>
     </row>
-    <row r="21" spans="2:39">
+    <row r="21" spans="2:40">
       <c r="B21" s="3" t="s">
         <v>62</v>
       </c>
@@ -14441,7 +14548,7 @@
         <v>120.70000000000039</v>
       </c>
     </row>
-    <row r="22" spans="2:39">
+    <row r="22" spans="2:40">
       <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
@@ -14551,7 +14658,7 @@
         <v>-43.6</v>
       </c>
     </row>
-    <row r="23" spans="2:39" s="2" customFormat="1">
+    <row r="23" spans="2:40" s="2" customFormat="1">
       <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
@@ -14696,7 +14803,7 @@
         <v>164.30000000000038</v>
       </c>
     </row>
-    <row r="24" spans="2:39" s="2" customFormat="1">
+    <row r="24" spans="2:40" s="2" customFormat="1">
       <c r="B24" s="26" t="s">
         <v>72</v>
       </c>
@@ -14806,7 +14913,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="2:39">
+    <row r="25" spans="2:40">
       <c r="B25" s="27" t="s">
         <v>73</v>
       </c>
@@ -14916,7 +15023,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="26" spans="2:39" s="99" customFormat="1">
+    <row r="26" spans="2:40" s="99" customFormat="1">
       <c r="B26" s="99" t="s">
         <v>65</v>
       </c>
@@ -15061,7 +15168,7 @@
         <v>0.22325074870677919</v>
       </c>
     </row>
-    <row r="27" spans="2:39" s="109" customFormat="1">
+    <row r="27" spans="2:40" s="109" customFormat="1">
       <c r="B27" s="109" t="s">
         <v>4</v>
       </c>
@@ -15172,7 +15279,7 @@
         <v>734.6</v>
       </c>
     </row>
-    <row r="30" spans="2:39" s="2" customFormat="1">
+    <row r="30" spans="2:40" s="2" customFormat="1">
       <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
@@ -15304,15 +15411,19 @@
         <v>0.11299090451062033</v>
       </c>
       <c r="AL30" s="31">
-        <f t="shared" ref="AL30:AM30" si="33">AL9/AK9-1</f>
+        <f t="shared" ref="AL30:AN30" si="33">AL9/AK9-1</f>
         <v>8.1768798246449892E-2</v>
       </c>
       <c r="AM30" s="31">
         <f t="shared" si="33"/>
         <v>0.16036032067659245</v>
       </c>
+      <c r="AN30" s="112">
+        <f t="shared" si="33"/>
+        <v>0.19199999999999995</v>
+      </c>
     </row>
-    <row r="31" spans="2:39" s="24" customFormat="1">
+    <row r="31" spans="2:40" s="24" customFormat="1">
       <c r="B31" s="24" t="s">
         <v>67</v>
       </c>
@@ -15446,7 +15557,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="2:39" s="60" customFormat="1">
+    <row r="32" spans="2:40" s="60" customFormat="1">
       <c r="B32" s="64" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
$ERJ Virgin Australia news
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733AA2DC-8E62-42FA-9F5F-C2DF80A36CB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CB985C-DA51-435C-B14B-054CF93B5525}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="2010" windowWidth="26610" windowHeight="12885" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="319">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1167,6 +1167,9 @@
   <si>
     <t>4 Oct 26 - 25 Oct 26</t>
   </si>
+  <si>
+    <t>Virgin Australia place firm order for 8 E190-E2 regional jets to replace their aging Fokker 100 fleet</t>
+  </si>
 </sst>
 </file>
 
@@ -1756,6 +1759,11 @@
     <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1765,31 +1773,37 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1819,37 +1833,26 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9948,10 +9951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC85"/>
+  <dimension ref="A2:AC87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9971,50 +9974,50 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="113"/>
-      <c r="G5" s="111" t="s">
+      <c r="C5" s="115"/>
+      <c r="D5" s="116"/>
+      <c r="G5" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="113"/>
-      <c r="T5" s="111" t="s">
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="115"/>
+      <c r="R5" s="116"/>
+      <c r="T5" s="114" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="113"/>
-      <c r="Y5" s="111" t="s">
+      <c r="U5" s="115"/>
+      <c r="V5" s="115"/>
+      <c r="W5" s="116"/>
+      <c r="Y5" s="114" t="s">
         <v>313</v>
       </c>
-      <c r="Z5" s="112"/>
-      <c r="AA5" s="113"/>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="116"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>31.22</v>
+        <v>32.75</v>
       </c>
       <c r="D6" s="17"/>
       <c r="G6" s="8">
-        <v>45474</v>
+        <v>45505</v>
       </c>
       <c r="H6" s="92" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
@@ -10035,7 +10038,7 @@
       <c r="Y6" s="39" t="s">
         <v>314</v>
       </c>
-      <c r="Z6" s="142"/>
+      <c r="Z6" s="112"/>
       <c r="AA6" s="35"/>
     </row>
     <row r="7" spans="1:29">
@@ -10070,7 +10073,7 @@
       <c r="Y7" s="41" t="s">
         <v>315</v>
       </c>
-      <c r="Z7" s="142"/>
+      <c r="Z7" s="112"/>
       <c r="AA7" s="35"/>
     </row>
     <row r="8" spans="1:29">
@@ -10079,14 +10082,14 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>5733.5529999999999</v>
+        <v>6014.5375000000004</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
         <v>45474</v>
       </c>
       <c r="H8" s="92" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
@@ -10105,7 +10108,7 @@
       <c r="V8" s="34"/>
       <c r="W8" s="35"/>
       <c r="Y8" s="39"/>
-      <c r="Z8" s="142"/>
+      <c r="Z8" s="112"/>
       <c r="AA8" s="35"/>
     </row>
     <row r="9" spans="1:29">
@@ -10140,7 +10143,7 @@
       <c r="Y9" s="39" t="s">
         <v>316</v>
       </c>
-      <c r="Z9" s="142"/>
+      <c r="Z9" s="112"/>
       <c r="AA9" s="35"/>
     </row>
     <row r="10" spans="1:29">
@@ -10155,10 +10158,10 @@
         <v>307</v>
       </c>
       <c r="G10" s="8">
-        <v>45413</v>
+        <v>45474</v>
       </c>
       <c r="H10" s="92" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -10176,7 +10179,7 @@
       <c r="U10" s="34"/>
       <c r="V10" s="34"/>
       <c r="W10" s="35"/>
-      <c r="Y10" s="143" t="s">
+      <c r="Y10" s="113" t="s">
         <v>317</v>
       </c>
       <c r="Z10" s="32"/>
@@ -10218,14 +10221,14 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>6941.2530000000006</v>
+        <v>7222.2375000000011</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
         <v>45413</v>
       </c>
       <c r="H12" s="92" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -10241,13 +10244,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="111" t="s">
+      <c r="Y12" s="114" t="s">
         <v>215</v>
       </c>
-      <c r="Z12" s="112"/>
-      <c r="AA12" s="112"/>
-      <c r="AB12" s="112"/>
-      <c r="AC12" s="113"/>
+      <c r="Z12" s="115"/>
+      <c r="AA12" s="115"/>
+      <c r="AB12" s="115"/>
+      <c r="AC12" s="116"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -10269,21 +10272,21 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="86"/>
-      <c r="Z13" s="135" t="s">
+      <c r="Z13" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="AA13" s="135"/>
-      <c r="AB13" s="135" t="s">
+      <c r="AA13" s="126"/>
+      <c r="AB13" s="126" t="s">
         <v>217</v>
       </c>
-      <c r="AC13" s="136"/>
+      <c r="AC13" s="127"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
-        <v>44986</v>
+        <v>45413</v>
       </c>
       <c r="H14" s="92" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
@@ -10304,21 +10307,21 @@
       <c r="Y14" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="Z14" s="116" t="s">
+      <c r="Z14" s="123" t="s">
         <v>227</v>
       </c>
-      <c r="AA14" s="116"/>
-      <c r="AB14" s="116" t="s">
+      <c r="AA14" s="123"/>
+      <c r="AB14" s="123" t="s">
         <v>228</v>
       </c>
-      <c r="AC14" s="117"/>
+      <c r="AC14" s="122"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="112"/>
-      <c r="D15" s="113"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="116"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -10340,14 +10343,14 @@
       <c r="Y15" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="Z15" s="116" t="s">
+      <c r="Z15" s="123" t="s">
         <v>223</v>
       </c>
-      <c r="AA15" s="116"/>
-      <c r="AB15" s="116" t="s">
+      <c r="AA15" s="123"/>
+      <c r="AB15" s="123" t="s">
         <v>229</v>
       </c>
-      <c r="AC15" s="117"/>
+      <c r="AC15" s="122"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -10356,10 +10359,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="117"/>
+      <c r="D16" s="122"/>
       <c r="E16" s="3" t="s">
         <v>301</v>
       </c>
@@ -10367,7 +10370,7 @@
         <v>44986</v>
       </c>
       <c r="H16" s="92" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
@@ -10388,23 +10391,23 @@
       <c r="Y16" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z16" s="116" t="s">
+      <c r="Z16" s="123" t="s">
         <v>224</v>
       </c>
-      <c r="AA16" s="116"/>
-      <c r="AB16" s="116" t="s">
+      <c r="AA16" s="123"/>
+      <c r="AB16" s="123" t="s">
         <v>230</v>
       </c>
-      <c r="AC16" s="117"/>
+      <c r="AC16" s="122"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="117"/>
+      <c r="D17" s="122"/>
       <c r="E17" s="3" t="s">
         <v>301</v>
       </c>
@@ -10427,24 +10430,24 @@
       <c r="Y17" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z17" s="116" t="s">
+      <c r="Z17" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="AA17" s="116"/>
-      <c r="AB17" s="116" t="s">
+      <c r="AA17" s="123"/>
+      <c r="AB17" s="123" t="s">
         <v>231</v>
       </c>
-      <c r="AC17" s="117"/>
+      <c r="AC17" s="122"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="117"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="122"/>
       <c r="G18" s="8">
         <v>44986</v>
       </c>
       <c r="H18" s="92" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
@@ -10465,19 +10468,19 @@
       <c r="Y18" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z18" s="116" t="s">
+      <c r="Z18" s="123" t="s">
         <v>226</v>
       </c>
-      <c r="AA18" s="116"/>
-      <c r="AB18" s="116" t="s">
+      <c r="AA18" s="123"/>
+      <c r="AB18" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="AC18" s="117"/>
+      <c r="AC18" s="122"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="140"/>
       <c r="G19" s="9"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -10499,21 +10502,21 @@
       <c r="Y19" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="Z19" s="116" t="s">
+      <c r="Z19" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="AA19" s="116"/>
-      <c r="AB19" s="116" t="s">
+      <c r="AA19" s="123"/>
+      <c r="AB19" s="123" t="s">
         <v>235</v>
       </c>
-      <c r="AC19" s="117"/>
+      <c r="AC19" s="122"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="8">
-        <v>45261</v>
+        <v>44986</v>
       </c>
       <c r="H20" s="92" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
@@ -10534,14 +10537,14 @@
       <c r="Y20" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="Z20" s="116" t="s">
+      <c r="Z20" s="123" t="s">
         <v>240</v>
       </c>
-      <c r="AA20" s="116"/>
-      <c r="AB20" s="116" t="s">
+      <c r="AA20" s="123"/>
+      <c r="AB20" s="123" t="s">
         <v>241</v>
       </c>
-      <c r="AC20" s="117"/>
+      <c r="AC20" s="122"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -10569,16 +10572,16 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="112"/>
-      <c r="D22" s="113"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="116"/>
       <c r="G22" s="8">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="H22" s="92" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
@@ -10606,10 +10609,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="123" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="117"/>
+      <c r="D23" s="122"/>
       <c r="G23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -10631,15 +10634,15 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="116">
+      <c r="C24" s="123">
         <v>1969</v>
       </c>
-      <c r="D24" s="117"/>
+      <c r="D24" s="122"/>
       <c r="G24" s="8">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="H24" s="92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
@@ -10660,8 +10663,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="117"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="122"/>
       <c r="G25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -10680,28 +10683,28 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="120" t="s">
+      <c r="Y25" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="Z25" s="121"/>
-      <c r="AA25" s="121"/>
-      <c r="AB25" s="121"/>
-      <c r="AC25" s="122"/>
+      <c r="Z25" s="142"/>
+      <c r="AA25" s="142"/>
+      <c r="AB25" s="142"/>
+      <c r="AC25" s="143"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="114">
+      <c r="C26" s="137">
         <f>'Financial Model'!Z70</f>
         <v>2636</v>
       </c>
-      <c r="D26" s="115"/>
+      <c r="D26" s="138"/>
       <c r="G26" s="8">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="H26" s="92" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
@@ -10729,8 +10732,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="117"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="122"/>
       <c r="G27" s="9"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -10761,16 +10764,16 @@
       <c r="B28" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="C28" s="132">
+      <c r="C28" s="121">
         <f>+'Order &amp; Backlog'!$AA$3</f>
         <v>2200</v>
       </c>
-      <c r="D28" s="117"/>
+      <c r="D28" s="122"/>
       <c r="G28" s="8">
-        <v>45017</v>
+        <v>45170</v>
       </c>
       <c r="H28" s="92" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I28" s="34"/>
       <c r="J28" s="34"/>
@@ -10800,11 +10803,11 @@
       <c r="B29" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="132">
+      <c r="C29" s="121">
         <f>'Order &amp; Backlog'!AA21</f>
         <v>382</v>
       </c>
-      <c r="D29" s="117"/>
+      <c r="D29" s="122"/>
       <c r="G29" s="9"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
@@ -10833,16 +10836,16 @@
       <c r="B30" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="116">
+      <c r="C30" s="123">
         <f>'Financial Model'!AB43</f>
         <v>47</v>
       </c>
-      <c r="D30" s="117"/>
+      <c r="D30" s="122"/>
       <c r="G30" s="8">
         <v>45017</v>
       </c>
-      <c r="H30" s="98" t="s">
-        <v>266</v>
+      <c r="H30" s="92" t="s">
+        <v>269</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
@@ -10870,10 +10873,10 @@
       <c r="B31" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C31" s="139">
+      <c r="C31" s="124">
         <v>36708</v>
       </c>
-      <c r="D31" s="140"/>
+      <c r="D31" s="125"/>
       <c r="G31" s="9"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -10902,13 +10905,13 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="116"/>
-      <c r="D32" s="117"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="122"/>
       <c r="G32" s="8">
-        <v>44927</v>
-      </c>
-      <c r="H32" s="94" t="s">
-        <v>263</v>
+        <v>45017</v>
+      </c>
+      <c r="H32" s="98" t="s">
+        <v>266</v>
       </c>
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
@@ -10970,15 +10973,15 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="128" t="s">
+      <c r="C34" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="129"/>
+      <c r="D34" s="134"/>
       <c r="G34" s="8">
-        <v>44896</v>
-      </c>
-      <c r="H34" s="92" t="s">
-        <v>261</v>
+        <v>44927</v>
+      </c>
+      <c r="H34" s="94" t="s">
+        <v>263</v>
       </c>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
@@ -11025,10 +11028,10 @@
     </row>
     <row r="36" spans="2:29">
       <c r="G36" s="8">
-        <v>44866</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>259</v>
+        <v>44896</v>
+      </c>
+      <c r="H36" s="92" t="s">
+        <v>261</v>
       </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
@@ -11047,11 +11050,11 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="111" t="s">
+      <c r="B37" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="112"/>
-      <c r="D37" s="113"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="116"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -11064,12 +11067,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="111" t="s">
+      <c r="T37" s="114" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="112"/>
-      <c r="V37" s="112"/>
-      <c r="W37" s="113"/>
+      <c r="U37" s="115"/>
+      <c r="V37" s="115"/>
+      <c r="W37" s="116"/>
       <c r="Y37" s="39" t="s">
         <v>278</v>
       </c>
@@ -11082,16 +11085,16 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="130">
+      <c r="C38" s="135">
         <f>C6/'Financial Model'!AB125</f>
-        <v>7.3653452373305992</v>
-      </c>
-      <c r="D38" s="131"/>
+        <v>7.7262990558160523</v>
+      </c>
+      <c r="D38" s="136"/>
       <c r="G38" s="8">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -11121,11 +11124,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="130">
+      <c r="C39" s="135">
         <f>+C8/SUM('Financial Model'!Y4:AB4)</f>
-        <v>2.9702911464539192</v>
-      </c>
-      <c r="D39" s="131"/>
+        <v>3.115856343573538</v>
+      </c>
+      <c r="D39" s="136"/>
       <c r="G39" s="9"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -11154,13 +11157,17 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="126">
+      <c r="C40" s="131">
         <f>C6/SUM('Financial Model'!Y26:AB26)</f>
-        <v>60.084390882892329</v>
-      </c>
-      <c r="D40" s="127"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="34"/>
+        <v>63.028949436730421</v>
+      </c>
+      <c r="D40" s="132"/>
+      <c r="G40" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
       <c r="K40" s="34"/>
@@ -11184,12 +11191,8 @@
       <c r="AC40" s="35"/>
     </row>
     <row r="41" spans="2:29">
-      <c r="G41" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="G41" s="9"/>
+      <c r="H41" s="34"/>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
       <c r="K41" s="34"/>
@@ -11214,9 +11217,7 @@
     </row>
     <row r="42" spans="2:29">
       <c r="G42" s="9"/>
-      <c r="H42" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="H42" s="34"/>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
       <c r="K42" s="34"/>
@@ -11238,14 +11239,16 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="111" t="s">
+      <c r="B43" s="114" t="s">
         <v>243</v>
       </c>
-      <c r="C43" s="112"/>
-      <c r="D43" s="113"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="7" t="s">
-        <v>13</v>
+      <c r="C43" s="115"/>
+      <c r="D43" s="116"/>
+      <c r="G43" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
@@ -11272,15 +11275,17 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="133" t="s">
+      <c r="B44" s="117" t="s">
         <v>244</v>
       </c>
-      <c r="C44" s="134"/>
+      <c r="C44" s="118"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
       <c r="G44" s="9"/>
-      <c r="H44" s="34"/>
+      <c r="H44" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="I44" s="34"/>
       <c r="J44" s="34"/>
       <c r="K44" s="34"/>
@@ -11306,18 +11311,16 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="133" t="s">
+      <c r="B45" s="117" t="s">
         <v>245</v>
       </c>
-      <c r="C45" s="134"/>
+      <c r="C45" s="118"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G45" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>29</v>
+      <c r="G45" s="9"/>
+      <c r="H45" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
@@ -11344,15 +11347,13 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="133"/>
-      <c r="C46" s="134"/>
+      <c r="B46" s="117"/>
+      <c r="C46" s="118"/>
       <c r="D46" s="83" t="s">
         <v>31</v>
       </c>
       <c r="G46" s="9"/>
-      <c r="H46" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="H46" s="34"/>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
@@ -11374,13 +11375,17 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="133"/>
-      <c r="C47" s="134"/>
+      <c r="B47" s="117"/>
+      <c r="C47" s="118"/>
       <c r="D47" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="34"/>
+      <c r="G47" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="I47" s="34"/>
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
@@ -11406,13 +11411,15 @@
       <c r="AC47" s="35"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="137"/>
-      <c r="C48" s="138"/>
+      <c r="B48" s="119"/>
+      <c r="C48" s="120"/>
       <c r="D48" s="84" t="s">
         <v>31</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" s="34"/>
+      <c r="H48" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
@@ -11438,12 +11445,8 @@
       <c r="AC48" s="35"/>
     </row>
     <row r="49" spans="7:29">
-      <c r="G49" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>187</v>
-      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="34"/>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
@@ -11490,8 +11493,12 @@
       <c r="AC50" s="35"/>
     </row>
     <row r="51" spans="7:29">
-      <c r="G51" s="9"/>
-      <c r="H51" s="34"/>
+      <c r="G51" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
@@ -11511,12 +11518,8 @@
       <c r="AC51" s="35"/>
     </row>
     <row r="52" spans="7:29">
-      <c r="G52" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="G52" s="9"/>
+      <c r="H52" s="34"/>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
       <c r="K52" s="34"/>
@@ -11535,9 +11538,7 @@
     </row>
     <row r="53" spans="7:29">
       <c r="G53" s="9"/>
-      <c r="H53" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="H53" s="34"/>
       <c r="I53" s="34"/>
       <c r="J53" s="34"/>
       <c r="K53" s="34"/>
@@ -11557,9 +11558,11 @@
       <c r="AC53" s="35"/>
     </row>
     <row r="54" spans="7:29">
-      <c r="G54" s="9"/>
-      <c r="H54" s="7" t="s">
-        <v>193</v>
+      <c r="G54" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
@@ -11582,7 +11585,7 @@
     <row r="55" spans="7:29">
       <c r="G55" s="9"/>
       <c r="H55" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I55" s="34"/>
       <c r="J55" s="34"/>
@@ -11593,9 +11596,7 @@
       <c r="O55" s="34"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="34"/>
-      <c r="R55" s="48" t="s">
-        <v>194</v>
-      </c>
+      <c r="R55" s="35"/>
       <c r="Y55" s="100" t="s">
         <v>292</v>
       </c>
@@ -11606,7 +11607,9 @@
     </row>
     <row r="56" spans="7:29">
       <c r="G56" s="9"/>
-      <c r="H56" s="34"/>
+      <c r="H56" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
       <c r="K56" s="34"/>
@@ -11625,7 +11628,9 @@
     </row>
     <row r="57" spans="7:29">
       <c r="G57" s="9"/>
-      <c r="H57" s="34"/>
+      <c r="H57" s="7" t="s">
+        <v>191</v>
+      </c>
       <c r="I57" s="34"/>
       <c r="J57" s="34"/>
       <c r="K57" s="34"/>
@@ -11635,7 +11640,9 @@
       <c r="O57" s="34"/>
       <c r="P57" s="34"/>
       <c r="Q57" s="34"/>
-      <c r="R57" s="35"/>
+      <c r="R57" s="48" t="s">
+        <v>194</v>
+      </c>
       <c r="Y57" s="101"/>
       <c r="Z57" s="102"/>
       <c r="AA57" s="102"/>
@@ -11643,12 +11650,8 @@
       <c r="AC57" s="103"/>
     </row>
     <row r="58" spans="7:29">
-      <c r="G58" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>196</v>
-      </c>
+      <c r="G58" s="9"/>
+      <c r="H58" s="34"/>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
@@ -11659,19 +11662,17 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
-      <c r="Y58" s="123" t="s">
+      <c r="Y58" s="128" t="s">
         <v>293</v>
       </c>
-      <c r="Z58" s="124"/>
-      <c r="AA58" s="124"/>
-      <c r="AB58" s="124"/>
-      <c r="AC58" s="125"/>
+      <c r="Z58" s="129"/>
+      <c r="AA58" s="129"/>
+      <c r="AB58" s="129"/>
+      <c r="AC58" s="130"/>
     </row>
     <row r="59" spans="7:29">
       <c r="G59" s="9"/>
-      <c r="H59" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="H59" s="34"/>
       <c r="I59" s="34"/>
       <c r="J59" s="34"/>
       <c r="K59" s="34"/>
@@ -11684,9 +11685,11 @@
       <c r="R59" s="35"/>
     </row>
     <row r="60" spans="7:29">
-      <c r="G60" s="9"/>
-      <c r="H60" s="47" t="s">
-        <v>198</v>
+      <c r="G60" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
@@ -11701,7 +11704,9 @@
     </row>
     <row r="61" spans="7:29">
       <c r="G61" s="9"/>
-      <c r="H61" s="34"/>
+      <c r="H61" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="I61" s="34"/>
       <c r="J61" s="34"/>
       <c r="K61" s="34"/>
@@ -11714,11 +11719,9 @@
       <c r="R61" s="35"/>
     </row>
     <row r="62" spans="7:29">
-      <c r="G62" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>237</v>
+      <c r="G62" s="9"/>
+      <c r="H62" s="47" t="s">
+        <v>198</v>
       </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
@@ -11733,9 +11736,7 @@
     </row>
     <row r="63" spans="7:29">
       <c r="G63" s="9"/>
-      <c r="H63" s="7" t="s">
-        <v>238</v>
-      </c>
+      <c r="H63" s="34"/>
       <c r="I63" s="34"/>
       <c r="J63" s="34"/>
       <c r="K63" s="34"/>
@@ -11748,8 +11749,12 @@
       <c r="R63" s="35"/>
     </row>
     <row r="64" spans="7:29">
-      <c r="G64" s="9"/>
-      <c r="H64" s="34"/>
+      <c r="G64" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>237</v>
+      </c>
       <c r="I64" s="34"/>
       <c r="J64" s="34"/>
       <c r="K64" s="34"/>
@@ -11762,11 +11767,9 @@
       <c r="R64" s="35"/>
     </row>
     <row r="65" spans="7:18">
-      <c r="G65" s="8">
-        <v>44682</v>
-      </c>
-      <c r="H65" s="34" t="s">
-        <v>246</v>
+      <c r="G65" s="9"/>
+      <c r="H65" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="I65" s="34"/>
       <c r="J65" s="34"/>
@@ -11781,9 +11784,7 @@
     </row>
     <row r="66" spans="7:18">
       <c r="G66" s="9"/>
-      <c r="H66" s="7" t="s">
-        <v>247</v>
-      </c>
+      <c r="H66" s="34"/>
       <c r="I66" s="34"/>
       <c r="J66" s="34"/>
       <c r="K66" s="34"/>
@@ -11793,13 +11794,15 @@
       <c r="O66" s="34"/>
       <c r="P66" s="34"/>
       <c r="Q66" s="34"/>
-      <c r="R66" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R66" s="35"/>
     </row>
     <row r="67" spans="7:18">
-      <c r="G67" s="9"/>
-      <c r="H67" s="34"/>
+      <c r="G67" s="8">
+        <v>44682</v>
+      </c>
+      <c r="H67" s="34" t="s">
+        <v>246</v>
+      </c>
       <c r="I67" s="34"/>
       <c r="J67" s="34"/>
       <c r="K67" s="34"/>
@@ -11812,11 +11815,9 @@
       <c r="R67" s="35"/>
     </row>
     <row r="68" spans="7:18">
-      <c r="G68" s="8">
-        <v>43922</v>
-      </c>
-      <c r="H68" s="34" t="s">
-        <v>164</v>
+      <c r="G68" s="9"/>
+      <c r="H68" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
@@ -11827,13 +11828,13 @@
       <c r="O68" s="34"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="34"/>
-      <c r="R68" s="35"/>
+      <c r="R68" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="69" spans="7:18">
       <c r="G69" s="9"/>
-      <c r="H69" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="H69" s="34"/>
       <c r="I69" s="34"/>
       <c r="J69" s="34"/>
       <c r="K69" s="34"/>
@@ -11846,8 +11847,12 @@
       <c r="R69" s="35"/>
     </row>
     <row r="70" spans="7:18">
-      <c r="G70" s="9"/>
-      <c r="H70" s="34"/>
+      <c r="G70" s="8">
+        <v>43922</v>
+      </c>
+      <c r="H70" s="34" t="s">
+        <v>164</v>
+      </c>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>
       <c r="K70" s="34"/>
@@ -11857,13 +11862,13 @@
       <c r="O70" s="34"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="34"/>
-      <c r="R70" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R70" s="35"/>
     </row>
     <row r="71" spans="7:18">
       <c r="G71" s="9"/>
-      <c r="H71" s="34"/>
+      <c r="H71" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="I71" s="34"/>
       <c r="J71" s="34"/>
       <c r="K71" s="34"/>
@@ -11876,12 +11881,8 @@
       <c r="R71" s="35"/>
     </row>
     <row r="72" spans="7:18">
-      <c r="G72" s="8">
-        <v>43770</v>
-      </c>
-      <c r="H72" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="G72" s="9"/>
+      <c r="H72" s="34"/>
       <c r="I72" s="34"/>
       <c r="J72" s="34"/>
       <c r="K72" s="34"/>
@@ -11891,13 +11892,13 @@
       <c r="O72" s="34"/>
       <c r="P72" s="34"/>
       <c r="Q72" s="34"/>
-      <c r="R72" s="35"/>
+      <c r="R72" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="73" spans="7:18">
       <c r="G73" s="9"/>
-      <c r="H73" s="47" t="s">
-        <v>168</v>
-      </c>
+      <c r="H73" s="34"/>
       <c r="I73" s="34"/>
       <c r="J73" s="34"/>
       <c r="K73" s="34"/>
@@ -11910,8 +11911,12 @@
       <c r="R73" s="35"/>
     </row>
     <row r="74" spans="7:18">
-      <c r="G74" s="9"/>
-      <c r="H74" s="34"/>
+      <c r="G74" s="8">
+        <v>43770</v>
+      </c>
+      <c r="H74" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="I74" s="34"/>
       <c r="J74" s="34"/>
       <c r="K74" s="34"/>
@@ -11924,11 +11929,9 @@
       <c r="R74" s="35"/>
     </row>
     <row r="75" spans="7:18">
-      <c r="G75" s="8">
-        <v>43739</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>242</v>
+      <c r="G75" s="9"/>
+      <c r="H75" s="47" t="s">
+        <v>168</v>
       </c>
       <c r="I75" s="34"/>
       <c r="J75" s="34"/>
@@ -11938,9 +11941,7 @@
       <c r="N75" s="34"/>
       <c r="O75" s="34"/>
       <c r="P75" s="34"/>
-      <c r="Q75" s="34" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q75" s="34"/>
       <c r="R75" s="35"/>
     </row>
     <row r="76" spans="7:18">
@@ -11958,8 +11959,12 @@
       <c r="R76" s="35"/>
     </row>
     <row r="77" spans="7:18">
-      <c r="G77" s="9"/>
-      <c r="H77" s="34"/>
+      <c r="G77" s="8">
+        <v>43739</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="I77" s="34"/>
       <c r="J77" s="34"/>
       <c r="K77" s="34"/>
@@ -11968,7 +11973,9 @@
       <c r="N77" s="34"/>
       <c r="O77" s="34"/>
       <c r="P77" s="34"/>
-      <c r="Q77" s="34"/>
+      <c r="Q77" s="34" t="s">
+        <v>179</v>
+      </c>
       <c r="R77" s="35"/>
     </row>
     <row r="78" spans="7:18">
@@ -11986,12 +11993,8 @@
       <c r="R78" s="35"/>
     </row>
     <row r="79" spans="7:18">
-      <c r="G79" s="8">
-        <v>43586</v>
-      </c>
-      <c r="H79" s="34" t="s">
-        <v>166</v>
-      </c>
+      <c r="G79" s="9"/>
+      <c r="H79" s="34"/>
       <c r="I79" s="34"/>
       <c r="J79" s="34"/>
       <c r="K79" s="34"/>
@@ -12019,10 +12022,10 @@
     </row>
     <row r="81" spans="7:18">
       <c r="G81" s="8">
-        <v>43282</v>
+        <v>43586</v>
       </c>
       <c r="H81" s="34" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I81" s="34"/>
       <c r="J81" s="34"/>
@@ -12037,9 +12040,7 @@
     </row>
     <row r="82" spans="7:18">
       <c r="G82" s="9"/>
-      <c r="H82" s="7" t="s">
-        <v>163</v>
-      </c>
+      <c r="H82" s="34"/>
       <c r="I82" s="34"/>
       <c r="J82" s="34"/>
       <c r="K82" s="34"/>
@@ -12052,9 +12053,11 @@
       <c r="R82" s="35"/>
     </row>
     <row r="83" spans="7:18">
-      <c r="G83" s="9"/>
-      <c r="H83" s="7" t="s">
-        <v>165</v>
+      <c r="G83" s="8">
+        <v>43282</v>
+      </c>
+      <c r="H83" s="34" t="s">
+        <v>162</v>
       </c>
       <c r="I83" s="34"/>
       <c r="J83" s="34"/>
@@ -12069,7 +12072,9 @@
     </row>
     <row r="84" spans="7:18">
       <c r="G84" s="9"/>
-      <c r="H84" s="34"/>
+      <c r="H84" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="I84" s="34"/>
       <c r="J84" s="34"/>
       <c r="K84" s="34"/>
@@ -12082,42 +12087,68 @@
       <c r="R84" s="35"/>
     </row>
     <row r="85" spans="7:18">
-      <c r="G85" s="85">
+      <c r="G85" s="9"/>
+      <c r="H85" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I85" s="34"/>
+      <c r="J85" s="34"/>
+      <c r="K85" s="34"/>
+      <c r="L85" s="34"/>
+      <c r="M85" s="34"/>
+      <c r="N85" s="34"/>
+      <c r="O85" s="34"/>
+      <c r="P85" s="34"/>
+      <c r="Q85" s="34"/>
+      <c r="R85" s="35"/>
+    </row>
+    <row r="86" spans="7:18">
+      <c r="G86" s="9"/>
+      <c r="H86" s="34"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="34"/>
+      <c r="K86" s="34"/>
+      <c r="L86" s="34"/>
+      <c r="M86" s="34"/>
+      <c r="N86" s="34"/>
+      <c r="O86" s="34"/>
+      <c r="P86" s="34"/>
+      <c r="Q86" s="34"/>
+      <c r="R86" s="35"/>
+    </row>
+    <row r="87" spans="7:18">
+      <c r="G87" s="85">
         <v>42552</v>
       </c>
-      <c r="H85" s="51" t="s">
+      <c r="H87" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="I85" s="32"/>
-      <c r="J85" s="32"/>
-      <c r="K85" s="32"/>
-      <c r="L85" s="32"/>
-      <c r="M85" s="32"/>
-      <c r="N85" s="32"/>
-      <c r="O85" s="32"/>
-      <c r="P85" s="32"/>
-      <c r="Q85" s="32"/>
-      <c r="R85" s="33"/>
+      <c r="I87" s="32"/>
+      <c r="J87" s="32"/>
+      <c r="K87" s="32"/>
+      <c r="L87" s="32"/>
+      <c r="M87" s="32"/>
+      <c r="N87" s="32"/>
+      <c r="O87" s="32"/>
+      <c r="P87" s="32"/>
+      <c r="Q87" s="32"/>
+      <c r="R87" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="AB16:AC16"/>
     <mergeCell ref="AB17:AC17"/>
     <mergeCell ref="AB18:AC18"/>
@@ -12134,67 +12165,72 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="B37:D37"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Y25:AC25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H41" r:id="rId1" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H45" r:id="rId2" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
-    <hyperlink ref="C34:D34" r:id="rId3" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
-    <hyperlink ref="R70" r:id="rId4" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H49" r:id="rId5" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H52" r:id="rId6" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R55" r:id="rId7" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H58" r:id="rId8" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
-    <hyperlink ref="W49" r:id="rId9" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
-    <hyperlink ref="Z13:AA13" r:id="rId10" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
-    <hyperlink ref="AB13:AC13" r:id="rId11" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
-    <hyperlink ref="H62" r:id="rId12" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H75" r:id="rId13" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
-    <hyperlink ref="D45" r:id="rId14" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
-    <hyperlink ref="D44" r:id="rId15" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
-    <hyperlink ref="R66" r:id="rId16" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H38" r:id="rId17" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
-    <hyperlink ref="H36" r:id="rId18" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
-    <hyperlink ref="H34" r:id="rId19" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
-    <hyperlink ref="H32" r:id="rId20" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
-    <hyperlink ref="H30" r:id="rId21" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
-    <hyperlink ref="H28" r:id="rId22" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
-    <hyperlink ref="H26" r:id="rId23" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
-    <hyperlink ref="Y25:AC25" r:id="rId24" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
-    <hyperlink ref="H20" r:id="rId25" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
-    <hyperlink ref="H22" r:id="rId26" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
-    <hyperlink ref="H24" r:id="rId27" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
-    <hyperlink ref="H18" r:id="rId28" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
-    <hyperlink ref="H16" r:id="rId29" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
-    <hyperlink ref="H14" r:id="rId30" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
-    <hyperlink ref="H12" r:id="rId31" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
-    <hyperlink ref="H10" r:id="rId32" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
-    <hyperlink ref="H8" r:id="rId33" xr:uid="{DE4DB842-01BE-405E-8254-AC1C82253C72}"/>
-    <hyperlink ref="H6" r:id="rId34" xr:uid="{645C2C50-2541-448D-9073-14E40D1DE986}"/>
+    <hyperlink ref="C34:D34" r:id="rId1" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
+    <hyperlink ref="W49" r:id="rId2" xr:uid="{F9FF1395-9489-4EC9-819E-D412DF0569AE}"/>
+    <hyperlink ref="Z13:AA13" r:id="rId3" display="A220-300" xr:uid="{76602C0E-D63D-8640-97A0-C7DAD332148A}"/>
+    <hyperlink ref="AB13:AC13" r:id="rId4" display="E195-E2" xr:uid="{A43FCCB3-64E0-D54D-A779-4F0C857321F6}"/>
+    <hyperlink ref="D45" r:id="rId5" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
+    <hyperlink ref="D44" r:id="rId6" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
+    <hyperlink ref="Y25:AC25" r:id="rId7" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
+    <hyperlink ref="H8" r:id="rId8" xr:uid="{645C2C50-2541-448D-9073-14E40D1DE986}"/>
+    <hyperlink ref="H43" r:id="rId9" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H47" r:id="rId10" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="R72" r:id="rId11" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H51" r:id="rId12" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H54" r:id="rId13" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R57" r:id="rId14" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H60" r:id="rId15" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="H64" r:id="rId16" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H77" r:id="rId17" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="R68" r:id="rId18" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H40" r:id="rId19" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H38" r:id="rId20" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
+    <hyperlink ref="H36" r:id="rId21" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
+    <hyperlink ref="H34" r:id="rId22" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
+    <hyperlink ref="H32" r:id="rId23" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
+    <hyperlink ref="H30" r:id="rId24" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="H28" r:id="rId25" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
+    <hyperlink ref="H22" r:id="rId26" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
+    <hyperlink ref="H24" r:id="rId27" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
+    <hyperlink ref="H26" r:id="rId28" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
+    <hyperlink ref="H20" r:id="rId29" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
+    <hyperlink ref="H18" r:id="rId30" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
+    <hyperlink ref="H16" r:id="rId31" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
+    <hyperlink ref="H14" r:id="rId32" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
+    <hyperlink ref="H12" r:id="rId33" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
+    <hyperlink ref="H10" r:id="rId34" xr:uid="{DE4DB842-01BE-405E-8254-AC1C82253C72}"/>
+    <hyperlink ref="H6" r:id="rId35" xr:uid="{098F501F-A48C-49AD-B4EE-8F3B4711DA32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId35"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId36"/>
   <ignoredErrors>
     <ignoredError sqref="C39:D40" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId36"/>
+  <drawing r:id="rId37"/>
 </worksheet>
 </file>
 
@@ -16642,7 +16678,7 @@
         <v>74</v>
       </c>
       <c r="AA43" s="2">
-        <f t="shared" ref="AA43:AB43" si="150">AA44+AA52</f>
+        <f t="shared" ref="AA43" si="150">AA44+AA52</f>
         <v>25</v>
       </c>
       <c r="AB43" s="2">
@@ -18030,79 +18066,79 @@
       <c r="B57" s="45" t="s">
         <v>312</v>
       </c>
-      <c r="C57" s="141">
-        <v>0</v>
-      </c>
-      <c r="D57" s="141">
-        <v>0</v>
-      </c>
-      <c r="E57" s="141">
-        <v>0</v>
-      </c>
-      <c r="F57" s="141">
-        <v>0</v>
-      </c>
-      <c r="G57" s="141">
-        <v>0</v>
-      </c>
-      <c r="H57" s="141">
-        <v>0</v>
-      </c>
-      <c r="I57" s="141">
-        <v>0</v>
-      </c>
-      <c r="J57" s="141">
-        <v>0</v>
-      </c>
-      <c r="K57" s="141">
-        <v>0</v>
-      </c>
-      <c r="L57" s="141">
-        <v>0</v>
-      </c>
-      <c r="M57" s="141">
-        <v>0</v>
-      </c>
-      <c r="N57" s="141">
-        <v>0</v>
-      </c>
-      <c r="O57" s="141">
-        <v>0</v>
-      </c>
-      <c r="P57" s="141">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="141">
-        <v>0</v>
-      </c>
-      <c r="R57" s="141">
-        <v>0</v>
-      </c>
-      <c r="S57" s="141">
-        <v>0</v>
-      </c>
-      <c r="T57" s="141">
-        <v>0</v>
-      </c>
-      <c r="U57" s="141">
-        <v>0</v>
-      </c>
-      <c r="V57" s="141">
-        <v>0</v>
-      </c>
-      <c r="W57" s="141">
-        <v>0</v>
-      </c>
-      <c r="X57" s="141">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="141">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="141">
-        <v>0</v>
-      </c>
-      <c r="AA57" s="141">
+      <c r="C57" s="111">
+        <v>0</v>
+      </c>
+      <c r="D57" s="111">
+        <v>0</v>
+      </c>
+      <c r="E57" s="111">
+        <v>0</v>
+      </c>
+      <c r="F57" s="111">
+        <v>0</v>
+      </c>
+      <c r="G57" s="111">
+        <v>0</v>
+      </c>
+      <c r="H57" s="111">
+        <v>0</v>
+      </c>
+      <c r="I57" s="111">
+        <v>0</v>
+      </c>
+      <c r="J57" s="111">
+        <v>0</v>
+      </c>
+      <c r="K57" s="111">
+        <v>0</v>
+      </c>
+      <c r="L57" s="111">
+        <v>0</v>
+      </c>
+      <c r="M57" s="111">
+        <v>0</v>
+      </c>
+      <c r="N57" s="111">
+        <v>0</v>
+      </c>
+      <c r="O57" s="111">
+        <v>0</v>
+      </c>
+      <c r="P57" s="111">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="111">
+        <v>0</v>
+      </c>
+      <c r="R57" s="111">
+        <v>0</v>
+      </c>
+      <c r="S57" s="111">
+        <v>0</v>
+      </c>
+      <c r="T57" s="111">
+        <v>0</v>
+      </c>
+      <c r="U57" s="111">
+        <v>0</v>
+      </c>
+      <c r="V57" s="111">
+        <v>0</v>
+      </c>
+      <c r="W57" s="111">
+        <v>0</v>
+      </c>
+      <c r="X57" s="111">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="111">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="111">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="111">
         <v>0</v>
       </c>
       <c r="AB57" s="36">
@@ -29082,11 +29118,11 @@
         <v>568</v>
       </c>
       <c r="Z6" s="72">
-        <f>+Y6</f>
+        <f t="shared" ref="Z6:AA8" si="19">+Y6</f>
         <v>568</v>
       </c>
       <c r="AA6" s="72">
-        <f>+Z6</f>
+        <f t="shared" si="19"/>
         <v>568</v>
       </c>
       <c r="AC6" s="72">
@@ -29191,11 +29227,11 @@
         <v>172</v>
       </c>
       <c r="Z7" s="72">
-        <f>+Y7</f>
+        <f t="shared" si="19"/>
         <v>172</v>
       </c>
       <c r="AA7" s="72">
-        <f>+Z7</f>
+        <f t="shared" si="19"/>
         <v>172</v>
       </c>
       <c r="AC7" s="72">
@@ -29300,11 +29336,11 @@
         <v>0</v>
       </c>
       <c r="Z8" s="72">
-        <f>+Y8</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA8" s="72">
-        <f>+Z8</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC8" s="72">
@@ -29552,139 +29588,139 @@
         <v>208</v>
       </c>
       <c r="B12" s="71">
-        <f t="shared" ref="B12:S12" si="19">SUM(B13:B19)</f>
+        <f t="shared" ref="B12:S12" si="20">SUM(B13:B19)</f>
         <v>1414</v>
       </c>
       <c r="C12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1442</v>
       </c>
       <c r="D12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1457</v>
       </c>
       <c r="E12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1490</v>
       </c>
       <c r="F12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1501</v>
       </c>
       <c r="G12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1527</v>
       </c>
       <c r="H12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1544</v>
       </c>
       <c r="I12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1579</v>
       </c>
       <c r="J12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1584</v>
       </c>
       <c r="K12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1588</v>
       </c>
       <c r="L12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1595</v>
       </c>
       <c r="M12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1623</v>
       </c>
       <c r="N12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1632</v>
       </c>
       <c r="O12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1646</v>
       </c>
       <c r="P12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1655</v>
       </c>
       <c r="Q12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1671</v>
       </c>
       <c r="R12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1677</v>
       </c>
       <c r="S12" s="71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1688</v>
       </c>
       <c r="T12" s="71">
-        <f t="shared" ref="T12:AA12" si="20">SUM(T13:T19)</f>
+        <f t="shared" ref="T12:AA12" si="21">SUM(T13:T19)</f>
         <v>1698</v>
       </c>
       <c r="U12" s="71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1728</v>
       </c>
       <c r="V12" s="71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1735</v>
       </c>
       <c r="W12" s="71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1752</v>
       </c>
       <c r="X12" s="71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1767</v>
       </c>
       <c r="Y12" s="71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1797</v>
       </c>
       <c r="Z12" s="71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1804</v>
       </c>
       <c r="AA12" s="71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1823</v>
       </c>
       <c r="AC12" s="71">
-        <f t="shared" ref="AC12:AJ12" si="21">SUM(AC13:AC19)</f>
+        <f t="shared" ref="AC12:AJ12" si="22">SUM(AC13:AC19)</f>
         <v>1090</v>
       </c>
       <c r="AD12" s="71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1181</v>
       </c>
       <c r="AE12" s="71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1299</v>
       </c>
       <c r="AF12" s="71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1400</v>
       </c>
       <c r="AG12" s="71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1490</v>
       </c>
       <c r="AH12" s="71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1579</v>
       </c>
       <c r="AI12" s="71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1623</v>
       </c>
       <c r="AJ12" s="71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1671</v>
       </c>
     </row>
@@ -29989,7 +30025,7 @@
         <v>571</v>
       </c>
       <c r="AA15" s="72">
-        <f t="shared" ref="AA15:AA17" si="22">+Z15</f>
+        <f t="shared" ref="AA15:AA17" si="23">+Z15</f>
         <v>571</v>
       </c>
       <c r="AC15" s="72">
@@ -30098,7 +30134,7 @@
         <v>172</v>
       </c>
       <c r="AA16" s="72">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>172</v>
       </c>
       <c r="AC16" s="72">
@@ -30206,7 +30242,7 @@
         <v>0</v>
       </c>
       <c r="AA17" s="72">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AC17" s="72">
@@ -30462,139 +30498,139 @@
         <v>207</v>
       </c>
       <c r="B21" s="71">
-        <f t="shared" ref="B21:AA21" si="23">SUM(B22:B28)</f>
+        <f t="shared" ref="B21:AA21" si="24">SUM(B22:B28)</f>
         <v>421</v>
       </c>
       <c r="C21" s="71">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>360</v>
       </c>
       <c r="D21" s="71">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>251</v>
       </c>
       <c r="E21" s="71">
-        <f t="shared" si="23"/>
-        <v>368</v>
-      </c>
-      <c r="F21" s="71">
-        <f t="shared" si="23"/>
-        <v>359</v>
-      </c>
-      <c r="G21" s="71">
-        <f t="shared" si="23"/>
-        <v>363</v>
-      </c>
-      <c r="H21" s="71">
-        <f t="shared" si="23"/>
-        <v>345</v>
-      </c>
-      <c r="I21" s="71">
-        <f t="shared" si="23"/>
-        <v>338</v>
-      </c>
-      <c r="J21" s="71">
-        <f t="shared" si="23"/>
-        <v>318</v>
-      </c>
-      <c r="K21" s="71">
-        <f t="shared" si="23"/>
-        <v>314</v>
-      </c>
-      <c r="L21" s="71">
-        <f t="shared" si="23"/>
-        <v>307</v>
-      </c>
-      <c r="M21" s="71">
-        <f t="shared" si="23"/>
-        <v>281</v>
-      </c>
-      <c r="N21" s="71">
-        <f t="shared" si="23"/>
-        <v>272</v>
-      </c>
-      <c r="O21" s="71">
-        <f t="shared" si="23"/>
-        <v>306</v>
-      </c>
-      <c r="P21" s="71">
-        <f t="shared" si="23"/>
-        <v>313</v>
-      </c>
-      <c r="Q21" s="71">
-        <f t="shared" si="23"/>
-        <v>325</v>
-      </c>
-      <c r="R21" s="71">
-        <f t="shared" si="23"/>
-        <v>315</v>
-      </c>
-      <c r="S21" s="71">
-        <f t="shared" si="23"/>
-        <v>312</v>
-      </c>
-      <c r="T21" s="71">
-        <f t="shared" si="23"/>
-        <v>297</v>
-      </c>
-      <c r="U21" s="71">
-        <f t="shared" si="23"/>
-        <v>291</v>
-      </c>
-      <c r="V21" s="71">
-        <f t="shared" si="23"/>
-        <v>281</v>
-      </c>
-      <c r="W21" s="71">
-        <f t="shared" si="23"/>
-        <v>271</v>
-      </c>
-      <c r="X21" s="71">
-        <f t="shared" si="23"/>
-        <v>291</v>
-      </c>
-      <c r="Y21" s="71">
-        <f t="shared" si="23"/>
-        <v>298</v>
-      </c>
-      <c r="Z21" s="71">
-        <f t="shared" si="23"/>
-        <v>381</v>
-      </c>
-      <c r="AA21" s="71">
-        <f t="shared" si="23"/>
-        <v>382</v>
-      </c>
-      <c r="AC21" s="71">
-        <f t="shared" ref="AC21:AJ21" si="24">SUM(AC22:AC28)</f>
-        <v>459</v>
-      </c>
-      <c r="AD21" s="71">
-        <f t="shared" si="24"/>
-        <v>513</v>
-      </c>
-      <c r="AE21" s="71">
-        <f t="shared" si="24"/>
-        <v>450</v>
-      </c>
-      <c r="AF21" s="71">
-        <f t="shared" si="24"/>
-        <v>435</v>
-      </c>
-      <c r="AG21" s="71">
         <f t="shared" si="24"/>
         <v>368</v>
       </c>
-      <c r="AH21" s="71">
+      <c r="F21" s="71">
+        <f t="shared" si="24"/>
+        <v>359</v>
+      </c>
+      <c r="G21" s="71">
+        <f t="shared" si="24"/>
+        <v>363</v>
+      </c>
+      <c r="H21" s="71">
+        <f t="shared" si="24"/>
+        <v>345</v>
+      </c>
+      <c r="I21" s="71">
         <f t="shared" si="24"/>
         <v>338</v>
       </c>
-      <c r="AI21" s="71">
+      <c r="J21" s="71">
+        <f t="shared" si="24"/>
+        <v>318</v>
+      </c>
+      <c r="K21" s="71">
+        <f t="shared" si="24"/>
+        <v>314</v>
+      </c>
+      <c r="L21" s="71">
+        <f t="shared" si="24"/>
+        <v>307</v>
+      </c>
+      <c r="M21" s="71">
         <f t="shared" si="24"/>
         <v>281</v>
       </c>
+      <c r="N21" s="71">
+        <f t="shared" si="24"/>
+        <v>272</v>
+      </c>
+      <c r="O21" s="71">
+        <f t="shared" si="24"/>
+        <v>306</v>
+      </c>
+      <c r="P21" s="71">
+        <f t="shared" si="24"/>
+        <v>313</v>
+      </c>
+      <c r="Q21" s="71">
+        <f t="shared" si="24"/>
+        <v>325</v>
+      </c>
+      <c r="R21" s="71">
+        <f t="shared" si="24"/>
+        <v>315</v>
+      </c>
+      <c r="S21" s="71">
+        <f t="shared" si="24"/>
+        <v>312</v>
+      </c>
+      <c r="T21" s="71">
+        <f t="shared" si="24"/>
+        <v>297</v>
+      </c>
+      <c r="U21" s="71">
+        <f t="shared" si="24"/>
+        <v>291</v>
+      </c>
+      <c r="V21" s="71">
+        <f t="shared" si="24"/>
+        <v>281</v>
+      </c>
+      <c r="W21" s="71">
+        <f t="shared" si="24"/>
+        <v>271</v>
+      </c>
+      <c r="X21" s="71">
+        <f t="shared" si="24"/>
+        <v>291</v>
+      </c>
+      <c r="Y21" s="71">
+        <f t="shared" si="24"/>
+        <v>298</v>
+      </c>
+      <c r="Z21" s="71">
+        <f t="shared" si="24"/>
+        <v>381</v>
+      </c>
+      <c r="AA21" s="71">
+        <f t="shared" si="24"/>
+        <v>382</v>
+      </c>
+      <c r="AC21" s="71">
+        <f t="shared" ref="AC21:AJ21" si="25">SUM(AC22:AC28)</f>
+        <v>459</v>
+      </c>
+      <c r="AD21" s="71">
+        <f t="shared" si="25"/>
+        <v>513</v>
+      </c>
+      <c r="AE21" s="71">
+        <f t="shared" si="25"/>
+        <v>450</v>
+      </c>
+      <c r="AF21" s="71">
+        <f t="shared" si="25"/>
+        <v>435</v>
+      </c>
+      <c r="AG21" s="71">
+        <f t="shared" si="25"/>
+        <v>368</v>
+      </c>
+      <c r="AH21" s="71">
+        <f t="shared" si="25"/>
+        <v>338</v>
+      </c>
+      <c r="AI21" s="71">
+        <f t="shared" si="25"/>
+        <v>281</v>
+      </c>
       <c r="AJ21" s="71">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>325</v>
       </c>
     </row>
@@ -31364,31 +31400,31 @@
         <v>186</v>
       </c>
       <c r="F31" s="31">
-        <f t="shared" ref="F31" si="25">F3/B3-1</f>
+        <f t="shared" ref="F31" si="26">F3/B3-1</f>
         <v>1.3623978201634968E-2</v>
       </c>
       <c r="G31" s="31">
-        <f t="shared" ref="G31" si="26">G3/C3-1</f>
+        <f t="shared" ref="G31" si="27">G3/C3-1</f>
         <v>4.8834628190898899E-2</v>
       </c>
       <c r="H31" s="31">
-        <f t="shared" ref="H31" si="27">H3/D3-1</f>
+        <f t="shared" ref="H31" si="28">H3/D3-1</f>
         <v>0.10597189695550346</v>
       </c>
       <c r="I31" s="31">
-        <f t="shared" ref="I31:L31" si="28">I3/E3-1</f>
+        <f t="shared" ref="I31:L31" si="29">I3/E3-1</f>
         <v>3.1754574811625469E-2</v>
       </c>
       <c r="J31" s="31">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2.2580645161290214E-2</v>
       </c>
       <c r="K31" s="31">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6.3492063492063266E-3</v>
       </c>
       <c r="L31" s="31">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6.8819481206987554E-3</v>
       </c>
       <c r="M31" s="31">
@@ -31396,15 +31432,15 @@
         <v>-6.7814293166406081E-3</v>
       </c>
       <c r="N31" s="31">
-        <f t="shared" ref="N31" si="29">N3/J3-1</f>
+        <f t="shared" ref="N31" si="30">N3/J3-1</f>
         <v>1.051524710830698E-3</v>
       </c>
       <c r="O31" s="31">
-        <f t="shared" ref="O31" si="30">O3/K3-1</f>
+        <f t="shared" ref="O31" si="31">O3/K3-1</f>
         <v>2.6288117770767672E-2</v>
       </c>
       <c r="P31" s="31">
-        <f t="shared" ref="P31" si="31">P3/L3-1</f>
+        <f t="shared" ref="P31" si="32">P3/L3-1</f>
         <v>3.4700315457413256E-2</v>
       </c>
       <c r="Q31" s="31">
@@ -31424,50 +31460,50 @@
         <v>1.3719512195121908E-2</v>
       </c>
       <c r="U31" s="31">
-        <f t="shared" ref="U31" si="32">U3/Q3-1</f>
+        <f t="shared" ref="U31" si="33">U3/Q3-1</f>
         <v>1.1523046092184464E-2</v>
       </c>
       <c r="V31" s="31">
-        <f t="shared" ref="V31" si="33">V3/R3-1</f>
+        <f t="shared" ref="V31" si="34">V3/R3-1</f>
         <v>1.2048192771084265E-2</v>
       </c>
       <c r="W31" s="31">
-        <f t="shared" ref="W31" si="34">W3/S3-1</f>
+        <f t="shared" ref="W31" si="35">W3/S3-1</f>
         <v>1.1500000000000066E-2</v>
       </c>
       <c r="X31" s="31">
-        <f t="shared" ref="X31" si="35">X3/T3-1</f>
+        <f t="shared" ref="X31" si="36">X3/T3-1</f>
         <v>3.1578947368421151E-2</v>
       </c>
       <c r="Y31" s="31">
-        <f t="shared" ref="Y31" si="36">Y3/U3-1</f>
+        <f t="shared" ref="Y31" si="37">Y3/U3-1</f>
         <v>3.5165923724616244E-2</v>
       </c>
       <c r="Z31" s="31">
-        <f t="shared" ref="Z31" si="37">Z3/V3-1</f>
+        <f t="shared" ref="Z31" si="38">Z3/V3-1</f>
         <v>8.1349206349206282E-2</v>
       </c>
       <c r="AA31" s="31">
-        <f t="shared" ref="AA31" si="38">AA3/W3-1</f>
+        <f t="shared" ref="AA31" si="39">AA3/W3-1</f>
         <v>8.7493821057834875E-2</v>
       </c>
       <c r="AC31" s="59" t="s">
         <v>186</v>
       </c>
       <c r="AD31" s="31">
-        <f t="shared" ref="AD31" si="39">AD3/AC3-1</f>
+        <f t="shared" ref="AD31" si="40">AD3/AC3-1</f>
         <v>0.1000645577792123</v>
       </c>
       <c r="AE31" s="31">
-        <f t="shared" ref="AE31" si="40">AE3/AD3-1</f>
+        <f t="shared" ref="AE31" si="41">AE3/AD3-1</f>
         <v>2.6408450704225261E-2</v>
       </c>
       <c r="AF31" s="31">
-        <f t="shared" ref="AF31:AG31" si="41">AF3/AE3-1</f>
+        <f t="shared" ref="AF31:AG31" si="42">AF3/AE3-1</f>
         <v>4.9170954831332159E-2</v>
       </c>
       <c r="AG31" s="31">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>1.2534059945504161E-2</v>
       </c>
       <c r="AH31" s="31">
@@ -31500,31 +31536,31 @@
         <v>186</v>
       </c>
       <c r="F32" s="75">
-        <f t="shared" ref="F32" si="42">F3-B3</f>
+        <f t="shared" ref="F32" si="43">F3-B3</f>
         <v>25</v>
       </c>
       <c r="G32" s="75">
-        <f t="shared" ref="G32" si="43">G3-C3</f>
+        <f t="shared" ref="G32" si="44">G3-C3</f>
         <v>88</v>
       </c>
       <c r="H32" s="75">
-        <f t="shared" ref="H32" si="44">H3-D3</f>
+        <f t="shared" ref="H32" si="45">H3-D3</f>
         <v>181</v>
       </c>
       <c r="I32" s="75">
-        <f t="shared" ref="I32:L32" si="45">I3-E3</f>
+        <f t="shared" ref="I32:L32" si="46">I3-E3</f>
         <v>59</v>
       </c>
       <c r="J32" s="75">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>42</v>
       </c>
       <c r="K32" s="75">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>12</v>
       </c>
       <c r="L32" s="75">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>13</v>
       </c>
       <c r="M32" s="75">
@@ -31532,15 +31568,15 @@
         <v>-13</v>
       </c>
       <c r="N32" s="75">
-        <f t="shared" ref="N32" si="46">N3-J3</f>
+        <f t="shared" ref="N32" si="47">N3-J3</f>
         <v>2</v>
       </c>
       <c r="O32" s="75">
-        <f t="shared" ref="O32" si="47">O3-K3</f>
+        <f t="shared" ref="O32" si="48">O3-K3</f>
         <v>50</v>
       </c>
       <c r="P32" s="75">
-        <f t="shared" ref="P32" si="48">P3-L3</f>
+        <f t="shared" ref="P32" si="49">P3-L3</f>
         <v>66</v>
       </c>
       <c r="Q32" s="75">
@@ -31560,50 +31596,50 @@
         <v>27</v>
       </c>
       <c r="U32" s="75">
-        <f t="shared" ref="U32" si="49">U3-Q3</f>
+        <f t="shared" ref="U32" si="50">U3-Q3</f>
         <v>23</v>
       </c>
       <c r="V32" s="75">
-        <f t="shared" ref="V32" si="50">V3-R3</f>
+        <f t="shared" ref="V32" si="51">V3-R3</f>
         <v>24</v>
       </c>
       <c r="W32" s="75">
-        <f t="shared" ref="W32" si="51">W3-S3</f>
+        <f t="shared" ref="W32" si="52">W3-S3</f>
         <v>23</v>
       </c>
       <c r="X32" s="75">
-        <f t="shared" ref="X32" si="52">X3-T3</f>
+        <f t="shared" ref="X32" si="53">X3-T3</f>
         <v>63</v>
       </c>
       <c r="Y32" s="75">
-        <f t="shared" ref="Y32" si="53">Y3-U3</f>
+        <f t="shared" ref="Y32" si="54">Y3-U3</f>
         <v>71</v>
       </c>
       <c r="Z32" s="75">
-        <f t="shared" ref="Z32" si="54">Z3-V3</f>
+        <f t="shared" ref="Z32" si="55">Z3-V3</f>
         <v>164</v>
       </c>
       <c r="AA32" s="75">
-        <f t="shared" ref="AA32" si="55">AA3-W3</f>
+        <f t="shared" ref="AA32" si="56">AA3-W3</f>
         <v>177</v>
       </c>
       <c r="AC32" s="59" t="s">
         <v>186</v>
       </c>
       <c r="AD32" s="75">
-        <f t="shared" ref="AD32" si="56">AD3-AC3</f>
+        <f t="shared" ref="AD32" si="57">AD3-AC3</f>
         <v>155</v>
       </c>
       <c r="AE32" s="75">
-        <f t="shared" ref="AE32" si="57">AE3-AD3</f>
+        <f t="shared" ref="AE32" si="58">AE3-AD3</f>
         <v>45</v>
       </c>
       <c r="AF32" s="75">
-        <f t="shared" ref="AF32:AG32" si="58">AF3-AE3</f>
+        <f t="shared" ref="AF32:AG32" si="59">AF3-AE3</f>
         <v>86</v>
       </c>
       <c r="AG32" s="75">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>23</v>
       </c>
       <c r="AH32" s="75">
@@ -31627,103 +31663,103 @@
         <v>186</v>
       </c>
       <c r="C33" s="24">
-        <f t="shared" ref="C33" si="59">C3/B3-1</f>
+        <f t="shared" ref="C33" si="60">C3/B3-1</f>
         <v>-1.7983651226158082E-2</v>
       </c>
       <c r="D33" s="24">
-        <f t="shared" ref="D33" si="60">D3/C3-1</f>
+        <f t="shared" ref="D33" si="61">D3/C3-1</f>
         <v>-5.2164261931187617E-2</v>
       </c>
       <c r="E33" s="24">
-        <f t="shared" ref="E33" si="61">E3/D3-1</f>
+        <f t="shared" ref="E33" si="62">E3/D3-1</f>
         <v>8.7822014051522235E-2</v>
       </c>
       <c r="F33" s="24">
-        <f t="shared" ref="F33" si="62">F3/E3-1</f>
+        <f t="shared" ref="F33" si="63">F3/E3-1</f>
         <v>1.0764262648008671E-3</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" ref="G33" si="63">G3/F3-1</f>
+        <f t="shared" ref="G33" si="64">G3/F3-1</f>
         <v>1.6129032258064502E-2</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" ref="H33" si="64">H3/G3-1</f>
+        <f t="shared" ref="H33" si="65">H3/G3-1</f>
         <v>-5.2910052910049021E-4</v>
       </c>
       <c r="I33" s="24">
-        <f t="shared" ref="I33" si="65">I3/H3-1</f>
+        <f t="shared" ref="I33" si="66">I3/H3-1</f>
         <v>1.4822657490735747E-2</v>
       </c>
       <c r="J33" s="24">
-        <f t="shared" ref="J33" si="66">J3/I3-1</f>
+        <f t="shared" ref="J33" si="67">J3/I3-1</f>
         <v>-7.8247261345852914E-3</v>
       </c>
       <c r="K33" s="24">
-        <f t="shared" ref="K33" si="67">K3/J3-1</f>
+        <f t="shared" ref="K33" si="68">K3/J3-1</f>
         <v>0</v>
       </c>
       <c r="L33" s="24">
-        <f t="shared" ref="L33" si="68">L3/K3-1</f>
+        <f t="shared" ref="L33" si="69">L3/K3-1</f>
         <v>0</v>
       </c>
       <c r="M33" s="24">
-        <f t="shared" ref="M33" si="69">M3/L3-1</f>
+        <f t="shared" ref="M33" si="70">M3/L3-1</f>
         <v>1.051524710830698E-3</v>
       </c>
       <c r="N33" s="24">
-        <f t="shared" ref="N33" si="70">N3/M3-1</f>
+        <f t="shared" ref="N33" si="71">N3/M3-1</f>
         <v>0</v>
       </c>
       <c r="O33" s="24">
-        <f t="shared" ref="O33" si="71">O3/N3-1</f>
+        <f t="shared" ref="O33" si="72">O3/N3-1</f>
         <v>2.5210084033613356E-2</v>
       </c>
       <c r="P33" s="24">
-        <f t="shared" ref="P33:T33" si="72">P3/O3-1</f>
+        <f t="shared" ref="P33:T33" si="73">P3/O3-1</f>
         <v>8.1967213114753079E-3</v>
       </c>
       <c r="Q33" s="24">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>1.4227642276422703E-2</v>
       </c>
       <c r="R33" s="24">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>-2.0040080160320661E-3</v>
       </c>
       <c r="S33" s="24">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>4.0160642570281624E-3</v>
       </c>
       <c r="T33" s="24">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>-2.4999999999999467E-3</v>
       </c>
       <c r="U33" s="24">
-        <f t="shared" ref="U33" si="73">U3/T3-1</f>
+        <f t="shared" ref="U33" si="74">U3/T3-1</f>
         <v>1.2030075187969835E-2</v>
       </c>
       <c r="V33" s="24">
-        <f t="shared" ref="V33" si="74">V3/U3-1</f>
+        <f t="shared" ref="V33" si="75">V3/U3-1</f>
         <v>-1.4858841010401136E-3</v>
       </c>
       <c r="W33" s="24">
-        <f t="shared" ref="W33" si="75">W3/V3-1</f>
+        <f t="shared" ref="W33" si="76">W3/V3-1</f>
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="X33" s="24">
-        <f t="shared" ref="X33" si="76">X3/W3-1</f>
+        <f t="shared" ref="X33" si="77">X3/W3-1</f>
         <v>1.730103806228378E-2</v>
       </c>
       <c r="Y33" s="24">
-        <f t="shared" ref="Y33" si="77">Y3/X3-1</f>
+        <f t="shared" ref="Y33" si="78">Y3/X3-1</f>
         <v>1.554907677356665E-2</v>
       </c>
       <c r="Z33" s="24">
-        <f t="shared" ref="Z33" si="78">Z3/Y3-1</f>
+        <f t="shared" ref="Z33" si="79">Z3/Y3-1</f>
         <v>4.3062200956937691E-2</v>
       </c>
       <c r="AA33" s="24">
-        <f t="shared" ref="AA33" si="79">AA3/Z3-1</f>
+        <f t="shared" ref="AA33" si="80">AA3/Z3-1</f>
         <v>9.1743119266054496E-3</v>
       </c>
       <c r="AC33" s="59" t="s">
@@ -31759,103 +31795,103 @@
         <v>186</v>
       </c>
       <c r="C34" s="75">
-        <f t="shared" ref="C34" si="80">C3-B3</f>
+        <f t="shared" ref="C34" si="81">C3-B3</f>
         <v>-33</v>
       </c>
       <c r="D34" s="75">
-        <f t="shared" ref="D34" si="81">D3-C3</f>
+        <f t="shared" ref="D34" si="82">D3-C3</f>
         <v>-94</v>
       </c>
       <c r="E34" s="75">
-        <f t="shared" ref="E34" si="82">E3-D3</f>
+        <f t="shared" ref="E34" si="83">E3-D3</f>
         <v>150</v>
       </c>
       <c r="F34" s="75">
-        <f t="shared" ref="F34" si="83">F3-E3</f>
+        <f t="shared" ref="F34" si="84">F3-E3</f>
         <v>2</v>
       </c>
       <c r="G34" s="75">
-        <f t="shared" ref="G34" si="84">G3-F3</f>
+        <f t="shared" ref="G34" si="85">G3-F3</f>
         <v>30</v>
       </c>
       <c r="H34" s="75">
-        <f t="shared" ref="H34" si="85">H3-G3</f>
+        <f t="shared" ref="H34" si="86">H3-G3</f>
         <v>-1</v>
       </c>
       <c r="I34" s="75">
-        <f t="shared" ref="I34" si="86">I3-H3</f>
+        <f t="shared" ref="I34" si="87">I3-H3</f>
         <v>28</v>
       </c>
       <c r="J34" s="75">
-        <f t="shared" ref="J34" si="87">J3-I3</f>
+        <f t="shared" ref="J34" si="88">J3-I3</f>
         <v>-15</v>
       </c>
       <c r="K34" s="75">
-        <f t="shared" ref="K34" si="88">K3-J3</f>
+        <f t="shared" ref="K34" si="89">K3-J3</f>
         <v>0</v>
       </c>
       <c r="L34" s="75">
-        <f t="shared" ref="L34" si="89">L3-K3</f>
+        <f t="shared" ref="L34" si="90">L3-K3</f>
         <v>0</v>
       </c>
       <c r="M34" s="75">
-        <f t="shared" ref="M34" si="90">M3-L3</f>
+        <f t="shared" ref="M34" si="91">M3-L3</f>
         <v>2</v>
       </c>
       <c r="N34" s="75">
-        <f t="shared" ref="N34" si="91">N3-M3</f>
+        <f t="shared" ref="N34" si="92">N3-M3</f>
         <v>0</v>
       </c>
       <c r="O34" s="75">
-        <f t="shared" ref="O34" si="92">O3-N3</f>
+        <f t="shared" ref="O34" si="93">O3-N3</f>
         <v>48</v>
       </c>
       <c r="P34" s="75">
-        <f t="shared" ref="P34:T34" si="93">P3-O3</f>
+        <f t="shared" ref="P34:T34" si="94">P3-O3</f>
         <v>16</v>
       </c>
       <c r="Q34" s="75">
-        <f t="shared" si="93"/>
+        <f t="shared" si="94"/>
         <v>28</v>
       </c>
       <c r="R34" s="75">
-        <f t="shared" si="93"/>
+        <f t="shared" si="94"/>
         <v>-4</v>
       </c>
       <c r="S34" s="75">
-        <f t="shared" si="93"/>
+        <f t="shared" si="94"/>
         <v>8</v>
       </c>
       <c r="T34" s="75">
-        <f t="shared" si="93"/>
+        <f t="shared" si="94"/>
         <v>-5</v>
       </c>
       <c r="U34" s="75">
-        <f t="shared" ref="U34" si="94">U3-T3</f>
+        <f t="shared" ref="U34" si="95">U3-T3</f>
         <v>24</v>
       </c>
       <c r="V34" s="75">
-        <f t="shared" ref="V34" si="95">V3-U3</f>
+        <f t="shared" ref="V34" si="96">V3-U3</f>
         <v>-3</v>
       </c>
       <c r="W34" s="75">
-        <f t="shared" ref="W34" si="96">W3-V3</f>
+        <f t="shared" ref="W34" si="97">W3-V3</f>
         <v>7</v>
       </c>
       <c r="X34" s="75">
-        <f t="shared" ref="X34" si="97">X3-W3</f>
+        <f t="shared" ref="X34" si="98">X3-W3</f>
         <v>35</v>
       </c>
       <c r="Y34" s="75">
-        <f t="shared" ref="Y34" si="98">Y3-X3</f>
+        <f t="shared" ref="Y34" si="99">Y3-X3</f>
         <v>32</v>
       </c>
       <c r="Z34" s="75">
-        <f t="shared" ref="Z34" si="99">Z3-Y3</f>
+        <f t="shared" ref="Z34" si="100">Z3-Y3</f>
         <v>90</v>
       </c>
       <c r="AA34" s="75">
-        <f t="shared" ref="AA34" si="100">AA3-Z3</f>
+        <f t="shared" ref="AA34" si="101">AA3-Z3</f>
         <v>20</v>
       </c>
       <c r="AC34" s="59" t="s">
@@ -31903,31 +31939,31 @@
         <v>186</v>
       </c>
       <c r="F36" s="31">
-        <f t="shared" ref="F36" si="101">F12/B12-1</f>
+        <f t="shared" ref="F36" si="102">F12/B12-1</f>
         <v>6.1527581329561487E-2</v>
       </c>
       <c r="G36" s="31">
-        <f t="shared" ref="G36" si="102">G12/C12-1</f>
+        <f t="shared" ref="G36" si="103">G12/C12-1</f>
         <v>5.8945908460471541E-2</v>
       </c>
       <c r="H36" s="31">
-        <f t="shared" ref="H36" si="103">H12/D12-1</f>
+        <f t="shared" ref="H36" si="104">H12/D12-1</f>
         <v>5.9711736444749475E-2</v>
       </c>
       <c r="I36" s="31">
-        <f t="shared" ref="I36:L36" si="104">I12/E12-1</f>
+        <f t="shared" ref="I36:L36" si="105">I12/E12-1</f>
         <v>5.9731543624160999E-2</v>
       </c>
       <c r="J36" s="31">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>5.5296469020652994E-2</v>
       </c>
       <c r="K36" s="31">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>3.9947609692206898E-2</v>
       </c>
       <c r="L36" s="31">
-        <f t="shared" si="104"/>
+        <f t="shared" si="105"/>
         <v>3.303108808290145E-2</v>
       </c>
       <c r="M36" s="31">
@@ -31935,15 +31971,15 @@
         <v>2.7865737808739688E-2</v>
       </c>
       <c r="N36" s="31">
-        <f t="shared" ref="N36" si="105">N12/J12-1</f>
+        <f t="shared" ref="N36" si="106">N12/J12-1</f>
         <v>3.0303030303030276E-2</v>
       </c>
       <c r="O36" s="31">
-        <f t="shared" ref="O36" si="106">O12/K12-1</f>
+        <f t="shared" ref="O36" si="107">O12/K12-1</f>
         <v>3.6523929471032668E-2</v>
       </c>
       <c r="P36" s="31">
-        <f t="shared" ref="P36" si="107">P12/L12-1</f>
+        <f t="shared" ref="P36" si="108">P12/L12-1</f>
         <v>3.7617554858934144E-2</v>
       </c>
       <c r="Q36" s="31">
@@ -31963,50 +31999,50 @@
         <v>2.5981873111782461E-2</v>
       </c>
       <c r="U36" s="31">
-        <f t="shared" ref="U36" si="108">U12/Q12-1</f>
+        <f t="shared" ref="U36" si="109">U12/Q12-1</f>
         <v>3.4111310592459532E-2</v>
       </c>
       <c r="V36" s="31">
-        <f t="shared" ref="V36" si="109">V12/R12-1</f>
+        <f t="shared" ref="V36" si="110">V12/R12-1</f>
         <v>3.4585569469290478E-2</v>
       </c>
       <c r="W36" s="31">
-        <f t="shared" ref="W36" si="110">W12/S12-1</f>
+        <f t="shared" ref="W36" si="111">W12/S12-1</f>
         <v>3.7914691943127909E-2</v>
       </c>
       <c r="X36" s="31">
-        <f t="shared" ref="X36" si="111">X12/T12-1</f>
+        <f t="shared" ref="X36" si="112">X12/T12-1</f>
         <v>4.0636042402826922E-2</v>
       </c>
       <c r="Y36" s="31">
-        <f t="shared" ref="Y36" si="112">Y12/U12-1</f>
+        <f t="shared" ref="Y36" si="113">Y12/U12-1</f>
         <v>3.993055555555558E-2</v>
       </c>
       <c r="Z36" s="31">
-        <f t="shared" ref="Z36" si="113">Z12/V12-1</f>
+        <f t="shared" ref="Z36" si="114">Z12/V12-1</f>
         <v>3.9769452449567755E-2</v>
       </c>
       <c r="AA36" s="31">
-        <f t="shared" ref="AA36" si="114">AA12/W12-1</f>
+        <f t="shared" ref="AA36" si="115">AA12/W12-1</f>
         <v>4.0525114155251174E-2</v>
       </c>
       <c r="AC36" s="59" t="s">
         <v>186</v>
       </c>
       <c r="AD36" s="31">
-        <f t="shared" ref="AD36" si="115">AD12/AC12-1</f>
+        <f t="shared" ref="AD36" si="116">AD12/AC12-1</f>
         <v>8.3486238532110013E-2</v>
       </c>
       <c r="AE36" s="31">
-        <f t="shared" ref="AE36" si="116">AE12/AD12-1</f>
+        <f t="shared" ref="AE36" si="117">AE12/AD12-1</f>
         <v>9.9915325994919479E-2</v>
       </c>
       <c r="AF36" s="31">
-        <f t="shared" ref="AF36:AG36" si="117">AF12/AE12-1</f>
+        <f t="shared" ref="AF36:AG36" si="118">AF12/AE12-1</f>
         <v>7.7752117013087041E-2</v>
       </c>
       <c r="AG36" s="31">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>6.4285714285714279E-2</v>
       </c>
       <c r="AH36" s="31">
@@ -32039,31 +32075,31 @@
         <v>186</v>
       </c>
       <c r="F37" s="75">
-        <f t="shared" ref="F37" si="118">F12-B12</f>
+        <f t="shared" ref="F37" si="119">F12-B12</f>
         <v>87</v>
       </c>
       <c r="G37" s="75">
-        <f t="shared" ref="G37" si="119">G12-C12</f>
+        <f t="shared" ref="G37" si="120">G12-C12</f>
         <v>85</v>
       </c>
       <c r="H37" s="75">
-        <f t="shared" ref="H37" si="120">H12-D12</f>
+        <f t="shared" ref="H37" si="121">H12-D12</f>
         <v>87</v>
       </c>
       <c r="I37" s="75">
-        <f t="shared" ref="I37:L37" si="121">I12-E12</f>
+        <f t="shared" ref="I37:L37" si="122">I12-E12</f>
         <v>89</v>
       </c>
       <c r="J37" s="75">
-        <f t="shared" si="121"/>
+        <f t="shared" si="122"/>
         <v>83</v>
       </c>
       <c r="K37" s="75">
-        <f t="shared" si="121"/>
+        <f t="shared" si="122"/>
         <v>61</v>
       </c>
       <c r="L37" s="75">
-        <f t="shared" si="121"/>
+        <f t="shared" si="122"/>
         <v>51</v>
       </c>
       <c r="M37" s="75">
@@ -32071,15 +32107,15 @@
         <v>44</v>
       </c>
       <c r="N37" s="75">
-        <f t="shared" ref="N37" si="122">N12-J12</f>
+        <f t="shared" ref="N37" si="123">N12-J12</f>
         <v>48</v>
       </c>
       <c r="O37" s="75">
-        <f t="shared" ref="O37" si="123">O12-K12</f>
+        <f t="shared" ref="O37" si="124">O12-K12</f>
         <v>58</v>
       </c>
       <c r="P37" s="75">
-        <f t="shared" ref="P37" si="124">P12-L12</f>
+        <f t="shared" ref="P37" si="125">P12-L12</f>
         <v>60</v>
       </c>
       <c r="Q37" s="75">
@@ -32099,50 +32135,50 @@
         <v>43</v>
       </c>
       <c r="U37" s="75">
-        <f t="shared" ref="U37" si="125">U12-Q12</f>
+        <f t="shared" ref="U37" si="126">U12-Q12</f>
         <v>57</v>
       </c>
       <c r="V37" s="75">
-        <f t="shared" ref="V37" si="126">V12-R12</f>
+        <f t="shared" ref="V37" si="127">V12-R12</f>
         <v>58</v>
       </c>
       <c r="W37" s="75">
-        <f t="shared" ref="W37" si="127">W12-S12</f>
+        <f t="shared" ref="W37" si="128">W12-S12</f>
         <v>64</v>
       </c>
       <c r="X37" s="75">
-        <f t="shared" ref="X37" si="128">X12-T12</f>
+        <f t="shared" ref="X37" si="129">X12-T12</f>
         <v>69</v>
       </c>
       <c r="Y37" s="75">
-        <f t="shared" ref="Y37" si="129">Y12-U12</f>
+        <f t="shared" ref="Y37" si="130">Y12-U12</f>
         <v>69</v>
       </c>
       <c r="Z37" s="75">
-        <f t="shared" ref="Z37" si="130">Z12-V12</f>
+        <f t="shared" ref="Z37" si="131">Z12-V12</f>
         <v>69</v>
       </c>
       <c r="AA37" s="75">
-        <f t="shared" ref="AA37" si="131">AA12-W12</f>
+        <f t="shared" ref="AA37" si="132">AA12-W12</f>
         <v>71</v>
       </c>
       <c r="AC37" s="59" t="s">
         <v>186</v>
       </c>
       <c r="AD37" s="75">
-        <f t="shared" ref="AD37" si="132">AD12-AC12</f>
+        <f t="shared" ref="AD37" si="133">AD12-AC12</f>
         <v>91</v>
       </c>
       <c r="AE37" s="75">
-        <f t="shared" ref="AE37" si="133">AE12-AD12</f>
+        <f t="shared" ref="AE37" si="134">AE12-AD12</f>
         <v>118</v>
       </c>
       <c r="AF37" s="75">
-        <f t="shared" ref="AF37:AG37" si="134">AF12-AE12</f>
+        <f t="shared" ref="AF37:AG37" si="135">AF12-AE12</f>
         <v>101</v>
       </c>
       <c r="AG37" s="75">
-        <f t="shared" si="134"/>
+        <f t="shared" si="135"/>
         <v>90</v>
       </c>
       <c r="AH37" s="75">
@@ -32166,103 +32202,103 @@
         <v>186</v>
       </c>
       <c r="C38" s="24">
-        <f t="shared" ref="C38" si="135">C12/B12-1</f>
+        <f t="shared" ref="C38" si="136">C12/B12-1</f>
         <v>1.980198019801982E-2</v>
       </c>
       <c r="D38" s="24">
-        <f t="shared" ref="D38" si="136">D12/C12-1</f>
+        <f t="shared" ref="D38" si="137">D12/C12-1</f>
         <v>1.0402219140083213E-2</v>
       </c>
       <c r="E38" s="24">
-        <f t="shared" ref="E38" si="137">E12/D12-1</f>
+        <f t="shared" ref="E38" si="138">E12/D12-1</f>
         <v>2.2649279341111939E-2</v>
       </c>
       <c r="F38" s="24">
-        <f t="shared" ref="F38" si="138">F12/E12-1</f>
+        <f t="shared" ref="F38" si="139">F12/E12-1</f>
         <v>7.382550335570448E-3</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" ref="G38" si="139">G12/F12-1</f>
+        <f t="shared" ref="G38" si="140">G12/F12-1</f>
         <v>1.7321785476348994E-2</v>
       </c>
       <c r="H38" s="24">
-        <f t="shared" ref="H38" si="140">H12/G12-1</f>
+        <f t="shared" ref="H38" si="141">H12/G12-1</f>
         <v>1.1132940406024971E-2</v>
       </c>
       <c r="I38" s="24">
-        <f t="shared" ref="I38" si="141">I12/H12-1</f>
+        <f t="shared" ref="I38" si="142">I12/H12-1</f>
         <v>2.26683937823835E-2</v>
       </c>
       <c r="J38" s="24">
-        <f t="shared" ref="J38" si="142">J12/I12-1</f>
+        <f t="shared" ref="J38" si="143">J12/I12-1</f>
         <v>3.1665611146294292E-3</v>
       </c>
       <c r="K38" s="24">
-        <f t="shared" ref="K38" si="143">K12/J12-1</f>
+        <f t="shared" ref="K38" si="144">K12/J12-1</f>
         <v>2.525252525252597E-3</v>
       </c>
       <c r="L38" s="24">
-        <f t="shared" ref="L38" si="144">L12/K12-1</f>
+        <f t="shared" ref="L38" si="145">L12/K12-1</f>
         <v>4.4080604534004753E-3</v>
       </c>
       <c r="M38" s="24">
-        <f t="shared" ref="M38" si="145">M12/L12-1</f>
+        <f t="shared" ref="M38" si="146">M12/L12-1</f>
         <v>1.7554858934169193E-2</v>
       </c>
       <c r="N38" s="24">
-        <f t="shared" ref="N38" si="146">N12/M12-1</f>
+        <f t="shared" ref="N38" si="147">N12/M12-1</f>
         <v>5.5452865064695711E-3</v>
       </c>
       <c r="O38" s="24">
-        <f t="shared" ref="O38" si="147">O12/N12-1</f>
+        <f t="shared" ref="O38" si="148">O12/N12-1</f>
         <v>8.5784313725489891E-3</v>
       </c>
       <c r="P38" s="24">
-        <f t="shared" ref="P38:T38" si="148">P12/O12-1</f>
+        <f t="shared" ref="P38:T38" si="149">P12/O12-1</f>
         <v>5.4678007290400732E-3</v>
       </c>
       <c r="Q38" s="24">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>9.6676737160121817E-3</v>
       </c>
       <c r="R38" s="24">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>3.5906642728904536E-3</v>
       </c>
       <c r="S38" s="24">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>6.5593321407275695E-3</v>
       </c>
       <c r="T38" s="24">
-        <f t="shared" si="148"/>
+        <f t="shared" si="149"/>
         <v>5.924170616113722E-3</v>
       </c>
       <c r="U38" s="24">
-        <f t="shared" ref="U38" si="149">U12/T12-1</f>
+        <f t="shared" ref="U38" si="150">U12/T12-1</f>
         <v>1.7667844522968101E-2</v>
       </c>
       <c r="V38" s="24">
-        <f t="shared" ref="V38" si="150">V12/U12-1</f>
+        <f t="shared" ref="V38" si="151">V12/U12-1</f>
         <v>4.050925925925819E-3</v>
       </c>
       <c r="W38" s="24">
-        <f t="shared" ref="W38" si="151">W12/V12-1</f>
+        <f t="shared" ref="W38" si="152">W12/V12-1</f>
         <v>9.7982708933717078E-3</v>
       </c>
       <c r="X38" s="24">
-        <f t="shared" ref="X38" si="152">X12/W12-1</f>
+        <f t="shared" ref="X38" si="153">X12/W12-1</f>
         <v>8.5616438356164171E-3</v>
       </c>
       <c r="Y38" s="24">
-        <f t="shared" ref="Y38" si="153">Y12/X12-1</f>
+        <f t="shared" ref="Y38" si="154">Y12/X12-1</f>
         <v>1.6977928692699429E-2</v>
       </c>
       <c r="Z38" s="24">
-        <f t="shared" ref="Z38" si="154">Z12/Y12-1</f>
+        <f t="shared" ref="Z38" si="155">Z12/Y12-1</f>
         <v>3.8953811908737368E-3</v>
       </c>
       <c r="AA38" s="24">
-        <f t="shared" ref="AA38" si="155">AA12/Z12-1</f>
+        <f t="shared" ref="AA38" si="156">AA12/Z12-1</f>
         <v>1.0532150776053184E-2</v>
       </c>
       <c r="AC38" s="59" t="s">
@@ -32298,103 +32334,103 @@
         <v>186</v>
       </c>
       <c r="C39" s="75">
-        <f t="shared" ref="C39" si="156">C12-B12</f>
+        <f t="shared" ref="C39" si="157">C12-B12</f>
         <v>28</v>
       </c>
       <c r="D39" s="75">
-        <f t="shared" ref="D39" si="157">D12-C12</f>
+        <f t="shared" ref="D39" si="158">D12-C12</f>
         <v>15</v>
       </c>
       <c r="E39" s="75">
-        <f t="shared" ref="E39" si="158">E12-D12</f>
+        <f t="shared" ref="E39" si="159">E12-D12</f>
         <v>33</v>
       </c>
       <c r="F39" s="75">
-        <f t="shared" ref="F39" si="159">F12-E12</f>
+        <f t="shared" ref="F39" si="160">F12-E12</f>
         <v>11</v>
       </c>
       <c r="G39" s="75">
-        <f t="shared" ref="G39" si="160">G12-F12</f>
+        <f t="shared" ref="G39" si="161">G12-F12</f>
         <v>26</v>
       </c>
       <c r="H39" s="75">
-        <f t="shared" ref="H39" si="161">H12-G12</f>
+        <f t="shared" ref="H39" si="162">H12-G12</f>
         <v>17</v>
       </c>
       <c r="I39" s="75">
-        <f t="shared" ref="I39" si="162">I12-H12</f>
+        <f t="shared" ref="I39" si="163">I12-H12</f>
         <v>35</v>
       </c>
       <c r="J39" s="75">
-        <f t="shared" ref="J39" si="163">J12-I12</f>
+        <f t="shared" ref="J39" si="164">J12-I12</f>
         <v>5</v>
       </c>
       <c r="K39" s="75">
-        <f t="shared" ref="K39" si="164">K12-J12</f>
+        <f t="shared" ref="K39" si="165">K12-J12</f>
         <v>4</v>
       </c>
       <c r="L39" s="75">
-        <f t="shared" ref="L39" si="165">L12-K12</f>
+        <f t="shared" ref="L39" si="166">L12-K12</f>
         <v>7</v>
       </c>
       <c r="M39" s="75">
-        <f t="shared" ref="M39" si="166">M12-L12</f>
+        <f t="shared" ref="M39" si="167">M12-L12</f>
         <v>28</v>
       </c>
       <c r="N39" s="75">
-        <f t="shared" ref="N39" si="167">N12-M12</f>
+        <f t="shared" ref="N39" si="168">N12-M12</f>
         <v>9</v>
       </c>
       <c r="O39" s="75">
-        <f t="shared" ref="O39" si="168">O12-N12</f>
+        <f t="shared" ref="O39" si="169">O12-N12</f>
         <v>14</v>
       </c>
       <c r="P39" s="75">
-        <f t="shared" ref="P39:T39" si="169">P12-O12</f>
+        <f t="shared" ref="P39:T39" si="170">P12-O12</f>
         <v>9</v>
       </c>
       <c r="Q39" s="75">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>16</v>
       </c>
       <c r="R39" s="75">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>6</v>
       </c>
       <c r="S39" s="75">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>11</v>
       </c>
       <c r="T39" s="75">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>10</v>
       </c>
       <c r="U39" s="75">
-        <f t="shared" ref="U39" si="170">U12-T12</f>
+        <f t="shared" ref="U39" si="171">U12-T12</f>
         <v>30</v>
       </c>
       <c r="V39" s="75">
-        <f t="shared" ref="V39" si="171">V12-U12</f>
+        <f t="shared" ref="V39" si="172">V12-U12</f>
         <v>7</v>
       </c>
       <c r="W39" s="75">
-        <f t="shared" ref="W39" si="172">W12-V12</f>
+        <f t="shared" ref="W39" si="173">W12-V12</f>
         <v>17</v>
       </c>
       <c r="X39" s="75">
-        <f t="shared" ref="X39" si="173">X12-W12</f>
+        <f t="shared" ref="X39" si="174">X12-W12</f>
         <v>15</v>
       </c>
       <c r="Y39" s="75">
-        <f t="shared" ref="Y39" si="174">Y12-X12</f>
+        <f t="shared" ref="Y39" si="175">Y12-X12</f>
         <v>30</v>
       </c>
       <c r="Z39" s="75">
-        <f t="shared" ref="Z39" si="175">Z12-Y12</f>
+        <f t="shared" ref="Z39" si="176">Z12-Y12</f>
         <v>7</v>
       </c>
       <c r="AA39" s="75">
-        <f t="shared" ref="AA39" si="176">AA12-Z12</f>
+        <f t="shared" ref="AA39" si="177">AA12-Z12</f>
         <v>19</v>
       </c>
       <c r="AC39" s="59" t="s">
@@ -32442,51 +32478,51 @@
         <v>186</v>
       </c>
       <c r="F41" s="31">
-        <f t="shared" ref="F41" si="177">F21/B21-1</f>
+        <f t="shared" ref="F41" si="178">F21/B21-1</f>
         <v>-0.14726840855106893</v>
       </c>
       <c r="G41" s="31">
-        <f t="shared" ref="G41" si="178">G21/C21-1</f>
+        <f t="shared" ref="G41" si="179">G21/C21-1</f>
         <v>8.3333333333333037E-3</v>
       </c>
       <c r="H41" s="31">
-        <f t="shared" ref="H41" si="179">H21/D21-1</f>
+        <f t="shared" ref="H41" si="180">H21/D21-1</f>
         <v>0.3745019920318724</v>
       </c>
       <c r="I41" s="31">
-        <f t="shared" ref="I41" si="180">I21/E21-1</f>
+        <f t="shared" ref="I41" si="181">I21/E21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
       <c r="J41" s="31">
-        <f t="shared" ref="J41" si="181">J21/F21-1</f>
+        <f t="shared" ref="J41" si="182">J21/F21-1</f>
         <v>-0.11420612813370479</v>
       </c>
       <c r="K41" s="31">
-        <f t="shared" ref="K41" si="182">K21/G21-1</f>
+        <f t="shared" ref="K41" si="183">K21/G21-1</f>
         <v>-0.13498622589531684</v>
       </c>
       <c r="L41" s="31">
-        <f t="shared" ref="L41" si="183">L21/H21-1</f>
+        <f t="shared" ref="L41" si="184">L21/H21-1</f>
         <v>-0.11014492753623184</v>
       </c>
       <c r="M41" s="31">
-        <f t="shared" ref="M41" si="184">M21/I21-1</f>
+        <f t="shared" ref="M41" si="185">M21/I21-1</f>
         <v>-0.16863905325443784</v>
       </c>
       <c r="N41" s="31">
-        <f t="shared" ref="N41" si="185">N21/J21-1</f>
+        <f t="shared" ref="N41" si="186">N21/J21-1</f>
         <v>-0.14465408805031443</v>
       </c>
       <c r="O41" s="31">
-        <f t="shared" ref="O41" si="186">O21/K21-1</f>
+        <f t="shared" ref="O41" si="187">O21/K21-1</f>
         <v>-2.5477707006369421E-2</v>
       </c>
       <c r="P41" s="31">
-        <f t="shared" ref="P41" si="187">P21/L21-1</f>
+        <f t="shared" ref="P41" si="188">P21/L21-1</f>
         <v>1.9543973941368087E-2</v>
       </c>
       <c r="Q41" s="31">
-        <f t="shared" ref="Q41" si="188">Q21/M21-1</f>
+        <f t="shared" ref="Q41" si="189">Q21/M21-1</f>
         <v>0.15658362989323837</v>
       </c>
       <c r="R41" s="31">
@@ -32494,62 +32530,62 @@
         <v>0.15808823529411775</v>
       </c>
       <c r="S41" s="31">
-        <f t="shared" ref="S41:T41" si="189">S21/O21-1</f>
+        <f t="shared" ref="S41:T41" si="190">S21/O21-1</f>
         <v>1.9607843137254832E-2</v>
       </c>
       <c r="T41" s="31">
-        <f t="shared" si="189"/>
+        <f t="shared" si="190"/>
         <v>-5.1118210862619806E-2</v>
       </c>
       <c r="U41" s="31">
-        <f t="shared" ref="U41" si="190">U21/Q21-1</f>
+        <f t="shared" ref="U41" si="191">U21/Q21-1</f>
         <v>-0.10461538461538467</v>
       </c>
       <c r="V41" s="31">
-        <f t="shared" ref="V41" si="191">V21/R21-1</f>
+        <f t="shared" ref="V41" si="192">V21/R21-1</f>
         <v>-0.10793650793650789</v>
       </c>
       <c r="W41" s="31">
-        <f t="shared" ref="W41" si="192">W21/S21-1</f>
+        <f t="shared" ref="W41" si="193">W21/S21-1</f>
         <v>-0.13141025641025639</v>
       </c>
       <c r="X41" s="31">
-        <f t="shared" ref="X41" si="193">X21/T21-1</f>
+        <f t="shared" ref="X41" si="194">X21/T21-1</f>
         <v>-2.0202020202020221E-2</v>
       </c>
       <c r="Y41" s="31">
-        <f t="shared" ref="Y41" si="194">Y21/U21-1</f>
+        <f t="shared" ref="Y41" si="195">Y21/U21-1</f>
         <v>2.405498281786933E-2</v>
       </c>
       <c r="Z41" s="31">
-        <f t="shared" ref="Z41" si="195">Z21/V21-1</f>
+        <f t="shared" ref="Z41" si="196">Z21/V21-1</f>
         <v>0.35587188612099641</v>
       </c>
       <c r="AA41" s="31">
-        <f t="shared" ref="AA41" si="196">AA21/W21-1</f>
+        <f t="shared" ref="AA41" si="197">AA21/W21-1</f>
         <v>0.40959409594095941</v>
       </c>
       <c r="AC41" s="59" t="s">
         <v>186</v>
       </c>
       <c r="AD41" s="31">
-        <f t="shared" ref="AD41" si="197">AD21/AC21-1</f>
+        <f t="shared" ref="AD41" si="198">AD21/AC21-1</f>
         <v>0.11764705882352944</v>
       </c>
       <c r="AE41" s="31">
-        <f t="shared" ref="AE41" si="198">AE21/AD21-1</f>
+        <f t="shared" ref="AE41" si="199">AE21/AD21-1</f>
         <v>-0.1228070175438597</v>
       </c>
       <c r="AF41" s="31">
-        <f t="shared" ref="AF41" si="199">AF21/AE21-1</f>
+        <f t="shared" ref="AF41" si="200">AF21/AE21-1</f>
         <v>-3.3333333333333326E-2</v>
       </c>
       <c r="AG41" s="31">
-        <f t="shared" ref="AG41" si="200">AG21/AF21-1</f>
+        <f t="shared" ref="AG41" si="201">AG21/AF21-1</f>
         <v>-0.15402298850574714</v>
       </c>
       <c r="AH41" s="31">
-        <f t="shared" ref="AH41" si="201">AH21/AG21-1</f>
+        <f t="shared" ref="AH41" si="202">AH21/AG21-1</f>
         <v>-8.1521739130434812E-2</v>
       </c>
       <c r="AI41" s="31">
@@ -32578,31 +32614,31 @@
         <v>186</v>
       </c>
       <c r="F42" s="78">
-        <f t="shared" ref="F42" si="202">F21-B21</f>
+        <f t="shared" ref="F42" si="203">F21-B21</f>
         <v>-62</v>
       </c>
       <c r="G42" s="78">
-        <f t="shared" ref="G42" si="203">G21-C21</f>
+        <f t="shared" ref="G42" si="204">G21-C21</f>
         <v>3</v>
       </c>
       <c r="H42" s="78">
-        <f t="shared" ref="H42" si="204">H21-D21</f>
+        <f t="shared" ref="H42" si="205">H21-D21</f>
         <v>94</v>
       </c>
       <c r="I42" s="78">
-        <f t="shared" ref="I42:L42" si="205">I21-E21</f>
+        <f t="shared" ref="I42:L42" si="206">I21-E21</f>
         <v>-30</v>
       </c>
       <c r="J42" s="78">
-        <f t="shared" si="205"/>
+        <f t="shared" si="206"/>
         <v>-41</v>
       </c>
       <c r="K42" s="78">
-        <f t="shared" si="205"/>
+        <f t="shared" si="206"/>
         <v>-49</v>
       </c>
       <c r="L42" s="78">
-        <f t="shared" si="205"/>
+        <f t="shared" si="206"/>
         <v>-38</v>
       </c>
       <c r="M42" s="78">
@@ -32610,23 +32646,23 @@
         <v>-57</v>
       </c>
       <c r="N42" s="78">
-        <f t="shared" ref="N42" si="206">N21-J21</f>
+        <f t="shared" ref="N42" si="207">N21-J21</f>
         <v>-46</v>
       </c>
       <c r="O42" s="78">
-        <f t="shared" ref="O42" si="207">O21-K21</f>
+        <f t="shared" ref="O42" si="208">O21-K21</f>
         <v>-8</v>
       </c>
       <c r="P42" s="78">
-        <f t="shared" ref="P42" si="208">P21-L21</f>
+        <f t="shared" ref="P42" si="209">P21-L21</f>
         <v>6</v>
       </c>
       <c r="Q42" s="78">
-        <f t="shared" ref="Q42:R42" si="209">Q21-M21</f>
+        <f t="shared" ref="Q42:R42" si="210">Q21-M21</f>
         <v>44</v>
       </c>
       <c r="R42" s="78">
-        <f t="shared" si="209"/>
+        <f t="shared" si="210"/>
         <v>43</v>
       </c>
       <c r="S42" s="78">
@@ -32638,58 +32674,58 @@
         <v>-16</v>
       </c>
       <c r="U42" s="78">
-        <f t="shared" ref="U42" si="210">U21-Q21</f>
+        <f t="shared" ref="U42" si="211">U21-Q21</f>
         <v>-34</v>
       </c>
       <c r="V42" s="78">
-        <f t="shared" ref="V42" si="211">V21-R21</f>
+        <f t="shared" ref="V42" si="212">V21-R21</f>
         <v>-34</v>
       </c>
       <c r="W42" s="78">
-        <f t="shared" ref="W42" si="212">W21-S21</f>
+        <f t="shared" ref="W42" si="213">W21-S21</f>
         <v>-41</v>
       </c>
       <c r="X42" s="78">
-        <f t="shared" ref="X42" si="213">X21-T21</f>
+        <f t="shared" ref="X42" si="214">X21-T21</f>
         <v>-6</v>
       </c>
       <c r="Y42" s="78">
-        <f t="shared" ref="Y42" si="214">Y21-U21</f>
+        <f t="shared" ref="Y42" si="215">Y21-U21</f>
         <v>7</v>
       </c>
       <c r="Z42" s="78">
-        <f t="shared" ref="Z42" si="215">Z21-V21</f>
+        <f t="shared" ref="Z42" si="216">Z21-V21</f>
         <v>100</v>
       </c>
       <c r="AA42" s="78">
-        <f t="shared" ref="AA42" si="216">AA21-W21</f>
+        <f t="shared" ref="AA42" si="217">AA21-W21</f>
         <v>111</v>
       </c>
       <c r="AC42" s="59" t="s">
         <v>186</v>
       </c>
       <c r="AD42" s="78">
-        <f t="shared" ref="AD42" si="217">AD21-AC21</f>
+        <f t="shared" ref="AD42" si="218">AD21-AC21</f>
         <v>54</v>
       </c>
       <c r="AE42" s="78">
-        <f t="shared" ref="AE42" si="218">AE21-AD21</f>
+        <f t="shared" ref="AE42" si="219">AE21-AD21</f>
         <v>-63</v>
       </c>
       <c r="AF42" s="78">
-        <f t="shared" ref="AF42" si="219">AF21-AE21</f>
+        <f t="shared" ref="AF42" si="220">AF21-AE21</f>
         <v>-15</v>
       </c>
       <c r="AG42" s="78">
-        <f t="shared" ref="AG42" si="220">AG21-AF21</f>
+        <f t="shared" ref="AG42" si="221">AG21-AF21</f>
         <v>-67</v>
       </c>
       <c r="AH42" s="78">
-        <f t="shared" ref="AH42:AI42" si="221">AH21-AG21</f>
+        <f t="shared" ref="AH42:AI42" si="222">AH21-AG21</f>
         <v>-30</v>
       </c>
       <c r="AI42" s="78">
-        <f t="shared" si="221"/>
+        <f t="shared" si="222"/>
         <v>-57</v>
       </c>
       <c r="AJ42" s="78">
@@ -32705,63 +32741,63 @@
         <v>186</v>
       </c>
       <c r="C43" s="24">
-        <f t="shared" ref="C43" si="222">C21/B21-1</f>
+        <f t="shared" ref="C43" si="223">C21/B21-1</f>
         <v>-0.14489311163895491</v>
       </c>
       <c r="D43" s="24">
-        <f t="shared" ref="D43" si="223">D21/C21-1</f>
+        <f t="shared" ref="D43" si="224">D21/C21-1</f>
         <v>-0.30277777777777781</v>
       </c>
       <c r="E43" s="24">
-        <f t="shared" ref="E43" si="224">E21/D21-1</f>
+        <f t="shared" ref="E43" si="225">E21/D21-1</f>
         <v>0.46613545816733071</v>
       </c>
       <c r="F43" s="24">
-        <f t="shared" ref="F43" si="225">F21/E21-1</f>
+        <f t="shared" ref="F43" si="226">F21/E21-1</f>
         <v>-2.4456521739130488E-2</v>
       </c>
       <c r="G43" s="24">
-        <f t="shared" ref="G43" si="226">G21/F21-1</f>
+        <f t="shared" ref="G43" si="227">G21/F21-1</f>
         <v>1.1142061281337101E-2</v>
       </c>
       <c r="H43" s="24">
-        <f t="shared" ref="H43" si="227">H21/G21-1</f>
+        <f t="shared" ref="H43" si="228">H21/G21-1</f>
         <v>-4.9586776859504078E-2</v>
       </c>
       <c r="I43" s="24">
-        <f t="shared" ref="I43" si="228">I21/H21-1</f>
+        <f t="shared" ref="I43" si="229">I21/H21-1</f>
         <v>-2.0289855072463725E-2</v>
       </c>
       <c r="J43" s="24">
-        <f t="shared" ref="J43" si="229">J21/I21-1</f>
+        <f t="shared" ref="J43" si="230">J21/I21-1</f>
         <v>-5.9171597633136064E-2</v>
       </c>
       <c r="K43" s="24">
-        <f t="shared" ref="K43" si="230">K21/J21-1</f>
+        <f t="shared" ref="K43" si="231">K21/J21-1</f>
         <v>-1.2578616352201255E-2</v>
       </c>
       <c r="L43" s="24">
-        <f t="shared" ref="L43" si="231">L21/K21-1</f>
+        <f t="shared" ref="L43" si="232">L21/K21-1</f>
         <v>-2.2292993630573243E-2</v>
       </c>
       <c r="M43" s="24">
-        <f t="shared" ref="M43" si="232">M21/L21-1</f>
+        <f t="shared" ref="M43" si="233">M21/L21-1</f>
         <v>-8.4690553745928376E-2</v>
       </c>
       <c r="N43" s="24">
-        <f t="shared" ref="N43" si="233">N21/M21-1</f>
+        <f t="shared" ref="N43" si="234">N21/M21-1</f>
         <v>-3.2028469750889688E-2</v>
       </c>
       <c r="O43" s="24">
-        <f t="shared" ref="O43" si="234">O21/N21-1</f>
+        <f t="shared" ref="O43" si="235">O21/N21-1</f>
         <v>0.125</v>
       </c>
       <c r="P43" s="24">
-        <f t="shared" ref="P43" si="235">P21/O21-1</f>
+        <f t="shared" ref="P43" si="236">P21/O21-1</f>
         <v>2.2875816993463971E-2</v>
       </c>
       <c r="Q43" s="24">
-        <f t="shared" ref="Q43" si="236">Q21/P21-1</f>
+        <f t="shared" ref="Q43" si="237">Q21/P21-1</f>
         <v>3.833865814696491E-2</v>
       </c>
       <c r="R43" s="24">
@@ -32769,39 +32805,39 @@
         <v>-3.0769230769230771E-2</v>
       </c>
       <c r="S43" s="24">
-        <f t="shared" ref="S43:T43" si="237">S21/R21-1</f>
+        <f t="shared" ref="S43:T43" si="238">S21/R21-1</f>
         <v>-9.52380952380949E-3</v>
       </c>
       <c r="T43" s="24">
-        <f t="shared" si="237"/>
+        <f t="shared" si="238"/>
         <v>-4.8076923076923128E-2</v>
       </c>
       <c r="U43" s="24">
-        <f t="shared" ref="U43" si="238">U21/T21-1</f>
+        <f t="shared" ref="U43" si="239">U21/T21-1</f>
         <v>-2.0202020202020221E-2</v>
       </c>
       <c r="V43" s="24">
-        <f t="shared" ref="V43" si="239">V21/U21-1</f>
+        <f t="shared" ref="V43" si="240">V21/U21-1</f>
         <v>-3.4364261168384869E-2</v>
       </c>
       <c r="W43" s="24">
-        <f t="shared" ref="W43" si="240">W21/V21-1</f>
+        <f t="shared" ref="W43" si="241">W21/V21-1</f>
         <v>-3.5587188612099641E-2</v>
       </c>
       <c r="X43" s="24">
-        <f t="shared" ref="X43" si="241">X21/W21-1</f>
+        <f t="shared" ref="X43" si="242">X21/W21-1</f>
         <v>7.3800738007380184E-2</v>
       </c>
       <c r="Y43" s="24">
-        <f t="shared" ref="Y43" si="242">Y21/X21-1</f>
+        <f t="shared" ref="Y43" si="243">Y21/X21-1</f>
         <v>2.405498281786933E-2</v>
       </c>
       <c r="Z43" s="24">
-        <f t="shared" ref="Z43" si="243">Z21/Y21-1</f>
+        <f t="shared" ref="Z43" si="244">Z21/Y21-1</f>
         <v>0.27852348993288589</v>
       </c>
       <c r="AA43" s="24">
-        <f t="shared" ref="AA43" si="244">AA21/Z21-1</f>
+        <f t="shared" ref="AA43" si="245">AA21/Z21-1</f>
         <v>2.624671916010568E-3</v>
       </c>
       <c r="AC43" s="59" t="s">
@@ -32837,67 +32873,67 @@
         <v>186</v>
       </c>
       <c r="C44" s="75">
-        <f t="shared" ref="C44" si="245">C21-B21</f>
+        <f t="shared" ref="C44" si="246">C21-B21</f>
         <v>-61</v>
       </c>
       <c r="D44" s="75">
-        <f t="shared" ref="D44" si="246">D21-C21</f>
+        <f t="shared" ref="D44" si="247">D21-C21</f>
         <v>-109</v>
       </c>
       <c r="E44" s="75">
-        <f t="shared" ref="E44" si="247">E21-D21</f>
+        <f t="shared" ref="E44" si="248">E21-D21</f>
         <v>117</v>
       </c>
       <c r="F44" s="75">
-        <f t="shared" ref="F44" si="248">F21-E21</f>
+        <f t="shared" ref="F44" si="249">F21-E21</f>
         <v>-9</v>
       </c>
       <c r="G44" s="75">
-        <f t="shared" ref="G44" si="249">G21-F21</f>
+        <f t="shared" ref="G44" si="250">G21-F21</f>
         <v>4</v>
       </c>
       <c r="H44" s="75">
-        <f t="shared" ref="H44" si="250">H21-G21</f>
+        <f t="shared" ref="H44" si="251">H21-G21</f>
         <v>-18</v>
       </c>
       <c r="I44" s="75">
-        <f t="shared" ref="I44" si="251">I21-H21</f>
+        <f t="shared" ref="I44" si="252">I21-H21</f>
         <v>-7</v>
       </c>
       <c r="J44" s="75">
-        <f t="shared" ref="J44" si="252">J21-I21</f>
+        <f t="shared" ref="J44" si="253">J21-I21</f>
         <v>-20</v>
       </c>
       <c r="K44" s="75">
-        <f t="shared" ref="K44" si="253">K21-J21</f>
+        <f t="shared" ref="K44" si="254">K21-J21</f>
         <v>-4</v>
       </c>
       <c r="L44" s="75">
-        <f t="shared" ref="L44" si="254">L21-K21</f>
+        <f t="shared" ref="L44" si="255">L21-K21</f>
         <v>-7</v>
       </c>
       <c r="M44" s="75">
-        <f t="shared" ref="M44" si="255">M21-L21</f>
+        <f t="shared" ref="M44" si="256">M21-L21</f>
         <v>-26</v>
       </c>
       <c r="N44" s="75">
-        <f t="shared" ref="N44" si="256">N21-M21</f>
+        <f t="shared" ref="N44" si="257">N21-M21</f>
         <v>-9</v>
       </c>
       <c r="O44" s="75">
-        <f t="shared" ref="O44" si="257">O21-N21</f>
+        <f t="shared" ref="O44" si="258">O21-N21</f>
         <v>34</v>
       </c>
       <c r="P44" s="75">
-        <f t="shared" ref="P44:R44" si="258">P21-O21</f>
+        <f t="shared" ref="P44:R44" si="259">P21-O21</f>
         <v>7</v>
       </c>
       <c r="Q44" s="75">
-        <f t="shared" si="258"/>
+        <f t="shared" si="259"/>
         <v>12</v>
       </c>
       <c r="R44" s="75">
-        <f t="shared" si="258"/>
+        <f t="shared" si="259"/>
         <v>-10</v>
       </c>
       <c r="S44" s="75">
@@ -32909,31 +32945,31 @@
         <v>-15</v>
       </c>
       <c r="U44" s="75">
-        <f t="shared" ref="U44" si="259">U21-T21</f>
+        <f t="shared" ref="U44" si="260">U21-T21</f>
         <v>-6</v>
       </c>
       <c r="V44" s="75">
-        <f t="shared" ref="V44" si="260">V21-U21</f>
+        <f t="shared" ref="V44" si="261">V21-U21</f>
         <v>-10</v>
       </c>
       <c r="W44" s="75">
-        <f t="shared" ref="W44" si="261">W21-V21</f>
+        <f t="shared" ref="W44" si="262">W21-V21</f>
         <v>-10</v>
       </c>
       <c r="X44" s="75">
-        <f t="shared" ref="X44" si="262">X21-W21</f>
+        <f t="shared" ref="X44" si="263">X21-W21</f>
         <v>20</v>
       </c>
       <c r="Y44" s="75">
-        <f t="shared" ref="Y44" si="263">Y21-X21</f>
+        <f t="shared" ref="Y44" si="264">Y21-X21</f>
         <v>7</v>
       </c>
       <c r="Z44" s="75">
-        <f t="shared" ref="Z44" si="264">Z21-Y21</f>
+        <f t="shared" ref="Z44" si="265">Z21-Y21</f>
         <v>83</v>
       </c>
       <c r="AA44" s="75">
-        <f t="shared" ref="AA44" si="265">AA21-Z21</f>
+        <f t="shared" ref="AA44" si="266">AA21-Z21</f>
         <v>1</v>
       </c>
       <c r="AC44" s="59" t="s">
@@ -32966,75 +33002,75 @@
         <v>260</v>
       </c>
       <c r="B46" s="24">
-        <f t="shared" ref="B46:S46" si="266">B12/B3</f>
+        <f t="shared" ref="B46:S46" si="267">B12/B3</f>
         <v>0.77057220708446872</v>
       </c>
       <c r="C46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.80022197558268593</v>
       </c>
       <c r="D46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.85304449648711944</v>
       </c>
       <c r="E46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.80193756727664156</v>
       </c>
       <c r="F46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.80698924731182797</v>
       </c>
       <c r="G46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.80793650793650795</v>
       </c>
       <c r="H46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.81736368448914765</v>
       </c>
       <c r="I46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.82368283776734486</v>
       </c>
       <c r="J46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.83280757097791802</v>
       </c>
       <c r="K46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.83491062039957942</v>
       </c>
       <c r="L46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.83859095688748686</v>
       </c>
       <c r="M46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.85241596638655459</v>
       </c>
       <c r="N46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="O46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.84323770491803274</v>
       </c>
       <c r="P46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.84095528455284552</v>
       </c>
       <c r="Q46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.83717434869739482</v>
       </c>
       <c r="R46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.8418674698795181</v>
       </c>
       <c r="S46" s="24">
-        <f t="shared" si="266"/>
+        <f t="shared" si="267"/>
         <v>0.84399999999999997</v>
       </c>
       <c r="T46" s="24">
@@ -33042,63 +33078,63 @@
         <v>0.85112781954887218</v>
       </c>
       <c r="U46" s="24">
-        <f t="shared" ref="U46:Y46" si="267">U12/U3</f>
+        <f t="shared" ref="U46:Y46" si="268">U12/U3</f>
         <v>0.85586924219910843</v>
       </c>
       <c r="V46" s="24">
-        <f t="shared" si="267"/>
+        <f t="shared" si="268"/>
         <v>0.86061507936507942</v>
       </c>
       <c r="W46" s="24">
-        <f t="shared" si="267"/>
+        <f t="shared" si="268"/>
         <v>0.86604053386060309</v>
       </c>
       <c r="X46" s="24">
-        <f t="shared" si="267"/>
+        <f t="shared" si="268"/>
         <v>0.85860058309037901</v>
       </c>
       <c r="Y46" s="24">
-        <f t="shared" si="267"/>
+        <f t="shared" si="268"/>
         <v>0.85980861244019136</v>
       </c>
       <c r="Z46" s="24">
-        <f t="shared" ref="Z46:AA46" si="268">Z12/Z3</f>
+        <f t="shared" ref="Z46:AA46" si="269">Z12/Z3</f>
         <v>0.8275229357798165</v>
       </c>
       <c r="AA46" s="24">
-        <f t="shared" si="268"/>
+        <f t="shared" si="269"/>
         <v>0.82863636363636362</v>
       </c>
       <c r="AC46" s="24">
-        <f t="shared" ref="AC46:AJ46" si="269">AC12/AC3</f>
+        <f t="shared" ref="AC46:AJ46" si="270">AC12/AC3</f>
         <v>0.70367979341510656</v>
       </c>
       <c r="AD46" s="24">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>0.693075117370892</v>
       </c>
       <c r="AE46" s="24">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>0.74271012006861059</v>
       </c>
       <c r="AF46" s="24">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>0.76294277929155319</v>
       </c>
       <c r="AG46" s="24">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>0.80193756727664156</v>
       </c>
       <c r="AH46" s="24">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>0.82368283776734486</v>
       </c>
       <c r="AI46" s="24">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>0.85241596638655459</v>
       </c>
       <c r="AJ46" s="24">
-        <f t="shared" si="269"/>
+        <f t="shared" si="270"/>
         <v>0.83717434869739482</v>
       </c>
     </row>

</xml_diff>

<commit_message>
$ERJ India news/speculation, 52wk high
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CB985C-DA51-435C-B14B-054CF93B5525}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2625A6-AD73-4272-BBD0-E3BE0B32F238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="2010" windowWidth="26610" windowHeight="12885" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="320">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1170,6 +1170,9 @@
   <si>
     <t>Virgin Australia place firm order for 8 E190-E2 regional jets to replace their aging Fokker 100 fleet</t>
   </si>
+  <si>
+    <t>Embraer in talks with Indian Govt. to set up manufacturing facility in India dependent on Indian adoption of E-Jets</t>
+  </si>
 </sst>
 </file>
 
@@ -1764,6 +1767,27 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1771,39 +1795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1827,6 +1818,33 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1837,21 +1855,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9951,7 +9954,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC87"/>
+  <dimension ref="A2:AC89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -9974,50 +9977,50 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="116"/>
-      <c r="G5" s="114" t="s">
+      <c r="C5" s="122"/>
+      <c r="D5" s="123"/>
+      <c r="G5" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115"/>
-      <c r="R5" s="116"/>
-      <c r="T5" s="114" t="s">
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="122"/>
+      <c r="N5" s="122"/>
+      <c r="O5" s="122"/>
+      <c r="P5" s="122"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="123"/>
+      <c r="T5" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="116"/>
-      <c r="Y5" s="114" t="s">
+      <c r="U5" s="122"/>
+      <c r="V5" s="122"/>
+      <c r="W5" s="123"/>
+      <c r="Y5" s="121" t="s">
         <v>313</v>
       </c>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="116"/>
+      <c r="Z5" s="122"/>
+      <c r="AA5" s="123"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>32.75</v>
+        <v>32.82</v>
       </c>
       <c r="D6" s="17"/>
       <c r="G6" s="8">
         <v>45505</v>
       </c>
       <c r="H6" s="92" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
@@ -10082,14 +10085,14 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>6014.5375000000004</v>
+        <v>6027.393</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
-        <v>45474</v>
+        <v>45505</v>
       </c>
       <c r="H8" s="92" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
@@ -10161,7 +10164,7 @@
         <v>45474</v>
       </c>
       <c r="H10" s="92" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -10221,14 +10224,14 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>7222.2375000000011</v>
+        <v>7235.0930000000008</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
-        <v>45413</v>
+        <v>45474</v>
       </c>
       <c r="H12" s="92" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -10244,13 +10247,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="114" t="s">
+      <c r="Y12" s="121" t="s">
         <v>215</v>
       </c>
-      <c r="Z12" s="115"/>
-      <c r="AA12" s="115"/>
-      <c r="AB12" s="115"/>
-      <c r="AC12" s="116"/>
+      <c r="Z12" s="122"/>
+      <c r="AA12" s="122"/>
+      <c r="AB12" s="122"/>
+      <c r="AC12" s="123"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -10272,21 +10275,21 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="86"/>
-      <c r="Z13" s="126" t="s">
+      <c r="Z13" s="131" t="s">
         <v>216</v>
       </c>
-      <c r="AA13" s="126"/>
-      <c r="AB13" s="126" t="s">
+      <c r="AA13" s="131"/>
+      <c r="AB13" s="131" t="s">
         <v>217</v>
       </c>
-      <c r="AC13" s="127"/>
+      <c r="AC13" s="132"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
         <v>45413</v>
       </c>
       <c r="H14" s="92" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
@@ -10307,21 +10310,21 @@
       <c r="Y14" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="Z14" s="123" t="s">
+      <c r="Z14" s="114" t="s">
         <v>227</v>
       </c>
-      <c r="AA14" s="123"/>
-      <c r="AB14" s="123" t="s">
+      <c r="AA14" s="114"/>
+      <c r="AB14" s="114" t="s">
         <v>228</v>
       </c>
-      <c r="AC14" s="122"/>
+      <c r="AC14" s="115"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="116"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="123"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -10343,14 +10346,14 @@
       <c r="Y15" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="Z15" s="123" t="s">
+      <c r="Z15" s="114" t="s">
         <v>223</v>
       </c>
-      <c r="AA15" s="123"/>
-      <c r="AB15" s="123" t="s">
+      <c r="AA15" s="114"/>
+      <c r="AB15" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="AC15" s="122"/>
+      <c r="AC15" s="115"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -10359,18 +10362,18 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="122"/>
+      <c r="D16" s="115"/>
       <c r="E16" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G16" s="8">
-        <v>44986</v>
+        <v>45413</v>
       </c>
       <c r="H16" s="92" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
@@ -10391,23 +10394,23 @@
       <c r="Y16" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z16" s="123" t="s">
+      <c r="Z16" s="114" t="s">
         <v>224</v>
       </c>
-      <c r="AA16" s="123"/>
-      <c r="AB16" s="123" t="s">
+      <c r="AA16" s="114"/>
+      <c r="AB16" s="114" t="s">
         <v>230</v>
       </c>
-      <c r="AC16" s="122"/>
+      <c r="AC16" s="115"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="123" t="s">
+      <c r="C17" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="122"/>
+      <c r="D17" s="115"/>
       <c r="E17" s="3" t="s">
         <v>301</v>
       </c>
@@ -10430,24 +10433,24 @@
       <c r="Y17" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z17" s="123" t="s">
+      <c r="Z17" s="114" t="s">
         <v>225</v>
       </c>
-      <c r="AA17" s="123"/>
-      <c r="AB17" s="123" t="s">
+      <c r="AA17" s="114"/>
+      <c r="AB17" s="114" t="s">
         <v>231</v>
       </c>
-      <c r="AC17" s="122"/>
+      <c r="AC17" s="115"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="122"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="115"/>
       <c r="G18" s="8">
         <v>44986</v>
       </c>
       <c r="H18" s="92" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
@@ -10468,19 +10471,19 @@
       <c r="Y18" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z18" s="123" t="s">
+      <c r="Z18" s="114" t="s">
         <v>226</v>
       </c>
-      <c r="AA18" s="123"/>
-      <c r="AB18" s="123" t="s">
+      <c r="AA18" s="114"/>
+      <c r="AB18" s="114" t="s">
         <v>232</v>
       </c>
-      <c r="AC18" s="122"/>
+      <c r="AC18" s="115"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="139"/>
-      <c r="D19" s="140"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="120"/>
       <c r="G19" s="9"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -10502,21 +10505,21 @@
       <c r="Y19" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="Z19" s="123" t="s">
+      <c r="Z19" s="114" t="s">
         <v>234</v>
       </c>
-      <c r="AA19" s="123"/>
-      <c r="AB19" s="123" t="s">
+      <c r="AA19" s="114"/>
+      <c r="AB19" s="114" t="s">
         <v>235</v>
       </c>
-      <c r="AC19" s="122"/>
+      <c r="AC19" s="115"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="8">
         <v>44986</v>
       </c>
       <c r="H20" s="92" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
@@ -10537,14 +10540,14 @@
       <c r="Y20" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="Z20" s="123" t="s">
+      <c r="Z20" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="AA20" s="123"/>
-      <c r="AB20" s="123" t="s">
+      <c r="AA20" s="114"/>
+      <c r="AB20" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="AC20" s="122"/>
+      <c r="AC20" s="115"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -10572,16 +10575,16 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="114" t="s">
+      <c r="B22" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="115"/>
-      <c r="D22" s="116"/>
+      <c r="C22" s="122"/>
+      <c r="D22" s="123"/>
       <c r="G22" s="8">
-        <v>45261</v>
+        <v>44986</v>
       </c>
       <c r="H22" s="92" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
@@ -10609,10 +10612,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="114" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="122"/>
+      <c r="D23" s="115"/>
       <c r="G23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -10634,15 +10637,15 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="123">
+      <c r="C24" s="114">
         <v>1969</v>
       </c>
-      <c r="D24" s="122"/>
+      <c r="D24" s="115"/>
       <c r="G24" s="8">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="H24" s="92" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
@@ -10663,8 +10666,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="122"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="115"/>
       <c r="G25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -10683,28 +10686,28 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="141" t="s">
+      <c r="Y25" s="116" t="s">
         <v>286</v>
       </c>
-      <c r="Z25" s="142"/>
-      <c r="AA25" s="142"/>
-      <c r="AB25" s="142"/>
-      <c r="AC25" s="143"/>
+      <c r="Z25" s="117"/>
+      <c r="AA25" s="117"/>
+      <c r="AB25" s="117"/>
+      <c r="AC25" s="118"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="137">
+      <c r="C26" s="142">
         <f>'Financial Model'!Z70</f>
         <v>2636</v>
       </c>
-      <c r="D26" s="138"/>
+      <c r="D26" s="143"/>
       <c r="G26" s="8">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="H26" s="92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
@@ -10732,8 +10735,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="122"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="115"/>
       <c r="G27" s="9"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -10764,16 +10767,16 @@
       <c r="B28" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="C28" s="121">
+      <c r="C28" s="137">
         <f>+'Order &amp; Backlog'!$AA$3</f>
         <v>2200</v>
       </c>
-      <c r="D28" s="122"/>
+      <c r="D28" s="115"/>
       <c r="G28" s="8">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="H28" s="92" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="I28" s="34"/>
       <c r="J28" s="34"/>
@@ -10803,11 +10806,11 @@
       <c r="B29" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="121">
+      <c r="C29" s="137">
         <f>'Order &amp; Backlog'!AA21</f>
         <v>382</v>
       </c>
-      <c r="D29" s="122"/>
+      <c r="D29" s="115"/>
       <c r="G29" s="9"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
@@ -10836,16 +10839,16 @@
       <c r="B30" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="123">
+      <c r="C30" s="114">
         <f>'Financial Model'!AB43</f>
         <v>47</v>
       </c>
-      <c r="D30" s="122"/>
+      <c r="D30" s="115"/>
       <c r="G30" s="8">
-        <v>45017</v>
+        <v>45170</v>
       </c>
       <c r="H30" s="92" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
@@ -10873,10 +10876,10 @@
       <c r="B31" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C31" s="124">
+      <c r="C31" s="138">
         <v>36708</v>
       </c>
-      <c r="D31" s="125"/>
+      <c r="D31" s="139"/>
       <c r="G31" s="9"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -10905,13 +10908,13 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="122"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="115"/>
       <c r="G32" s="8">
         <v>45017</v>
       </c>
-      <c r="H32" s="98" t="s">
-        <v>266</v>
+      <c r="H32" s="92" t="s">
+        <v>269</v>
       </c>
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
@@ -10973,15 +10976,15 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="133" t="s">
+      <c r="C34" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="134"/>
+      <c r="D34" s="130"/>
       <c r="G34" s="8">
-        <v>44927</v>
-      </c>
-      <c r="H34" s="94" t="s">
-        <v>263</v>
+        <v>45017</v>
+      </c>
+      <c r="H34" s="98" t="s">
+        <v>266</v>
       </c>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
@@ -11028,10 +11031,10 @@
     </row>
     <row r="36" spans="2:29">
       <c r="G36" s="8">
-        <v>44896</v>
-      </c>
-      <c r="H36" s="92" t="s">
-        <v>261</v>
+        <v>44927</v>
+      </c>
+      <c r="H36" s="94" t="s">
+        <v>263</v>
       </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
@@ -11050,11 +11053,11 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="114" t="s">
+      <c r="B37" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="115"/>
-      <c r="D37" s="116"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="123"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -11067,12 +11070,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="114" t="s">
+      <c r="T37" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="115"/>
-      <c r="V37" s="115"/>
-      <c r="W37" s="116"/>
+      <c r="U37" s="122"/>
+      <c r="V37" s="122"/>
+      <c r="W37" s="123"/>
       <c r="Y37" s="39" t="s">
         <v>278</v>
       </c>
@@ -11085,16 +11088,16 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="135">
+      <c r="C38" s="140">
         <f>C6/'Financial Model'!AB125</f>
-        <v>7.7262990558160523</v>
-      </c>
-      <c r="D38" s="136"/>
+        <v>7.7428132828055825</v>
+      </c>
+      <c r="D38" s="141"/>
       <c r="G38" s="8">
-        <v>44866</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>259</v>
+        <v>44896</v>
+      </c>
+      <c r="H38" s="92" t="s">
+        <v>261</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -11124,11 +11127,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="135">
+      <c r="C39" s="140">
         <f>+C8/SUM('Financial Model'!Y4:AB4)</f>
-        <v>3.115856343573538</v>
-      </c>
-      <c r="D39" s="136"/>
+        <v>3.1225161891933899</v>
+      </c>
+      <c r="D39" s="141"/>
       <c r="G39" s="9"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -11157,16 +11160,16 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="131">
+      <c r="C40" s="127">
         <f>C6/SUM('Financial Model'!Y26:AB26)</f>
-        <v>63.028949436730421</v>
-      </c>
-      <c r="D40" s="132"/>
+        <v>63.163667801938701</v>
+      </c>
+      <c r="D40" s="128"/>
       <c r="G40" s="8">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
@@ -11216,8 +11219,12 @@
       <c r="AC41" s="35"/>
     </row>
     <row r="42" spans="2:29">
-      <c r="G42" s="9"/>
-      <c r="H42" s="34"/>
+      <c r="G42" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
       <c r="K42" s="34"/>
@@ -11239,17 +11246,13 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="114" t="s">
+      <c r="B43" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="C43" s="115"/>
-      <c r="D43" s="116"/>
-      <c r="G43" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="C43" s="122"/>
+      <c r="D43" s="123"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="34"/>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
       <c r="K43" s="34"/>
@@ -11275,17 +11278,15 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="117" t="s">
+      <c r="B44" s="133" t="s">
         <v>244</v>
       </c>
-      <c r="C44" s="118"/>
+      <c r="C44" s="134"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
       <c r="G44" s="9"/>
-      <c r="H44" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="H44" s="34"/>
       <c r="I44" s="34"/>
       <c r="J44" s="34"/>
       <c r="K44" s="34"/>
@@ -11311,16 +11312,18 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="117" t="s">
+      <c r="B45" s="133" t="s">
         <v>245</v>
       </c>
-      <c r="C45" s="118"/>
+      <c r="C45" s="134"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="7" t="s">
-        <v>13</v>
+      <c r="G45" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
@@ -11347,13 +11350,15 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="117"/>
-      <c r="C46" s="118"/>
+      <c r="B46" s="133"/>
+      <c r="C46" s="134"/>
       <c r="D46" s="83" t="s">
         <v>31</v>
       </c>
       <c r="G46" s="9"/>
-      <c r="H46" s="34"/>
+      <c r="H46" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
@@ -11375,16 +11380,14 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="117"/>
-      <c r="C47" s="118"/>
+      <c r="B47" s="133"/>
+      <c r="C47" s="134"/>
       <c r="D47" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>29</v>
+      <c r="G47" s="9"/>
+      <c r="H47" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I47" s="34"/>
       <c r="J47" s="34"/>
@@ -11411,15 +11414,13 @@
       <c r="AC47" s="35"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="119"/>
-      <c r="C48" s="120"/>
+      <c r="B48" s="135"/>
+      <c r="C48" s="136"/>
       <c r="D48" s="84" t="s">
         <v>31</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="H48" s="34"/>
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
@@ -11445,8 +11446,12 @@
       <c r="AC48" s="35"/>
     </row>
     <row r="49" spans="7:29">
-      <c r="G49" s="9"/>
-      <c r="H49" s="34"/>
+      <c r="G49" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
@@ -11473,7 +11478,9 @@
     </row>
     <row r="50" spans="7:29">
       <c r="G50" s="9"/>
-      <c r="H50" s="34"/>
+      <c r="H50" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I50" s="34"/>
       <c r="J50" s="34"/>
       <c r="K50" s="34"/>
@@ -11493,12 +11500,8 @@
       <c r="AC50" s="35"/>
     </row>
     <row r="51" spans="7:29">
-      <c r="G51" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>187</v>
-      </c>
+      <c r="G51" s="9"/>
+      <c r="H51" s="34"/>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
@@ -11537,8 +11540,12 @@
       <c r="AC52" s="35"/>
     </row>
     <row r="53" spans="7:29">
-      <c r="G53" s="9"/>
-      <c r="H53" s="34"/>
+      <c r="G53" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="I53" s="34"/>
       <c r="J53" s="34"/>
       <c r="K53" s="34"/>
@@ -11558,12 +11565,8 @@
       <c r="AC53" s="35"/>
     </row>
     <row r="54" spans="7:29">
-      <c r="G54" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="G54" s="9"/>
+      <c r="H54" s="34"/>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
       <c r="K54" s="34"/>
@@ -11584,9 +11587,7 @@
     </row>
     <row r="55" spans="7:29">
       <c r="G55" s="9"/>
-      <c r="H55" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="H55" s="34"/>
       <c r="I55" s="34"/>
       <c r="J55" s="34"/>
       <c r="K55" s="34"/>
@@ -11606,9 +11607,11 @@
       <c r="AC55" s="35"/>
     </row>
     <row r="56" spans="7:29">
-      <c r="G56" s="9"/>
-      <c r="H56" s="7" t="s">
-        <v>193</v>
+      <c r="G56" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
@@ -11629,7 +11632,7 @@
     <row r="57" spans="7:29">
       <c r="G57" s="9"/>
       <c r="H57" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I57" s="34"/>
       <c r="J57" s="34"/>
@@ -11640,9 +11643,7 @@
       <c r="O57" s="34"/>
       <c r="P57" s="34"/>
       <c r="Q57" s="34"/>
-      <c r="R57" s="48" t="s">
-        <v>194</v>
-      </c>
+      <c r="R57" s="35"/>
       <c r="Y57" s="101"/>
       <c r="Z57" s="102"/>
       <c r="AA57" s="102"/>
@@ -11651,7 +11652,9 @@
     </row>
     <row r="58" spans="7:29">
       <c r="G58" s="9"/>
-      <c r="H58" s="34"/>
+      <c r="H58" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
@@ -11662,17 +11665,19 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
-      <c r="Y58" s="128" t="s">
+      <c r="Y58" s="124" t="s">
         <v>293</v>
       </c>
-      <c r="Z58" s="129"/>
-      <c r="AA58" s="129"/>
-      <c r="AB58" s="129"/>
-      <c r="AC58" s="130"/>
+      <c r="Z58" s="125"/>
+      <c r="AA58" s="125"/>
+      <c r="AB58" s="125"/>
+      <c r="AC58" s="126"/>
     </row>
     <row r="59" spans="7:29">
       <c r="G59" s="9"/>
-      <c r="H59" s="34"/>
+      <c r="H59" s="7" t="s">
+        <v>191</v>
+      </c>
       <c r="I59" s="34"/>
       <c r="J59" s="34"/>
       <c r="K59" s="34"/>
@@ -11682,15 +11687,13 @@
       <c r="O59" s="34"/>
       <c r="P59" s="34"/>
       <c r="Q59" s="34"/>
-      <c r="R59" s="35"/>
+      <c r="R59" s="48" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="60" spans="7:29">
-      <c r="G60" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>196</v>
-      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="34"/>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
       <c r="K60" s="34"/>
@@ -11704,9 +11707,7 @@
     </row>
     <row r="61" spans="7:29">
       <c r="G61" s="9"/>
-      <c r="H61" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="H61" s="34"/>
       <c r="I61" s="34"/>
       <c r="J61" s="34"/>
       <c r="K61" s="34"/>
@@ -11719,9 +11720,11 @@
       <c r="R61" s="35"/>
     </row>
     <row r="62" spans="7:29">
-      <c r="G62" s="9"/>
-      <c r="H62" s="47" t="s">
-        <v>198</v>
+      <c r="G62" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
@@ -11736,7 +11739,9 @@
     </row>
     <row r="63" spans="7:29">
       <c r="G63" s="9"/>
-      <c r="H63" s="34"/>
+      <c r="H63" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="I63" s="34"/>
       <c r="J63" s="34"/>
       <c r="K63" s="34"/>
@@ -11749,11 +11754,9 @@
       <c r="R63" s="35"/>
     </row>
     <row r="64" spans="7:29">
-      <c r="G64" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>237</v>
+      <c r="G64" s="9"/>
+      <c r="H64" s="47" t="s">
+        <v>198</v>
       </c>
       <c r="I64" s="34"/>
       <c r="J64" s="34"/>
@@ -11768,9 +11771,7 @@
     </row>
     <row r="65" spans="7:18">
       <c r="G65" s="9"/>
-      <c r="H65" s="7" t="s">
-        <v>238</v>
-      </c>
+      <c r="H65" s="34"/>
       <c r="I65" s="34"/>
       <c r="J65" s="34"/>
       <c r="K65" s="34"/>
@@ -11783,8 +11784,12 @@
       <c r="R65" s="35"/>
     </row>
     <row r="66" spans="7:18">
-      <c r="G66" s="9"/>
-      <c r="H66" s="34"/>
+      <c r="G66" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>237</v>
+      </c>
       <c r="I66" s="34"/>
       <c r="J66" s="34"/>
       <c r="K66" s="34"/>
@@ -11797,11 +11802,9 @@
       <c r="R66" s="35"/>
     </row>
     <row r="67" spans="7:18">
-      <c r="G67" s="8">
-        <v>44682</v>
-      </c>
-      <c r="H67" s="34" t="s">
-        <v>246</v>
+      <c r="G67" s="9"/>
+      <c r="H67" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="I67" s="34"/>
       <c r="J67" s="34"/>
@@ -11816,9 +11819,7 @@
     </row>
     <row r="68" spans="7:18">
       <c r="G68" s="9"/>
-      <c r="H68" s="7" t="s">
-        <v>247</v>
-      </c>
+      <c r="H68" s="34"/>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
       <c r="K68" s="34"/>
@@ -11828,13 +11829,15 @@
       <c r="O68" s="34"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="34"/>
-      <c r="R68" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R68" s="35"/>
     </row>
     <row r="69" spans="7:18">
-      <c r="G69" s="9"/>
-      <c r="H69" s="34"/>
+      <c r="G69" s="8">
+        <v>44682</v>
+      </c>
+      <c r="H69" s="34" t="s">
+        <v>246</v>
+      </c>
       <c r="I69" s="34"/>
       <c r="J69" s="34"/>
       <c r="K69" s="34"/>
@@ -11847,11 +11850,9 @@
       <c r="R69" s="35"/>
     </row>
     <row r="70" spans="7:18">
-      <c r="G70" s="8">
-        <v>43922</v>
-      </c>
-      <c r="H70" s="34" t="s">
-        <v>164</v>
+      <c r="G70" s="9"/>
+      <c r="H70" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>
@@ -11862,13 +11863,13 @@
       <c r="O70" s="34"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="34"/>
-      <c r="R70" s="35"/>
+      <c r="R70" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="71" spans="7:18">
       <c r="G71" s="9"/>
-      <c r="H71" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="H71" s="34"/>
       <c r="I71" s="34"/>
       <c r="J71" s="34"/>
       <c r="K71" s="34"/>
@@ -11881,8 +11882,12 @@
       <c r="R71" s="35"/>
     </row>
     <row r="72" spans="7:18">
-      <c r="G72" s="9"/>
-      <c r="H72" s="34"/>
+      <c r="G72" s="8">
+        <v>43922</v>
+      </c>
+      <c r="H72" s="34" t="s">
+        <v>164</v>
+      </c>
       <c r="I72" s="34"/>
       <c r="J72" s="34"/>
       <c r="K72" s="34"/>
@@ -11892,13 +11897,13 @@
       <c r="O72" s="34"/>
       <c r="P72" s="34"/>
       <c r="Q72" s="34"/>
-      <c r="R72" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R72" s="35"/>
     </row>
     <row r="73" spans="7:18">
       <c r="G73" s="9"/>
-      <c r="H73" s="34"/>
+      <c r="H73" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="I73" s="34"/>
       <c r="J73" s="34"/>
       <c r="K73" s="34"/>
@@ -11911,12 +11916,8 @@
       <c r="R73" s="35"/>
     </row>
     <row r="74" spans="7:18">
-      <c r="G74" s="8">
-        <v>43770</v>
-      </c>
-      <c r="H74" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="G74" s="9"/>
+      <c r="H74" s="34"/>
       <c r="I74" s="34"/>
       <c r="J74" s="34"/>
       <c r="K74" s="34"/>
@@ -11926,13 +11927,13 @@
       <c r="O74" s="34"/>
       <c r="P74" s="34"/>
       <c r="Q74" s="34"/>
-      <c r="R74" s="35"/>
+      <c r="R74" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="75" spans="7:18">
       <c r="G75" s="9"/>
-      <c r="H75" s="47" t="s">
-        <v>168</v>
-      </c>
+      <c r="H75" s="34"/>
       <c r="I75" s="34"/>
       <c r="J75" s="34"/>
       <c r="K75" s="34"/>
@@ -11945,8 +11946,12 @@
       <c r="R75" s="35"/>
     </row>
     <row r="76" spans="7:18">
-      <c r="G76" s="9"/>
-      <c r="H76" s="34"/>
+      <c r="G76" s="8">
+        <v>43770</v>
+      </c>
+      <c r="H76" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="I76" s="34"/>
       <c r="J76" s="34"/>
       <c r="K76" s="34"/>
@@ -11959,11 +11964,9 @@
       <c r="R76" s="35"/>
     </row>
     <row r="77" spans="7:18">
-      <c r="G77" s="8">
-        <v>43739</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>242</v>
+      <c r="G77" s="9"/>
+      <c r="H77" s="47" t="s">
+        <v>168</v>
       </c>
       <c r="I77" s="34"/>
       <c r="J77" s="34"/>
@@ -11973,9 +11976,7 @@
       <c r="N77" s="34"/>
       <c r="O77" s="34"/>
       <c r="P77" s="34"/>
-      <c r="Q77" s="34" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q77" s="34"/>
       <c r="R77" s="35"/>
     </row>
     <row r="78" spans="7:18">
@@ -11993,8 +11994,12 @@
       <c r="R78" s="35"/>
     </row>
     <row r="79" spans="7:18">
-      <c r="G79" s="9"/>
-      <c r="H79" s="34"/>
+      <c r="G79" s="8">
+        <v>43739</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="I79" s="34"/>
       <c r="J79" s="34"/>
       <c r="K79" s="34"/>
@@ -12003,7 +12008,9 @@
       <c r="N79" s="34"/>
       <c r="O79" s="34"/>
       <c r="P79" s="34"/>
-      <c r="Q79" s="34"/>
+      <c r="Q79" s="34" t="s">
+        <v>179</v>
+      </c>
       <c r="R79" s="35"/>
     </row>
     <row r="80" spans="7:18">
@@ -12021,12 +12028,8 @@
       <c r="R80" s="35"/>
     </row>
     <row r="81" spans="7:18">
-      <c r="G81" s="8">
-        <v>43586</v>
-      </c>
-      <c r="H81" s="34" t="s">
-        <v>166</v>
-      </c>
+      <c r="G81" s="9"/>
+      <c r="H81" s="34"/>
       <c r="I81" s="34"/>
       <c r="J81" s="34"/>
       <c r="K81" s="34"/>
@@ -12054,10 +12057,10 @@
     </row>
     <row r="83" spans="7:18">
       <c r="G83" s="8">
-        <v>43282</v>
+        <v>43586</v>
       </c>
       <c r="H83" s="34" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I83" s="34"/>
       <c r="J83" s="34"/>
@@ -12072,9 +12075,7 @@
     </row>
     <row r="84" spans="7:18">
       <c r="G84" s="9"/>
-      <c r="H84" s="7" t="s">
-        <v>163</v>
-      </c>
+      <c r="H84" s="34"/>
       <c r="I84" s="34"/>
       <c r="J84" s="34"/>
       <c r="K84" s="34"/>
@@ -12087,9 +12088,11 @@
       <c r="R84" s="35"/>
     </row>
     <row r="85" spans="7:18">
-      <c r="G85" s="9"/>
-      <c r="H85" s="7" t="s">
-        <v>165</v>
+      <c r="G85" s="8">
+        <v>43282</v>
+      </c>
+      <c r="H85" s="34" t="s">
+        <v>162</v>
       </c>
       <c r="I85" s="34"/>
       <c r="J85" s="34"/>
@@ -12104,7 +12107,9 @@
     </row>
     <row r="86" spans="7:18">
       <c r="G86" s="9"/>
-      <c r="H86" s="34"/>
+      <c r="H86" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="I86" s="34"/>
       <c r="J86" s="34"/>
       <c r="K86" s="34"/>
@@ -12117,38 +12122,77 @@
       <c r="R86" s="35"/>
     </row>
     <row r="87" spans="7:18">
-      <c r="G87" s="85">
+      <c r="G87" s="9"/>
+      <c r="H87" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I87" s="34"/>
+      <c r="J87" s="34"/>
+      <c r="K87" s="34"/>
+      <c r="L87" s="34"/>
+      <c r="M87" s="34"/>
+      <c r="N87" s="34"/>
+      <c r="O87" s="34"/>
+      <c r="P87" s="34"/>
+      <c r="Q87" s="34"/>
+      <c r="R87" s="35"/>
+    </row>
+    <row r="88" spans="7:18">
+      <c r="G88" s="9"/>
+      <c r="H88" s="34"/>
+      <c r="I88" s="34"/>
+      <c r="J88" s="34"/>
+      <c r="K88" s="34"/>
+      <c r="L88" s="34"/>
+      <c r="M88" s="34"/>
+      <c r="N88" s="34"/>
+      <c r="O88" s="34"/>
+      <c r="P88" s="34"/>
+      <c r="Q88" s="34"/>
+      <c r="R88" s="35"/>
+    </row>
+    <row r="89" spans="7:18">
+      <c r="G89" s="85">
         <v>42552</v>
       </c>
-      <c r="H87" s="51" t="s">
+      <c r="H89" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="I87" s="32"/>
-      <c r="J87" s="32"/>
-      <c r="K87" s="32"/>
-      <c r="L87" s="32"/>
-      <c r="M87" s="32"/>
-      <c r="N87" s="32"/>
-      <c r="O87" s="32"/>
-      <c r="P87" s="32"/>
-      <c r="Q87" s="32"/>
-      <c r="R87" s="33"/>
+      <c r="I89" s="32"/>
+      <c r="J89" s="32"/>
+      <c r="K89" s="32"/>
+      <c r="L89" s="32"/>
+      <c r="M89" s="32"/>
+      <c r="N89" s="32"/>
+      <c r="O89" s="32"/>
+      <c r="P89" s="32"/>
+      <c r="Q89" s="32"/>
+      <c r="R89" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Y25:AC25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="AB16:AC16"/>
     <mergeCell ref="AB17:AC17"/>
     <mergeCell ref="AB18:AC18"/>
@@ -12165,28 +12209,19 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C34:D34" r:id="rId1" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
@@ -12196,41 +12231,42 @@
     <hyperlink ref="D45" r:id="rId5" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D44" r:id="rId6" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
     <hyperlink ref="Y25:AC25" r:id="rId7" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
-    <hyperlink ref="H8" r:id="rId8" xr:uid="{645C2C50-2541-448D-9073-14E40D1DE986}"/>
-    <hyperlink ref="H43" r:id="rId9" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H47" r:id="rId10" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
-    <hyperlink ref="R72" r:id="rId11" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H51" r:id="rId12" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H54" r:id="rId13" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R57" r:id="rId14" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H60" r:id="rId15" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
-    <hyperlink ref="H64" r:id="rId16" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H77" r:id="rId17" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
-    <hyperlink ref="R68" r:id="rId18" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H40" r:id="rId19" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
-    <hyperlink ref="H38" r:id="rId20" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
-    <hyperlink ref="H36" r:id="rId21" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
-    <hyperlink ref="H34" r:id="rId22" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
-    <hyperlink ref="H32" r:id="rId23" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
-    <hyperlink ref="H30" r:id="rId24" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
-    <hyperlink ref="H28" r:id="rId25" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
-    <hyperlink ref="H22" r:id="rId26" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
-    <hyperlink ref="H24" r:id="rId27" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
-    <hyperlink ref="H26" r:id="rId28" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
-    <hyperlink ref="H20" r:id="rId29" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
-    <hyperlink ref="H18" r:id="rId30" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
-    <hyperlink ref="H16" r:id="rId31" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
-    <hyperlink ref="H14" r:id="rId32" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
-    <hyperlink ref="H12" r:id="rId33" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
-    <hyperlink ref="H10" r:id="rId34" xr:uid="{DE4DB842-01BE-405E-8254-AC1C82253C72}"/>
-    <hyperlink ref="H6" r:id="rId35" xr:uid="{098F501F-A48C-49AD-B4EE-8F3B4711DA32}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{645C2C50-2541-448D-9073-14E40D1DE986}"/>
+    <hyperlink ref="H45" r:id="rId9" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H49" r:id="rId10" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="R74" r:id="rId11" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H53" r:id="rId12" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H56" r:id="rId13" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R59" r:id="rId14" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H62" r:id="rId15" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="H66" r:id="rId16" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H79" r:id="rId17" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="R70" r:id="rId18" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H42" r:id="rId19" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H40" r:id="rId20" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
+    <hyperlink ref="H38" r:id="rId21" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
+    <hyperlink ref="H36" r:id="rId22" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
+    <hyperlink ref="H34" r:id="rId23" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
+    <hyperlink ref="H32" r:id="rId24" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="H30" r:id="rId25" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
+    <hyperlink ref="H24" r:id="rId26" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
+    <hyperlink ref="H26" r:id="rId27" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
+    <hyperlink ref="H28" r:id="rId28" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
+    <hyperlink ref="H22" r:id="rId29" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
+    <hyperlink ref="H20" r:id="rId30" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
+    <hyperlink ref="H18" r:id="rId31" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
+    <hyperlink ref="H16" r:id="rId32" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
+    <hyperlink ref="H14" r:id="rId33" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
+    <hyperlink ref="H12" r:id="rId34" xr:uid="{DE4DB842-01BE-405E-8254-AC1C82253C72}"/>
+    <hyperlink ref="H8" r:id="rId35" xr:uid="{098F501F-A48C-49AD-B4EE-8F3B4711DA32}"/>
+    <hyperlink ref="H6" r:id="rId36" xr:uid="{EC3AC3B6-D20B-4612-96C2-C088131B252D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId36"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId37"/>
   <ignoredErrors>
     <ignoredError sqref="C39:D40" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId37"/>
+  <drawing r:id="rId38"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
$ERJ Czech Republic C390 order update
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59AD1A3-6672-48EC-88A9-B67B5CF789AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4E1E60-83FE-4D0F-9A7F-21BB1787A674}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="195" yWindow="2010" windowWidth="26610" windowHeight="12885" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="324">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1179,6 +1179,12 @@
   <si>
     <t>Embraer say South Africa have been progressing in talks to acquire C-390 millenium, details sparse but talks progressing</t>
   </si>
+  <si>
+    <t>Czech Republic confirms order for two Embraer C-390 millenium airlifters</t>
+  </si>
+  <si>
+    <t>! Confirmed Oct 24</t>
+  </si>
 </sst>
 </file>
 
@@ -1382,7 +1388,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1434,6 +1440,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1531,7 +1543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1760,6 +1772,27 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1767,51 +1800,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1835,21 +1823,48 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9950,7 +9965,7 @@
   <dimension ref="A2:AC95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9970,47 +9985,51 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="116"/>
-      <c r="G5" s="114" t="s">
+      <c r="C5" s="122"/>
+      <c r="D5" s="123"/>
+      <c r="G5" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115"/>
-      <c r="R5" s="116"/>
-      <c r="T5" s="114" t="s">
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="122"/>
+      <c r="N5" s="122"/>
+      <c r="O5" s="122"/>
+      <c r="P5" s="122"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="123"/>
+      <c r="T5" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="116"/>
-      <c r="Y5" s="114" t="s">
+      <c r="U5" s="122"/>
+      <c r="V5" s="122"/>
+      <c r="W5" s="123"/>
+      <c r="Y5" s="121" t="s">
         <v>313</v>
       </c>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="116"/>
+      <c r="Z5" s="122"/>
+      <c r="AA5" s="123"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>37.24</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="D6" s="17"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="8">
+        <v>45566</v>
+      </c>
+      <c r="H6" s="92" t="s">
+        <v>322</v>
+      </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
@@ -10074,7 +10093,7 @@
       </c>
       <c r="C8" s="11">
         <f>C6*C7</f>
-        <v>6839.1260000000002</v>
+        <v>6189.005000000001</v>
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
@@ -10213,7 +10232,7 @@
       </c>
       <c r="C12" s="12">
         <f>C8-C11</f>
-        <v>8046.8260000000009</v>
+        <v>7396.7050000000017</v>
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
@@ -10236,13 +10255,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="114" t="s">
+      <c r="Y12" s="121" t="s">
         <v>215</v>
       </c>
-      <c r="Z12" s="115"/>
-      <c r="AA12" s="115"/>
-      <c r="AB12" s="115"/>
-      <c r="AC12" s="116"/>
+      <c r="Z12" s="122"/>
+      <c r="AA12" s="122"/>
+      <c r="AB12" s="122"/>
+      <c r="AC12" s="123"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -10264,14 +10283,14 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="86"/>
-      <c r="Z13" s="126" t="s">
+      <c r="Z13" s="131" t="s">
         <v>216</v>
       </c>
-      <c r="AA13" s="126"/>
-      <c r="AB13" s="126" t="s">
+      <c r="AA13" s="131"/>
+      <c r="AB13" s="131" t="s">
         <v>217</v>
       </c>
-      <c r="AC13" s="131"/>
+      <c r="AC13" s="132"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
@@ -10299,21 +10318,21 @@
       <c r="Y14" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="Z14" s="123" t="s">
+      <c r="Z14" s="114" t="s">
         <v>227</v>
       </c>
-      <c r="AA14" s="123"/>
-      <c r="AB14" s="123" t="s">
+      <c r="AA14" s="114"/>
+      <c r="AB14" s="114" t="s">
         <v>228</v>
       </c>
-      <c r="AC14" s="122"/>
+      <c r="AC14" s="115"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="116"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="123"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -10335,14 +10354,14 @@
       <c r="Y15" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="Z15" s="123" t="s">
+      <c r="Z15" s="114" t="s">
         <v>223</v>
       </c>
-      <c r="AA15" s="123"/>
-      <c r="AB15" s="123" t="s">
+      <c r="AA15" s="114"/>
+      <c r="AB15" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="AC15" s="122"/>
+      <c r="AC15" s="115"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -10351,10 +10370,10 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="122"/>
+      <c r="D16" s="115"/>
       <c r="E16" s="3" t="s">
         <v>301</v>
       </c>
@@ -10383,23 +10402,23 @@
       <c r="Y16" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z16" s="123" t="s">
+      <c r="Z16" s="114" t="s">
         <v>224</v>
       </c>
-      <c r="AA16" s="123"/>
-      <c r="AB16" s="123" t="s">
+      <c r="AA16" s="114"/>
+      <c r="AB16" s="114" t="s">
         <v>230</v>
       </c>
-      <c r="AC16" s="122"/>
+      <c r="AC16" s="115"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="123" t="s">
+      <c r="C17" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="122"/>
+      <c r="D17" s="115"/>
       <c r="E17" s="3" t="s">
         <v>301</v>
       </c>
@@ -10422,19 +10441,19 @@
       <c r="Y17" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z17" s="123" t="s">
+      <c r="Z17" s="114" t="s">
         <v>225</v>
       </c>
-      <c r="AA17" s="123"/>
-      <c r="AB17" s="123" t="s">
+      <c r="AA17" s="114"/>
+      <c r="AB17" s="114" t="s">
         <v>231</v>
       </c>
-      <c r="AC17" s="122"/>
+      <c r="AC17" s="115"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="122"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="115"/>
       <c r="G18" s="8">
         <v>45474</v>
       </c>
@@ -10460,19 +10479,19 @@
       <c r="Y18" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z18" s="123" t="s">
+      <c r="Z18" s="114" t="s">
         <v>226</v>
       </c>
-      <c r="AA18" s="123"/>
-      <c r="AB18" s="123" t="s">
+      <c r="AA18" s="114"/>
+      <c r="AB18" s="114" t="s">
         <v>232</v>
       </c>
-      <c r="AC18" s="122"/>
+      <c r="AC18" s="115"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="142"/>
-      <c r="D19" s="143"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="120"/>
       <c r="G19" s="9"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -10494,14 +10513,14 @@
       <c r="Y19" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="Z19" s="123" t="s">
+      <c r="Z19" s="114" t="s">
         <v>234</v>
       </c>
-      <c r="AA19" s="123"/>
-      <c r="AB19" s="123" t="s">
+      <c r="AA19" s="114"/>
+      <c r="AB19" s="114" t="s">
         <v>235</v>
       </c>
-      <c r="AC19" s="122"/>
+      <c r="AC19" s="115"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="8">
@@ -10529,14 +10548,14 @@
       <c r="Y20" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="Z20" s="123" t="s">
+      <c r="Z20" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="AA20" s="123"/>
-      <c r="AB20" s="123" t="s">
+      <c r="AA20" s="114"/>
+      <c r="AB20" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="AC20" s="122"/>
+      <c r="AC20" s="115"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -10564,11 +10583,11 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="114" t="s">
+      <c r="B22" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="115"/>
-      <c r="D22" s="116"/>
+      <c r="C22" s="122"/>
+      <c r="D22" s="123"/>
       <c r="G22" s="8">
         <v>45413</v>
       </c>
@@ -10601,10 +10620,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="114" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="122"/>
+      <c r="D23" s="115"/>
       <c r="G23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -10626,10 +10645,10 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="123">
+      <c r="C24" s="114">
         <v>1969</v>
       </c>
-      <c r="D24" s="122"/>
+      <c r="D24" s="115"/>
       <c r="G24" s="8">
         <v>44986</v>
       </c>
@@ -10655,8 +10674,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="122"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="115"/>
       <c r="G25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -10675,23 +10694,23 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="139" t="s">
+      <c r="Y25" s="116" t="s">
         <v>286</v>
       </c>
-      <c r="Z25" s="140"/>
-      <c r="AA25" s="140"/>
-      <c r="AB25" s="140"/>
-      <c r="AC25" s="141"/>
+      <c r="Z25" s="117"/>
+      <c r="AA25" s="117"/>
+      <c r="AB25" s="117"/>
+      <c r="AC25" s="118"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="129">
+      <c r="C26" s="142">
         <f>'Financial Model'!Z70</f>
         <v>2636</v>
       </c>
-      <c r="D26" s="130"/>
+      <c r="D26" s="143"/>
       <c r="G26" s="8">
         <v>44986</v>
       </c>
@@ -10724,8 +10743,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="122"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="115"/>
       <c r="G27" s="9"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -10756,11 +10775,11 @@
       <c r="B28" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="C28" s="121">
+      <c r="C28" s="137">
         <f>+'Order &amp; Backlog'!$AA$3</f>
         <v>2200</v>
       </c>
-      <c r="D28" s="122"/>
+      <c r="D28" s="115"/>
       <c r="G28" s="8">
         <v>44986</v>
       </c>
@@ -10795,11 +10814,11 @@
       <c r="B29" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="121">
+      <c r="C29" s="137">
         <f>'Order &amp; Backlog'!AA21</f>
         <v>382</v>
       </c>
-      <c r="D29" s="122"/>
+      <c r="D29" s="115"/>
       <c r="G29" s="9"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
@@ -10828,11 +10847,11 @@
       <c r="B30" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="123">
+      <c r="C30" s="114">
         <f>'Financial Model'!AB43</f>
         <v>47</v>
       </c>
-      <c r="D30" s="122"/>
+      <c r="D30" s="115"/>
       <c r="G30" s="8">
         <v>45261</v>
       </c>
@@ -10865,10 +10884,10 @@
       <c r="B31" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C31" s="124">
+      <c r="C31" s="138">
         <v>36708</v>
       </c>
-      <c r="D31" s="125"/>
+      <c r="D31" s="139"/>
       <c r="G31" s="9"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -10897,8 +10916,8 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="122"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="115"/>
       <c r="G32" s="8">
         <v>45231</v>
       </c>
@@ -10965,10 +10984,10 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="137" t="s">
+      <c r="C34" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="138"/>
+      <c r="D34" s="130"/>
       <c r="G34" s="8">
         <v>45200</v>
       </c>
@@ -11042,11 +11061,11 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="114" t="s">
+      <c r="B37" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="115"/>
-      <c r="D37" s="116"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="123"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -11059,12 +11078,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="114" t="s">
+      <c r="T37" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="115"/>
-      <c r="V37" s="115"/>
-      <c r="W37" s="116"/>
+      <c r="U37" s="122"/>
+      <c r="V37" s="122"/>
+      <c r="W37" s="123"/>
       <c r="Y37" s="39" t="s">
         <v>278</v>
       </c>
@@ -11077,11 +11096,11 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="127">
+      <c r="C38" s="140">
         <f>C6/'Financial Model'!AB125</f>
-        <v>8.7855687584302231</v>
-      </c>
-      <c r="D38" s="128"/>
+        <v>7.9504207078168241</v>
+      </c>
+      <c r="D38" s="141"/>
       <c r="G38" s="8">
         <v>45017</v>
       </c>
@@ -11116,11 +11135,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="127">
+      <c r="C39" s="140">
         <f>+C8/SUM('Financial Model'!Y4:AB4)</f>
-        <v>3.5430378697611773</v>
-      </c>
-      <c r="D39" s="128"/>
+        <v>3.2062399627000993</v>
+      </c>
+      <c r="D39" s="141"/>
       <c r="G39" s="9"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -11149,11 +11168,11 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="135">
+      <c r="C40" s="127">
         <f>C6/SUM('Financial Model'!Y26:AB26)</f>
-        <v>71.670170290804307</v>
-      </c>
-      <c r="D40" s="136"/>
+        <v>64.857270107414209</v>
+      </c>
+      <c r="D40" s="128"/>
       <c r="G40" s="8">
         <v>45017</v>
       </c>
@@ -11235,11 +11254,11 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="114" t="s">
+      <c r="B43" s="121" t="s">
         <v>243</v>
       </c>
-      <c r="C43" s="115"/>
-      <c r="D43" s="116"/>
+      <c r="C43" s="122"/>
+      <c r="D43" s="123"/>
       <c r="G43" s="9"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -11267,10 +11286,10 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="117" t="s">
+      <c r="B44" s="133" t="s">
         <v>244</v>
       </c>
-      <c r="C44" s="118"/>
+      <c r="C44" s="134"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
@@ -11305,10 +11324,10 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="117" t="s">
+      <c r="B45" s="133" t="s">
         <v>245</v>
       </c>
-      <c r="C45" s="118"/>
+      <c r="C45" s="134"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
@@ -11339,8 +11358,8 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="117"/>
-      <c r="C46" s="118"/>
+      <c r="B46" s="133"/>
+      <c r="C46" s="134"/>
       <c r="D46" s="83" t="s">
         <v>31</v>
       </c>
@@ -11371,8 +11390,8 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="117"/>
-      <c r="C47" s="118"/>
+      <c r="B47" s="133"/>
+      <c r="C47" s="134"/>
       <c r="D47" s="83" t="s">
         <v>31</v>
       </c>
@@ -11394,17 +11413,19 @@
       <c r="U47" s="34"/>
       <c r="V47" s="34"/>
       <c r="W47" s="35"/>
-      <c r="Y47" s="39" t="s">
+      <c r="Y47" s="144" t="s">
         <v>285</v>
       </c>
-      <c r="Z47" s="34"/>
-      <c r="AA47" s="34"/>
-      <c r="AB47" s="34"/>
-      <c r="AC47" s="35"/>
+      <c r="Z47" s="145"/>
+      <c r="AA47" s="145"/>
+      <c r="AB47" s="145" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC47" s="146"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="119"/>
-      <c r="C48" s="120"/>
+      <c r="B48" s="135"/>
+      <c r="C48" s="136"/>
       <c r="D48" s="84" t="s">
         <v>31</v>
       </c>
@@ -11654,13 +11675,13 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
-      <c r="Y58" s="132" t="s">
+      <c r="Y58" s="124" t="s">
         <v>293</v>
       </c>
-      <c r="Z58" s="133"/>
-      <c r="AA58" s="133"/>
-      <c r="AB58" s="133"/>
-      <c r="AC58" s="134"/>
+      <c r="Z58" s="125"/>
+      <c r="AA58" s="125"/>
+      <c r="AB58" s="125"/>
+      <c r="AC58" s="126"/>
     </row>
     <row r="59" spans="7:29">
       <c r="G59" s="8">
@@ -12256,19 +12277,28 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Y25:AC25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="AB16:AC16"/>
     <mergeCell ref="AB17:AC17"/>
     <mergeCell ref="AB18:AC18"/>
@@ -12285,28 +12315,19 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C34:D34" r:id="rId1" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
@@ -12347,13 +12368,14 @@
     <hyperlink ref="H12" r:id="rId36" xr:uid="{EC3AC3B6-D20B-4612-96C2-C088131B252D}"/>
     <hyperlink ref="H10" r:id="rId37" xr:uid="{327A318F-D59B-4B08-A396-86E7866F07CE}"/>
     <hyperlink ref="H8" r:id="rId38" xr:uid="{F0AB9CE8-A127-4A54-A49C-B0BFF1ECBCFB}"/>
+    <hyperlink ref="H6" r:id="rId39" xr:uid="{2BC9EAF5-1571-44CC-AC7B-DE21B8FC3951}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId39"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId40"/>
   <ignoredErrors>
     <ignoredError sqref="C39:D40" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId40"/>
+  <drawing r:id="rId41"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
$ERJ C-390 Morocco news
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4E1E60-83FE-4D0F-9A7F-21BB1787A674}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ABCD1C-1986-490D-9006-E6C5F5F9A3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="2010" windowWidth="26610" windowHeight="12885" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -170,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="326">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1185,6 +1194,12 @@
   <si>
     <t>! Confirmed Oct 24</t>
   </si>
+  <si>
+    <t>Morocco - Unknown Qty</t>
+  </si>
+  <si>
+    <t>Morocco believed to bew new customer of C-390 Millenium of unknown quantity</t>
+  </si>
 </sst>
 </file>
 
@@ -1543,7 +1558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1768,31 +1783,12 @@
     <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1800,6 +1796,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1823,48 +1864,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9962,10 +9976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F324B-1DEB-44A7-A7E2-319E26170844}">
-  <dimension ref="A2:AC95"/>
+  <dimension ref="A2:AC97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9985,36 +9999,36 @@
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="122"/>
-      <c r="D5" s="123"/>
-      <c r="G5" s="121" t="s">
+      <c r="C5" s="117"/>
+      <c r="D5" s="118"/>
+      <c r="G5" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="122"/>
-      <c r="I5" s="122"/>
-      <c r="J5" s="122"/>
-      <c r="K5" s="122"/>
-      <c r="L5" s="122"/>
-      <c r="M5" s="122"/>
-      <c r="N5" s="122"/>
-      <c r="O5" s="122"/>
-      <c r="P5" s="122"/>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="123"/>
-      <c r="T5" s="121" t="s">
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="118"/>
+      <c r="T5" s="116" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="122"/>
-      <c r="V5" s="122"/>
-      <c r="W5" s="123"/>
-      <c r="Y5" s="121" t="s">
+      <c r="U5" s="117"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="118"/>
+      <c r="Y5" s="116" t="s">
         <v>313</v>
       </c>
-      <c r="Z5" s="122"/>
-      <c r="AA5" s="123"/>
+      <c r="Z5" s="117"/>
+      <c r="AA5" s="118"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" s="4" t="s">
@@ -10028,7 +10042,7 @@
         <v>45566</v>
       </c>
       <c r="H6" s="92" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
@@ -10049,7 +10063,7 @@
       <c r="Y6" s="39" t="s">
         <v>314</v>
       </c>
-      <c r="Z6" s="112"/>
+      <c r="Z6" s="34"/>
       <c r="AA6" s="35"/>
     </row>
     <row r="7" spans="1:29">
@@ -10084,7 +10098,7 @@
       <c r="Y7" s="41" t="s">
         <v>315</v>
       </c>
-      <c r="Z7" s="112"/>
+      <c r="Z7" s="34"/>
       <c r="AA7" s="35"/>
     </row>
     <row r="8" spans="1:29">
@@ -10097,10 +10111,10 @@
       </c>
       <c r="D8" s="17"/>
       <c r="G8" s="8">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="H8" s="92" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
@@ -10119,7 +10133,7 @@
       <c r="V8" s="34"/>
       <c r="W8" s="35"/>
       <c r="Y8" s="39"/>
-      <c r="Z8" s="112"/>
+      <c r="Z8" s="34"/>
       <c r="AA8" s="35"/>
     </row>
     <row r="9" spans="1:29">
@@ -10154,7 +10168,7 @@
       <c r="Y9" s="39" t="s">
         <v>316</v>
       </c>
-      <c r="Z9" s="112"/>
+      <c r="Z9" s="34"/>
       <c r="AA9" s="35"/>
     </row>
     <row r="10" spans="1:29">
@@ -10172,7 +10186,7 @@
         <v>45536</v>
       </c>
       <c r="H10" s="92" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -10190,7 +10204,7 @@
       <c r="U10" s="34"/>
       <c r="V10" s="34"/>
       <c r="W10" s="35"/>
-      <c r="Y10" s="113" t="s">
+      <c r="Y10" s="112" t="s">
         <v>317</v>
       </c>
       <c r="Z10" s="32"/>
@@ -10236,10 +10250,10 @@
       </c>
       <c r="D12" s="18"/>
       <c r="G12" s="8">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="H12" s="92" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -10255,13 +10269,13 @@
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
       <c r="W12" s="35"/>
-      <c r="Y12" s="121" t="s">
+      <c r="Y12" s="116" t="s">
         <v>215</v>
       </c>
-      <c r="Z12" s="122"/>
-      <c r="AA12" s="122"/>
-      <c r="AB12" s="122"/>
-      <c r="AC12" s="123"/>
+      <c r="Z12" s="117"/>
+      <c r="AA12" s="117"/>
+      <c r="AB12" s="117"/>
+      <c r="AC12" s="118"/>
     </row>
     <row r="13" spans="1:29">
       <c r="G13" s="9"/>
@@ -10283,21 +10297,21 @@
       <c r="V13" s="34"/>
       <c r="W13" s="35"/>
       <c r="Y13" s="86"/>
-      <c r="Z13" s="131" t="s">
+      <c r="Z13" s="128" t="s">
         <v>216</v>
       </c>
-      <c r="AA13" s="131"/>
-      <c r="AB13" s="131" t="s">
+      <c r="AA13" s="128"/>
+      <c r="AB13" s="128" t="s">
         <v>217</v>
       </c>
-      <c r="AC13" s="132"/>
+      <c r="AC13" s="133"/>
     </row>
     <row r="14" spans="1:29">
       <c r="G14" s="8">
         <v>45505</v>
       </c>
       <c r="H14" s="92" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
@@ -10318,21 +10332,21 @@
       <c r="Y14" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="Z14" s="114" t="s">
+      <c r="Z14" s="125" t="s">
         <v>227</v>
       </c>
-      <c r="AA14" s="114"/>
-      <c r="AB14" s="114" t="s">
+      <c r="AA14" s="125"/>
+      <c r="AB14" s="125" t="s">
         <v>228</v>
       </c>
-      <c r="AC14" s="115"/>
+      <c r="AC14" s="124"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="121" t="s">
+      <c r="B15" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="122"/>
-      <c r="D15" s="123"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="118"/>
       <c r="G15" s="9"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -10354,14 +10368,14 @@
       <c r="Y15" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="Z15" s="114" t="s">
+      <c r="Z15" s="125" t="s">
         <v>223</v>
       </c>
-      <c r="AA15" s="114"/>
-      <c r="AB15" s="114" t="s">
+      <c r="AA15" s="125"/>
+      <c r="AB15" s="125" t="s">
         <v>229</v>
       </c>
-      <c r="AC15" s="115"/>
+      <c r="AC15" s="124"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="13" t="s">
@@ -10370,18 +10384,18 @@
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="115"/>
+      <c r="D16" s="124"/>
       <c r="E16" s="3" t="s">
         <v>301</v>
       </c>
       <c r="G16" s="8">
-        <v>45474</v>
+        <v>45505</v>
       </c>
       <c r="H16" s="92" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
@@ -10402,23 +10416,23 @@
       <c r="Y16" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Z16" s="114" t="s">
+      <c r="Z16" s="125" t="s">
         <v>224</v>
       </c>
-      <c r="AA16" s="114"/>
-      <c r="AB16" s="114" t="s">
+      <c r="AA16" s="125"/>
+      <c r="AB16" s="125" t="s">
         <v>230</v>
       </c>
-      <c r="AC16" s="115"/>
+      <c r="AC16" s="124"/>
     </row>
     <row r="17" spans="2:29">
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="114" t="s">
+      <c r="C17" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="115"/>
+      <c r="D17" s="124"/>
       <c r="E17" s="3" t="s">
         <v>301</v>
       </c>
@@ -10441,24 +10455,24 @@
       <c r="Y17" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="Z17" s="114" t="s">
+      <c r="Z17" s="125" t="s">
         <v>225</v>
       </c>
-      <c r="AA17" s="114"/>
-      <c r="AB17" s="114" t="s">
+      <c r="AA17" s="125"/>
+      <c r="AB17" s="125" t="s">
         <v>231</v>
       </c>
-      <c r="AC17" s="115"/>
+      <c r="AC17" s="124"/>
     </row>
     <row r="18" spans="2:29">
       <c r="B18" s="15"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="115"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="124"/>
       <c r="G18" s="8">
         <v>45474</v>
       </c>
       <c r="H18" s="92" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
@@ -10479,19 +10493,19 @@
       <c r="Y18" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="Z18" s="114" t="s">
+      <c r="Z18" s="125" t="s">
         <v>226</v>
       </c>
-      <c r="AA18" s="114"/>
-      <c r="AB18" s="114" t="s">
+      <c r="AA18" s="125"/>
+      <c r="AB18" s="125" t="s">
         <v>232</v>
       </c>
-      <c r="AC18" s="115"/>
+      <c r="AC18" s="124"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="16"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="120"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="145"/>
       <c r="G19" s="9"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -10513,21 +10527,21 @@
       <c r="Y19" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="Z19" s="114" t="s">
+      <c r="Z19" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="AA19" s="114"/>
-      <c r="AB19" s="114" t="s">
+      <c r="AA19" s="125"/>
+      <c r="AB19" s="125" t="s">
         <v>235</v>
       </c>
-      <c r="AC19" s="115"/>
+      <c r="AC19" s="124"/>
     </row>
     <row r="20" spans="2:29">
       <c r="G20" s="8">
-        <v>45413</v>
+        <v>45474</v>
       </c>
       <c r="H20" s="92" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
@@ -10548,14 +10562,14 @@
       <c r="Y20" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="Z20" s="114" t="s">
+      <c r="Z20" s="125" t="s">
         <v>240</v>
       </c>
-      <c r="AA20" s="114"/>
-      <c r="AB20" s="114" t="s">
+      <c r="AA20" s="125"/>
+      <c r="AB20" s="125" t="s">
         <v>241</v>
       </c>
-      <c r="AC20" s="115"/>
+      <c r="AC20" s="124"/>
     </row>
     <row r="21" spans="2:29">
       <c r="G21" s="9"/>
@@ -10583,16 +10597,16 @@
       <c r="AC21" s="35"/>
     </row>
     <row r="22" spans="2:29">
-      <c r="B22" s="121" t="s">
+      <c r="B22" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="122"/>
-      <c r="D22" s="123"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
       <c r="G22" s="8">
         <v>45413</v>
       </c>
       <c r="H22" s="92" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
@@ -10620,10 +10634,10 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="114" t="s">
+      <c r="C23" s="125" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="115"/>
+      <c r="D23" s="124"/>
       <c r="G23" s="9"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
@@ -10645,15 +10659,15 @@
       <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="114">
+      <c r="C24" s="125">
         <v>1969</v>
       </c>
-      <c r="D24" s="115"/>
+      <c r="D24" s="124"/>
       <c r="G24" s="8">
-        <v>44986</v>
+        <v>45413</v>
       </c>
       <c r="H24" s="92" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="34"/>
@@ -10674,8 +10688,8 @@
     </row>
     <row r="25" spans="2:29">
       <c r="B25" s="9"/>
-      <c r="C25" s="114"/>
-      <c r="D25" s="115"/>
+      <c r="C25" s="125"/>
+      <c r="D25" s="124"/>
       <c r="G25" s="9"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -10694,28 +10708,28 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="35"/>
-      <c r="Y25" s="116" t="s">
+      <c r="Y25" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="Z25" s="117"/>
-      <c r="AA25" s="117"/>
-      <c r="AB25" s="117"/>
-      <c r="AC25" s="118"/>
+      <c r="Z25" s="142"/>
+      <c r="AA25" s="142"/>
+      <c r="AB25" s="142"/>
+      <c r="AC25" s="143"/>
     </row>
     <row r="26" spans="2:29">
       <c r="B26" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="142">
+      <c r="C26" s="131">
         <f>'Financial Model'!Z70</f>
         <v>2636</v>
       </c>
-      <c r="D26" s="143"/>
+      <c r="D26" s="132"/>
       <c r="G26" s="8">
         <v>44986</v>
       </c>
       <c r="H26" s="92" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
@@ -10743,8 +10757,8 @@
     </row>
     <row r="27" spans="2:29">
       <c r="B27" s="9"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="115"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="124"/>
       <c r="G27" s="9"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
@@ -10775,16 +10789,16 @@
       <c r="B28" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="C28" s="137">
+      <c r="C28" s="123">
         <f>+'Order &amp; Backlog'!$AA$3</f>
         <v>2200</v>
       </c>
-      <c r="D28" s="115"/>
+      <c r="D28" s="124"/>
       <c r="G28" s="8">
         <v>44986</v>
       </c>
       <c r="H28" s="92" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I28" s="34"/>
       <c r="J28" s="34"/>
@@ -10814,11 +10828,11 @@
       <c r="B29" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="137">
+      <c r="C29" s="123">
         <f>'Order &amp; Backlog'!AA21</f>
         <v>382</v>
       </c>
-      <c r="D29" s="115"/>
+      <c r="D29" s="124"/>
       <c r="G29" s="9"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
@@ -10847,16 +10861,16 @@
       <c r="B30" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="114">
+      <c r="C30" s="125">
         <f>'Financial Model'!AB43</f>
         <v>47</v>
       </c>
-      <c r="D30" s="115"/>
+      <c r="D30" s="124"/>
       <c r="G30" s="8">
-        <v>45261</v>
+        <v>44986</v>
       </c>
       <c r="H30" s="92" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
@@ -10884,10 +10898,10 @@
       <c r="B31" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C31" s="138">
+      <c r="C31" s="126">
         <v>36708</v>
       </c>
-      <c r="D31" s="139"/>
+      <c r="D31" s="127"/>
       <c r="G31" s="9"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -10916,13 +10930,13 @@
     </row>
     <row r="32" spans="2:29">
       <c r="B32" s="9"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="115"/>
+      <c r="C32" s="125"/>
+      <c r="D32" s="124"/>
       <c r="G32" s="8">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="H32" s="92" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
@@ -10984,15 +10998,15 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="129" t="s">
+      <c r="C34" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="130"/>
+      <c r="D34" s="140"/>
       <c r="G34" s="8">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="H34" s="92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I34" s="34"/>
       <c r="J34" s="34"/>
@@ -11039,10 +11053,10 @@
     </row>
     <row r="36" spans="2:29">
       <c r="G36" s="8">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="H36" s="92" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
@@ -11061,11 +11075,11 @@
       <c r="AC36" s="35"/>
     </row>
     <row r="37" spans="2:29">
-      <c r="B37" s="121" t="s">
+      <c r="B37" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="122"/>
-      <c r="D37" s="123"/>
+      <c r="C37" s="117"/>
+      <c r="D37" s="118"/>
       <c r="G37" s="9"/>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -11078,12 +11092,12 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
-      <c r="T37" s="121" t="s">
+      <c r="T37" s="116" t="s">
         <v>158</v>
       </c>
-      <c r="U37" s="122"/>
-      <c r="V37" s="122"/>
-      <c r="W37" s="123"/>
+      <c r="U37" s="117"/>
+      <c r="V37" s="117"/>
+      <c r="W37" s="118"/>
       <c r="Y37" s="39" t="s">
         <v>278</v>
       </c>
@@ -11096,16 +11110,16 @@
       <c r="B38" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="140">
+      <c r="C38" s="129">
         <f>C6/'Financial Model'!AB125</f>
         <v>7.9504207078168241</v>
       </c>
-      <c r="D38" s="141"/>
+      <c r="D38" s="130"/>
       <c r="G38" s="8">
-        <v>45017</v>
+        <v>45170</v>
       </c>
       <c r="H38" s="92" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -11135,11 +11149,11 @@
       <c r="B39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="140">
+      <c r="C39" s="129">
         <f>+C8/SUM('Financial Model'!Y4:AB4)</f>
         <v>3.2062399627000993</v>
       </c>
-      <c r="D39" s="141"/>
+      <c r="D39" s="130"/>
       <c r="G39" s="9"/>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
@@ -11168,16 +11182,16 @@
       <c r="B40" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="127">
+      <c r="C40" s="137">
         <f>C6/SUM('Financial Model'!Y26:AB26)</f>
         <v>64.857270107414209</v>
       </c>
-      <c r="D40" s="128"/>
+      <c r="D40" s="138"/>
       <c r="G40" s="8">
         <v>45017</v>
       </c>
-      <c r="H40" s="98" t="s">
-        <v>266</v>
+      <c r="H40" s="92" t="s">
+        <v>269</v>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
@@ -11228,10 +11242,10 @@
     </row>
     <row r="42" spans="2:29">
       <c r="G42" s="8">
-        <v>44927</v>
-      </c>
-      <c r="H42" s="94" t="s">
-        <v>263</v>
+        <v>45017</v>
+      </c>
+      <c r="H42" s="98" t="s">
+        <v>266</v>
       </c>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
@@ -11254,11 +11268,11 @@
       <c r="AC42" s="35"/>
     </row>
     <row r="43" spans="2:29">
-      <c r="B43" s="121" t="s">
+      <c r="B43" s="116" t="s">
         <v>243</v>
       </c>
-      <c r="C43" s="122"/>
-      <c r="D43" s="123"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="118"/>
       <c r="G43" s="9"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -11286,18 +11300,18 @@
       <c r="AC43" s="35"/>
     </row>
     <row r="44" spans="2:29">
-      <c r="B44" s="133" t="s">
+      <c r="B44" s="119" t="s">
         <v>244</v>
       </c>
-      <c r="C44" s="134"/>
+      <c r="C44" s="120"/>
       <c r="D44" s="48" t="s">
         <v>31</v>
       </c>
       <c r="G44" s="8">
-        <v>44896</v>
-      </c>
-      <c r="H44" s="92" t="s">
-        <v>261</v>
+        <v>44927</v>
+      </c>
+      <c r="H44" s="94" t="s">
+        <v>263</v>
       </c>
       <c r="I44" s="34"/>
       <c r="J44" s="34"/>
@@ -11324,10 +11338,10 @@
       <c r="AC44" s="35"/>
     </row>
     <row r="45" spans="2:29">
-      <c r="B45" s="133" t="s">
+      <c r="B45" s="119" t="s">
         <v>245</v>
       </c>
-      <c r="C45" s="134"/>
+      <c r="C45" s="120"/>
       <c r="D45" s="48" t="s">
         <v>31</v>
       </c>
@@ -11358,16 +11372,16 @@
       <c r="AC45" s="35"/>
     </row>
     <row r="46" spans="2:29">
-      <c r="B46" s="133"/>
-      <c r="C46" s="134"/>
+      <c r="B46" s="119"/>
+      <c r="C46" s="120"/>
       <c r="D46" s="83" t="s">
         <v>31</v>
       </c>
       <c r="G46" s="8">
-        <v>44866</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>259</v>
+        <v>44896</v>
+      </c>
+      <c r="H46" s="92" t="s">
+        <v>261</v>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="34"/>
@@ -11390,8 +11404,8 @@
       <c r="AC46" s="35"/>
     </row>
     <row r="47" spans="2:29">
-      <c r="B47" s="133"/>
-      <c r="C47" s="134"/>
+      <c r="B47" s="119"/>
+      <c r="C47" s="120"/>
       <c r="D47" s="83" t="s">
         <v>31</v>
       </c>
@@ -11413,27 +11427,27 @@
       <c r="U47" s="34"/>
       <c r="V47" s="34"/>
       <c r="W47" s="35"/>
-      <c r="Y47" s="144" t="s">
+      <c r="Y47" s="113" t="s">
         <v>285</v>
       </c>
-      <c r="Z47" s="145"/>
-      <c r="AA47" s="145"/>
-      <c r="AB47" s="145" t="s">
+      <c r="Z47" s="114"/>
+      <c r="AA47" s="114"/>
+      <c r="AB47" s="114" t="s">
         <v>323</v>
       </c>
-      <c r="AC47" s="146"/>
+      <c r="AC47" s="115"/>
     </row>
     <row r="48" spans="2:29">
-      <c r="B48" s="135"/>
-      <c r="C48" s="136"/>
+      <c r="B48" s="121"/>
+      <c r="C48" s="122"/>
       <c r="D48" s="84" t="s">
         <v>31</v>
       </c>
       <c r="G48" s="8">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="I48" s="34"/>
       <c r="J48" s="34"/>
@@ -11487,8 +11501,12 @@
       <c r="AC49" s="35"/>
     </row>
     <row r="50" spans="7:29">
-      <c r="G50" s="9"/>
-      <c r="H50" s="34"/>
+      <c r="G50" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="I50" s="34"/>
       <c r="J50" s="34"/>
       <c r="K50" s="34"/>
@@ -11508,12 +11526,8 @@
       <c r="AC50" s="35"/>
     </row>
     <row r="51" spans="7:29">
-      <c r="G51" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="G51" s="9"/>
+      <c r="H51" s="34"/>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
@@ -11534,9 +11548,7 @@
     </row>
     <row r="52" spans="7:29">
       <c r="G52" s="9"/>
-      <c r="H52" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="H52" s="34"/>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
       <c r="K52" s="34"/>
@@ -11554,9 +11566,11 @@
       <c r="AC52" s="35"/>
     </row>
     <row r="53" spans="7:29">
-      <c r="G53" s="9"/>
-      <c r="H53" s="7" t="s">
-        <v>13</v>
+      <c r="G53" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="I53" s="34"/>
       <c r="J53" s="34"/>
@@ -11578,7 +11592,9 @@
     </row>
     <row r="54" spans="7:29">
       <c r="G54" s="9"/>
-      <c r="H54" s="34"/>
+      <c r="H54" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
       <c r="K54" s="34"/>
@@ -11598,11 +11614,9 @@
       <c r="AC54" s="35"/>
     </row>
     <row r="55" spans="7:29">
-      <c r="G55" s="8">
-        <v>44835</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>29</v>
+      <c r="G55" s="9"/>
+      <c r="H55" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I55" s="34"/>
       <c r="J55" s="34"/>
@@ -11624,9 +11638,7 @@
     </row>
     <row r="56" spans="7:29">
       <c r="G56" s="9"/>
-      <c r="H56" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="H56" s="34"/>
       <c r="I56" s="34"/>
       <c r="J56" s="34"/>
       <c r="K56" s="34"/>
@@ -11644,8 +11656,12 @@
       <c r="AC56" s="35"/>
     </row>
     <row r="57" spans="7:29">
-      <c r="G57" s="9"/>
-      <c r="H57" s="34"/>
+      <c r="G57" s="8">
+        <v>44835</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="I57" s="34"/>
       <c r="J57" s="34"/>
       <c r="K57" s="34"/>
@@ -11656,15 +11672,19 @@
       <c r="P57" s="34"/>
       <c r="Q57" s="34"/>
       <c r="R57" s="35"/>
-      <c r="Y57" s="101"/>
-      <c r="Z57" s="102"/>
-      <c r="AA57" s="102"/>
-      <c r="AB57" s="102"/>
-      <c r="AC57" s="103"/>
+      <c r="Y57" s="39" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z57" s="34"/>
+      <c r="AA57" s="34"/>
+      <c r="AB57" s="34"/>
+      <c r="AC57" s="35"/>
     </row>
     <row r="58" spans="7:29">
       <c r="G58" s="9"/>
-      <c r="H58" s="34"/>
+      <c r="H58" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
@@ -11675,21 +11695,15 @@
       <c r="P58" s="34"/>
       <c r="Q58" s="34"/>
       <c r="R58" s="35"/>
-      <c r="Y58" s="124" t="s">
-        <v>293</v>
-      </c>
-      <c r="Z58" s="125"/>
-      <c r="AA58" s="125"/>
-      <c r="AB58" s="125"/>
-      <c r="AC58" s="126"/>
+      <c r="Y58" s="39"/>
+      <c r="Z58" s="34"/>
+      <c r="AA58" s="34"/>
+      <c r="AB58" s="34"/>
+      <c r="AC58" s="35"/>
     </row>
     <row r="59" spans="7:29">
-      <c r="G59" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>187</v>
-      </c>
+      <c r="G59" s="9"/>
+      <c r="H59" s="34"/>
       <c r="I59" s="34"/>
       <c r="J59" s="34"/>
       <c r="K59" s="34"/>
@@ -11700,6 +11714,11 @@
       <c r="P59" s="34"/>
       <c r="Q59" s="34"/>
       <c r="R59" s="35"/>
+      <c r="Y59" s="39"/>
+      <c r="Z59" s="34"/>
+      <c r="AA59" s="34"/>
+      <c r="AB59" s="34"/>
+      <c r="AC59" s="35"/>
     </row>
     <row r="60" spans="7:29">
       <c r="G60" s="9"/>
@@ -11714,10 +11733,19 @@
       <c r="P60" s="34"/>
       <c r="Q60" s="34"/>
       <c r="R60" s="35"/>
+      <c r="Y60" s="101"/>
+      <c r="Z60" s="102"/>
+      <c r="AA60" s="102"/>
+      <c r="AB60" s="102"/>
+      <c r="AC60" s="103"/>
     </row>
     <row r="61" spans="7:29">
-      <c r="G61" s="9"/>
-      <c r="H61" s="34"/>
+      <c r="G61" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="I61" s="34"/>
       <c r="J61" s="34"/>
       <c r="K61" s="34"/>
@@ -11728,14 +11756,17 @@
       <c r="P61" s="34"/>
       <c r="Q61" s="34"/>
       <c r="R61" s="35"/>
+      <c r="Y61" s="134" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z61" s="135"/>
+      <c r="AA61" s="135"/>
+      <c r="AB61" s="135"/>
+      <c r="AC61" s="136"/>
     </row>
     <row r="62" spans="7:29">
-      <c r="G62" s="8">
-        <v>44805</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>195</v>
-      </c>
+      <c r="G62" s="9"/>
+      <c r="H62" s="34"/>
       <c r="I62" s="34"/>
       <c r="J62" s="34"/>
       <c r="K62" s="34"/>
@@ -11749,9 +11780,7 @@
     </row>
     <row r="63" spans="7:29">
       <c r="G63" s="9"/>
-      <c r="H63" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="H63" s="34"/>
       <c r="I63" s="34"/>
       <c r="J63" s="34"/>
       <c r="K63" s="34"/>
@@ -11764,9 +11793,11 @@
       <c r="R63" s="35"/>
     </row>
     <row r="64" spans="7:29">
-      <c r="G64" s="9"/>
-      <c r="H64" s="7" t="s">
-        <v>193</v>
+      <c r="G64" s="8">
+        <v>44805</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="I64" s="34"/>
       <c r="J64" s="34"/>
@@ -11782,7 +11813,7 @@
     <row r="65" spans="7:18">
       <c r="G65" s="9"/>
       <c r="H65" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I65" s="34"/>
       <c r="J65" s="34"/>
@@ -11793,13 +11824,13 @@
       <c r="O65" s="34"/>
       <c r="P65" s="34"/>
       <c r="Q65" s="34"/>
-      <c r="R65" s="48" t="s">
-        <v>194</v>
-      </c>
+      <c r="R65" s="35"/>
     </row>
     <row r="66" spans="7:18">
       <c r="G66" s="9"/>
-      <c r="H66" s="34"/>
+      <c r="H66" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="I66" s="34"/>
       <c r="J66" s="34"/>
       <c r="K66" s="34"/>
@@ -11813,7 +11844,9 @@
     </row>
     <row r="67" spans="7:18">
       <c r="G67" s="9"/>
-      <c r="H67" s="34"/>
+      <c r="H67" s="7" t="s">
+        <v>191</v>
+      </c>
       <c r="I67" s="34"/>
       <c r="J67" s="34"/>
       <c r="K67" s="34"/>
@@ -11823,15 +11856,13 @@
       <c r="O67" s="34"/>
       <c r="P67" s="34"/>
       <c r="Q67" s="34"/>
-      <c r="R67" s="35"/>
+      <c r="R67" s="48" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="68" spans="7:18">
-      <c r="G68" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>196</v>
-      </c>
+      <c r="G68" s="9"/>
+      <c r="H68" s="34"/>
       <c r="I68" s="34"/>
       <c r="J68" s="34"/>
       <c r="K68" s="34"/>
@@ -11845,9 +11876,7 @@
     </row>
     <row r="69" spans="7:18">
       <c r="G69" s="9"/>
-      <c r="H69" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="H69" s="34"/>
       <c r="I69" s="34"/>
       <c r="J69" s="34"/>
       <c r="K69" s="34"/>
@@ -11860,9 +11889,11 @@
       <c r="R69" s="35"/>
     </row>
     <row r="70" spans="7:18">
-      <c r="G70" s="9"/>
-      <c r="H70" s="47" t="s">
-        <v>198</v>
+      <c r="G70" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>
@@ -11877,7 +11908,9 @@
     </row>
     <row r="71" spans="7:18">
       <c r="G71" s="9"/>
-      <c r="H71" s="34"/>
+      <c r="H71" s="7" t="s">
+        <v>197</v>
+      </c>
       <c r="I71" s="34"/>
       <c r="J71" s="34"/>
       <c r="K71" s="34"/>
@@ -11890,11 +11923,9 @@
       <c r="R71" s="35"/>
     </row>
     <row r="72" spans="7:18">
-      <c r="G72" s="8">
-        <v>44743</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>237</v>
+      <c r="G72" s="9"/>
+      <c r="H72" s="47" t="s">
+        <v>198</v>
       </c>
       <c r="I72" s="34"/>
       <c r="J72" s="34"/>
@@ -11909,9 +11940,7 @@
     </row>
     <row r="73" spans="7:18">
       <c r="G73" s="9"/>
-      <c r="H73" s="7" t="s">
-        <v>238</v>
-      </c>
+      <c r="H73" s="34"/>
       <c r="I73" s="34"/>
       <c r="J73" s="34"/>
       <c r="K73" s="34"/>
@@ -11924,8 +11953,12 @@
       <c r="R73" s="35"/>
     </row>
     <row r="74" spans="7:18">
-      <c r="G74" s="9"/>
-      <c r="H74" s="34"/>
+      <c r="G74" s="8">
+        <v>44743</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>237</v>
+      </c>
       <c r="I74" s="34"/>
       <c r="J74" s="34"/>
       <c r="K74" s="34"/>
@@ -11938,11 +11971,9 @@
       <c r="R74" s="35"/>
     </row>
     <row r="75" spans="7:18">
-      <c r="G75" s="8">
-        <v>44682</v>
-      </c>
-      <c r="H75" s="34" t="s">
-        <v>246</v>
+      <c r="G75" s="9"/>
+      <c r="H75" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="I75" s="34"/>
       <c r="J75" s="34"/>
@@ -11957,9 +11988,7 @@
     </row>
     <row r="76" spans="7:18">
       <c r="G76" s="9"/>
-      <c r="H76" s="7" t="s">
-        <v>247</v>
-      </c>
+      <c r="H76" s="34"/>
       <c r="I76" s="34"/>
       <c r="J76" s="34"/>
       <c r="K76" s="34"/>
@@ -11969,13 +11998,15 @@
       <c r="O76" s="34"/>
       <c r="P76" s="34"/>
       <c r="Q76" s="34"/>
-      <c r="R76" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R76" s="35"/>
     </row>
     <row r="77" spans="7:18">
-      <c r="G77" s="9"/>
-      <c r="H77" s="34"/>
+      <c r="G77" s="8">
+        <v>44682</v>
+      </c>
+      <c r="H77" s="34" t="s">
+        <v>246</v>
+      </c>
       <c r="I77" s="34"/>
       <c r="J77" s="34"/>
       <c r="K77" s="34"/>
@@ -11988,11 +12019,9 @@
       <c r="R77" s="35"/>
     </row>
     <row r="78" spans="7:18">
-      <c r="G78" s="8">
-        <v>43922</v>
-      </c>
-      <c r="H78" s="34" t="s">
-        <v>164</v>
+      <c r="G78" s="9"/>
+      <c r="H78" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="I78" s="34"/>
       <c r="J78" s="34"/>
@@ -12003,13 +12032,13 @@
       <c r="O78" s="34"/>
       <c r="P78" s="34"/>
       <c r="Q78" s="34"/>
-      <c r="R78" s="35"/>
+      <c r="R78" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="79" spans="7:18">
       <c r="G79" s="9"/>
-      <c r="H79" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="H79" s="34"/>
       <c r="I79" s="34"/>
       <c r="J79" s="34"/>
       <c r="K79" s="34"/>
@@ -12022,8 +12051,12 @@
       <c r="R79" s="35"/>
     </row>
     <row r="80" spans="7:18">
-      <c r="G80" s="9"/>
-      <c r="H80" s="34"/>
+      <c r="G80" s="8">
+        <v>43922</v>
+      </c>
+      <c r="H80" s="34" t="s">
+        <v>164</v>
+      </c>
       <c r="I80" s="34"/>
       <c r="J80" s="34"/>
       <c r="K80" s="34"/>
@@ -12033,13 +12066,13 @@
       <c r="O80" s="34"/>
       <c r="P80" s="34"/>
       <c r="Q80" s="34"/>
-      <c r="R80" s="48" t="s">
-        <v>31</v>
-      </c>
+      <c r="R80" s="35"/>
     </row>
     <row r="81" spans="7:18">
       <c r="G81" s="9"/>
-      <c r="H81" s="34"/>
+      <c r="H81" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="I81" s="34"/>
       <c r="J81" s="34"/>
       <c r="K81" s="34"/>
@@ -12052,12 +12085,8 @@
       <c r="R81" s="35"/>
     </row>
     <row r="82" spans="7:18">
-      <c r="G82" s="8">
-        <v>43770</v>
-      </c>
-      <c r="H82" s="34" t="s">
-        <v>167</v>
-      </c>
+      <c r="G82" s="9"/>
+      <c r="H82" s="34"/>
       <c r="I82" s="34"/>
       <c r="J82" s="34"/>
       <c r="K82" s="34"/>
@@ -12067,13 +12096,13 @@
       <c r="O82" s="34"/>
       <c r="P82" s="34"/>
       <c r="Q82" s="34"/>
-      <c r="R82" s="35"/>
+      <c r="R82" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="83" spans="7:18">
       <c r="G83" s="9"/>
-      <c r="H83" s="47" t="s">
-        <v>168</v>
-      </c>
+      <c r="H83" s="34"/>
       <c r="I83" s="34"/>
       <c r="J83" s="34"/>
       <c r="K83" s="34"/>
@@ -12086,8 +12115,12 @@
       <c r="R83" s="35"/>
     </row>
     <row r="84" spans="7:18">
-      <c r="G84" s="9"/>
-      <c r="H84" s="34"/>
+      <c r="G84" s="8">
+        <v>43770</v>
+      </c>
+      <c r="H84" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="I84" s="34"/>
       <c r="J84" s="34"/>
       <c r="K84" s="34"/>
@@ -12100,11 +12133,9 @@
       <c r="R84" s="35"/>
     </row>
     <row r="85" spans="7:18">
-      <c r="G85" s="8">
-        <v>43739</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>242</v>
+      <c r="G85" s="9"/>
+      <c r="H85" s="47" t="s">
+        <v>168</v>
       </c>
       <c r="I85" s="34"/>
       <c r="J85" s="34"/>
@@ -12114,9 +12145,7 @@
       <c r="N85" s="34"/>
       <c r="O85" s="34"/>
       <c r="P85" s="34"/>
-      <c r="Q85" s="34" t="s">
-        <v>179</v>
-      </c>
+      <c r="Q85" s="34"/>
       <c r="R85" s="35"/>
     </row>
     <row r="86" spans="7:18">
@@ -12134,8 +12163,12 @@
       <c r="R86" s="35"/>
     </row>
     <row r="87" spans="7:18">
-      <c r="G87" s="9"/>
-      <c r="H87" s="34"/>
+      <c r="G87" s="8">
+        <v>43739</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="I87" s="34"/>
       <c r="J87" s="34"/>
       <c r="K87" s="34"/>
@@ -12144,7 +12177,9 @@
       <c r="N87" s="34"/>
       <c r="O87" s="34"/>
       <c r="P87" s="34"/>
-      <c r="Q87" s="34"/>
+      <c r="Q87" s="34" t="s">
+        <v>179</v>
+      </c>
       <c r="R87" s="35"/>
     </row>
     <row r="88" spans="7:18">
@@ -12162,12 +12197,8 @@
       <c r="R88" s="35"/>
     </row>
     <row r="89" spans="7:18">
-      <c r="G89" s="8">
-        <v>43586</v>
-      </c>
-      <c r="H89" s="34" t="s">
-        <v>166</v>
-      </c>
+      <c r="G89" s="9"/>
+      <c r="H89" s="34"/>
       <c r="I89" s="34"/>
       <c r="J89" s="34"/>
       <c r="K89" s="34"/>
@@ -12195,10 +12226,10 @@
     </row>
     <row r="91" spans="7:18">
       <c r="G91" s="8">
-        <v>43282</v>
+        <v>43586</v>
       </c>
       <c r="H91" s="34" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I91" s="34"/>
       <c r="J91" s="34"/>
@@ -12213,9 +12244,7 @@
     </row>
     <row r="92" spans="7:18">
       <c r="G92" s="9"/>
-      <c r="H92" s="7" t="s">
-        <v>163</v>
-      </c>
+      <c r="H92" s="34"/>
       <c r="I92" s="34"/>
       <c r="J92" s="34"/>
       <c r="K92" s="34"/>
@@ -12228,9 +12257,11 @@
       <c r="R92" s="35"/>
     </row>
     <row r="93" spans="7:18">
-      <c r="G93" s="9"/>
-      <c r="H93" s="7" t="s">
-        <v>165</v>
+      <c r="G93" s="8">
+        <v>43282</v>
+      </c>
+      <c r="H93" s="34" t="s">
+        <v>162</v>
       </c>
       <c r="I93" s="34"/>
       <c r="J93" s="34"/>
@@ -12245,7 +12276,9 @@
     </row>
     <row r="94" spans="7:18">
       <c r="G94" s="9"/>
-      <c r="H94" s="34"/>
+      <c r="H94" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="I94" s="34"/>
       <c r="J94" s="34"/>
       <c r="K94" s="34"/>
@@ -12258,25 +12291,90 @@
       <c r="R94" s="35"/>
     </row>
     <row r="95" spans="7:18">
-      <c r="G95" s="85">
+      <c r="G95" s="9"/>
+      <c r="H95" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I95" s="34"/>
+      <c r="J95" s="34"/>
+      <c r="K95" s="34"/>
+      <c r="L95" s="34"/>
+      <c r="M95" s="34"/>
+      <c r="N95" s="34"/>
+      <c r="O95" s="34"/>
+      <c r="P95" s="34"/>
+      <c r="Q95" s="34"/>
+      <c r="R95" s="35"/>
+    </row>
+    <row r="96" spans="7:18">
+      <c r="G96" s="9"/>
+      <c r="H96" s="34"/>
+      <c r="I96" s="34"/>
+      <c r="J96" s="34"/>
+      <c r="K96" s="34"/>
+      <c r="L96" s="34"/>
+      <c r="M96" s="34"/>
+      <c r="N96" s="34"/>
+      <c r="O96" s="34"/>
+      <c r="P96" s="34"/>
+      <c r="Q96" s="34"/>
+      <c r="R96" s="35"/>
+    </row>
+    <row r="97" spans="7:18">
+      <c r="G97" s="85">
         <v>42552</v>
       </c>
-      <c r="H95" s="51" t="s">
+      <c r="H97" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="I95" s="32"/>
-      <c r="J95" s="32"/>
-      <c r="K95" s="32"/>
-      <c r="L95" s="32"/>
-      <c r="M95" s="32"/>
-      <c r="N95" s="32"/>
-      <c r="O95" s="32"/>
-      <c r="P95" s="32"/>
-      <c r="Q95" s="32"/>
-      <c r="R95" s="33"/>
+      <c r="I97" s="32"/>
+      <c r="J97" s="32"/>
+      <c r="K97" s="32"/>
+      <c r="L97" s="32"/>
+      <c r="M97" s="32"/>
+      <c r="N97" s="32"/>
+      <c r="O97" s="32"/>
+      <c r="P97" s="32"/>
+      <c r="Q97" s="32"/>
+      <c r="R97" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="Y61:AC61"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="Y5:AA5"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
@@ -12293,41 +12391,6 @@
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Y58:AC58"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="Y25:AC25"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C34:D34" r:id="rId1" display="Link" xr:uid="{11C3F337-5FA5-4654-84A9-81E0FD7B340B}"/>
@@ -12337,45 +12400,46 @@
     <hyperlink ref="D45" r:id="rId5" xr:uid="{127B302A-DD6D-6242-BA6C-25C1ED72AA7F}"/>
     <hyperlink ref="D44" r:id="rId6" xr:uid="{5B8750C0-94FB-994C-A836-E02A7A36CFF2}"/>
     <hyperlink ref="Y25:AC25" r:id="rId7" display="KC-390 Potential Buyers" xr:uid="{97B87E97-AF36-4B57-991B-B88C1F014D3C}"/>
-    <hyperlink ref="H16" r:id="rId8" xr:uid="{645C2C50-2541-448D-9073-14E40D1DE986}"/>
-    <hyperlink ref="H51" r:id="rId9" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
-    <hyperlink ref="H55" r:id="rId10" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
-    <hyperlink ref="R80" r:id="rId11" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
-    <hyperlink ref="H59" r:id="rId12" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
-    <hyperlink ref="H62" r:id="rId13" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
-    <hyperlink ref="R65" r:id="rId14" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
-    <hyperlink ref="H68" r:id="rId15" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
-    <hyperlink ref="H72" r:id="rId16" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
-    <hyperlink ref="H85" r:id="rId17" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
-    <hyperlink ref="R76" r:id="rId18" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
-    <hyperlink ref="H48" r:id="rId19" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
-    <hyperlink ref="H46" r:id="rId20" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
-    <hyperlink ref="H44" r:id="rId21" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
-    <hyperlink ref="H42" r:id="rId22" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
-    <hyperlink ref="H40" r:id="rId23" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
-    <hyperlink ref="H38" r:id="rId24" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
-    <hyperlink ref="H36" r:id="rId25" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
-    <hyperlink ref="H30" r:id="rId26" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
-    <hyperlink ref="H32" r:id="rId27" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
-    <hyperlink ref="H34" r:id="rId28" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
-    <hyperlink ref="H28" r:id="rId29" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
-    <hyperlink ref="H26" r:id="rId30" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
-    <hyperlink ref="H24" r:id="rId31" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
-    <hyperlink ref="H22" r:id="rId32" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
-    <hyperlink ref="H20" r:id="rId33" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
-    <hyperlink ref="H18" r:id="rId34" xr:uid="{DE4DB842-01BE-405E-8254-AC1C82253C72}"/>
-    <hyperlink ref="H14" r:id="rId35" xr:uid="{098F501F-A48C-49AD-B4EE-8F3B4711DA32}"/>
-    <hyperlink ref="H12" r:id="rId36" xr:uid="{EC3AC3B6-D20B-4612-96C2-C088131B252D}"/>
-    <hyperlink ref="H10" r:id="rId37" xr:uid="{327A318F-D59B-4B08-A396-86E7866F07CE}"/>
-    <hyperlink ref="H8" r:id="rId38" xr:uid="{F0AB9CE8-A127-4A54-A49C-B0BFF1ECBCFB}"/>
-    <hyperlink ref="H6" r:id="rId39" xr:uid="{2BC9EAF5-1571-44CC-AC7B-DE21B8FC3951}"/>
+    <hyperlink ref="H18" r:id="rId8" xr:uid="{645C2C50-2541-448D-9073-14E40D1DE986}"/>
+    <hyperlink ref="H53" r:id="rId9" xr:uid="{0E1650AB-35EE-47C2-9B99-22A7BB88CC6F}"/>
+    <hyperlink ref="H57" r:id="rId10" xr:uid="{64917365-2EAB-45F1-BFD3-E1E4F5A494BB}"/>
+    <hyperlink ref="R82" r:id="rId11" location="Boeing_Embraer_-_Defense" xr:uid="{CC492105-8696-4FC6-849B-A673602C4CB8}"/>
+    <hyperlink ref="H61" r:id="rId12" xr:uid="{E8520AE3-EE90-4F9C-82B7-9DC79CF177B0}"/>
+    <hyperlink ref="H64" r:id="rId13" display="L3Harris &amp; Embraer to develop new agile tanker varient of KC-390 to support USAF Operational Imperatives" xr:uid="{51AAA14D-A039-4171-BC04-5AAB9894A308}"/>
+    <hyperlink ref="R67" r:id="rId14" display="Link" xr:uid="{AE9B4E32-1957-4A54-8E54-10A62C8F25C4}"/>
+    <hyperlink ref="H70" r:id="rId15" display="Reuters report $ERJ expected to select engine in Q4 for potential turboprop launch in 2023" xr:uid="{3D245668-921A-4888-B384-DE0FC15EB559}"/>
+    <hyperlink ref="H74" r:id="rId16" xr:uid="{3143C16C-C4FE-C24A-A852-CE844A7EAA94}"/>
+    <hyperlink ref="H87" r:id="rId17" display="Airbus confirmed there are no plans to certify the A220-300 for LCY steep approach operations" xr:uid="{4BC4DC42-4422-D843-BFC6-DF67D759C7CD}"/>
+    <hyperlink ref="R78" r:id="rId18" xr:uid="{A3EFD621-318B-6143-AEF4-A74D7A31D835}"/>
+    <hyperlink ref="H50" r:id="rId19" xr:uid="{78DCAE8D-F9F2-4AFF-AEAC-B88136D9C452}"/>
+    <hyperlink ref="H48" r:id="rId20" xr:uid="{3999C1A1-07EF-48B9-810B-2F4E5BB942AE}"/>
+    <hyperlink ref="H46" r:id="rId21" xr:uid="{69C93ABC-34D8-0F45-AA69-CEEFC27F1A39}"/>
+    <hyperlink ref="H44" r:id="rId22" xr:uid="{6C54B13E-8F7B-4DCC-9E6A-C54F18CCE658}"/>
+    <hyperlink ref="H42" r:id="rId23" display="Embraer announce 2024 launch for the E-Jet P2F (cargo conversion) programme" xr:uid="{B3E5B1EC-A783-473C-B70D-A70E417CF572}"/>
+    <hyperlink ref="H40" r:id="rId24" xr:uid="{8C20766F-7147-41A6-A699-7D50EF5D73DA}"/>
+    <hyperlink ref="H38" r:id="rId25" xr:uid="{56959BC1-F64E-43D0-A4E0-57BAD8FCBCB7}"/>
+    <hyperlink ref="H32" r:id="rId26" xr:uid="{84A4CBC1-0653-495A-8986-5434F4F936B2}"/>
+    <hyperlink ref="H34" r:id="rId27" xr:uid="{7B01ED77-0E0F-4A8F-9A90-ADADF2B221C0}"/>
+    <hyperlink ref="H36" r:id="rId28" xr:uid="{ABF212CC-9083-4443-9432-F7D8F2F254A7}"/>
+    <hyperlink ref="H30" r:id="rId29" xr:uid="{689458CC-3F8D-48D3-BFB6-9021D5C41BFE}"/>
+    <hyperlink ref="H28" r:id="rId30" display="E2 Jets are approved for ETOPS-120 flight operations" xr:uid="{AFE0E501-14CD-4D1A-91DD-7F4349F2F287}"/>
+    <hyperlink ref="H26" r:id="rId31" xr:uid="{C86C50C0-49BF-42B4-ABB6-111374E16D26}"/>
+    <hyperlink ref="H24" r:id="rId32" display="Rumours that $ERJ wish to develop a competitor to A320/B737 series of aircraft within the next decade" xr:uid="{F075E770-E613-4A93-8C01-FCD751972BCD}"/>
+    <hyperlink ref="H22" r:id="rId33" xr:uid="{922CF349-49E0-4AFB-A330-58034F640FB7}"/>
+    <hyperlink ref="H20" r:id="rId34" xr:uid="{DE4DB842-01BE-405E-8254-AC1C82253C72}"/>
+    <hyperlink ref="H16" r:id="rId35" xr:uid="{098F501F-A48C-49AD-B4EE-8F3B4711DA32}"/>
+    <hyperlink ref="H14" r:id="rId36" xr:uid="{EC3AC3B6-D20B-4612-96C2-C088131B252D}"/>
+    <hyperlink ref="H12" r:id="rId37" xr:uid="{327A318F-D59B-4B08-A396-86E7866F07CE}"/>
+    <hyperlink ref="H10" r:id="rId38" xr:uid="{F0AB9CE8-A127-4A54-A49C-B0BFF1ECBCFB}"/>
+    <hyperlink ref="H8" r:id="rId39" xr:uid="{2BC9EAF5-1571-44CC-AC7B-DE21B8FC3951}"/>
+    <hyperlink ref="H6" r:id="rId40" display="Morroco believed to bew new customer of C-390 Millenium of unknown quantity" xr:uid="{3F47C2DD-329C-4BC5-A6B5-C20176AFBF93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId40"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId41"/>
   <ignoredErrors>
     <ignoredError sqref="C39:D40" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId41"/>
+  <drawing r:id="rId42"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
$RBLX Q424, $ERJ flexjets news
</commit_message>
<xml_diff>
--- a/$ERJ.xlsx
+++ b/$ERJ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF205616-A3EB-4103-B5D8-0F0A61518A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0FF019-3AAA-49E5-AF65-9AC6D4FB74AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
+    <workbookView xWindow="1320" yWindow="0" windowWidth="18090" windowHeight="15585" xr2:uid="{BFBD9EDE-FC47-49BF-96FE-182E73BB21C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="340">
   <si>
     <t>$ERJ</t>
   </si>
@@ -1239,6 +1239,9 @@
   <si>
     <t>Astral Aviation, the launch operator of E-Freighter, has exited deal to be launch operator of the type</t>
   </si>
+  <si>
+    <t>Embraer &amp; Flexjet sign $7bn agreement for ERJ to supply up to 182 aircraft &amp; options for another 30</t>
+  </si>
 </sst>
 </file>
 
@@ -1251,7 +1254,7 @@
     <numFmt numFmtId="167" formatCode="0.0000\x"/>
     <numFmt numFmtId="168" formatCode="mmmm\ yyyy;"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1441,6 +1444,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Aal"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1597,7 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1828,6 +1837,27 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1835,51 +1865,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1903,21 +1888,46 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
  